<commit_message>
Raw and Clean Data from SSA for June 5th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D39DF14-2BCD-7049-A266-4335DB6042D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3BB487-B333-0C4E-BF7C-CE700364685D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11600" yWindow="460" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="3340" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -444,6 +444,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -463,7 +487,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -608,6 +632,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1098,6 +1152,38 @@
         <v>314063</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>43987</v>
+      </c>
+      <c r="B6" s="56">
+        <v>110026</v>
+      </c>
+      <c r="C6" s="57">
+        <v>166049</v>
+      </c>
+      <c r="D6" s="58">
+        <v>48822</v>
+      </c>
+      <c r="E6" s="59">
+        <v>13170</v>
+      </c>
+      <c r="F6" s="60">
+        <v>34.025593950520786</v>
+      </c>
+      <c r="G6" s="61">
+        <v>37437</v>
+      </c>
+      <c r="H6" s="62">
+        <v>3501</v>
+      </c>
+      <c r="I6" s="63">
+        <v>3670</v>
+      </c>
+      <c r="J6" s="64">
+        <v>324897</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1108,7 +1194,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,15 +1350,33 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
+      <c r="A6" s="48">
+        <v>43987</v>
+      </c>
+      <c r="B6" s="49">
+        <v>0</v>
+      </c>
+      <c r="C6" s="49">
+        <v>1</v>
+      </c>
+      <c r="D6" s="49">
+        <v>1</v>
+      </c>
+      <c r="E6" s="49">
+        <v>1</v>
+      </c>
+      <c r="F6" s="49">
+        <v>0</v>
+      </c>
+      <c r="G6" s="49">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49">
+        <v>0</v>
+      </c>
+      <c r="I6" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="48"/>
@@ -1446,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1641,6 +1745,44 @@
         <v>0</v>
       </c>
       <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="48">
+        <v>43987</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
     </row>
@@ -1651,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1794,6 +1936,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="48">
+        <v>43987</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1801,10 +1969,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,7 +1980,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -1828,8 +1996,11 @@
       <c r="E1" s="50">
         <v>43986</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="50">
+        <v>43987</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>23</v>
       </c>
@@ -1842,11 +2013,14 @@
       <c r="D2" s="52">
         <v>3113</v>
       </c>
-      <c r="E2" s="52">
+      <c r="E2" s="66">
         <v>3145</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="49">
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
@@ -1859,11 +2033,14 @@
       <c r="D3" s="52">
         <v>2933</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="66">
         <v>2965</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="49">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>25</v>
       </c>
@@ -1876,11 +2053,14 @@
       <c r="D4" s="52">
         <v>2933</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="66">
         <v>2965</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="49">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>26</v>
       </c>
@@ -1893,11 +2073,14 @@
       <c r="D5" s="52">
         <v>2933</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="66">
         <v>2965</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="49">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>27</v>
       </c>
@@ -1910,11 +2093,14 @@
       <c r="D6" s="52">
         <v>2933</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="66">
         <v>2965</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="49">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>28</v>
       </c>
@@ -1927,11 +2113,14 @@
       <c r="D7" s="52">
         <v>2203</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="66">
         <v>2235</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="55">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>29</v>
       </c>
@@ -1944,18 +2133,22 @@
       <c r="D8" s="52">
         <v>4750</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="66">
         <v>4782</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="55">
+        <v>4814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="37"/>
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
       <c r="D9" s="54"/>
       <c r="E9" s="53"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>30</v>
       </c>
@@ -1968,11 +2161,14 @@
       <c r="D10" s="52">
         <v>143</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="66">
         <v>144</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>31</v>
       </c>
@@ -1985,11 +2181,14 @@
       <c r="D11" s="52">
         <v>143</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="66">
         <v>144</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>32</v>
       </c>
@@ -2002,11 +2201,14 @@
       <c r="D12" s="52">
         <v>143</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="66">
         <v>144</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>33</v>
       </c>
@@ -2019,11 +2221,14 @@
       <c r="D13" s="52">
         <v>143</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="66">
         <v>144</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
@@ -2036,11 +2241,14 @@
       <c r="D14" s="52">
         <v>143</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="66">
         <v>144</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="55">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
         <v>35</v>
       </c>
@@ -2053,11 +2261,14 @@
       <c r="D15" s="52">
         <v>120</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="66">
         <v>121</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="55">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>36</v>
       </c>
@@ -2070,18 +2281,21 @@
       <c r="D16" s="55">
         <v>155</v>
       </c>
-      <c r="E16" s="55">
+      <c r="E16" s="67">
         <v>156</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="55">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
       <c r="E17" s="53"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
@@ -2097,15 +2311,18 @@
       <c r="E18" s="52">
         <v>764</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="65">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>38</v>
       </c>
@@ -2114,7 +2331,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:E20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:F20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -2124,6 +2341,10 @@
       <c r="E20" s="52">
         <f t="shared" si="0"/>
         <v>23783</v>
+      </c>
+      <c r="F20" s="52">
+        <f t="shared" si="0"/>
+        <v>24021</v>
       </c>
     </row>
   </sheetData>
@@ -2330,7 +2551,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="323" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 6th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2429F27-4F74-044F-9A24-AAA1ACC14126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60D2CA-FF9C-7B46-89A6-6BCF6AFD77F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="3280" yWindow="480" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t xml:space="preserve">Porcentaje hospitalizados </t>
+  </si>
+  <si>
+    <t>2020-06-06</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,8 +397,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -448,17 +463,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -487,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -630,7 +634,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
@@ -659,9 +662,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,32 +1192,64 @@
       <c r="A6" s="15">
         <v>43987</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="55">
         <v>110026</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="56">
         <v>166049</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="57">
         <v>48822</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="58">
         <v>13170</v>
       </c>
-      <c r="F6" s="60">
+      <c r="F6" s="59">
         <v>34.025593950520786</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="60">
         <v>37437</v>
       </c>
-      <c r="H6" s="62">
+      <c r="H6" s="61">
         <v>3501</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="62">
         <v>3670</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="63">
         <v>324897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>43988</v>
+      </c>
+      <c r="B7" s="66">
+        <v>113619</v>
+      </c>
+      <c r="C7" s="67">
+        <v>170434</v>
+      </c>
+      <c r="D7" s="68">
+        <v>48273</v>
+      </c>
+      <c r="E7" s="69">
+        <v>13511</v>
+      </c>
+      <c r="F7" s="70">
+        <v>33.724993178957746</v>
+      </c>
+      <c r="G7" s="71">
+        <v>38318</v>
+      </c>
+      <c r="H7" s="72">
+        <v>3603</v>
+      </c>
+      <c r="I7" s="73">
+        <v>3761</v>
+      </c>
+      <c r="J7" s="74">
+        <v>332326</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1262,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,16 +1446,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="49">
+        <v>0</v>
+      </c>
+      <c r="C7" s="49">
+        <v>1</v>
+      </c>
+      <c r="D7" s="49">
+        <v>1</v>
+      </c>
+      <c r="E7" s="49">
+        <v>1</v>
+      </c>
+      <c r="F7" s="49">
+        <v>0</v>
+      </c>
+      <c r="G7" s="49">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49">
+        <v>0</v>
+      </c>
+      <c r="I7" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="48"/>
@@ -1550,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1783,6 +1869,44 @@
         <v>0</v>
       </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
     </row>
@@ -1793,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1962,6 +2086,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1969,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1980,7 +2130,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -1999,8 +2149,11 @@
       <c r="F1" s="50">
         <v>43987</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="50">
+        <v>43988</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>23</v>
       </c>
@@ -2013,14 +2166,17 @@
       <c r="D2" s="52">
         <v>3113</v>
       </c>
-      <c r="E2" s="66">
+      <c r="E2" s="64">
         <v>3145</v>
       </c>
       <c r="F2" s="49">
         <v>3177</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="75">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
@@ -2033,14 +2189,17 @@
       <c r="D3" s="52">
         <v>2933</v>
       </c>
-      <c r="E3" s="66">
+      <c r="E3" s="64">
         <v>2965</v>
       </c>
       <c r="F3" s="49">
         <v>2997</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="75">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>25</v>
       </c>
@@ -2053,14 +2212,17 @@
       <c r="D4" s="52">
         <v>2933</v>
       </c>
-      <c r="E4" s="66">
+      <c r="E4" s="64">
         <v>2965</v>
       </c>
       <c r="F4" s="49">
         <v>2997</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="75">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>26</v>
       </c>
@@ -2073,14 +2235,17 @@
       <c r="D5" s="52">
         <v>2933</v>
       </c>
-      <c r="E5" s="66">
+      <c r="E5" s="64">
         <v>2965</v>
       </c>
       <c r="F5" s="49">
         <v>2997</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="75">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>27</v>
       </c>
@@ -2093,14 +2258,17 @@
       <c r="D6" s="52">
         <v>2933</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="64">
         <v>2965</v>
       </c>
       <c r="F6" s="49">
         <v>2997</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="75">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>28</v>
       </c>
@@ -2113,14 +2281,17 @@
       <c r="D7" s="52">
         <v>2203</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="64">
         <v>2235</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="54">
         <v>2267</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="75">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>29</v>
       </c>
@@ -2133,22 +2304,26 @@
       <c r="D8" s="52">
         <v>4750</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="64">
         <v>4782</v>
       </c>
-      <c r="F8" s="55">
+      <c r="F8" s="54">
         <v>4814</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="75">
+        <v>4846</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="76"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>30</v>
       </c>
@@ -2161,14 +2336,17 @@
       <c r="D10" s="52">
         <v>143</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="64">
         <v>144</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="54">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="54">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>31</v>
       </c>
@@ -2181,14 +2359,17 @@
       <c r="D11" s="52">
         <v>143</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="64">
         <v>144</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="54">
         <v>145</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="54">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>32</v>
       </c>
@@ -2201,14 +2382,17 @@
       <c r="D12" s="52">
         <v>143</v>
       </c>
-      <c r="E12" s="66">
+      <c r="E12" s="64">
         <v>144</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="54">
         <v>145</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="54">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>33</v>
       </c>
@@ -2221,14 +2405,17 @@
       <c r="D13" s="52">
         <v>143</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="64">
         <v>144</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="54">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="54">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
@@ -2241,14 +2428,17 @@
       <c r="D14" s="52">
         <v>143</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="64">
         <v>144</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="54">
         <v>145</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="54">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
         <v>35</v>
       </c>
@@ -2261,41 +2451,47 @@
       <c r="D15" s="52">
         <v>120</v>
       </c>
-      <c r="E15" s="66">
+      <c r="E15" s="64">
         <v>121</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="54">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="54">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="54">
         <v>153</v>
       </c>
-      <c r="C16" s="55">
+      <c r="C16" s="54">
         <v>154</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="54">
         <v>155</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="65">
         <v>156</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="54">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="54">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
       <c r="E17" s="53"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
@@ -2311,18 +2507,21 @@
       <c r="E18" s="52">
         <v>764</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="54">
         <v>771</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="54">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>38</v>
       </c>
@@ -2331,7 +2530,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:F20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:G20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -2345,6 +2544,10 @@
       <c r="F20" s="52">
         <f t="shared" si="0"/>
         <v>24021</v>
+      </c>
+      <c r="G20" s="52">
+        <f t="shared" si="0"/>
+        <v>24259</v>
       </c>
     </row>
   </sheetData>
@@ -2357,7 +2560,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2508,7 +2711,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 7th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60D2CA-FF9C-7B46-89A6-6BCF6AFD77F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9334CF5A-3F86-AB4D-A103-53D4D504958A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="480" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="1160" yWindow="480" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -698,6 +698,34 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,6 +1280,38 @@
         <v>332326</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>43989</v>
+      </c>
+      <c r="B8" s="80">
+        <v>117103</v>
+      </c>
+      <c r="C8" s="81">
+        <v>173975</v>
+      </c>
+      <c r="D8" s="82">
+        <v>45317</v>
+      </c>
+      <c r="E8" s="83">
+        <v>13699</v>
+      </c>
+      <c r="F8" s="84">
+        <v>33.479073977609453</v>
+      </c>
+      <c r="G8" s="85">
+        <v>39205</v>
+      </c>
+      <c r="H8" s="86">
+        <v>3670</v>
+      </c>
+      <c r="I8" s="87">
+        <v>3828</v>
+      </c>
+      <c r="J8" s="88">
+        <v>336395</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1262,7 +1322,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,9 +1506,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
-        <v>67</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="48">
+        <v>43988</v>
       </c>
       <c r="B7" s="49">
         <v>0</v>
@@ -1476,15 +1536,33 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
+      <c r="A8" s="48">
+        <v>43989</v>
+      </c>
+      <c r="B8" s="49">
+        <v>0</v>
+      </c>
+      <c r="C8" s="49">
+        <v>1</v>
+      </c>
+      <c r="D8" s="49">
+        <v>1</v>
+      </c>
+      <c r="E8" s="49">
+        <v>1</v>
+      </c>
+      <c r="F8" s="49">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49">
+        <v>0</v>
+      </c>
+      <c r="I8" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
@@ -1636,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1907,6 +1985,44 @@
         <v>0</v>
       </c>
       <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="48">
+        <v>43989</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>0</v>
       </c>
     </row>
@@ -1917,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2112,6 +2228,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="48">
+        <v>43989</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2119,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2130,7 +2272,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -2152,8 +2294,21 @@
       <c r="G1" s="50">
         <v>43988</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="50">
+        <v>43989</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>23</v>
       </c>
@@ -2175,8 +2330,21 @@
       <c r="G2" s="75">
         <v>3209</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="49">
+        <v>3241</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
@@ -2198,8 +2366,21 @@
       <c r="G3" s="75">
         <v>3029</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="49">
+        <v>3061</v>
+      </c>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>25</v>
       </c>
@@ -2221,8 +2402,21 @@
       <c r="G4" s="75">
         <v>3029</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="49">
+        <v>3061</v>
+      </c>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>26</v>
       </c>
@@ -2244,8 +2438,21 @@
       <c r="G5" s="75">
         <v>3029</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="49">
+        <v>3061</v>
+      </c>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>27</v>
       </c>
@@ -2267,8 +2474,21 @@
       <c r="G6" s="75">
         <v>3029</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="49">
+        <v>3061</v>
+      </c>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>28</v>
       </c>
@@ -2290,8 +2510,21 @@
       <c r="G7" s="75">
         <v>2299</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="75">
+        <v>2331</v>
+      </c>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>29</v>
       </c>
@@ -2313,8 +2546,21 @@
       <c r="G8" s="75">
         <v>4846</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="75">
+        <v>4878</v>
+      </c>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="76"/>
       <c r="B9" s="77"/>
       <c r="C9" s="77"/>
@@ -2322,8 +2568,19 @@
       <c r="E9" s="77"/>
       <c r="F9" s="79"/>
       <c r="G9" s="79"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+      <c r="P9" s="89"/>
+      <c r="Q9" s="89"/>
+      <c r="R9" s="89"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>30</v>
       </c>
@@ -2345,8 +2602,21 @@
       <c r="G10" s="54">
         <v>146</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="49">
+        <v>147</v>
+      </c>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>31</v>
       </c>
@@ -2368,8 +2638,21 @@
       <c r="G11" s="54">
         <v>146</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="49">
+        <v>147</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>32</v>
       </c>
@@ -2391,8 +2674,21 @@
       <c r="G12" s="54">
         <v>146</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="49">
+        <v>147</v>
+      </c>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>33</v>
       </c>
@@ -2414,8 +2710,21 @@
       <c r="G13" s="54">
         <v>146</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="49">
+        <v>147</v>
+      </c>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
@@ -2437,8 +2746,21 @@
       <c r="G14" s="54">
         <v>146</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="49">
+        <v>147</v>
+      </c>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
         <v>35</v>
       </c>
@@ -2460,8 +2782,21 @@
       <c r="G15" s="54">
         <v>123</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="49">
+        <v>124</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>36</v>
       </c>
@@ -2483,15 +2818,41 @@
       <c r="G16" s="54">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="49">
+        <v>159</v>
+      </c>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="76"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="89"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="89"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
@@ -2513,15 +2874,28 @@
       <c r="G18" s="54">
         <v>778</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="49">
+        <v>785</v>
+      </c>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>38</v>
       </c>
@@ -2530,7 +2904,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:G20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:H20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -2549,6 +2923,20 @@
         <f t="shared" si="0"/>
         <v>24259</v>
       </c>
+      <c r="H20" s="52">
+        <f t="shared" si="0"/>
+        <v>24497</v>
+      </c>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 8th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9334CF5A-3F86-AB4D-A103-53D4D504958A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B826CDC-E268-7A49-A6B2-CA2C53E7465C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="480" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="6840" yWindow="500" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -726,6 +726,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1045,15 +1072,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -1310,6 +1337,38 @@
       </c>
       <c r="J8" s="88">
         <v>336395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>43990</v>
+      </c>
+      <c r="B9" s="90">
+        <v>120102</v>
+      </c>
+      <c r="C9" s="91">
+        <v>177875</v>
+      </c>
+      <c r="D9" s="92">
+        <v>46398</v>
+      </c>
+      <c r="E9" s="93">
+        <v>14053</v>
+      </c>
+      <c r="F9" s="94">
+        <v>33.315015570098751</v>
+      </c>
+      <c r="G9" s="95">
+        <v>40012</v>
+      </c>
+      <c r="H9" s="96">
+        <v>3733</v>
+      </c>
+      <c r="I9" s="97">
+        <v>3891</v>
+      </c>
+      <c r="J9" s="98">
+        <v>344375</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1381,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,15 +1624,33 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
+      <c r="A9" s="48">
+        <v>43990</v>
+      </c>
+      <c r="B9" s="49">
+        <v>0</v>
+      </c>
+      <c r="C9" s="49">
+        <v>1</v>
+      </c>
+      <c r="D9" s="49">
+        <v>1</v>
+      </c>
+      <c r="E9" s="49">
+        <v>1</v>
+      </c>
+      <c r="F9" s="49">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49">
+        <v>0</v>
+      </c>
+      <c r="I9" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
@@ -1714,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2025,6 +2102,47 @@
       <c r="L8">
         <v>0</v>
       </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="48">
+        <v>43990</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2033,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2254,6 +2372,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="48">
+        <v>43990</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2264,7 +2408,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2297,7 +2441,9 @@
       <c r="H1" s="50">
         <v>43989</v>
       </c>
-      <c r="I1" s="50"/>
+      <c r="I1" s="50">
+        <v>43990</v>
+      </c>
       <c r="J1" s="50"/>
       <c r="K1" s="50"/>
       <c r="L1" s="50"/>
@@ -2333,7 +2479,9 @@
       <c r="H2" s="49">
         <v>3241</v>
       </c>
-      <c r="I2" s="49"/>
+      <c r="I2" s="49">
+        <v>3273</v>
+      </c>
       <c r="J2" s="49"/>
       <c r="K2" s="49"/>
       <c r="L2" s="49"/>
@@ -2369,7 +2517,9 @@
       <c r="H3" s="49">
         <v>3061</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="49">
+        <v>3093</v>
+      </c>
       <c r="J3" s="49"/>
       <c r="K3" s="49"/>
       <c r="L3" s="49"/>
@@ -2405,7 +2555,9 @@
       <c r="H4" s="49">
         <v>3061</v>
       </c>
-      <c r="I4" s="49"/>
+      <c r="I4" s="49">
+        <v>3093</v>
+      </c>
       <c r="J4" s="49"/>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
@@ -2441,7 +2593,9 @@
       <c r="H5" s="49">
         <v>3061</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="49">
+        <v>3093</v>
+      </c>
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
@@ -2477,7 +2631,9 @@
       <c r="H6" s="49">
         <v>3061</v>
       </c>
-      <c r="I6" s="49"/>
+      <c r="I6" s="49">
+        <v>3093</v>
+      </c>
       <c r="J6" s="49"/>
       <c r="K6" s="49"/>
       <c r="L6" s="49"/>
@@ -2513,7 +2669,9 @@
       <c r="H7" s="75">
         <v>2331</v>
       </c>
-      <c r="I7" s="49"/>
+      <c r="I7" s="49">
+        <v>2363</v>
+      </c>
       <c r="J7" s="49"/>
       <c r="K7" s="49"/>
       <c r="L7" s="49"/>
@@ -2549,7 +2707,9 @@
       <c r="H8" s="75">
         <v>4878</v>
       </c>
-      <c r="I8" s="49"/>
+      <c r="I8" s="49">
+        <v>4910</v>
+      </c>
       <c r="J8" s="49"/>
       <c r="K8" s="49"/>
       <c r="L8" s="49"/>
@@ -2605,7 +2765,9 @@
       <c r="H10" s="49">
         <v>147</v>
       </c>
-      <c r="I10" s="49"/>
+      <c r="I10" s="49">
+        <v>148</v>
+      </c>
       <c r="J10" s="49"/>
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
@@ -2641,7 +2803,9 @@
       <c r="H11" s="49">
         <v>147</v>
       </c>
-      <c r="I11" s="49"/>
+      <c r="I11" s="49">
+        <v>148</v>
+      </c>
       <c r="J11" s="49"/>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
@@ -2677,7 +2841,9 @@
       <c r="H12" s="49">
         <v>147</v>
       </c>
-      <c r="I12" s="49"/>
+      <c r="I12" s="49">
+        <v>148</v>
+      </c>
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
@@ -2713,7 +2879,9 @@
       <c r="H13" s="49">
         <v>147</v>
       </c>
-      <c r="I13" s="49"/>
+      <c r="I13" s="49">
+        <v>148</v>
+      </c>
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
@@ -2749,7 +2917,9 @@
       <c r="H14" s="49">
         <v>147</v>
       </c>
-      <c r="I14" s="49"/>
+      <c r="I14" s="49">
+        <v>148</v>
+      </c>
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
@@ -2785,7 +2955,9 @@
       <c r="H15" s="49">
         <v>124</v>
       </c>
-      <c r="I15" s="49"/>
+      <c r="I15" s="49">
+        <v>125</v>
+      </c>
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
@@ -2821,7 +2993,9 @@
       <c r="H16" s="49">
         <v>159</v>
       </c>
-      <c r="I16" s="49"/>
+      <c r="I16" s="49">
+        <v>160</v>
+      </c>
       <c r="J16" s="49"/>
       <c r="K16" s="49"/>
       <c r="L16" s="49"/>
@@ -2877,7 +3051,9 @@
       <c r="H18" s="49">
         <v>785</v>
       </c>
-      <c r="I18" s="49"/>
+      <c r="I18" s="49">
+        <v>792</v>
+      </c>
       <c r="J18" s="49"/>
       <c r="K18" s="49"/>
       <c r="L18" s="49"/>
@@ -2904,7 +3080,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:H20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:I20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -2927,7 +3103,10 @@
         <f t="shared" si="0"/>
         <v>24497</v>
       </c>
-      <c r="I20" s="49"/>
+      <c r="I20" s="52">
+        <f t="shared" si="0"/>
+        <v>24735</v>
+      </c>
       <c r="J20" s="49"/>
       <c r="K20" s="49"/>
       <c r="L20" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 9th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B826CDC-E268-7A49-A6B2-CA2C53E7465C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507E799F-1CFA-F842-9E1E-53456D2EC597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="500" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2060" yWindow="580" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -753,6 +753,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,6 +1399,38 @@
         <v>344375</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>43991</v>
+      </c>
+      <c r="B10" s="99">
+        <v>124301</v>
+      </c>
+      <c r="C10" s="100">
+        <v>182077</v>
+      </c>
+      <c r="D10" s="101">
+        <v>50677</v>
+      </c>
+      <c r="E10" s="102">
+        <v>14649</v>
+      </c>
+      <c r="F10" s="103">
+        <v>33.206490695971873</v>
+      </c>
+      <c r="G10" s="104">
+        <v>41276</v>
+      </c>
+      <c r="H10" s="105">
+        <v>3826</v>
+      </c>
+      <c r="I10" s="106">
+        <v>3982</v>
+      </c>
+      <c r="J10" s="107">
+        <v>357055</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1381,7 +1441,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1653,15 +1713,33 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
+      <c r="A10" s="48">
+        <v>43991</v>
+      </c>
+      <c r="B10" s="49">
+        <v>0</v>
+      </c>
+      <c r="C10" s="49">
+        <v>1</v>
+      </c>
+      <c r="D10" s="49">
+        <v>1</v>
+      </c>
+      <c r="E10" s="49">
+        <v>1</v>
+      </c>
+      <c r="F10" s="49">
+        <v>0</v>
+      </c>
+      <c r="G10" s="49">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49">
+        <v>0</v>
+      </c>
+      <c r="I10" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="48"/>
@@ -1794,7 +1872,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2142,7 +2220,42 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
+      <c r="A10" s="48">
+        <v>43991</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2398,6 +2511,101 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="48">
+        <v>43991</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="108"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="108"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="108"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="108"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="108"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="108"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="108"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="108"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="108"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="108"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="108"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="108"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="108"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="108"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="108"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="108"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="108"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="108"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="108"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="108"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="108"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="108"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="108"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2408,7 +2616,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,7 +2652,9 @@
       <c r="I1" s="50">
         <v>43990</v>
       </c>
-      <c r="J1" s="50"/>
+      <c r="J1" s="50">
+        <v>43991</v>
+      </c>
       <c r="K1" s="50"/>
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
@@ -2482,7 +2692,9 @@
       <c r="I2" s="49">
         <v>3273</v>
       </c>
-      <c r="J2" s="49"/>
+      <c r="J2" s="49">
+        <v>3305</v>
+      </c>
       <c r="K2" s="49"/>
       <c r="L2" s="49"/>
       <c r="M2" s="49"/>
@@ -2520,7 +2732,9 @@
       <c r="I3" s="49">
         <v>3093</v>
       </c>
-      <c r="J3" s="49"/>
+      <c r="J3" s="49">
+        <v>3120</v>
+      </c>
       <c r="K3" s="49"/>
       <c r="L3" s="49"/>
       <c r="M3" s="49"/>
@@ -2558,7 +2772,9 @@
       <c r="I4" s="49">
         <v>3093</v>
       </c>
-      <c r="J4" s="49"/>
+      <c r="J4" s="49">
+        <v>3120</v>
+      </c>
       <c r="K4" s="49"/>
       <c r="L4" s="49"/>
       <c r="M4" s="49"/>
@@ -2596,7 +2812,9 @@
       <c r="I5" s="49">
         <v>3093</v>
       </c>
-      <c r="J5" s="49"/>
+      <c r="J5" s="49">
+        <v>3120</v>
+      </c>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
       <c r="M5" s="49"/>
@@ -2634,7 +2852,9 @@
       <c r="I6" s="49">
         <v>3093</v>
       </c>
-      <c r="J6" s="49"/>
+      <c r="J6" s="49">
+        <v>3120</v>
+      </c>
       <c r="K6" s="49"/>
       <c r="L6" s="49"/>
       <c r="M6" s="49"/>
@@ -2672,7 +2892,9 @@
       <c r="I7" s="49">
         <v>2363</v>
       </c>
-      <c r="J7" s="49"/>
+      <c r="J7" s="49">
+        <v>2395</v>
+      </c>
       <c r="K7" s="49"/>
       <c r="L7" s="49"/>
       <c r="M7" s="49"/>
@@ -2710,7 +2932,9 @@
       <c r="I8" s="49">
         <v>4910</v>
       </c>
-      <c r="J8" s="49"/>
+      <c r="J8" s="49">
+        <v>4942</v>
+      </c>
       <c r="K8" s="49"/>
       <c r="L8" s="49"/>
       <c r="M8" s="49"/>
@@ -2768,7 +2992,9 @@
       <c r="I10" s="49">
         <v>148</v>
       </c>
-      <c r="J10" s="49"/>
+      <c r="J10" s="49">
+        <v>149</v>
+      </c>
       <c r="K10" s="49"/>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
@@ -2806,7 +3032,9 @@
       <c r="I11" s="49">
         <v>148</v>
       </c>
-      <c r="J11" s="49"/>
+      <c r="J11" s="49">
+        <v>149</v>
+      </c>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
@@ -2844,7 +3072,9 @@
       <c r="I12" s="49">
         <v>148</v>
       </c>
-      <c r="J12" s="49"/>
+      <c r="J12" s="49">
+        <v>149</v>
+      </c>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
       <c r="M12" s="49"/>
@@ -2882,7 +3112,9 @@
       <c r="I13" s="49">
         <v>148</v>
       </c>
-      <c r="J13" s="49"/>
+      <c r="J13" s="49">
+        <v>149</v>
+      </c>
       <c r="K13" s="49"/>
       <c r="L13" s="49"/>
       <c r="M13" s="49"/>
@@ -2920,7 +3152,9 @@
       <c r="I14" s="49">
         <v>148</v>
       </c>
-      <c r="J14" s="49"/>
+      <c r="J14" s="49">
+        <v>149</v>
+      </c>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
       <c r="M14" s="49"/>
@@ -2958,7 +3192,9 @@
       <c r="I15" s="49">
         <v>125</v>
       </c>
-      <c r="J15" s="49"/>
+      <c r="J15" s="49">
+        <v>126</v>
+      </c>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
       <c r="M15" s="49"/>
@@ -2996,7 +3232,9 @@
       <c r="I16" s="49">
         <v>160</v>
       </c>
-      <c r="J16" s="49"/>
+      <c r="J16" s="49">
+        <v>161</v>
+      </c>
       <c r="K16" s="49"/>
       <c r="L16" s="49"/>
       <c r="M16" s="49"/>
@@ -3054,7 +3292,9 @@
       <c r="I18" s="49">
         <v>792</v>
       </c>
-      <c r="J18" s="49"/>
+      <c r="J18" s="49">
+        <v>799</v>
+      </c>
       <c r="K18" s="49"/>
       <c r="L18" s="49"/>
       <c r="M18" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 10th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507E799F-1CFA-F842-9E1E-53456D2EC597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2ECDEA-D4E5-314A-9F8F-D7F3E5617EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="580" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +781,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1431,6 +1458,38 @@
         <v>357055</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
+        <v>43992</v>
+      </c>
+      <c r="B11" s="109">
+        <v>129184</v>
+      </c>
+      <c r="C11" s="110">
+        <v>186570</v>
+      </c>
+      <c r="D11" s="111">
+        <v>53608</v>
+      </c>
+      <c r="E11" s="112">
+        <v>15357</v>
+      </c>
+      <c r="F11" s="113">
+        <v>33.110137478325491</v>
+      </c>
+      <c r="G11" s="114">
+        <v>42773</v>
+      </c>
+      <c r="H11" s="115">
+        <v>3970</v>
+      </c>
+      <c r="I11" s="116">
+        <v>4126</v>
+      </c>
+      <c r="J11" s="117">
+        <v>369362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1441,7 +1500,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1742,15 +1801,33 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
+      <c r="A11" s="48">
+        <v>43992</v>
+      </c>
+      <c r="B11" s="49">
+        <v>0</v>
+      </c>
+      <c r="C11" s="49">
+        <v>1</v>
+      </c>
+      <c r="D11" s="49">
+        <v>1</v>
+      </c>
+      <c r="E11" s="49">
+        <v>1</v>
+      </c>
+      <c r="F11" s="49">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49">
+        <v>0</v>
+      </c>
+      <c r="I11" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
@@ -1869,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2254,6 +2331,44 @@
         <v>0</v>
       </c>
       <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="48">
+        <v>43992</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>0</v>
       </c>
     </row>
@@ -2267,7 +2382,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2538,7 +2653,30 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="108"/>
+      <c r="A11" s="48">
+        <v>43992</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="108"/>
@@ -2616,7 +2754,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2655,7 +2793,9 @@
       <c r="J1" s="50">
         <v>43991</v>
       </c>
-      <c r="K1" s="50"/>
+      <c r="K1" s="50">
+        <v>43992</v>
+      </c>
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
       <c r="N1" s="50"/>
@@ -2695,7 +2835,9 @@
       <c r="J2" s="49">
         <v>3305</v>
       </c>
-      <c r="K2" s="49"/>
+      <c r="K2" s="49">
+        <v>3337</v>
+      </c>
       <c r="L2" s="49"/>
       <c r="M2" s="49"/>
       <c r="N2" s="49"/>
@@ -2735,7 +2877,9 @@
       <c r="J3" s="49">
         <v>3120</v>
       </c>
-      <c r="K3" s="49"/>
+      <c r="K3" s="49">
+        <v>3152</v>
+      </c>
       <c r="L3" s="49"/>
       <c r="M3" s="49"/>
       <c r="N3" s="49"/>
@@ -2775,7 +2919,9 @@
       <c r="J4" s="49">
         <v>3120</v>
       </c>
-      <c r="K4" s="49"/>
+      <c r="K4" s="49">
+        <v>3152</v>
+      </c>
       <c r="L4" s="49"/>
       <c r="M4" s="49"/>
       <c r="N4" s="49"/>
@@ -2815,7 +2961,9 @@
       <c r="J5" s="49">
         <v>3120</v>
       </c>
-      <c r="K5" s="49"/>
+      <c r="K5" s="49">
+        <v>3152</v>
+      </c>
       <c r="L5" s="49"/>
       <c r="M5" s="49"/>
       <c r="N5" s="49"/>
@@ -2855,7 +3003,9 @@
       <c r="J6" s="49">
         <v>3120</v>
       </c>
-      <c r="K6" s="49"/>
+      <c r="K6" s="49">
+        <v>3152</v>
+      </c>
       <c r="L6" s="49"/>
       <c r="M6" s="49"/>
       <c r="N6" s="49"/>
@@ -2895,7 +3045,9 @@
       <c r="J7" s="49">
         <v>2395</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="49">
+        <v>2449</v>
+      </c>
       <c r="L7" s="49"/>
       <c r="M7" s="49"/>
       <c r="N7" s="49"/>
@@ -2935,7 +3087,9 @@
       <c r="J8" s="49">
         <v>4942</v>
       </c>
-      <c r="K8" s="49"/>
+      <c r="K8" s="49">
+        <v>4974</v>
+      </c>
       <c r="L8" s="49"/>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
@@ -2995,7 +3149,9 @@
       <c r="J10" s="49">
         <v>149</v>
       </c>
-      <c r="K10" s="49"/>
+      <c r="K10" s="49">
+        <v>150</v>
+      </c>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
       <c r="N10" s="49"/>
@@ -3035,7 +3191,9 @@
       <c r="J11" s="49">
         <v>149</v>
       </c>
-      <c r="K11" s="49"/>
+      <c r="K11" s="49">
+        <v>150</v>
+      </c>
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
@@ -3075,7 +3233,9 @@
       <c r="J12" s="49">
         <v>149</v>
       </c>
-      <c r="K12" s="49"/>
+      <c r="K12" s="49">
+        <v>150</v>
+      </c>
       <c r="L12" s="49"/>
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
@@ -3115,7 +3275,9 @@
       <c r="J13" s="49">
         <v>149</v>
       </c>
-      <c r="K13" s="49"/>
+      <c r="K13" s="49">
+        <v>150</v>
+      </c>
       <c r="L13" s="49"/>
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
@@ -3155,7 +3317,9 @@
       <c r="J14" s="49">
         <v>149</v>
       </c>
-      <c r="K14" s="49"/>
+      <c r="K14" s="49">
+        <v>150</v>
+      </c>
       <c r="L14" s="49"/>
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
@@ -3195,7 +3359,9 @@
       <c r="J15" s="49">
         <v>126</v>
       </c>
-      <c r="K15" s="49"/>
+      <c r="K15" s="49">
+        <v>127</v>
+      </c>
       <c r="L15" s="49"/>
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
@@ -3235,7 +3401,9 @@
       <c r="J16" s="49">
         <v>161</v>
       </c>
-      <c r="K16" s="49"/>
+      <c r="K16" s="49">
+        <v>162</v>
+      </c>
       <c r="L16" s="49"/>
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
@@ -3295,7 +3463,9 @@
       <c r="J18" s="49">
         <v>799</v>
       </c>
-      <c r="K18" s="49"/>
+      <c r="K18" s="49">
+        <v>806</v>
+      </c>
       <c r="L18" s="49"/>
       <c r="M18" s="49"/>
       <c r="N18" s="49"/>
@@ -3320,7 +3490,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:I20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:K20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -3347,8 +3517,14 @@
         <f t="shared" si="0"/>
         <v>24735</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
+      <c r="J20" s="52">
+        <f t="shared" si="0"/>
+        <v>24953</v>
+      </c>
+      <c r="K20" s="52">
+        <f t="shared" si="0"/>
+        <v>25213</v>
+      </c>
       <c r="L20" s="49"/>
       <c r="M20" s="49"/>
       <c r="N20" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 11th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2ECDEA-D4E5-314A-9F8F-D7F3E5617EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F750466-1016-D548-8EA7-02B119BE371E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +781,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1127,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1490,6 +1517,38 @@
         <v>369362</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
+        <v>43993</v>
+      </c>
+      <c r="B12" s="118">
+        <v>133974</v>
+      </c>
+      <c r="C12" s="119">
+        <v>191465</v>
+      </c>
+      <c r="D12" s="120">
+        <v>55700</v>
+      </c>
+      <c r="E12" s="121">
+        <v>15944</v>
+      </c>
+      <c r="F12" s="122">
+        <v>33.006404227685969</v>
+      </c>
+      <c r="G12" s="123">
+        <v>44220</v>
+      </c>
+      <c r="H12" s="124">
+        <v>4087</v>
+      </c>
+      <c r="I12" s="125">
+        <v>4256</v>
+      </c>
+      <c r="J12" s="126">
+        <v>381139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1500,7 +1559,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1830,15 +1889,33 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
+      <c r="A12" s="48">
+        <v>43993</v>
+      </c>
+      <c r="B12" s="49">
+        <v>0</v>
+      </c>
+      <c r="C12" s="49">
+        <v>1</v>
+      </c>
+      <c r="D12" s="49">
+        <v>1</v>
+      </c>
+      <c r="E12" s="49">
+        <v>1</v>
+      </c>
+      <c r="F12" s="49">
+        <v>0</v>
+      </c>
+      <c r="G12" s="49">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49">
+        <v>0</v>
+      </c>
+      <c r="I12" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
@@ -1946,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2371,6 +2448,47 @@
       <c r="L11">
         <v>0</v>
       </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="48">
+        <v>43993</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2382,7 +2500,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2679,7 +2797,30 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="108"/>
+      <c r="A12" s="48">
+        <v>43993</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="108"/>
@@ -2753,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2796,7 +2937,9 @@
       <c r="K1" s="50">
         <v>43992</v>
       </c>
-      <c r="L1" s="50"/>
+      <c r="L1" s="50">
+        <v>43993</v>
+      </c>
       <c r="M1" s="50"/>
       <c r="N1" s="50"/>
       <c r="O1" s="50"/>
@@ -2838,7 +2981,9 @@
       <c r="K2" s="49">
         <v>3337</v>
       </c>
-      <c r="L2" s="49"/>
+      <c r="L2" s="49">
+        <v>3369</v>
+      </c>
       <c r="M2" s="49"/>
       <c r="N2" s="49"/>
       <c r="O2" s="49"/>
@@ -2880,7 +3025,9 @@
       <c r="K3" s="49">
         <v>3152</v>
       </c>
-      <c r="L3" s="49"/>
+      <c r="L3" s="49">
+        <v>3184</v>
+      </c>
       <c r="M3" s="49"/>
       <c r="N3" s="49"/>
       <c r="O3" s="49"/>
@@ -2922,7 +3069,9 @@
       <c r="K4" s="49">
         <v>3152</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="49">
+        <v>3184</v>
+      </c>
       <c r="M4" s="49"/>
       <c r="N4" s="49"/>
       <c r="O4" s="49"/>
@@ -2964,7 +3113,9 @@
       <c r="K5" s="49">
         <v>3152</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="49">
+        <v>3184</v>
+      </c>
       <c r="M5" s="49"/>
       <c r="N5" s="49"/>
       <c r="O5" s="49"/>
@@ -3006,7 +3157,9 @@
       <c r="K6" s="49">
         <v>3152</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="49">
+        <v>3184</v>
+      </c>
       <c r="M6" s="49"/>
       <c r="N6" s="49"/>
       <c r="O6" s="49"/>
@@ -3048,7 +3201,9 @@
       <c r="K7" s="49">
         <v>2449</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="49">
+        <v>2481</v>
+      </c>
       <c r="M7" s="49"/>
       <c r="N7" s="49"/>
       <c r="O7" s="49"/>
@@ -3090,7 +3245,9 @@
       <c r="K8" s="49">
         <v>4974</v>
       </c>
-      <c r="L8" s="49"/>
+      <c r="L8" s="49">
+        <v>5006</v>
+      </c>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
       <c r="O8" s="49"/>
@@ -3152,7 +3309,9 @@
       <c r="K10" s="49">
         <v>150</v>
       </c>
-      <c r="L10" s="49"/>
+      <c r="L10" s="49">
+        <v>151</v>
+      </c>
       <c r="M10" s="49"/>
       <c r="N10" s="49"/>
       <c r="O10" s="49"/>
@@ -3194,7 +3353,9 @@
       <c r="K11" s="49">
         <v>150</v>
       </c>
-      <c r="L11" s="49"/>
+      <c r="L11" s="49">
+        <v>151</v>
+      </c>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
       <c r="O11" s="49"/>
@@ -3236,7 +3397,9 @@
       <c r="K12" s="49">
         <v>150</v>
       </c>
-      <c r="L12" s="49"/>
+      <c r="L12" s="49">
+        <v>151</v>
+      </c>
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
       <c r="O12" s="49"/>
@@ -3278,7 +3441,9 @@
       <c r="K13" s="49">
         <v>150</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="49">
+        <v>151</v>
+      </c>
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
       <c r="O13" s="49"/>
@@ -3320,7 +3485,9 @@
       <c r="K14" s="49">
         <v>150</v>
       </c>
-      <c r="L14" s="49"/>
+      <c r="L14" s="49">
+        <v>151</v>
+      </c>
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
@@ -3362,7 +3529,9 @@
       <c r="K15" s="49">
         <v>127</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="49">
+        <v>128</v>
+      </c>
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
       <c r="O15" s="49"/>
@@ -3404,7 +3573,9 @@
       <c r="K16" s="49">
         <v>162</v>
       </c>
-      <c r="L16" s="49"/>
+      <c r="L16" s="49">
+        <v>163</v>
+      </c>
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
       <c r="O16" s="49"/>
@@ -3466,7 +3637,9 @@
       <c r="K18" s="49">
         <v>806</v>
       </c>
-      <c r="L18" s="49"/>
+      <c r="L18" s="49">
+        <v>813</v>
+      </c>
       <c r="M18" s="49"/>
       <c r="N18" s="49"/>
       <c r="O18" s="49"/>
@@ -3490,7 +3663,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:K20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:L20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -3525,7 +3698,10 @@
         <f t="shared" si="0"/>
         <v>25213</v>
       </c>
-      <c r="L20" s="49"/>
+      <c r="L20" s="52">
+        <f t="shared" si="0"/>
+        <v>25451</v>
+      </c>
       <c r="M20" s="49"/>
       <c r="N20" s="49"/>
       <c r="O20" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 12th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F750466-1016-D548-8EA7-02B119BE371E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D545DDE2-7A46-D743-ACA7-5E068CE8B087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="560" windowWidth="27640" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="540" yWindow="920" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +781,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1154,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1549,6 +1576,38 @@
         <v>381139</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
+        <v>43994</v>
+      </c>
+      <c r="B13" s="127">
+        <v>139196</v>
+      </c>
+      <c r="C13" s="128">
+        <v>197590</v>
+      </c>
+      <c r="D13" s="129">
+        <v>56928</v>
+      </c>
+      <c r="E13" s="130">
+        <v>16448</v>
+      </c>
+      <c r="F13" s="131">
+        <v>32.77824075404466</v>
+      </c>
+      <c r="G13" s="132">
+        <v>45626</v>
+      </c>
+      <c r="H13" s="133">
+        <v>4198</v>
+      </c>
+      <c r="I13" s="134">
+        <v>4369</v>
+      </c>
+      <c r="J13" s="135">
+        <v>393714</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1559,7 +1618,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1918,15 +1977,33 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
+      <c r="A13" s="48">
+        <v>43994</v>
+      </c>
+      <c r="B13" s="49">
+        <v>0</v>
+      </c>
+      <c r="C13" s="49">
+        <v>1</v>
+      </c>
+      <c r="D13" s="49">
+        <v>1</v>
+      </c>
+      <c r="E13" s="49">
+        <v>1</v>
+      </c>
+      <c r="F13" s="49">
+        <v>0</v>
+      </c>
+      <c r="G13" s="49">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49">
+        <v>0</v>
+      </c>
+      <c r="I13" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
@@ -2026,7 +2103,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2488,7 +2565,42 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
+      <c r="A13" s="48">
+        <v>43994</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2500,7 +2612,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I30" sqref="I30:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2823,10 +2935,33 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="108"/>
+      <c r="A13" s="48">
+        <v>43994</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="108"/>
+      <c r="A14" s="48"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="108"/>
@@ -2894,8 +3029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2940,7 +3075,9 @@
       <c r="L1" s="50">
         <v>43993</v>
       </c>
-      <c r="M1" s="50"/>
+      <c r="M1" s="50">
+        <v>43994</v>
+      </c>
       <c r="N1" s="50"/>
       <c r="O1" s="50"/>
       <c r="P1" s="50"/>
@@ -2984,7 +3121,9 @@
       <c r="L2" s="49">
         <v>3369</v>
       </c>
-      <c r="M2" s="49"/>
+      <c r="M2" s="49">
+        <v>3401</v>
+      </c>
       <c r="N2" s="49"/>
       <c r="O2" s="49"/>
       <c r="P2" s="49"/>
@@ -3028,7 +3167,9 @@
       <c r="L3" s="49">
         <v>3184</v>
       </c>
-      <c r="M3" s="49"/>
+      <c r="M3" s="49">
+        <v>3216</v>
+      </c>
       <c r="N3" s="49"/>
       <c r="O3" s="49"/>
       <c r="P3" s="49"/>
@@ -3072,7 +3213,9 @@
       <c r="L4" s="49">
         <v>3184</v>
       </c>
-      <c r="M4" s="49"/>
+      <c r="M4" s="49">
+        <v>3216</v>
+      </c>
       <c r="N4" s="49"/>
       <c r="O4" s="49"/>
       <c r="P4" s="49"/>
@@ -3116,7 +3259,9 @@
       <c r="L5" s="49">
         <v>3184</v>
       </c>
-      <c r="M5" s="49"/>
+      <c r="M5" s="49">
+        <v>3216</v>
+      </c>
       <c r="N5" s="49"/>
       <c r="O5" s="49"/>
       <c r="P5" s="49"/>
@@ -3160,7 +3305,9 @@
       <c r="L6" s="49">
         <v>3184</v>
       </c>
-      <c r="M6" s="49"/>
+      <c r="M6" s="49">
+        <v>3216</v>
+      </c>
       <c r="N6" s="49"/>
       <c r="O6" s="49"/>
       <c r="P6" s="49"/>
@@ -3204,7 +3351,9 @@
       <c r="L7" s="49">
         <v>2481</v>
       </c>
-      <c r="M7" s="49"/>
+      <c r="M7" s="49">
+        <v>2513</v>
+      </c>
       <c r="N7" s="49"/>
       <c r="O7" s="49"/>
       <c r="P7" s="49"/>
@@ -3248,7 +3397,9 @@
       <c r="L8" s="49">
         <v>5006</v>
       </c>
-      <c r="M8" s="49"/>
+      <c r="M8" s="49">
+        <v>5038</v>
+      </c>
       <c r="N8" s="49"/>
       <c r="O8" s="49"/>
       <c r="P8" s="49"/>
@@ -3312,7 +3463,9 @@
       <c r="L10" s="49">
         <v>151</v>
       </c>
-      <c r="M10" s="49"/>
+      <c r="M10" s="49">
+        <v>152</v>
+      </c>
       <c r="N10" s="49"/>
       <c r="O10" s="49"/>
       <c r="P10" s="49"/>
@@ -3356,7 +3509,9 @@
       <c r="L11" s="49">
         <v>151</v>
       </c>
-      <c r="M11" s="49"/>
+      <c r="M11" s="49">
+        <v>152</v>
+      </c>
       <c r="N11" s="49"/>
       <c r="O11" s="49"/>
       <c r="P11" s="49"/>
@@ -3400,7 +3555,9 @@
       <c r="L12" s="49">
         <v>151</v>
       </c>
-      <c r="M12" s="49"/>
+      <c r="M12" s="49">
+        <v>152</v>
+      </c>
       <c r="N12" s="49"/>
       <c r="O12" s="49"/>
       <c r="P12" s="49"/>
@@ -3444,7 +3601,9 @@
       <c r="L13" s="49">
         <v>151</v>
       </c>
-      <c r="M13" s="49"/>
+      <c r="M13" s="49">
+        <v>152</v>
+      </c>
       <c r="N13" s="49"/>
       <c r="O13" s="49"/>
       <c r="P13" s="49"/>
@@ -3488,7 +3647,9 @@
       <c r="L14" s="49">
         <v>151</v>
       </c>
-      <c r="M14" s="49"/>
+      <c r="M14" s="49">
+        <v>152</v>
+      </c>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
       <c r="P14" s="49"/>
@@ -3532,7 +3693,9 @@
       <c r="L15" s="49">
         <v>128</v>
       </c>
-      <c r="M15" s="49"/>
+      <c r="M15" s="49">
+        <v>129</v>
+      </c>
       <c r="N15" s="49"/>
       <c r="O15" s="49"/>
       <c r="P15" s="49"/>
@@ -3576,7 +3739,9 @@
       <c r="L16" s="49">
         <v>163</v>
       </c>
-      <c r="M16" s="49"/>
+      <c r="M16" s="49">
+        <v>164</v>
+      </c>
       <c r="N16" s="49"/>
       <c r="O16" s="49"/>
       <c r="P16" s="49"/>
@@ -3640,7 +3805,9 @@
       <c r="L18" s="49">
         <v>813</v>
       </c>
-      <c r="M18" s="49"/>
+      <c r="M18" s="49">
+        <v>820</v>
+      </c>
       <c r="N18" s="49"/>
       <c r="O18" s="49"/>
       <c r="P18" s="49"/>
@@ -3663,7 +3830,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:L20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:M20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -3702,7 +3869,10 @@
         <f t="shared" si="0"/>
         <v>25451</v>
       </c>
-      <c r="M20" s="49"/>
+      <c r="M20" s="52">
+        <f t="shared" si="0"/>
+        <v>25689</v>
+      </c>
       <c r="N20" s="49"/>
       <c r="O20" s="49"/>
       <c r="P20" s="49"/>
@@ -3719,7 +3889,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Raw and clean Data from SSA for June 13th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D545DDE2-7A46-D743-ACA7-5E068CE8B087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67C6DE6-4469-7048-8510-3C049553B41C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="920" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="680" yWindow="1360" windowWidth="13140" windowHeight="15680" firstSheet="1" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +781,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1181,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1608,6 +1635,38 @@
         <v>393714</v>
       </c>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>43995</v>
+      </c>
+      <c r="B14" s="136">
+        <v>142690</v>
+      </c>
+      <c r="C14" s="137">
+        <v>202139</v>
+      </c>
+      <c r="D14" s="138">
+        <v>56926</v>
+      </c>
+      <c r="E14" s="139">
+        <v>16872</v>
+      </c>
+      <c r="F14" s="140">
+        <v>32.661714205620576</v>
+      </c>
+      <c r="G14" s="141">
+        <v>46605</v>
+      </c>
+      <c r="H14" s="142">
+        <v>4248</v>
+      </c>
+      <c r="I14" s="143">
+        <v>4426</v>
+      </c>
+      <c r="J14" s="144">
+        <v>401755</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1617,8 +1676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2006,15 +2065,33 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
+      <c r="A14" s="48">
+        <v>43995</v>
+      </c>
+      <c r="B14" s="49">
+        <v>0</v>
+      </c>
+      <c r="C14" s="49">
+        <v>1</v>
+      </c>
+      <c r="D14" s="49">
+        <v>1</v>
+      </c>
+      <c r="E14" s="49">
+        <v>1</v>
+      </c>
+      <c r="F14" s="49">
+        <v>0</v>
+      </c>
+      <c r="G14" s="49">
+        <v>0</v>
+      </c>
+      <c r="H14" s="49">
+        <v>0</v>
+      </c>
+      <c r="I14" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
@@ -2100,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2599,6 +2676,44 @@
         <v>0</v>
       </c>
       <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="48">
+        <v>43995</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>0</v>
       </c>
     </row>
@@ -2611,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:I31"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2961,7 +3076,30 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="48"/>
+      <c r="A14" s="48">
+        <v>43995</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="108"/>
@@ -3029,8 +3167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3078,7 +3216,9 @@
       <c r="M1" s="50">
         <v>43994</v>
       </c>
-      <c r="N1" s="50"/>
+      <c r="N1" s="50">
+        <v>43995</v>
+      </c>
       <c r="O1" s="50"/>
       <c r="P1" s="50"/>
       <c r="Q1" s="50"/>
@@ -3124,7 +3264,9 @@
       <c r="M2" s="49">
         <v>3401</v>
       </c>
-      <c r="N2" s="49"/>
+      <c r="N2" s="49">
+        <v>3433</v>
+      </c>
       <c r="O2" s="49"/>
       <c r="P2" s="49"/>
       <c r="Q2" s="49"/>
@@ -3170,7 +3312,9 @@
       <c r="M3" s="49">
         <v>3216</v>
       </c>
-      <c r="N3" s="49"/>
+      <c r="N3" s="49">
+        <v>3248</v>
+      </c>
       <c r="O3" s="49"/>
       <c r="P3" s="49"/>
       <c r="Q3" s="49"/>
@@ -3216,7 +3360,9 @@
       <c r="M4" s="49">
         <v>3216</v>
       </c>
-      <c r="N4" s="49"/>
+      <c r="N4" s="49">
+        <v>3248</v>
+      </c>
       <c r="O4" s="49"/>
       <c r="P4" s="49"/>
       <c r="Q4" s="49"/>
@@ -3262,7 +3408,9 @@
       <c r="M5" s="49">
         <v>3216</v>
       </c>
-      <c r="N5" s="49"/>
+      <c r="N5" s="49">
+        <v>3248</v>
+      </c>
       <c r="O5" s="49"/>
       <c r="P5" s="49"/>
       <c r="Q5" s="49"/>
@@ -3308,7 +3456,9 @@
       <c r="M6" s="49">
         <v>3216</v>
       </c>
-      <c r="N6" s="49"/>
+      <c r="N6" s="49">
+        <v>3248</v>
+      </c>
       <c r="O6" s="49"/>
       <c r="P6" s="49"/>
       <c r="Q6" s="49"/>
@@ -3354,7 +3504,9 @@
       <c r="M7" s="49">
         <v>2513</v>
       </c>
-      <c r="N7" s="49"/>
+      <c r="N7" s="49">
+        <v>2461</v>
+      </c>
       <c r="O7" s="49"/>
       <c r="P7" s="49"/>
       <c r="Q7" s="49"/>
@@ -3400,7 +3552,9 @@
       <c r="M8" s="49">
         <v>5038</v>
       </c>
-      <c r="N8" s="49"/>
+      <c r="N8" s="49">
+        <v>5070</v>
+      </c>
       <c r="O8" s="49"/>
       <c r="P8" s="49"/>
       <c r="Q8" s="49"/>
@@ -3466,7 +3620,9 @@
       <c r="M10" s="49">
         <v>152</v>
       </c>
-      <c r="N10" s="49"/>
+      <c r="N10" s="49">
+        <v>153</v>
+      </c>
       <c r="O10" s="49"/>
       <c r="P10" s="49"/>
       <c r="Q10" s="49"/>
@@ -3512,7 +3668,9 @@
       <c r="M11" s="49">
         <v>152</v>
       </c>
-      <c r="N11" s="49"/>
+      <c r="N11" s="49">
+        <v>153</v>
+      </c>
       <c r="O11" s="49"/>
       <c r="P11" s="49"/>
       <c r="Q11" s="49"/>
@@ -3558,7 +3716,9 @@
       <c r="M12" s="49">
         <v>152</v>
       </c>
-      <c r="N12" s="49"/>
+      <c r="N12" s="49">
+        <v>153</v>
+      </c>
       <c r="O12" s="49"/>
       <c r="P12" s="49"/>
       <c r="Q12" s="49"/>
@@ -3604,7 +3764,9 @@
       <c r="M13" s="49">
         <v>152</v>
       </c>
-      <c r="N13" s="49"/>
+      <c r="N13" s="49">
+        <v>153</v>
+      </c>
       <c r="O13" s="49"/>
       <c r="P13" s="49"/>
       <c r="Q13" s="49"/>
@@ -3650,7 +3812,9 @@
       <c r="M14" s="49">
         <v>152</v>
       </c>
-      <c r="N14" s="49"/>
+      <c r="N14" s="49">
+        <v>153</v>
+      </c>
       <c r="O14" s="49"/>
       <c r="P14" s="49"/>
       <c r="Q14" s="49"/>
@@ -3696,7 +3860,9 @@
       <c r="M15" s="49">
         <v>129</v>
       </c>
-      <c r="N15" s="49"/>
+      <c r="N15" s="49">
+        <v>100</v>
+      </c>
       <c r="O15" s="49"/>
       <c r="P15" s="49"/>
       <c r="Q15" s="49"/>
@@ -3742,7 +3908,9 @@
       <c r="M16" s="49">
         <v>164</v>
       </c>
-      <c r="N16" s="49"/>
+      <c r="N16" s="49">
+        <v>165</v>
+      </c>
       <c r="O16" s="49"/>
       <c r="P16" s="49"/>
       <c r="Q16" s="49"/>
@@ -3808,7 +3976,9 @@
       <c r="M18" s="49">
         <v>820</v>
       </c>
-      <c r="N18" s="49"/>
+      <c r="N18" s="49">
+        <v>800</v>
+      </c>
       <c r="O18" s="49"/>
       <c r="P18" s="49"/>
       <c r="Q18" s="49"/>
@@ -3830,7 +4000,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:M20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:N20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -3873,7 +4043,10 @@
         <f t="shared" si="0"/>
         <v>25689</v>
       </c>
-      <c r="N20" s="49"/>
+      <c r="N20" s="52">
+        <f t="shared" si="0"/>
+        <v>25786</v>
+      </c>
       <c r="O20" s="49"/>
       <c r="P20" s="49"/>
       <c r="Q20" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 14th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67C6DE6-4469-7048-8510-3C049553B41C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4E2E35-1666-4740-B1E5-B73ADF4076DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1360" windowWidth="13140" windowHeight="15680" firstSheet="1" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="680" yWindow="1360" windowWidth="22000" windowHeight="15680" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +781,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1208,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1667,6 +1694,38 @@
         <v>401755</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>43996</v>
+      </c>
+      <c r="B15" s="145">
+        <v>146837</v>
+      </c>
+      <c r="C15" s="146">
+        <v>207076</v>
+      </c>
+      <c r="D15" s="147">
+        <v>52636</v>
+      </c>
+      <c r="E15" s="148">
+        <v>17141</v>
+      </c>
+      <c r="F15" s="149">
+        <v>32.503388110626069</v>
+      </c>
+      <c r="G15" s="150">
+        <v>47727</v>
+      </c>
+      <c r="H15" s="151">
+        <v>4323</v>
+      </c>
+      <c r="I15" s="152">
+        <v>4483</v>
+      </c>
+      <c r="J15" s="153">
+        <v>406549</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1676,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2094,15 +2153,33 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="A15" s="48">
+        <v>43996</v>
+      </c>
+      <c r="B15" s="49">
+        <v>0</v>
+      </c>
+      <c r="C15" s="49">
+        <v>1</v>
+      </c>
+      <c r="D15" s="49">
+        <v>1</v>
+      </c>
+      <c r="E15" s="49">
+        <v>1</v>
+      </c>
+      <c r="F15" s="49">
+        <v>0</v>
+      </c>
+      <c r="G15" s="49">
+        <v>0</v>
+      </c>
+      <c r="H15" s="49">
+        <v>0</v>
+      </c>
+      <c r="I15" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="48"/>
@@ -2177,10 +2254,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2714,6 +2791,44 @@
         <v>0</v>
       </c>
       <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="48">
+        <v>43996</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>0</v>
       </c>
     </row>
@@ -2726,8 +2841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,7 +3217,30 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="108"/>
+      <c r="A15" s="48">
+        <v>43996</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="108"/>
@@ -3167,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3219,7 +3357,9 @@
       <c r="N1" s="50">
         <v>43995</v>
       </c>
-      <c r="O1" s="50"/>
+      <c r="O1" s="50">
+        <v>43996</v>
+      </c>
       <c r="P1" s="50"/>
       <c r="Q1" s="50"/>
       <c r="R1" s="50"/>
@@ -3267,7 +3407,9 @@
       <c r="N2" s="49">
         <v>3433</v>
       </c>
-      <c r="O2" s="49"/>
+      <c r="O2" s="49">
+        <v>3465</v>
+      </c>
       <c r="P2" s="49"/>
       <c r="Q2" s="49"/>
       <c r="R2" s="49"/>
@@ -3315,7 +3457,9 @@
       <c r="N3" s="49">
         <v>3248</v>
       </c>
-      <c r="O3" s="49"/>
+      <c r="O3" s="49">
+        <v>3280</v>
+      </c>
       <c r="P3" s="49"/>
       <c r="Q3" s="49"/>
       <c r="R3" s="49"/>
@@ -3363,7 +3507,9 @@
       <c r="N4" s="49">
         <v>3248</v>
       </c>
-      <c r="O4" s="49"/>
+      <c r="O4" s="49">
+        <v>3280</v>
+      </c>
       <c r="P4" s="49"/>
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
@@ -3411,7 +3557,9 @@
       <c r="N5" s="49">
         <v>3248</v>
       </c>
-      <c r="O5" s="49"/>
+      <c r="O5" s="49">
+        <v>3280</v>
+      </c>
       <c r="P5" s="49"/>
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
@@ -3459,7 +3607,9 @@
       <c r="N6" s="49">
         <v>3248</v>
       </c>
-      <c r="O6" s="49"/>
+      <c r="O6" s="49">
+        <v>3280</v>
+      </c>
       <c r="P6" s="49"/>
       <c r="Q6" s="49"/>
       <c r="R6" s="49"/>
@@ -3507,7 +3657,9 @@
       <c r="N7" s="49">
         <v>2461</v>
       </c>
-      <c r="O7" s="49"/>
+      <c r="O7" s="49">
+        <v>2493</v>
+      </c>
       <c r="P7" s="49"/>
       <c r="Q7" s="49"/>
       <c r="R7" s="49"/>
@@ -3555,7 +3707,9 @@
       <c r="N8" s="49">
         <v>5070</v>
       </c>
-      <c r="O8" s="49"/>
+      <c r="O8" s="49">
+        <v>5102</v>
+      </c>
       <c r="P8" s="49"/>
       <c r="Q8" s="49"/>
       <c r="R8" s="49"/>
@@ -3623,7 +3777,9 @@
       <c r="N10" s="49">
         <v>153</v>
       </c>
-      <c r="O10" s="49"/>
+      <c r="O10" s="49">
+        <v>154</v>
+      </c>
       <c r="P10" s="49"/>
       <c r="Q10" s="49"/>
       <c r="R10" s="49"/>
@@ -3671,7 +3827,9 @@
       <c r="N11" s="49">
         <v>153</v>
       </c>
-      <c r="O11" s="49"/>
+      <c r="O11" s="49">
+        <v>154</v>
+      </c>
       <c r="P11" s="49"/>
       <c r="Q11" s="49"/>
       <c r="R11" s="49"/>
@@ -3719,7 +3877,9 @@
       <c r="N12" s="49">
         <v>153</v>
       </c>
-      <c r="O12" s="49"/>
+      <c r="O12" s="49">
+        <v>154</v>
+      </c>
       <c r="P12" s="49"/>
       <c r="Q12" s="49"/>
       <c r="R12" s="49"/>
@@ -3767,7 +3927,9 @@
       <c r="N13" s="49">
         <v>153</v>
       </c>
-      <c r="O13" s="49"/>
+      <c r="O13" s="49">
+        <v>154</v>
+      </c>
       <c r="P13" s="49"/>
       <c r="Q13" s="49"/>
       <c r="R13" s="49"/>
@@ -3815,7 +3977,9 @@
       <c r="N14" s="49">
         <v>153</v>
       </c>
-      <c r="O14" s="49"/>
+      <c r="O14" s="49">
+        <v>154</v>
+      </c>
       <c r="P14" s="49"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="49"/>
@@ -3863,7 +4027,9 @@
       <c r="N15" s="49">
         <v>100</v>
       </c>
-      <c r="O15" s="49"/>
+      <c r="O15" s="49">
+        <v>101</v>
+      </c>
       <c r="P15" s="49"/>
       <c r="Q15" s="49"/>
       <c r="R15" s="49"/>
@@ -3911,7 +4077,9 @@
       <c r="N16" s="49">
         <v>165</v>
       </c>
-      <c r="O16" s="49"/>
+      <c r="O16" s="49">
+        <v>166</v>
+      </c>
       <c r="P16" s="49"/>
       <c r="Q16" s="49"/>
       <c r="R16" s="49"/>
@@ -3979,7 +4147,9 @@
       <c r="N18" s="49">
         <v>800</v>
       </c>
-      <c r="O18" s="49"/>
+      <c r="O18" s="49">
+        <v>807</v>
+      </c>
       <c r="P18" s="49"/>
       <c r="Q18" s="49"/>
       <c r="R18" s="49"/>
@@ -4000,7 +4170,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:N20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:O20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -4047,7 +4217,10 @@
         <f t="shared" si="0"/>
         <v>25786</v>
       </c>
-      <c r="O20" s="49"/>
+      <c r="O20" s="52">
+        <f t="shared" si="0"/>
+        <v>26024</v>
+      </c>
       <c r="P20" s="49"/>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 15th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4E2E35-1666-4740-B1E5-B73ADF4076DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47FE5CC-F202-4C4E-8E88-5EBDAE7086E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1360" windowWidth="22000" windowHeight="15680" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="7800" yWindow="780" windowWidth="22000" windowHeight="15680" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>2020-06-06</t>
+  </si>
+  <si>
+    <t>13 de enero</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,6 +784,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1235,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1726,6 +1756,38 @@
         <v>406549</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>43997</v>
+      </c>
+      <c r="B16" s="154">
+        <v>150264</v>
+      </c>
+      <c r="C16" s="155">
+        <v>211616</v>
+      </c>
+      <c r="D16" s="156">
+        <v>53217</v>
+      </c>
+      <c r="E16" s="157">
+        <v>17580</v>
+      </c>
+      <c r="F16" s="158">
+        <v>32.357051589203003</v>
+      </c>
+      <c r="G16" s="159">
+        <v>48621</v>
+      </c>
+      <c r="H16" s="160">
+        <v>4387</v>
+      </c>
+      <c r="I16" s="161">
+        <v>4555</v>
+      </c>
+      <c r="J16" s="162">
+        <v>415097</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1733,20 +1795,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1754,37 +1817,38 @@
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="48">
         <v>43983</v>
       </c>
       <c r="B2" s="49">
         <v>0</v>
       </c>
-      <c r="C2" s="49">
-        <v>1</v>
-      </c>
+      <c r="C2" s="49"/>
       <c r="D2" s="49">
         <v>1</v>
       </c>
@@ -1792,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="49">
         <v>0</v>
@@ -1801,19 +1865,20 @@
         <v>0</v>
       </c>
       <c r="I2" s="49">
+        <v>0</v>
+      </c>
+      <c r="J2" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="48">
         <v>43984</v>
       </c>
       <c r="B3" s="49">
         <v>0</v>
       </c>
-      <c r="C3" s="49">
-        <v>1</v>
-      </c>
+      <c r="C3" s="49"/>
       <c r="D3" s="49">
         <v>1</v>
       </c>
@@ -1821,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="49">
         <v>0</v>
@@ -1830,19 +1895,20 @@
         <v>0</v>
       </c>
       <c r="I3" s="49">
+        <v>0</v>
+      </c>
+      <c r="J3" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="48">
         <v>43985</v>
       </c>
       <c r="B4" s="49">
         <v>0</v>
       </c>
-      <c r="C4" s="49">
-        <v>1</v>
-      </c>
+      <c r="C4" s="49"/>
       <c r="D4" s="49">
         <v>1</v>
       </c>
@@ -1850,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="49">
         <v>0</v>
@@ -1859,19 +1925,20 @@
         <v>0</v>
       </c>
       <c r="I4" s="49">
+        <v>0</v>
+      </c>
+      <c r="J4" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="48">
         <v>43986</v>
       </c>
       <c r="B5" s="49">
         <v>0</v>
       </c>
-      <c r="C5" s="49">
-        <v>1</v>
-      </c>
+      <c r="C5" s="49"/>
       <c r="D5" s="49">
         <v>1</v>
       </c>
@@ -1879,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="49">
         <v>0</v>
@@ -1888,19 +1955,20 @@
         <v>0</v>
       </c>
       <c r="I5" s="49">
+        <v>0</v>
+      </c>
+      <c r="J5" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="48">
         <v>43987</v>
       </c>
       <c r="B6" s="49">
         <v>0</v>
       </c>
-      <c r="C6" s="49">
-        <v>1</v>
-      </c>
+      <c r="C6" s="49"/>
       <c r="D6" s="49">
         <v>1</v>
       </c>
@@ -1908,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="49">
         <v>0</v>
@@ -1917,19 +1985,20 @@
         <v>0</v>
       </c>
       <c r="I6" s="49">
+        <v>0</v>
+      </c>
+      <c r="J6" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="48">
         <v>43988</v>
       </c>
       <c r="B7" s="49">
         <v>0</v>
       </c>
-      <c r="C7" s="49">
-        <v>1</v>
-      </c>
+      <c r="C7" s="49"/>
       <c r="D7" s="49">
         <v>1</v>
       </c>
@@ -1937,7 +2006,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="49">
         <v>0</v>
@@ -1946,19 +2015,20 @@
         <v>0</v>
       </c>
       <c r="I7" s="49">
+        <v>0</v>
+      </c>
+      <c r="J7" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="48">
         <v>43989</v>
       </c>
       <c r="B8" s="49">
         <v>0</v>
       </c>
-      <c r="C8" s="49">
-        <v>1</v>
-      </c>
+      <c r="C8" s="49"/>
       <c r="D8" s="49">
         <v>1</v>
       </c>
@@ -1966,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="49">
         <v>0</v>
@@ -1975,19 +2045,20 @@
         <v>0</v>
       </c>
       <c r="I8" s="49">
+        <v>0</v>
+      </c>
+      <c r="J8" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="48">
         <v>43990</v>
       </c>
       <c r="B9" s="49">
         <v>0</v>
       </c>
-      <c r="C9" s="49">
-        <v>1</v>
-      </c>
+      <c r="C9" s="49"/>
       <c r="D9" s="49">
         <v>1</v>
       </c>
@@ -1995,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="49">
         <v>0</v>
@@ -2004,19 +2075,20 @@
         <v>0</v>
       </c>
       <c r="I9" s="49">
+        <v>0</v>
+      </c>
+      <c r="J9" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="48">
         <v>43991</v>
       </c>
       <c r="B10" s="49">
         <v>0</v>
       </c>
-      <c r="C10" s="49">
-        <v>1</v>
-      </c>
+      <c r="C10" s="49"/>
       <c r="D10" s="49">
         <v>1</v>
       </c>
@@ -2024,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="49">
         <v>0</v>
@@ -2033,19 +2105,20 @@
         <v>0</v>
       </c>
       <c r="I10" s="49">
+        <v>0</v>
+      </c>
+      <c r="J10" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="48">
         <v>43992</v>
       </c>
       <c r="B11" s="49">
         <v>0</v>
       </c>
-      <c r="C11" s="49">
-        <v>1</v>
-      </c>
+      <c r="C11" s="49"/>
       <c r="D11" s="49">
         <v>1</v>
       </c>
@@ -2053,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="49">
         <v>0</v>
@@ -2062,19 +2135,20 @@
         <v>0</v>
       </c>
       <c r="I11" s="49">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="48">
         <v>43993</v>
       </c>
       <c r="B12" s="49">
         <v>0</v>
       </c>
-      <c r="C12" s="49">
-        <v>1</v>
-      </c>
+      <c r="C12" s="49"/>
       <c r="D12" s="49">
         <v>1</v>
       </c>
@@ -2082,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="49">
         <v>0</v>
@@ -2091,19 +2165,20 @@
         <v>0</v>
       </c>
       <c r="I12" s="49">
+        <v>0</v>
+      </c>
+      <c r="J12" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="48">
         <v>43994</v>
       </c>
       <c r="B13" s="49">
         <v>0</v>
       </c>
-      <c r="C13" s="49">
-        <v>1</v>
-      </c>
+      <c r="C13" s="49"/>
       <c r="D13" s="49">
         <v>1</v>
       </c>
@@ -2111,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="49">
         <v>0</v>
@@ -2120,19 +2195,20 @@
         <v>0</v>
       </c>
       <c r="I13" s="49">
+        <v>0</v>
+      </c>
+      <c r="J13" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="48">
         <v>43995</v>
       </c>
       <c r="B14" s="49">
         <v>0</v>
       </c>
-      <c r="C14" s="49">
-        <v>1</v>
-      </c>
+      <c r="C14" s="49"/>
       <c r="D14" s="49">
         <v>1</v>
       </c>
@@ -2140,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="49">
         <v>0</v>
@@ -2149,19 +2225,20 @@
         <v>0</v>
       </c>
       <c r="I14" s="49">
+        <v>0</v>
+      </c>
+      <c r="J14" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="48">
         <v>43996</v>
       </c>
       <c r="B15" s="49">
         <v>0</v>
       </c>
-      <c r="C15" s="49">
-        <v>1</v>
-      </c>
+      <c r="C15" s="49"/>
       <c r="D15" s="49">
         <v>1</v>
       </c>
@@ -2169,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="49">
         <v>0</v>
@@ -2178,21 +2255,45 @@
         <v>0</v>
       </c>
       <c r="I15" s="49">
+        <v>0</v>
+      </c>
+      <c r="J15" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="48">
+        <v>43997</v>
+      </c>
+      <c r="B16" s="49">
+        <v>0</v>
+      </c>
+      <c r="C16" s="49">
+        <v>1</v>
+      </c>
+      <c r="D16" s="49">
+        <v>1</v>
+      </c>
+      <c r="E16" s="49">
+        <v>1</v>
+      </c>
+      <c r="F16" s="49">
+        <v>1</v>
+      </c>
+      <c r="G16" s="49">
+        <v>0</v>
+      </c>
+      <c r="H16" s="49">
+        <v>0</v>
+      </c>
+      <c r="I16" s="49">
+        <v>0</v>
+      </c>
+      <c r="J16" s="49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -2202,8 +2303,9 @@
       <c r="G17" s="49"/>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="49"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -2213,8 +2315,9 @@
       <c r="G18" s="49"/>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="49"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
@@ -2224,8 +2327,9 @@
       <c r="G19" s="49"/>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="49"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -2235,8 +2339,9 @@
       <c r="G20" s="49"/>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -2246,6 +2351,7 @@
       <c r="G21" s="49"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2254,15 +2360,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -2270,51 +2376,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="48">
         <v>43983</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -2323,36 +2429,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="48">
         <v>43984</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2361,36 +2467,36 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="48">
         <v>43985</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2399,36 +2505,36 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="48">
         <v>43986</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2437,36 +2543,36 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="48">
         <v>43987</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2475,36 +2581,36 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="s">
         <v>67</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -2513,36 +2619,36 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="48">
         <v>43989</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2551,36 +2657,36 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="48">
         <v>43990</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -2589,36 +2695,36 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="48">
         <v>43991</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2627,36 +2733,36 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="48">
         <v>43992</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2665,36 +2771,36 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="48">
         <v>43993</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -2703,36 +2809,36 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="48">
         <v>43994</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2741,36 +2847,36 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="48">
         <v>43995</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2779,36 +2885,36 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="48">
         <v>43996</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2817,18 +2923,62 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="48">
+        <v>43997</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>0</v>
       </c>
     </row>
@@ -2842,7 +2992,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3243,10 +3393,33 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="108"/>
+      <c r="A16" s="48">
+        <v>43997</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="108"/>
+      <c r="A17" s="48"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="108"/>
@@ -3305,8 +3478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3360,7 +3533,9 @@
       <c r="O1" s="50">
         <v>43996</v>
       </c>
-      <c r="P1" s="50"/>
+      <c r="P1" s="15">
+        <v>43997</v>
+      </c>
       <c r="Q1" s="50"/>
       <c r="R1" s="50"/>
     </row>
@@ -3410,7 +3585,9 @@
       <c r="O2" s="49">
         <v>3465</v>
       </c>
-      <c r="P2" s="49"/>
+      <c r="P2" s="49">
+        <v>3497</v>
+      </c>
       <c r="Q2" s="49"/>
       <c r="R2" s="49"/>
     </row>
@@ -3460,7 +3637,9 @@
       <c r="O3" s="49">
         <v>3280</v>
       </c>
-      <c r="P3" s="49"/>
+      <c r="P3" s="49">
+        <v>3312</v>
+      </c>
       <c r="Q3" s="49"/>
       <c r="R3" s="49"/>
     </row>
@@ -3510,7 +3689,9 @@
       <c r="O4" s="49">
         <v>3280</v>
       </c>
-      <c r="P4" s="49"/>
+      <c r="P4" s="49">
+        <v>3312</v>
+      </c>
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
     </row>
@@ -3560,7 +3741,9 @@
       <c r="O5" s="49">
         <v>3280</v>
       </c>
-      <c r="P5" s="49"/>
+      <c r="P5" s="49">
+        <v>3312</v>
+      </c>
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
     </row>
@@ -3610,7 +3793,9 @@
       <c r="O6" s="49">
         <v>3280</v>
       </c>
-      <c r="P6" s="49"/>
+      <c r="P6" s="49">
+        <v>3312</v>
+      </c>
       <c r="Q6" s="49"/>
       <c r="R6" s="49"/>
     </row>
@@ -3660,7 +3845,9 @@
       <c r="O7" s="49">
         <v>2493</v>
       </c>
-      <c r="P7" s="49"/>
+      <c r="P7" s="49">
+        <v>2503</v>
+      </c>
       <c r="Q7" s="49"/>
       <c r="R7" s="49"/>
     </row>
@@ -3710,7 +3897,9 @@
       <c r="O8" s="49">
         <v>5102</v>
       </c>
-      <c r="P8" s="49"/>
+      <c r="P8" s="49">
+        <v>5134</v>
+      </c>
       <c r="Q8" s="49"/>
       <c r="R8" s="49"/>
     </row>
@@ -3780,7 +3969,9 @@
       <c r="O10" s="49">
         <v>154</v>
       </c>
-      <c r="P10" s="49"/>
+      <c r="P10" s="49">
+        <v>155</v>
+      </c>
       <c r="Q10" s="49"/>
       <c r="R10" s="49"/>
     </row>
@@ -3830,7 +4021,9 @@
       <c r="O11" s="49">
         <v>154</v>
       </c>
-      <c r="P11" s="49"/>
+      <c r="P11" s="49">
+        <v>155</v>
+      </c>
       <c r="Q11" s="49"/>
       <c r="R11" s="49"/>
     </row>
@@ -3880,7 +4073,9 @@
       <c r="O12" s="49">
         <v>154</v>
       </c>
-      <c r="P12" s="49"/>
+      <c r="P12" s="49">
+        <v>155</v>
+      </c>
       <c r="Q12" s="49"/>
       <c r="R12" s="49"/>
     </row>
@@ -3930,7 +4125,9 @@
       <c r="O13" s="49">
         <v>154</v>
       </c>
-      <c r="P13" s="49"/>
+      <c r="P13" s="49">
+        <v>155</v>
+      </c>
       <c r="Q13" s="49"/>
       <c r="R13" s="49"/>
     </row>
@@ -3980,7 +4177,9 @@
       <c r="O14" s="49">
         <v>154</v>
       </c>
-      <c r="P14" s="49"/>
+      <c r="P14" s="49">
+        <v>155</v>
+      </c>
       <c r="Q14" s="49"/>
       <c r="R14" s="49"/>
     </row>
@@ -4030,7 +4229,9 @@
       <c r="O15" s="49">
         <v>101</v>
       </c>
-      <c r="P15" s="49"/>
+      <c r="P15" s="49">
+        <v>90</v>
+      </c>
       <c r="Q15" s="49"/>
       <c r="R15" s="49"/>
     </row>
@@ -4080,7 +4281,9 @@
       <c r="O16" s="49">
         <v>166</v>
       </c>
-      <c r="P16" s="49"/>
+      <c r="P16" s="49">
+        <v>167</v>
+      </c>
       <c r="Q16" s="49"/>
       <c r="R16" s="49"/>
     </row>
@@ -4150,7 +4353,9 @@
       <c r="O18" s="49">
         <v>807</v>
       </c>
-      <c r="P18" s="49"/>
+      <c r="P18" s="49">
+        <v>814</v>
+      </c>
       <c r="Q18" s="49"/>
       <c r="R18" s="49"/>
     </row>
@@ -4170,7 +4375,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:O20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:P20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -4221,7 +4426,10 @@
         <f t="shared" si="0"/>
         <v>26024</v>
       </c>
-      <c r="P20" s="49"/>
+      <c r="P20" s="52">
+        <f t="shared" si="0"/>
+        <v>26228</v>
+      </c>
       <c r="Q20" s="49"/>
       <c r="R20" s="49"/>
     </row>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 16th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210FDFE-12BC-E941-8198-35AEFE072C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB27419-2696-964E-827F-8C3BB0C1E3C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="1260" windowWidth="20100" windowHeight="14620" activeTab="3" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="3840" yWindow="1280" windowWidth="20100" windowHeight="14620" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -423,7 +423,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,7 +509,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -961,8 +961,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1805,6 +1832,38 @@
         <v>415097</v>
       </c>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>43998</v>
+      </c>
+      <c r="B17" s="164">
+        <v>154863</v>
+      </c>
+      <c r="C17" s="165">
+        <v>216857</v>
+      </c>
+      <c r="D17" s="166">
+        <v>56843</v>
+      </c>
+      <c r="E17" s="167">
+        <v>18310</v>
+      </c>
+      <c r="F17" s="168">
+        <v>32.287247438058152</v>
+      </c>
+      <c r="G17" s="169">
+        <v>50001</v>
+      </c>
+      <c r="H17" s="170">
+        <v>4540</v>
+      </c>
+      <c r="I17" s="171">
+        <v>4700</v>
+      </c>
+      <c r="J17" s="172">
+        <v>428563</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1815,7 +1874,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2387,17 +2446,39 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
+      <c r="A17" s="48">
+        <v>43998</v>
+      </c>
+      <c r="B17" s="49">
+        <v>0</v>
+      </c>
+      <c r="C17" s="49">
+        <v>1</v>
+      </c>
+      <c r="D17" s="49">
+        <v>1</v>
+      </c>
+      <c r="E17" s="49">
+        <v>1</v>
+      </c>
+      <c r="F17" s="49">
+        <v>1</v>
+      </c>
+      <c r="G17" s="49">
+        <v>0</v>
+      </c>
+      <c r="H17" s="49">
+        <v>0</v>
+      </c>
+      <c r="I17" s="49">
+        <v>1</v>
+      </c>
+      <c r="J17" s="49">
+        <v>0</v>
+      </c>
+      <c r="K17" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
@@ -2458,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3116,6 +3197,47 @@
         <v>0</v>
       </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="48">
+        <v>43998</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>0</v>
       </c>
     </row>
@@ -3128,8 +3250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3334,9 +3456,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
-        <v>67</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="48">
+        <v>43988</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3530,7 +3652,7 @@
       <c r="A13" s="48">
         <v>43994</v>
       </c>
-      <c r="B13" s="164">
+      <c r="B13" s="163">
         <v>1</v>
       </c>
       <c r="C13">
@@ -3654,52 +3776,81 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="48">
+        <v>43998</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="108"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="108"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="108"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="108"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="108"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="108"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="108"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="108"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="108"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="108"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="108"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="108"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="108"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="108"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="108"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -3714,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3772,7 +3923,9 @@
       <c r="P1" s="50">
         <v>43997</v>
       </c>
-      <c r="Q1" s="50"/>
+      <c r="Q1" s="50">
+        <v>43998</v>
+      </c>
       <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -3824,7 +3977,9 @@
       <c r="P2" s="49">
         <v>3497</v>
       </c>
-      <c r="Q2" s="49"/>
+      <c r="Q2" s="49">
+        <v>3529</v>
+      </c>
       <c r="R2" s="49"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -3876,7 +4031,9 @@
       <c r="P3" s="49">
         <v>3312</v>
       </c>
-      <c r="Q3" s="49"/>
+      <c r="Q3" s="49">
+        <v>3344</v>
+      </c>
       <c r="R3" s="49"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -3928,7 +4085,9 @@
       <c r="P4" s="49">
         <v>3312</v>
       </c>
-      <c r="Q4" s="49"/>
+      <c r="Q4" s="49">
+        <v>3344</v>
+      </c>
       <c r="R4" s="49"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -3980,7 +4139,9 @@
       <c r="P5" s="49">
         <v>3312</v>
       </c>
-      <c r="Q5" s="49"/>
+      <c r="Q5" s="49">
+        <v>3344</v>
+      </c>
       <c r="R5" s="49"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -4032,7 +4193,9 @@
       <c r="P6" s="49">
         <v>3312</v>
       </c>
-      <c r="Q6" s="49"/>
+      <c r="Q6" s="49">
+        <v>3344</v>
+      </c>
       <c r="R6" s="49"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -4084,7 +4247,9 @@
       <c r="P7" s="49">
         <v>2503</v>
       </c>
-      <c r="Q7" s="49"/>
+      <c r="Q7" s="49">
+        <v>2535</v>
+      </c>
       <c r="R7" s="49"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -4136,7 +4301,9 @@
       <c r="P8" s="49">
         <v>5134</v>
       </c>
-      <c r="Q8" s="49"/>
+      <c r="Q8" s="49">
+        <v>5166</v>
+      </c>
       <c r="R8" s="49"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -4208,7 +4375,9 @@
       <c r="P10" s="49">
         <v>155</v>
       </c>
-      <c r="Q10" s="49"/>
+      <c r="Q10" s="49">
+        <v>156</v>
+      </c>
       <c r="R10" s="49"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -4260,7 +4429,9 @@
       <c r="P11" s="49">
         <v>155</v>
       </c>
-      <c r="Q11" s="49"/>
+      <c r="Q11" s="49">
+        <v>156</v>
+      </c>
       <c r="R11" s="49"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -4312,7 +4483,9 @@
       <c r="P12" s="49">
         <v>155</v>
       </c>
-      <c r="Q12" s="49"/>
+      <c r="Q12" s="49">
+        <v>156</v>
+      </c>
       <c r="R12" s="49"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -4364,7 +4537,9 @@
       <c r="P13" s="49">
         <v>155</v>
       </c>
-      <c r="Q13" s="49"/>
+      <c r="Q13" s="49">
+        <v>156</v>
+      </c>
       <c r="R13" s="49"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -4416,7 +4591,9 @@
       <c r="P14" s="49">
         <v>155</v>
       </c>
-      <c r="Q14" s="49"/>
+      <c r="Q14" s="49">
+        <v>156</v>
+      </c>
       <c r="R14" s="49"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -4456,19 +4633,21 @@
       <c r="L15" s="49">
         <v>128</v>
       </c>
-      <c r="M15" s="163">
+      <c r="M15" s="173">
         <v>129</v>
       </c>
       <c r="N15" s="49">
         <v>100</v>
       </c>
-      <c r="O15" s="49">
+      <c r="O15" s="173">
         <v>101</v>
       </c>
-      <c r="P15" s="49">
+      <c r="P15" s="173">
         <v>90</v>
       </c>
-      <c r="Q15" s="49"/>
+      <c r="Q15" s="49">
+        <v>91</v>
+      </c>
       <c r="R15" s="49"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -4520,7 +4699,9 @@
       <c r="P16" s="49">
         <v>167</v>
       </c>
-      <c r="Q16" s="49"/>
+      <c r="Q16" s="49">
+        <v>168</v>
+      </c>
       <c r="R16" s="49"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -4592,7 +4773,9 @@
       <c r="P18" s="49">
         <v>814</v>
       </c>
-      <c r="Q18" s="49"/>
+      <c r="Q18" s="49">
+        <v>821</v>
+      </c>
       <c r="R18" s="49"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -4611,7 +4794,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:P20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:Q20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -4666,7 +4849,10 @@
         <f t="shared" si="0"/>
         <v>26228</v>
       </c>
-      <c r="Q20" s="49"/>
+      <c r="Q20" s="52">
+        <f t="shared" si="0"/>
+        <v>26466</v>
+      </c>
       <c r="R20" s="49"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 17th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB27419-2696-964E-827F-8C3BB0C1E3C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4F2914-82CE-FD40-9584-C801A5D4A865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1280" windowWidth="20100" windowHeight="14620" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2100" yWindow="1120" windowWidth="22840" windowHeight="15400" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -255,6 +255,15 @@
   </si>
   <si>
     <t>5 de febrero</t>
+  </si>
+  <si>
+    <t>17 de junio</t>
+  </si>
+  <si>
+    <t>En serie de defunciones el día 12 de junio de 2020 la serie comenzó el 5 de febrero de 2020, para el 13 de junio la serie comenzó el 6 de marzo por lo cual hay una diferencia de 29 días, es decir 29 observaciones</t>
+  </si>
+  <si>
+    <t>En serie de defunciones el día 14 de junio, la serie comenzó el 6 de marzo, el día 15 de junio comenzó el 18 de marzo; lo cual es una diferencia de 11 días es decir 11 observaciones.</t>
   </si>
 </sst>
 </file>
@@ -509,7 +518,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -990,6 +999,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1864,6 +1906,38 @@
         <v>428563</v>
       </c>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>43999</v>
+      </c>
+      <c r="B18" s="174">
+        <v>159793</v>
+      </c>
+      <c r="C18" s="175">
+        <v>222801</v>
+      </c>
+      <c r="D18" s="176">
+        <v>59076</v>
+      </c>
+      <c r="E18" s="177">
+        <v>19080</v>
+      </c>
+      <c r="F18" s="178">
+        <v>32.055221442741548</v>
+      </c>
+      <c r="G18" s="179">
+        <v>51222</v>
+      </c>
+      <c r="H18" s="180">
+        <v>4654</v>
+      </c>
+      <c r="I18" s="181">
+        <v>4828</v>
+      </c>
+      <c r="J18" s="182">
+        <v>441670</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1874,7 +1948,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2481,17 +2555,39 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="48"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
+      <c r="A18" s="48">
+        <v>43999</v>
+      </c>
+      <c r="B18" s="49">
+        <v>0</v>
+      </c>
+      <c r="C18" s="49">
+        <v>1</v>
+      </c>
+      <c r="D18" s="49">
+        <v>1</v>
+      </c>
+      <c r="E18" s="49">
+        <v>1</v>
+      </c>
+      <c r="F18" s="49">
+        <v>1</v>
+      </c>
+      <c r="G18" s="49">
+        <v>0</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0</v>
+      </c>
+      <c r="I18" s="49">
+        <v>1</v>
+      </c>
+      <c r="J18" s="49">
+        <v>0</v>
+      </c>
+      <c r="K18" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
@@ -2539,10 +2635,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3238,6 +3334,47 @@
         <v>0</v>
       </c>
       <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="48">
+        <v>43999</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>0</v>
       </c>
     </row>
@@ -3251,7 +3388,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3809,7 +3946,36 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="108"/>
+      <c r="A18" s="48">
+        <v>43999</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="108"/>
@@ -3863,10 +4029,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3874,7 +4040,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -3926,9 +4092,16 @@
       <c r="Q1" s="50">
         <v>43998</v>
       </c>
-      <c r="R1" s="50"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R1" s="50">
+        <v>43999</v>
+      </c>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>23</v>
       </c>
@@ -3980,9 +4153,16 @@
       <c r="Q2" s="49">
         <v>3529</v>
       </c>
-      <c r="R2" s="49"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R2" s="49">
+        <v>3561</v>
+      </c>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
@@ -4034,9 +4214,16 @@
       <c r="Q3" s="49">
         <v>3344</v>
       </c>
-      <c r="R3" s="49"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R3" s="49">
+        <v>3376</v>
+      </c>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>25</v>
       </c>
@@ -4088,9 +4275,16 @@
       <c r="Q4" s="49">
         <v>3344</v>
       </c>
-      <c r="R4" s="49"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="49">
+        <v>3376</v>
+      </c>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>26</v>
       </c>
@@ -4142,9 +4336,16 @@
       <c r="Q5" s="49">
         <v>3344</v>
       </c>
-      <c r="R5" s="49"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R5" s="49">
+        <v>3376</v>
+      </c>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>27</v>
       </c>
@@ -4196,9 +4397,16 @@
       <c r="Q6" s="49">
         <v>3344</v>
       </c>
-      <c r="R6" s="49"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R6" s="49">
+        <v>3376</v>
+      </c>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>28</v>
       </c>
@@ -4250,9 +4458,16 @@
       <c r="Q7" s="49">
         <v>2535</v>
       </c>
-      <c r="R7" s="49"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R7" s="49">
+        <v>2567</v>
+      </c>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>29</v>
       </c>
@@ -4304,9 +4519,16 @@
       <c r="Q8" s="49">
         <v>5166</v>
       </c>
-      <c r="R8" s="49"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" s="49">
+        <v>5198</v>
+      </c>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="76"/>
       <c r="B9" s="77"/>
       <c r="C9" s="77"/>
@@ -4325,8 +4547,13 @@
       <c r="P9" s="89"/>
       <c r="Q9" s="89"/>
       <c r="R9" s="89"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>30</v>
       </c>
@@ -4378,9 +4605,16 @@
       <c r="Q10" s="49">
         <v>156</v>
       </c>
-      <c r="R10" s="49"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R10" s="49">
+        <v>157</v>
+      </c>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>31</v>
       </c>
@@ -4432,9 +4666,16 @@
       <c r="Q11" s="49">
         <v>156</v>
       </c>
-      <c r="R11" s="49"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11" s="49">
+        <v>157</v>
+      </c>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>32</v>
       </c>
@@ -4486,9 +4727,16 @@
       <c r="Q12" s="49">
         <v>156</v>
       </c>
-      <c r="R12" s="49"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" s="49">
+        <v>157</v>
+      </c>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>33</v>
       </c>
@@ -4540,9 +4788,16 @@
       <c r="Q13" s="49">
         <v>156</v>
       </c>
-      <c r="R13" s="49"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R13" s="49">
+        <v>157</v>
+      </c>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
@@ -4594,9 +4849,16 @@
       <c r="Q14" s="49">
         <v>156</v>
       </c>
-      <c r="R14" s="49"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R14" s="49">
+        <v>157</v>
+      </c>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="37" t="s">
         <v>35</v>
       </c>
@@ -4648,9 +4910,16 @@
       <c r="Q15" s="49">
         <v>91</v>
       </c>
-      <c r="R15" s="49"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R15" s="49">
+        <v>92</v>
+      </c>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>36</v>
       </c>
@@ -4702,9 +4971,16 @@
       <c r="Q16" s="49">
         <v>168</v>
       </c>
-      <c r="R16" s="49"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R16" s="49">
+        <v>169</v>
+      </c>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="76"/>
       <c r="B17" s="77"/>
       <c r="C17" s="77"/>
@@ -4723,8 +4999,13 @@
       <c r="P17" s="89"/>
       <c r="Q17" s="89"/>
       <c r="R17" s="89"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>37</v>
       </c>
@@ -4776,16 +5057,23 @@
       <c r="Q18" s="49">
         <v>821</v>
       </c>
-      <c r="R18" s="49"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R18" s="49">
+        <v>828</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="53"/>
       <c r="C19" s="53"/>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>38</v>
       </c>
@@ -4794,7 +5082,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:Q20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:R20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -4853,7 +5141,15 @@
         <f t="shared" si="0"/>
         <v>26466</v>
       </c>
-      <c r="R20" s="49"/>
+      <c r="R20" s="52">
+        <f t="shared" si="0"/>
+        <v>26704</v>
+      </c>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4865,7 +5161,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5013,10 +5309,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5094,7 +5390,42 @@
         <v>56</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="183" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="183"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="183"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="183"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="184" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="184"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="184"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 18th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4F2914-82CE-FD40-9584-C801A5D4A865}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDC3DD-1512-5146-8CA0-47424244688B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1120" windowWidth="22840" windowHeight="15400" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -999,6 +999,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1351,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,6 +1965,38 @@
         <v>441670</v>
       </c>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>44000</v>
+      </c>
+      <c r="B19" s="183">
+        <v>165455</v>
+      </c>
+      <c r="C19" s="184">
+        <v>228248</v>
+      </c>
+      <c r="D19" s="185">
+        <v>59778</v>
+      </c>
+      <c r="E19" s="186">
+        <v>19747</v>
+      </c>
+      <c r="F19" s="187">
+        <v>31.855791604968118</v>
+      </c>
+      <c r="G19" s="188">
+        <v>52707</v>
+      </c>
+      <c r="H19" s="189">
+        <v>4758</v>
+      </c>
+      <c r="I19" s="190">
+        <v>4939</v>
+      </c>
+      <c r="J19" s="191">
+        <v>453481</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1948,7 +2007,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2590,17 +2649,39 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="48"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
+      <c r="A19" s="48">
+        <v>44000</v>
+      </c>
+      <c r="B19" s="49">
+        <v>0</v>
+      </c>
+      <c r="C19" s="49">
+        <v>1</v>
+      </c>
+      <c r="D19" s="49">
+        <v>1</v>
+      </c>
+      <c r="E19" s="49">
+        <v>1</v>
+      </c>
+      <c r="F19" s="49">
+        <v>1</v>
+      </c>
+      <c r="G19" s="49">
+        <v>0</v>
+      </c>
+      <c r="H19" s="49">
+        <v>0</v>
+      </c>
+      <c r="I19" s="49">
+        <v>1</v>
+      </c>
+      <c r="J19" s="49">
+        <v>0</v>
+      </c>
+      <c r="K19" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
@@ -2635,10 +2716,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3376,6 +3457,11 @@
       </c>
       <c r="M18">
         <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="48">
+        <v>44000</v>
       </c>
     </row>
   </sheetData>
@@ -3388,7 +3474,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3978,7 +4064,36 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="108"/>
+      <c r="A19" s="48">
+        <v>44000</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="108"/>
@@ -4031,8 +4146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4095,7 +4210,9 @@
       <c r="R1" s="50">
         <v>43999</v>
       </c>
-      <c r="S1" s="50"/>
+      <c r="S1" s="50">
+        <v>44000</v>
+      </c>
       <c r="T1" s="50"/>
       <c r="U1" s="50"/>
       <c r="V1" s="50"/>
@@ -4156,7 +4273,9 @@
       <c r="R2" s="49">
         <v>3561</v>
       </c>
-      <c r="S2" s="49"/>
+      <c r="S2" s="49">
+        <v>3593</v>
+      </c>
       <c r="T2" s="49"/>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
@@ -4217,7 +4336,9 @@
       <c r="R3" s="49">
         <v>3376</v>
       </c>
-      <c r="S3" s="49"/>
+      <c r="S3" s="49">
+        <v>3408</v>
+      </c>
       <c r="T3" s="49"/>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
@@ -4278,7 +4399,9 @@
       <c r="R4" s="49">
         <v>3376</v>
       </c>
-      <c r="S4" s="49"/>
+      <c r="S4" s="49">
+        <v>3408</v>
+      </c>
       <c r="T4" s="49"/>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
@@ -4339,7 +4462,9 @@
       <c r="R5" s="49">
         <v>3376</v>
       </c>
-      <c r="S5" s="49"/>
+      <c r="S5" s="49">
+        <v>3408</v>
+      </c>
       <c r="T5" s="49"/>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
@@ -4400,7 +4525,9 @@
       <c r="R6" s="49">
         <v>3376</v>
       </c>
-      <c r="S6" s="49"/>
+      <c r="S6" s="49">
+        <v>3408</v>
+      </c>
       <c r="T6" s="49"/>
       <c r="U6" s="49"/>
       <c r="V6" s="49"/>
@@ -4461,7 +4588,9 @@
       <c r="R7" s="49">
         <v>2567</v>
       </c>
-      <c r="S7" s="49"/>
+      <c r="S7" s="49">
+        <v>2599</v>
+      </c>
       <c r="T7" s="49"/>
       <c r="U7" s="49"/>
       <c r="V7" s="49"/>
@@ -4522,7 +4651,9 @@
       <c r="R8" s="49">
         <v>5198</v>
       </c>
-      <c r="S8" s="49"/>
+      <c r="S8" s="49">
+        <v>5230</v>
+      </c>
       <c r="T8" s="49"/>
       <c r="U8" s="49"/>
       <c r="V8" s="49"/>
@@ -4608,7 +4739,9 @@
       <c r="R10" s="49">
         <v>157</v>
       </c>
-      <c r="S10" s="49"/>
+      <c r="S10" s="49">
+        <v>158</v>
+      </c>
       <c r="T10" s="49"/>
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
@@ -4669,7 +4802,9 @@
       <c r="R11" s="49">
         <v>157</v>
       </c>
-      <c r="S11" s="49"/>
+      <c r="S11" s="49">
+        <v>158</v>
+      </c>
       <c r="T11" s="49"/>
       <c r="U11" s="49"/>
       <c r="V11" s="49"/>
@@ -4730,7 +4865,9 @@
       <c r="R12" s="49">
         <v>157</v>
       </c>
-      <c r="S12" s="49"/>
+      <c r="S12" s="49">
+        <v>158</v>
+      </c>
       <c r="T12" s="49"/>
       <c r="U12" s="49"/>
       <c r="V12" s="49"/>
@@ -4791,7 +4928,9 @@
       <c r="R13" s="49">
         <v>157</v>
       </c>
-      <c r="S13" s="49"/>
+      <c r="S13" s="49">
+        <v>158</v>
+      </c>
       <c r="T13" s="49"/>
       <c r="U13" s="49"/>
       <c r="V13" s="49"/>
@@ -4852,7 +4991,9 @@
       <c r="R14" s="49">
         <v>157</v>
       </c>
-      <c r="S14" s="49"/>
+      <c r="S14" s="49">
+        <v>158</v>
+      </c>
       <c r="T14" s="49"/>
       <c r="U14" s="49"/>
       <c r="V14" s="49"/>
@@ -4913,7 +5054,9 @@
       <c r="R15" s="49">
         <v>92</v>
       </c>
-      <c r="S15" s="49"/>
+      <c r="S15" s="49">
+        <v>93</v>
+      </c>
       <c r="T15" s="49"/>
       <c r="U15" s="49"/>
       <c r="V15" s="49"/>
@@ -4974,7 +5117,9 @@
       <c r="R16" s="49">
         <v>169</v>
       </c>
-      <c r="S16" s="49"/>
+      <c r="S16" s="49">
+        <v>170</v>
+      </c>
       <c r="T16" s="49"/>
       <c r="U16" s="49"/>
       <c r="V16" s="49"/>
@@ -5060,7 +5205,9 @@
       <c r="R18" s="49">
         <v>828</v>
       </c>
-      <c r="S18" s="49"/>
+      <c r="S18" s="49">
+        <v>835</v>
+      </c>
       <c r="T18" s="49"/>
       <c r="U18" s="49"/>
       <c r="V18" s="49"/>
@@ -5082,7 +5229,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:R20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:S20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -5145,7 +5292,10 @@
         <f t="shared" si="0"/>
         <v>26704</v>
       </c>
-      <c r="S20" s="49"/>
+      <c r="S20" s="52">
+        <f t="shared" si="0"/>
+        <v>26942</v>
+      </c>
       <c r="T20" s="49"/>
       <c r="U20" s="49"/>
       <c r="V20" s="49"/>
@@ -5394,32 +5544,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="183" t="s">
+      <c r="B8" s="192" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="183"/>
+      <c r="B9" s="192"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="183"/>
+      <c r="B10" s="192"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="183"/>
+      <c r="B11" s="192"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="184" t="s">
+      <c r="B12" s="193" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="184"/>
+      <c r="B13" s="193"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="184"/>
+      <c r="B14" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 19th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CDC3DD-1512-5146-8CA0-47424244688B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBB5E20-FEB3-DE4A-91CB-753D3AEC7490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -999,6 +999,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1378,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1997,6 +2024,38 @@
         <v>453481</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>44001</v>
+      </c>
+      <c r="B20" s="192">
+        <v>170485</v>
+      </c>
+      <c r="C20" s="193">
+        <v>233137</v>
+      </c>
+      <c r="D20" s="194">
+        <v>62245</v>
+      </c>
+      <c r="E20" s="195">
+        <v>20394</v>
+      </c>
+      <c r="F20" s="196">
+        <v>31.724198609848376</v>
+      </c>
+      <c r="G20" s="197">
+        <v>54085</v>
+      </c>
+      <c r="H20" s="198">
+        <v>4876</v>
+      </c>
+      <c r="I20" s="199">
+        <v>5058</v>
+      </c>
+      <c r="J20" s="200">
+        <v>465867</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2007,7 +2066,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2684,17 +2743,39 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
+      <c r="A20" s="48">
+        <v>44001</v>
+      </c>
+      <c r="B20" s="49">
+        <v>0</v>
+      </c>
+      <c r="C20" s="49">
+        <v>1</v>
+      </c>
+      <c r="D20" s="49">
+        <v>1</v>
+      </c>
+      <c r="E20" s="49">
+        <v>1</v>
+      </c>
+      <c r="F20" s="49">
+        <v>1</v>
+      </c>
+      <c r="G20" s="49">
+        <v>0</v>
+      </c>
+      <c r="H20" s="49">
+        <v>0</v>
+      </c>
+      <c r="I20" s="49">
+        <v>1</v>
+      </c>
+      <c r="J20" s="49">
+        <v>0</v>
+      </c>
+      <c r="K20" s="49">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="48"/>
@@ -2716,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3462,6 +3543,83 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="48">
         <v>44000</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="48">
+        <v>44001</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3474,7 +3632,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4096,7 +4254,36 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="108"/>
+      <c r="A20" s="48">
+        <v>44001</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="108"/>
@@ -4146,8 +4333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4213,7 +4400,9 @@
       <c r="S1" s="50">
         <v>44000</v>
       </c>
-      <c r="T1" s="50"/>
+      <c r="T1" s="50">
+        <v>44001</v>
+      </c>
       <c r="U1" s="50"/>
       <c r="V1" s="50"/>
       <c r="W1" s="50"/>
@@ -4276,7 +4465,9 @@
       <c r="S2" s="49">
         <v>3593</v>
       </c>
-      <c r="T2" s="49"/>
+      <c r="T2" s="49">
+        <v>3625</v>
+      </c>
       <c r="U2" s="49"/>
       <c r="V2" s="49"/>
       <c r="W2" s="49"/>
@@ -4339,7 +4530,9 @@
       <c r="S3" s="49">
         <v>3408</v>
       </c>
-      <c r="T3" s="49"/>
+      <c r="T3" s="49">
+        <v>3440</v>
+      </c>
       <c r="U3" s="49"/>
       <c r="V3" s="49"/>
       <c r="W3" s="49"/>
@@ -4402,7 +4595,9 @@
       <c r="S4" s="49">
         <v>3408</v>
       </c>
-      <c r="T4" s="49"/>
+      <c r="T4" s="49">
+        <v>3440</v>
+      </c>
       <c r="U4" s="49"/>
       <c r="V4" s="49"/>
       <c r="W4" s="49"/>
@@ -4465,7 +4660,9 @@
       <c r="S5" s="49">
         <v>3408</v>
       </c>
-      <c r="T5" s="49"/>
+      <c r="T5" s="49">
+        <v>3440</v>
+      </c>
       <c r="U5" s="49"/>
       <c r="V5" s="49"/>
       <c r="W5" s="49"/>
@@ -4528,7 +4725,9 @@
       <c r="S6" s="49">
         <v>3408</v>
       </c>
-      <c r="T6" s="49"/>
+      <c r="T6" s="49">
+        <v>3440</v>
+      </c>
       <c r="U6" s="49"/>
       <c r="V6" s="49"/>
       <c r="W6" s="49"/>
@@ -4591,7 +4790,9 @@
       <c r="S7" s="49">
         <v>2599</v>
       </c>
-      <c r="T7" s="49"/>
+      <c r="T7" s="49">
+        <v>2631</v>
+      </c>
       <c r="U7" s="49"/>
       <c r="V7" s="49"/>
       <c r="W7" s="49"/>
@@ -4654,7 +4855,9 @@
       <c r="S8" s="49">
         <v>5230</v>
       </c>
-      <c r="T8" s="49"/>
+      <c r="T8" s="49">
+        <v>5262</v>
+      </c>
       <c r="U8" s="49"/>
       <c r="V8" s="49"/>
       <c r="W8" s="49"/>
@@ -4742,7 +4945,9 @@
       <c r="S10" s="49">
         <v>158</v>
       </c>
-      <c r="T10" s="49"/>
+      <c r="T10" s="49">
+        <v>159</v>
+      </c>
       <c r="U10" s="49"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49"/>
@@ -4805,7 +5010,9 @@
       <c r="S11" s="49">
         <v>158</v>
       </c>
-      <c r="T11" s="49"/>
+      <c r="T11" s="49">
+        <v>159</v>
+      </c>
       <c r="U11" s="49"/>
       <c r="V11" s="49"/>
       <c r="W11" s="49"/>
@@ -4868,7 +5075,9 @@
       <c r="S12" s="49">
         <v>158</v>
       </c>
-      <c r="T12" s="49"/>
+      <c r="T12" s="49">
+        <v>159</v>
+      </c>
       <c r="U12" s="49"/>
       <c r="V12" s="49"/>
       <c r="W12" s="49"/>
@@ -4931,7 +5140,9 @@
       <c r="S13" s="49">
         <v>158</v>
       </c>
-      <c r="T13" s="49"/>
+      <c r="T13" s="49">
+        <v>159</v>
+      </c>
       <c r="U13" s="49"/>
       <c r="V13" s="49"/>
       <c r="W13" s="49"/>
@@ -4994,7 +5205,9 @@
       <c r="S14" s="49">
         <v>158</v>
       </c>
-      <c r="T14" s="49"/>
+      <c r="T14" s="49">
+        <v>159</v>
+      </c>
       <c r="U14" s="49"/>
       <c r="V14" s="49"/>
       <c r="W14" s="49"/>
@@ -5057,7 +5270,9 @@
       <c r="S15" s="49">
         <v>93</v>
       </c>
-      <c r="T15" s="49"/>
+      <c r="T15" s="49">
+        <v>94</v>
+      </c>
       <c r="U15" s="49"/>
       <c r="V15" s="49"/>
       <c r="W15" s="49"/>
@@ -5120,7 +5335,9 @@
       <c r="S16" s="49">
         <v>170</v>
       </c>
-      <c r="T16" s="49"/>
+      <c r="T16" s="49">
+        <v>171</v>
+      </c>
       <c r="U16" s="49"/>
       <c r="V16" s="49"/>
       <c r="W16" s="49"/>
@@ -5208,7 +5425,9 @@
       <c r="S18" s="49">
         <v>835</v>
       </c>
-      <c r="T18" s="49"/>
+      <c r="T18" s="49">
+        <v>842</v>
+      </c>
       <c r="U18" s="49"/>
       <c r="V18" s="49"/>
       <c r="W18" s="49"/>
@@ -5229,7 +5448,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="52">
-        <f t="shared" ref="C20:S20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:T20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="52">
@@ -5296,7 +5515,10 @@
         <f t="shared" si="0"/>
         <v>26942</v>
       </c>
-      <c r="T20" s="49"/>
+      <c r="T20" s="52">
+        <f t="shared" si="0"/>
+        <v>27180</v>
+      </c>
       <c r="U20" s="49"/>
       <c r="V20" s="49"/>
       <c r="W20" s="49"/>
@@ -5461,8 +5683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5544,32 +5766,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="192" t="s">
+      <c r="B8" s="201" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="192"/>
+      <c r="B9" s="201"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="192"/>
+      <c r="B10" s="201"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="192"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="193" t="s">
+      <c r="B12" s="202" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="193"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="193"/>
+      <c r="B14" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 22th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF8FE97-38D5-FE41-ABC3-208C5EF895D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A25703-C478-1043-9D67-6199993CDE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="8320" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -523,6 +523,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -542,7 +551,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1154,18 +1163,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="11" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="11" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,6 +2241,38 @@
         <v>479528</v>
       </c>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>44004</v>
+      </c>
+      <c r="B23" s="221">
+        <v>185122</v>
+      </c>
+      <c r="C23" s="222">
+        <v>246147</v>
+      </c>
+      <c r="D23" s="223">
+        <v>57281</v>
+      </c>
+      <c r="E23" s="224">
+        <v>22584</v>
+      </c>
+      <c r="F23" s="225">
+        <v>31.687751860934949</v>
+      </c>
+      <c r="G23" s="226">
+        <v>58661</v>
+      </c>
+      <c r="H23" s="227">
+        <v>5112</v>
+      </c>
+      <c r="I23" s="228">
+        <v>5280</v>
+      </c>
+      <c r="J23" s="229">
+        <v>488550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2209,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2957,52 +3030,74 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="220">
+      <c r="A22" s="218">
         <v>44003</v>
       </c>
-      <c r="B22" s="219">
-        <v>0</v>
-      </c>
-      <c r="C22" s="219">
-        <v>1</v>
-      </c>
-      <c r="D22" s="219">
-        <v>1</v>
-      </c>
-      <c r="E22" s="219">
-        <v>1</v>
-      </c>
-      <c r="F22" s="219">
-        <v>1</v>
-      </c>
-      <c r="G22" s="219">
-        <v>0</v>
-      </c>
-      <c r="H22" s="219">
-        <v>0</v>
-      </c>
-      <c r="I22" s="219">
-        <v>1</v>
-      </c>
-      <c r="J22" s="219">
-        <v>9</v>
-      </c>
-      <c r="K22" s="219">
+      <c r="B22" s="217">
+        <v>0</v>
+      </c>
+      <c r="C22" s="217">
+        <v>1</v>
+      </c>
+      <c r="D22" s="217">
+        <v>1</v>
+      </c>
+      <c r="E22" s="217">
+        <v>1</v>
+      </c>
+      <c r="F22" s="217">
+        <v>1</v>
+      </c>
+      <c r="G22" s="217">
+        <v>0</v>
+      </c>
+      <c r="H22" s="217">
+        <v>0</v>
+      </c>
+      <c r="I22" s="217">
+        <v>1</v>
+      </c>
+      <c r="J22" s="217">
+        <v>0</v>
+      </c>
+      <c r="K22" s="217">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
+      <c r="A23" s="218">
+        <v>44004</v>
+      </c>
+      <c r="B23" s="48">
+        <v>0</v>
+      </c>
+      <c r="C23" s="48">
+        <v>1</v>
+      </c>
+      <c r="D23" s="48">
+        <v>1</v>
+      </c>
+      <c r="E23" s="48">
+        <v>1</v>
+      </c>
+      <c r="F23" s="48">
+        <v>1</v>
+      </c>
+      <c r="G23" s="48">
+        <v>0</v>
+      </c>
+      <c r="H23" s="48">
+        <v>0</v>
+      </c>
+      <c r="I23" s="48">
+        <v>1</v>
+      </c>
+      <c r="J23" s="48">
+        <v>0</v>
+      </c>
+      <c r="K23" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
@@ -3195,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4102,19 +4197,45 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
+      <c r="A23" s="47">
+        <v>44004</v>
+      </c>
+      <c r="B23" s="48">
+        <v>0</v>
+      </c>
+      <c r="C23" s="48">
+        <v>1</v>
+      </c>
+      <c r="D23" s="48">
+        <v>1</v>
+      </c>
+      <c r="E23" s="48">
+        <v>0</v>
+      </c>
+      <c r="F23" s="48">
+        <v>1</v>
+      </c>
+      <c r="G23" s="48">
+        <v>1</v>
+      </c>
+      <c r="H23" s="48">
+        <v>1</v>
+      </c>
+      <c r="I23" s="48">
+        <v>0</v>
+      </c>
+      <c r="J23" s="48">
+        <v>1</v>
+      </c>
+      <c r="K23" s="48">
+        <v>1</v>
+      </c>
+      <c r="L23" s="48">
+        <v>0</v>
+      </c>
+      <c r="M23" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
@@ -4200,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4602,7 +4723,7 @@
       <c r="A13" s="47">
         <v>43994</v>
       </c>
-      <c r="B13" s="221">
+      <c r="B13" s="219">
         <v>1</v>
       </c>
       <c r="C13" s="48">
@@ -4919,19 +5040,39 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="222"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
+      <c r="A23" s="47">
+        <v>44004</v>
+      </c>
+      <c r="B23" s="48">
+        <v>0</v>
+      </c>
+      <c r="C23" s="48">
+        <v>0</v>
+      </c>
+      <c r="D23" s="48">
+        <v>0</v>
+      </c>
+      <c r="E23" s="48">
+        <v>0</v>
+      </c>
+      <c r="F23" s="48">
+        <v>2</v>
+      </c>
+      <c r="G23" s="48">
+        <v>1</v>
+      </c>
+      <c r="H23" s="48">
+        <v>1</v>
+      </c>
+      <c r="I23" s="48">
+        <v>1</v>
+      </c>
+      <c r="J23" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="222"/>
+      <c r="A24" s="220"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
@@ -4943,7 +5084,7 @@
       <c r="J24" s="48"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="222"/>
+      <c r="A25" s="220"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
       <c r="D25" s="48"/>
@@ -4955,7 +5096,7 @@
       <c r="J25" s="48"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="222"/>
+      <c r="A26" s="220"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
       <c r="D26" s="48"/>
@@ -4967,7 +5108,7 @@
       <c r="J26" s="48"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="222"/>
+      <c r="A27" s="220"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
       <c r="D27" s="48"/>
@@ -4979,7 +5120,7 @@
       <c r="J27" s="48"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="222"/>
+      <c r="A28" s="220"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
@@ -5012,10 +5153,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5023,7 +5164,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -5087,12 +5228,39 @@
       <c r="U1" s="49">
         <v>44002</v>
       </c>
-      <c r="V1" s="49">
+      <c r="V1" s="232">
         <v>44003</v>
       </c>
-      <c r="W1" s="49"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W1" s="49">
+        <v>44004</v>
+      </c>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -5156,12 +5324,39 @@
       <c r="U2" s="48">
         <v>3657</v>
       </c>
-      <c r="V2" s="48">
+      <c r="V2" s="233">
         <v>3689</v>
       </c>
-      <c r="W2" s="48"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W2" s="234">
+        <v>3721</v>
+      </c>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48"/>
+      <c r="AG2" s="48"/>
+      <c r="AH2" s="48"/>
+      <c r="AI2" s="48"/>
+      <c r="AJ2" s="48"/>
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="48"/>
+      <c r="AM2" s="48"/>
+      <c r="AN2" s="48"/>
+      <c r="AO2" s="48"/>
+      <c r="AP2" s="48"/>
+      <c r="AQ2" s="48"/>
+      <c r="AR2" s="48"/>
+      <c r="AS2" s="48"/>
+      <c r="AT2" s="48"/>
+      <c r="AU2" s="48"/>
+      <c r="AV2" s="48"/>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -5225,12 +5420,39 @@
       <c r="U3" s="48">
         <v>3472</v>
       </c>
-      <c r="V3" s="48">
+      <c r="V3" s="233">
         <v>3504</v>
       </c>
-      <c r="W3" s="48"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W3" s="48">
+        <v>3536</v>
+      </c>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="48"/>
+      <c r="AL3" s="48"/>
+      <c r="AM3" s="48"/>
+      <c r="AN3" s="48"/>
+      <c r="AO3" s="48"/>
+      <c r="AP3" s="48"/>
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="48"/>
+      <c r="AS3" s="48"/>
+      <c r="AT3" s="48"/>
+      <c r="AU3" s="48"/>
+      <c r="AV3" s="48"/>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -5294,12 +5516,39 @@
       <c r="U4" s="48">
         <v>3472</v>
       </c>
-      <c r="V4" s="48">
+      <c r="V4" s="233">
         <v>3504</v>
       </c>
-      <c r="W4" s="48"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W4" s="48">
+        <v>3536</v>
+      </c>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
+      <c r="AG4" s="48"/>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="48"/>
+      <c r="AK4" s="48"/>
+      <c r="AL4" s="48"/>
+      <c r="AM4" s="48"/>
+      <c r="AN4" s="48"/>
+      <c r="AO4" s="48"/>
+      <c r="AP4" s="48"/>
+      <c r="AQ4" s="48"/>
+      <c r="AR4" s="48"/>
+      <c r="AS4" s="48"/>
+      <c r="AT4" s="48"/>
+      <c r="AU4" s="48"/>
+      <c r="AV4" s="48"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -5363,12 +5612,39 @@
       <c r="U5" s="48">
         <v>3472</v>
       </c>
-      <c r="V5" s="48">
+      <c r="V5" s="233">
         <v>3504</v>
       </c>
-      <c r="W5" s="48"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W5" s="48">
+        <v>3536</v>
+      </c>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="48"/>
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="48"/>
+      <c r="AL5" s="48"/>
+      <c r="AM5" s="48"/>
+      <c r="AN5" s="48"/>
+      <c r="AO5" s="48"/>
+      <c r="AP5" s="48"/>
+      <c r="AQ5" s="48"/>
+      <c r="AR5" s="48"/>
+      <c r="AS5" s="48"/>
+      <c r="AT5" s="48"/>
+      <c r="AU5" s="48"/>
+      <c r="AV5" s="48"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -5432,12 +5708,39 @@
       <c r="U6" s="48">
         <v>3472</v>
       </c>
-      <c r="V6" s="48">
+      <c r="V6" s="233">
         <v>3504</v>
       </c>
-      <c r="W6" s="48"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W6" s="48">
+        <v>3536</v>
+      </c>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="48"/>
+      <c r="AE6" s="48"/>
+      <c r="AF6" s="48"/>
+      <c r="AG6" s="48"/>
+      <c r="AH6" s="48"/>
+      <c r="AI6" s="48"/>
+      <c r="AJ6" s="48"/>
+      <c r="AK6" s="48"/>
+      <c r="AL6" s="48"/>
+      <c r="AM6" s="48"/>
+      <c r="AN6" s="48"/>
+      <c r="AO6" s="48"/>
+      <c r="AP6" s="48"/>
+      <c r="AQ6" s="48"/>
+      <c r="AR6" s="48"/>
+      <c r="AS6" s="48"/>
+      <c r="AT6" s="48"/>
+      <c r="AU6" s="48"/>
+      <c r="AV6" s="48"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -5501,12 +5804,39 @@
       <c r="U7" s="48">
         <v>2663</v>
       </c>
-      <c r="V7" s="48">
+      <c r="V7" s="233">
         <v>2695</v>
       </c>
-      <c r="W7" s="48"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W7" s="48">
+        <v>2727</v>
+      </c>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="48"/>
+      <c r="AB7" s="48"/>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="48"/>
+      <c r="AE7" s="48"/>
+      <c r="AF7" s="48"/>
+      <c r="AG7" s="48"/>
+      <c r="AH7" s="48"/>
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="48"/>
+      <c r="AK7" s="48"/>
+      <c r="AL7" s="48"/>
+      <c r="AM7" s="48"/>
+      <c r="AN7" s="48"/>
+      <c r="AO7" s="48"/>
+      <c r="AP7" s="48"/>
+      <c r="AQ7" s="48"/>
+      <c r="AR7" s="48"/>
+      <c r="AS7" s="48"/>
+      <c r="AT7" s="48"/>
+      <c r="AU7" s="48"/>
+      <c r="AV7" s="48"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -5570,12 +5900,39 @@
       <c r="U8" s="48">
         <v>5294</v>
       </c>
-      <c r="V8" s="48">
+      <c r="V8" s="233">
         <v>5326</v>
       </c>
-      <c r="W8" s="48"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W8" s="48">
+        <v>5358</v>
+      </c>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
+      <c r="AB8" s="48"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="48"/>
+      <c r="AE8" s="48"/>
+      <c r="AF8" s="48"/>
+      <c r="AG8" s="48"/>
+      <c r="AH8" s="48"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="48"/>
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="48"/>
+      <c r="AN8" s="48"/>
+      <c r="AO8" s="48"/>
+      <c r="AP8" s="48"/>
+      <c r="AQ8" s="48"/>
+      <c r="AR8" s="48"/>
+      <c r="AS8" s="48"/>
+      <c r="AT8" s="48"/>
+      <c r="AU8" s="48"/>
+      <c r="AV8" s="48"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -5598,9 +5955,34 @@
       <c r="T9" s="88"/>
       <c r="U9" s="88"/>
       <c r="V9" s="88"/>
-      <c r="W9" s="88"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W9" s="78"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="78"/>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78"/>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78"/>
+      <c r="AD9" s="78"/>
+      <c r="AE9" s="78"/>
+      <c r="AF9" s="48"/>
+      <c r="AG9" s="48"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="48"/>
+      <c r="AK9" s="48"/>
+      <c r="AL9" s="48"/>
+      <c r="AM9" s="48"/>
+      <c r="AN9" s="48"/>
+      <c r="AO9" s="48"/>
+      <c r="AP9" s="48"/>
+      <c r="AQ9" s="48"/>
+      <c r="AR9" s="48"/>
+      <c r="AS9" s="48"/>
+      <c r="AT9" s="48"/>
+      <c r="AU9" s="48"/>
+      <c r="AV9" s="48"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -5664,12 +6046,39 @@
       <c r="U10" s="48">
         <v>160</v>
       </c>
-      <c r="V10" s="48">
+      <c r="V10" s="233">
         <v>161</v>
       </c>
-      <c r="W10" s="48"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W10" s="48">
+        <v>162</v>
+      </c>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48"/>
+      <c r="AA10" s="48"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="48"/>
+      <c r="AF10" s="48"/>
+      <c r="AG10" s="48"/>
+      <c r="AH10" s="48"/>
+      <c r="AI10" s="48"/>
+      <c r="AJ10" s="48"/>
+      <c r="AK10" s="48"/>
+      <c r="AL10" s="48"/>
+      <c r="AM10" s="48"/>
+      <c r="AN10" s="48"/>
+      <c r="AO10" s="48"/>
+      <c r="AP10" s="48"/>
+      <c r="AQ10" s="48"/>
+      <c r="AR10" s="48"/>
+      <c r="AS10" s="48"/>
+      <c r="AT10" s="48"/>
+      <c r="AU10" s="48"/>
+      <c r="AV10" s="48"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -5733,12 +6142,39 @@
       <c r="U11" s="48">
         <v>160</v>
       </c>
-      <c r="V11" s="48">
+      <c r="V11" s="233">
         <v>161</v>
       </c>
-      <c r="W11" s="48"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W11" s="48">
+        <v>162</v>
+      </c>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+      <c r="AA11" s="48"/>
+      <c r="AB11" s="48"/>
+      <c r="AC11" s="48"/>
+      <c r="AD11" s="48"/>
+      <c r="AE11" s="48"/>
+      <c r="AF11" s="48"/>
+      <c r="AG11" s="48"/>
+      <c r="AH11" s="48"/>
+      <c r="AI11" s="48"/>
+      <c r="AJ11" s="48"/>
+      <c r="AK11" s="48"/>
+      <c r="AL11" s="48"/>
+      <c r="AM11" s="48"/>
+      <c r="AN11" s="48"/>
+      <c r="AO11" s="48"/>
+      <c r="AP11" s="48"/>
+      <c r="AQ11" s="48"/>
+      <c r="AR11" s="48"/>
+      <c r="AS11" s="48"/>
+      <c r="AT11" s="48"/>
+      <c r="AU11" s="48"/>
+      <c r="AV11" s="48"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -5802,12 +6238,39 @@
       <c r="U12" s="48">
         <v>160</v>
       </c>
-      <c r="V12" s="48">
+      <c r="V12" s="233">
         <v>161</v>
       </c>
-      <c r="W12" s="48"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W12" s="48">
+        <v>162</v>
+      </c>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+      <c r="AC12" s="48"/>
+      <c r="AD12" s="48"/>
+      <c r="AE12" s="48"/>
+      <c r="AF12" s="48"/>
+      <c r="AG12" s="48"/>
+      <c r="AH12" s="48"/>
+      <c r="AI12" s="48"/>
+      <c r="AJ12" s="48"/>
+      <c r="AK12" s="48"/>
+      <c r="AL12" s="48"/>
+      <c r="AM12" s="48"/>
+      <c r="AN12" s="48"/>
+      <c r="AO12" s="48"/>
+      <c r="AP12" s="48"/>
+      <c r="AQ12" s="48"/>
+      <c r="AR12" s="48"/>
+      <c r="AS12" s="48"/>
+      <c r="AT12" s="48"/>
+      <c r="AU12" s="48"/>
+      <c r="AV12" s="48"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -5871,12 +6334,39 @@
       <c r="U13" s="48">
         <v>160</v>
       </c>
-      <c r="V13" s="48">
+      <c r="V13" s="233">
         <v>161</v>
       </c>
-      <c r="W13" s="48"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W13" s="48">
+        <v>162</v>
+      </c>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="48"/>
+      <c r="AC13" s="48"/>
+      <c r="AD13" s="48"/>
+      <c r="AE13" s="48"/>
+      <c r="AF13" s="48"/>
+      <c r="AG13" s="48"/>
+      <c r="AH13" s="48"/>
+      <c r="AI13" s="48"/>
+      <c r="AJ13" s="48"/>
+      <c r="AK13" s="48"/>
+      <c r="AL13" s="48"/>
+      <c r="AM13" s="48"/>
+      <c r="AN13" s="48"/>
+      <c r="AO13" s="48"/>
+      <c r="AP13" s="48"/>
+      <c r="AQ13" s="48"/>
+      <c r="AR13" s="48"/>
+      <c r="AS13" s="48"/>
+      <c r="AT13" s="48"/>
+      <c r="AU13" s="48"/>
+      <c r="AV13" s="48"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -5940,12 +6430,39 @@
       <c r="U14" s="48">
         <v>160</v>
       </c>
-      <c r="V14" s="48">
+      <c r="V14" s="233">
         <v>161</v>
       </c>
-      <c r="W14" s="48"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W14" s="48">
+        <v>162</v>
+      </c>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="48"/>
+      <c r="AB14" s="48"/>
+      <c r="AC14" s="48"/>
+      <c r="AD14" s="48"/>
+      <c r="AE14" s="48"/>
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="48"/>
+      <c r="AH14" s="48"/>
+      <c r="AI14" s="48"/>
+      <c r="AJ14" s="48"/>
+      <c r="AK14" s="48"/>
+      <c r="AL14" s="48"/>
+      <c r="AM14" s="48"/>
+      <c r="AN14" s="48"/>
+      <c r="AO14" s="48"/>
+      <c r="AP14" s="48"/>
+      <c r="AQ14" s="48"/>
+      <c r="AR14" s="48"/>
+      <c r="AS14" s="48"/>
+      <c r="AT14" s="48"/>
+      <c r="AU14" s="48"/>
+      <c r="AV14" s="48"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -6009,12 +6526,39 @@
       <c r="U15" s="48">
         <v>95</v>
       </c>
-      <c r="V15" s="48">
+      <c r="V15" s="233">
         <v>96</v>
       </c>
-      <c r="W15" s="48"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W15" s="48">
+        <v>97</v>
+      </c>
+      <c r="X15" s="48"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="48"/>
+      <c r="AB15" s="48"/>
+      <c r="AC15" s="48"/>
+      <c r="AD15" s="48"/>
+      <c r="AE15" s="48"/>
+      <c r="AF15" s="48"/>
+      <c r="AG15" s="48"/>
+      <c r="AH15" s="48"/>
+      <c r="AI15" s="48"/>
+      <c r="AJ15" s="48"/>
+      <c r="AK15" s="48"/>
+      <c r="AL15" s="48"/>
+      <c r="AM15" s="48"/>
+      <c r="AN15" s="48"/>
+      <c r="AO15" s="48"/>
+      <c r="AP15" s="48"/>
+      <c r="AQ15" s="48"/>
+      <c r="AR15" s="48"/>
+      <c r="AS15" s="48"/>
+      <c r="AT15" s="48"/>
+      <c r="AU15" s="48"/>
+      <c r="AV15" s="48"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -6078,12 +6622,39 @@
       <c r="U16" s="48">
         <v>172</v>
       </c>
-      <c r="V16" s="48">
+      <c r="V16" s="233">
         <v>173</v>
       </c>
-      <c r="W16" s="48"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W16" s="48">
+        <v>174</v>
+      </c>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="48"/>
+      <c r="AE16" s="48"/>
+      <c r="AF16" s="48"/>
+      <c r="AG16" s="48"/>
+      <c r="AH16" s="48"/>
+      <c r="AI16" s="48"/>
+      <c r="AJ16" s="48"/>
+      <c r="AK16" s="48"/>
+      <c r="AL16" s="48"/>
+      <c r="AM16" s="48"/>
+      <c r="AN16" s="48"/>
+      <c r="AO16" s="48"/>
+      <c r="AP16" s="48"/>
+      <c r="AQ16" s="48"/>
+      <c r="AR16" s="48"/>
+      <c r="AS16" s="48"/>
+      <c r="AT16" s="48"/>
+      <c r="AU16" s="48"/>
+      <c r="AV16" s="48"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -6106,9 +6677,34 @@
       <c r="T17" s="88"/>
       <c r="U17" s="88"/>
       <c r="V17" s="88"/>
-      <c r="W17" s="88"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W17" s="78"/>
+      <c r="X17" s="78"/>
+      <c r="Y17" s="78"/>
+      <c r="Z17" s="78"/>
+      <c r="AA17" s="78"/>
+      <c r="AB17" s="78"/>
+      <c r="AC17" s="78"/>
+      <c r="AD17" s="78"/>
+      <c r="AE17" s="78"/>
+      <c r="AF17" s="48"/>
+      <c r="AG17" s="48"/>
+      <c r="AH17" s="48"/>
+      <c r="AI17" s="48"/>
+      <c r="AJ17" s="48"/>
+      <c r="AK17" s="48"/>
+      <c r="AL17" s="48"/>
+      <c r="AM17" s="48"/>
+      <c r="AN17" s="48"/>
+      <c r="AO17" s="48"/>
+      <c r="AP17" s="48"/>
+      <c r="AQ17" s="48"/>
+      <c r="AR17" s="48"/>
+      <c r="AS17" s="48"/>
+      <c r="AT17" s="48"/>
+      <c r="AU17" s="48"/>
+      <c r="AV17" s="48"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -6172,19 +6768,46 @@
       <c r="U18" s="48">
         <v>849</v>
       </c>
-      <c r="V18" s="48">
+      <c r="V18" s="233">
         <v>856</v>
       </c>
-      <c r="W18" s="48"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W18" s="48">
+        <v>863</v>
+      </c>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="48"/>
+      <c r="AC18" s="48"/>
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="48"/>
+      <c r="AF18" s="48"/>
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="48"/>
+      <c r="AI18" s="48"/>
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="48"/>
+      <c r="AL18" s="48"/>
+      <c r="AM18" s="48"/>
+      <c r="AN18" s="48"/>
+      <c r="AO18" s="48"/>
+      <c r="AP18" s="48"/>
+      <c r="AQ18" s="48"/>
+      <c r="AR18" s="48"/>
+      <c r="AS18" s="48"/>
+      <c r="AT18" s="48"/>
+      <c r="AU18" s="48"/>
+      <c r="AV18" s="48"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -6193,7 +6816,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:V20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:W20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -6272,7 +6895,18 @@
         <f t="shared" si="0"/>
         <v>27656</v>
       </c>
-      <c r="W20" s="48"/>
+      <c r="W20" s="51">
+        <f t="shared" si="0"/>
+        <v>27894</v>
+      </c>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6517,32 +7151,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="217" t="s">
+      <c r="B8" s="230" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="217"/>
+      <c r="B9" s="230"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="217"/>
+      <c r="B10" s="230"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="217"/>
+      <c r="B11" s="230"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="218" t="s">
+      <c r="B12" s="231" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="218"/>
+      <c r="B13" s="231"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="218"/>
+      <c r="B14" s="231"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 23th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A25703-C478-1043-9D67-6199993CDE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E8BE76-0E10-B049-B621-331D7189933A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="235">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1196,17 +1196,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="12" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,6 +2300,38 @@
         <v>488550</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
+        <v>44005</v>
+      </c>
+      <c r="B24" s="233">
+        <v>191410</v>
+      </c>
+      <c r="C24" s="234">
+        <v>251355</v>
+      </c>
+      <c r="D24" s="235">
+        <v>59106</v>
+      </c>
+      <c r="E24" s="236">
+        <v>23377</v>
+      </c>
+      <c r="F24" s="237">
+        <v>31.598140118071154</v>
+      </c>
+      <c r="G24" s="238">
+        <v>60482</v>
+      </c>
+      <c r="H24" s="239">
+        <v>5219</v>
+      </c>
+      <c r="I24" s="240">
+        <v>5402</v>
+      </c>
+      <c r="J24" s="241">
+        <v>501871</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2282,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3100,17 +3159,39 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
+      <c r="A24" s="15">
+        <v>44005</v>
+      </c>
+      <c r="B24" s="48">
+        <v>0</v>
+      </c>
+      <c r="C24" s="48">
+        <v>1</v>
+      </c>
+      <c r="D24" s="48">
+        <v>1</v>
+      </c>
+      <c r="E24" s="48">
+        <v>1</v>
+      </c>
+      <c r="F24" s="48">
+        <v>1</v>
+      </c>
+      <c r="G24" s="48">
+        <v>0</v>
+      </c>
+      <c r="H24" s="48">
+        <v>0</v>
+      </c>
+      <c r="I24" s="48">
+        <v>1</v>
+      </c>
+      <c r="J24" s="48">
+        <v>0</v>
+      </c>
+      <c r="K24" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
@@ -3290,8 +3371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4238,19 +4319,45 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
+      <c r="A24" s="47">
+        <v>44005</v>
+      </c>
+      <c r="B24" s="48">
+        <v>0</v>
+      </c>
+      <c r="C24" s="48">
+        <v>1</v>
+      </c>
+      <c r="D24" s="48">
+        <v>1</v>
+      </c>
+      <c r="E24" s="48">
+        <v>0</v>
+      </c>
+      <c r="F24" s="48">
+        <v>1</v>
+      </c>
+      <c r="G24" s="48">
+        <v>1</v>
+      </c>
+      <c r="H24" s="48">
+        <v>1</v>
+      </c>
+      <c r="I24" s="48">
+        <v>0</v>
+      </c>
+      <c r="J24" s="48">
+        <v>1</v>
+      </c>
+      <c r="K24" s="48">
+        <v>1</v>
+      </c>
+      <c r="L24" s="48">
+        <v>0</v>
+      </c>
+      <c r="M24" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
@@ -4322,7 +4429,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5072,16 +5179,36 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="220"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
+      <c r="A24" s="47">
+        <v>44005</v>
+      </c>
+      <c r="B24" s="48">
+        <v>0</v>
+      </c>
+      <c r="C24" s="48">
+        <v>0</v>
+      </c>
+      <c r="D24" s="48">
+        <v>0</v>
+      </c>
+      <c r="E24" s="48">
+        <v>0</v>
+      </c>
+      <c r="F24" s="48">
+        <v>2</v>
+      </c>
+      <c r="G24" s="48">
+        <v>1</v>
+      </c>
+      <c r="H24" s="48">
+        <v>1</v>
+      </c>
+      <c r="I24" s="48">
+        <v>1</v>
+      </c>
+      <c r="J24" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="220"/>
@@ -5155,8 +5282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5228,13 +5355,15 @@
       <c r="U1" s="49">
         <v>44002</v>
       </c>
-      <c r="V1" s="232">
+      <c r="V1" s="230">
         <v>44003</v>
       </c>
       <c r="W1" s="49">
         <v>44004</v>
       </c>
-      <c r="X1" s="48"/>
+      <c r="X1" s="49">
+        <v>44005</v>
+      </c>
       <c r="Y1" s="48"/>
       <c r="Z1" s="48"/>
       <c r="AA1" s="48"/>
@@ -5324,13 +5453,15 @@
       <c r="U2" s="48">
         <v>3657</v>
       </c>
-      <c r="V2" s="233">
+      <c r="V2" s="231">
         <v>3689</v>
       </c>
-      <c r="W2" s="234">
+      <c r="W2" s="232">
         <v>3721</v>
       </c>
-      <c r="X2" s="48"/>
+      <c r="X2" s="48">
+        <v>3753</v>
+      </c>
       <c r="Y2" s="48"/>
       <c r="Z2" s="48"/>
       <c r="AA2" s="48"/>
@@ -5420,13 +5551,15 @@
       <c r="U3" s="48">
         <v>3472</v>
       </c>
-      <c r="V3" s="233">
+      <c r="V3" s="231">
         <v>3504</v>
       </c>
       <c r="W3" s="48">
         <v>3536</v>
       </c>
-      <c r="X3" s="48"/>
+      <c r="X3" s="48">
+        <v>3568</v>
+      </c>
       <c r="Y3" s="48"/>
       <c r="Z3" s="48"/>
       <c r="AA3" s="48"/>
@@ -5516,13 +5649,15 @@
       <c r="U4" s="48">
         <v>3472</v>
       </c>
-      <c r="V4" s="233">
+      <c r="V4" s="231">
         <v>3504</v>
       </c>
       <c r="W4" s="48">
         <v>3536</v>
       </c>
-      <c r="X4" s="48"/>
+      <c r="X4" s="48">
+        <v>3568</v>
+      </c>
       <c r="Y4" s="48"/>
       <c r="Z4" s="48"/>
       <c r="AA4" s="48"/>
@@ -5612,13 +5747,15 @@
       <c r="U5" s="48">
         <v>3472</v>
       </c>
-      <c r="V5" s="233">
+      <c r="V5" s="231">
         <v>3504</v>
       </c>
       <c r="W5" s="48">
         <v>3536</v>
       </c>
-      <c r="X5" s="48"/>
+      <c r="X5" s="48">
+        <v>3568</v>
+      </c>
       <c r="Y5" s="48"/>
       <c r="Z5" s="48"/>
       <c r="AA5" s="48"/>
@@ -5708,13 +5845,15 @@
       <c r="U6" s="48">
         <v>3472</v>
       </c>
-      <c r="V6" s="233">
+      <c r="V6" s="231">
         <v>3504</v>
       </c>
       <c r="W6" s="48">
         <v>3536</v>
       </c>
-      <c r="X6" s="48"/>
+      <c r="X6" s="48">
+        <v>3568</v>
+      </c>
       <c r="Y6" s="48"/>
       <c r="Z6" s="48"/>
       <c r="AA6" s="48"/>
@@ -5804,13 +5943,15 @@
       <c r="U7" s="48">
         <v>2663</v>
       </c>
-      <c r="V7" s="233">
+      <c r="V7" s="231">
         <v>2695</v>
       </c>
       <c r="W7" s="48">
         <v>2727</v>
       </c>
-      <c r="X7" s="48"/>
+      <c r="X7" s="48">
+        <v>2759</v>
+      </c>
       <c r="Y7" s="48"/>
       <c r="Z7" s="48"/>
       <c r="AA7" s="48"/>
@@ -5900,13 +6041,15 @@
       <c r="U8" s="48">
         <v>5294</v>
       </c>
-      <c r="V8" s="233">
+      <c r="V8" s="231">
         <v>5326</v>
       </c>
       <c r="W8" s="48">
         <v>5358</v>
       </c>
-      <c r="X8" s="48"/>
+      <c r="X8" s="48">
+        <v>5390</v>
+      </c>
       <c r="Y8" s="48"/>
       <c r="Z8" s="48"/>
       <c r="AA8" s="48"/>
@@ -6046,13 +6189,15 @@
       <c r="U10" s="48">
         <v>160</v>
       </c>
-      <c r="V10" s="233">
+      <c r="V10" s="231">
         <v>161</v>
       </c>
       <c r="W10" s="48">
         <v>162</v>
       </c>
-      <c r="X10" s="48"/>
+      <c r="X10" s="48">
+        <v>163</v>
+      </c>
       <c r="Y10" s="48"/>
       <c r="Z10" s="48"/>
       <c r="AA10" s="48"/>
@@ -6142,13 +6287,15 @@
       <c r="U11" s="48">
         <v>160</v>
       </c>
-      <c r="V11" s="233">
+      <c r="V11" s="231">
         <v>161</v>
       </c>
       <c r="W11" s="48">
         <v>162</v>
       </c>
-      <c r="X11" s="48"/>
+      <c r="X11" s="48">
+        <v>163</v>
+      </c>
       <c r="Y11" s="48"/>
       <c r="Z11" s="48"/>
       <c r="AA11" s="48"/>
@@ -6238,13 +6385,15 @@
       <c r="U12" s="48">
         <v>160</v>
       </c>
-      <c r="V12" s="233">
+      <c r="V12" s="231">
         <v>161</v>
       </c>
       <c r="W12" s="48">
         <v>162</v>
       </c>
-      <c r="X12" s="48"/>
+      <c r="X12" s="48">
+        <v>163</v>
+      </c>
       <c r="Y12" s="48"/>
       <c r="Z12" s="48"/>
       <c r="AA12" s="48"/>
@@ -6334,13 +6483,15 @@
       <c r="U13" s="48">
         <v>160</v>
       </c>
-      <c r="V13" s="233">
+      <c r="V13" s="231">
         <v>161</v>
       </c>
       <c r="W13" s="48">
         <v>162</v>
       </c>
-      <c r="X13" s="48"/>
+      <c r="X13" s="48">
+        <v>163</v>
+      </c>
       <c r="Y13" s="48"/>
       <c r="Z13" s="48"/>
       <c r="AA13" s="48"/>
@@ -6430,13 +6581,15 @@
       <c r="U14" s="48">
         <v>160</v>
       </c>
-      <c r="V14" s="233">
+      <c r="V14" s="231">
         <v>161</v>
       </c>
       <c r="W14" s="48">
         <v>162</v>
       </c>
-      <c r="X14" s="48"/>
+      <c r="X14" s="48">
+        <v>163</v>
+      </c>
       <c r="Y14" s="48"/>
       <c r="Z14" s="48"/>
       <c r="AA14" s="48"/>
@@ -6526,13 +6679,15 @@
       <c r="U15" s="48">
         <v>95</v>
       </c>
-      <c r="V15" s="233">
+      <c r="V15" s="231">
         <v>96</v>
       </c>
       <c r="W15" s="48">
         <v>97</v>
       </c>
-      <c r="X15" s="48"/>
+      <c r="X15" s="48">
+        <v>98</v>
+      </c>
       <c r="Y15" s="48"/>
       <c r="Z15" s="48"/>
       <c r="AA15" s="48"/>
@@ -6622,13 +6777,15 @@
       <c r="U16" s="48">
         <v>172</v>
       </c>
-      <c r="V16" s="233">
+      <c r="V16" s="231">
         <v>173</v>
       </c>
       <c r="W16" s="48">
         <v>174</v>
       </c>
-      <c r="X16" s="48"/>
+      <c r="X16" s="48">
+        <v>175</v>
+      </c>
       <c r="Y16" s="48"/>
       <c r="Z16" s="48"/>
       <c r="AA16" s="48"/>
@@ -6768,13 +6925,15 @@
       <c r="U18" s="48">
         <v>849</v>
       </c>
-      <c r="V18" s="233">
+      <c r="V18" s="231">
         <v>856</v>
       </c>
       <c r="W18" s="48">
         <v>863</v>
       </c>
-      <c r="X18" s="48"/>
+      <c r="X18" s="48">
+        <v>870</v>
+      </c>
       <c r="Y18" s="48"/>
       <c r="Z18" s="48"/>
       <c r="AA18" s="48"/>
@@ -6816,7 +6975,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:W20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:X20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -6899,7 +7058,10 @@
         <f t="shared" si="0"/>
         <v>27894</v>
       </c>
-      <c r="X20" s="48"/>
+      <c r="X20" s="51">
+        <f t="shared" si="0"/>
+        <v>28132</v>
+      </c>
       <c r="Y20" s="48"/>
       <c r="Z20" s="48"/>
       <c r="AA20" s="48"/>
@@ -7151,32 +7313,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="230" t="s">
+      <c r="B8" s="242" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="230"/>
+      <c r="B9" s="242"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="230"/>
+      <c r="B10" s="242"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="230"/>
+      <c r="B11" s="242"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="231" t="s">
+      <c r="B12" s="243" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="231"/>
+      <c r="B13" s="243"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="231"/>
+      <c r="B14" s="243"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Adding clean data by states and age groups.
Added a script called 02-wrangle-data-covid-ssa-mx-state-age-groups.R that creates clean data by states and age groups. Added a folder in data/state_age_groups where we will put csv and RData coming from that script.
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E8BE76-0E10-B049-B621-331D7189933A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE7C421-011E-3E4B-9ECF-9724BD31A422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2341,8 +2341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3371,8 +3372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4428,8 +4430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5282,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Remove data/states/*csv  from April to May
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE7C421-011E-3E4B-9ECF-9724BD31A422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ABB751-3D76-7A49-A390-38B909B8767F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2342,8 +2342,8 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3160,7 +3160,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="15">
+      <c r="A24" s="218">
         <v>44005</v>
       </c>
       <c r="B24" s="48">
@@ -3373,7 +3373,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4431,7 +4431,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -5285,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7233,7 +7233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding clean data by county containing ZMVM for June 23
The csv file couldn't be added because it is over 100 MB and GitHub did not hold it
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ABB751-3D76-7A49-A390-38B909B8767F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A3419B-9685-6F4B-B34B-DA9B0961C8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7082,8 +7082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7101,7 +7101,9 @@
       <c r="D1" s="38">
         <v>43986</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="38">
+        <v>44005</v>
+      </c>
       <c r="F1" s="38"/>
       <c r="G1" s="38"/>
       <c r="H1" s="38"/>
@@ -7119,6 +7121,9 @@
       <c r="D2">
         <v>74829</v>
       </c>
+      <c r="E2">
+        <v>117023</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -7133,6 +7138,9 @@
       <c r="D3">
         <v>67914</v>
       </c>
+      <c r="E3">
+        <v>108604</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
@@ -7147,6 +7155,9 @@
       <c r="D4">
         <v>67914</v>
       </c>
+      <c r="E4">
+        <v>108604</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -7161,6 +7172,9 @@
       <c r="D5">
         <v>67914</v>
       </c>
+      <c r="E5">
+        <v>108604</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
@@ -7175,6 +7189,9 @@
       <c r="D6">
         <v>67914</v>
       </c>
+      <c r="E6">
+        <v>108604</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
@@ -7189,6 +7206,9 @@
       <c r="D7">
         <v>31690</v>
       </c>
+      <c r="E7">
+        <v>57360</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
@@ -7203,6 +7223,9 @@
       <c r="D8">
         <v>129929</v>
       </c>
+      <c r="E8">
+        <v>178929</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -7222,6 +7245,10 @@
       <c r="D10">
         <f>SUM(D2:D8)</f>
         <v>508104</v>
+      </c>
+      <c r="E10">
+        <f>SUM(E2:E8)</f>
+        <v>787728</v>
       </c>
     </row>
   </sheetData>
@@ -7233,7 +7260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 24th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A3419B-9685-6F4B-B34B-DA9B0961C8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C1E6B8-155B-9E4A-A7FF-7568B5DF3CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1201,6 +1201,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1257,7 +1284,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1553,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2332,6 +2359,38 @@
         <v>501871</v>
       </c>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
+        <v>44006</v>
+      </c>
+      <c r="B25" s="242">
+        <v>196847</v>
+      </c>
+      <c r="C25" s="243">
+        <v>256336</v>
+      </c>
+      <c r="D25" s="244">
+        <v>62475</v>
+      </c>
+      <c r="E25" s="245">
+        <v>24324</v>
+      </c>
+      <c r="F25" s="246">
+        <v>31.576300375418469</v>
+      </c>
+      <c r="G25" s="247">
+        <v>62157</v>
+      </c>
+      <c r="H25" s="248">
+        <v>5350</v>
+      </c>
+      <c r="I25" s="249">
+        <v>5532</v>
+      </c>
+      <c r="J25" s="250">
+        <v>515658</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2342,8 +2401,8 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3195,17 +3254,39 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
+      <c r="A25" s="218">
+        <v>44006</v>
+      </c>
+      <c r="B25" s="48">
+        <v>0</v>
+      </c>
+      <c r="C25" s="48">
+        <v>1</v>
+      </c>
+      <c r="D25" s="48">
+        <v>1</v>
+      </c>
+      <c r="E25" s="48">
+        <v>1</v>
+      </c>
+      <c r="F25" s="48">
+        <v>1</v>
+      </c>
+      <c r="G25" s="48">
+        <v>0</v>
+      </c>
+      <c r="H25" s="48">
+        <v>0</v>
+      </c>
+      <c r="I25" s="48">
+        <v>1</v>
+      </c>
+      <c r="J25" s="48">
+        <v>0</v>
+      </c>
+      <c r="K25" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
@@ -3374,7 +3455,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4362,19 +4443,45 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
+      <c r="A25" s="47">
+        <v>44006</v>
+      </c>
+      <c r="B25" s="48">
+        <v>0</v>
+      </c>
+      <c r="C25" s="48">
+        <v>1</v>
+      </c>
+      <c r="D25" s="48">
+        <v>1</v>
+      </c>
+      <c r="E25" s="48">
+        <v>0</v>
+      </c>
+      <c r="F25" s="48">
+        <v>1</v>
+      </c>
+      <c r="G25" s="48">
+        <v>1</v>
+      </c>
+      <c r="H25" s="48">
+        <v>1</v>
+      </c>
+      <c r="I25" s="48">
+        <v>0</v>
+      </c>
+      <c r="J25" s="48">
+        <v>1</v>
+      </c>
+      <c r="K25" s="48">
+        <v>1</v>
+      </c>
+      <c r="L25" s="48">
+        <v>0</v>
+      </c>
+      <c r="M25" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
@@ -4431,8 +4538,8 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5214,16 +5321,36 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="220"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
+      <c r="A25" s="47">
+        <v>44006</v>
+      </c>
+      <c r="B25" s="48">
+        <v>0</v>
+      </c>
+      <c r="C25" s="48">
+        <v>0</v>
+      </c>
+      <c r="D25" s="48">
+        <v>0</v>
+      </c>
+      <c r="E25" s="48">
+        <v>0</v>
+      </c>
+      <c r="F25" s="48">
+        <v>2</v>
+      </c>
+      <c r="G25" s="48">
+        <v>1</v>
+      </c>
+      <c r="H25" s="48">
+        <v>1</v>
+      </c>
+      <c r="I25" s="48">
+        <v>1</v>
+      </c>
+      <c r="J25" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="220"/>
@@ -5285,8 +5412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5367,7 +5494,9 @@
       <c r="X1" s="49">
         <v>44005</v>
       </c>
-      <c r="Y1" s="48"/>
+      <c r="Y1" s="49">
+        <v>44006</v>
+      </c>
       <c r="Z1" s="48"/>
       <c r="AA1" s="48"/>
       <c r="AB1" s="48"/>
@@ -5465,7 +5594,9 @@
       <c r="X2" s="48">
         <v>3753</v>
       </c>
-      <c r="Y2" s="48"/>
+      <c r="Y2" s="48">
+        <v>3785</v>
+      </c>
       <c r="Z2" s="48"/>
       <c r="AA2" s="48"/>
       <c r="AB2" s="48"/>
@@ -5563,7 +5694,9 @@
       <c r="X3" s="48">
         <v>3568</v>
       </c>
-      <c r="Y3" s="48"/>
+      <c r="Y3" s="48">
+        <v>3600</v>
+      </c>
       <c r="Z3" s="48"/>
       <c r="AA3" s="48"/>
       <c r="AB3" s="48"/>
@@ -5661,7 +5794,9 @@
       <c r="X4" s="48">
         <v>3568</v>
       </c>
-      <c r="Y4" s="48"/>
+      <c r="Y4" s="48">
+        <v>3600</v>
+      </c>
       <c r="Z4" s="48"/>
       <c r="AA4" s="48"/>
       <c r="AB4" s="48"/>
@@ -5759,7 +5894,9 @@
       <c r="X5" s="48">
         <v>3568</v>
       </c>
-      <c r="Y5" s="48"/>
+      <c r="Y5" s="48">
+        <v>3600</v>
+      </c>
       <c r="Z5" s="48"/>
       <c r="AA5" s="48"/>
       <c r="AB5" s="48"/>
@@ -5857,7 +5994,9 @@
       <c r="X6" s="48">
         <v>3568</v>
       </c>
-      <c r="Y6" s="48"/>
+      <c r="Y6" s="48">
+        <v>3600</v>
+      </c>
       <c r="Z6" s="48"/>
       <c r="AA6" s="48"/>
       <c r="AB6" s="48"/>
@@ -5955,7 +6094,9 @@
       <c r="X7" s="48">
         <v>2759</v>
       </c>
-      <c r="Y7" s="48"/>
+      <c r="Y7" s="48">
+        <v>2791</v>
+      </c>
       <c r="Z7" s="48"/>
       <c r="AA7" s="48"/>
       <c r="AB7" s="48"/>
@@ -6053,7 +6194,9 @@
       <c r="X8" s="48">
         <v>5390</v>
       </c>
-      <c r="Y8" s="48"/>
+      <c r="Y8" s="48">
+        <v>5422</v>
+      </c>
       <c r="Z8" s="48"/>
       <c r="AA8" s="48"/>
       <c r="AB8" s="48"/>
@@ -6201,7 +6344,9 @@
       <c r="X10" s="48">
         <v>163</v>
       </c>
-      <c r="Y10" s="48"/>
+      <c r="Y10" s="48">
+        <v>164</v>
+      </c>
       <c r="Z10" s="48"/>
       <c r="AA10" s="48"/>
       <c r="AB10" s="48"/>
@@ -6299,7 +6444,9 @@
       <c r="X11" s="48">
         <v>163</v>
       </c>
-      <c r="Y11" s="48"/>
+      <c r="Y11" s="48">
+        <v>164</v>
+      </c>
       <c r="Z11" s="48"/>
       <c r="AA11" s="48"/>
       <c r="AB11" s="48"/>
@@ -6397,7 +6544,9 @@
       <c r="X12" s="48">
         <v>163</v>
       </c>
-      <c r="Y12" s="48"/>
+      <c r="Y12" s="48">
+        <v>164</v>
+      </c>
       <c r="Z12" s="48"/>
       <c r="AA12" s="48"/>
       <c r="AB12" s="48"/>
@@ -6495,7 +6644,9 @@
       <c r="X13" s="48">
         <v>163</v>
       </c>
-      <c r="Y13" s="48"/>
+      <c r="Y13" s="48">
+        <v>164</v>
+      </c>
       <c r="Z13" s="48"/>
       <c r="AA13" s="48"/>
       <c r="AB13" s="48"/>
@@ -6593,7 +6744,9 @@
       <c r="X14" s="48">
         <v>163</v>
       </c>
-      <c r="Y14" s="48"/>
+      <c r="Y14" s="48">
+        <v>164</v>
+      </c>
       <c r="Z14" s="48"/>
       <c r="AA14" s="48"/>
       <c r="AB14" s="48"/>
@@ -6691,7 +6844,9 @@
       <c r="X15" s="48">
         <v>98</v>
       </c>
-      <c r="Y15" s="48"/>
+      <c r="Y15" s="48">
+        <v>99</v>
+      </c>
       <c r="Z15" s="48"/>
       <c r="AA15" s="48"/>
       <c r="AB15" s="48"/>
@@ -6789,7 +6944,9 @@
       <c r="X16" s="48">
         <v>175</v>
       </c>
-      <c r="Y16" s="48"/>
+      <c r="Y16" s="48">
+        <v>176</v>
+      </c>
       <c r="Z16" s="48"/>
       <c r="AA16" s="48"/>
       <c r="AB16" s="48"/>
@@ -6937,7 +7094,9 @@
       <c r="X18" s="48">
         <v>870</v>
       </c>
-      <c r="Y18" s="48"/>
+      <c r="Y18" s="48">
+        <v>877</v>
+      </c>
       <c r="Z18" s="48"/>
       <c r="AA18" s="48"/>
       <c r="AB18" s="48"/>
@@ -6978,7 +7137,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:X20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:Y20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -7065,7 +7224,10 @@
         <f t="shared" si="0"/>
         <v>28132</v>
       </c>
-      <c r="Y20" s="48"/>
+      <c r="Y20" s="51">
+        <f t="shared" si="0"/>
+        <v>28370</v>
+      </c>
       <c r="Z20" s="48"/>
       <c r="AA20" s="48"/>
       <c r="AB20" s="48"/>
@@ -7082,7 +7244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7260,7 +7422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7343,32 +7505,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="242" t="s">
+      <c r="B8" s="251" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="242"/>
+      <c r="B9" s="251"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="242"/>
+      <c r="B10" s="251"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="242"/>
+      <c r="B11" s="251"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="243" t="s">
+      <c r="B12" s="252" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="243"/>
+      <c r="B13" s="252"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="243"/>
+      <c r="B14" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and Clean data from SSA for June 25th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C1E6B8-155B-9E4A-A7FF-7568B5DF3CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731DEF9A-4215-E045-A231-1BC5453E3608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="480" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="7280" yWindow="1440" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1201,6 +1201,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1580,10 +1607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,6 +2416,38 @@
       </c>
       <c r="J25" s="250">
         <v>515658</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <v>44007</v>
+      </c>
+      <c r="B26" s="251">
+        <v>202951</v>
+      </c>
+      <c r="C26" s="252">
+        <v>262117</v>
+      </c>
+      <c r="D26" s="253">
+        <v>63583</v>
+      </c>
+      <c r="E26" s="254">
+        <v>25060</v>
+      </c>
+      <c r="F26" s="255">
+        <v>31.457839577040765</v>
+      </c>
+      <c r="G26" s="256">
+        <v>63844</v>
+      </c>
+      <c r="H26" s="257">
+        <v>5483</v>
+      </c>
+      <c r="I26" s="258">
+        <v>5681</v>
+      </c>
+      <c r="J26" s="259">
+        <v>528651</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3289,17 +3348,39 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
+      <c r="A26" s="218">
+        <v>44007</v>
+      </c>
+      <c r="B26" s="48">
+        <v>0</v>
+      </c>
+      <c r="C26" s="48">
+        <v>1</v>
+      </c>
+      <c r="D26" s="48">
+        <v>1</v>
+      </c>
+      <c r="E26" s="48">
+        <v>1</v>
+      </c>
+      <c r="F26" s="48">
+        <v>1</v>
+      </c>
+      <c r="G26" s="48">
+        <v>0</v>
+      </c>
+      <c r="H26" s="48">
+        <v>0</v>
+      </c>
+      <c r="I26" s="48">
+        <v>1</v>
+      </c>
+      <c r="J26" s="48">
+        <v>0</v>
+      </c>
+      <c r="K26" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
@@ -3455,7 +3536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4484,19 +4565,45 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
+      <c r="A26" s="47">
+        <v>44007</v>
+      </c>
+      <c r="B26" s="48">
+        <v>0</v>
+      </c>
+      <c r="C26" s="48">
+        <v>1</v>
+      </c>
+      <c r="D26" s="48">
+        <v>1</v>
+      </c>
+      <c r="E26" s="48">
+        <v>0</v>
+      </c>
+      <c r="F26" s="48">
+        <v>1</v>
+      </c>
+      <c r="G26" s="48">
+        <v>1</v>
+      </c>
+      <c r="H26" s="48">
+        <v>1</v>
+      </c>
+      <c r="I26" s="48">
+        <v>0</v>
+      </c>
+      <c r="J26" s="48">
+        <v>1</v>
+      </c>
+      <c r="K26" s="48">
+        <v>1</v>
+      </c>
+      <c r="L26" s="48">
+        <v>0</v>
+      </c>
+      <c r="M26" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
@@ -4539,7 +4646,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5353,16 +5460,36 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="220"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
+      <c r="A26" s="47">
+        <v>44007</v>
+      </c>
+      <c r="B26" s="48">
+        <v>0</v>
+      </c>
+      <c r="C26" s="48">
+        <v>0</v>
+      </c>
+      <c r="D26" s="48">
+        <v>0</v>
+      </c>
+      <c r="E26" s="48">
+        <v>0</v>
+      </c>
+      <c r="F26" s="48">
+        <v>2</v>
+      </c>
+      <c r="G26" s="48">
+        <v>1</v>
+      </c>
+      <c r="H26" s="48">
+        <v>1</v>
+      </c>
+      <c r="I26" s="48">
+        <v>1</v>
+      </c>
+      <c r="J26" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="220"/>
@@ -5413,7 +5540,7 @@
   <dimension ref="A1:AV20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5497,7 +5624,9 @@
       <c r="Y1" s="49">
         <v>44006</v>
       </c>
-      <c r="Z1" s="48"/>
+      <c r="Z1" s="49">
+        <v>44007</v>
+      </c>
       <c r="AA1" s="48"/>
       <c r="AB1" s="48"/>
       <c r="AC1" s="48"/>
@@ -5597,7 +5726,9 @@
       <c r="Y2" s="48">
         <v>3785</v>
       </c>
-      <c r="Z2" s="48"/>
+      <c r="Z2" s="48">
+        <v>3817</v>
+      </c>
       <c r="AA2" s="48"/>
       <c r="AB2" s="48"/>
       <c r="AC2" s="48"/>
@@ -5697,7 +5828,9 @@
       <c r="Y3" s="48">
         <v>3600</v>
       </c>
-      <c r="Z3" s="48"/>
+      <c r="Z3" s="48">
+        <v>3632</v>
+      </c>
       <c r="AA3" s="48"/>
       <c r="AB3" s="48"/>
       <c r="AC3" s="48"/>
@@ -5797,7 +5930,9 @@
       <c r="Y4" s="48">
         <v>3600</v>
       </c>
-      <c r="Z4" s="48"/>
+      <c r="Z4" s="48">
+        <v>3632</v>
+      </c>
       <c r="AA4" s="48"/>
       <c r="AB4" s="48"/>
       <c r="AC4" s="48"/>
@@ -5897,7 +6032,9 @@
       <c r="Y5" s="48">
         <v>3600</v>
       </c>
-      <c r="Z5" s="48"/>
+      <c r="Z5" s="48">
+        <v>3632</v>
+      </c>
       <c r="AA5" s="48"/>
       <c r="AB5" s="48"/>
       <c r="AC5" s="48"/>
@@ -5997,7 +6134,9 @@
       <c r="Y6" s="48">
         <v>3600</v>
       </c>
-      <c r="Z6" s="48"/>
+      <c r="Z6" s="48">
+        <v>3632</v>
+      </c>
       <c r="AA6" s="48"/>
       <c r="AB6" s="48"/>
       <c r="AC6" s="48"/>
@@ -6097,7 +6236,9 @@
       <c r="Y7" s="48">
         <v>2791</v>
       </c>
-      <c r="Z7" s="48"/>
+      <c r="Z7" s="48">
+        <v>2823</v>
+      </c>
       <c r="AA7" s="48"/>
       <c r="AB7" s="48"/>
       <c r="AC7" s="48"/>
@@ -6197,7 +6338,9 @@
       <c r="Y8" s="48">
         <v>5422</v>
       </c>
-      <c r="Z8" s="48"/>
+      <c r="Z8" s="48">
+        <v>5454</v>
+      </c>
       <c r="AA8" s="48"/>
       <c r="AB8" s="48"/>
       <c r="AC8" s="48"/>
@@ -6347,7 +6490,9 @@
       <c r="Y10" s="48">
         <v>164</v>
       </c>
-      <c r="Z10" s="48"/>
+      <c r="Z10" s="48">
+        <v>165</v>
+      </c>
       <c r="AA10" s="48"/>
       <c r="AB10" s="48"/>
       <c r="AC10" s="48"/>
@@ -6447,7 +6592,9 @@
       <c r="Y11" s="48">
         <v>164</v>
       </c>
-      <c r="Z11" s="48"/>
+      <c r="Z11" s="48">
+        <v>165</v>
+      </c>
       <c r="AA11" s="48"/>
       <c r="AB11" s="48"/>
       <c r="AC11" s="48"/>
@@ -6547,7 +6694,9 @@
       <c r="Y12" s="48">
         <v>164</v>
       </c>
-      <c r="Z12" s="48"/>
+      <c r="Z12" s="48">
+        <v>165</v>
+      </c>
       <c r="AA12" s="48"/>
       <c r="AB12" s="48"/>
       <c r="AC12" s="48"/>
@@ -6647,7 +6796,9 @@
       <c r="Y13" s="48">
         <v>164</v>
       </c>
-      <c r="Z13" s="48"/>
+      <c r="Z13" s="48">
+        <v>165</v>
+      </c>
       <c r="AA13" s="48"/>
       <c r="AB13" s="48"/>
       <c r="AC13" s="48"/>
@@ -6747,7 +6898,9 @@
       <c r="Y14" s="48">
         <v>164</v>
       </c>
-      <c r="Z14" s="48"/>
+      <c r="Z14" s="48">
+        <v>165</v>
+      </c>
       <c r="AA14" s="48"/>
       <c r="AB14" s="48"/>
       <c r="AC14" s="48"/>
@@ -6847,7 +7000,9 @@
       <c r="Y15" s="48">
         <v>99</v>
       </c>
-      <c r="Z15" s="48"/>
+      <c r="Z15" s="48">
+        <v>100</v>
+      </c>
       <c r="AA15" s="48"/>
       <c r="AB15" s="48"/>
       <c r="AC15" s="48"/>
@@ -6947,7 +7102,9 @@
       <c r="Y16" s="48">
         <v>176</v>
       </c>
-      <c r="Z16" s="48"/>
+      <c r="Z16" s="48">
+        <v>177</v>
+      </c>
       <c r="AA16" s="48"/>
       <c r="AB16" s="48"/>
       <c r="AC16" s="48"/>
@@ -7097,7 +7254,9 @@
       <c r="Y18" s="48">
         <v>877</v>
       </c>
-      <c r="Z18" s="48"/>
+      <c r="Z18" s="48">
+        <v>884</v>
+      </c>
       <c r="AA18" s="48"/>
       <c r="AB18" s="48"/>
       <c r="AC18" s="48"/>
@@ -7137,7 +7296,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:Y20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:Z20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -7228,7 +7387,10 @@
         <f t="shared" si="0"/>
         <v>28370</v>
       </c>
-      <c r="Z20" s="48"/>
+      <c r="Z20" s="51">
+        <f t="shared" si="0"/>
+        <v>28608</v>
+      </c>
       <c r="AA20" s="48"/>
       <c r="AB20" s="48"/>
       <c r="AC20" s="48"/>
@@ -7422,7 +7584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7505,32 +7667,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="251" t="s">
+      <c r="B8" s="260" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="251"/>
+      <c r="B9" s="260"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="251"/>
+      <c r="B10" s="260"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="251"/>
+      <c r="B11" s="260"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="252" t="s">
+      <c r="B12" s="261" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="252"/>
+      <c r="B13" s="261"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="252"/>
+      <c r="B14" s="261"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 26th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731DEF9A-4215-E045-A231-1BC5453E3608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D002A2-0AB0-344F-AD9E-24F16915D846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="1440" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="262">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1201,6 +1201,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1607,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2448,6 +2475,38 @@
       </c>
       <c r="J26" s="259">
         <v>528651</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
+        <v>44008</v>
+      </c>
+      <c r="B27" s="260">
+        <v>208392</v>
+      </c>
+      <c r="C27" s="261">
+        <v>267288</v>
+      </c>
+      <c r="D27" s="262">
+        <v>66440</v>
+      </c>
+      <c r="E27" s="263">
+        <v>25779</v>
+      </c>
+      <c r="F27" s="264">
+        <v>31.374524933778648</v>
+      </c>
+      <c r="G27" s="265">
+        <v>65382</v>
+      </c>
+      <c r="H27" s="266">
+        <v>5570</v>
+      </c>
+      <c r="I27" s="267">
+        <v>5844</v>
+      </c>
+      <c r="J27" s="268">
+        <v>542120</v>
       </c>
     </row>
   </sheetData>
@@ -2461,7 +2520,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3383,17 +3442,39 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="48"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
+      <c r="A27" s="218">
+        <v>44008</v>
+      </c>
+      <c r="B27" s="48">
+        <v>0</v>
+      </c>
+      <c r="C27" s="48">
+        <v>1</v>
+      </c>
+      <c r="D27" s="48">
+        <v>1</v>
+      </c>
+      <c r="E27" s="48">
+        <v>1</v>
+      </c>
+      <c r="F27" s="48">
+        <v>1</v>
+      </c>
+      <c r="G27" s="48">
+        <v>0</v>
+      </c>
+      <c r="H27" s="48">
+        <v>0</v>
+      </c>
+      <c r="I27" s="48">
+        <v>1</v>
+      </c>
+      <c r="J27" s="48">
+        <v>0</v>
+      </c>
+      <c r="K27" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="48"/>
@@ -3536,7 +3617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4606,19 +4687,45 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="48"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
+      <c r="A27" s="47">
+        <v>44008</v>
+      </c>
+      <c r="B27" s="48">
+        <v>0</v>
+      </c>
+      <c r="C27" s="48">
+        <v>1</v>
+      </c>
+      <c r="D27" s="48">
+        <v>1</v>
+      </c>
+      <c r="E27" s="48">
+        <v>0</v>
+      </c>
+      <c r="F27" s="48">
+        <v>1</v>
+      </c>
+      <c r="G27" s="48">
+        <v>1</v>
+      </c>
+      <c r="H27" s="48">
+        <v>1</v>
+      </c>
+      <c r="I27" s="48">
+        <v>0</v>
+      </c>
+      <c r="J27" s="48">
+        <v>1</v>
+      </c>
+      <c r="K27" s="48">
+        <v>1</v>
+      </c>
+      <c r="L27" s="48">
+        <v>0</v>
+      </c>
+      <c r="M27" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="48"/>
@@ -4646,7 +4753,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5492,16 +5599,36 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="220"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
+      <c r="A27" s="47">
+        <v>44008</v>
+      </c>
+      <c r="B27" s="48">
+        <v>0</v>
+      </c>
+      <c r="C27" s="48">
+        <v>0</v>
+      </c>
+      <c r="D27" s="48">
+        <v>0</v>
+      </c>
+      <c r="E27" s="48">
+        <v>0</v>
+      </c>
+      <c r="F27" s="48">
+        <v>2</v>
+      </c>
+      <c r="G27" s="48">
+        <v>1</v>
+      </c>
+      <c r="H27" s="48">
+        <v>1</v>
+      </c>
+      <c r="I27" s="48">
+        <v>1</v>
+      </c>
+      <c r="J27" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="220"/>
@@ -5539,8 +5666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5627,7 +5754,9 @@
       <c r="Z1" s="49">
         <v>44007</v>
       </c>
-      <c r="AA1" s="48"/>
+      <c r="AA1" s="49">
+        <v>44008</v>
+      </c>
       <c r="AB1" s="48"/>
       <c r="AC1" s="48"/>
       <c r="AD1" s="48"/>
@@ -5729,7 +5858,9 @@
       <c r="Z2" s="48">
         <v>3817</v>
       </c>
-      <c r="AA2" s="48"/>
+      <c r="AA2" s="48">
+        <v>3849</v>
+      </c>
       <c r="AB2" s="48"/>
       <c r="AC2" s="48"/>
       <c r="AD2" s="48"/>
@@ -5831,7 +5962,9 @@
       <c r="Z3" s="48">
         <v>3632</v>
       </c>
-      <c r="AA3" s="48"/>
+      <c r="AA3" s="48">
+        <v>3664</v>
+      </c>
       <c r="AB3" s="48"/>
       <c r="AC3" s="48"/>
       <c r="AD3" s="48"/>
@@ -5933,7 +6066,9 @@
       <c r="Z4" s="48">
         <v>3632</v>
       </c>
-      <c r="AA4" s="48"/>
+      <c r="AA4" s="48">
+        <v>3664</v>
+      </c>
       <c r="AB4" s="48"/>
       <c r="AC4" s="48"/>
       <c r="AD4" s="48"/>
@@ -6035,7 +6170,9 @@
       <c r="Z5" s="48">
         <v>3632</v>
       </c>
-      <c r="AA5" s="48"/>
+      <c r="AA5" s="48">
+        <v>3664</v>
+      </c>
       <c r="AB5" s="48"/>
       <c r="AC5" s="48"/>
       <c r="AD5" s="48"/>
@@ -6137,7 +6274,9 @@
       <c r="Z6" s="48">
         <v>3632</v>
       </c>
-      <c r="AA6" s="48"/>
+      <c r="AA6" s="48">
+        <v>3664</v>
+      </c>
       <c r="AB6" s="48"/>
       <c r="AC6" s="48"/>
       <c r="AD6" s="48"/>
@@ -6239,7 +6378,9 @@
       <c r="Z7" s="48">
         <v>2823</v>
       </c>
-      <c r="AA7" s="48"/>
+      <c r="AA7" s="48">
+        <v>2855</v>
+      </c>
       <c r="AB7" s="48"/>
       <c r="AC7" s="48"/>
       <c r="AD7" s="48"/>
@@ -6341,7 +6482,9 @@
       <c r="Z8" s="48">
         <v>5454</v>
       </c>
-      <c r="AA8" s="48"/>
+      <c r="AA8" s="48">
+        <v>5486</v>
+      </c>
       <c r="AB8" s="48"/>
       <c r="AC8" s="48"/>
       <c r="AD8" s="48"/>
@@ -6493,7 +6636,9 @@
       <c r="Z10" s="48">
         <v>165</v>
       </c>
-      <c r="AA10" s="48"/>
+      <c r="AA10" s="48">
+        <v>166</v>
+      </c>
       <c r="AB10" s="48"/>
       <c r="AC10" s="48"/>
       <c r="AD10" s="48"/>
@@ -6595,7 +6740,9 @@
       <c r="Z11" s="48">
         <v>165</v>
       </c>
-      <c r="AA11" s="48"/>
+      <c r="AA11" s="48">
+        <v>166</v>
+      </c>
       <c r="AB11" s="48"/>
       <c r="AC11" s="48"/>
       <c r="AD11" s="48"/>
@@ -6697,7 +6844,9 @@
       <c r="Z12" s="48">
         <v>165</v>
       </c>
-      <c r="AA12" s="48"/>
+      <c r="AA12" s="48">
+        <v>166</v>
+      </c>
       <c r="AB12" s="48"/>
       <c r="AC12" s="48"/>
       <c r="AD12" s="48"/>
@@ -6799,7 +6948,9 @@
       <c r="Z13" s="48">
         <v>165</v>
       </c>
-      <c r="AA13" s="48"/>
+      <c r="AA13" s="48">
+        <v>166</v>
+      </c>
       <c r="AB13" s="48"/>
       <c r="AC13" s="48"/>
       <c r="AD13" s="48"/>
@@ -6901,7 +7052,9 @@
       <c r="Z14" s="48">
         <v>165</v>
       </c>
-      <c r="AA14" s="48"/>
+      <c r="AA14" s="48">
+        <v>166</v>
+      </c>
       <c r="AB14" s="48"/>
       <c r="AC14" s="48"/>
       <c r="AD14" s="48"/>
@@ -7003,7 +7156,9 @@
       <c r="Z15" s="48">
         <v>100</v>
       </c>
-      <c r="AA15" s="48"/>
+      <c r="AA15" s="48">
+        <v>101</v>
+      </c>
       <c r="AB15" s="48"/>
       <c r="AC15" s="48"/>
       <c r="AD15" s="48"/>
@@ -7105,7 +7260,9 @@
       <c r="Z16" s="48">
         <v>177</v>
       </c>
-      <c r="AA16" s="48"/>
+      <c r="AA16" s="48">
+        <v>178</v>
+      </c>
       <c r="AB16" s="48"/>
       <c r="AC16" s="48"/>
       <c r="AD16" s="48"/>
@@ -7257,7 +7414,9 @@
       <c r="Z18" s="48">
         <v>884</v>
       </c>
-      <c r="AA18" s="48"/>
+      <c r="AA18" s="48">
+        <v>891</v>
+      </c>
       <c r="AB18" s="48"/>
       <c r="AC18" s="48"/>
       <c r="AD18" s="48"/>
@@ -7296,7 +7455,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:Z20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AA20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -7391,7 +7550,10 @@
         <f t="shared" si="0"/>
         <v>28608</v>
       </c>
-      <c r="AA20" s="48"/>
+      <c r="AA20" s="51">
+        <f t="shared" si="0"/>
+        <v>28846</v>
+      </c>
       <c r="AB20" s="48"/>
       <c r="AC20" s="48"/>
       <c r="AD20" s="48"/>
@@ -7407,7 +7569,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7667,32 +7829,32 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="260" t="s">
+      <c r="B8" s="269" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="260"/>
+      <c r="B9" s="269"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="260"/>
+      <c r="B10" s="269"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="260"/>
+      <c r="B11" s="269"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="261" t="s">
+      <c r="B12" s="270" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="261"/>
+      <c r="B13" s="270"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="261"/>
+      <c r="B14" s="270"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Raw and clean data from SSA for June 27th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D002A2-0AB0-344F-AD9E-24F16915D846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E77ACA-3919-1342-907F-E68701B2AC3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>En serie de defunciones el día 14 de junio, la serie comenzó el 6 de marzo, el día 15 de junio comenzó el 18 de marzo; lo cual es una diferencia de 11 días es decir 11 observaciones.</t>
+  </si>
+  <si>
+    <t>27 de junio</t>
+  </si>
+  <si>
+    <t>Se agrego una nueva fecha a la serie de dates_dx, dates_sx el con fecha del 5 de febrero</t>
   </si>
 </sst>
 </file>
@@ -551,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="280">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1168,7 +1174,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1309,11 +1314,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1634,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2353,31 +2388,31 @@
       <c r="A23" s="15">
         <v>44004</v>
       </c>
-      <c r="B23" s="221">
+      <c r="B23" s="220">
         <v>185122</v>
       </c>
-      <c r="C23" s="222">
+      <c r="C23" s="221">
         <v>246147</v>
       </c>
-      <c r="D23" s="223">
+      <c r="D23" s="222">
         <v>57281</v>
       </c>
-      <c r="E23" s="224">
+      <c r="E23" s="223">
         <v>22584</v>
       </c>
-      <c r="F23" s="225">
+      <c r="F23" s="224">
         <v>31.687751860934949</v>
       </c>
-      <c r="G23" s="226">
+      <c r="G23" s="225">
         <v>58661</v>
       </c>
-      <c r="H23" s="227">
+      <c r="H23" s="226">
         <v>5112</v>
       </c>
-      <c r="I23" s="228">
+      <c r="I23" s="227">
         <v>5280</v>
       </c>
-      <c r="J23" s="229">
+      <c r="J23" s="228">
         <v>488550</v>
       </c>
     </row>
@@ -2385,31 +2420,31 @@
       <c r="A24" s="15">
         <v>44005</v>
       </c>
-      <c r="B24" s="233">
+      <c r="B24" s="232">
         <v>191410</v>
       </c>
-      <c r="C24" s="234">
+      <c r="C24" s="233">
         <v>251355</v>
       </c>
-      <c r="D24" s="235">
+      <c r="D24" s="234">
         <v>59106</v>
       </c>
-      <c r="E24" s="236">
+      <c r="E24" s="235">
         <v>23377</v>
       </c>
-      <c r="F24" s="237">
+      <c r="F24" s="236">
         <v>31.598140118071154</v>
       </c>
-      <c r="G24" s="238">
+      <c r="G24" s="237">
         <v>60482</v>
       </c>
-      <c r="H24" s="239">
+      <c r="H24" s="238">
         <v>5219</v>
       </c>
-      <c r="I24" s="240">
+      <c r="I24" s="239">
         <v>5402</v>
       </c>
-      <c r="J24" s="241">
+      <c r="J24" s="240">
         <v>501871</v>
       </c>
     </row>
@@ -2417,31 +2452,31 @@
       <c r="A25" s="15">
         <v>44006</v>
       </c>
-      <c r="B25" s="242">
+      <c r="B25" s="241">
         <v>196847</v>
       </c>
-      <c r="C25" s="243">
+      <c r="C25" s="242">
         <v>256336</v>
       </c>
-      <c r="D25" s="244">
+      <c r="D25" s="243">
         <v>62475</v>
       </c>
-      <c r="E25" s="245">
+      <c r="E25" s="244">
         <v>24324</v>
       </c>
-      <c r="F25" s="246">
+      <c r="F25" s="245">
         <v>31.576300375418469</v>
       </c>
-      <c r="G25" s="247">
+      <c r="G25" s="246">
         <v>62157</v>
       </c>
-      <c r="H25" s="248">
+      <c r="H25" s="247">
         <v>5350</v>
       </c>
-      <c r="I25" s="249">
+      <c r="I25" s="248">
         <v>5532</v>
       </c>
-      <c r="J25" s="250">
+      <c r="J25" s="249">
         <v>515658</v>
       </c>
     </row>
@@ -2449,31 +2484,31 @@
       <c r="A26" s="15">
         <v>44007</v>
       </c>
-      <c r="B26" s="251">
+      <c r="B26" s="250">
         <v>202951</v>
       </c>
-      <c r="C26" s="252">
+      <c r="C26" s="251">
         <v>262117</v>
       </c>
-      <c r="D26" s="253">
+      <c r="D26" s="252">
         <v>63583</v>
       </c>
-      <c r="E26" s="254">
+      <c r="E26" s="253">
         <v>25060</v>
       </c>
-      <c r="F26" s="255">
+      <c r="F26" s="254">
         <v>31.457839577040765</v>
       </c>
-      <c r="G26" s="256">
+      <c r="G26" s="255">
         <v>63844</v>
       </c>
-      <c r="H26" s="257">
+      <c r="H26" s="256">
         <v>5483</v>
       </c>
-      <c r="I26" s="258">
+      <c r="I26" s="257">
         <v>5681</v>
       </c>
-      <c r="J26" s="259">
+      <c r="J26" s="258">
         <v>528651</v>
       </c>
     </row>
@@ -2481,32 +2516,64 @@
       <c r="A27" s="15">
         <v>44008</v>
       </c>
-      <c r="B27" s="260">
+      <c r="B27" s="259">
         <v>208392</v>
       </c>
-      <c r="C27" s="261">
+      <c r="C27" s="260">
         <v>267288</v>
       </c>
-      <c r="D27" s="262">
+      <c r="D27" s="261">
         <v>66440</v>
       </c>
-      <c r="E27" s="263">
+      <c r="E27" s="262">
         <v>25779</v>
       </c>
-      <c r="F27" s="264">
+      <c r="F27" s="263">
         <v>31.374524933778648</v>
       </c>
-      <c r="G27" s="265">
+      <c r="G27" s="264">
         <v>65382</v>
       </c>
-      <c r="H27" s="266">
+      <c r="H27" s="265">
         <v>5570</v>
       </c>
-      <c r="I27" s="267">
+      <c r="I27" s="266">
         <v>5844</v>
       </c>
-      <c r="J27" s="268">
+      <c r="J27" s="267">
         <v>542120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
+        <v>44009</v>
+      </c>
+      <c r="B28" s="268">
+        <v>212802</v>
+      </c>
+      <c r="C28" s="269">
+        <v>271151</v>
+      </c>
+      <c r="D28" s="270">
+        <v>67099</v>
+      </c>
+      <c r="E28" s="271">
+        <v>26381</v>
+      </c>
+      <c r="F28" s="272">
+        <v>31.241247732634093</v>
+      </c>
+      <c r="G28" s="273">
+        <v>66482</v>
+      </c>
+      <c r="H28" s="274">
+        <v>5661</v>
+      </c>
+      <c r="I28" s="275">
+        <v>6361</v>
+      </c>
+      <c r="J28" s="276">
+        <v>551052</v>
       </c>
     </row>
   </sheetData>
@@ -2516,11 +2583,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2531,7 +2598,7 @@
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -2554,19 +2621,22 @@
         <v>5</v>
       </c>
       <c r="H1" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="47">
         <v>43983</v>
       </c>
@@ -2588,20 +2658,21 @@
       <c r="G2" s="48">
         <v>0</v>
       </c>
-      <c r="H2" s="48">
-        <v>0</v>
-      </c>
+      <c r="H2" s="48"/>
       <c r="I2" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="48">
+        <v>0</v>
+      </c>
+      <c r="L2" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="47">
         <v>43984</v>
       </c>
@@ -2623,20 +2694,21 @@
       <c r="G3" s="48">
         <v>0</v>
       </c>
-      <c r="H3" s="48">
-        <v>0</v>
-      </c>
+      <c r="H3" s="48"/>
       <c r="I3" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="48">
+        <v>0</v>
+      </c>
+      <c r="L3" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="47">
         <v>43985</v>
       </c>
@@ -2658,20 +2730,21 @@
       <c r="G4" s="48">
         <v>0</v>
       </c>
-      <c r="H4" s="48">
-        <v>0</v>
-      </c>
+      <c r="H4" s="48"/>
       <c r="I4" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="48">
+        <v>0</v>
+      </c>
+      <c r="L4" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="47">
         <v>43986</v>
       </c>
@@ -2693,20 +2766,21 @@
       <c r="G5" s="48">
         <v>0</v>
       </c>
-      <c r="H5" s="48">
-        <v>0</v>
-      </c>
+      <c r="H5" s="48"/>
       <c r="I5" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="48">
+        <v>0</v>
+      </c>
+      <c r="L5" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="47">
         <v>43987</v>
       </c>
@@ -2728,20 +2802,21 @@
       <c r="G6" s="48">
         <v>0</v>
       </c>
-      <c r="H6" s="48">
-        <v>0</v>
-      </c>
+      <c r="H6" s="48"/>
       <c r="I6" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="48">
+        <v>0</v>
+      </c>
+      <c r="L6" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="47">
         <v>43988</v>
       </c>
@@ -2763,20 +2838,21 @@
       <c r="G7" s="48">
         <v>0</v>
       </c>
-      <c r="H7" s="48">
-        <v>0</v>
-      </c>
+      <c r="H7" s="48"/>
       <c r="I7" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="48">
+        <v>0</v>
+      </c>
+      <c r="L7" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
         <v>43989</v>
       </c>
@@ -2798,20 +2874,21 @@
       <c r="G8" s="48">
         <v>0</v>
       </c>
-      <c r="H8" s="48">
-        <v>0</v>
-      </c>
+      <c r="H8" s="48"/>
       <c r="I8" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="48">
+        <v>0</v>
+      </c>
+      <c r="L8" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="47">
         <v>43990</v>
       </c>
@@ -2833,20 +2910,21 @@
       <c r="G9" s="48">
         <v>0</v>
       </c>
-      <c r="H9" s="48">
-        <v>0</v>
-      </c>
+      <c r="H9" s="48"/>
       <c r="I9" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="48">
+        <v>0</v>
+      </c>
+      <c r="L9" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="47">
         <v>43991</v>
       </c>
@@ -2868,20 +2946,21 @@
       <c r="G10" s="48">
         <v>0</v>
       </c>
-      <c r="H10" s="48">
-        <v>0</v>
-      </c>
+      <c r="H10" s="48"/>
       <c r="I10" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="48">
+        <v>0</v>
+      </c>
+      <c r="L10" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="47">
         <v>43992</v>
       </c>
@@ -2903,20 +2982,21 @@
       <c r="G11" s="48">
         <v>0</v>
       </c>
-      <c r="H11" s="48">
-        <v>0</v>
-      </c>
+      <c r="H11" s="48"/>
       <c r="I11" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="48">
+        <v>0</v>
+      </c>
+      <c r="L11" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="47">
         <v>43993</v>
       </c>
@@ -2938,20 +3018,21 @@
       <c r="G12" s="48">
         <v>0</v>
       </c>
-      <c r="H12" s="48">
-        <v>0</v>
-      </c>
+      <c r="H12" s="48"/>
       <c r="I12" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="48">
+        <v>0</v>
+      </c>
+      <c r="L12" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="47">
         <v>43994</v>
       </c>
@@ -2973,20 +3054,21 @@
       <c r="G13" s="48">
         <v>0</v>
       </c>
-      <c r="H13" s="48">
-        <v>0</v>
-      </c>
+      <c r="H13" s="48"/>
       <c r="I13" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="48">
+        <v>0</v>
+      </c>
+      <c r="L13" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="47">
         <v>43995</v>
       </c>
@@ -3008,20 +3090,21 @@
       <c r="G14" s="48">
         <v>0</v>
       </c>
-      <c r="H14" s="48">
-        <v>0</v>
-      </c>
+      <c r="H14" s="48"/>
       <c r="I14" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="48">
+        <v>0</v>
+      </c>
+      <c r="L14" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="47">
         <v>43996</v>
       </c>
@@ -3043,20 +3126,21 @@
       <c r="G15" s="48">
         <v>0</v>
       </c>
-      <c r="H15" s="48">
-        <v>0</v>
-      </c>
+      <c r="H15" s="48"/>
       <c r="I15" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="48">
+        <v>0</v>
+      </c>
+      <c r="L15" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="47">
         <v>43997</v>
       </c>
@@ -3078,20 +3162,21 @@
       <c r="G16" s="48">
         <v>0</v>
       </c>
-      <c r="H16" s="48">
-        <v>0</v>
-      </c>
+      <c r="H16" s="48"/>
       <c r="I16" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="48">
+        <v>0</v>
+      </c>
+      <c r="L16" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="47">
         <v>43998</v>
       </c>
@@ -3113,20 +3198,21 @@
       <c r="G17" s="48">
         <v>0</v>
       </c>
-      <c r="H17" s="48">
-        <v>0</v>
-      </c>
+      <c r="H17" s="48"/>
       <c r="I17" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="48">
+        <v>0</v>
+      </c>
+      <c r="L17" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="47">
         <v>43999</v>
       </c>
@@ -3148,20 +3234,21 @@
       <c r="G18" s="48">
         <v>0</v>
       </c>
-      <c r="H18" s="48">
-        <v>0</v>
-      </c>
+      <c r="H18" s="48"/>
       <c r="I18" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="48">
+        <v>0</v>
+      </c>
+      <c r="L18" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="47">
         <v>44000</v>
       </c>
@@ -3183,20 +3270,21 @@
       <c r="G19" s="48">
         <v>0</v>
       </c>
-      <c r="H19" s="48">
-        <v>0</v>
-      </c>
+      <c r="H19" s="48"/>
       <c r="I19" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="48">
+        <v>0</v>
+      </c>
+      <c r="L19" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="47">
         <v>44001</v>
       </c>
@@ -3218,20 +3306,21 @@
       <c r="G20" s="48">
         <v>0</v>
       </c>
-      <c r="H20" s="48">
-        <v>0</v>
-      </c>
+      <c r="H20" s="48"/>
       <c r="I20" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="48">
+        <v>0</v>
+      </c>
+      <c r="L20" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="47">
         <v>44002</v>
       </c>
@@ -3253,20 +3342,21 @@
       <c r="G21" s="48">
         <v>0</v>
       </c>
-      <c r="H21" s="48">
-        <v>0</v>
-      </c>
+      <c r="H21" s="48"/>
       <c r="I21" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="48">
+        <v>0</v>
+      </c>
+      <c r="L21" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="218">
         <v>44003</v>
       </c>
@@ -3288,20 +3378,21 @@
       <c r="G22" s="217">
         <v>0</v>
       </c>
-      <c r="H22" s="217">
-        <v>0</v>
-      </c>
+      <c r="H22" s="217"/>
       <c r="I22" s="217">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="217">
+        <v>0</v>
+      </c>
+      <c r="L22" s="217">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="218">
         <v>44004</v>
       </c>
@@ -3323,20 +3414,21 @@
       <c r="G23" s="48">
         <v>0</v>
       </c>
-      <c r="H23" s="48">
-        <v>0</v>
-      </c>
+      <c r="H23" s="48"/>
       <c r="I23" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="48">
+        <v>0</v>
+      </c>
+      <c r="L23" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="218">
         <v>44005</v>
       </c>
@@ -3358,20 +3450,21 @@
       <c r="G24" s="48">
         <v>0</v>
       </c>
-      <c r="H24" s="48">
-        <v>0</v>
-      </c>
+      <c r="H24" s="48"/>
       <c r="I24" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="48">
+        <v>0</v>
+      </c>
+      <c r="L24" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="218">
         <v>44006</v>
       </c>
@@ -3393,20 +3486,21 @@
       <c r="G25" s="48">
         <v>0</v>
       </c>
-      <c r="H25" s="48">
-        <v>0</v>
-      </c>
+      <c r="H25" s="48"/>
       <c r="I25" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="48">
+        <v>0</v>
+      </c>
+      <c r="L25" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="218">
         <v>44007</v>
       </c>
@@ -3428,20 +3522,21 @@
       <c r="G26" s="48">
         <v>0</v>
       </c>
-      <c r="H26" s="48">
-        <v>0</v>
-      </c>
+      <c r="H26" s="48"/>
       <c r="I26" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="48">
+        <v>0</v>
+      </c>
+      <c r="L26" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="218">
         <v>44008</v>
       </c>
@@ -3463,33 +3558,59 @@
       <c r="G27" s="48">
         <v>0</v>
       </c>
-      <c r="H27" s="48">
-        <v>0</v>
-      </c>
+      <c r="H27" s="48"/>
       <c r="I27" s="48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="48">
+        <v>0</v>
+      </c>
+      <c r="L27" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="218">
+        <v>44009</v>
+      </c>
+      <c r="B28" s="48">
+        <v>0</v>
+      </c>
+      <c r="C28" s="48">
+        <v>1</v>
+      </c>
+      <c r="D28" s="48">
+        <v>1</v>
+      </c>
+      <c r="E28" s="48">
+        <v>1</v>
+      </c>
+      <c r="F28" s="48">
+        <v>1</v>
+      </c>
+      <c r="G28" s="48">
+        <v>0</v>
+      </c>
+      <c r="H28" s="48">
+        <v>1</v>
+      </c>
+      <c r="I28" s="48">
+        <v>0</v>
+      </c>
+      <c r="J28" s="48">
+        <v>1</v>
+      </c>
+      <c r="K28" s="48">
+        <v>0</v>
+      </c>
+      <c r="L28" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="48"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
@@ -3501,8 +3622,9 @@
       <c r="I29" s="48"/>
       <c r="J29" s="48"/>
       <c r="K29" s="48"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" s="48"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="48"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
@@ -3514,8 +3636,9 @@
       <c r="I30" s="48"/>
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" s="48"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
@@ -3527,8 +3650,9 @@
       <c r="I31" s="48"/>
       <c r="J31" s="48"/>
       <c r="K31" s="48"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" s="48"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
@@ -3540,8 +3664,9 @@
       <c r="I32" s="48"/>
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" s="48"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -3553,8 +3678,9 @@
       <c r="I33" s="48"/>
       <c r="J33" s="48"/>
       <c r="K33" s="48"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="48"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
@@ -3566,8 +3692,9 @@
       <c r="I34" s="48"/>
       <c r="J34" s="48"/>
       <c r="K34" s="48"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="48"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -3579,8 +3706,9 @@
       <c r="I35" s="48"/>
       <c r="J35" s="48"/>
       <c r="K35" s="48"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="48"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="48"/>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -3592,8 +3720,9 @@
       <c r="I36" s="48"/>
       <c r="J36" s="48"/>
       <c r="K36" s="48"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="48"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="48"/>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
@@ -3605,6 +3734,7 @@
       <c r="I37" s="48"/>
       <c r="J37" s="48"/>
       <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3613,16 +3743,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -3651,19 +3781,22 @@
         <v>11</v>
       </c>
       <c r="J1" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="47">
         <v>43983</v>
       </c>
@@ -3691,20 +3824,21 @@
       <c r="I2" s="48">
         <v>0</v>
       </c>
-      <c r="J2" s="48">
-        <v>1</v>
-      </c>
+      <c r="J2" s="48"/>
       <c r="K2" s="48">
         <v>1</v>
       </c>
       <c r="L2" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="47">
         <v>43984</v>
       </c>
@@ -3732,20 +3866,21 @@
       <c r="I3" s="48">
         <v>0</v>
       </c>
-      <c r="J3" s="48">
-        <v>1</v>
-      </c>
+      <c r="J3" s="48"/>
       <c r="K3" s="48">
         <v>1</v>
       </c>
       <c r="L3" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="47">
         <v>43985</v>
       </c>
@@ -3773,20 +3908,21 @@
       <c r="I4" s="48">
         <v>0</v>
       </c>
-      <c r="J4" s="48">
-        <v>1</v>
-      </c>
+      <c r="J4" s="48"/>
       <c r="K4" s="48">
         <v>1</v>
       </c>
       <c r="L4" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="47">
         <v>43986</v>
       </c>
@@ -3812,20 +3948,21 @@
       <c r="I5" s="48">
         <v>0</v>
       </c>
-      <c r="J5" s="48">
-        <v>1</v>
-      </c>
+      <c r="J5" s="48"/>
       <c r="K5" s="48">
         <v>1</v>
       </c>
       <c r="L5" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="47">
         <v>43987</v>
       </c>
@@ -3853,20 +3990,21 @@
       <c r="I6" s="48">
         <v>0</v>
       </c>
-      <c r="J6" s="48">
-        <v>1</v>
-      </c>
+      <c r="J6" s="48"/>
       <c r="K6" s="48">
         <v>1</v>
       </c>
       <c r="L6" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="N6" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="47" t="s">
         <v>67</v>
       </c>
@@ -3894,20 +4032,21 @@
       <c r="I7" s="48">
         <v>0</v>
       </c>
-      <c r="J7" s="48">
-        <v>1</v>
-      </c>
+      <c r="J7" s="48"/>
       <c r="K7" s="48">
         <v>1</v>
       </c>
       <c r="L7" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
         <v>43989</v>
       </c>
@@ -3935,20 +4074,21 @@
       <c r="I8" s="48">
         <v>0</v>
       </c>
-      <c r="J8" s="48">
-        <v>1</v>
-      </c>
+      <c r="J8" s="48"/>
       <c r="K8" s="48">
         <v>1</v>
       </c>
       <c r="L8" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="47">
         <v>43990</v>
       </c>
@@ -3976,20 +4116,21 @@
       <c r="I9" s="48">
         <v>0</v>
       </c>
-      <c r="J9" s="48">
-        <v>1</v>
-      </c>
+      <c r="J9" s="48"/>
       <c r="K9" s="48">
         <v>1</v>
       </c>
       <c r="L9" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="47">
         <v>43991</v>
       </c>
@@ -4017,20 +4158,21 @@
       <c r="I10" s="48">
         <v>0</v>
       </c>
-      <c r="J10" s="48">
-        <v>1</v>
-      </c>
+      <c r="J10" s="48"/>
       <c r="K10" s="48">
         <v>1</v>
       </c>
       <c r="L10" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="47">
         <v>43992</v>
       </c>
@@ -4058,20 +4200,21 @@
       <c r="I11" s="48">
         <v>0</v>
       </c>
-      <c r="J11" s="48">
-        <v>1</v>
-      </c>
+      <c r="J11" s="48"/>
       <c r="K11" s="48">
         <v>1</v>
       </c>
       <c r="L11" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="47">
         <v>43993</v>
       </c>
@@ -4099,20 +4242,21 @@
       <c r="I12" s="48">
         <v>0</v>
       </c>
-      <c r="J12" s="48">
-        <v>1</v>
-      </c>
+      <c r="J12" s="48"/>
       <c r="K12" s="48">
         <v>1</v>
       </c>
       <c r="L12" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="47">
         <v>43994</v>
       </c>
@@ -4140,20 +4284,21 @@
       <c r="I13" s="48">
         <v>0</v>
       </c>
-      <c r="J13" s="48">
-        <v>1</v>
-      </c>
+      <c r="J13" s="48"/>
       <c r="K13" s="48">
         <v>1</v>
       </c>
       <c r="L13" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="47">
         <v>43995</v>
       </c>
@@ -4181,20 +4326,21 @@
       <c r="I14" s="48">
         <v>0</v>
       </c>
-      <c r="J14" s="48">
-        <v>1</v>
-      </c>
+      <c r="J14" s="48"/>
       <c r="K14" s="48">
         <v>1</v>
       </c>
       <c r="L14" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="47">
         <v>43996</v>
       </c>
@@ -4222,20 +4368,21 @@
       <c r="I15" s="48">
         <v>0</v>
       </c>
-      <c r="J15" s="48">
-        <v>1</v>
-      </c>
+      <c r="J15" s="48"/>
       <c r="K15" s="48">
         <v>1</v>
       </c>
       <c r="L15" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="47">
         <v>43997</v>
       </c>
@@ -4263,20 +4410,21 @@
       <c r="I16" s="48">
         <v>0</v>
       </c>
-      <c r="J16" s="48">
-        <v>1</v>
-      </c>
+      <c r="J16" s="48"/>
       <c r="K16" s="48">
         <v>1</v>
       </c>
       <c r="L16" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="47">
         <v>43998</v>
       </c>
@@ -4304,20 +4452,21 @@
       <c r="I17" s="48">
         <v>0</v>
       </c>
-      <c r="J17" s="48">
-        <v>1</v>
-      </c>
+      <c r="J17" s="48"/>
       <c r="K17" s="48">
         <v>1</v>
       </c>
       <c r="L17" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="47">
         <v>43999</v>
       </c>
@@ -4345,20 +4494,21 @@
       <c r="I18" s="48">
         <v>0</v>
       </c>
-      <c r="J18" s="48">
-        <v>1</v>
-      </c>
+      <c r="J18" s="48"/>
       <c r="K18" s="48">
         <v>1</v>
       </c>
       <c r="L18" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="47">
         <v>44000</v>
       </c>
@@ -4386,20 +4536,21 @@
       <c r="I19" s="48">
         <v>0</v>
       </c>
-      <c r="J19" s="48">
-        <v>1</v>
-      </c>
+      <c r="J19" s="48"/>
       <c r="K19" s="48">
         <v>1</v>
       </c>
       <c r="L19" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="47">
         <v>44001</v>
       </c>
@@ -4427,20 +4578,21 @@
       <c r="I20" s="48">
         <v>0</v>
       </c>
-      <c r="J20" s="48">
-        <v>1</v>
-      </c>
+      <c r="J20" s="48"/>
       <c r="K20" s="48">
         <v>1</v>
       </c>
       <c r="L20" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="47">
         <v>44002</v>
       </c>
@@ -4468,20 +4620,21 @@
       <c r="I21" s="48">
         <v>0</v>
       </c>
-      <c r="J21" s="48">
-        <v>1</v>
-      </c>
+      <c r="J21" s="48"/>
       <c r="K21" s="48">
         <v>1</v>
       </c>
       <c r="L21" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="47">
         <v>44003</v>
       </c>
@@ -4509,20 +4662,21 @@
       <c r="I22" s="48">
         <v>0</v>
       </c>
-      <c r="J22" s="48">
-        <v>1</v>
-      </c>
+      <c r="J22" s="48"/>
       <c r="K22" s="48">
         <v>1</v>
       </c>
       <c r="L22" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="47">
         <v>44004</v>
       </c>
@@ -4550,20 +4704,21 @@
       <c r="I23" s="48">
         <v>0</v>
       </c>
-      <c r="J23" s="48">
-        <v>1</v>
-      </c>
+      <c r="J23" s="48"/>
       <c r="K23" s="48">
         <v>1</v>
       </c>
       <c r="L23" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="47">
         <v>44005</v>
       </c>
@@ -4591,20 +4746,21 @@
       <c r="I24" s="48">
         <v>0</v>
       </c>
-      <c r="J24" s="48">
-        <v>1</v>
-      </c>
+      <c r="J24" s="48"/>
       <c r="K24" s="48">
         <v>1</v>
       </c>
       <c r="L24" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="47">
         <v>44006</v>
       </c>
@@ -4632,20 +4788,21 @@
       <c r="I25" s="48">
         <v>0</v>
       </c>
-      <c r="J25" s="48">
-        <v>1</v>
-      </c>
+      <c r="J25" s="48"/>
       <c r="K25" s="48">
         <v>1</v>
       </c>
       <c r="L25" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="47">
         <v>44007</v>
       </c>
@@ -4673,20 +4830,21 @@
       <c r="I26" s="48">
         <v>0</v>
       </c>
-      <c r="J26" s="48">
-        <v>1</v>
-      </c>
+      <c r="J26" s="48"/>
       <c r="K26" s="48">
         <v>1</v>
       </c>
       <c r="L26" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="47">
         <v>44008</v>
       </c>
@@ -4714,33 +4872,63 @@
       <c r="I27" s="48">
         <v>0</v>
       </c>
-      <c r="J27" s="48">
-        <v>1</v>
-      </c>
+      <c r="J27" s="48"/>
       <c r="K27" s="48">
         <v>1</v>
       </c>
       <c r="L27" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="48">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="48"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
+      <c r="N27" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="47">
+        <v>44009</v>
+      </c>
+      <c r="B28" s="48">
+        <v>0</v>
+      </c>
+      <c r="C28" s="48">
+        <v>1</v>
+      </c>
+      <c r="D28" s="48">
+        <v>1</v>
+      </c>
+      <c r="E28" s="48">
+        <v>0</v>
+      </c>
+      <c r="F28" s="48">
+        <v>1</v>
+      </c>
+      <c r="G28" s="48">
+        <v>1</v>
+      </c>
+      <c r="H28" s="48">
+        <v>1</v>
+      </c>
+      <c r="I28" s="48">
+        <v>0</v>
+      </c>
+      <c r="J28" s="48">
+        <v>1</v>
+      </c>
+      <c r="K28" s="48">
+        <v>1</v>
+      </c>
+      <c r="L28" s="48">
+        <v>1</v>
+      </c>
+      <c r="M28" s="48">
+        <v>0</v>
+      </c>
+      <c r="N28" s="48">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4753,7 +4941,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5631,16 +5819,36 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="220"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
+      <c r="A28" s="47">
+        <v>44009</v>
+      </c>
+      <c r="B28" s="48">
+        <v>0</v>
+      </c>
+      <c r="C28" s="48">
+        <v>0</v>
+      </c>
+      <c r="D28" s="48">
+        <v>0</v>
+      </c>
+      <c r="E28" s="48">
+        <v>0</v>
+      </c>
+      <c r="F28" s="48">
+        <v>2</v>
+      </c>
+      <c r="G28" s="48">
+        <v>1</v>
+      </c>
+      <c r="H28" s="48">
+        <v>1</v>
+      </c>
+      <c r="I28" s="48">
+        <v>1</v>
+      </c>
+      <c r="J28" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="107"/>
@@ -5666,8 +5874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5739,7 +5947,7 @@
       <c r="U1" s="49">
         <v>44002</v>
       </c>
-      <c r="V1" s="230">
+      <c r="V1" s="229">
         <v>44003</v>
       </c>
       <c r="W1" s="49">
@@ -5757,7 +5965,9 @@
       <c r="AA1" s="49">
         <v>44008</v>
       </c>
-      <c r="AB1" s="48"/>
+      <c r="AB1" s="49">
+        <v>44009</v>
+      </c>
       <c r="AC1" s="48"/>
       <c r="AD1" s="48"/>
       <c r="AE1" s="48"/>
@@ -5843,10 +6053,10 @@
       <c r="U2" s="48">
         <v>3657</v>
       </c>
-      <c r="V2" s="231">
+      <c r="V2" s="230">
         <v>3689</v>
       </c>
-      <c r="W2" s="232">
+      <c r="W2" s="231">
         <v>3721</v>
       </c>
       <c r="X2" s="48">
@@ -5861,7 +6071,9 @@
       <c r="AA2" s="48">
         <v>3849</v>
       </c>
-      <c r="AB2" s="48"/>
+      <c r="AB2" s="48">
+        <v>3881</v>
+      </c>
       <c r="AC2" s="48"/>
       <c r="AD2" s="48"/>
       <c r="AE2" s="48"/>
@@ -5947,7 +6159,7 @@
       <c r="U3" s="48">
         <v>3472</v>
       </c>
-      <c r="V3" s="231">
+      <c r="V3" s="230">
         <v>3504</v>
       </c>
       <c r="W3" s="48">
@@ -5965,7 +6177,9 @@
       <c r="AA3" s="48">
         <v>3664</v>
       </c>
-      <c r="AB3" s="48"/>
+      <c r="AB3" s="74">
+        <v>3696</v>
+      </c>
       <c r="AC3" s="48"/>
       <c r="AD3" s="48"/>
       <c r="AE3" s="48"/>
@@ -6051,7 +6265,7 @@
       <c r="U4" s="48">
         <v>3472</v>
       </c>
-      <c r="V4" s="231">
+      <c r="V4" s="230">
         <v>3504</v>
       </c>
       <c r="W4" s="48">
@@ -6069,7 +6283,9 @@
       <c r="AA4" s="48">
         <v>3664</v>
       </c>
-      <c r="AB4" s="48"/>
+      <c r="AB4" s="74">
+        <v>3696</v>
+      </c>
       <c r="AC4" s="48"/>
       <c r="AD4" s="48"/>
       <c r="AE4" s="48"/>
@@ -6155,7 +6371,7 @@
       <c r="U5" s="48">
         <v>3472</v>
       </c>
-      <c r="V5" s="231">
+      <c r="V5" s="230">
         <v>3504</v>
       </c>
       <c r="W5" s="48">
@@ -6173,7 +6389,9 @@
       <c r="AA5" s="48">
         <v>3664</v>
       </c>
-      <c r="AB5" s="48"/>
+      <c r="AB5" s="74">
+        <v>3696</v>
+      </c>
       <c r="AC5" s="48"/>
       <c r="AD5" s="48"/>
       <c r="AE5" s="48"/>
@@ -6259,7 +6477,7 @@
       <c r="U6" s="48">
         <v>3472</v>
       </c>
-      <c r="V6" s="231">
+      <c r="V6" s="230">
         <v>3504</v>
       </c>
       <c r="W6" s="48">
@@ -6277,7 +6495,9 @@
       <c r="AA6" s="48">
         <v>3664</v>
       </c>
-      <c r="AB6" s="48"/>
+      <c r="AB6" s="74">
+        <v>3696</v>
+      </c>
       <c r="AC6" s="48"/>
       <c r="AD6" s="48"/>
       <c r="AE6" s="48"/>
@@ -6363,7 +6583,7 @@
       <c r="U7" s="48">
         <v>2663</v>
       </c>
-      <c r="V7" s="231">
+      <c r="V7" s="230">
         <v>2695</v>
       </c>
       <c r="W7" s="48">
@@ -6381,7 +6601,9 @@
       <c r="AA7" s="48">
         <v>2855</v>
       </c>
-      <c r="AB7" s="48"/>
+      <c r="AB7" s="48">
+        <v>3696</v>
+      </c>
       <c r="AC7" s="48"/>
       <c r="AD7" s="48"/>
       <c r="AE7" s="48"/>
@@ -6467,7 +6689,7 @@
       <c r="U8" s="48">
         <v>5294</v>
       </c>
-      <c r="V8" s="231">
+      <c r="V8" s="230">
         <v>5326</v>
       </c>
       <c r="W8" s="48">
@@ -6485,7 +6707,9 @@
       <c r="AA8" s="48">
         <v>5486</v>
       </c>
-      <c r="AB8" s="48"/>
+      <c r="AB8" s="48">
+        <v>5518</v>
+      </c>
       <c r="AC8" s="48"/>
       <c r="AD8" s="48"/>
       <c r="AE8" s="48"/>
@@ -6621,7 +6845,7 @@
       <c r="U10" s="48">
         <v>160</v>
       </c>
-      <c r="V10" s="231">
+      <c r="V10" s="230">
         <v>161</v>
       </c>
       <c r="W10" s="48">
@@ -6639,7 +6863,9 @@
       <c r="AA10" s="48">
         <v>166</v>
       </c>
-      <c r="AB10" s="48"/>
+      <c r="AB10" s="48">
+        <v>167</v>
+      </c>
       <c r="AC10" s="48"/>
       <c r="AD10" s="48"/>
       <c r="AE10" s="48"/>
@@ -6725,7 +6951,7 @@
       <c r="U11" s="48">
         <v>160</v>
       </c>
-      <c r="V11" s="231">
+      <c r="V11" s="230">
         <v>161</v>
       </c>
       <c r="W11" s="48">
@@ -6743,7 +6969,9 @@
       <c r="AA11" s="48">
         <v>166</v>
       </c>
-      <c r="AB11" s="48"/>
+      <c r="AB11" s="48">
+        <v>167</v>
+      </c>
       <c r="AC11" s="48"/>
       <c r="AD11" s="48"/>
       <c r="AE11" s="48"/>
@@ -6829,7 +7057,7 @@
       <c r="U12" s="48">
         <v>160</v>
       </c>
-      <c r="V12" s="231">
+      <c r="V12" s="230">
         <v>161</v>
       </c>
       <c r="W12" s="48">
@@ -6847,7 +7075,9 @@
       <c r="AA12" s="48">
         <v>166</v>
       </c>
-      <c r="AB12" s="48"/>
+      <c r="AB12" s="48">
+        <v>167</v>
+      </c>
       <c r="AC12" s="48"/>
       <c r="AD12" s="48"/>
       <c r="AE12" s="48"/>
@@ -6933,7 +7163,7 @@
       <c r="U13" s="48">
         <v>160</v>
       </c>
-      <c r="V13" s="231">
+      <c r="V13" s="230">
         <v>161</v>
       </c>
       <c r="W13" s="48">
@@ -6951,7 +7181,9 @@
       <c r="AA13" s="48">
         <v>166</v>
       </c>
-      <c r="AB13" s="48"/>
+      <c r="AB13" s="48">
+        <v>167</v>
+      </c>
       <c r="AC13" s="48"/>
       <c r="AD13" s="48"/>
       <c r="AE13" s="48"/>
@@ -7037,7 +7269,7 @@
       <c r="U14" s="48">
         <v>160</v>
       </c>
-      <c r="V14" s="231">
+      <c r="V14" s="230">
         <v>161</v>
       </c>
       <c r="W14" s="48">
@@ -7055,7 +7287,9 @@
       <c r="AA14" s="48">
         <v>166</v>
       </c>
-      <c r="AB14" s="48"/>
+      <c r="AB14" s="48">
+        <v>167</v>
+      </c>
       <c r="AC14" s="48"/>
       <c r="AD14" s="48"/>
       <c r="AE14" s="48"/>
@@ -7141,7 +7375,7 @@
       <c r="U15" s="48">
         <v>95</v>
       </c>
-      <c r="V15" s="231">
+      <c r="V15" s="230">
         <v>96</v>
       </c>
       <c r="W15" s="48">
@@ -7159,7 +7393,9 @@
       <c r="AA15" s="48">
         <v>101</v>
       </c>
-      <c r="AB15" s="48"/>
+      <c r="AB15" s="48">
+        <v>102</v>
+      </c>
       <c r="AC15" s="48"/>
       <c r="AD15" s="48"/>
       <c r="AE15" s="48"/>
@@ -7245,7 +7481,7 @@
       <c r="U16" s="48">
         <v>172</v>
       </c>
-      <c r="V16" s="231">
+      <c r="V16" s="230">
         <v>173</v>
       </c>
       <c r="W16" s="48">
@@ -7263,7 +7499,9 @@
       <c r="AA16" s="48">
         <v>178</v>
       </c>
-      <c r="AB16" s="48"/>
+      <c r="AB16" s="48">
+        <v>179</v>
+      </c>
       <c r="AC16" s="48"/>
       <c r="AD16" s="48"/>
       <c r="AE16" s="48"/>
@@ -7399,7 +7637,7 @@
       <c r="U18" s="48">
         <v>849</v>
       </c>
-      <c r="V18" s="231">
+      <c r="V18" s="230">
         <v>856</v>
       </c>
       <c r="W18" s="48">
@@ -7417,7 +7655,9 @@
       <c r="AA18" s="48">
         <v>891</v>
       </c>
-      <c r="AB18" s="48"/>
+      <c r="AB18" s="48">
+        <v>905</v>
+      </c>
       <c r="AC18" s="48"/>
       <c r="AD18" s="48"/>
       <c r="AE18" s="48"/>
@@ -7455,7 +7695,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AA20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AB20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -7554,7 +7794,10 @@
         <f t="shared" si="0"/>
         <v>28846</v>
       </c>
-      <c r="AB20" s="48"/>
+      <c r="AB20" s="51">
+        <f t="shared" si="0"/>
+        <v>29900</v>
+      </c>
       <c r="AC20" s="48"/>
       <c r="AD20" s="48"/>
       <c r="AE20" s="48"/>
@@ -7744,10 +7987,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7829,37 +8072,49 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="269" t="s">
+      <c r="B8" s="277" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="269"/>
+      <c r="B9" s="277"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="269"/>
+      <c r="B10" s="277"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="269"/>
+      <c r="B11" s="277"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="270" t="s">
+      <c r="B12" s="278" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="270"/>
+      <c r="B13" s="278"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="270"/>
+      <c r="B14" s="278"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="279" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="279"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 28th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E77ACA-3919-1342-907F-E68701B2AC3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A75E45-D33E-314D-B4FA-4B32A9E32DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="280">
+  <cellXfs count="290">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1341,6 +1341,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1350,6 +1377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1669,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2574,6 +2602,38 @@
       </c>
       <c r="J28" s="276">
         <v>551052</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
+        <v>44010</v>
+      </c>
+      <c r="B29" s="277">
+        <v>216852</v>
+      </c>
+      <c r="C29" s="278">
+        <v>275203</v>
+      </c>
+      <c r="D29" s="279">
+        <v>64143</v>
+      </c>
+      <c r="E29" s="280">
+        <v>26648</v>
+      </c>
+      <c r="F29" s="281">
+        <v>31.106930072122925</v>
+      </c>
+      <c r="G29" s="282">
+        <v>67456</v>
+      </c>
+      <c r="H29" s="283">
+        <v>5718</v>
+      </c>
+      <c r="I29" s="284">
+        <v>6432</v>
+      </c>
+      <c r="J29" s="285">
+        <v>556198</v>
       </c>
     </row>
   </sheetData>
@@ -2587,7 +2647,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3611,18 +3671,42 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="48"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
+      <c r="A29" s="218">
+        <v>44010</v>
+      </c>
+      <c r="B29" s="48">
+        <v>0</v>
+      </c>
+      <c r="C29" s="48">
+        <v>1</v>
+      </c>
+      <c r="D29" s="48">
+        <v>1</v>
+      </c>
+      <c r="E29" s="48">
+        <v>1</v>
+      </c>
+      <c r="F29" s="48">
+        <v>1</v>
+      </c>
+      <c r="G29" s="48">
+        <v>0</v>
+      </c>
+      <c r="H29" s="48">
+        <v>1</v>
+      </c>
+      <c r="I29" s="48">
+        <v>0</v>
+      </c>
+      <c r="J29" s="48">
+        <v>1</v>
+      </c>
+      <c r="K29" s="48">
+        <v>0</v>
+      </c>
+      <c r="L29" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="48"/>
@@ -3743,11 +3827,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4929,6 +5013,146 @@
       <c r="N28" s="48">
         <v>0</v>
       </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="47">
+        <v>44010</v>
+      </c>
+      <c r="B29" s="74">
+        <v>0</v>
+      </c>
+      <c r="C29" s="74">
+        <v>1</v>
+      </c>
+      <c r="D29" s="74">
+        <v>1</v>
+      </c>
+      <c r="E29" s="74">
+        <v>0</v>
+      </c>
+      <c r="F29" s="74">
+        <v>1</v>
+      </c>
+      <c r="G29" s="74">
+        <v>1</v>
+      </c>
+      <c r="H29" s="74">
+        <v>1</v>
+      </c>
+      <c r="I29" s="74">
+        <v>0</v>
+      </c>
+      <c r="J29" s="74">
+        <v>1</v>
+      </c>
+      <c r="K29" s="74">
+        <v>1</v>
+      </c>
+      <c r="L29" s="74">
+        <v>1</v>
+      </c>
+      <c r="M29" s="74">
+        <v>0</v>
+      </c>
+      <c r="N29" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="48"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4941,7 +5165,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5851,16 +6075,72 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="107"/>
+      <c r="A29" s="47">
+        <v>44010</v>
+      </c>
+      <c r="B29" s="74">
+        <v>0</v>
+      </c>
+      <c r="C29" s="74">
+        <v>0</v>
+      </c>
+      <c r="D29" s="74">
+        <v>0</v>
+      </c>
+      <c r="E29" s="74">
+        <v>0</v>
+      </c>
+      <c r="F29" s="74">
+        <v>2</v>
+      </c>
+      <c r="G29" s="74">
+        <v>1</v>
+      </c>
+      <c r="H29" s="74">
+        <v>1</v>
+      </c>
+      <c r="I29" s="74">
+        <v>1</v>
+      </c>
+      <c r="J29" s="74">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="107"/>
+      <c r="A30" s="289"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="107"/>
+      <c r="A31" s="289"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="107"/>
+      <c r="A32" s="289"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="107"/>
@@ -5874,8 +6154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5968,7 +6248,9 @@
       <c r="AB1" s="49">
         <v>44009</v>
       </c>
-      <c r="AC1" s="48"/>
+      <c r="AC1" s="49">
+        <v>44010</v>
+      </c>
       <c r="AD1" s="48"/>
       <c r="AE1" s="48"/>
       <c r="AF1" s="48"/>
@@ -6074,7 +6356,9 @@
       <c r="AB2" s="48">
         <v>3881</v>
       </c>
-      <c r="AC2" s="48"/>
+      <c r="AC2" s="48">
+        <v>3913</v>
+      </c>
       <c r="AD2" s="48"/>
       <c r="AE2" s="48"/>
       <c r="AF2" s="48"/>
@@ -6180,7 +6464,9 @@
       <c r="AB3" s="74">
         <v>3696</v>
       </c>
-      <c r="AC3" s="48"/>
+      <c r="AC3" s="48">
+        <v>3728</v>
+      </c>
       <c r="AD3" s="48"/>
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
@@ -6286,7 +6572,9 @@
       <c r="AB4" s="74">
         <v>3696</v>
       </c>
-      <c r="AC4" s="48"/>
+      <c r="AC4" s="48">
+        <v>3728</v>
+      </c>
       <c r="AD4" s="48"/>
       <c r="AE4" s="48"/>
       <c r="AF4" s="48"/>
@@ -6392,7 +6680,9 @@
       <c r="AB5" s="74">
         <v>3696</v>
       </c>
-      <c r="AC5" s="48"/>
+      <c r="AC5" s="48">
+        <v>3728</v>
+      </c>
       <c r="AD5" s="48"/>
       <c r="AE5" s="48"/>
       <c r="AF5" s="48"/>
@@ -6498,7 +6788,9 @@
       <c r="AB6" s="74">
         <v>3696</v>
       </c>
-      <c r="AC6" s="48"/>
+      <c r="AC6" s="48">
+        <v>3728</v>
+      </c>
       <c r="AD6" s="48"/>
       <c r="AE6" s="48"/>
       <c r="AF6" s="48"/>
@@ -6604,7 +6896,9 @@
       <c r="AB7" s="48">
         <v>3696</v>
       </c>
-      <c r="AC7" s="48"/>
+      <c r="AC7" s="48">
+        <v>3728</v>
+      </c>
       <c r="AD7" s="48"/>
       <c r="AE7" s="48"/>
       <c r="AF7" s="48"/>
@@ -6710,7 +7004,9 @@
       <c r="AB8" s="48">
         <v>5518</v>
       </c>
-      <c r="AC8" s="48"/>
+      <c r="AC8" s="48">
+        <v>5550</v>
+      </c>
       <c r="AD8" s="48"/>
       <c r="AE8" s="48"/>
       <c r="AF8" s="48"/>
@@ -6866,7 +7162,9 @@
       <c r="AB10" s="48">
         <v>167</v>
       </c>
-      <c r="AC10" s="48"/>
+      <c r="AC10" s="48">
+        <v>168</v>
+      </c>
       <c r="AD10" s="48"/>
       <c r="AE10" s="48"/>
       <c r="AF10" s="48"/>
@@ -6972,7 +7270,9 @@
       <c r="AB11" s="48">
         <v>167</v>
       </c>
-      <c r="AC11" s="48"/>
+      <c r="AC11" s="48">
+        <v>168</v>
+      </c>
       <c r="AD11" s="48"/>
       <c r="AE11" s="48"/>
       <c r="AF11" s="48"/>
@@ -7078,7 +7378,9 @@
       <c r="AB12" s="48">
         <v>167</v>
       </c>
-      <c r="AC12" s="48"/>
+      <c r="AC12" s="48">
+        <v>168</v>
+      </c>
       <c r="AD12" s="48"/>
       <c r="AE12" s="48"/>
       <c r="AF12" s="48"/>
@@ -7184,7 +7486,9 @@
       <c r="AB13" s="48">
         <v>167</v>
       </c>
-      <c r="AC13" s="48"/>
+      <c r="AC13" s="48">
+        <v>168</v>
+      </c>
       <c r="AD13" s="48"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
@@ -7290,7 +7594,9 @@
       <c r="AB14" s="48">
         <v>167</v>
       </c>
-      <c r="AC14" s="48"/>
+      <c r="AC14" s="48">
+        <v>168</v>
+      </c>
       <c r="AD14" s="48"/>
       <c r="AE14" s="48"/>
       <c r="AF14" s="48"/>
@@ -7396,7 +7702,9 @@
       <c r="AB15" s="48">
         <v>102</v>
       </c>
-      <c r="AC15" s="48"/>
+      <c r="AC15" s="48">
+        <v>103</v>
+      </c>
       <c r="AD15" s="48"/>
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
@@ -7502,7 +7810,9 @@
       <c r="AB16" s="48">
         <v>179</v>
       </c>
-      <c r="AC16" s="48"/>
+      <c r="AC16" s="48">
+        <v>180</v>
+      </c>
       <c r="AD16" s="48"/>
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
@@ -7658,7 +7968,9 @@
       <c r="AB18" s="48">
         <v>905</v>
       </c>
-      <c r="AC18" s="48"/>
+      <c r="AC18" s="48">
+        <v>905</v>
+      </c>
       <c r="AD18" s="48"/>
       <c r="AE18" s="48"/>
       <c r="AF18" s="48"/>
@@ -7695,7 +8007,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AB20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AC20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -7798,7 +8110,10 @@
         <f t="shared" si="0"/>
         <v>29900</v>
       </c>
-      <c r="AC20" s="48"/>
+      <c r="AC20" s="51">
+        <f t="shared" si="0"/>
+        <v>30131</v>
+      </c>
       <c r="AD20" s="48"/>
       <c r="AE20" s="48"/>
     </row>
@@ -8072,43 +8387,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="277" t="s">
+      <c r="B8" s="286" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="277"/>
+      <c r="B9" s="286"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="277"/>
+      <c r="B10" s="286"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="277"/>
+      <c r="B11" s="286"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="278" t="s">
+      <c r="B12" s="287" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="278"/>
+      <c r="B13" s="287"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="278"/>
+      <c r="B14" s="287"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="279" t="s">
+      <c r="B15" s="288" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="279"/>
+      <c r="B16" s="288"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 29th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A75E45-D33E-314D-B4FA-4B32A9E32DF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E17D8F9-FA95-694A-B8D7-A3341D73D754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="290">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1368,6 +1368,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1377,7 +1405,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1697,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2634,6 +2661,38 @@
       </c>
       <c r="J29" s="285">
         <v>556198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="15">
+        <v>44011</v>
+      </c>
+      <c r="B30" s="287">
+        <v>220657</v>
+      </c>
+      <c r="C30" s="288">
+        <v>279035</v>
+      </c>
+      <c r="D30" s="289">
+        <v>66910</v>
+      </c>
+      <c r="E30" s="290">
+        <v>27121</v>
+      </c>
+      <c r="F30" s="291">
+        <v>30.951204811086892</v>
+      </c>
+      <c r="G30" s="292">
+        <v>68296</v>
+      </c>
+      <c r="H30" s="293">
+        <v>5822</v>
+      </c>
+      <c r="I30" s="294">
+        <v>6549</v>
+      </c>
+      <c r="J30" s="295">
+        <v>566602</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +2706,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3709,18 +3768,42 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
+      <c r="A30" s="218">
+        <v>44011</v>
+      </c>
+      <c r="B30" s="48">
+        <v>0</v>
+      </c>
+      <c r="C30" s="48">
+        <v>1</v>
+      </c>
+      <c r="D30" s="48">
+        <v>1</v>
+      </c>
+      <c r="E30" s="48">
+        <v>1</v>
+      </c>
+      <c r="F30" s="48">
+        <v>1</v>
+      </c>
+      <c r="G30" s="48">
+        <v>0</v>
+      </c>
+      <c r="H30" s="48">
+        <v>1</v>
+      </c>
+      <c r="I30" s="48">
+        <v>0</v>
+      </c>
+      <c r="J30" s="48">
+        <v>1</v>
+      </c>
+      <c r="K30" s="48">
+        <v>0</v>
+      </c>
+      <c r="L30" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
@@ -3831,7 +3914,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5059,20 +5142,48 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
+      <c r="A30" s="47">
+        <v>44011</v>
+      </c>
+      <c r="B30" s="48">
+        <v>0</v>
+      </c>
+      <c r="C30" s="48">
+        <v>1</v>
+      </c>
+      <c r="D30" s="48">
+        <v>1</v>
+      </c>
+      <c r="E30" s="48">
+        <v>0</v>
+      </c>
+      <c r="F30" s="48">
+        <v>1</v>
+      </c>
+      <c r="G30" s="48">
+        <v>1</v>
+      </c>
+      <c r="H30" s="48">
+        <v>1</v>
+      </c>
+      <c r="I30" s="48">
+        <v>0</v>
+      </c>
+      <c r="J30" s="48">
+        <v>1</v>
+      </c>
+      <c r="K30" s="48">
+        <v>1</v>
+      </c>
+      <c r="L30" s="48">
+        <v>1</v>
+      </c>
+      <c r="M30" s="48">
+        <v>0</v>
+      </c>
+      <c r="N30" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
@@ -5165,7 +5276,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6107,19 +6218,39 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="289"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
+      <c r="A30" s="47">
+        <v>44011</v>
+      </c>
+      <c r="B30" s="48">
+        <v>0</v>
+      </c>
+      <c r="C30" s="48">
+        <v>0</v>
+      </c>
+      <c r="D30" s="48">
+        <v>0</v>
+      </c>
+      <c r="E30" s="48">
+        <v>0</v>
+      </c>
+      <c r="F30" s="48">
+        <v>2</v>
+      </c>
+      <c r="G30" s="48">
+        <v>1</v>
+      </c>
+      <c r="H30" s="48">
+        <v>1</v>
+      </c>
+      <c r="I30" s="48">
+        <v>1</v>
+      </c>
+      <c r="J30" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="289"/>
+      <c r="A31" s="286"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
@@ -6131,7 +6262,7 @@
       <c r="J31" s="48"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="289"/>
+      <c r="A32" s="286"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
@@ -6154,8 +6285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20:AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6251,7 +6382,9 @@
       <c r="AC1" s="49">
         <v>44010</v>
       </c>
-      <c r="AD1" s="48"/>
+      <c r="AD1" s="49">
+        <v>44011</v>
+      </c>
       <c r="AE1" s="48"/>
       <c r="AF1" s="48"/>
       <c r="AG1" s="48"/>
@@ -6359,7 +6492,9 @@
       <c r="AC2" s="48">
         <v>3913</v>
       </c>
-      <c r="AD2" s="48"/>
+      <c r="AD2" s="48">
+        <v>3945</v>
+      </c>
       <c r="AE2" s="48"/>
       <c r="AF2" s="48"/>
       <c r="AG2" s="48"/>
@@ -6467,7 +6602,9 @@
       <c r="AC3" s="48">
         <v>3728</v>
       </c>
-      <c r="AD3" s="48"/>
+      <c r="AD3" s="48">
+        <v>3760</v>
+      </c>
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
       <c r="AG3" s="48"/>
@@ -6575,7 +6712,9 @@
       <c r="AC4" s="48">
         <v>3728</v>
       </c>
-      <c r="AD4" s="48"/>
+      <c r="AD4" s="48">
+        <v>3760</v>
+      </c>
       <c r="AE4" s="48"/>
       <c r="AF4" s="48"/>
       <c r="AG4" s="48"/>
@@ -6683,7 +6822,9 @@
       <c r="AC5" s="48">
         <v>3728</v>
       </c>
-      <c r="AD5" s="48"/>
+      <c r="AD5" s="48">
+        <v>3760</v>
+      </c>
       <c r="AE5" s="48"/>
       <c r="AF5" s="48"/>
       <c r="AG5" s="48"/>
@@ -6791,7 +6932,9 @@
       <c r="AC6" s="48">
         <v>3728</v>
       </c>
-      <c r="AD6" s="48"/>
+      <c r="AD6" s="48">
+        <v>3760</v>
+      </c>
       <c r="AE6" s="48"/>
       <c r="AF6" s="48"/>
       <c r="AG6" s="48"/>
@@ -6899,7 +7042,9 @@
       <c r="AC7" s="48">
         <v>3728</v>
       </c>
-      <c r="AD7" s="48"/>
+      <c r="AD7" s="48">
+        <v>2951</v>
+      </c>
       <c r="AE7" s="48"/>
       <c r="AF7" s="48"/>
       <c r="AG7" s="48"/>
@@ -7007,7 +7152,9 @@
       <c r="AC8" s="48">
         <v>5550</v>
       </c>
-      <c r="AD8" s="48"/>
+      <c r="AD8" s="48">
+        <v>5582</v>
+      </c>
       <c r="AE8" s="48"/>
       <c r="AF8" s="48"/>
       <c r="AG8" s="48"/>
@@ -7165,7 +7312,9 @@
       <c r="AC10" s="48">
         <v>168</v>
       </c>
-      <c r="AD10" s="48"/>
+      <c r="AD10" s="48">
+        <v>169</v>
+      </c>
       <c r="AE10" s="48"/>
       <c r="AF10" s="48"/>
       <c r="AG10" s="48"/>
@@ -7273,7 +7422,9 @@
       <c r="AC11" s="48">
         <v>168</v>
       </c>
-      <c r="AD11" s="48"/>
+      <c r="AD11" s="48">
+        <v>169</v>
+      </c>
       <c r="AE11" s="48"/>
       <c r="AF11" s="48"/>
       <c r="AG11" s="48"/>
@@ -7381,7 +7532,9 @@
       <c r="AC12" s="48">
         <v>168</v>
       </c>
-      <c r="AD12" s="48"/>
+      <c r="AD12" s="48">
+        <v>169</v>
+      </c>
       <c r="AE12" s="48"/>
       <c r="AF12" s="48"/>
       <c r="AG12" s="48"/>
@@ -7489,7 +7642,9 @@
       <c r="AC13" s="48">
         <v>168</v>
       </c>
-      <c r="AD13" s="48"/>
+      <c r="AD13" s="48">
+        <v>169</v>
+      </c>
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
       <c r="AG13" s="48"/>
@@ -7597,7 +7752,9 @@
       <c r="AC14" s="48">
         <v>168</v>
       </c>
-      <c r="AD14" s="48"/>
+      <c r="AD14" s="48">
+        <v>169</v>
+      </c>
       <c r="AE14" s="48"/>
       <c r="AF14" s="48"/>
       <c r="AG14" s="48"/>
@@ -7705,7 +7862,9 @@
       <c r="AC15" s="48">
         <v>103</v>
       </c>
-      <c r="AD15" s="48"/>
+      <c r="AD15" s="48">
+        <v>104</v>
+      </c>
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
       <c r="AG15" s="48"/>
@@ -7813,7 +7972,9 @@
       <c r="AC16" s="48">
         <v>180</v>
       </c>
-      <c r="AD16" s="48"/>
+      <c r="AD16" s="48">
+        <v>181</v>
+      </c>
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
       <c r="AG16" s="48"/>
@@ -7971,7 +8132,9 @@
       <c r="AC18" s="48">
         <v>905</v>
       </c>
-      <c r="AD18" s="48"/>
+      <c r="AD18" s="48">
+        <v>912</v>
+      </c>
       <c r="AE18" s="48"/>
       <c r="AF18" s="48"/>
       <c r="AG18" s="48"/>
@@ -8007,7 +8170,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AC20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AD20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -8114,7 +8277,10 @@
         <f t="shared" si="0"/>
         <v>30131</v>
       </c>
-      <c r="AD20" s="48"/>
+      <c r="AD20" s="51">
+        <f t="shared" si="0"/>
+        <v>29560</v>
+      </c>
       <c r="AE20" s="48"/>
     </row>
   </sheetData>
@@ -8387,43 +8553,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="286" t="s">
+      <c r="B8" s="296" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="286"/>
+      <c r="B9" s="296"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="286"/>
+      <c r="B10" s="296"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="286"/>
+      <c r="B11" s="296"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="287" t="s">
+      <c r="B12" s="297" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="287"/>
+      <c r="B13" s="297"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="287"/>
+      <c r="B14" s="297"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="288" t="s">
+      <c r="B15" s="298" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="288"/>
+      <c r="B16" s="298"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean data from SSA for June 30th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E17D8F9-FA95-694A-B8D7-A3341D73D754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426EC641-973D-D14A-AFFF-B5369C63DC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="299">
+  <cellXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1369,6 +1369,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1724,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2693,6 +2720,38 @@
       </c>
       <c r="J30" s="295">
         <v>566602</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="15">
+        <v>44012</v>
+      </c>
+      <c r="B31" s="296">
+        <v>226089</v>
+      </c>
+      <c r="C31" s="297">
+        <v>283450</v>
+      </c>
+      <c r="D31" s="298">
+        <v>72041</v>
+      </c>
+      <c r="E31" s="299">
+        <v>27769</v>
+      </c>
+      <c r="F31" s="300">
+        <v>30.779029497233388</v>
+      </c>
+      <c r="G31" s="301">
+        <v>69588</v>
+      </c>
+      <c r="H31" s="302">
+        <v>5961</v>
+      </c>
+      <c r="I31" s="303">
+        <v>6725</v>
+      </c>
+      <c r="J31" s="304">
+        <v>581580</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +2765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3806,18 +3865,42 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
+      <c r="A31" s="218">
+        <v>44012</v>
+      </c>
+      <c r="B31" s="48">
+        <v>0</v>
+      </c>
+      <c r="C31" s="48">
+        <v>1</v>
+      </c>
+      <c r="D31" s="48">
+        <v>1</v>
+      </c>
+      <c r="E31" s="48">
+        <v>1</v>
+      </c>
+      <c r="F31" s="48">
+        <v>1</v>
+      </c>
+      <c r="G31" s="48">
+        <v>0</v>
+      </c>
+      <c r="H31" s="48">
+        <v>1</v>
+      </c>
+      <c r="I31" s="48">
+        <v>0</v>
+      </c>
+      <c r="J31" s="48">
+        <v>1</v>
+      </c>
+      <c r="K31" s="48">
+        <v>0</v>
+      </c>
+      <c r="L31" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
@@ -3914,7 +3997,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5186,20 +5269,48 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
+      <c r="A31" s="47">
+        <v>44012</v>
+      </c>
+      <c r="B31" s="48">
+        <v>0</v>
+      </c>
+      <c r="C31" s="48">
+        <v>1</v>
+      </c>
+      <c r="D31" s="48">
+        <v>1</v>
+      </c>
+      <c r="E31" s="48">
+        <v>0</v>
+      </c>
+      <c r="F31" s="48">
+        <v>1</v>
+      </c>
+      <c r="G31" s="48">
+        <v>1</v>
+      </c>
+      <c r="H31" s="48">
+        <v>1</v>
+      </c>
+      <c r="I31" s="48">
+        <v>0</v>
+      </c>
+      <c r="J31" s="48">
+        <v>1</v>
+      </c>
+      <c r="K31" s="48">
+        <v>1</v>
+      </c>
+      <c r="L31" s="48">
+        <v>1</v>
+      </c>
+      <c r="M31" s="48">
+        <v>0</v>
+      </c>
+      <c r="N31" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
@@ -5275,8 +5386,8 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6250,16 +6361,36 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="286"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
+      <c r="A31" s="47">
+        <v>44012</v>
+      </c>
+      <c r="B31" s="48">
+        <v>0</v>
+      </c>
+      <c r="C31" s="48">
+        <v>0</v>
+      </c>
+      <c r="D31" s="48">
+        <v>0</v>
+      </c>
+      <c r="E31" s="48">
+        <v>0</v>
+      </c>
+      <c r="F31" s="48">
+        <v>2</v>
+      </c>
+      <c r="G31" s="48">
+        <v>1</v>
+      </c>
+      <c r="H31" s="48">
+        <v>1</v>
+      </c>
+      <c r="I31" s="48">
+        <v>1</v>
+      </c>
+      <c r="J31" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="286"/>
@@ -6285,8 +6416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20:AD20"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20:AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6385,7 +6516,9 @@
       <c r="AD1" s="49">
         <v>44011</v>
       </c>
-      <c r="AE1" s="48"/>
+      <c r="AE1" s="49">
+        <v>44012</v>
+      </c>
       <c r="AF1" s="48"/>
       <c r="AG1" s="48"/>
       <c r="AH1" s="48"/>
@@ -6495,7 +6628,9 @@
       <c r="AD2" s="48">
         <v>3945</v>
       </c>
-      <c r="AE2" s="48"/>
+      <c r="AE2" s="48">
+        <v>3977</v>
+      </c>
       <c r="AF2" s="48"/>
       <c r="AG2" s="48"/>
       <c r="AH2" s="48"/>
@@ -6605,7 +6740,9 @@
       <c r="AD3" s="48">
         <v>3760</v>
       </c>
-      <c r="AE3" s="48"/>
+      <c r="AE3" s="48">
+        <v>3792</v>
+      </c>
       <c r="AF3" s="48"/>
       <c r="AG3" s="48"/>
       <c r="AH3" s="48"/>
@@ -6715,7 +6852,9 @@
       <c r="AD4" s="48">
         <v>3760</v>
       </c>
-      <c r="AE4" s="48"/>
+      <c r="AE4" s="48">
+        <v>3792</v>
+      </c>
       <c r="AF4" s="48"/>
       <c r="AG4" s="48"/>
       <c r="AH4" s="48"/>
@@ -6825,7 +6964,9 @@
       <c r="AD5" s="48">
         <v>3760</v>
       </c>
-      <c r="AE5" s="48"/>
+      <c r="AE5" s="48">
+        <v>3792</v>
+      </c>
       <c r="AF5" s="48"/>
       <c r="AG5" s="48"/>
       <c r="AH5" s="48"/>
@@ -6935,7 +7076,9 @@
       <c r="AD6" s="48">
         <v>3760</v>
       </c>
-      <c r="AE6" s="48"/>
+      <c r="AE6" s="48">
+        <v>3792</v>
+      </c>
       <c r="AF6" s="48"/>
       <c r="AG6" s="48"/>
       <c r="AH6" s="48"/>
@@ -7045,7 +7188,9 @@
       <c r="AD7" s="48">
         <v>2951</v>
       </c>
-      <c r="AE7" s="48"/>
+      <c r="AE7" s="48">
+        <v>2983</v>
+      </c>
       <c r="AF7" s="48"/>
       <c r="AG7" s="48"/>
       <c r="AH7" s="48"/>
@@ -7155,7 +7300,9 @@
       <c r="AD8" s="48">
         <v>5582</v>
       </c>
-      <c r="AE8" s="48"/>
+      <c r="AE8" s="48">
+        <v>5614</v>
+      </c>
       <c r="AF8" s="48"/>
       <c r="AG8" s="48"/>
       <c r="AH8" s="48"/>
@@ -7315,7 +7462,9 @@
       <c r="AD10" s="48">
         <v>169</v>
       </c>
-      <c r="AE10" s="48"/>
+      <c r="AE10" s="48">
+        <v>170</v>
+      </c>
       <c r="AF10" s="48"/>
       <c r="AG10" s="48"/>
       <c r="AH10" s="48"/>
@@ -7425,7 +7574,9 @@
       <c r="AD11" s="48">
         <v>169</v>
       </c>
-      <c r="AE11" s="48"/>
+      <c r="AE11" s="48">
+        <v>170</v>
+      </c>
       <c r="AF11" s="48"/>
       <c r="AG11" s="48"/>
       <c r="AH11" s="48"/>
@@ -7535,7 +7686,9 @@
       <c r="AD12" s="48">
         <v>169</v>
       </c>
-      <c r="AE12" s="48"/>
+      <c r="AE12" s="48">
+        <v>170</v>
+      </c>
       <c r="AF12" s="48"/>
       <c r="AG12" s="48"/>
       <c r="AH12" s="48"/>
@@ -7645,7 +7798,9 @@
       <c r="AD13" s="48">
         <v>169</v>
       </c>
-      <c r="AE13" s="48"/>
+      <c r="AE13" s="48">
+        <v>170</v>
+      </c>
       <c r="AF13" s="48"/>
       <c r="AG13" s="48"/>
       <c r="AH13" s="48"/>
@@ -7755,7 +7910,9 @@
       <c r="AD14" s="48">
         <v>169</v>
       </c>
-      <c r="AE14" s="48"/>
+      <c r="AE14" s="48">
+        <v>170</v>
+      </c>
       <c r="AF14" s="48"/>
       <c r="AG14" s="48"/>
       <c r="AH14" s="48"/>
@@ -7865,7 +8022,9 @@
       <c r="AD15" s="48">
         <v>104</v>
       </c>
-      <c r="AE15" s="48"/>
+      <c r="AE15" s="48">
+        <v>105</v>
+      </c>
       <c r="AF15" s="48"/>
       <c r="AG15" s="48"/>
       <c r="AH15" s="48"/>
@@ -7975,7 +8134,9 @@
       <c r="AD16" s="48">
         <v>181</v>
       </c>
-      <c r="AE16" s="48"/>
+      <c r="AE16" s="48">
+        <v>182</v>
+      </c>
       <c r="AF16" s="48"/>
       <c r="AG16" s="48"/>
       <c r="AH16" s="48"/>
@@ -8135,7 +8296,9 @@
       <c r="AD18" s="48">
         <v>912</v>
       </c>
-      <c r="AE18" s="48"/>
+      <c r="AE18" s="48">
+        <v>919</v>
+      </c>
       <c r="AF18" s="48"/>
       <c r="AG18" s="48"/>
       <c r="AH18" s="48"/>
@@ -8170,7 +8333,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AD20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AE20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -8281,7 +8444,10 @@
         <f t="shared" si="0"/>
         <v>29560</v>
       </c>
-      <c r="AE20" s="48"/>
+      <c r="AE20" s="51">
+        <f t="shared" si="0"/>
+        <v>29798</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8470,8 +8636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8553,43 +8719,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="296" t="s">
+      <c r="B8" s="305" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="296"/>
+      <c r="B9" s="305"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="296"/>
+      <c r="B10" s="305"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="296"/>
+      <c r="B11" s="305"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="297" t="s">
+      <c r="B12" s="306" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="297"/>
+      <c r="B13" s="306"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="297"/>
+      <c r="B14" s="306"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="298" t="s">
+      <c r="B15" s="307" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="298"/>
+      <c r="B16" s="307"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 1st
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426EC641-973D-D14A-AFFF-B5369C63DC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEF2CCC-2A1C-534D-A1F5-4D59D870E064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="308">
+  <cellXfs count="317">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1368,7 +1368,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1432,6 +1458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1751,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2694,31 +2721,31 @@
       <c r="A30" s="15">
         <v>44011</v>
       </c>
-      <c r="B30" s="287">
+      <c r="B30" s="286">
         <v>220657</v>
       </c>
-      <c r="C30" s="288">
+      <c r="C30" s="287">
         <v>279035</v>
       </c>
-      <c r="D30" s="289">
+      <c r="D30" s="288">
         <v>66910</v>
       </c>
-      <c r="E30" s="290">
+      <c r="E30" s="289">
         <v>27121</v>
       </c>
-      <c r="F30" s="291">
+      <c r="F30" s="290">
         <v>30.951204811086892</v>
       </c>
-      <c r="G30" s="292">
+      <c r="G30" s="291">
         <v>68296</v>
       </c>
-      <c r="H30" s="293">
+      <c r="H30" s="292">
         <v>5822</v>
       </c>
-      <c r="I30" s="294">
+      <c r="I30" s="293">
         <v>6549</v>
       </c>
-      <c r="J30" s="295">
+      <c r="J30" s="294">
         <v>566602</v>
       </c>
     </row>
@@ -2726,32 +2753,64 @@
       <c r="A31" s="15">
         <v>44012</v>
       </c>
-      <c r="B31" s="296">
+      <c r="B31" s="295">
         <v>226089</v>
       </c>
-      <c r="C31" s="297">
+      <c r="C31" s="296">
         <v>283450</v>
       </c>
-      <c r="D31" s="298">
+      <c r="D31" s="297">
         <v>72041</v>
       </c>
-      <c r="E31" s="299">
+      <c r="E31" s="298">
         <v>27769</v>
       </c>
-      <c r="F31" s="300">
+      <c r="F31" s="299">
         <v>30.779029497233388</v>
       </c>
-      <c r="G31" s="301">
+      <c r="G31" s="300">
         <v>69588</v>
       </c>
-      <c r="H31" s="302">
+      <c r="H31" s="301">
         <v>5961</v>
       </c>
-      <c r="I31" s="303">
+      <c r="I31" s="302">
         <v>6725</v>
       </c>
-      <c r="J31" s="304">
+      <c r="J31" s="303">
         <v>581580</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="15">
+        <v>44013</v>
+      </c>
+      <c r="B32" s="304">
+        <v>231770</v>
+      </c>
+      <c r="C32" s="305">
+        <v>289142</v>
+      </c>
+      <c r="D32" s="306">
+        <v>75005</v>
+      </c>
+      <c r="E32" s="307">
+        <v>28510</v>
+      </c>
+      <c r="F32" s="308">
+        <v>30.733054321094187</v>
+      </c>
+      <c r="G32" s="309">
+        <v>71230</v>
+      </c>
+      <c r="H32" s="310">
+        <v>6092</v>
+      </c>
+      <c r="I32" s="311">
+        <v>6898</v>
+      </c>
+      <c r="J32" s="312">
+        <v>595917</v>
       </c>
     </row>
   </sheetData>
@@ -2764,8 +2823,8 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3903,18 +3962,42 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
+      <c r="A32" s="218">
+        <v>44013</v>
+      </c>
+      <c r="B32" s="48">
+        <v>0</v>
+      </c>
+      <c r="C32" s="48">
+        <v>1</v>
+      </c>
+      <c r="D32" s="48">
+        <v>1</v>
+      </c>
+      <c r="E32" s="48">
+        <v>1</v>
+      </c>
+      <c r="F32" s="48">
+        <v>1</v>
+      </c>
+      <c r="G32" s="48">
+        <v>0</v>
+      </c>
+      <c r="H32" s="48">
+        <v>1</v>
+      </c>
+      <c r="I32" s="48">
+        <v>0</v>
+      </c>
+      <c r="J32" s="48">
+        <v>1</v>
+      </c>
+      <c r="K32" s="48">
+        <v>0</v>
+      </c>
+      <c r="L32" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
@@ -3997,7 +4080,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5313,9 +5396,15 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
+      <c r="A32" s="47">
+        <v>44013</v>
+      </c>
+      <c r="B32" s="48">
+        <v>0</v>
+      </c>
+      <c r="C32" s="48">
+        <v>1</v>
+      </c>
       <c r="D32" s="48"/>
       <c r="E32" s="48"/>
       <c r="F32" s="48"/>
@@ -5387,7 +5476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6393,16 +6482,36 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="286"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
+      <c r="A32" s="47">
+        <v>44013</v>
+      </c>
+      <c r="B32" s="48">
+        <v>0</v>
+      </c>
+      <c r="C32" s="48">
+        <v>0</v>
+      </c>
+      <c r="D32" s="48">
+        <v>0</v>
+      </c>
+      <c r="E32" s="48">
+        <v>0</v>
+      </c>
+      <c r="F32" s="48">
+        <v>2</v>
+      </c>
+      <c r="G32" s="48">
+        <v>1</v>
+      </c>
+      <c r="H32" s="48">
+        <v>1</v>
+      </c>
+      <c r="I32" s="48">
+        <v>1</v>
+      </c>
+      <c r="J32" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="107"/>
@@ -6416,8 +6525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20:AE20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6519,7 +6628,9 @@
       <c r="AE1" s="49">
         <v>44012</v>
       </c>
-      <c r="AF1" s="48"/>
+      <c r="AF1" s="49">
+        <v>44013</v>
+      </c>
       <c r="AG1" s="48"/>
       <c r="AH1" s="48"/>
       <c r="AI1" s="48"/>
@@ -6631,7 +6742,9 @@
       <c r="AE2" s="48">
         <v>3977</v>
       </c>
-      <c r="AF2" s="48"/>
+      <c r="AF2" s="48">
+        <v>4009</v>
+      </c>
       <c r="AG2" s="48"/>
       <c r="AH2" s="48"/>
       <c r="AI2" s="48"/>
@@ -6743,7 +6856,9 @@
       <c r="AE3" s="48">
         <v>3792</v>
       </c>
-      <c r="AF3" s="48"/>
+      <c r="AF3" s="48">
+        <v>3824</v>
+      </c>
       <c r="AG3" s="48"/>
       <c r="AH3" s="48"/>
       <c r="AI3" s="48"/>
@@ -6855,7 +6970,9 @@
       <c r="AE4" s="48">
         <v>3792</v>
       </c>
-      <c r="AF4" s="48"/>
+      <c r="AF4" s="48">
+        <v>3824</v>
+      </c>
       <c r="AG4" s="48"/>
       <c r="AH4" s="48"/>
       <c r="AI4" s="48"/>
@@ -6967,7 +7084,9 @@
       <c r="AE5" s="48">
         <v>3792</v>
       </c>
-      <c r="AF5" s="48"/>
+      <c r="AF5" s="48">
+        <v>3824</v>
+      </c>
       <c r="AG5" s="48"/>
       <c r="AH5" s="48"/>
       <c r="AI5" s="48"/>
@@ -7079,7 +7198,9 @@
       <c r="AE6" s="48">
         <v>3792</v>
       </c>
-      <c r="AF6" s="48"/>
+      <c r="AF6" s="48">
+        <v>3824</v>
+      </c>
       <c r="AG6" s="48"/>
       <c r="AH6" s="48"/>
       <c r="AI6" s="48"/>
@@ -7191,7 +7312,9 @@
       <c r="AE7" s="48">
         <v>2983</v>
       </c>
-      <c r="AF7" s="48"/>
+      <c r="AF7" s="48">
+        <v>3015</v>
+      </c>
       <c r="AG7" s="48"/>
       <c r="AH7" s="48"/>
       <c r="AI7" s="48"/>
@@ -7303,7 +7426,9 @@
       <c r="AE8" s="48">
         <v>5614</v>
       </c>
-      <c r="AF8" s="48"/>
+      <c r="AF8" s="48">
+        <v>5646</v>
+      </c>
       <c r="AG8" s="48"/>
       <c r="AH8" s="48"/>
       <c r="AI8" s="48"/>
@@ -7352,8 +7477,8 @@
       <c r="AB9" s="78"/>
       <c r="AC9" s="78"/>
       <c r="AD9" s="78"/>
-      <c r="AE9" s="78"/>
-      <c r="AF9" s="48"/>
+      <c r="AE9" s="316"/>
+      <c r="AF9" s="316"/>
       <c r="AG9" s="48"/>
       <c r="AH9" s="48"/>
       <c r="AI9" s="48"/>
@@ -7465,7 +7590,9 @@
       <c r="AE10" s="48">
         <v>170</v>
       </c>
-      <c r="AF10" s="48"/>
+      <c r="AF10" s="48">
+        <v>171</v>
+      </c>
       <c r="AG10" s="48"/>
       <c r="AH10" s="48"/>
       <c r="AI10" s="48"/>
@@ -7577,7 +7704,9 @@
       <c r="AE11" s="48">
         <v>170</v>
       </c>
-      <c r="AF11" s="48"/>
+      <c r="AF11" s="48">
+        <v>171</v>
+      </c>
       <c r="AG11" s="48"/>
       <c r="AH11" s="48"/>
       <c r="AI11" s="48"/>
@@ -7689,7 +7818,9 @@
       <c r="AE12" s="48">
         <v>170</v>
       </c>
-      <c r="AF12" s="48"/>
+      <c r="AF12" s="48">
+        <v>171</v>
+      </c>
       <c r="AG12" s="48"/>
       <c r="AH12" s="48"/>
       <c r="AI12" s="48"/>
@@ -7801,7 +7932,9 @@
       <c r="AE13" s="48">
         <v>170</v>
       </c>
-      <c r="AF13" s="48"/>
+      <c r="AF13" s="48">
+        <v>171</v>
+      </c>
       <c r="AG13" s="48"/>
       <c r="AH13" s="48"/>
       <c r="AI13" s="48"/>
@@ -7913,7 +8046,9 @@
       <c r="AE14" s="48">
         <v>170</v>
       </c>
-      <c r="AF14" s="48"/>
+      <c r="AF14" s="48">
+        <v>171</v>
+      </c>
       <c r="AG14" s="48"/>
       <c r="AH14" s="48"/>
       <c r="AI14" s="48"/>
@@ -8025,7 +8160,9 @@
       <c r="AE15" s="48">
         <v>105</v>
       </c>
-      <c r="AF15" s="48"/>
+      <c r="AF15" s="48">
+        <v>106</v>
+      </c>
       <c r="AG15" s="48"/>
       <c r="AH15" s="48"/>
       <c r="AI15" s="48"/>
@@ -8137,7 +8274,9 @@
       <c r="AE16" s="48">
         <v>182</v>
       </c>
-      <c r="AF16" s="48"/>
+      <c r="AF16" s="48">
+        <v>183</v>
+      </c>
       <c r="AG16" s="48"/>
       <c r="AH16" s="48"/>
       <c r="AI16" s="48"/>
@@ -8186,8 +8325,8 @@
       <c r="AB17" s="78"/>
       <c r="AC17" s="78"/>
       <c r="AD17" s="78"/>
-      <c r="AE17" s="78"/>
-      <c r="AF17" s="48"/>
+      <c r="AE17" s="316"/>
+      <c r="AF17" s="316"/>
       <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
@@ -8299,7 +8438,9 @@
       <c r="AE18" s="48">
         <v>919</v>
       </c>
-      <c r="AF18" s="48"/>
+      <c r="AF18" s="48">
+        <v>926</v>
+      </c>
       <c r="AG18" s="48"/>
       <c r="AH18" s="48"/>
       <c r="AI18" s="48"/>
@@ -8636,7 +8777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
@@ -8719,43 +8860,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="305" t="s">
+      <c r="B8" s="313" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="305"/>
+      <c r="B9" s="313"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="305"/>
+      <c r="B10" s="313"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="305"/>
+      <c r="B11" s="313"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="306" t="s">
+      <c r="B12" s="314" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="306"/>
+      <c r="B13" s="314"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="306"/>
+      <c r="B14" s="314"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="307" t="s">
+      <c r="B15" s="315" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="307"/>
+      <c r="B16" s="315"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 2nd
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEF2CCC-2A1C-534D-A1F5-4D59D870E064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D639E84C-F2F9-784C-A2A2-8565931F3EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -843,7 +843,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -1449,6 +1448,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1458,7 +1485,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1778,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2113,31 +2139,31 @@
       <c r="A11" s="15">
         <v>43992</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="107">
         <v>129184</v>
       </c>
-      <c r="C11" s="109">
+      <c r="C11" s="108">
         <v>186570</v>
       </c>
-      <c r="D11" s="110">
+      <c r="D11" s="109">
         <v>53608</v>
       </c>
-      <c r="E11" s="111">
+      <c r="E11" s="110">
         <v>15357</v>
       </c>
-      <c r="F11" s="112">
+      <c r="F11" s="111">
         <v>33.110137478325491</v>
       </c>
-      <c r="G11" s="113">
+      <c r="G11" s="112">
         <v>42773</v>
       </c>
-      <c r="H11" s="114">
+      <c r="H11" s="113">
         <v>3970</v>
       </c>
-      <c r="I11" s="115">
+      <c r="I11" s="114">
         <v>4126</v>
       </c>
-      <c r="J11" s="116">
+      <c r="J11" s="115">
         <v>369362</v>
       </c>
     </row>
@@ -2145,31 +2171,31 @@
       <c r="A12" s="15">
         <v>43993</v>
       </c>
-      <c r="B12" s="117">
+      <c r="B12" s="116">
         <v>133974</v>
       </c>
-      <c r="C12" s="118">
+      <c r="C12" s="117">
         <v>191465</v>
       </c>
-      <c r="D12" s="119">
+      <c r="D12" s="118">
         <v>55700</v>
       </c>
-      <c r="E12" s="120">
+      <c r="E12" s="119">
         <v>15944</v>
       </c>
-      <c r="F12" s="121">
+      <c r="F12" s="120">
         <v>33.006404227685969</v>
       </c>
-      <c r="G12" s="122">
+      <c r="G12" s="121">
         <v>44220</v>
       </c>
-      <c r="H12" s="123">
+      <c r="H12" s="122">
         <v>4087</v>
       </c>
-      <c r="I12" s="124">
+      <c r="I12" s="123">
         <v>4256</v>
       </c>
-      <c r="J12" s="125">
+      <c r="J12" s="124">
         <v>381139</v>
       </c>
     </row>
@@ -2177,31 +2203,31 @@
       <c r="A13" s="15">
         <v>43994</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="125">
         <v>139196</v>
       </c>
-      <c r="C13" s="127">
+      <c r="C13" s="126">
         <v>197590</v>
       </c>
-      <c r="D13" s="128">
+      <c r="D13" s="127">
         <v>56928</v>
       </c>
-      <c r="E13" s="129">
+      <c r="E13" s="128">
         <v>16448</v>
       </c>
-      <c r="F13" s="130">
+      <c r="F13" s="129">
         <v>32.77824075404466</v>
       </c>
-      <c r="G13" s="131">
+      <c r="G13" s="130">
         <v>45626</v>
       </c>
-      <c r="H13" s="132">
+      <c r="H13" s="131">
         <v>4198</v>
       </c>
-      <c r="I13" s="133">
+      <c r="I13" s="132">
         <v>4369</v>
       </c>
-      <c r="J13" s="134">
+      <c r="J13" s="133">
         <v>393714</v>
       </c>
     </row>
@@ -2209,31 +2235,31 @@
       <c r="A14" s="15">
         <v>43995</v>
       </c>
-      <c r="B14" s="135">
+      <c r="B14" s="134">
         <v>142690</v>
       </c>
-      <c r="C14" s="136">
+      <c r="C14" s="135">
         <v>202139</v>
       </c>
-      <c r="D14" s="137">
+      <c r="D14" s="136">
         <v>56926</v>
       </c>
-      <c r="E14" s="138">
+      <c r="E14" s="137">
         <v>16872</v>
       </c>
-      <c r="F14" s="139">
+      <c r="F14" s="138">
         <v>32.661714205620576</v>
       </c>
-      <c r="G14" s="140">
+      <c r="G14" s="139">
         <v>46605</v>
       </c>
-      <c r="H14" s="141">
+      <c r="H14" s="140">
         <v>4248</v>
       </c>
-      <c r="I14" s="142">
+      <c r="I14" s="141">
         <v>4426</v>
       </c>
-      <c r="J14" s="143">
+      <c r="J14" s="142">
         <v>401755</v>
       </c>
     </row>
@@ -2241,31 +2267,31 @@
       <c r="A15" s="15">
         <v>43996</v>
       </c>
-      <c r="B15" s="144">
+      <c r="B15" s="143">
         <v>146837</v>
       </c>
-      <c r="C15" s="145">
+      <c r="C15" s="144">
         <v>207076</v>
       </c>
-      <c r="D15" s="146">
+      <c r="D15" s="145">
         <v>52636</v>
       </c>
-      <c r="E15" s="147">
+      <c r="E15" s="146">
         <v>17141</v>
       </c>
-      <c r="F15" s="148">
+      <c r="F15" s="147">
         <v>32.503388110626069</v>
       </c>
-      <c r="G15" s="149">
+      <c r="G15" s="148">
         <v>47727</v>
       </c>
-      <c r="H15" s="150">
+      <c r="H15" s="149">
         <v>4323</v>
       </c>
-      <c r="I15" s="151">
+      <c r="I15" s="150">
         <v>4483</v>
       </c>
-      <c r="J15" s="152">
+      <c r="J15" s="151">
         <v>406549</v>
       </c>
     </row>
@@ -2273,31 +2299,31 @@
       <c r="A16" s="15">
         <v>43997</v>
       </c>
-      <c r="B16" s="153">
+      <c r="B16" s="152">
         <v>150264</v>
       </c>
-      <c r="C16" s="154">
+      <c r="C16" s="153">
         <v>211616</v>
       </c>
-      <c r="D16" s="155">
+      <c r="D16" s="154">
         <v>53217</v>
       </c>
-      <c r="E16" s="156">
+      <c r="E16" s="155">
         <v>17580</v>
       </c>
-      <c r="F16" s="157">
+      <c r="F16" s="156">
         <v>32.357051589203003</v>
       </c>
-      <c r="G16" s="158">
+      <c r="G16" s="157">
         <v>48621</v>
       </c>
-      <c r="H16" s="159">
+      <c r="H16" s="158">
         <v>4387</v>
       </c>
-      <c r="I16" s="160">
+      <c r="I16" s="159">
         <v>4555</v>
       </c>
-      <c r="J16" s="161">
+      <c r="J16" s="160">
         <v>415097</v>
       </c>
     </row>
@@ -2305,31 +2331,31 @@
       <c r="A17" s="15">
         <v>43998</v>
       </c>
-      <c r="B17" s="162">
+      <c r="B17" s="161">
         <v>154863</v>
       </c>
-      <c r="C17" s="163">
+      <c r="C17" s="162">
         <v>216857</v>
       </c>
-      <c r="D17" s="164">
+      <c r="D17" s="163">
         <v>56843</v>
       </c>
-      <c r="E17" s="165">
+      <c r="E17" s="164">
         <v>18310</v>
       </c>
-      <c r="F17" s="166">
+      <c r="F17" s="165">
         <v>32.287247438058152</v>
       </c>
-      <c r="G17" s="167">
+      <c r="G17" s="166">
         <v>50001</v>
       </c>
-      <c r="H17" s="168">
+      <c r="H17" s="167">
         <v>4540</v>
       </c>
-      <c r="I17" s="169">
+      <c r="I17" s="168">
         <v>4700</v>
       </c>
-      <c r="J17" s="170">
+      <c r="J17" s="169">
         <v>428563</v>
       </c>
     </row>
@@ -2337,31 +2363,31 @@
       <c r="A18" s="15">
         <v>43999</v>
       </c>
-      <c r="B18" s="172">
+      <c r="B18" s="171">
         <v>159793</v>
       </c>
-      <c r="C18" s="173">
+      <c r="C18" s="172">
         <v>222801</v>
       </c>
-      <c r="D18" s="174">
+      <c r="D18" s="173">
         <v>59076</v>
       </c>
-      <c r="E18" s="175">
+      <c r="E18" s="174">
         <v>19080</v>
       </c>
-      <c r="F18" s="176">
+      <c r="F18" s="175">
         <v>32.055221442741548</v>
       </c>
-      <c r="G18" s="177">
+      <c r="G18" s="176">
         <v>51222</v>
       </c>
-      <c r="H18" s="178">
+      <c r="H18" s="177">
         <v>4654</v>
       </c>
-      <c r="I18" s="179">
+      <c r="I18" s="178">
         <v>4828</v>
       </c>
-      <c r="J18" s="180">
+      <c r="J18" s="179">
         <v>441670</v>
       </c>
     </row>
@@ -2369,31 +2395,31 @@
       <c r="A19" s="15">
         <v>44000</v>
       </c>
-      <c r="B19" s="181">
+      <c r="B19" s="180">
         <v>165455</v>
       </c>
-      <c r="C19" s="182">
+      <c r="C19" s="181">
         <v>228248</v>
       </c>
-      <c r="D19" s="183">
+      <c r="D19" s="182">
         <v>59778</v>
       </c>
-      <c r="E19" s="184">
+      <c r="E19" s="183">
         <v>19747</v>
       </c>
-      <c r="F19" s="185">
+      <c r="F19" s="184">
         <v>31.855791604968118</v>
       </c>
-      <c r="G19" s="186">
+      <c r="G19" s="185">
         <v>52707</v>
       </c>
-      <c r="H19" s="187">
+      <c r="H19" s="186">
         <v>4758</v>
       </c>
-      <c r="I19" s="188">
+      <c r="I19" s="187">
         <v>4939</v>
       </c>
-      <c r="J19" s="189">
+      <c r="J19" s="188">
         <v>453481</v>
       </c>
     </row>
@@ -2401,31 +2427,31 @@
       <c r="A20" s="15">
         <v>44001</v>
       </c>
-      <c r="B20" s="190">
+      <c r="B20" s="189">
         <v>170485</v>
       </c>
-      <c r="C20" s="191">
+      <c r="C20" s="190">
         <v>233137</v>
       </c>
-      <c r="D20" s="192">
+      <c r="D20" s="191">
         <v>62245</v>
       </c>
-      <c r="E20" s="193">
+      <c r="E20" s="192">
         <v>20394</v>
       </c>
-      <c r="F20" s="194">
+      <c r="F20" s="193">
         <v>31.724198609848376</v>
       </c>
-      <c r="G20" s="195">
+      <c r="G20" s="194">
         <v>54085</v>
       </c>
-      <c r="H20" s="196">
+      <c r="H20" s="195">
         <v>4876</v>
       </c>
-      <c r="I20" s="197">
+      <c r="I20" s="196">
         <v>5058</v>
       </c>
-      <c r="J20" s="198">
+      <c r="J20" s="197">
         <v>465867</v>
       </c>
     </row>
@@ -2433,31 +2459,31 @@
       <c r="A21" s="15">
         <v>44002</v>
       </c>
-      <c r="B21" s="199">
+      <c r="B21" s="198">
         <v>175202</v>
       </c>
-      <c r="C21" s="200">
+      <c r="C21" s="199">
         <v>238129</v>
       </c>
-      <c r="D21" s="201">
+      <c r="D21" s="200">
         <v>60621</v>
       </c>
-      <c r="E21" s="202">
+      <c r="E21" s="201">
         <v>20781</v>
       </c>
-      <c r="F21" s="203">
+      <c r="F21" s="202">
         <v>31.456261914818324</v>
       </c>
-      <c r="G21" s="204">
+      <c r="G21" s="203">
         <v>55112</v>
       </c>
-      <c r="H21" s="205">
+      <c r="H21" s="204">
         <v>4951</v>
       </c>
-      <c r="I21" s="206">
+      <c r="I21" s="205">
         <v>5117</v>
       </c>
-      <c r="J21" s="207">
+      <c r="J21" s="206">
         <v>473952</v>
       </c>
     </row>
@@ -2465,31 +2491,31 @@
       <c r="A22" s="15">
         <v>44003</v>
       </c>
-      <c r="B22" s="208">
+      <c r="B22" s="207">
         <v>180545</v>
       </c>
-      <c r="C22" s="209">
+      <c r="C22" s="208">
         <v>242393</v>
       </c>
-      <c r="D22" s="210">
+      <c r="D22" s="209">
         <v>56590</v>
       </c>
-      <c r="E22" s="211">
+      <c r="E22" s="210">
         <v>21825</v>
       </c>
-      <c r="F22" s="212">
+      <c r="F22" s="211">
         <v>31.609847960342297</v>
       </c>
-      <c r="G22" s="213">
+      <c r="G22" s="212">
         <v>57070</v>
       </c>
-      <c r="H22" s="214">
+      <c r="H22" s="213">
         <v>5029</v>
       </c>
-      <c r="I22" s="215">
+      <c r="I22" s="214">
         <v>5191</v>
       </c>
-      <c r="J22" s="216">
+      <c r="J22" s="215">
         <v>479528</v>
       </c>
     </row>
@@ -2497,31 +2523,31 @@
       <c r="A23" s="15">
         <v>44004</v>
       </c>
-      <c r="B23" s="220">
+      <c r="B23" s="219">
         <v>185122</v>
       </c>
-      <c r="C23" s="221">
+      <c r="C23" s="220">
         <v>246147</v>
       </c>
-      <c r="D23" s="222">
+      <c r="D23" s="221">
         <v>57281</v>
       </c>
-      <c r="E23" s="223">
+      <c r="E23" s="222">
         <v>22584</v>
       </c>
-      <c r="F23" s="224">
+      <c r="F23" s="223">
         <v>31.687751860934949</v>
       </c>
-      <c r="G23" s="225">
+      <c r="G23" s="224">
         <v>58661</v>
       </c>
-      <c r="H23" s="226">
+      <c r="H23" s="225">
         <v>5112</v>
       </c>
-      <c r="I23" s="227">
+      <c r="I23" s="226">
         <v>5280</v>
       </c>
-      <c r="J23" s="228">
+      <c r="J23" s="227">
         <v>488550</v>
       </c>
     </row>
@@ -2529,31 +2555,31 @@
       <c r="A24" s="15">
         <v>44005</v>
       </c>
-      <c r="B24" s="232">
+      <c r="B24" s="231">
         <v>191410</v>
       </c>
-      <c r="C24" s="233">
+      <c r="C24" s="232">
         <v>251355</v>
       </c>
-      <c r="D24" s="234">
+      <c r="D24" s="233">
         <v>59106</v>
       </c>
-      <c r="E24" s="235">
+      <c r="E24" s="234">
         <v>23377</v>
       </c>
-      <c r="F24" s="236">
+      <c r="F24" s="235">
         <v>31.598140118071154</v>
       </c>
-      <c r="G24" s="237">
+      <c r="G24" s="236">
         <v>60482</v>
       </c>
-      <c r="H24" s="238">
+      <c r="H24" s="237">
         <v>5219</v>
       </c>
-      <c r="I24" s="239">
+      <c r="I24" s="238">
         <v>5402</v>
       </c>
-      <c r="J24" s="240">
+      <c r="J24" s="239">
         <v>501871</v>
       </c>
     </row>
@@ -2561,31 +2587,31 @@
       <c r="A25" s="15">
         <v>44006</v>
       </c>
-      <c r="B25" s="241">
+      <c r="B25" s="240">
         <v>196847</v>
       </c>
-      <c r="C25" s="242">
+      <c r="C25" s="241">
         <v>256336</v>
       </c>
-      <c r="D25" s="243">
+      <c r="D25" s="242">
         <v>62475</v>
       </c>
-      <c r="E25" s="244">
+      <c r="E25" s="243">
         <v>24324</v>
       </c>
-      <c r="F25" s="245">
+      <c r="F25" s="244">
         <v>31.576300375418469</v>
       </c>
-      <c r="G25" s="246">
+      <c r="G25" s="245">
         <v>62157</v>
       </c>
-      <c r="H25" s="247">
+      <c r="H25" s="246">
         <v>5350</v>
       </c>
-      <c r="I25" s="248">
+      <c r="I25" s="247">
         <v>5532</v>
       </c>
-      <c r="J25" s="249">
+      <c r="J25" s="248">
         <v>515658</v>
       </c>
     </row>
@@ -2593,31 +2619,31 @@
       <c r="A26" s="15">
         <v>44007</v>
       </c>
-      <c r="B26" s="250">
+      <c r="B26" s="249">
         <v>202951</v>
       </c>
-      <c r="C26" s="251">
+      <c r="C26" s="250">
         <v>262117</v>
       </c>
-      <c r="D26" s="252">
+      <c r="D26" s="251">
         <v>63583</v>
       </c>
-      <c r="E26" s="253">
+      <c r="E26" s="252">
         <v>25060</v>
       </c>
-      <c r="F26" s="254">
+      <c r="F26" s="253">
         <v>31.457839577040765</v>
       </c>
-      <c r="G26" s="255">
+      <c r="G26" s="254">
         <v>63844</v>
       </c>
-      <c r="H26" s="256">
+      <c r="H26" s="255">
         <v>5483</v>
       </c>
-      <c r="I26" s="257">
+      <c r="I26" s="256">
         <v>5681</v>
       </c>
-      <c r="J26" s="258">
+      <c r="J26" s="257">
         <v>528651</v>
       </c>
     </row>
@@ -2625,31 +2651,31 @@
       <c r="A27" s="15">
         <v>44008</v>
       </c>
-      <c r="B27" s="259">
+      <c r="B27" s="258">
         <v>208392</v>
       </c>
-      <c r="C27" s="260">
+      <c r="C27" s="259">
         <v>267288</v>
       </c>
-      <c r="D27" s="261">
+      <c r="D27" s="260">
         <v>66440</v>
       </c>
-      <c r="E27" s="262">
+      <c r="E27" s="261">
         <v>25779</v>
       </c>
-      <c r="F27" s="263">
+      <c r="F27" s="262">
         <v>31.374524933778648</v>
       </c>
-      <c r="G27" s="264">
+      <c r="G27" s="263">
         <v>65382</v>
       </c>
-      <c r="H27" s="265">
+      <c r="H27" s="264">
         <v>5570</v>
       </c>
-      <c r="I27" s="266">
+      <c r="I27" s="265">
         <v>5844</v>
       </c>
-      <c r="J27" s="267">
+      <c r="J27" s="266">
         <v>542120</v>
       </c>
     </row>
@@ -2657,31 +2683,31 @@
       <c r="A28" s="15">
         <v>44009</v>
       </c>
-      <c r="B28" s="268">
+      <c r="B28" s="267">
         <v>212802</v>
       </c>
-      <c r="C28" s="269">
+      <c r="C28" s="268">
         <v>271151</v>
       </c>
-      <c r="D28" s="270">
+      <c r="D28" s="269">
         <v>67099</v>
       </c>
-      <c r="E28" s="271">
+      <c r="E28" s="270">
         <v>26381</v>
       </c>
-      <c r="F28" s="272">
+      <c r="F28" s="271">
         <v>31.241247732634093</v>
       </c>
-      <c r="G28" s="273">
+      <c r="G28" s="272">
         <v>66482</v>
       </c>
-      <c r="H28" s="274">
+      <c r="H28" s="273">
         <v>5661</v>
       </c>
-      <c r="I28" s="275">
+      <c r="I28" s="274">
         <v>6361</v>
       </c>
-      <c r="J28" s="276">
+      <c r="J28" s="275">
         <v>551052</v>
       </c>
     </row>
@@ -2689,31 +2715,31 @@
       <c r="A29" s="15">
         <v>44010</v>
       </c>
-      <c r="B29" s="277">
+      <c r="B29" s="276">
         <v>216852</v>
       </c>
-      <c r="C29" s="278">
+      <c r="C29" s="277">
         <v>275203</v>
       </c>
-      <c r="D29" s="279">
+      <c r="D29" s="278">
         <v>64143</v>
       </c>
-      <c r="E29" s="280">
+      <c r="E29" s="279">
         <v>26648</v>
       </c>
-      <c r="F29" s="281">
+      <c r="F29" s="280">
         <v>31.106930072122925</v>
       </c>
-      <c r="G29" s="282">
+      <c r="G29" s="281">
         <v>67456</v>
       </c>
-      <c r="H29" s="283">
+      <c r="H29" s="282">
         <v>5718</v>
       </c>
-      <c r="I29" s="284">
+      <c r="I29" s="283">
         <v>6432</v>
       </c>
-      <c r="J29" s="285">
+      <c r="J29" s="284">
         <v>556198</v>
       </c>
     </row>
@@ -2721,31 +2747,31 @@
       <c r="A30" s="15">
         <v>44011</v>
       </c>
-      <c r="B30" s="286">
+      <c r="B30" s="285">
         <v>220657</v>
       </c>
-      <c r="C30" s="287">
+      <c r="C30" s="286">
         <v>279035</v>
       </c>
-      <c r="D30" s="288">
+      <c r="D30" s="287">
         <v>66910</v>
       </c>
-      <c r="E30" s="289">
+      <c r="E30" s="288">
         <v>27121</v>
       </c>
-      <c r="F30" s="290">
+      <c r="F30" s="289">
         <v>30.951204811086892</v>
       </c>
-      <c r="G30" s="291">
+      <c r="G30" s="290">
         <v>68296</v>
       </c>
-      <c r="H30" s="292">
+      <c r="H30" s="291">
         <v>5822</v>
       </c>
-      <c r="I30" s="293">
+      <c r="I30" s="292">
         <v>6549</v>
       </c>
-      <c r="J30" s="294">
+      <c r="J30" s="293">
         <v>566602</v>
       </c>
     </row>
@@ -2753,31 +2779,31 @@
       <c r="A31" s="15">
         <v>44012</v>
       </c>
-      <c r="B31" s="295">
+      <c r="B31" s="294">
         <v>226089</v>
       </c>
-      <c r="C31" s="296">
+      <c r="C31" s="295">
         <v>283450</v>
       </c>
-      <c r="D31" s="297">
+      <c r="D31" s="296">
         <v>72041</v>
       </c>
-      <c r="E31" s="298">
+      <c r="E31" s="297">
         <v>27769</v>
       </c>
-      <c r="F31" s="299">
+      <c r="F31" s="298">
         <v>30.779029497233388</v>
       </c>
-      <c r="G31" s="300">
+      <c r="G31" s="299">
         <v>69588</v>
       </c>
-      <c r="H31" s="301">
+      <c r="H31" s="300">
         <v>5961</v>
       </c>
-      <c r="I31" s="302">
+      <c r="I31" s="301">
         <v>6725</v>
       </c>
-      <c r="J31" s="303">
+      <c r="J31" s="302">
         <v>581580</v>
       </c>
     </row>
@@ -2785,32 +2811,64 @@
       <c r="A32" s="15">
         <v>44013</v>
       </c>
-      <c r="B32" s="304">
+      <c r="B32" s="303">
         <v>231770</v>
       </c>
-      <c r="C32" s="305">
+      <c r="C32" s="304">
         <v>289142</v>
       </c>
-      <c r="D32" s="306">
+      <c r="D32" s="305">
         <v>75005</v>
       </c>
-      <c r="E32" s="307">
+      <c r="E32" s="306">
         <v>28510</v>
       </c>
-      <c r="F32" s="308">
+      <c r="F32" s="307">
         <v>30.733054321094187</v>
       </c>
-      <c r="G32" s="309">
+      <c r="G32" s="308">
         <v>71230</v>
       </c>
-      <c r="H32" s="310">
+      <c r="H32" s="309">
         <v>6092</v>
       </c>
-      <c r="I32" s="311">
+      <c r="I32" s="310">
         <v>6898</v>
       </c>
-      <c r="J32" s="312">
+      <c r="J32" s="311">
         <v>595917</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="15">
+        <v>44014</v>
+      </c>
+      <c r="B33" s="313">
+        <v>238511</v>
+      </c>
+      <c r="C33" s="314">
+        <v>295561</v>
+      </c>
+      <c r="D33" s="315">
+        <v>76423</v>
+      </c>
+      <c r="E33" s="316">
+        <v>29189</v>
+      </c>
+      <c r="F33" s="317">
+        <v>30.515573705195987</v>
+      </c>
+      <c r="G33" s="318">
+        <v>72783</v>
+      </c>
+      <c r="H33" s="319">
+        <v>6214</v>
+      </c>
+      <c r="I33" s="320">
+        <v>7080</v>
+      </c>
+      <c r="J33" s="321">
+        <v>610495</v>
       </c>
     </row>
   </sheetData>
@@ -2824,7 +2882,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3594,43 +3652,43 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="218">
+      <c r="A22" s="217">
         <v>44003</v>
       </c>
-      <c r="B22" s="217">
-        <v>0</v>
-      </c>
-      <c r="C22" s="217">
-        <v>1</v>
-      </c>
-      <c r="D22" s="217">
-        <v>1</v>
-      </c>
-      <c r="E22" s="217">
-        <v>1</v>
-      </c>
-      <c r="F22" s="217">
-        <v>1</v>
-      </c>
-      <c r="G22" s="217">
-        <v>0</v>
-      </c>
-      <c r="H22" s="217"/>
-      <c r="I22" s="217">
-        <v>0</v>
-      </c>
-      <c r="J22" s="217">
-        <v>1</v>
-      </c>
-      <c r="K22" s="217">
-        <v>0</v>
-      </c>
-      <c r="L22" s="217">
+      <c r="B22" s="216">
+        <v>0</v>
+      </c>
+      <c r="C22" s="216">
+        <v>1</v>
+      </c>
+      <c r="D22" s="216">
+        <v>1</v>
+      </c>
+      <c r="E22" s="216">
+        <v>1</v>
+      </c>
+      <c r="F22" s="216">
+        <v>1</v>
+      </c>
+      <c r="G22" s="216">
+        <v>0</v>
+      </c>
+      <c r="H22" s="216"/>
+      <c r="I22" s="216">
+        <v>0</v>
+      </c>
+      <c r="J22" s="216">
+        <v>1</v>
+      </c>
+      <c r="K22" s="216">
+        <v>0</v>
+      </c>
+      <c r="L22" s="216">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="218">
+      <c r="A23" s="217">
         <v>44004</v>
       </c>
       <c r="B23" s="48">
@@ -3666,7 +3724,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="218">
+      <c r="A24" s="217">
         <v>44005</v>
       </c>
       <c r="B24" s="48">
@@ -3702,7 +3760,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="218">
+      <c r="A25" s="217">
         <v>44006</v>
       </c>
       <c r="B25" s="48">
@@ -3738,7 +3796,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="218">
+      <c r="A26" s="217">
         <v>44007</v>
       </c>
       <c r="B26" s="48">
@@ -3774,7 +3832,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="218">
+      <c r="A27" s="217">
         <v>44008</v>
       </c>
       <c r="B27" s="48">
@@ -3810,7 +3868,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="218">
+      <c r="A28" s="217">
         <v>44009</v>
       </c>
       <c r="B28" s="48">
@@ -3848,7 +3906,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="218">
+      <c r="A29" s="217">
         <v>44010</v>
       </c>
       <c r="B29" s="48">
@@ -3886,7 +3944,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="218">
+      <c r="A30" s="217">
         <v>44011</v>
       </c>
       <c r="B30" s="48">
@@ -3924,7 +3982,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="218">
+      <c r="A31" s="217">
         <v>44012</v>
       </c>
       <c r="B31" s="48">
@@ -3962,7 +4020,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="218">
+      <c r="A32" s="217">
         <v>44013</v>
       </c>
       <c r="B32" s="48">
@@ -4000,18 +4058,42 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
+      <c r="A33" s="217">
+        <v>44014</v>
+      </c>
+      <c r="B33" s="48">
+        <v>0</v>
+      </c>
+      <c r="C33" s="48">
+        <v>1</v>
+      </c>
+      <c r="D33" s="48">
+        <v>1</v>
+      </c>
+      <c r="E33" s="48">
+        <v>1</v>
+      </c>
+      <c r="F33" s="48">
+        <v>1</v>
+      </c>
+      <c r="G33" s="48">
+        <v>0</v>
+      </c>
+      <c r="H33" s="48">
+        <v>1</v>
+      </c>
+      <c r="I33" s="48">
+        <v>0</v>
+      </c>
+      <c r="J33" s="48">
+        <v>1</v>
+      </c>
+      <c r="K33" s="48">
+        <v>0</v>
+      </c>
+      <c r="L33" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
@@ -4080,7 +4162,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5405,33 +5487,83 @@
       <c r="C32" s="48">
         <v>1</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
+      <c r="D32" s="48">
+        <v>1</v>
+      </c>
+      <c r="E32" s="48">
+        <v>0</v>
+      </c>
+      <c r="F32" s="48">
+        <v>1</v>
+      </c>
+      <c r="G32" s="48">
+        <v>1</v>
+      </c>
+      <c r="H32" s="48">
+        <v>1</v>
+      </c>
+      <c r="I32" s="48">
+        <v>0</v>
+      </c>
+      <c r="J32" s="48">
+        <v>1</v>
+      </c>
+      <c r="K32" s="48">
+        <v>1</v>
+      </c>
+      <c r="L32" s="48">
+        <v>1</v>
+      </c>
+      <c r="M32" s="48">
+        <v>0</v>
+      </c>
+      <c r="N32" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
+      <c r="A33" s="47">
+        <v>44014</v>
+      </c>
+      <c r="B33" s="48">
+        <v>0</v>
+      </c>
+      <c r="C33" s="48">
+        <v>1</v>
+      </c>
+      <c r="D33" s="48">
+        <v>1</v>
+      </c>
+      <c r="E33" s="48">
+        <v>0</v>
+      </c>
+      <c r="F33" s="48">
+        <v>1</v>
+      </c>
+      <c r="G33" s="48">
+        <v>1</v>
+      </c>
+      <c r="H33" s="48">
+        <v>1</v>
+      </c>
+      <c r="I33" s="48">
+        <v>0</v>
+      </c>
+      <c r="J33" s="48">
+        <v>1</v>
+      </c>
+      <c r="K33" s="48">
+        <v>1</v>
+      </c>
+      <c r="L33" s="48">
+        <v>1</v>
+      </c>
+      <c r="M33" s="48">
+        <v>0</v>
+      </c>
+      <c r="N33" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
@@ -5476,7 +5608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5877,7 +6009,7 @@
       <c r="A13" s="47">
         <v>43994</v>
       </c>
-      <c r="B13" s="219">
+      <c r="B13" s="218">
         <v>1</v>
       </c>
       <c r="C13" s="48">
@@ -6513,8 +6645,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="107"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="47">
+        <v>44014</v>
+      </c>
+      <c r="B33" s="216">
+        <v>0</v>
+      </c>
+      <c r="C33" s="216">
+        <v>0</v>
+      </c>
+      <c r="D33" s="216">
+        <v>0</v>
+      </c>
+      <c r="E33" s="216">
+        <v>0</v>
+      </c>
+      <c r="F33" s="216">
+        <v>2</v>
+      </c>
+      <c r="G33" s="216">
+        <v>1</v>
+      </c>
+      <c r="H33" s="216">
+        <v>1</v>
+      </c>
+      <c r="I33" s="216">
+        <v>1</v>
+      </c>
+      <c r="J33" s="216">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6525,8 +6686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6598,7 +6759,7 @@
       <c r="U1" s="49">
         <v>44002</v>
       </c>
-      <c r="V1" s="229">
+      <c r="V1" s="228">
         <v>44003</v>
       </c>
       <c r="W1" s="49">
@@ -6631,7 +6792,9 @@
       <c r="AF1" s="49">
         <v>44013</v>
       </c>
-      <c r="AG1" s="48"/>
+      <c r="AG1" s="49">
+        <v>44014</v>
+      </c>
       <c r="AH1" s="48"/>
       <c r="AI1" s="48"/>
       <c r="AJ1" s="48"/>
@@ -6712,10 +6875,10 @@
       <c r="U2" s="48">
         <v>3657</v>
       </c>
-      <c r="V2" s="230">
+      <c r="V2" s="229">
         <v>3689</v>
       </c>
-      <c r="W2" s="231">
+      <c r="W2" s="230">
         <v>3721</v>
       </c>
       <c r="X2" s="48">
@@ -6745,7 +6908,9 @@
       <c r="AF2" s="48">
         <v>4009</v>
       </c>
-      <c r="AG2" s="48"/>
+      <c r="AG2" s="48">
+        <v>4041</v>
+      </c>
       <c r="AH2" s="48"/>
       <c r="AI2" s="48"/>
       <c r="AJ2" s="48"/>
@@ -6826,7 +6991,7 @@
       <c r="U3" s="48">
         <v>3472</v>
       </c>
-      <c r="V3" s="230">
+      <c r="V3" s="229">
         <v>3504</v>
       </c>
       <c r="W3" s="48">
@@ -6859,7 +7024,9 @@
       <c r="AF3" s="48">
         <v>3824</v>
       </c>
-      <c r="AG3" s="48"/>
+      <c r="AG3" s="48">
+        <v>3856</v>
+      </c>
       <c r="AH3" s="48"/>
       <c r="AI3" s="48"/>
       <c r="AJ3" s="48"/>
@@ -6940,7 +7107,7 @@
       <c r="U4" s="48">
         <v>3472</v>
       </c>
-      <c r="V4" s="230">
+      <c r="V4" s="229">
         <v>3504</v>
       </c>
       <c r="W4" s="48">
@@ -6973,7 +7140,9 @@
       <c r="AF4" s="48">
         <v>3824</v>
       </c>
-      <c r="AG4" s="48"/>
+      <c r="AG4" s="48">
+        <v>3856</v>
+      </c>
       <c r="AH4" s="48"/>
       <c r="AI4" s="48"/>
       <c r="AJ4" s="48"/>
@@ -7054,7 +7223,7 @@
       <c r="U5" s="48">
         <v>3472</v>
       </c>
-      <c r="V5" s="230">
+      <c r="V5" s="229">
         <v>3504</v>
       </c>
       <c r="W5" s="48">
@@ -7087,7 +7256,9 @@
       <c r="AF5" s="48">
         <v>3824</v>
       </c>
-      <c r="AG5" s="48"/>
+      <c r="AG5" s="48">
+        <v>3856</v>
+      </c>
       <c r="AH5" s="48"/>
       <c r="AI5" s="48"/>
       <c r="AJ5" s="48"/>
@@ -7168,7 +7339,7 @@
       <c r="U6" s="48">
         <v>3472</v>
       </c>
-      <c r="V6" s="230">
+      <c r="V6" s="229">
         <v>3504</v>
       </c>
       <c r="W6" s="48">
@@ -7201,7 +7372,9 @@
       <c r="AF6" s="48">
         <v>3824</v>
       </c>
-      <c r="AG6" s="48"/>
+      <c r="AG6" s="48">
+        <v>3856</v>
+      </c>
       <c r="AH6" s="48"/>
       <c r="AI6" s="48"/>
       <c r="AJ6" s="48"/>
@@ -7282,7 +7455,7 @@
       <c r="U7" s="48">
         <v>2663</v>
       </c>
-      <c r="V7" s="230">
+      <c r="V7" s="229">
         <v>2695</v>
       </c>
       <c r="W7" s="48">
@@ -7315,7 +7488,9 @@
       <c r="AF7" s="48">
         <v>3015</v>
       </c>
-      <c r="AG7" s="48"/>
+      <c r="AG7" s="48">
+        <v>3047</v>
+      </c>
       <c r="AH7" s="48"/>
       <c r="AI7" s="48"/>
       <c r="AJ7" s="48"/>
@@ -7396,7 +7571,7 @@
       <c r="U8" s="48">
         <v>5294</v>
       </c>
-      <c r="V8" s="230">
+      <c r="V8" s="229">
         <v>5326</v>
       </c>
       <c r="W8" s="48">
@@ -7429,7 +7604,9 @@
       <c r="AF8" s="48">
         <v>5646</v>
       </c>
-      <c r="AG8" s="48"/>
+      <c r="AG8" s="48">
+        <v>5678</v>
+      </c>
       <c r="AH8" s="48"/>
       <c r="AI8" s="48"/>
       <c r="AJ8" s="48"/>
@@ -7477,9 +7654,9 @@
       <c r="AB9" s="78"/>
       <c r="AC9" s="78"/>
       <c r="AD9" s="78"/>
-      <c r="AE9" s="316"/>
-      <c r="AF9" s="316"/>
-      <c r="AG9" s="48"/>
+      <c r="AE9" s="312"/>
+      <c r="AF9" s="312"/>
+      <c r="AG9" s="312"/>
       <c r="AH9" s="48"/>
       <c r="AI9" s="48"/>
       <c r="AJ9" s="48"/>
@@ -7560,7 +7737,7 @@
       <c r="U10" s="48">
         <v>160</v>
       </c>
-      <c r="V10" s="230">
+      <c r="V10" s="229">
         <v>161</v>
       </c>
       <c r="W10" s="48">
@@ -7593,7 +7770,9 @@
       <c r="AF10" s="48">
         <v>171</v>
       </c>
-      <c r="AG10" s="48"/>
+      <c r="AG10" s="48">
+        <v>172</v>
+      </c>
       <c r="AH10" s="48"/>
       <c r="AI10" s="48"/>
       <c r="AJ10" s="48"/>
@@ -7674,7 +7853,7 @@
       <c r="U11" s="48">
         <v>160</v>
       </c>
-      <c r="V11" s="230">
+      <c r="V11" s="229">
         <v>161</v>
       </c>
       <c r="W11" s="48">
@@ -7707,7 +7886,9 @@
       <c r="AF11" s="48">
         <v>171</v>
       </c>
-      <c r="AG11" s="48"/>
+      <c r="AG11" s="48">
+        <v>172</v>
+      </c>
       <c r="AH11" s="48"/>
       <c r="AI11" s="48"/>
       <c r="AJ11" s="48"/>
@@ -7788,7 +7969,7 @@
       <c r="U12" s="48">
         <v>160</v>
       </c>
-      <c r="V12" s="230">
+      <c r="V12" s="229">
         <v>161</v>
       </c>
       <c r="W12" s="48">
@@ -7821,7 +8002,9 @@
       <c r="AF12" s="48">
         <v>171</v>
       </c>
-      <c r="AG12" s="48"/>
+      <c r="AG12" s="48">
+        <v>172</v>
+      </c>
       <c r="AH12" s="48"/>
       <c r="AI12" s="48"/>
       <c r="AJ12" s="48"/>
@@ -7902,7 +8085,7 @@
       <c r="U13" s="48">
         <v>160</v>
       </c>
-      <c r="V13" s="230">
+      <c r="V13" s="229">
         <v>161</v>
       </c>
       <c r="W13" s="48">
@@ -7935,7 +8118,9 @@
       <c r="AF13" s="48">
         <v>171</v>
       </c>
-      <c r="AG13" s="48"/>
+      <c r="AG13" s="48">
+        <v>172</v>
+      </c>
       <c r="AH13" s="48"/>
       <c r="AI13" s="48"/>
       <c r="AJ13" s="48"/>
@@ -8016,7 +8201,7 @@
       <c r="U14" s="48">
         <v>160</v>
       </c>
-      <c r="V14" s="230">
+      <c r="V14" s="229">
         <v>161</v>
       </c>
       <c r="W14" s="48">
@@ -8049,7 +8234,9 @@
       <c r="AF14" s="48">
         <v>171</v>
       </c>
-      <c r="AG14" s="48"/>
+      <c r="AG14" s="48">
+        <v>172</v>
+      </c>
       <c r="AH14" s="48"/>
       <c r="AI14" s="48"/>
       <c r="AJ14" s="48"/>
@@ -8103,16 +8290,16 @@
       <c r="L15" s="48">
         <v>128</v>
       </c>
-      <c r="M15" s="171">
+      <c r="M15" s="170">
         <v>129</v>
       </c>
       <c r="N15" s="48">
         <v>100</v>
       </c>
-      <c r="O15" s="171">
+      <c r="O15" s="170">
         <v>101</v>
       </c>
-      <c r="P15" s="171">
+      <c r="P15" s="170">
         <v>90</v>
       </c>
       <c r="Q15" s="48">
@@ -8130,7 +8317,7 @@
       <c r="U15" s="48">
         <v>95</v>
       </c>
-      <c r="V15" s="230">
+      <c r="V15" s="229">
         <v>96</v>
       </c>
       <c r="W15" s="48">
@@ -8163,7 +8350,9 @@
       <c r="AF15" s="48">
         <v>106</v>
       </c>
-      <c r="AG15" s="48"/>
+      <c r="AG15" s="48">
+        <v>107</v>
+      </c>
       <c r="AH15" s="48"/>
       <c r="AI15" s="48"/>
       <c r="AJ15" s="48"/>
@@ -8244,7 +8433,7 @@
       <c r="U16" s="48">
         <v>172</v>
       </c>
-      <c r="V16" s="230">
+      <c r="V16" s="229">
         <v>173</v>
       </c>
       <c r="W16" s="48">
@@ -8277,7 +8466,9 @@
       <c r="AF16" s="48">
         <v>183</v>
       </c>
-      <c r="AG16" s="48"/>
+      <c r="AG16" s="48">
+        <v>184</v>
+      </c>
       <c r="AH16" s="48"/>
       <c r="AI16" s="48"/>
       <c r="AJ16" s="48"/>
@@ -8325,8 +8516,8 @@
       <c r="AB17" s="78"/>
       <c r="AC17" s="78"/>
       <c r="AD17" s="78"/>
-      <c r="AE17" s="316"/>
-      <c r="AF17" s="316"/>
+      <c r="AE17" s="312"/>
+      <c r="AF17" s="312"/>
       <c r="AG17" s="48"/>
       <c r="AH17" s="48"/>
       <c r="AI17" s="48"/>
@@ -8408,7 +8599,7 @@
       <c r="U18" s="48">
         <v>849</v>
       </c>
-      <c r="V18" s="230">
+      <c r="V18" s="229">
         <v>856</v>
       </c>
       <c r="W18" s="48">
@@ -8441,7 +8632,9 @@
       <c r="AF18" s="48">
         <v>926</v>
       </c>
-      <c r="AG18" s="48"/>
+      <c r="AG18" s="48">
+        <v>933</v>
+      </c>
       <c r="AH18" s="48"/>
       <c r="AI18" s="48"/>
       <c r="AJ18" s="48"/>
@@ -8474,7 +8667,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AE20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AG20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -8588,6 +8781,14 @@
       <c r="AE20" s="51">
         <f t="shared" si="0"/>
         <v>29798</v>
+      </c>
+      <c r="AF20" s="51">
+        <f t="shared" si="0"/>
+        <v>30036</v>
+      </c>
+      <c r="AG20" s="51">
+        <f t="shared" si="0"/>
+        <v>30274</v>
       </c>
     </row>
   </sheetData>
@@ -8860,43 +9061,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="313" t="s">
+      <c r="B8" s="322" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="313"/>
+      <c r="B9" s="322"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="313"/>
+      <c r="B10" s="322"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="313"/>
+      <c r="B11" s="322"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="314" t="s">
+      <c r="B12" s="323" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="314"/>
+      <c r="B13" s="323"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="314"/>
+      <c r="B14" s="323"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="315" t="s">
+      <c r="B15" s="324" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="315"/>
+      <c r="B16" s="324"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for Jul  3rd
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D639E84C-F2F9-784C-A2A2-8565931F3EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C82797A-2311-5745-A4EB-E870DA4C4E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="325">
+  <cellXfs count="335">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1476,6 +1476,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1484,6 +1511,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1804,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2869,6 +2899,38 @@
       </c>
       <c r="J33" s="321">
         <v>610495</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="15">
+        <v>44015</v>
+      </c>
+      <c r="B34" s="322">
+        <v>245251</v>
+      </c>
+      <c r="C34" s="323">
+        <v>301986</v>
+      </c>
+      <c r="D34" s="324">
+        <v>77750</v>
+      </c>
+      <c r="E34" s="325">
+        <v>29843</v>
+      </c>
+      <c r="F34" s="326">
+        <v>30.351762072325904</v>
+      </c>
+      <c r="G34" s="327">
+        <v>74438</v>
+      </c>
+      <c r="H34" s="328">
+        <v>6348</v>
+      </c>
+      <c r="I34" s="329">
+        <v>7259</v>
+      </c>
+      <c r="J34" s="330">
+        <v>624987</v>
       </c>
     </row>
   </sheetData>
@@ -2882,7 +2944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4096,18 +4158,42 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
+      <c r="A34" s="217">
+        <v>44015</v>
+      </c>
+      <c r="B34" s="48">
+        <v>0</v>
+      </c>
+      <c r="C34" s="48">
+        <v>1</v>
+      </c>
+      <c r="D34" s="48">
+        <v>1</v>
+      </c>
+      <c r="E34" s="48">
+        <v>1</v>
+      </c>
+      <c r="F34" s="48">
+        <v>1</v>
+      </c>
+      <c r="G34" s="48">
+        <v>0</v>
+      </c>
+      <c r="H34" s="48">
+        <v>1</v>
+      </c>
+      <c r="I34" s="48">
+        <v>0</v>
+      </c>
+      <c r="J34" s="48">
+        <v>1</v>
+      </c>
+      <c r="K34" s="48">
+        <v>0</v>
+      </c>
+      <c r="L34" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
@@ -4162,7 +4248,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5566,20 +5652,48 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
+      <c r="A34" s="47">
+        <v>44015</v>
+      </c>
+      <c r="B34" s="48">
+        <v>0</v>
+      </c>
+      <c r="C34" s="48">
+        <v>1</v>
+      </c>
+      <c r="D34" s="48">
+        <v>1</v>
+      </c>
+      <c r="E34" s="48">
+        <v>0</v>
+      </c>
+      <c r="F34" s="48">
+        <v>1</v>
+      </c>
+      <c r="G34" s="48">
+        <v>1</v>
+      </c>
+      <c r="H34" s="48">
+        <v>1</v>
+      </c>
+      <c r="I34" s="48">
+        <v>0</v>
+      </c>
+      <c r="J34" s="48">
+        <v>1</v>
+      </c>
+      <c r="K34" s="48">
+        <v>1</v>
+      </c>
+      <c r="L34" s="48">
+        <v>1</v>
+      </c>
+      <c r="M34" s="48">
+        <v>0</v>
+      </c>
+      <c r="N34" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
@@ -5604,11 +5718,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6646,36 +6760,92 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="47">
+      <c r="A33" s="334">
         <v>44014</v>
       </c>
-      <c r="B33" s="216">
-        <v>0</v>
-      </c>
-      <c r="C33" s="216">
-        <v>0</v>
-      </c>
-      <c r="D33" s="216">
-        <v>0</v>
-      </c>
-      <c r="E33" s="216">
-        <v>0</v>
-      </c>
-      <c r="F33" s="216">
+      <c r="B33" s="74">
+        <v>0</v>
+      </c>
+      <c r="C33" s="74">
+        <v>0</v>
+      </c>
+      <c r="D33" s="74">
+        <v>0</v>
+      </c>
+      <c r="E33" s="74">
+        <v>0</v>
+      </c>
+      <c r="F33" s="74">
         <v>2</v>
       </c>
-      <c r="G33" s="216">
-        <v>1</v>
-      </c>
-      <c r="H33" s="216">
-        <v>1</v>
-      </c>
-      <c r="I33" s="216">
-        <v>1</v>
-      </c>
-      <c r="J33" s="216">
+      <c r="G33" s="74">
+        <v>1</v>
+      </c>
+      <c r="H33" s="74">
+        <v>1</v>
+      </c>
+      <c r="I33" s="74">
+        <v>1</v>
+      </c>
+      <c r="J33" s="74">
         <v>2</v>
       </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="334">
+        <v>44015</v>
+      </c>
+      <c r="B34" s="74">
+        <v>0</v>
+      </c>
+      <c r="C34" s="74">
+        <v>0</v>
+      </c>
+      <c r="D34" s="74">
+        <v>0</v>
+      </c>
+      <c r="E34" s="74">
+        <v>0</v>
+      </c>
+      <c r="F34" s="74">
+        <v>2</v>
+      </c>
+      <c r="G34" s="74">
+        <v>1</v>
+      </c>
+      <c r="H34" s="74">
+        <v>1</v>
+      </c>
+      <c r="I34" s="74">
+        <v>1</v>
+      </c>
+      <c r="J34" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6686,8 +6856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6795,7 +6965,9 @@
       <c r="AG1" s="49">
         <v>44014</v>
       </c>
-      <c r="AH1" s="48"/>
+      <c r="AH1" s="49">
+        <v>44015</v>
+      </c>
       <c r="AI1" s="48"/>
       <c r="AJ1" s="48"/>
       <c r="AK1" s="48"/>
@@ -6911,7 +7083,9 @@
       <c r="AG2" s="48">
         <v>4041</v>
       </c>
-      <c r="AH2" s="48"/>
+      <c r="AH2" s="48">
+        <v>4073</v>
+      </c>
       <c r="AI2" s="48"/>
       <c r="AJ2" s="48"/>
       <c r="AK2" s="48"/>
@@ -7027,7 +7201,9 @@
       <c r="AG3" s="48">
         <v>3856</v>
       </c>
-      <c r="AH3" s="48"/>
+      <c r="AH3" s="48">
+        <v>3888</v>
+      </c>
       <c r="AI3" s="48"/>
       <c r="AJ3" s="48"/>
       <c r="AK3" s="48"/>
@@ -7143,7 +7319,9 @@
       <c r="AG4" s="48">
         <v>3856</v>
       </c>
-      <c r="AH4" s="48"/>
+      <c r="AH4" s="48">
+        <v>3888</v>
+      </c>
       <c r="AI4" s="48"/>
       <c r="AJ4" s="48"/>
       <c r="AK4" s="48"/>
@@ -7259,7 +7437,9 @@
       <c r="AG5" s="48">
         <v>3856</v>
       </c>
-      <c r="AH5" s="48"/>
+      <c r="AH5" s="48">
+        <v>3888</v>
+      </c>
       <c r="AI5" s="48"/>
       <c r="AJ5" s="48"/>
       <c r="AK5" s="48"/>
@@ -7375,7 +7555,9 @@
       <c r="AG6" s="48">
         <v>3856</v>
       </c>
-      <c r="AH6" s="48"/>
+      <c r="AH6" s="48">
+        <v>3888</v>
+      </c>
       <c r="AI6" s="48"/>
       <c r="AJ6" s="48"/>
       <c r="AK6" s="48"/>
@@ -7491,7 +7673,9 @@
       <c r="AG7" s="48">
         <v>3047</v>
       </c>
-      <c r="AH7" s="48"/>
+      <c r="AH7" s="48">
+        <v>3079</v>
+      </c>
       <c r="AI7" s="48"/>
       <c r="AJ7" s="48"/>
       <c r="AK7" s="48"/>
@@ -7607,7 +7791,9 @@
       <c r="AG8" s="48">
         <v>5678</v>
       </c>
-      <c r="AH8" s="48"/>
+      <c r="AH8" s="48">
+        <v>5710</v>
+      </c>
       <c r="AI8" s="48"/>
       <c r="AJ8" s="48"/>
       <c r="AK8" s="48"/>
@@ -7657,8 +7843,8 @@
       <c r="AE9" s="312"/>
       <c r="AF9" s="312"/>
       <c r="AG9" s="312"/>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="48"/>
+      <c r="AH9" s="312"/>
+      <c r="AI9" s="312"/>
       <c r="AJ9" s="48"/>
       <c r="AK9" s="48"/>
       <c r="AL9" s="48"/>
@@ -7773,7 +7959,9 @@
       <c r="AG10" s="48">
         <v>172</v>
       </c>
-      <c r="AH10" s="48"/>
+      <c r="AH10" s="48">
+        <v>173</v>
+      </c>
       <c r="AI10" s="48"/>
       <c r="AJ10" s="48"/>
       <c r="AK10" s="48"/>
@@ -7889,7 +8077,9 @@
       <c r="AG11" s="48">
         <v>172</v>
       </c>
-      <c r="AH11" s="48"/>
+      <c r="AH11" s="48">
+        <v>173</v>
+      </c>
       <c r="AI11" s="48"/>
       <c r="AJ11" s="48"/>
       <c r="AK11" s="48"/>
@@ -8005,7 +8195,9 @@
       <c r="AG12" s="48">
         <v>172</v>
       </c>
-      <c r="AH12" s="48"/>
+      <c r="AH12" s="48">
+        <v>173</v>
+      </c>
       <c r="AI12" s="48"/>
       <c r="AJ12" s="48"/>
       <c r="AK12" s="48"/>
@@ -8121,7 +8313,9 @@
       <c r="AG13" s="48">
         <v>172</v>
       </c>
-      <c r="AH13" s="48"/>
+      <c r="AH13" s="48">
+        <v>173</v>
+      </c>
       <c r="AI13" s="48"/>
       <c r="AJ13" s="48"/>
       <c r="AK13" s="48"/>
@@ -8237,7 +8431,9 @@
       <c r="AG14" s="48">
         <v>172</v>
       </c>
-      <c r="AH14" s="48"/>
+      <c r="AH14" s="48">
+        <v>173</v>
+      </c>
       <c r="AI14" s="48"/>
       <c r="AJ14" s="48"/>
       <c r="AK14" s="48"/>
@@ -8353,7 +8549,9 @@
       <c r="AG15" s="48">
         <v>107</v>
       </c>
-      <c r="AH15" s="48"/>
+      <c r="AH15" s="48">
+        <v>108</v>
+      </c>
       <c r="AI15" s="48"/>
       <c r="AJ15" s="48"/>
       <c r="AK15" s="48"/>
@@ -8469,7 +8667,9 @@
       <c r="AG16" s="48">
         <v>184</v>
       </c>
-      <c r="AH16" s="48"/>
+      <c r="AH16" s="48">
+        <v>185</v>
+      </c>
       <c r="AI16" s="48"/>
       <c r="AJ16" s="48"/>
       <c r="AK16" s="48"/>
@@ -8518,9 +8718,9 @@
       <c r="AD17" s="78"/>
       <c r="AE17" s="312"/>
       <c r="AF17" s="312"/>
-      <c r="AG17" s="48"/>
-      <c r="AH17" s="48"/>
-      <c r="AI17" s="48"/>
+      <c r="AG17" s="312"/>
+      <c r="AH17" s="312"/>
+      <c r="AI17" s="312"/>
       <c r="AJ17" s="48"/>
       <c r="AK17" s="48"/>
       <c r="AL17" s="48"/>
@@ -8635,7 +8835,9 @@
       <c r="AG18" s="48">
         <v>933</v>
       </c>
-      <c r="AH18" s="48"/>
+      <c r="AH18" s="48">
+        <v>940</v>
+      </c>
       <c r="AI18" s="48"/>
       <c r="AJ18" s="48"/>
       <c r="AK18" s="48"/>
@@ -8667,7 +8869,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AG20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AH20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -8789,6 +8991,10 @@
       <c r="AG20" s="51">
         <f t="shared" si="0"/>
         <v>30274</v>
+      </c>
+      <c r="AH20" s="51">
+        <f t="shared" si="0"/>
+        <v>30512</v>
       </c>
     </row>
   </sheetData>
@@ -9061,43 +9267,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="322" t="s">
+      <c r="B8" s="331" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="322"/>
+      <c r="B9" s="331"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="322"/>
+      <c r="B10" s="331"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="322"/>
+      <c r="B11" s="331"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="323" t="s">
+      <c r="B12" s="332" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="323"/>
+      <c r="B13" s="332"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="323"/>
+      <c r="B14" s="332"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="324" t="s">
+      <c r="B15" s="333" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="324"/>
+      <c r="B16" s="333"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean data from SSA for July 13th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C82797A-2311-5745-A4EB-E870DA4C4E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239394D1-8310-6240-8938-8C5413DD8E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="335">
+  <cellXfs count="425">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1503,6 +1503,279 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1511,9 +1784,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="11" borderId="4" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1834,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2933,6 +3203,326 @@
         <v>624987</v>
       </c>
     </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="15">
+        <v>44016</v>
+      </c>
+      <c r="B35" s="332">
+        <v>252165</v>
+      </c>
+      <c r="C35" s="333">
+        <v>308439</v>
+      </c>
+      <c r="D35" s="334">
+        <v>74387</v>
+      </c>
+      <c r="E35" s="335">
+        <v>30366</v>
+      </c>
+      <c r="F35" s="336">
+        <v>30.184997918029861</v>
+      </c>
+      <c r="G35" s="337">
+        <v>76116</v>
+      </c>
+      <c r="H35" s="338">
+        <v>6462</v>
+      </c>
+      <c r="I35" s="339">
+        <v>7396</v>
+      </c>
+      <c r="J35" s="340">
+        <v>634991</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="15">
+        <v>44017</v>
+      </c>
+      <c r="B36" s="341">
+        <v>256848</v>
+      </c>
+      <c r="C36" s="342">
+        <v>312989</v>
+      </c>
+      <c r="D36" s="343">
+        <v>71305</v>
+      </c>
+      <c r="E36" s="344">
+        <v>30639</v>
+      </c>
+      <c r="F36" s="345">
+        <v>30.029044415374074</v>
+      </c>
+      <c r="G36" s="346">
+        <v>77129</v>
+      </c>
+      <c r="H36" s="347">
+        <v>6534</v>
+      </c>
+      <c r="I36" s="348">
+        <v>7457</v>
+      </c>
+      <c r="J36" s="349">
+        <v>641142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="15">
+        <v>44018</v>
+      </c>
+      <c r="B37" s="350">
+        <v>261750</v>
+      </c>
+      <c r="C37" s="351">
+        <v>317446</v>
+      </c>
+      <c r="D37" s="352">
+        <v>73035</v>
+      </c>
+      <c r="E37" s="353">
+        <v>31119</v>
+      </c>
+      <c r="F37" s="354">
+        <v>29.941165234001911</v>
+      </c>
+      <c r="G37" s="355">
+        <v>78371</v>
+      </c>
+      <c r="H37" s="356">
+        <v>6611</v>
+      </c>
+      <c r="I37" s="357">
+        <v>7568</v>
+      </c>
+      <c r="J37" s="358">
+        <v>652231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="15">
+        <v>44019</v>
+      </c>
+      <c r="B38" s="359">
+        <v>268008</v>
+      </c>
+      <c r="C38" s="360">
+        <v>322826</v>
+      </c>
+      <c r="D38" s="361">
+        <v>77703</v>
+      </c>
+      <c r="E38" s="362">
+        <v>32014</v>
+      </c>
+      <c r="F38" s="363">
+        <v>29.892764395092687</v>
+      </c>
+      <c r="G38" s="364">
+        <v>80115</v>
+      </c>
+      <c r="H38" s="365">
+        <v>6748</v>
+      </c>
+      <c r="I38" s="366">
+        <v>7769</v>
+      </c>
+      <c r="J38" s="367">
+        <v>668537</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="15">
+        <v>44020</v>
+      </c>
+      <c r="B39" s="368">
+        <v>275003</v>
+      </c>
+      <c r="C39" s="369">
+        <v>328908</v>
+      </c>
+      <c r="D39" s="370">
+        <v>80893</v>
+      </c>
+      <c r="E39" s="371">
+        <v>32796</v>
+      </c>
+      <c r="F39" s="372">
+        <v>29.784038719577605</v>
+      </c>
+      <c r="G39" s="373">
+        <v>81907</v>
+      </c>
+      <c r="H39" s="374">
+        <v>6903</v>
+      </c>
+      <c r="I39" s="375">
+        <v>7979</v>
+      </c>
+      <c r="J39" s="376">
+        <v>684804</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="15">
+        <v>44021</v>
+      </c>
+      <c r="B40" s="377">
+        <v>282283</v>
+      </c>
+      <c r="C40" s="378">
+        <v>336673</v>
+      </c>
+      <c r="D40" s="379">
+        <v>80988</v>
+      </c>
+      <c r="E40" s="380">
+        <v>33526</v>
+      </c>
+      <c r="F40" s="381">
+        <v>29.673058597223356</v>
+      </c>
+      <c r="G40" s="382">
+        <v>83762</v>
+      </c>
+      <c r="H40" s="383">
+        <v>7074</v>
+      </c>
+      <c r="I40" s="384">
+        <v>8180</v>
+      </c>
+      <c r="J40" s="385">
+        <v>699944</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="15">
+        <v>44022</v>
+      </c>
+      <c r="B41" s="386">
+        <v>289174</v>
+      </c>
+      <c r="C41" s="387">
+        <v>344283</v>
+      </c>
+      <c r="D41" s="388">
+        <v>81838</v>
+      </c>
+      <c r="E41" s="389">
+        <v>34191</v>
+      </c>
+      <c r="F41" s="390">
+        <v>29.507839570639131</v>
+      </c>
+      <c r="G41" s="391">
+        <v>85329</v>
+      </c>
+      <c r="H41" s="392">
+        <v>7212</v>
+      </c>
+      <c r="I41" s="393">
+        <v>8338</v>
+      </c>
+      <c r="J41" s="394">
+        <v>715295</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="15">
+        <v>44023</v>
+      </c>
+      <c r="B42" s="395">
+        <v>295268</v>
+      </c>
+      <c r="C42" s="396">
+        <v>350007</v>
+      </c>
+      <c r="D42" s="397">
+        <v>78393</v>
+      </c>
+      <c r="E42" s="398">
+        <v>34730</v>
+      </c>
+      <c r="F42" s="399">
+        <v>29.338770201985991</v>
+      </c>
+      <c r="G42" s="400">
+        <v>86628</v>
+      </c>
+      <c r="H42" s="401">
+        <v>7298</v>
+      </c>
+      <c r="I42" s="402">
+        <v>8437</v>
+      </c>
+      <c r="J42" s="403">
+        <v>723668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="15">
+        <v>44024</v>
+      </c>
+      <c r="B43" s="404">
+        <v>299750</v>
+      </c>
+      <c r="C43" s="405">
+        <v>354171</v>
+      </c>
+      <c r="D43" s="406">
+        <v>74563</v>
+      </c>
+      <c r="E43" s="407">
+        <v>35006</v>
+      </c>
+      <c r="F43" s="408">
+        <v>29.259382819015844</v>
+      </c>
+      <c r="G43" s="409">
+        <v>87705</v>
+      </c>
+      <c r="H43" s="410">
+        <v>7356</v>
+      </c>
+      <c r="I43" s="411">
+        <v>8484</v>
+      </c>
+      <c r="J43" s="412">
+        <v>728484</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="15">
+        <v>44025</v>
+      </c>
+      <c r="B44" s="413">
+        <v>304435</v>
+      </c>
+      <c r="C44" s="414">
+        <v>358663</v>
+      </c>
+      <c r="D44" s="415">
+        <v>76824</v>
+      </c>
+      <c r="E44" s="416">
+        <v>35491</v>
+      </c>
+      <c r="F44" s="417">
+        <v>29.208205364035017</v>
+      </c>
+      <c r="G44" s="418">
+        <v>88920</v>
+      </c>
+      <c r="H44" s="419">
+        <v>7431</v>
+      </c>
+      <c r="I44" s="420">
+        <v>8579</v>
+      </c>
+      <c r="J44" s="421">
+        <v>739922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2940,11 +3530,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4196,46 +4786,384 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
+      <c r="A35" s="217">
+        <v>44016</v>
+      </c>
+      <c r="B35" s="48">
+        <v>0</v>
+      </c>
+      <c r="C35" s="48">
+        <v>1</v>
+      </c>
+      <c r="D35" s="48">
+        <v>1</v>
+      </c>
+      <c r="E35" s="48">
+        <v>1</v>
+      </c>
+      <c r="F35" s="48">
+        <v>1</v>
+      </c>
+      <c r="G35" s="48">
+        <v>0</v>
+      </c>
+      <c r="H35" s="48">
+        <v>1</v>
+      </c>
+      <c r="I35" s="48">
+        <v>0</v>
+      </c>
+      <c r="J35" s="48">
+        <v>1</v>
+      </c>
+      <c r="K35" s="48">
+        <v>0</v>
+      </c>
+      <c r="L35" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
+      <c r="A36" s="217">
+        <v>44017</v>
+      </c>
+      <c r="B36" s="48">
+        <v>0</v>
+      </c>
+      <c r="C36" s="48">
+        <v>1</v>
+      </c>
+      <c r="D36" s="48">
+        <v>1</v>
+      </c>
+      <c r="E36" s="48">
+        <v>1</v>
+      </c>
+      <c r="F36" s="48">
+        <v>1</v>
+      </c>
+      <c r="G36" s="48">
+        <v>0</v>
+      </c>
+      <c r="H36" s="48">
+        <v>1</v>
+      </c>
+      <c r="I36" s="48">
+        <v>0</v>
+      </c>
+      <c r="J36" s="48">
+        <v>1</v>
+      </c>
+      <c r="K36" s="48">
+        <v>0</v>
+      </c>
+      <c r="L36" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
+      <c r="A37" s="217">
+        <v>44018</v>
+      </c>
+      <c r="B37" s="48">
+        <v>0</v>
+      </c>
+      <c r="C37" s="48">
+        <v>1</v>
+      </c>
+      <c r="D37" s="48">
+        <v>1</v>
+      </c>
+      <c r="E37" s="48">
+        <v>1</v>
+      </c>
+      <c r="F37" s="48">
+        <v>1</v>
+      </c>
+      <c r="G37" s="48">
+        <v>0</v>
+      </c>
+      <c r="H37" s="48">
+        <v>1</v>
+      </c>
+      <c r="I37" s="48">
+        <v>0</v>
+      </c>
+      <c r="J37" s="48">
+        <v>1</v>
+      </c>
+      <c r="K37" s="48">
+        <v>0</v>
+      </c>
+      <c r="L37" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="47">
+        <v>44019</v>
+      </c>
+      <c r="B38" s="74">
+        <v>0</v>
+      </c>
+      <c r="C38" s="74">
+        <v>1</v>
+      </c>
+      <c r="D38" s="74">
+        <v>1</v>
+      </c>
+      <c r="E38" s="74">
+        <v>1</v>
+      </c>
+      <c r="F38" s="74">
+        <v>1</v>
+      </c>
+      <c r="G38" s="74">
+        <v>0</v>
+      </c>
+      <c r="H38" s="74">
+        <v>1</v>
+      </c>
+      <c r="I38" s="74">
+        <v>0</v>
+      </c>
+      <c r="J38" s="74">
+        <v>1</v>
+      </c>
+      <c r="K38" s="74">
+        <v>0</v>
+      </c>
+      <c r="L38" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="47">
+        <v>44020</v>
+      </c>
+      <c r="B39" s="74">
+        <v>0</v>
+      </c>
+      <c r="C39" s="74">
+        <v>1</v>
+      </c>
+      <c r="D39" s="74">
+        <v>1</v>
+      </c>
+      <c r="E39" s="74">
+        <v>1</v>
+      </c>
+      <c r="F39" s="74">
+        <v>1</v>
+      </c>
+      <c r="G39" s="216">
+        <v>0</v>
+      </c>
+      <c r="H39" s="74">
+        <v>1</v>
+      </c>
+      <c r="I39" s="74">
+        <v>0</v>
+      </c>
+      <c r="J39" s="74">
+        <v>1</v>
+      </c>
+      <c r="K39" s="74">
+        <v>0</v>
+      </c>
+      <c r="L39" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="47">
+        <v>44021</v>
+      </c>
+      <c r="B40" s="74">
+        <v>0</v>
+      </c>
+      <c r="C40" s="74">
+        <v>1</v>
+      </c>
+      <c r="D40" s="74">
+        <v>1</v>
+      </c>
+      <c r="E40" s="74">
+        <v>1</v>
+      </c>
+      <c r="F40" s="74">
+        <v>1</v>
+      </c>
+      <c r="G40" s="74">
+        <v>0</v>
+      </c>
+      <c r="H40" s="74">
+        <v>1</v>
+      </c>
+      <c r="I40" s="74">
+        <v>0</v>
+      </c>
+      <c r="J40" s="74">
+        <v>1</v>
+      </c>
+      <c r="K40" s="74">
+        <v>0</v>
+      </c>
+      <c r="L40" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="47">
+        <v>44022</v>
+      </c>
+      <c r="B41" s="74">
+        <v>0</v>
+      </c>
+      <c r="C41" s="74">
+        <v>1</v>
+      </c>
+      <c r="D41" s="74">
+        <v>1</v>
+      </c>
+      <c r="E41" s="74">
+        <v>1</v>
+      </c>
+      <c r="F41" s="74">
+        <v>1</v>
+      </c>
+      <c r="G41" s="74">
+        <v>0</v>
+      </c>
+      <c r="H41" s="74">
+        <v>1</v>
+      </c>
+      <c r="I41" s="74">
+        <v>0</v>
+      </c>
+      <c r="J41" s="74">
+        <v>1</v>
+      </c>
+      <c r="K41" s="74">
+        <v>0</v>
+      </c>
+      <c r="L41" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="47">
+        <v>44023</v>
+      </c>
+      <c r="B42" s="74">
+        <v>0</v>
+      </c>
+      <c r="C42" s="74">
+        <v>1</v>
+      </c>
+      <c r="D42" s="74">
+        <v>1</v>
+      </c>
+      <c r="E42" s="74">
+        <v>1</v>
+      </c>
+      <c r="F42" s="74">
+        <v>1</v>
+      </c>
+      <c r="G42" s="74">
+        <v>0</v>
+      </c>
+      <c r="H42" s="74">
+        <v>1</v>
+      </c>
+      <c r="I42" s="74">
+        <v>0</v>
+      </c>
+      <c r="J42" s="74">
+        <v>1</v>
+      </c>
+      <c r="K42" s="74">
+        <v>0</v>
+      </c>
+      <c r="L42" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="47">
+        <v>44024</v>
+      </c>
+      <c r="B43" s="74">
+        <v>0</v>
+      </c>
+      <c r="C43" s="74">
+        <v>1</v>
+      </c>
+      <c r="D43" s="74">
+        <v>1</v>
+      </c>
+      <c r="E43" s="74">
+        <v>1</v>
+      </c>
+      <c r="F43" s="74">
+        <v>1</v>
+      </c>
+      <c r="G43" s="48">
+        <v>0</v>
+      </c>
+      <c r="H43" s="74">
+        <v>1</v>
+      </c>
+      <c r="I43" s="74">
+        <v>0</v>
+      </c>
+      <c r="J43" s="74">
+        <v>1</v>
+      </c>
+      <c r="K43" s="74">
+        <v>0</v>
+      </c>
+      <c r="L43" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="47">
+        <v>44025</v>
+      </c>
+      <c r="B44" s="74">
+        <v>0</v>
+      </c>
+      <c r="C44" s="74">
+        <v>1</v>
+      </c>
+      <c r="D44" s="48">
+        <v>1</v>
+      </c>
+      <c r="E44" s="48">
+        <v>1</v>
+      </c>
+      <c r="F44" s="48">
+        <v>1</v>
+      </c>
+      <c r="G44" s="48">
+        <v>0</v>
+      </c>
+      <c r="H44" s="48">
+        <v>1</v>
+      </c>
+      <c r="I44" s="48">
+        <v>0</v>
+      </c>
+      <c r="J44" s="48">
+        <v>1</v>
+      </c>
+      <c r="K44" s="48">
+        <v>0</v>
+      </c>
+      <c r="L44" s="48">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4244,11 +5172,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5696,20 +6624,460 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
+      <c r="A35" s="47">
+        <v>44016</v>
+      </c>
+      <c r="B35" s="48">
+        <v>0</v>
+      </c>
+      <c r="C35" s="48">
+        <v>1</v>
+      </c>
+      <c r="D35" s="48">
+        <v>1</v>
+      </c>
+      <c r="E35" s="48">
+        <v>0</v>
+      </c>
+      <c r="F35" s="48">
+        <v>1</v>
+      </c>
+      <c r="G35" s="48">
+        <v>1</v>
+      </c>
+      <c r="H35" s="48">
+        <v>1</v>
+      </c>
+      <c r="I35" s="48">
+        <v>0</v>
+      </c>
+      <c r="J35" s="48">
+        <v>1</v>
+      </c>
+      <c r="K35" s="48">
+        <v>1</v>
+      </c>
+      <c r="L35" s="48">
+        <v>1</v>
+      </c>
+      <c r="M35" s="48">
+        <v>0</v>
+      </c>
+      <c r="N35" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="47">
+        <v>44017</v>
+      </c>
+      <c r="B36" s="74">
+        <v>0</v>
+      </c>
+      <c r="C36" s="74">
+        <v>1</v>
+      </c>
+      <c r="D36" s="74">
+        <v>1</v>
+      </c>
+      <c r="E36" s="74">
+        <v>0</v>
+      </c>
+      <c r="F36" s="74">
+        <v>1</v>
+      </c>
+      <c r="G36" s="74">
+        <v>1</v>
+      </c>
+      <c r="H36" s="74">
+        <v>1</v>
+      </c>
+      <c r="I36" s="74">
+        <v>0</v>
+      </c>
+      <c r="J36" s="74">
+        <v>1</v>
+      </c>
+      <c r="K36" s="74">
+        <v>1</v>
+      </c>
+      <c r="L36" s="74">
+        <v>1</v>
+      </c>
+      <c r="M36" s="74">
+        <v>0</v>
+      </c>
+      <c r="N36" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="47">
+        <v>44018</v>
+      </c>
+      <c r="B37" s="74">
+        <v>0</v>
+      </c>
+      <c r="C37" s="74">
+        <v>1</v>
+      </c>
+      <c r="D37" s="74">
+        <v>1</v>
+      </c>
+      <c r="E37" s="74">
+        <v>0</v>
+      </c>
+      <c r="F37" s="74">
+        <v>1</v>
+      </c>
+      <c r="G37" s="74">
+        <v>1</v>
+      </c>
+      <c r="H37" s="74">
+        <v>1</v>
+      </c>
+      <c r="I37" s="74">
+        <v>0</v>
+      </c>
+      <c r="J37" s="74">
+        <v>1</v>
+      </c>
+      <c r="K37" s="74">
+        <v>1</v>
+      </c>
+      <c r="L37" s="74">
+        <v>1</v>
+      </c>
+      <c r="M37" s="74">
+        <v>0</v>
+      </c>
+      <c r="N37" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="47">
+        <v>44019</v>
+      </c>
+      <c r="B38" s="74">
+        <v>0</v>
+      </c>
+      <c r="C38" s="74">
+        <v>1</v>
+      </c>
+      <c r="D38" s="74">
+        <v>1</v>
+      </c>
+      <c r="E38" s="74">
+        <v>0</v>
+      </c>
+      <c r="F38" s="74">
+        <v>1</v>
+      </c>
+      <c r="G38" s="74">
+        <v>1</v>
+      </c>
+      <c r="H38" s="74">
+        <v>1</v>
+      </c>
+      <c r="I38" s="74">
+        <v>0</v>
+      </c>
+      <c r="J38" s="74">
+        <v>1</v>
+      </c>
+      <c r="K38" s="74">
+        <v>1</v>
+      </c>
+      <c r="L38" s="74">
+        <v>1</v>
+      </c>
+      <c r="M38" s="74">
+        <v>0</v>
+      </c>
+      <c r="N38" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="47">
+        <v>44020</v>
+      </c>
+      <c r="B39" s="74">
+        <v>0</v>
+      </c>
+      <c r="C39" s="74">
+        <v>1</v>
+      </c>
+      <c r="D39" s="74">
+        <v>1</v>
+      </c>
+      <c r="E39" s="74">
+        <v>0</v>
+      </c>
+      <c r="F39" s="74">
+        <v>1</v>
+      </c>
+      <c r="G39" s="74">
+        <v>1</v>
+      </c>
+      <c r="H39" s="74">
+        <v>1</v>
+      </c>
+      <c r="I39" s="74">
+        <v>0</v>
+      </c>
+      <c r="J39" s="74">
+        <v>1</v>
+      </c>
+      <c r="K39" s="74">
+        <v>1</v>
+      </c>
+      <c r="L39" s="74">
+        <v>1</v>
+      </c>
+      <c r="M39" s="74">
+        <v>0</v>
+      </c>
+      <c r="N39" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="47">
+        <v>44021</v>
+      </c>
+      <c r="B40" s="74">
+        <v>0</v>
+      </c>
+      <c r="C40" s="74">
+        <v>1</v>
+      </c>
+      <c r="D40" s="74">
+        <v>1</v>
+      </c>
+      <c r="E40" s="74">
+        <v>0</v>
+      </c>
+      <c r="F40" s="74">
+        <v>1</v>
+      </c>
+      <c r="G40" s="74">
+        <v>1</v>
+      </c>
+      <c r="H40" s="74">
+        <v>1</v>
+      </c>
+      <c r="I40" s="74">
+        <v>0</v>
+      </c>
+      <c r="J40" s="74">
+        <v>1</v>
+      </c>
+      <c r="K40" s="74">
+        <v>1</v>
+      </c>
+      <c r="L40" s="74">
+        <v>1</v>
+      </c>
+      <c r="M40" s="74">
+        <v>0</v>
+      </c>
+      <c r="N40" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="47">
+        <v>44022</v>
+      </c>
+      <c r="B41" s="74">
+        <v>0</v>
+      </c>
+      <c r="C41" s="74">
+        <v>1</v>
+      </c>
+      <c r="D41" s="74">
+        <v>1</v>
+      </c>
+      <c r="E41" s="74">
+        <v>0</v>
+      </c>
+      <c r="F41" s="74">
+        <v>1</v>
+      </c>
+      <c r="G41" s="74">
+        <v>1</v>
+      </c>
+      <c r="H41" s="74">
+        <v>1</v>
+      </c>
+      <c r="I41" s="74">
+        <v>0</v>
+      </c>
+      <c r="J41" s="74">
+        <v>1</v>
+      </c>
+      <c r="K41" s="74">
+        <v>1</v>
+      </c>
+      <c r="L41" s="74">
+        <v>1</v>
+      </c>
+      <c r="M41" s="74">
+        <v>0</v>
+      </c>
+      <c r="N41" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="47">
+        <v>44023</v>
+      </c>
+      <c r="B42" s="74">
+        <v>0</v>
+      </c>
+      <c r="C42" s="74">
+        <v>1</v>
+      </c>
+      <c r="D42" s="74">
+        <v>1</v>
+      </c>
+      <c r="E42" s="74">
+        <v>0</v>
+      </c>
+      <c r="F42" s="74">
+        <v>1</v>
+      </c>
+      <c r="G42" s="74">
+        <v>1</v>
+      </c>
+      <c r="H42" s="74">
+        <v>1</v>
+      </c>
+      <c r="I42" s="74">
+        <v>0</v>
+      </c>
+      <c r="J42" s="74">
+        <v>1</v>
+      </c>
+      <c r="K42" s="74">
+        <v>1</v>
+      </c>
+      <c r="L42" s="74">
+        <v>1</v>
+      </c>
+      <c r="M42" s="74">
+        <v>0</v>
+      </c>
+      <c r="N42" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="47">
+        <v>44024</v>
+      </c>
+      <c r="B43" s="74">
+        <v>0</v>
+      </c>
+      <c r="C43" s="74">
+        <v>1</v>
+      </c>
+      <c r="D43" s="74">
+        <v>1</v>
+      </c>
+      <c r="E43" s="74">
+        <v>0</v>
+      </c>
+      <c r="F43" s="74">
+        <v>1</v>
+      </c>
+      <c r="G43" s="74">
+        <v>1</v>
+      </c>
+      <c r="H43" s="74">
+        <v>1</v>
+      </c>
+      <c r="I43" s="74">
+        <v>0</v>
+      </c>
+      <c r="J43" s="74">
+        <v>1</v>
+      </c>
+      <c r="K43" s="74">
+        <v>1</v>
+      </c>
+      <c r="L43" s="74">
+        <v>1</v>
+      </c>
+      <c r="M43" s="74">
+        <v>0</v>
+      </c>
+      <c r="N43" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="47">
+        <v>44025</v>
+      </c>
+      <c r="B44" s="48">
+        <v>0</v>
+      </c>
+      <c r="C44" s="48">
+        <v>1</v>
+      </c>
+      <c r="D44" s="48">
+        <v>1</v>
+      </c>
+      <c r="E44" s="48">
+        <v>0</v>
+      </c>
+      <c r="F44" s="48">
+        <v>1</v>
+      </c>
+      <c r="G44" s="48">
+        <v>1</v>
+      </c>
+      <c r="H44" s="48">
+        <v>1</v>
+      </c>
+      <c r="I44" s="48">
+        <v>0</v>
+      </c>
+      <c r="J44" s="48">
+        <v>1</v>
+      </c>
+      <c r="K44" s="48">
+        <v>1</v>
+      </c>
+      <c r="L44" s="48">
+        <v>1</v>
+      </c>
+      <c r="M44" s="48">
+        <v>0</v>
+      </c>
+      <c r="N44" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5718,11 +7086,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6760,7 +8128,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="334">
+      <c r="A33" s="331">
         <v>44014</v>
       </c>
       <c r="B33" s="74">
@@ -6792,7 +8160,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="334">
+      <c r="A34" s="331">
         <v>44015</v>
       </c>
       <c r="B34" s="74">
@@ -6824,28 +8192,324 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
+      <c r="A35" s="331">
+        <v>44016</v>
+      </c>
+      <c r="B35" s="48">
+        <v>0</v>
+      </c>
+      <c r="C35" s="48">
+        <v>0</v>
+      </c>
+      <c r="D35" s="48">
+        <v>0</v>
+      </c>
+      <c r="E35" s="48">
+        <v>0</v>
+      </c>
+      <c r="F35" s="48">
+        <v>2</v>
+      </c>
+      <c r="G35" s="48">
+        <v>1</v>
+      </c>
+      <c r="H35" s="48">
+        <v>1</v>
+      </c>
+      <c r="I35" s="48">
+        <v>1</v>
+      </c>
+      <c r="J35" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="A36" s="331">
+        <v>44017</v>
+      </c>
+      <c r="B36" s="48">
+        <v>0</v>
+      </c>
+      <c r="C36" s="48">
+        <v>0</v>
+      </c>
+      <c r="D36" s="48">
+        <v>0</v>
+      </c>
+      <c r="E36" s="48">
+        <v>0</v>
+      </c>
+      <c r="F36" s="48">
+        <v>2</v>
+      </c>
+      <c r="G36" s="48">
+        <v>1</v>
+      </c>
+      <c r="H36" s="48">
+        <v>1</v>
+      </c>
+      <c r="I36" s="48">
+        <v>1</v>
+      </c>
+      <c r="J36" s="48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="331">
+        <v>44018</v>
+      </c>
+      <c r="B37" s="74">
+        <v>0</v>
+      </c>
+      <c r="C37" s="74">
+        <v>0</v>
+      </c>
+      <c r="D37" s="74">
+        <v>0</v>
+      </c>
+      <c r="E37" s="74">
+        <v>0</v>
+      </c>
+      <c r="F37" s="74">
+        <v>2</v>
+      </c>
+      <c r="G37" s="74">
+        <v>1</v>
+      </c>
+      <c r="H37" s="74">
+        <v>1</v>
+      </c>
+      <c r="I37" s="74">
+        <v>1</v>
+      </c>
+      <c r="J37" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="331">
+        <v>44019</v>
+      </c>
+      <c r="B38" s="74">
+        <v>0</v>
+      </c>
+      <c r="C38" s="74">
+        <v>0</v>
+      </c>
+      <c r="D38" s="74">
+        <v>0</v>
+      </c>
+      <c r="E38" s="74">
+        <v>0</v>
+      </c>
+      <c r="F38" s="74">
+        <v>2</v>
+      </c>
+      <c r="G38" s="74">
+        <v>1</v>
+      </c>
+      <c r="H38" s="74">
+        <v>1</v>
+      </c>
+      <c r="I38" s="74">
+        <v>1</v>
+      </c>
+      <c r="J38" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="331">
+        <v>44020</v>
+      </c>
+      <c r="B39" s="74">
+        <v>0</v>
+      </c>
+      <c r="C39" s="74">
+        <v>0</v>
+      </c>
+      <c r="D39" s="74">
+        <v>0</v>
+      </c>
+      <c r="E39" s="74">
+        <v>0</v>
+      </c>
+      <c r="F39" s="74">
+        <v>2</v>
+      </c>
+      <c r="G39" s="74">
+        <v>1</v>
+      </c>
+      <c r="H39" s="74">
+        <v>1</v>
+      </c>
+      <c r="I39" s="74">
+        <v>1</v>
+      </c>
+      <c r="J39" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="331">
+        <v>44021</v>
+      </c>
+      <c r="B40" s="74">
+        <v>0</v>
+      </c>
+      <c r="C40" s="74">
+        <v>0</v>
+      </c>
+      <c r="D40" s="74">
+        <v>0</v>
+      </c>
+      <c r="E40" s="74">
+        <v>0</v>
+      </c>
+      <c r="F40" s="74">
+        <v>2</v>
+      </c>
+      <c r="G40" s="74">
+        <v>1</v>
+      </c>
+      <c r="H40" s="74">
+        <v>1</v>
+      </c>
+      <c r="I40" s="74">
+        <v>1</v>
+      </c>
+      <c r="J40" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="331">
+        <v>44022</v>
+      </c>
+      <c r="B41" s="74">
+        <v>0</v>
+      </c>
+      <c r="C41" s="74">
+        <v>0</v>
+      </c>
+      <c r="D41" s="74">
+        <v>0</v>
+      </c>
+      <c r="E41" s="74">
+        <v>0</v>
+      </c>
+      <c r="F41" s="74">
+        <v>2</v>
+      </c>
+      <c r="G41" s="74">
+        <v>1</v>
+      </c>
+      <c r="H41" s="74">
+        <v>1</v>
+      </c>
+      <c r="I41" s="74">
+        <v>1</v>
+      </c>
+      <c r="J41" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="331">
+        <v>44023</v>
+      </c>
+      <c r="B42" s="74">
+        <v>0</v>
+      </c>
+      <c r="C42" s="74">
+        <v>0</v>
+      </c>
+      <c r="D42" s="74">
+        <v>0</v>
+      </c>
+      <c r="E42" s="74">
+        <v>0</v>
+      </c>
+      <c r="F42" s="74">
+        <v>2</v>
+      </c>
+      <c r="G42" s="74">
+        <v>1</v>
+      </c>
+      <c r="H42" s="74">
+        <v>1</v>
+      </c>
+      <c r="I42" s="74">
+        <v>1</v>
+      </c>
+      <c r="J42" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="331">
+        <v>44024</v>
+      </c>
+      <c r="B43" s="74">
+        <v>0</v>
+      </c>
+      <c r="C43" s="74">
+        <v>0</v>
+      </c>
+      <c r="D43" s="74">
+        <v>0</v>
+      </c>
+      <c r="E43" s="74">
+        <v>0</v>
+      </c>
+      <c r="F43" s="74">
+        <v>2</v>
+      </c>
+      <c r="G43" s="74">
+        <v>1</v>
+      </c>
+      <c r="H43" s="74">
+        <v>1</v>
+      </c>
+      <c r="I43" s="74">
+        <v>1</v>
+      </c>
+      <c r="J43" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="47">
+        <v>44025</v>
+      </c>
+      <c r="B44" s="74">
+        <v>0</v>
+      </c>
+      <c r="C44" s="74">
+        <v>0</v>
+      </c>
+      <c r="D44" s="74">
+        <v>0</v>
+      </c>
+      <c r="E44" s="74">
+        <v>0</v>
+      </c>
+      <c r="F44" s="74">
+        <v>2</v>
+      </c>
+      <c r="G44" s="74">
+        <v>1</v>
+      </c>
+      <c r="H44" s="74">
+        <v>1</v>
+      </c>
+      <c r="I44" s="74">
+        <v>1</v>
+      </c>
+      <c r="J44" s="74">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6857,7 +8521,7 @@
   <dimension ref="A1:AV20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6968,16 +8632,36 @@
       <c r="AH1" s="49">
         <v>44015</v>
       </c>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
+      <c r="AI1" s="49">
+        <v>44016</v>
+      </c>
+      <c r="AJ1" s="49">
+        <v>44017</v>
+      </c>
+      <c r="AK1" s="49">
+        <v>44018</v>
+      </c>
+      <c r="AL1" s="49">
+        <v>44019</v>
+      </c>
+      <c r="AM1" s="49">
+        <v>44020</v>
+      </c>
+      <c r="AN1" s="49">
+        <v>44021</v>
+      </c>
+      <c r="AO1" s="49">
+        <v>44022</v>
+      </c>
+      <c r="AP1" s="49">
+        <v>44023</v>
+      </c>
+      <c r="AQ1" s="49">
+        <v>44024</v>
+      </c>
+      <c r="AR1" s="49">
+        <v>44025</v>
+      </c>
       <c r="AS1" s="48"/>
       <c r="AT1" s="48"/>
       <c r="AU1" s="48"/>
@@ -7086,16 +8770,36 @@
       <c r="AH2" s="48">
         <v>4073</v>
       </c>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="48"/>
+      <c r="AI2" s="48">
+        <v>4105</v>
+      </c>
+      <c r="AJ2" s="48">
+        <v>4137</v>
+      </c>
+      <c r="AK2" s="48">
+        <v>4116</v>
+      </c>
+      <c r="AL2" s="48">
+        <v>4148</v>
+      </c>
+      <c r="AM2" s="48">
+        <v>4180</v>
+      </c>
+      <c r="AN2" s="48">
+        <v>4212</v>
+      </c>
+      <c r="AO2" s="48">
+        <v>4244</v>
+      </c>
+      <c r="AP2" s="48">
+        <v>4276</v>
+      </c>
+      <c r="AQ2" s="48">
+        <v>4308</v>
+      </c>
+      <c r="AR2" s="48">
+        <v>4340</v>
+      </c>
       <c r="AS2" s="48"/>
       <c r="AT2" s="48"/>
       <c r="AU2" s="48"/>
@@ -7204,16 +8908,36 @@
       <c r="AH3" s="48">
         <v>3888</v>
       </c>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
+      <c r="AI3" s="48">
+        <v>3920</v>
+      </c>
+      <c r="AJ3" s="48">
+        <v>3952</v>
+      </c>
+      <c r="AK3" s="48">
+        <v>3924</v>
+      </c>
+      <c r="AL3" s="48">
+        <v>3956</v>
+      </c>
+      <c r="AM3" s="48">
+        <v>3988</v>
+      </c>
+      <c r="AN3" s="48">
+        <v>4020</v>
+      </c>
+      <c r="AO3" s="48">
+        <v>4052</v>
+      </c>
+      <c r="AP3" s="48">
+        <v>4084</v>
+      </c>
+      <c r="AQ3" s="48">
+        <v>4116</v>
+      </c>
+      <c r="AR3" s="48">
+        <v>4148</v>
+      </c>
       <c r="AS3" s="48"/>
       <c r="AT3" s="48"/>
       <c r="AU3" s="48"/>
@@ -7322,16 +9046,36 @@
       <c r="AH4" s="48">
         <v>3888</v>
       </c>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48"/>
-      <c r="AM4" s="48"/>
-      <c r="AN4" s="48"/>
-      <c r="AO4" s="48"/>
-      <c r="AP4" s="48"/>
-      <c r="AQ4" s="48"/>
-      <c r="AR4" s="48"/>
+      <c r="AI4" s="48">
+        <v>3920</v>
+      </c>
+      <c r="AJ4" s="48">
+        <v>3952</v>
+      </c>
+      <c r="AK4" s="48">
+        <v>3924</v>
+      </c>
+      <c r="AL4" s="48">
+        <v>3956</v>
+      </c>
+      <c r="AM4" s="48">
+        <v>3988</v>
+      </c>
+      <c r="AN4" s="48">
+        <v>4020</v>
+      </c>
+      <c r="AO4" s="48">
+        <v>4052</v>
+      </c>
+      <c r="AP4" s="48">
+        <v>4084</v>
+      </c>
+      <c r="AQ4" s="48">
+        <v>4116</v>
+      </c>
+      <c r="AR4" s="48">
+        <v>4148</v>
+      </c>
       <c r="AS4" s="48"/>
       <c r="AT4" s="48"/>
       <c r="AU4" s="48"/>
@@ -7440,16 +9184,36 @@
       <c r="AH5" s="48">
         <v>3888</v>
       </c>
-      <c r="AI5" s="48"/>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="48"/>
-      <c r="AN5" s="48"/>
-      <c r="AO5" s="48"/>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="48"/>
-      <c r="AR5" s="48"/>
+      <c r="AI5" s="48">
+        <v>3920</v>
+      </c>
+      <c r="AJ5" s="48">
+        <v>3952</v>
+      </c>
+      <c r="AK5" s="48">
+        <v>3924</v>
+      </c>
+      <c r="AL5" s="48">
+        <v>3956</v>
+      </c>
+      <c r="AM5" s="48">
+        <v>3988</v>
+      </c>
+      <c r="AN5" s="48">
+        <v>4020</v>
+      </c>
+      <c r="AO5" s="48">
+        <v>4052</v>
+      </c>
+      <c r="AP5" s="48">
+        <v>4084</v>
+      </c>
+      <c r="AQ5" s="48">
+        <v>4116</v>
+      </c>
+      <c r="AR5" s="48">
+        <v>4148</v>
+      </c>
       <c r="AS5" s="48"/>
       <c r="AT5" s="48"/>
       <c r="AU5" s="48"/>
@@ -7558,16 +9322,36 @@
       <c r="AH6" s="48">
         <v>3888</v>
       </c>
-      <c r="AI6" s="48"/>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="48"/>
-      <c r="AN6" s="48"/>
-      <c r="AO6" s="48"/>
-      <c r="AP6" s="48"/>
-      <c r="AQ6" s="48"/>
-      <c r="AR6" s="48"/>
+      <c r="AI6" s="48">
+        <v>3920</v>
+      </c>
+      <c r="AJ6" s="48">
+        <v>3952</v>
+      </c>
+      <c r="AK6" s="48">
+        <v>3924</v>
+      </c>
+      <c r="AL6" s="48">
+        <v>3956</v>
+      </c>
+      <c r="AM6" s="48">
+        <v>3988</v>
+      </c>
+      <c r="AN6" s="48">
+        <v>4020</v>
+      </c>
+      <c r="AO6" s="48">
+        <v>4052</v>
+      </c>
+      <c r="AP6" s="48">
+        <v>4084</v>
+      </c>
+      <c r="AQ6" s="48">
+        <v>4116</v>
+      </c>
+      <c r="AR6" s="48">
+        <v>4148</v>
+      </c>
       <c r="AS6" s="48"/>
       <c r="AT6" s="48"/>
       <c r="AU6" s="48"/>
@@ -7676,16 +9460,36 @@
       <c r="AH7" s="48">
         <v>3079</v>
       </c>
-      <c r="AI7" s="48"/>
-      <c r="AJ7" s="48"/>
-      <c r="AK7" s="48"/>
-      <c r="AL7" s="48"/>
-      <c r="AM7" s="48"/>
-      <c r="AN7" s="48"/>
-      <c r="AO7" s="48"/>
-      <c r="AP7" s="48"/>
-      <c r="AQ7" s="48"/>
-      <c r="AR7" s="48"/>
+      <c r="AI7" s="48">
+        <v>3111</v>
+      </c>
+      <c r="AJ7" s="48">
+        <v>3143</v>
+      </c>
+      <c r="AK7" s="48">
+        <v>3175</v>
+      </c>
+      <c r="AL7" s="48">
+        <v>3207</v>
+      </c>
+      <c r="AM7" s="48">
+        <v>3239</v>
+      </c>
+      <c r="AN7" s="48">
+        <v>3271</v>
+      </c>
+      <c r="AO7" s="48">
+        <v>3303</v>
+      </c>
+      <c r="AP7" s="48">
+        <v>3335</v>
+      </c>
+      <c r="AQ7" s="48">
+        <v>3367</v>
+      </c>
+      <c r="AR7" s="48">
+        <v>3399</v>
+      </c>
       <c r="AS7" s="48"/>
       <c r="AT7" s="48"/>
       <c r="AU7" s="48"/>
@@ -7794,16 +9598,36 @@
       <c r="AH8" s="48">
         <v>5710</v>
       </c>
-      <c r="AI8" s="48"/>
-      <c r="AJ8" s="48"/>
-      <c r="AK8" s="48"/>
-      <c r="AL8" s="48"/>
-      <c r="AM8" s="48"/>
-      <c r="AN8" s="48"/>
-      <c r="AO8" s="48"/>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="48"/>
-      <c r="AR8" s="48"/>
+      <c r="AI8" s="48">
+        <v>5742</v>
+      </c>
+      <c r="AJ8" s="48">
+        <v>5774</v>
+      </c>
+      <c r="AK8" s="48">
+        <v>5806</v>
+      </c>
+      <c r="AL8" s="48">
+        <v>5838</v>
+      </c>
+      <c r="AM8" s="48">
+        <v>5870</v>
+      </c>
+      <c r="AN8" s="48">
+        <v>5902</v>
+      </c>
+      <c r="AO8" s="48">
+        <v>5934</v>
+      </c>
+      <c r="AP8" s="48">
+        <v>5966</v>
+      </c>
+      <c r="AQ8" s="48">
+        <v>5998</v>
+      </c>
+      <c r="AR8" s="48">
+        <v>6030</v>
+      </c>
       <c r="AS8" s="48"/>
       <c r="AT8" s="48"/>
       <c r="AU8" s="48"/>
@@ -7845,15 +9669,15 @@
       <c r="AG9" s="312"/>
       <c r="AH9" s="312"/>
       <c r="AI9" s="312"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="48"/>
-      <c r="AM9" s="48"/>
-      <c r="AN9" s="48"/>
-      <c r="AO9" s="48"/>
-      <c r="AP9" s="48"/>
-      <c r="AQ9" s="48"/>
-      <c r="AR9" s="48"/>
+      <c r="AJ9" s="312"/>
+      <c r="AK9" s="312"/>
+      <c r="AL9" s="312"/>
+      <c r="AM9" s="312"/>
+      <c r="AN9" s="312"/>
+      <c r="AO9" s="312"/>
+      <c r="AP9" s="312"/>
+      <c r="AQ9" s="312"/>
+      <c r="AR9" s="312"/>
       <c r="AS9" s="48"/>
       <c r="AT9" s="48"/>
       <c r="AU9" s="48"/>
@@ -7962,16 +9786,36 @@
       <c r="AH10" s="48">
         <v>173</v>
       </c>
-      <c r="AI10" s="48"/>
-      <c r="AJ10" s="48"/>
-      <c r="AK10" s="48"/>
-      <c r="AL10" s="48"/>
-      <c r="AM10" s="48"/>
-      <c r="AN10" s="48"/>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="48"/>
-      <c r="AR10" s="48"/>
+      <c r="AI10" s="48">
+        <v>174</v>
+      </c>
+      <c r="AJ10" s="48">
+        <v>175</v>
+      </c>
+      <c r="AK10" s="48">
+        <v>176</v>
+      </c>
+      <c r="AL10" s="48">
+        <v>177</v>
+      </c>
+      <c r="AM10" s="48">
+        <v>178</v>
+      </c>
+      <c r="AN10" s="48">
+        <v>179</v>
+      </c>
+      <c r="AO10" s="48">
+        <v>180</v>
+      </c>
+      <c r="AP10" s="48">
+        <v>181</v>
+      </c>
+      <c r="AQ10" s="48">
+        <v>182</v>
+      </c>
+      <c r="AR10" s="48">
+        <v>183</v>
+      </c>
       <c r="AS10" s="48"/>
       <c r="AT10" s="48"/>
       <c r="AU10" s="48"/>
@@ -8080,16 +9924,36 @@
       <c r="AH11" s="48">
         <v>173</v>
       </c>
-      <c r="AI11" s="48"/>
-      <c r="AJ11" s="48"/>
-      <c r="AK11" s="48"/>
-      <c r="AL11" s="48"/>
-      <c r="AM11" s="48"/>
-      <c r="AN11" s="48"/>
-      <c r="AO11" s="48"/>
-      <c r="AP11" s="48"/>
-      <c r="AQ11" s="48"/>
-      <c r="AR11" s="48"/>
+      <c r="AI11" s="48">
+        <v>174</v>
+      </c>
+      <c r="AJ11" s="48">
+        <v>175</v>
+      </c>
+      <c r="AK11" s="48">
+        <v>176</v>
+      </c>
+      <c r="AL11" s="48">
+        <v>177</v>
+      </c>
+      <c r="AM11" s="48">
+        <v>178</v>
+      </c>
+      <c r="AN11" s="48">
+        <v>179</v>
+      </c>
+      <c r="AO11" s="48">
+        <v>180</v>
+      </c>
+      <c r="AP11" s="48">
+        <v>181</v>
+      </c>
+      <c r="AQ11" s="48">
+        <v>182</v>
+      </c>
+      <c r="AR11" s="48">
+        <v>183</v>
+      </c>
       <c r="AS11" s="48"/>
       <c r="AT11" s="48"/>
       <c r="AU11" s="48"/>
@@ -8198,16 +10062,36 @@
       <c r="AH12" s="48">
         <v>173</v>
       </c>
-      <c r="AI12" s="48"/>
-      <c r="AJ12" s="48"/>
-      <c r="AK12" s="48"/>
-      <c r="AL12" s="48"/>
-      <c r="AM12" s="48"/>
-      <c r="AN12" s="48"/>
-      <c r="AO12" s="48"/>
-      <c r="AP12" s="48"/>
-      <c r="AQ12" s="48"/>
-      <c r="AR12" s="48"/>
+      <c r="AI12" s="48">
+        <v>174</v>
+      </c>
+      <c r="AJ12" s="48">
+        <v>175</v>
+      </c>
+      <c r="AK12" s="48">
+        <v>176</v>
+      </c>
+      <c r="AL12" s="48">
+        <v>177</v>
+      </c>
+      <c r="AM12" s="48">
+        <v>178</v>
+      </c>
+      <c r="AN12" s="48">
+        <v>179</v>
+      </c>
+      <c r="AO12" s="48">
+        <v>180</v>
+      </c>
+      <c r="AP12" s="48">
+        <v>181</v>
+      </c>
+      <c r="AQ12" s="48">
+        <v>182</v>
+      </c>
+      <c r="AR12" s="48">
+        <v>183</v>
+      </c>
       <c r="AS12" s="48"/>
       <c r="AT12" s="48"/>
       <c r="AU12" s="48"/>
@@ -8316,16 +10200,36 @@
       <c r="AH13" s="48">
         <v>173</v>
       </c>
-      <c r="AI13" s="48"/>
-      <c r="AJ13" s="48"/>
-      <c r="AK13" s="48"/>
-      <c r="AL13" s="48"/>
-      <c r="AM13" s="48"/>
-      <c r="AN13" s="48"/>
-      <c r="AO13" s="48"/>
-      <c r="AP13" s="48"/>
-      <c r="AQ13" s="48"/>
-      <c r="AR13" s="48"/>
+      <c r="AI13" s="48">
+        <v>174</v>
+      </c>
+      <c r="AJ13" s="48">
+        <v>175</v>
+      </c>
+      <c r="AK13" s="48">
+        <v>176</v>
+      </c>
+      <c r="AL13" s="48">
+        <v>177</v>
+      </c>
+      <c r="AM13" s="48">
+        <v>178</v>
+      </c>
+      <c r="AN13" s="48">
+        <v>179</v>
+      </c>
+      <c r="AO13" s="48">
+        <v>180</v>
+      </c>
+      <c r="AP13" s="48">
+        <v>181</v>
+      </c>
+      <c r="AQ13" s="48">
+        <v>182</v>
+      </c>
+      <c r="AR13" s="48">
+        <v>183</v>
+      </c>
       <c r="AS13" s="48"/>
       <c r="AT13" s="48"/>
       <c r="AU13" s="48"/>
@@ -8434,16 +10338,36 @@
       <c r="AH14" s="48">
         <v>173</v>
       </c>
-      <c r="AI14" s="48"/>
-      <c r="AJ14" s="48"/>
-      <c r="AK14" s="48"/>
-      <c r="AL14" s="48"/>
-      <c r="AM14" s="48"/>
-      <c r="AN14" s="48"/>
-      <c r="AO14" s="48"/>
-      <c r="AP14" s="48"/>
-      <c r="AQ14" s="48"/>
-      <c r="AR14" s="48"/>
+      <c r="AI14" s="48">
+        <v>174</v>
+      </c>
+      <c r="AJ14" s="48">
+        <v>175</v>
+      </c>
+      <c r="AK14" s="48">
+        <v>176</v>
+      </c>
+      <c r="AL14" s="48">
+        <v>177</v>
+      </c>
+      <c r="AM14" s="48">
+        <v>178</v>
+      </c>
+      <c r="AN14" s="48">
+        <v>179</v>
+      </c>
+      <c r="AO14" s="48">
+        <v>180</v>
+      </c>
+      <c r="AP14" s="48">
+        <v>181</v>
+      </c>
+      <c r="AQ14" s="48">
+        <v>182</v>
+      </c>
+      <c r="AR14" s="48">
+        <v>183</v>
+      </c>
       <c r="AS14" s="48"/>
       <c r="AT14" s="48"/>
       <c r="AU14" s="48"/>
@@ -8552,16 +10476,36 @@
       <c r="AH15" s="48">
         <v>108</v>
       </c>
-      <c r="AI15" s="48"/>
-      <c r="AJ15" s="48"/>
-      <c r="AK15" s="48"/>
-      <c r="AL15" s="48"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="48"/>
-      <c r="AO15" s="48"/>
-      <c r="AP15" s="48"/>
-      <c r="AQ15" s="48"/>
-      <c r="AR15" s="48"/>
+      <c r="AI15" s="48">
+        <v>109</v>
+      </c>
+      <c r="AJ15" s="48">
+        <v>110</v>
+      </c>
+      <c r="AK15" s="48">
+        <v>111</v>
+      </c>
+      <c r="AL15" s="48">
+        <v>112</v>
+      </c>
+      <c r="AM15" s="48">
+        <v>113</v>
+      </c>
+      <c r="AN15" s="48">
+        <v>114</v>
+      </c>
+      <c r="AO15" s="48">
+        <v>115</v>
+      </c>
+      <c r="AP15" s="48">
+        <v>116</v>
+      </c>
+      <c r="AQ15" s="48">
+        <v>117</v>
+      </c>
+      <c r="AR15" s="48">
+        <v>118</v>
+      </c>
       <c r="AS15" s="48"/>
       <c r="AT15" s="48"/>
       <c r="AU15" s="48"/>
@@ -8670,16 +10614,36 @@
       <c r="AH16" s="48">
         <v>185</v>
       </c>
-      <c r="AI16" s="48"/>
-      <c r="AJ16" s="48"/>
-      <c r="AK16" s="48"/>
-      <c r="AL16" s="48"/>
-      <c r="AM16" s="48"/>
-      <c r="AN16" s="48"/>
-      <c r="AO16" s="48"/>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="48"/>
-      <c r="AR16" s="48"/>
+      <c r="AI16" s="48">
+        <v>186</v>
+      </c>
+      <c r="AJ16" s="48">
+        <v>187</v>
+      </c>
+      <c r="AK16" s="48">
+        <v>188</v>
+      </c>
+      <c r="AL16" s="48">
+        <v>189</v>
+      </c>
+      <c r="AM16" s="48">
+        <v>190</v>
+      </c>
+      <c r="AN16" s="48">
+        <v>191</v>
+      </c>
+      <c r="AO16" s="48">
+        <v>192</v>
+      </c>
+      <c r="AP16" s="48">
+        <v>193</v>
+      </c>
+      <c r="AQ16" s="48">
+        <v>194</v>
+      </c>
+      <c r="AR16" s="48">
+        <v>195</v>
+      </c>
       <c r="AS16" s="48"/>
       <c r="AT16" s="48"/>
       <c r="AU16" s="48"/>
@@ -8721,15 +10685,15 @@
       <c r="AG17" s="312"/>
       <c r="AH17" s="312"/>
       <c r="AI17" s="312"/>
-      <c r="AJ17" s="48"/>
-      <c r="AK17" s="48"/>
-      <c r="AL17" s="48"/>
-      <c r="AM17" s="48"/>
-      <c r="AN17" s="48"/>
-      <c r="AO17" s="48"/>
-      <c r="AP17" s="48"/>
-      <c r="AQ17" s="48"/>
-      <c r="AR17" s="48"/>
+      <c r="AJ17" s="312"/>
+      <c r="AK17" s="312"/>
+      <c r="AL17" s="312"/>
+      <c r="AM17" s="312"/>
+      <c r="AN17" s="312"/>
+      <c r="AO17" s="312"/>
+      <c r="AP17" s="312"/>
+      <c r="AQ17" s="312"/>
+      <c r="AR17" s="312"/>
       <c r="AS17" s="48"/>
       <c r="AT17" s="48"/>
       <c r="AU17" s="48"/>
@@ -8838,16 +10802,36 @@
       <c r="AH18" s="48">
         <v>940</v>
       </c>
-      <c r="AI18" s="48"/>
-      <c r="AJ18" s="48"/>
-      <c r="AK18" s="48"/>
-      <c r="AL18" s="48"/>
-      <c r="AM18" s="48"/>
-      <c r="AN18" s="48"/>
-      <c r="AO18" s="48"/>
-      <c r="AP18" s="48"/>
-      <c r="AQ18" s="48"/>
-      <c r="AR18" s="48"/>
+      <c r="AI18" s="48">
+        <v>947</v>
+      </c>
+      <c r="AJ18" s="48">
+        <v>954</v>
+      </c>
+      <c r="AK18" s="48">
+        <v>961</v>
+      </c>
+      <c r="AL18" s="48">
+        <v>968</v>
+      </c>
+      <c r="AM18" s="48">
+        <v>975</v>
+      </c>
+      <c r="AN18" s="48">
+        <v>982</v>
+      </c>
+      <c r="AO18" s="48">
+        <v>989</v>
+      </c>
+      <c r="AP18" s="48">
+        <v>996</v>
+      </c>
+      <c r="AQ18" s="48">
+        <v>1003</v>
+      </c>
+      <c r="AR18" s="48">
+        <v>1010</v>
+      </c>
       <c r="AS18" s="48"/>
       <c r="AT18" s="48"/>
       <c r="AU18" s="48"/>
@@ -8869,7 +10853,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AH20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AQ20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -8995,6 +10979,46 @@
       <c r="AH20" s="51">
         <f t="shared" si="0"/>
         <v>30512</v>
+      </c>
+      <c r="AI20" s="51">
+        <f t="shared" si="0"/>
+        <v>30750</v>
+      </c>
+      <c r="AJ20" s="51">
+        <f t="shared" si="0"/>
+        <v>30988</v>
+      </c>
+      <c r="AK20" s="51">
+        <f t="shared" si="0"/>
+        <v>30933</v>
+      </c>
+      <c r="AL20" s="51">
+        <f t="shared" si="0"/>
+        <v>31171</v>
+      </c>
+      <c r="AM20" s="51">
+        <f t="shared" si="0"/>
+        <v>31409</v>
+      </c>
+      <c r="AN20" s="51">
+        <f t="shared" si="0"/>
+        <v>31647</v>
+      </c>
+      <c r="AO20" s="51">
+        <f t="shared" si="0"/>
+        <v>31885</v>
+      </c>
+      <c r="AP20" s="51">
+        <f t="shared" si="0"/>
+        <v>32123</v>
+      </c>
+      <c r="AQ20" s="51">
+        <f>SUM(AQ2:AQ18)</f>
+        <v>32361</v>
+      </c>
+      <c r="AR20" s="51">
+        <f>SUM(AR2:AR18)</f>
+        <v>32599</v>
       </c>
     </row>
   </sheetData>
@@ -9185,7 +11209,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B14"/>
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9267,43 +11291,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="331" t="s">
+      <c r="B8" s="422" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="331"/>
+      <c r="B9" s="422"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="331"/>
+      <c r="B10" s="422"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="331"/>
+      <c r="B11" s="422"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="332" t="s">
+      <c r="B12" s="423" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="332"/>
+      <c r="B13" s="423"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="332"/>
+      <c r="B14" s="423"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="333" t="s">
+      <c r="B15" s="424" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="333"/>
+      <c r="B16" s="424"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
County and age-groups data of July 13th
Adding clean data by county and by state & agre-groups as of July 13th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239394D1-8310-6240-8938-8C5413DD8E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC1DF8-509C-D54E-8CF7-156383153CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +439,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,7 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="426">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1785,6 +1791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1808,7 +1815,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2107,7 +2114,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="B44" sqref="B44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3533,8 +3540,8 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5137,8 +5144,8 @@
       <c r="C44" s="74">
         <v>1</v>
       </c>
-      <c r="D44" s="48">
-        <v>1</v>
+      <c r="D44" s="425">
+        <v>0</v>
       </c>
       <c r="E44" s="48">
         <v>1</v>
@@ -5149,8 +5156,8 @@
       <c r="G44" s="48">
         <v>0</v>
       </c>
-      <c r="H44" s="48">
-        <v>1</v>
+      <c r="H44" s="425">
+        <v>0</v>
       </c>
       <c r="I44" s="48">
         <v>0</v>
@@ -5175,8 +5182,8 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7029,8 +7036,8 @@
       <c r="C44" s="48">
         <v>1</v>
       </c>
-      <c r="D44" s="48">
-        <v>1</v>
+      <c r="D44" s="425">
+        <v>0</v>
       </c>
       <c r="E44" s="48">
         <v>0</v>
@@ -7047,8 +7054,8 @@
       <c r="I44" s="48">
         <v>0</v>
       </c>
-      <c r="J44" s="48">
-        <v>1</v>
+      <c r="J44" s="425">
+        <v>0</v>
       </c>
       <c r="K44" s="48">
         <v>1</v>
@@ -7090,7 +7097,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8520,7 +8527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
@@ -10853,7 +10860,7 @@
         <v>23069</v>
       </c>
       <c r="C20" s="51">
-        <f t="shared" ref="C20:AQ20" si="0">SUM(C2:C18)</f>
+        <f t="shared" ref="C20:AP20" si="0">SUM(C2:C18)</f>
         <v>23137</v>
       </c>
       <c r="D20" s="51">
@@ -11030,8 +11037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11052,7 +11059,9 @@
       <c r="E1" s="38">
         <v>44005</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="38">
+        <v>44025</v>
+      </c>
       <c r="G1" s="38"/>
       <c r="H1" s="38"/>
     </row>
@@ -11072,6 +11081,9 @@
       <c r="E2">
         <v>117023</v>
       </c>
+      <c r="F2">
+        <v>158794</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -11089,6 +11101,9 @@
       <c r="E3">
         <v>108604</v>
       </c>
+      <c r="F3">
+        <v>149677</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
@@ -11106,6 +11121,9 @@
       <c r="E4">
         <v>108604</v>
       </c>
+      <c r="F4">
+        <v>149677</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -11123,6 +11141,9 @@
       <c r="E5">
         <v>108604</v>
       </c>
+      <c r="F5">
+        <v>149677</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
@@ -11140,6 +11161,9 @@
       <c r="E6">
         <v>108604</v>
       </c>
+      <c r="F6">
+        <v>149677</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
@@ -11157,6 +11181,9 @@
       <c r="E7">
         <v>57360</v>
       </c>
+      <c r="F7">
+        <v>86350</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
@@ -11174,6 +11201,9 @@
       <c r="E8">
         <v>178929</v>
       </c>
+      <c r="F8">
+        <v>224128</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -11197,6 +11227,10 @@
       <c r="E10">
         <f>SUM(E2:E8)</f>
         <v>787728</v>
+      </c>
+      <c r="F10">
+        <f>SUM(F2:F8)</f>
+        <v>1067980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data From SSA for July 14th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC1DF8-509C-D54E-8CF7-156383153CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F2B371-B1DD-1040-A617-DE13C43AABE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2760" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -279,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +344,13 @@
       <color theme="1"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="18">
@@ -563,7 +570,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="426">
+  <cellXfs count="437">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1782,6 +1789,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1791,7 +1826,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1815,7 +1855,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2111,10 +2151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:D44"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3530,6 +3570,38 @@
         <v>739922</v>
       </c>
     </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="15">
+        <v>44026</v>
+      </c>
+      <c r="B45" s="423">
+        <v>311486</v>
+      </c>
+      <c r="C45" s="424">
+        <v>363930</v>
+      </c>
+      <c r="D45" s="425">
+        <v>80721</v>
+      </c>
+      <c r="E45" s="426">
+        <v>36327</v>
+      </c>
+      <c r="F45" s="427">
+        <v>29.115915322036944</v>
+      </c>
+      <c r="G45" s="428">
+        <v>90692</v>
+      </c>
+      <c r="H45" s="429">
+        <v>7578</v>
+      </c>
+      <c r="I45" s="430">
+        <v>8772</v>
+      </c>
+      <c r="J45" s="431">
+        <v>756137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3537,11 +3609,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5144,7 +5216,7 @@
       <c r="C44" s="74">
         <v>1</v>
       </c>
-      <c r="D44" s="425">
+      <c r="D44" s="422">
         <v>0</v>
       </c>
       <c r="E44" s="48">
@@ -5156,7 +5228,7 @@
       <c r="G44" s="48">
         <v>0</v>
       </c>
-      <c r="H44" s="425">
+      <c r="H44" s="422">
         <v>0</v>
       </c>
       <c r="I44" s="48">
@@ -5171,6 +5243,58 @@
       <c r="L44" s="48">
         <v>4</v>
       </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="435">
+        <v>44026</v>
+      </c>
+      <c r="B45" s="74">
+        <v>0</v>
+      </c>
+      <c r="C45" s="74">
+        <v>1</v>
+      </c>
+      <c r="D45" s="74">
+        <v>0</v>
+      </c>
+      <c r="E45" s="74">
+        <v>1</v>
+      </c>
+      <c r="F45" s="74">
+        <v>1</v>
+      </c>
+      <c r="G45" s="74">
+        <v>0</v>
+      </c>
+      <c r="H45" s="74">
+        <v>0</v>
+      </c>
+      <c r="I45" s="74">
+        <v>0</v>
+      </c>
+      <c r="J45" s="74">
+        <v>1</v>
+      </c>
+      <c r="K45" s="74">
+        <v>0</v>
+      </c>
+      <c r="L45" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5183,7 +5307,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7036,7 +7160,7 @@
       <c r="C44" s="48">
         <v>1</v>
       </c>
-      <c r="D44" s="425">
+      <c r="D44" s="422">
         <v>0</v>
       </c>
       <c r="E44" s="48">
@@ -7054,7 +7178,7 @@
       <c r="I44" s="48">
         <v>0</v>
       </c>
-      <c r="J44" s="425">
+      <c r="J44" s="422">
         <v>0</v>
       </c>
       <c r="K44" s="48">
@@ -7071,20 +7195,48 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
+      <c r="A45" s="436">
+        <v>44026</v>
+      </c>
+      <c r="B45" s="48">
+        <v>0</v>
+      </c>
+      <c r="C45" s="48">
+        <v>1</v>
+      </c>
+      <c r="D45" s="48">
+        <v>0</v>
+      </c>
+      <c r="E45" s="48">
+        <v>0</v>
+      </c>
+      <c r="F45" s="48">
+        <v>1</v>
+      </c>
+      <c r="G45" s="48">
+        <v>1</v>
+      </c>
+      <c r="H45" s="48">
+        <v>1</v>
+      </c>
+      <c r="I45" s="48">
+        <v>0</v>
+      </c>
+      <c r="J45" s="48">
+        <v>0</v>
+      </c>
+      <c r="K45" s="48">
+        <v>1</v>
+      </c>
+      <c r="L45" s="48">
+        <v>1</v>
+      </c>
+      <c r="M45" s="48">
+        <v>0</v>
+      </c>
+      <c r="N45" s="48">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7093,11 +7245,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8518,6 +8670,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="47">
+        <v>44026</v>
+      </c>
+      <c r="B45" s="74">
+        <v>0</v>
+      </c>
+      <c r="C45" s="74">
+        <v>0</v>
+      </c>
+      <c r="D45" s="74">
+        <v>0</v>
+      </c>
+      <c r="E45" s="74">
+        <v>0</v>
+      </c>
+      <c r="F45" s="74">
+        <v>2</v>
+      </c>
+      <c r="G45" s="74">
+        <v>1</v>
+      </c>
+      <c r="H45" s="74">
+        <v>1</v>
+      </c>
+      <c r="I45" s="74">
+        <v>1</v>
+      </c>
+      <c r="J45" s="74">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8527,8 +8711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8669,7 +8853,9 @@
       <c r="AR1" s="49">
         <v>44025</v>
       </c>
-      <c r="AS1" s="48"/>
+      <c r="AS1" s="49">
+        <v>44026</v>
+      </c>
       <c r="AT1" s="48"/>
       <c r="AU1" s="48"/>
       <c r="AV1" s="48"/>
@@ -8807,7 +8993,9 @@
       <c r="AR2" s="48">
         <v>4340</v>
       </c>
-      <c r="AS2" s="48"/>
+      <c r="AS2" s="48">
+        <v>4372</v>
+      </c>
       <c r="AT2" s="48"/>
       <c r="AU2" s="48"/>
       <c r="AV2" s="48"/>
@@ -8945,7 +9133,9 @@
       <c r="AR3" s="48">
         <v>4148</v>
       </c>
-      <c r="AS3" s="48"/>
+      <c r="AS3" s="48">
+        <v>4180</v>
+      </c>
       <c r="AT3" s="48"/>
       <c r="AU3" s="48"/>
       <c r="AV3" s="48"/>
@@ -9083,7 +9273,9 @@
       <c r="AR4" s="48">
         <v>4148</v>
       </c>
-      <c r="AS4" s="48"/>
+      <c r="AS4" s="48">
+        <v>4180</v>
+      </c>
       <c r="AT4" s="48"/>
       <c r="AU4" s="48"/>
       <c r="AV4" s="48"/>
@@ -9221,7 +9413,9 @@
       <c r="AR5" s="48">
         <v>4148</v>
       </c>
-      <c r="AS5" s="48"/>
+      <c r="AS5" s="48">
+        <v>4180</v>
+      </c>
       <c r="AT5" s="48"/>
       <c r="AU5" s="48"/>
       <c r="AV5" s="48"/>
@@ -9359,7 +9553,9 @@
       <c r="AR6" s="48">
         <v>4148</v>
       </c>
-      <c r="AS6" s="48"/>
+      <c r="AS6" s="48">
+        <v>4180</v>
+      </c>
       <c r="AT6" s="48"/>
       <c r="AU6" s="48"/>
       <c r="AV6" s="48"/>
@@ -9497,7 +9693,9 @@
       <c r="AR7" s="48">
         <v>3399</v>
       </c>
-      <c r="AS7" s="48"/>
+      <c r="AS7" s="48">
+        <v>3431</v>
+      </c>
       <c r="AT7" s="48"/>
       <c r="AU7" s="48"/>
       <c r="AV7" s="48"/>
@@ -9635,7 +9833,9 @@
       <c r="AR8" s="48">
         <v>6030</v>
       </c>
-      <c r="AS8" s="48"/>
+      <c r="AS8" s="48">
+        <v>6062</v>
+      </c>
       <c r="AT8" s="48"/>
       <c r="AU8" s="48"/>
       <c r="AV8" s="48"/>
@@ -9685,7 +9885,7 @@
       <c r="AP9" s="312"/>
       <c r="AQ9" s="312"/>
       <c r="AR9" s="312"/>
-      <c r="AS9" s="48"/>
+      <c r="AS9" s="312"/>
       <c r="AT9" s="48"/>
       <c r="AU9" s="48"/>
       <c r="AV9" s="48"/>
@@ -9823,7 +10023,9 @@
       <c r="AR10" s="48">
         <v>183</v>
       </c>
-      <c r="AS10" s="48"/>
+      <c r="AS10" s="48">
+        <v>184</v>
+      </c>
       <c r="AT10" s="48"/>
       <c r="AU10" s="48"/>
       <c r="AV10" s="48"/>
@@ -9961,7 +10163,9 @@
       <c r="AR11" s="48">
         <v>183</v>
       </c>
-      <c r="AS11" s="48"/>
+      <c r="AS11" s="48">
+        <v>184</v>
+      </c>
       <c r="AT11" s="48"/>
       <c r="AU11" s="48"/>
       <c r="AV11" s="48"/>
@@ -10099,7 +10303,9 @@
       <c r="AR12" s="48">
         <v>183</v>
       </c>
-      <c r="AS12" s="48"/>
+      <c r="AS12" s="48">
+        <v>184</v>
+      </c>
       <c r="AT12" s="48"/>
       <c r="AU12" s="48"/>
       <c r="AV12" s="48"/>
@@ -10237,7 +10443,9 @@
       <c r="AR13" s="48">
         <v>183</v>
       </c>
-      <c r="AS13" s="48"/>
+      <c r="AS13" s="48">
+        <v>184</v>
+      </c>
       <c r="AT13" s="48"/>
       <c r="AU13" s="48"/>
       <c r="AV13" s="48"/>
@@ -10375,7 +10583,9 @@
       <c r="AR14" s="48">
         <v>183</v>
       </c>
-      <c r="AS14" s="48"/>
+      <c r="AS14" s="48">
+        <v>184</v>
+      </c>
       <c r="AT14" s="48"/>
       <c r="AU14" s="48"/>
       <c r="AV14" s="48"/>
@@ -10513,7 +10723,9 @@
       <c r="AR15" s="48">
         <v>118</v>
       </c>
-      <c r="AS15" s="48"/>
+      <c r="AS15" s="48">
+        <v>119</v>
+      </c>
       <c r="AT15" s="48"/>
       <c r="AU15" s="48"/>
       <c r="AV15" s="48"/>
@@ -10651,7 +10863,9 @@
       <c r="AR16" s="48">
         <v>195</v>
       </c>
-      <c r="AS16" s="48"/>
+      <c r="AS16" s="48">
+        <v>196</v>
+      </c>
       <c r="AT16" s="48"/>
       <c r="AU16" s="48"/>
       <c r="AV16" s="48"/>
@@ -10701,7 +10915,7 @@
       <c r="AP17" s="312"/>
       <c r="AQ17" s="312"/>
       <c r="AR17" s="312"/>
-      <c r="AS17" s="48"/>
+      <c r="AS17" s="312"/>
       <c r="AT17" s="48"/>
       <c r="AU17" s="48"/>
       <c r="AV17" s="48"/>
@@ -10839,7 +11053,9 @@
       <c r="AR18" s="48">
         <v>1010</v>
       </c>
-      <c r="AS18" s="48"/>
+      <c r="AS18" s="48">
+        <v>1017</v>
+      </c>
       <c r="AT18" s="48"/>
       <c r="AU18" s="48"/>
       <c r="AV18" s="48"/>
@@ -11027,6 +11243,13 @@
         <f>SUM(AR2:AR18)</f>
         <v>32599</v>
       </c>
+      <c r="AS20" s="51">
+        <f>SUM(AS2:AS18)</f>
+        <v>32837</v>
+      </c>
+      <c r="AT20" s="48"/>
+      <c r="AU20" s="48"/>
+      <c r="AV20" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11037,7 +11260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -11325,43 +11548,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="422" t="s">
+      <c r="B8" s="432" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="422"/>
+      <c r="B9" s="432"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="422"/>
+      <c r="B10" s="432"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="422"/>
+      <c r="B11" s="432"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="423" t="s">
+      <c r="B12" s="433" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="423"/>
+      <c r="B13" s="433"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="423"/>
+      <c r="B14" s="433"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="424" t="s">
+      <c r="B15" s="434" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="424"/>
+      <c r="B16" s="434"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 15th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F2B371-B1DD-1040-A617-DE13C43AABE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F7BE7B-A801-4043-A058-CE5E2CF7172B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1420" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="3140" yWindow="460" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -279,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,13 +344,6 @@
       <color theme="1"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="18">
@@ -570,7 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="437">
+  <cellXfs count="444">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1817,6 +1810,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1825,12 +1845,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2151,15 +2165,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3600,6 +3614,38 @@
       </c>
       <c r="J45" s="431">
         <v>756137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="15">
+        <v>44027</v>
+      </c>
+      <c r="B46" s="432">
+        <v>317635</v>
+      </c>
+      <c r="C46" s="433">
+        <v>369411</v>
+      </c>
+      <c r="D46" s="434">
+        <v>81411</v>
+      </c>
+      <c r="E46" s="435">
+        <v>36906</v>
+      </c>
+      <c r="F46" s="436">
+        <v>29.054732633368491</v>
+      </c>
+      <c r="G46" s="437">
+        <v>92288</v>
+      </c>
+      <c r="H46" s="438">
+        <v>7681</v>
+      </c>
+      <c r="I46" s="439">
+        <v>8921</v>
+      </c>
+      <c r="J46" s="440">
+        <v>768457</v>
       </c>
     </row>
   </sheetData>
@@ -3613,15 +3659,15 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -5245,7 +5291,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="435">
+      <c r="A45" s="47">
         <v>44026</v>
       </c>
       <c r="B45" s="74">
@@ -5283,18 +5329,42 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
+      <c r="A46" s="47">
+        <v>44027</v>
+      </c>
+      <c r="B46" s="48">
+        <v>0</v>
+      </c>
+      <c r="C46" s="48">
+        <v>1</v>
+      </c>
+      <c r="D46" s="48">
+        <v>0</v>
+      </c>
+      <c r="E46" s="48">
+        <v>0</v>
+      </c>
+      <c r="F46" s="48">
+        <v>1</v>
+      </c>
+      <c r="G46" s="48">
+        <v>0</v>
+      </c>
+      <c r="H46" s="48">
+        <v>0</v>
+      </c>
+      <c r="I46" s="48">
+        <v>0</v>
+      </c>
+      <c r="J46" s="48">
+        <v>1</v>
+      </c>
+      <c r="K46" s="48">
+        <v>0</v>
+      </c>
+      <c r="L46" s="48">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5303,11 +5373,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7195,7 +7265,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="436">
+      <c r="A45" s="47">
         <v>44026</v>
       </c>
       <c r="B45" s="48">
@@ -7235,6 +7305,50 @@
         <v>0</v>
       </c>
       <c r="N45" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="47">
+        <v>44027</v>
+      </c>
+      <c r="B46" s="74">
+        <v>0</v>
+      </c>
+      <c r="C46" s="74">
+        <v>1</v>
+      </c>
+      <c r="D46" s="74">
+        <v>0</v>
+      </c>
+      <c r="E46" s="74">
+        <v>0</v>
+      </c>
+      <c r="F46" s="74">
+        <v>1</v>
+      </c>
+      <c r="G46" s="74">
+        <v>0</v>
+      </c>
+      <c r="H46" s="74">
+        <v>1</v>
+      </c>
+      <c r="I46" s="74">
+        <v>0</v>
+      </c>
+      <c r="J46" s="74">
+        <v>0</v>
+      </c>
+      <c r="K46" s="74">
+        <v>1</v>
+      </c>
+      <c r="L46" s="74">
+        <v>1</v>
+      </c>
+      <c r="M46" s="74">
+        <v>0</v>
+      </c>
+      <c r="N46" s="74">
         <v>0</v>
       </c>
     </row>
@@ -7245,21 +7359,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -8701,6 +8815,50 @@
       <c r="J45" s="74">
         <v>2</v>
       </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="47">
+        <v>44027</v>
+      </c>
+      <c r="B46" s="74">
+        <v>0</v>
+      </c>
+      <c r="C46" s="74">
+        <v>0</v>
+      </c>
+      <c r="D46" s="74">
+        <v>0</v>
+      </c>
+      <c r="E46" s="74">
+        <v>0</v>
+      </c>
+      <c r="F46" s="74">
+        <v>2</v>
+      </c>
+      <c r="G46" s="74">
+        <v>1</v>
+      </c>
+      <c r="H46" s="74">
+        <v>1</v>
+      </c>
+      <c r="I46" s="74">
+        <v>1</v>
+      </c>
+      <c r="J46" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8712,12 +8870,12 @@
   <dimension ref="A1:AV20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AV17" sqref="AV17"/>
+      <selection activeCell="AU12" sqref="AU12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
@@ -8856,7 +9014,9 @@
       <c r="AS1" s="49">
         <v>44026</v>
       </c>
-      <c r="AT1" s="48"/>
+      <c r="AT1" s="49">
+        <v>44027</v>
+      </c>
       <c r="AU1" s="48"/>
       <c r="AV1" s="48"/>
     </row>
@@ -8996,7 +9156,9 @@
       <c r="AS2" s="48">
         <v>4372</v>
       </c>
-      <c r="AT2" s="48"/>
+      <c r="AT2" s="48">
+        <v>4374</v>
+      </c>
       <c r="AU2" s="48"/>
       <c r="AV2" s="48"/>
     </row>
@@ -9136,7 +9298,9 @@
       <c r="AS3" s="48">
         <v>4180</v>
       </c>
-      <c r="AT3" s="48"/>
+      <c r="AT3" s="48">
+        <v>4181</v>
+      </c>
       <c r="AU3" s="48"/>
       <c r="AV3" s="48"/>
     </row>
@@ -9276,7 +9440,9 @@
       <c r="AS4" s="48">
         <v>4180</v>
       </c>
-      <c r="AT4" s="48"/>
+      <c r="AT4" s="48">
+        <v>4181</v>
+      </c>
       <c r="AU4" s="48"/>
       <c r="AV4" s="48"/>
     </row>
@@ -9416,7 +9582,9 @@
       <c r="AS5" s="48">
         <v>4180</v>
       </c>
-      <c r="AT5" s="48"/>
+      <c r="AT5" s="48">
+        <v>4181</v>
+      </c>
       <c r="AU5" s="48"/>
       <c r="AV5" s="48"/>
     </row>
@@ -9556,7 +9724,9 @@
       <c r="AS6" s="48">
         <v>4180</v>
       </c>
-      <c r="AT6" s="48"/>
+      <c r="AT6" s="48">
+        <v>4181</v>
+      </c>
       <c r="AU6" s="48"/>
       <c r="AV6" s="48"/>
     </row>
@@ -9696,7 +9866,9 @@
       <c r="AS7" s="48">
         <v>3431</v>
       </c>
-      <c r="AT7" s="48"/>
+      <c r="AT7" s="48">
+        <v>3463</v>
+      </c>
       <c r="AU7" s="48"/>
       <c r="AV7" s="48"/>
     </row>
@@ -9836,7 +10008,9 @@
       <c r="AS8" s="48">
         <v>6062</v>
       </c>
-      <c r="AT8" s="48"/>
+      <c r="AT8" s="48">
+        <v>6094</v>
+      </c>
       <c r="AU8" s="48"/>
       <c r="AV8" s="48"/>
     </row>
@@ -9886,7 +10060,7 @@
       <c r="AQ9" s="312"/>
       <c r="AR9" s="312"/>
       <c r="AS9" s="312"/>
-      <c r="AT9" s="48"/>
+      <c r="AT9" s="312"/>
       <c r="AU9" s="48"/>
       <c r="AV9" s="48"/>
     </row>
@@ -10026,7 +10200,9 @@
       <c r="AS10" s="48">
         <v>184</v>
       </c>
-      <c r="AT10" s="48"/>
+      <c r="AT10" s="48">
+        <v>185</v>
+      </c>
       <c r="AU10" s="48"/>
       <c r="AV10" s="48"/>
     </row>
@@ -10166,7 +10342,9 @@
       <c r="AS11" s="48">
         <v>184</v>
       </c>
-      <c r="AT11" s="48"/>
+      <c r="AT11" s="48">
+        <v>185</v>
+      </c>
       <c r="AU11" s="48"/>
       <c r="AV11" s="48"/>
     </row>
@@ -10306,7 +10484,9 @@
       <c r="AS12" s="48">
         <v>184</v>
       </c>
-      <c r="AT12" s="48"/>
+      <c r="AT12" s="48">
+        <v>185</v>
+      </c>
       <c r="AU12" s="48"/>
       <c r="AV12" s="48"/>
     </row>
@@ -10446,7 +10626,9 @@
       <c r="AS13" s="48">
         <v>184</v>
       </c>
-      <c r="AT13" s="48"/>
+      <c r="AT13" s="48">
+        <v>185</v>
+      </c>
       <c r="AU13" s="48"/>
       <c r="AV13" s="48"/>
     </row>
@@ -10586,7 +10768,9 @@
       <c r="AS14" s="48">
         <v>184</v>
       </c>
-      <c r="AT14" s="48"/>
+      <c r="AT14" s="48">
+        <v>185</v>
+      </c>
       <c r="AU14" s="48"/>
       <c r="AV14" s="48"/>
     </row>
@@ -10726,7 +10910,9 @@
       <c r="AS15" s="48">
         <v>119</v>
       </c>
-      <c r="AT15" s="48"/>
+      <c r="AT15" s="48">
+        <v>120</v>
+      </c>
       <c r="AU15" s="48"/>
       <c r="AV15" s="48"/>
     </row>
@@ -10866,7 +11052,9 @@
       <c r="AS16" s="48">
         <v>196</v>
       </c>
-      <c r="AT16" s="48"/>
+      <c r="AT16" s="48">
+        <v>197</v>
+      </c>
       <c r="AU16" s="48"/>
       <c r="AV16" s="48"/>
     </row>
@@ -10916,7 +11104,7 @@
       <c r="AQ17" s="312"/>
       <c r="AR17" s="312"/>
       <c r="AS17" s="312"/>
-      <c r="AT17" s="48"/>
+      <c r="AT17" s="312"/>
       <c r="AU17" s="48"/>
       <c r="AV17" s="48"/>
     </row>
@@ -11056,7 +11244,9 @@
       <c r="AS18" s="48">
         <v>1017</v>
       </c>
-      <c r="AT18" s="48"/>
+      <c r="AT18" s="48">
+        <v>1024</v>
+      </c>
       <c r="AU18" s="48"/>
       <c r="AV18" s="48"/>
     </row>
@@ -11247,7 +11437,10 @@
         <f>SUM(AS2:AS18)</f>
         <v>32837</v>
       </c>
-      <c r="AT20" s="48"/>
+      <c r="AT20" s="51">
+        <f>SUM(AT2:AT18)</f>
+        <v>32921</v>
+      </c>
       <c r="AU20" s="48"/>
       <c r="AV20" s="48"/>
     </row>
@@ -11471,9 +11664,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -11548,43 +11741,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="432" t="s">
+      <c r="B8" s="441" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="432"/>
+      <c r="B9" s="441"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="432"/>
+      <c r="B10" s="441"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="432"/>
+      <c r="B11" s="441"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="433" t="s">
+      <c r="B12" s="442" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="433"/>
+      <c r="B13" s="442"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="433"/>
+      <c r="B14" s="442"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="434" t="s">
+      <c r="B15" s="443" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="434"/>
+      <c r="B16" s="443"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 16th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F7BE7B-A801-4043-A058-CE5E2CF7172B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2B84F0-0113-344B-B132-4A94373F132B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="460" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33660" yWindow="10100" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="444">
+  <cellXfs count="453">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1783,6 +1783,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2165,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3648,6 +3675,38 @@
         <v>768457</v>
       </c>
     </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="15">
+        <v>44028</v>
+      </c>
+      <c r="B47" s="441">
+        <v>324041</v>
+      </c>
+      <c r="C47" s="442">
+        <v>375455</v>
+      </c>
+      <c r="D47" s="443">
+        <v>82567</v>
+      </c>
+      <c r="E47" s="444">
+        <v>37574</v>
+      </c>
+      <c r="F47" s="445">
+        <v>28.953743507765996</v>
+      </c>
+      <c r="G47" s="446">
+        <v>93822</v>
+      </c>
+      <c r="H47" s="447">
+        <v>7801</v>
+      </c>
+      <c r="I47" s="448">
+        <v>9092</v>
+      </c>
+      <c r="J47" s="449">
+        <v>782063</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3655,11 +3714,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5366,6 +5425,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="47">
+        <v>44028</v>
+      </c>
+      <c r="B47" s="74">
+        <v>0</v>
+      </c>
+      <c r="C47" s="74">
+        <v>1</v>
+      </c>
+      <c r="D47" s="74">
+        <v>0</v>
+      </c>
+      <c r="E47" s="74">
+        <v>0</v>
+      </c>
+      <c r="F47" s="74">
+        <v>1</v>
+      </c>
+      <c r="G47" s="74">
+        <v>0</v>
+      </c>
+      <c r="H47" s="74">
+        <v>0</v>
+      </c>
+      <c r="I47" s="74">
+        <v>0</v>
+      </c>
+      <c r="J47" s="74">
+        <v>1</v>
+      </c>
+      <c r="K47" s="74">
+        <v>0</v>
+      </c>
+      <c r="L47" s="74">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5373,11 +5470,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7349,6 +7446,50 @@
         <v>0</v>
       </c>
       <c r="N46" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="47">
+        <v>44028</v>
+      </c>
+      <c r="B47" s="74">
+        <v>0</v>
+      </c>
+      <c r="C47" s="74">
+        <v>1</v>
+      </c>
+      <c r="D47" s="74">
+        <v>0</v>
+      </c>
+      <c r="E47" s="74">
+        <v>0</v>
+      </c>
+      <c r="F47" s="74">
+        <v>1</v>
+      </c>
+      <c r="G47" s="74">
+        <v>0</v>
+      </c>
+      <c r="H47" s="74">
+        <v>1</v>
+      </c>
+      <c r="I47" s="74">
+        <v>0</v>
+      </c>
+      <c r="J47" s="74">
+        <v>0</v>
+      </c>
+      <c r="K47" s="74">
+        <v>1</v>
+      </c>
+      <c r="L47" s="74">
+        <v>1</v>
+      </c>
+      <c r="M47" s="74">
+        <v>0</v>
+      </c>
+      <c r="N47" s="74">
         <v>0</v>
       </c>
     </row>
@@ -7363,7 +7504,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:J47"/>
+      <selection pane="bottomLeft" activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8849,16 +8990,36 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="48"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
+      <c r="A47" s="47">
+        <v>44028</v>
+      </c>
+      <c r="B47" s="48">
+        <v>0</v>
+      </c>
+      <c r="C47" s="48">
+        <v>0</v>
+      </c>
+      <c r="D47" s="48">
+        <v>0</v>
+      </c>
+      <c r="E47" s="48">
+        <v>0</v>
+      </c>
+      <c r="F47" s="48">
+        <v>2</v>
+      </c>
+      <c r="G47" s="48">
+        <v>1</v>
+      </c>
+      <c r="H47" s="48">
+        <v>1</v>
+      </c>
+      <c r="I47" s="48">
+        <v>1</v>
+      </c>
+      <c r="J47" s="48">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8869,8 +9030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AU12" sqref="AU12"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AQ13" sqref="AQ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9017,7 +9178,9 @@
       <c r="AT1" s="49">
         <v>44027</v>
       </c>
-      <c r="AU1" s="48"/>
+      <c r="AU1" s="49">
+        <v>44028</v>
+      </c>
       <c r="AV1" s="48"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
@@ -9159,7 +9322,9 @@
       <c r="AT2" s="48">
         <v>4374</v>
       </c>
-      <c r="AU2" s="48"/>
+      <c r="AU2" s="48">
+        <v>4406</v>
+      </c>
       <c r="AV2" s="48"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
@@ -9301,7 +9466,9 @@
       <c r="AT3" s="48">
         <v>4181</v>
       </c>
-      <c r="AU3" s="48"/>
+      <c r="AU3" s="48">
+        <v>4213</v>
+      </c>
       <c r="AV3" s="48"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
@@ -9443,7 +9610,9 @@
       <c r="AT4" s="48">
         <v>4181</v>
       </c>
-      <c r="AU4" s="48"/>
+      <c r="AU4" s="48">
+        <v>4213</v>
+      </c>
       <c r="AV4" s="48"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -9585,7 +9754,9 @@
       <c r="AT5" s="48">
         <v>4181</v>
       </c>
-      <c r="AU5" s="48"/>
+      <c r="AU5" s="48">
+        <v>4213</v>
+      </c>
       <c r="AV5" s="48"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
@@ -9727,7 +9898,9 @@
       <c r="AT6" s="48">
         <v>4181</v>
       </c>
-      <c r="AU6" s="48"/>
+      <c r="AU6" s="48">
+        <v>4213</v>
+      </c>
       <c r="AV6" s="48"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.2">
@@ -9869,7 +10042,9 @@
       <c r="AT7" s="48">
         <v>3463</v>
       </c>
-      <c r="AU7" s="48"/>
+      <c r="AU7" s="48">
+        <v>3495</v>
+      </c>
       <c r="AV7" s="48"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
@@ -10011,7 +10186,9 @@
       <c r="AT8" s="48">
         <v>6094</v>
       </c>
-      <c r="AU8" s="48"/>
+      <c r="AU8" s="48">
+        <v>6126</v>
+      </c>
       <c r="AV8" s="48"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.2">
@@ -10061,7 +10238,7 @@
       <c r="AR9" s="312"/>
       <c r="AS9" s="312"/>
       <c r="AT9" s="312"/>
-      <c r="AU9" s="48"/>
+      <c r="AU9" s="312"/>
       <c r="AV9" s="48"/>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.2">
@@ -10203,7 +10380,9 @@
       <c r="AT10" s="48">
         <v>185</v>
       </c>
-      <c r="AU10" s="48"/>
+      <c r="AU10" s="48">
+        <v>186</v>
+      </c>
       <c r="AV10" s="48"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.2">
@@ -10345,7 +10524,9 @@
       <c r="AT11" s="48">
         <v>185</v>
       </c>
-      <c r="AU11" s="48"/>
+      <c r="AU11" s="48">
+        <v>186</v>
+      </c>
       <c r="AV11" s="48"/>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.2">
@@ -10487,7 +10668,9 @@
       <c r="AT12" s="48">
         <v>185</v>
       </c>
-      <c r="AU12" s="48"/>
+      <c r="AU12" s="48">
+        <v>186</v>
+      </c>
       <c r="AV12" s="48"/>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.2">
@@ -10629,7 +10812,9 @@
       <c r="AT13" s="48">
         <v>185</v>
       </c>
-      <c r="AU13" s="48"/>
+      <c r="AU13" s="48">
+        <v>186</v>
+      </c>
       <c r="AV13" s="48"/>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.2">
@@ -10771,7 +10956,9 @@
       <c r="AT14" s="48">
         <v>185</v>
       </c>
-      <c r="AU14" s="48"/>
+      <c r="AU14" s="48">
+        <v>186</v>
+      </c>
       <c r="AV14" s="48"/>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.2">
@@ -10913,7 +11100,9 @@
       <c r="AT15" s="48">
         <v>120</v>
       </c>
-      <c r="AU15" s="48"/>
+      <c r="AU15" s="48">
+        <v>121</v>
+      </c>
       <c r="AV15" s="48"/>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.2">
@@ -11055,7 +11244,9 @@
       <c r="AT16" s="48">
         <v>197</v>
       </c>
-      <c r="AU16" s="48"/>
+      <c r="AU16" s="48">
+        <v>198</v>
+      </c>
       <c r="AV16" s="48"/>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.2">
@@ -11105,7 +11296,7 @@
       <c r="AR17" s="312"/>
       <c r="AS17" s="312"/>
       <c r="AT17" s="312"/>
-      <c r="AU17" s="48"/>
+      <c r="AU17" s="312"/>
       <c r="AV17" s="48"/>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.2">
@@ -11247,7 +11438,9 @@
       <c r="AT18" s="48">
         <v>1024</v>
       </c>
-      <c r="AU18" s="48"/>
+      <c r="AU18" s="48">
+        <v>1031</v>
+      </c>
       <c r="AV18" s="48"/>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.2">
@@ -11441,7 +11634,10 @@
         <f>SUM(AT2:AT18)</f>
         <v>32921</v>
       </c>
-      <c r="AU20" s="48"/>
+      <c r="AU20" s="51">
+        <f>SUM(AU2:AU18)</f>
+        <v>33159</v>
+      </c>
       <c r="AV20" s="48"/>
     </row>
   </sheetData>
@@ -11741,43 +11937,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="441" t="s">
+      <c r="B8" s="450" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="441"/>
+      <c r="B9" s="450"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="441"/>
+      <c r="B10" s="450"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="441"/>
+      <c r="B11" s="450"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="442" t="s">
+      <c r="B12" s="451" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="442"/>
+      <c r="B13" s="451"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="442"/>
+      <c r="B14" s="451"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="443" t="s">
+      <c r="B15" s="452" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="443"/>
+      <c r="B16" s="452"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 17th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2B84F0-0113-344B-B132-4A94373F132B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC9B238-AC06-8F40-9FC7-5DE73F6DECF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33660" yWindow="10100" windowWidth="22840" windowHeight="12040" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33660" yWindow="10100" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="453">
+  <cellXfs count="462">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1783,6 +1783,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2192,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3707,6 +3734,38 @@
         <v>782063</v>
       </c>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
+        <v>44029</v>
+      </c>
+      <c r="B48" s="450">
+        <v>331298</v>
+      </c>
+      <c r="C48" s="451">
+        <v>382003</v>
+      </c>
+      <c r="D48" s="452">
+        <v>85877</v>
+      </c>
+      <c r="E48" s="453">
+        <v>38310</v>
+      </c>
+      <c r="F48" s="454">
+        <v>28.813334218739623</v>
+      </c>
+      <c r="G48" s="455">
+        <v>95458</v>
+      </c>
+      <c r="H48" s="456">
+        <v>7904</v>
+      </c>
+      <c r="I48" s="457">
+        <v>9237</v>
+      </c>
+      <c r="J48" s="458">
+        <v>799178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3714,11 +3773,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5463,6 +5522,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="47">
+        <v>44029</v>
+      </c>
+      <c r="B48" s="216">
+        <v>0</v>
+      </c>
+      <c r="C48" s="216">
+        <v>1</v>
+      </c>
+      <c r="D48" s="216">
+        <v>0</v>
+      </c>
+      <c r="E48" s="216">
+        <v>0</v>
+      </c>
+      <c r="F48" s="216">
+        <v>1</v>
+      </c>
+      <c r="G48" s="216">
+        <v>0</v>
+      </c>
+      <c r="H48" s="216">
+        <v>0</v>
+      </c>
+      <c r="I48" s="216">
+        <v>0</v>
+      </c>
+      <c r="J48" s="216">
+        <v>1</v>
+      </c>
+      <c r="K48" s="216">
+        <v>0</v>
+      </c>
+      <c r="L48" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5470,11 +5567,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7490,6 +7587,50 @@
         <v>0</v>
       </c>
       <c r="N47" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="47">
+        <v>44029</v>
+      </c>
+      <c r="B48" s="216">
+        <v>0</v>
+      </c>
+      <c r="C48" s="216">
+        <v>1</v>
+      </c>
+      <c r="D48" s="216">
+        <v>0</v>
+      </c>
+      <c r="E48" s="216">
+        <v>0</v>
+      </c>
+      <c r="F48" s="216">
+        <v>1</v>
+      </c>
+      <c r="G48" s="216">
+        <v>0</v>
+      </c>
+      <c r="H48" s="216">
+        <v>1</v>
+      </c>
+      <c r="I48" s="216">
+        <v>0</v>
+      </c>
+      <c r="J48" s="216">
+        <v>0</v>
+      </c>
+      <c r="K48" s="216">
+        <v>1</v>
+      </c>
+      <c r="L48" s="216">
+        <v>1</v>
+      </c>
+      <c r="M48" s="216">
+        <v>0</v>
+      </c>
+      <c r="N48" s="216">
         <v>0</v>
       </c>
     </row>
@@ -7500,11 +7641,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L47" sqref="L47"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9021,6 +9162,41 @@
         <v>2</v>
       </c>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="47">
+        <v>44029</v>
+      </c>
+      <c r="B48" s="216">
+        <v>0</v>
+      </c>
+      <c r="C48" s="216">
+        <v>0</v>
+      </c>
+      <c r="D48" s="216">
+        <v>0</v>
+      </c>
+      <c r="E48" s="216">
+        <v>0</v>
+      </c>
+      <c r="F48" s="216">
+        <v>2</v>
+      </c>
+      <c r="G48" s="216">
+        <v>1</v>
+      </c>
+      <c r="H48" s="216">
+        <v>1</v>
+      </c>
+      <c r="I48" s="216">
+        <v>1</v>
+      </c>
+      <c r="J48" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="47"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9030,8 +9206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:AV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AQ13" sqref="AQ13"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW12" sqref="AW12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9181,7 +9357,9 @@
       <c r="AU1" s="49">
         <v>44028</v>
       </c>
-      <c r="AV1" s="48"/>
+      <c r="AV1" s="49">
+        <v>44029</v>
+      </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -9325,7 +9503,9 @@
       <c r="AU2" s="48">
         <v>4406</v>
       </c>
-      <c r="AV2" s="48"/>
+      <c r="AV2" s="48">
+        <v>4438</v>
+      </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -9469,7 +9649,9 @@
       <c r="AU3" s="48">
         <v>4213</v>
       </c>
-      <c r="AV3" s="48"/>
+      <c r="AV3" s="48">
+        <v>4245</v>
+      </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -9613,7 +9795,9 @@
       <c r="AU4" s="48">
         <v>4213</v>
       </c>
-      <c r="AV4" s="48"/>
+      <c r="AV4" s="48">
+        <v>4245</v>
+      </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -9757,7 +9941,9 @@
       <c r="AU5" s="48">
         <v>4213</v>
       </c>
-      <c r="AV5" s="48"/>
+      <c r="AV5" s="48">
+        <v>4245</v>
+      </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -9901,7 +10087,9 @@
       <c r="AU6" s="48">
         <v>4213</v>
       </c>
-      <c r="AV6" s="48"/>
+      <c r="AV6" s="48">
+        <v>4245</v>
+      </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -10045,7 +10233,9 @@
       <c r="AU7" s="48">
         <v>3495</v>
       </c>
-      <c r="AV7" s="48"/>
+      <c r="AV7" s="48">
+        <v>3527</v>
+      </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -10189,7 +10379,9 @@
       <c r="AU8" s="48">
         <v>6126</v>
       </c>
-      <c r="AV8" s="48"/>
+      <c r="AV8" s="48">
+        <v>6158</v>
+      </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
@@ -10239,7 +10431,7 @@
       <c r="AS9" s="312"/>
       <c r="AT9" s="312"/>
       <c r="AU9" s="312"/>
-      <c r="AV9" s="48"/>
+      <c r="AV9" s="312"/>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
@@ -10383,7 +10575,9 @@
       <c r="AU10" s="48">
         <v>186</v>
       </c>
-      <c r="AV10" s="48"/>
+      <c r="AV10" s="48">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -10527,7 +10721,9 @@
       <c r="AU11" s="48">
         <v>186</v>
       </c>
-      <c r="AV11" s="48"/>
+      <c r="AV11" s="48">
+        <v>187</v>
+      </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -10671,7 +10867,9 @@
       <c r="AU12" s="48">
         <v>186</v>
       </c>
-      <c r="AV12" s="48"/>
+      <c r="AV12" s="48">
+        <v>187</v>
+      </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -10815,7 +11013,9 @@
       <c r="AU13" s="48">
         <v>186</v>
       </c>
-      <c r="AV13" s="48"/>
+      <c r="AV13" s="48">
+        <v>187</v>
+      </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -10959,7 +11159,9 @@
       <c r="AU14" s="48">
         <v>186</v>
       </c>
-      <c r="AV14" s="48"/>
+      <c r="AV14" s="48">
+        <v>187</v>
+      </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -11103,7 +11305,9 @@
       <c r="AU15" s="48">
         <v>121</v>
       </c>
-      <c r="AV15" s="48"/>
+      <c r="AV15" s="48">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -11247,7 +11451,9 @@
       <c r="AU16" s="48">
         <v>198</v>
       </c>
-      <c r="AV16" s="48"/>
+      <c r="AV16" s="48">
+        <v>199</v>
+      </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
@@ -11297,7 +11503,7 @@
       <c r="AS17" s="312"/>
       <c r="AT17" s="312"/>
       <c r="AU17" s="312"/>
-      <c r="AV17" s="48"/>
+      <c r="AV17" s="312"/>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
@@ -11441,7 +11647,9 @@
       <c r="AU18" s="48">
         <v>1031</v>
       </c>
-      <c r="AV18" s="48"/>
+      <c r="AV18" s="48">
+        <v>1038</v>
+      </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -11638,7 +11846,10 @@
         <f>SUM(AU2:AU18)</f>
         <v>33159</v>
       </c>
-      <c r="AV20" s="48"/>
+      <c r="AV20" s="51">
+        <f>SUM(AV2:AV18)</f>
+        <v>33397</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11937,43 +12148,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="450" t="s">
+      <c r="B8" s="459" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="450"/>
+      <c r="B9" s="459"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="450"/>
+      <c r="B10" s="459"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="450"/>
+      <c r="B11" s="459"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="451" t="s">
+      <c r="B12" s="460" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="451"/>
+      <c r="B13" s="460"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="451"/>
+      <c r="B14" s="460"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="452" t="s">
+      <c r="B15" s="461" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="452"/>
+      <c r="B16" s="461"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 18th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>Se agrego una nueva fecha a la serie de dates_dx, dates_sx el con fecha del 5 de febrero</t>
+  </si>
+  <si>
+    <t>2020-07-18</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="462">
+  <cellXfs count="472">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1899,6 +1902,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2219,7 +2252,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
@@ -2227,7 +2260,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3764,6 +3797,38 @@
       </c>
       <c r="J48" s="458">
         <v>799178</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="462">
+        <v>77</v>
+      </c>
+      <c r="B49" t="n" s="463">
+        <v>338913.0</v>
+      </c>
+      <c r="C49" t="n" s="464">
+        <v>388636.0</v>
+      </c>
+      <c r="D49" t="n" s="465">
+        <v>87104.0</v>
+      </c>
+      <c r="E49" t="n" s="466">
+        <v>38888.0</v>
+      </c>
+      <c r="F49" t="n" s="467">
+        <v>28.660157621572495</v>
+      </c>
+      <c r="G49" t="n" s="468">
+        <v>97133.0</v>
+      </c>
+      <c r="H49" t="n" s="469">
+        <v>8019.0</v>
+      </c>
+      <c r="I49" t="n" s="470">
+        <v>9412.0</v>
+      </c>
+      <c r="J49" t="n" s="471">
+        <v>814653.0</v>
       </c>
     </row>
   </sheetData>
@@ -3782,10 +3847,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.83203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -7650,12 +7715,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -9212,7 +9277,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.2">
@@ -12071,9 +12136,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="60.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Raw and Clean Data from SSSA for July 19th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>2020-07-18</t>
+  </si>
+  <si>
+    <t>2020-07-19</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="472">
+  <cellXfs count="482">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1902,6 +1905,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -2252,7 +2285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
@@ -3829,6 +3862,38 @@
       </c>
       <c r="J49" t="n" s="471">
         <v>814653.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="472">
+        <v>78</v>
+      </c>
+      <c r="B50" t="n" s="473">
+        <v>344224.0</v>
+      </c>
+      <c r="C50" t="n" s="474">
+        <v>394156.0</v>
+      </c>
+      <c r="D50" t="n" s="475">
+        <v>83542.0</v>
+      </c>
+      <c r="E50" t="n" s="476">
+        <v>39184.0</v>
+      </c>
+      <c r="F50" t="n" s="477">
+        <v>28.552047503950917</v>
+      </c>
+      <c r="G50" t="n" s="478">
+        <v>98283.0</v>
+      </c>
+      <c r="H50" t="n" s="479">
+        <v>8085.0</v>
+      </c>
+      <c r="I50" t="n" s="480">
+        <v>9493.0</v>
+      </c>
+      <c r="J50" t="n" s="481">
+        <v>821922.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 20th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC9B238-AC06-8F40-9FC7-5DE73F6DECF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E10A74-C96C-1349-8C1D-09D5643A1EF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33660" yWindow="10100" windowWidth="22840" windowHeight="12040" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -270,12 +270,6 @@
   </si>
   <si>
     <t>Se agrego una nueva fecha a la serie de dates_dx, dates_sx el con fecha del 5 de febrero</t>
-  </si>
-  <si>
-    <t>2020-07-18</t>
-  </si>
-  <si>
-    <t>2020-07-19</t>
   </si>
 </sst>
 </file>
@@ -569,7 +563,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="482">
+  <cellXfs count="489">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1897,6 +1891,87 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1905,66 +1980,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2285,15 +2300,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -3832,68 +3847,100 @@
         <v>799178</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="s" s="462">
-        <v>77</v>
-      </c>
-      <c r="B49" t="n" s="463">
-        <v>338913.0</v>
-      </c>
-      <c r="C49" t="n" s="464">
-        <v>388636.0</v>
-      </c>
-      <c r="D49" t="n" s="465">
-        <v>87104.0</v>
-      </c>
-      <c r="E49" t="n" s="466">
-        <v>38888.0</v>
-      </c>
-      <c r="F49" t="n" s="467">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="15">
+        <v>44030</v>
+      </c>
+      <c r="B49" s="459">
+        <v>338913</v>
+      </c>
+      <c r="C49" s="460">
+        <v>388636</v>
+      </c>
+      <c r="D49" s="461">
+        <v>87104</v>
+      </c>
+      <c r="E49" s="462">
+        <v>38888</v>
+      </c>
+      <c r="F49" s="463">
         <v>28.660157621572495</v>
       </c>
-      <c r="G49" t="n" s="468">
-        <v>97133.0</v>
-      </c>
-      <c r="H49" t="n" s="469">
-        <v>8019.0</v>
-      </c>
-      <c r="I49" t="n" s="470">
-        <v>9412.0</v>
-      </c>
-      <c r="J49" t="n" s="471">
-        <v>814653.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="472">
-        <v>78</v>
-      </c>
-      <c r="B50" t="n" s="473">
-        <v>344224.0</v>
-      </c>
-      <c r="C50" t="n" s="474">
-        <v>394156.0</v>
-      </c>
-      <c r="D50" t="n" s="475">
-        <v>83542.0</v>
-      </c>
-      <c r="E50" t="n" s="476">
-        <v>39184.0</v>
-      </c>
-      <c r="F50" t="n" s="477">
+      <c r="G49" s="464">
+        <v>97133</v>
+      </c>
+      <c r="H49" s="465">
+        <v>8019</v>
+      </c>
+      <c r="I49" s="466">
+        <v>9412</v>
+      </c>
+      <c r="J49" s="467">
+        <v>814653</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
+        <v>44031</v>
+      </c>
+      <c r="B50" s="468">
+        <v>344224</v>
+      </c>
+      <c r="C50" s="469">
+        <v>394156</v>
+      </c>
+      <c r="D50" s="470">
+        <v>83542</v>
+      </c>
+      <c r="E50" s="471">
+        <v>39184</v>
+      </c>
+      <c r="F50" s="472">
         <v>28.552047503950917</v>
       </c>
-      <c r="G50" t="n" s="478">
-        <v>98283.0</v>
-      </c>
-      <c r="H50" t="n" s="479">
-        <v>8085.0</v>
-      </c>
-      <c r="I50" t="n" s="480">
-        <v>9493.0</v>
-      </c>
-      <c r="J50" t="n" s="481">
-        <v>821922.0</v>
+      <c r="G50" s="473">
+        <v>98283</v>
+      </c>
+      <c r="H50" s="474">
+        <v>8085</v>
+      </c>
+      <c r="I50" s="475">
+        <v>9493</v>
+      </c>
+      <c r="J50" s="476">
+        <v>821922</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="15">
+        <v>44032</v>
+      </c>
+      <c r="B51" s="477">
+        <v>349396</v>
+      </c>
+      <c r="C51" s="478">
+        <v>399443</v>
+      </c>
+      <c r="D51" s="479">
+        <v>79112</v>
+      </c>
+      <c r="E51" s="480">
+        <v>39485</v>
+      </c>
+      <c r="F51" s="481">
+        <v>28.428488019324778</v>
+      </c>
+      <c r="G51" s="482">
+        <v>99328</v>
+      </c>
+      <c r="H51" s="483">
+        <v>8153</v>
+      </c>
+      <c r="I51" s="484">
+        <v>9573</v>
+      </c>
+      <c r="J51" s="485">
+        <v>827951</v>
       </c>
     </row>
   </sheetData>
@@ -3903,19 +3950,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -5653,42 +5700,310 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="47">
+      <c r="A48" s="217">
         <v>44029</v>
       </c>
-      <c r="B48" s="216">
-        <v>0</v>
-      </c>
-      <c r="C48" s="216">
-        <v>1</v>
-      </c>
-      <c r="D48" s="216">
-        <v>0</v>
-      </c>
-      <c r="E48" s="216">
-        <v>0</v>
-      </c>
-      <c r="F48" s="216">
-        <v>1</v>
-      </c>
-      <c r="G48" s="216">
-        <v>0</v>
-      </c>
-      <c r="H48" s="216">
-        <v>0</v>
-      </c>
-      <c r="I48" s="216">
-        <v>0</v>
-      </c>
-      <c r="J48" s="216">
-        <v>1</v>
-      </c>
-      <c r="K48" s="216">
-        <v>0</v>
-      </c>
-      <c r="L48" s="216">
+      <c r="B48" s="74">
+        <v>0</v>
+      </c>
+      <c r="C48" s="74">
+        <v>1</v>
+      </c>
+      <c r="D48" s="74">
+        <v>0</v>
+      </c>
+      <c r="E48" s="74">
+        <v>0</v>
+      </c>
+      <c r="F48" s="74">
+        <v>1</v>
+      </c>
+      <c r="G48" s="74">
+        <v>0</v>
+      </c>
+      <c r="H48" s="74">
+        <v>0</v>
+      </c>
+      <c r="I48" s="74">
+        <v>0</v>
+      </c>
+      <c r="J48" s="74">
+        <v>1</v>
+      </c>
+      <c r="K48" s="74">
+        <v>0</v>
+      </c>
+      <c r="L48" s="74">
         <v>4</v>
       </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="217">
+        <v>44030</v>
+      </c>
+      <c r="B49" s="74">
+        <v>0</v>
+      </c>
+      <c r="C49" s="74">
+        <v>1</v>
+      </c>
+      <c r="D49" s="74">
+        <v>0</v>
+      </c>
+      <c r="E49" s="74">
+        <v>0</v>
+      </c>
+      <c r="F49" s="74">
+        <v>1</v>
+      </c>
+      <c r="G49" s="74">
+        <v>0</v>
+      </c>
+      <c r="H49" s="74">
+        <v>0</v>
+      </c>
+      <c r="I49" s="74">
+        <v>0</v>
+      </c>
+      <c r="J49" s="74">
+        <v>1</v>
+      </c>
+      <c r="K49" s="74">
+        <v>0</v>
+      </c>
+      <c r="L49" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="217">
+        <v>44031</v>
+      </c>
+      <c r="B50" s="74">
+        <v>0</v>
+      </c>
+      <c r="C50" s="74">
+        <v>1</v>
+      </c>
+      <c r="D50" s="74">
+        <v>0</v>
+      </c>
+      <c r="E50" s="74">
+        <v>0</v>
+      </c>
+      <c r="F50" s="74">
+        <v>1</v>
+      </c>
+      <c r="G50" s="74">
+        <v>0</v>
+      </c>
+      <c r="H50" s="74">
+        <v>0</v>
+      </c>
+      <c r="I50" s="74">
+        <v>0</v>
+      </c>
+      <c r="J50" s="74">
+        <v>1</v>
+      </c>
+      <c r="K50" s="74">
+        <v>0</v>
+      </c>
+      <c r="L50" s="74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="217">
+        <v>44032</v>
+      </c>
+      <c r="B51" s="48">
+        <v>0</v>
+      </c>
+      <c r="C51" s="48">
+        <v>1</v>
+      </c>
+      <c r="D51" s="48">
+        <v>0</v>
+      </c>
+      <c r="E51" s="48">
+        <v>0</v>
+      </c>
+      <c r="F51" s="48">
+        <v>1</v>
+      </c>
+      <c r="G51" s="48">
+        <v>0</v>
+      </c>
+      <c r="H51" s="48">
+        <v>0</v>
+      </c>
+      <c r="I51" s="48">
+        <v>0</v>
+      </c>
+      <c r="J51" s="74">
+        <v>1</v>
+      </c>
+      <c r="K51" s="48">
+        <v>0</v>
+      </c>
+      <c r="L51" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="217"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="48"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="48"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="48"/>
+      <c r="L56" s="48"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="48"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="48"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="48"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="48"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5697,11 +6012,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7721,7 +8036,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="47">
+      <c r="A48" s="217">
         <v>44029</v>
       </c>
       <c r="B48" s="216">
@@ -7763,6 +8078,182 @@
       <c r="N48" s="216">
         <v>0</v>
       </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="217">
+        <v>44030</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="217">
+        <v>44031</v>
+      </c>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="217">
+        <v>44032</v>
+      </c>
+      <c r="B51" s="48">
+        <v>0</v>
+      </c>
+      <c r="C51" s="48">
+        <v>1</v>
+      </c>
+      <c r="D51" s="48">
+        <v>0</v>
+      </c>
+      <c r="E51" s="48">
+        <v>0</v>
+      </c>
+      <c r="F51" s="48">
+        <v>1</v>
+      </c>
+      <c r="G51" s="48">
+        <v>0</v>
+      </c>
+      <c r="H51" s="48">
+        <v>1</v>
+      </c>
+      <c r="I51" s="48">
+        <v>0</v>
+      </c>
+      <c r="J51" s="48">
+        <v>0</v>
+      </c>
+      <c r="K51" s="48">
+        <v>1</v>
+      </c>
+      <c r="L51" s="48">
+        <v>1</v>
+      </c>
+      <c r="M51" s="48">
+        <v>0</v>
+      </c>
+      <c r="N51" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
+      <c r="N55" s="48"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
+      <c r="K56" s="48"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="48"/>
+      <c r="N56" s="48"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
+      <c r="N57" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7771,21 +8262,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -9293,39 +9784,288 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="47">
+      <c r="A48" s="217">
         <v>44029</v>
       </c>
-      <c r="B48" s="216">
-        <v>0</v>
-      </c>
-      <c r="C48" s="216">
-        <v>0</v>
-      </c>
-      <c r="D48" s="216">
-        <v>0</v>
-      </c>
-      <c r="E48" s="216">
-        <v>0</v>
-      </c>
-      <c r="F48" s="216">
+      <c r="B48" s="74">
+        <v>0</v>
+      </c>
+      <c r="C48" s="74">
+        <v>0</v>
+      </c>
+      <c r="D48" s="74">
+        <v>0</v>
+      </c>
+      <c r="E48" s="74">
+        <v>0</v>
+      </c>
+      <c r="F48" s="74">
         <v>2</v>
       </c>
-      <c r="G48" s="216">
-        <v>1</v>
-      </c>
-      <c r="H48" s="216">
-        <v>1</v>
-      </c>
-      <c r="I48" s="216">
-        <v>1</v>
-      </c>
-      <c r="J48" s="216">
+      <c r="G48" s="74">
+        <v>1</v>
+      </c>
+      <c r="H48" s="74">
+        <v>1</v>
+      </c>
+      <c r="I48" s="74">
+        <v>1</v>
+      </c>
+      <c r="J48" s="74">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="47"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="217">
+        <v>44030</v>
+      </c>
+      <c r="B49" s="74">
+        <v>0</v>
+      </c>
+      <c r="C49" s="74">
+        <v>0</v>
+      </c>
+      <c r="D49" s="74">
+        <v>0</v>
+      </c>
+      <c r="E49" s="74">
+        <v>0</v>
+      </c>
+      <c r="F49" s="74">
+        <v>2</v>
+      </c>
+      <c r="G49" s="74">
+        <v>1</v>
+      </c>
+      <c r="H49" s="74">
+        <v>1</v>
+      </c>
+      <c r="I49" s="74">
+        <v>1</v>
+      </c>
+      <c r="J49" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="217">
+        <v>44031</v>
+      </c>
+      <c r="B50" s="74">
+        <v>0</v>
+      </c>
+      <c r="C50" s="74">
+        <v>0</v>
+      </c>
+      <c r="D50" s="74">
+        <v>0</v>
+      </c>
+      <c r="E50" s="74">
+        <v>0</v>
+      </c>
+      <c r="F50" s="74">
+        <v>2</v>
+      </c>
+      <c r="G50" s="74">
+        <v>1</v>
+      </c>
+      <c r="H50" s="74">
+        <v>1</v>
+      </c>
+      <c r="I50" s="74">
+        <v>1</v>
+      </c>
+      <c r="J50" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="217">
+        <v>44032</v>
+      </c>
+      <c r="B51" s="48">
+        <v>0</v>
+      </c>
+      <c r="C51" s="48">
+        <v>0</v>
+      </c>
+      <c r="D51" s="74">
+        <v>0</v>
+      </c>
+      <c r="E51" s="48">
+        <v>0</v>
+      </c>
+      <c r="F51" s="48">
+        <v>2</v>
+      </c>
+      <c r="G51" s="48">
+        <v>1</v>
+      </c>
+      <c r="H51" s="48">
+        <v>1</v>
+      </c>
+      <c r="I51" s="48">
+        <v>1</v>
+      </c>
+      <c r="J51" s="48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="48"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="48"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="48"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="48"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="48"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="48"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="48"/>
+      <c r="J63" s="48"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9334,18 +10074,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:AV20"/>
+  <dimension ref="A1:AZ20"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AW12" sqref="AW12"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BA20" sqref="BA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -9490,8 +10230,18 @@
       <c r="AV1" s="49">
         <v>44029</v>
       </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW1" s="49">
+        <v>44030</v>
+      </c>
+      <c r="AX1" s="49">
+        <v>44031</v>
+      </c>
+      <c r="AY1" s="49">
+        <v>44032</v>
+      </c>
+      <c r="AZ1" s="49"/>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -9636,8 +10386,17 @@
       <c r="AV2" s="48">
         <v>4438</v>
       </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW2" s="48">
+        <v>4470</v>
+      </c>
+      <c r="AX2" s="48">
+        <v>4502</v>
+      </c>
+      <c r="AY2" s="48">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -9782,8 +10541,17 @@
       <c r="AV3" s="48">
         <v>4245</v>
       </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW3" s="48">
+        <v>4277</v>
+      </c>
+      <c r="AX3" s="48">
+        <v>4309</v>
+      </c>
+      <c r="AY3" s="48">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -9928,8 +10696,17 @@
       <c r="AV4" s="48">
         <v>4245</v>
       </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW4" s="48">
+        <v>4277</v>
+      </c>
+      <c r="AX4" s="48">
+        <v>4309</v>
+      </c>
+      <c r="AY4" s="48">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -10074,8 +10851,17 @@
       <c r="AV5" s="48">
         <v>4245</v>
       </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW5" s="48">
+        <v>4277</v>
+      </c>
+      <c r="AX5" s="48">
+        <v>4309</v>
+      </c>
+      <c r="AY5" s="48">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -10220,8 +11006,17 @@
       <c r="AV6" s="48">
         <v>4245</v>
       </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW6" s="48">
+        <v>4277</v>
+      </c>
+      <c r="AX6" s="48">
+        <v>4309</v>
+      </c>
+      <c r="AY6" s="48">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -10366,8 +11161,17 @@
       <c r="AV7" s="48">
         <v>3527</v>
       </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW7" s="48">
+        <v>3559</v>
+      </c>
+      <c r="AX7" s="48">
+        <v>3591</v>
+      </c>
+      <c r="AY7" s="48">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -10512,8 +11316,17 @@
       <c r="AV8" s="48">
         <v>6158</v>
       </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW8" s="48">
+        <v>6190</v>
+      </c>
+      <c r="AX8" s="48">
+        <v>6222</v>
+      </c>
+      <c r="AY8" s="48">
+        <v>6254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -10562,8 +11375,11 @@
       <c r="AT9" s="312"/>
       <c r="AU9" s="312"/>
       <c r="AV9" s="312"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW9" s="312"/>
+      <c r="AX9" s="312"/>
+      <c r="AY9" s="312"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -10708,8 +11524,17 @@
       <c r="AV10" s="48">
         <v>187</v>
       </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW10" s="48">
+        <v>188</v>
+      </c>
+      <c r="AX10" s="48">
+        <v>189</v>
+      </c>
+      <c r="AY10" s="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -10854,8 +11679,17 @@
       <c r="AV11" s="48">
         <v>187</v>
       </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW11" s="48">
+        <v>188</v>
+      </c>
+      <c r="AX11" s="48">
+        <v>189</v>
+      </c>
+      <c r="AY11" s="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -11000,8 +11834,17 @@
       <c r="AV12" s="48">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW12" s="48">
+        <v>188</v>
+      </c>
+      <c r="AX12" s="48">
+        <v>189</v>
+      </c>
+      <c r="AY12" s="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -11146,8 +11989,17 @@
       <c r="AV13" s="48">
         <v>187</v>
       </c>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW13" s="48">
+        <v>188</v>
+      </c>
+      <c r="AX13" s="48">
+        <v>189</v>
+      </c>
+      <c r="AY13" s="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -11292,8 +12144,17 @@
       <c r="AV14" s="48">
         <v>187</v>
       </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW14" s="48">
+        <v>188</v>
+      </c>
+      <c r="AX14" s="48">
+        <v>189</v>
+      </c>
+      <c r="AY14" s="48">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -11438,8 +12299,17 @@
       <c r="AV15" s="48">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW15" s="48">
+        <v>123</v>
+      </c>
+      <c r="AX15" s="48">
+        <v>124</v>
+      </c>
+      <c r="AY15" s="48">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -11584,8 +12454,17 @@
       <c r="AV16" s="48">
         <v>199</v>
       </c>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW16" s="48">
+        <v>200</v>
+      </c>
+      <c r="AX16" s="48">
+        <v>201</v>
+      </c>
+      <c r="AY16" s="48">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -11634,8 +12513,11 @@
       <c r="AT17" s="312"/>
       <c r="AU17" s="312"/>
       <c r="AV17" s="312"/>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW17" s="312"/>
+      <c r="AX17" s="312"/>
+      <c r="AY17" s="312"/>
+    </row>
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -11780,15 +12662,24 @@
       <c r="AV18" s="48">
         <v>1038</v>
       </c>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AW18" s="48">
+        <v>1045</v>
+      </c>
+      <c r="AX18" s="48">
+        <v>1052</v>
+      </c>
+      <c r="AY18" s="48">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -11957,28 +12848,40 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f>SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:AY20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
-        <f>SUM(AR2:AR18)</f>
+        <f t="shared" si="1"/>
         <v>32599</v>
       </c>
       <c r="AS20" s="51">
-        <f>SUM(AS2:AS18)</f>
+        <f t="shared" si="1"/>
         <v>32837</v>
       </c>
       <c r="AT20" s="51">
-        <f>SUM(AT2:AT18)</f>
+        <f t="shared" si="1"/>
         <v>32921</v>
       </c>
       <c r="AU20" s="51">
-        <f>SUM(AU2:AU18)</f>
+        <f t="shared" si="1"/>
         <v>33159</v>
       </c>
       <c r="AV20" s="51">
-        <f>SUM(AV2:AV18)</f>
+        <f t="shared" si="1"/>
         <v>33397</v>
+      </c>
+      <c r="AW20" s="51">
+        <f t="shared" si="1"/>
+        <v>33635</v>
+      </c>
+      <c r="AX20" s="51">
+        <f t="shared" si="1"/>
+        <v>33873</v>
+      </c>
+      <c r="AY20" s="51">
+        <f t="shared" si="1"/>
+        <v>34111</v>
       </c>
     </row>
   </sheetData>
@@ -12195,15 +13098,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -12278,43 +13181,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="459" t="s">
+      <c r="B8" s="486" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="459"/>
+      <c r="B9" s="486"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="459"/>
+      <c r="B10" s="486"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="459"/>
+      <c r="B11" s="486"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="460" t="s">
+      <c r="B12" s="487" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="460"/>
+      <c r="B13" s="487"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="460"/>
+      <c r="B14" s="487"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="461" t="s">
+      <c r="B15" s="488" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="461"/>
+      <c r="B16" s="488"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 21th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E10A74-C96C-1349-8C1D-09D5643A1EF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E103F7-FE30-BF43-B055-726E75314497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-30080" yWindow="5220" windowWidth="28800" windowHeight="16540" activeTab="2" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -271,6 +271,9 @@
   <si>
     <t>Se agrego una nueva fecha a la serie de dates_dx, dates_sx el con fecha del 5 de febrero</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +282,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,8 +348,15 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,6 +456,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -563,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="489">
+  <cellXfs count="499">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1972,6 +1988,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1980,6 +2023,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2300,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3941,6 +3987,38 @@
       </c>
       <c r="J51" s="485">
         <v>827951</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="15">
+        <v>44033</v>
+      </c>
+      <c r="B52" s="486">
+        <v>356255</v>
+      </c>
+      <c r="C52" s="487">
+        <v>406151</v>
+      </c>
+      <c r="D52" s="488">
+        <v>82866</v>
+      </c>
+      <c r="E52" s="489">
+        <v>40400</v>
+      </c>
+      <c r="F52" s="490">
+        <v>28.333637422632663</v>
+      </c>
+      <c r="G52" s="491">
+        <v>100940</v>
+      </c>
+      <c r="H52" s="492">
+        <v>8282</v>
+      </c>
+      <c r="I52" s="493">
+        <v>9731</v>
+      </c>
+      <c r="J52" s="494">
+        <v>845272</v>
       </c>
     </row>
   </sheetData>
@@ -3954,7 +4032,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49:A52"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5852,18 +5930,42 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="217"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
+      <c r="A52" s="217">
+        <v>44033</v>
+      </c>
+      <c r="B52" s="48">
+        <v>0</v>
+      </c>
+      <c r="C52" s="48">
+        <v>1</v>
+      </c>
+      <c r="D52" s="48">
+        <v>0</v>
+      </c>
+      <c r="E52" s="48">
+        <v>0</v>
+      </c>
+      <c r="F52" s="48">
+        <v>1</v>
+      </c>
+      <c r="G52" s="48">
+        <v>0</v>
+      </c>
+      <c r="H52" s="48">
+        <v>0</v>
+      </c>
+      <c r="I52" s="48">
+        <v>0</v>
+      </c>
+      <c r="J52" s="48">
+        <v>1</v>
+      </c>
+      <c r="K52" s="48">
+        <v>0</v>
+      </c>
+      <c r="L52" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="48"/>
@@ -6012,11 +6114,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49:A51"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8039,90 +8141,142 @@
       <c r="A48" s="217">
         <v>44029</v>
       </c>
-      <c r="B48" s="216">
-        <v>0</v>
-      </c>
-      <c r="C48" s="216">
-        <v>1</v>
-      </c>
-      <c r="D48" s="216">
-        <v>0</v>
-      </c>
-      <c r="E48" s="216">
-        <v>0</v>
-      </c>
-      <c r="F48" s="216">
-        <v>1</v>
-      </c>
-      <c r="G48" s="216">
-        <v>0</v>
-      </c>
-      <c r="H48" s="216">
-        <v>1</v>
-      </c>
-      <c r="I48" s="216">
-        <v>0</v>
-      </c>
-      <c r="J48" s="216">
-        <v>0</v>
-      </c>
-      <c r="K48" s="216">
-        <v>1</v>
-      </c>
-      <c r="L48" s="216">
-        <v>1</v>
-      </c>
-      <c r="M48" s="216">
-        <v>0</v>
-      </c>
-      <c r="N48" s="216">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="74">
+        <v>0</v>
+      </c>
+      <c r="C48" s="74">
+        <v>1</v>
+      </c>
+      <c r="D48" s="74">
+        <v>0</v>
+      </c>
+      <c r="E48" s="74">
+        <v>0</v>
+      </c>
+      <c r="F48" s="74">
+        <v>1</v>
+      </c>
+      <c r="G48" s="74">
+        <v>0</v>
+      </c>
+      <c r="H48" s="74">
+        <v>1</v>
+      </c>
+      <c r="I48" s="74">
+        <v>0</v>
+      </c>
+      <c r="J48" s="74">
+        <v>0</v>
+      </c>
+      <c r="K48" s="74">
+        <v>1</v>
+      </c>
+      <c r="L48" s="74">
+        <v>1</v>
+      </c>
+      <c r="M48" s="74">
+        <v>0</v>
+      </c>
+      <c r="N48" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="217">
         <v>44030</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B49" s="74">
+        <v>0</v>
+      </c>
+      <c r="C49" s="74">
+        <v>1</v>
+      </c>
+      <c r="D49" s="74">
+        <v>0</v>
+      </c>
+      <c r="E49" s="74">
+        <v>0</v>
+      </c>
+      <c r="F49" s="74">
+        <v>1</v>
+      </c>
+      <c r="G49" s="74">
+        <v>0</v>
+      </c>
+      <c r="H49" s="48">
+        <v>1</v>
+      </c>
+      <c r="I49" s="74">
+        <v>0</v>
+      </c>
+      <c r="J49" s="74">
+        <v>0</v>
+      </c>
+      <c r="K49" s="74">
+        <v>1</v>
+      </c>
+      <c r="L49" s="74">
+        <v>1</v>
+      </c>
+      <c r="M49" s="74">
+        <v>0</v>
+      </c>
+      <c r="N49" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="217">
         <v>44031</v>
       </c>
-      <c r="B50" s="48"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B50" s="74">
+        <v>0</v>
+      </c>
+      <c r="C50" s="74">
+        <v>1</v>
+      </c>
+      <c r="D50" s="74">
+        <v>0</v>
+      </c>
+      <c r="E50" s="74">
+        <v>0</v>
+      </c>
+      <c r="F50" s="74">
+        <v>1</v>
+      </c>
+      <c r="G50" s="48">
+        <v>0</v>
+      </c>
+      <c r="H50" s="48">
+        <v>1</v>
+      </c>
+      <c r="I50" s="74">
+        <v>0</v>
+      </c>
+      <c r="J50" s="74">
+        <v>0</v>
+      </c>
+      <c r="K50" s="74">
+        <v>1</v>
+      </c>
+      <c r="L50" s="74">
+        <v>1</v>
+      </c>
+      <c r="M50" s="74">
+        <v>0</v>
+      </c>
+      <c r="N50" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="217">
         <v>44032</v>
       </c>
-      <c r="B51" s="48">
-        <v>0</v>
-      </c>
-      <c r="C51" s="48">
+      <c r="B51" s="74">
+        <v>0</v>
+      </c>
+      <c r="C51" s="74">
         <v>1</v>
       </c>
       <c r="D51" s="48">
@@ -8159,23 +8313,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="48"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="217">
+        <v>44033</v>
+      </c>
+      <c r="B52" s="48">
+        <v>0</v>
+      </c>
+      <c r="C52" s="48">
+        <v>1</v>
+      </c>
+      <c r="D52" s="48">
+        <v>0</v>
+      </c>
+      <c r="E52" s="48">
+        <v>0</v>
+      </c>
+      <c r="F52" s="48">
+        <v>1</v>
+      </c>
+      <c r="G52" s="48">
+        <v>0</v>
+      </c>
+      <c r="H52" s="48">
+        <v>1</v>
+      </c>
+      <c r="I52" s="48">
+        <v>0</v>
+      </c>
+      <c r="J52" s="48">
+        <v>0</v>
+      </c>
+      <c r="K52" s="48">
+        <v>1</v>
+      </c>
+      <c r="L52" s="48">
+        <v>1</v>
+      </c>
+      <c r="M52" s="48">
+        <v>0</v>
+      </c>
+      <c r="N52" s="48">
+        <v>0</v>
+      </c>
+      <c r="O52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="48"/>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
@@ -8191,7 +8376,7 @@
       <c r="M53" s="48"/>
       <c r="N53" s="48"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="48"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
@@ -8207,7 +8392,7 @@
       <c r="M54" s="48"/>
       <c r="N54" s="48"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="48"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
@@ -8223,7 +8408,7 @@
       <c r="M55" s="48"/>
       <c r="N55" s="48"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="48"/>
       <c r="B56" s="48"/>
       <c r="C56" s="48"/>
@@ -8239,7 +8424,7 @@
       <c r="M56" s="48"/>
       <c r="N56" s="48"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="48"/>
       <c r="B57" s="48"/>
       <c r="C57" s="48"/>
@@ -8266,7 +8451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9912,16 +10097,36 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="48"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-      <c r="J52" s="48"/>
+      <c r="A52" s="498">
+        <v>44033</v>
+      </c>
+      <c r="B52" s="48">
+        <v>0</v>
+      </c>
+      <c r="C52" s="48">
+        <v>0</v>
+      </c>
+      <c r="D52" s="48">
+        <v>0</v>
+      </c>
+      <c r="E52" s="48">
+        <v>0</v>
+      </c>
+      <c r="F52" s="48">
+        <v>2</v>
+      </c>
+      <c r="G52" s="48">
+        <v>1</v>
+      </c>
+      <c r="H52" s="48">
+        <v>1</v>
+      </c>
+      <c r="I52" s="48">
+        <v>1</v>
+      </c>
+      <c r="J52" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="48"/>
@@ -10077,7 +10282,7 @@
   <dimension ref="A1:AZ20"/>
   <sheetViews>
     <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BA20" sqref="BA20"/>
+      <selection activeCell="BC17" sqref="BC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10239,7 +10444,9 @@
       <c r="AY1" s="49">
         <v>44032</v>
       </c>
-      <c r="AZ1" s="49"/>
+      <c r="AZ1" s="49">
+        <v>44033</v>
+      </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -10395,6 +10602,9 @@
       <c r="AY2" s="48">
         <v>4534</v>
       </c>
+      <c r="AZ2">
+        <v>4566</v>
+      </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -10550,6 +10760,9 @@
       <c r="AY3" s="48">
         <v>4341</v>
       </c>
+      <c r="AZ3">
+        <v>4373</v>
+      </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -10705,6 +10918,9 @@
       <c r="AY4" s="48">
         <v>4341</v>
       </c>
+      <c r="AZ4">
+        <v>4373</v>
+      </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -10860,6 +11076,9 @@
       <c r="AY5" s="48">
         <v>4341</v>
       </c>
+      <c r="AZ5">
+        <v>4373</v>
+      </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -11015,6 +11234,9 @@
       <c r="AY6" s="48">
         <v>4341</v>
       </c>
+      <c r="AZ6">
+        <v>4373</v>
+      </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -11170,6 +11392,9 @@
       <c r="AY7" s="48">
         <v>3623</v>
       </c>
+      <c r="AZ7" s="216">
+        <v>3655</v>
+      </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -11324,6 +11549,9 @@
       </c>
       <c r="AY8" s="48">
         <v>6254</v>
+      </c>
+      <c r="AZ8" s="230">
+        <v>6258</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.2">
@@ -11378,6 +11606,7 @@
       <c r="AW9" s="312"/>
       <c r="AX9" s="312"/>
       <c r="AY9" s="312"/>
+      <c r="AZ9" s="312"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
@@ -11533,6 +11762,9 @@
       <c r="AY10" s="48">
         <v>190</v>
       </c>
+      <c r="AZ10" s="216">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -11688,6 +11920,9 @@
       <c r="AY11" s="48">
         <v>190</v>
       </c>
+      <c r="AZ11" s="216">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -11843,6 +12078,9 @@
       <c r="AY12" s="48">
         <v>190</v>
       </c>
+      <c r="AZ12" s="216">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -11998,6 +12236,9 @@
       <c r="AY13" s="48">
         <v>190</v>
       </c>
+      <c r="AZ13" s="216">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -12153,6 +12394,9 @@
       <c r="AY14" s="48">
         <v>190</v>
       </c>
+      <c r="AZ14" s="216">
+        <v>191</v>
+      </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -12308,6 +12552,9 @@
       <c r="AY15" s="48">
         <v>125</v>
       </c>
+      <c r="AZ15" s="216">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -12463,8 +12710,11 @@
       <c r="AY16" s="48">
         <v>202</v>
       </c>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ16" s="216">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -12516,8 +12766,9 @@
       <c r="AW17" s="312"/>
       <c r="AX17" s="312"/>
       <c r="AY17" s="312"/>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ17" s="312"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -12671,15 +12922,18 @@
       <c r="AY18" s="48">
         <v>1059</v>
       </c>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ18" s="216">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -12848,7 +13102,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:AY20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:AZ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -12882,6 +13136,10 @@
       <c r="AY20" s="51">
         <f t="shared" si="1"/>
         <v>34111</v>
+      </c>
+      <c r="AZ20" s="51">
+        <f t="shared" si="1"/>
+        <v>34321</v>
       </c>
     </row>
   </sheetData>
@@ -13098,7 +13356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -13181,43 +13439,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="486" t="s">
+      <c r="B8" s="495" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="486"/>
+      <c r="B9" s="495"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="486"/>
+      <c r="B10" s="495"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="486"/>
+      <c r="B11" s="495"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="487" t="s">
+      <c r="B12" s="496" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="487"/>
+      <c r="B13" s="496"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="487"/>
+      <c r="B14" s="496"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="488" t="s">
+      <c r="B15" s="497" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="488"/>
+      <c r="B16" s="497"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 22th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E103F7-FE30-BF43-B055-726E75314497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1793C-7DFB-3A46-98D9-7C22CC411964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30080" yWindow="5220" windowWidth="28800" windowHeight="16540" activeTab="2" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="6060" yWindow="460" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="499">
+  <cellXfs count="508">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2015,6 +2015,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2023,9 +2053,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2346,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4019,6 +4046,38 @@
       </c>
       <c r="J52" s="494">
         <v>845272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="15">
+        <v>44034</v>
+      </c>
+      <c r="B53" s="496">
+        <v>362274</v>
+      </c>
+      <c r="C53" s="497">
+        <v>411673</v>
+      </c>
+      <c r="D53" s="498">
+        <v>87905</v>
+      </c>
+      <c r="E53" s="499">
+        <v>41190</v>
+      </c>
+      <c r="F53" s="500">
+        <v>28.236086498064999</v>
+      </c>
+      <c r="G53" s="501">
+        <v>102292</v>
+      </c>
+      <c r="H53" s="502">
+        <v>8406</v>
+      </c>
+      <c r="I53" s="503">
+        <v>9903</v>
+      </c>
+      <c r="J53" s="504">
+        <v>861852</v>
       </c>
     </row>
   </sheetData>
@@ -4032,7 +4091,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5968,18 +6027,42 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="48"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
-      <c r="J53" s="48"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
+      <c r="A53" s="217">
+        <v>44034</v>
+      </c>
+      <c r="B53" s="48">
+        <v>0</v>
+      </c>
+      <c r="C53" s="48">
+        <v>1</v>
+      </c>
+      <c r="D53" s="48">
+        <v>0</v>
+      </c>
+      <c r="E53" s="48">
+        <v>0</v>
+      </c>
+      <c r="F53" s="48">
+        <v>1</v>
+      </c>
+      <c r="G53" s="48">
+        <v>0</v>
+      </c>
+      <c r="H53" s="48">
+        <v>0</v>
+      </c>
+      <c r="I53" s="48">
+        <v>0</v>
+      </c>
+      <c r="J53" s="48">
+        <v>0</v>
+      </c>
+      <c r="K53" s="48">
+        <v>0</v>
+      </c>
+      <c r="L53" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="48"/>
@@ -6116,9 +6199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8361,20 +8444,48 @@
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="48"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
-      <c r="J53" s="48"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="48"/>
-      <c r="N53" s="48"/>
+      <c r="A53" s="217">
+        <v>44034</v>
+      </c>
+      <c r="B53" s="48">
+        <v>0</v>
+      </c>
+      <c r="C53" s="48">
+        <v>1</v>
+      </c>
+      <c r="D53" s="48">
+        <v>0</v>
+      </c>
+      <c r="E53" s="48">
+        <v>0</v>
+      </c>
+      <c r="F53" s="48">
+        <v>0</v>
+      </c>
+      <c r="G53" s="48">
+        <v>0</v>
+      </c>
+      <c r="H53" s="48">
+        <v>1</v>
+      </c>
+      <c r="I53" s="48">
+        <v>0</v>
+      </c>
+      <c r="J53" s="48">
+        <v>0</v>
+      </c>
+      <c r="K53" s="48">
+        <v>1</v>
+      </c>
+      <c r="L53" s="48">
+        <v>0</v>
+      </c>
+      <c r="M53" s="48">
+        <v>0</v>
+      </c>
+      <c r="N53" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="48"/>
@@ -8451,7 +8562,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10097,7 +10208,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="498">
+      <c r="A52" s="495">
         <v>44033</v>
       </c>
       <c r="B52" s="48">
@@ -10129,16 +10240,36 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="48"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
-      <c r="J53" s="48"/>
+      <c r="A53" s="15">
+        <v>44034</v>
+      </c>
+      <c r="B53" s="48">
+        <v>0</v>
+      </c>
+      <c r="C53" s="48">
+        <v>0</v>
+      </c>
+      <c r="D53" s="48">
+        <v>0</v>
+      </c>
+      <c r="E53" s="48">
+        <v>0</v>
+      </c>
+      <c r="F53" s="48">
+        <v>2</v>
+      </c>
+      <c r="G53" s="48">
+        <v>1</v>
+      </c>
+      <c r="H53" s="48">
+        <v>1</v>
+      </c>
+      <c r="I53" s="48">
+        <v>1</v>
+      </c>
+      <c r="J53" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="48"/>
@@ -10279,10 +10410,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:AZ20"/>
+  <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BC17" sqref="BC17"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BD17" sqref="BD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10290,7 +10421,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -10447,8 +10578,11 @@
       <c r="AZ1" s="49">
         <v>44033</v>
       </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA1" s="49">
+        <v>44034</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -10605,8 +10739,11 @@
       <c r="AZ2">
         <v>4566</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA2">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -10763,8 +10900,11 @@
       <c r="AZ3">
         <v>4373</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA3">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -10921,8 +11061,11 @@
       <c r="AZ4">
         <v>4373</v>
       </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA4">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -11079,8 +11222,11 @@
       <c r="AZ5">
         <v>4373</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA5">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -11237,8 +11383,11 @@
       <c r="AZ6">
         <v>4373</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA6">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -11395,8 +11544,11 @@
       <c r="AZ7" s="216">
         <v>3655</v>
       </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA7">
+        <v>3687</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -11553,8 +11705,11 @@
       <c r="AZ8" s="230">
         <v>6258</v>
       </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA8">
+        <v>6318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -11608,7 +11763,7 @@
       <c r="AY9" s="312"/>
       <c r="AZ9" s="312"/>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -11765,8 +11920,11 @@
       <c r="AZ10" s="216">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA10" s="216">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -11923,8 +12081,11 @@
       <c r="AZ11" s="216">
         <v>191</v>
       </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA11" s="216">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -12081,8 +12242,11 @@
       <c r="AZ12" s="216">
         <v>191</v>
       </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA12" s="216">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -12239,8 +12403,11 @@
       <c r="AZ13" s="216">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA13" s="216">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -12397,8 +12564,11 @@
       <c r="AZ14" s="216">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA14" s="216">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -12555,8 +12725,11 @@
       <c r="AZ15" s="216">
         <v>126</v>
       </c>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA15" s="216">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -12713,8 +12886,11 @@
       <c r="AZ16" s="216">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA16" s="216">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -12768,7 +12944,7 @@
       <c r="AY17" s="312"/>
       <c r="AZ17" s="312"/>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -12925,15 +13101,18 @@
       <c r="AZ18" s="216">
         <v>1066</v>
       </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BA18">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -13102,7 +13281,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:AZ20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BA20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -13140,6 +13319,10 @@
       <c r="AZ20" s="51">
         <f t="shared" si="1"/>
         <v>34321</v>
+      </c>
+      <c r="BA20" s="51">
+        <f t="shared" si="1"/>
+        <v>34455</v>
       </c>
     </row>
   </sheetData>
@@ -13439,43 +13622,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="495" t="s">
+      <c r="B8" s="505" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="495"/>
+      <c r="B9" s="505"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="495"/>
+      <c r="B10" s="505"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="495"/>
+      <c r="B11" s="505"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="496" t="s">
+      <c r="B12" s="506" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="496"/>
+      <c r="B13" s="506"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="496"/>
+      <c r="B14" s="506"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="497" t="s">
+      <c r="B15" s="507" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="497"/>
+      <c r="B16" s="507"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 23th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1793C-7DFB-3A46-98D9-7C22CC411964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB9AA5B-396B-9144-8A7D-737734342E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="460" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="2660" yWindow="460" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="508">
+  <cellXfs count="517">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2016,6 +2016,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -2373,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4078,6 +4105,38 @@
       </c>
       <c r="J53" s="504">
         <v>861852</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="15">
+        <v>44035</v>
+      </c>
+      <c r="B54" s="505">
+        <v>370712</v>
+      </c>
+      <c r="C54" s="506">
+        <v>419349</v>
+      </c>
+      <c r="D54" s="507">
+        <v>89547</v>
+      </c>
+      <c r="E54" s="508">
+        <v>41908</v>
+      </c>
+      <c r="F54" s="509">
+        <v>28.116435399987051</v>
+      </c>
+      <c r="G54" s="510">
+        <v>104231</v>
+      </c>
+      <c r="H54" s="511">
+        <v>8536</v>
+      </c>
+      <c r="I54" s="512">
+        <v>10034</v>
+      </c>
+      <c r="J54" s="513">
+        <v>879608</v>
       </c>
     </row>
   </sheetData>
@@ -4091,7 +4150,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6065,18 +6124,42 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="48"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
+      <c r="A54" s="217">
+        <v>44035</v>
+      </c>
+      <c r="B54" s="48">
+        <v>0</v>
+      </c>
+      <c r="C54" s="48">
+        <v>1</v>
+      </c>
+      <c r="D54" s="48">
+        <v>0</v>
+      </c>
+      <c r="E54" s="48">
+        <v>0</v>
+      </c>
+      <c r="F54" s="48">
+        <v>1</v>
+      </c>
+      <c r="G54" s="48">
+        <v>0</v>
+      </c>
+      <c r="H54" s="48">
+        <v>0</v>
+      </c>
+      <c r="I54" s="48">
+        <v>0</v>
+      </c>
+      <c r="J54" s="48">
+        <v>0</v>
+      </c>
+      <c r="K54" s="48">
+        <v>0</v>
+      </c>
+      <c r="L54" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="48"/>
@@ -6201,7 +6284,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8488,20 +8571,48 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="48"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="48"/>
-      <c r="N54" s="48"/>
+      <c r="A54" s="217">
+        <v>44035</v>
+      </c>
+      <c r="B54" s="48">
+        <v>0</v>
+      </c>
+      <c r="C54" s="48">
+        <v>1</v>
+      </c>
+      <c r="D54" s="48">
+        <v>0</v>
+      </c>
+      <c r="E54" s="48">
+        <v>0</v>
+      </c>
+      <c r="F54" s="48">
+        <v>0</v>
+      </c>
+      <c r="G54" s="48">
+        <v>0</v>
+      </c>
+      <c r="H54" s="48">
+        <v>1</v>
+      </c>
+      <c r="I54" s="48">
+        <v>0</v>
+      </c>
+      <c r="J54" s="48">
+        <v>0</v>
+      </c>
+      <c r="K54" s="48">
+        <v>1</v>
+      </c>
+      <c r="L54" s="48">
+        <v>0</v>
+      </c>
+      <c r="M54" s="48">
+        <v>0</v>
+      </c>
+      <c r="N54" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="48"/>
@@ -8562,7 +8673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10240,7 +10351,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="15">
+      <c r="A53" s="495">
         <v>44034</v>
       </c>
       <c r="B53" s="48">
@@ -10272,19 +10383,39 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="48"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
-      <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="48"/>
+      <c r="A54" s="495">
+        <v>44035</v>
+      </c>
+      <c r="B54" s="48">
+        <v>0</v>
+      </c>
+      <c r="C54" s="48">
+        <v>0</v>
+      </c>
+      <c r="D54" s="48">
+        <v>0</v>
+      </c>
+      <c r="E54" s="48">
+        <v>0</v>
+      </c>
+      <c r="F54" s="48">
+        <v>2</v>
+      </c>
+      <c r="G54" s="48">
+        <v>1</v>
+      </c>
+      <c r="H54" s="48">
+        <v>1</v>
+      </c>
+      <c r="I54" s="48">
+        <v>1</v>
+      </c>
+      <c r="J54" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
+      <c r="A55" s="495"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
       <c r="D55" s="48"/>
@@ -10410,10 +10541,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:BA20"/>
+  <dimension ref="A1:BE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BD17" sqref="BD17"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BE11" sqref="BE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10421,7 +10552,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -10581,8 +10712,14 @@
       <c r="BA1" s="49">
         <v>44034</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB1" s="49">
+        <v>44035</v>
+      </c>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -10736,14 +10873,20 @@
       <c r="AY2" s="48">
         <v>4534</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="48">
         <v>4566</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="48">
         <v>4578</v>
       </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB2" s="48">
+        <v>4610</v>
+      </c>
+      <c r="BC2" s="48"/>
+      <c r="BD2" s="48"/>
+      <c r="BE2" s="48"/>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -10897,14 +11040,20 @@
       <c r="AY3" s="48">
         <v>4341</v>
       </c>
-      <c r="AZ3">
+      <c r="AZ3" s="48">
         <v>4373</v>
       </c>
-      <c r="BA3">
+      <c r="BA3" s="48">
         <v>4377</v>
       </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB3" s="48">
+        <v>4409</v>
+      </c>
+      <c r="BC3" s="48"/>
+      <c r="BD3" s="48"/>
+      <c r="BE3" s="48"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -11058,14 +11207,20 @@
       <c r="AY4" s="48">
         <v>4341</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="48">
         <v>4373</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="48">
         <v>4377</v>
       </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB4" s="48">
+        <v>4409</v>
+      </c>
+      <c r="BC4" s="48"/>
+      <c r="BD4" s="48"/>
+      <c r="BE4" s="48"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -11219,14 +11374,20 @@
       <c r="AY5" s="48">
         <v>4341</v>
       </c>
-      <c r="AZ5">
+      <c r="AZ5" s="48">
         <v>4373</v>
       </c>
-      <c r="BA5">
+      <c r="BA5" s="48">
         <v>4377</v>
       </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB5" s="48">
+        <v>4409</v>
+      </c>
+      <c r="BC5" s="48"/>
+      <c r="BD5" s="48"/>
+      <c r="BE5" s="48"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -11380,14 +11541,20 @@
       <c r="AY6" s="48">
         <v>4341</v>
       </c>
-      <c r="AZ6">
+      <c r="AZ6" s="48">
         <v>4373</v>
       </c>
-      <c r="BA6">
+      <c r="BA6" s="48">
         <v>4377</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB6" s="48">
+        <v>4409</v>
+      </c>
+      <c r="BC6" s="48"/>
+      <c r="BD6" s="48"/>
+      <c r="BE6" s="48"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -11541,14 +11708,20 @@
       <c r="AY7" s="48">
         <v>3623</v>
       </c>
-      <c r="AZ7" s="216">
+      <c r="AZ7" s="74">
         <v>3655</v>
       </c>
-      <c r="BA7">
+      <c r="BA7" s="48">
         <v>3687</v>
       </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB7" s="48">
+        <v>3719</v>
+      </c>
+      <c r="BC7" s="48"/>
+      <c r="BD7" s="48"/>
+      <c r="BE7" s="48"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -11702,14 +11875,20 @@
       <c r="AY8" s="48">
         <v>6254</v>
       </c>
-      <c r="AZ8" s="230">
+      <c r="AZ8" s="74">
         <v>6258</v>
       </c>
-      <c r="BA8">
+      <c r="BA8" s="48">
         <v>6318</v>
       </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB8" s="48">
+        <v>6350</v>
+      </c>
+      <c r="BC8" s="48"/>
+      <c r="BD8" s="48"/>
+      <c r="BE8" s="48"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -11762,8 +11941,13 @@
       <c r="AX9" s="312"/>
       <c r="AY9" s="312"/>
       <c r="AZ9" s="312"/>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BA9" s="312"/>
+      <c r="BB9" s="312"/>
+      <c r="BC9" s="48"/>
+      <c r="BD9" s="48"/>
+      <c r="BE9" s="48"/>
+    </row>
+    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -11917,14 +12101,20 @@
       <c r="AY10" s="48">
         <v>190</v>
       </c>
-      <c r="AZ10" s="216">
+      <c r="AZ10" s="74">
         <v>191</v>
       </c>
-      <c r="BA10" s="216">
+      <c r="BA10" s="74">
         <v>192</v>
       </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB10" s="48">
+        <v>193</v>
+      </c>
+      <c r="BC10" s="48"/>
+      <c r="BD10" s="48"/>
+      <c r="BE10" s="48"/>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -12078,14 +12268,20 @@
       <c r="AY11" s="48">
         <v>190</v>
       </c>
-      <c r="AZ11" s="216">
+      <c r="AZ11" s="74">
         <v>191</v>
       </c>
-      <c r="BA11" s="216">
+      <c r="BA11" s="74">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB11" s="48">
+        <v>193</v>
+      </c>
+      <c r="BC11" s="48"/>
+      <c r="BD11" s="48"/>
+      <c r="BE11" s="48"/>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -12239,14 +12435,20 @@
       <c r="AY12" s="48">
         <v>190</v>
       </c>
-      <c r="AZ12" s="216">
+      <c r="AZ12" s="74">
         <v>191</v>
       </c>
-      <c r="BA12" s="216">
+      <c r="BA12" s="74">
         <v>192</v>
       </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB12" s="48">
+        <v>193</v>
+      </c>
+      <c r="BC12" s="48"/>
+      <c r="BD12" s="48"/>
+      <c r="BE12" s="48"/>
+    </row>
+    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -12400,14 +12602,20 @@
       <c r="AY13" s="48">
         <v>190</v>
       </c>
-      <c r="AZ13" s="216">
+      <c r="AZ13" s="74">
         <v>191</v>
       </c>
-      <c r="BA13" s="216">
+      <c r="BA13" s="74">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB13" s="48">
+        <v>193</v>
+      </c>
+      <c r="BC13" s="48"/>
+      <c r="BD13" s="48"/>
+      <c r="BE13" s="48"/>
+    </row>
+    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -12561,14 +12769,20 @@
       <c r="AY14" s="48">
         <v>190</v>
       </c>
-      <c r="AZ14" s="216">
+      <c r="AZ14" s="74">
         <v>191</v>
       </c>
-      <c r="BA14" s="216">
+      <c r="BA14" s="74">
         <v>192</v>
       </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB14" s="48">
+        <v>193</v>
+      </c>
+      <c r="BC14" s="48"/>
+      <c r="BD14" s="48"/>
+      <c r="BE14" s="48"/>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -12722,14 +12936,20 @@
       <c r="AY15" s="48">
         <v>125</v>
       </c>
-      <c r="AZ15" s="216">
+      <c r="AZ15" s="74">
         <v>126</v>
       </c>
-      <c r="BA15" s="216">
+      <c r="BA15" s="74">
         <v>127</v>
       </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB15" s="48">
+        <v>128</v>
+      </c>
+      <c r="BC15" s="48"/>
+      <c r="BD15" s="48"/>
+      <c r="BE15" s="48"/>
+    </row>
+    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -12883,14 +13103,20 @@
       <c r="AY16" s="48">
         <v>202</v>
       </c>
-      <c r="AZ16" s="216">
+      <c r="AZ16" s="74">
         <v>203</v>
       </c>
-      <c r="BA16" s="216">
+      <c r="BA16" s="74">
         <v>204</v>
       </c>
-    </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB16" s="48">
+        <v>205</v>
+      </c>
+      <c r="BC16" s="48"/>
+      <c r="BD16" s="48"/>
+      <c r="BE16" s="48"/>
+    </row>
+    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -12943,8 +13169,13 @@
       <c r="AX17" s="312"/>
       <c r="AY17" s="312"/>
       <c r="AZ17" s="312"/>
-    </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BA17" s="312"/>
+      <c r="BB17" s="312"/>
+      <c r="BC17" s="48"/>
+      <c r="BD17" s="48"/>
+      <c r="BE17" s="48"/>
+    </row>
+    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -13098,21 +13329,27 @@
       <c r="AY18" s="48">
         <v>1059</v>
       </c>
-      <c r="AZ18" s="216">
+      <c r="AZ18" s="74">
         <v>1066</v>
       </c>
-      <c r="BA18">
+      <c r="BA18" s="48">
         <v>1073</v>
       </c>
-    </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="BB18" s="48">
+        <v>1080</v>
+      </c>
+      <c r="BC18" s="48"/>
+      <c r="BD18" s="48"/>
+      <c r="BE18" s="48"/>
+    </row>
+    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -13281,7 +13518,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BA20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BB20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -13324,6 +13561,13 @@
         <f t="shared" si="1"/>
         <v>34455</v>
       </c>
+      <c r="BB20" s="51">
+        <f t="shared" si="1"/>
+        <v>34693</v>
+      </c>
+      <c r="BC20" s="48"/>
+      <c r="BD20" s="48"/>
+      <c r="BE20" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13622,43 +13866,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="505" t="s">
+      <c r="B8" s="514" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="505"/>
+      <c r="B9" s="514"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="505"/>
+      <c r="B10" s="514"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="505"/>
+      <c r="B11" s="514"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="506" t="s">
+      <c r="B12" s="515" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="506"/>
+      <c r="B13" s="515"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="506"/>
+      <c r="B14" s="515"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="507" t="s">
+      <c r="B15" s="516" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="507"/>
+      <c r="B16" s="516"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 25th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB9AA5B-396B-9144-8A7D-737734342E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833E085D-9B04-0642-9F84-4407D049ACFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="460" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="517">
+  <cellXfs count="535">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2016,6 +2016,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -2400,10 +2454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4137,6 +4191,70 @@
       </c>
       <c r="J54" s="513">
         <v>879608</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="15">
+        <v>44036</v>
+      </c>
+      <c r="B55" s="514">
+        <v>378285</v>
+      </c>
+      <c r="C55" s="515">
+        <v>426869</v>
+      </c>
+      <c r="D55" s="516">
+        <v>90970</v>
+      </c>
+      <c r="E55" s="517">
+        <v>42645</v>
+      </c>
+      <c r="F55" s="518">
+        <v>27.968330755911548</v>
+      </c>
+      <c r="G55" s="519">
+        <v>105800</v>
+      </c>
+      <c r="H55" s="520">
+        <v>8643</v>
+      </c>
+      <c r="I55" s="521">
+        <v>10189</v>
+      </c>
+      <c r="J55" s="522">
+        <v>896124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="15">
+        <v>44037</v>
+      </c>
+      <c r="B56" s="523">
+        <v>385036</v>
+      </c>
+      <c r="C56" s="524">
+        <v>433384</v>
+      </c>
+      <c r="D56" s="525">
+        <v>93433</v>
+      </c>
+      <c r="E56" s="526">
+        <v>43374</v>
+      </c>
+      <c r="F56" s="527">
+        <v>27.887522205715833</v>
+      </c>
+      <c r="G56" s="528">
+        <v>107377</v>
+      </c>
+      <c r="H56" s="529">
+        <v>8739</v>
+      </c>
+      <c r="I56" s="530">
+        <v>10294</v>
+      </c>
+      <c r="J56" s="531">
+        <v>911853</v>
       </c>
     </row>
   </sheetData>
@@ -4150,7 +4268,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6162,32 +6280,80 @@
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48"/>
-      <c r="J55" s="48"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="48"/>
+      <c r="A55" s="217">
+        <v>44036</v>
+      </c>
+      <c r="B55" s="48">
+        <v>0</v>
+      </c>
+      <c r="C55" s="48">
+        <v>1</v>
+      </c>
+      <c r="D55" s="48">
+        <v>0</v>
+      </c>
+      <c r="E55" s="48">
+        <v>0</v>
+      </c>
+      <c r="F55" s="48">
+        <v>1</v>
+      </c>
+      <c r="G55" s="48">
+        <v>0</v>
+      </c>
+      <c r="H55" s="48">
+        <v>0</v>
+      </c>
+      <c r="I55" s="48">
+        <v>0</v>
+      </c>
+      <c r="J55" s="48">
+        <v>0</v>
+      </c>
+      <c r="K55" s="48">
+        <v>0</v>
+      </c>
+      <c r="L55" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="48"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
+      <c r="A56" s="217">
+        <v>44037</v>
+      </c>
+      <c r="B56" s="48">
+        <v>0</v>
+      </c>
+      <c r="C56" s="48">
+        <v>1</v>
+      </c>
+      <c r="D56" s="48">
+        <v>0</v>
+      </c>
+      <c r="E56" s="48">
+        <v>0</v>
+      </c>
+      <c r="F56" s="48">
+        <v>1</v>
+      </c>
+      <c r="G56" s="48">
+        <v>0</v>
+      </c>
+      <c r="H56" s="48">
+        <v>0</v>
+      </c>
+      <c r="I56" s="48">
+        <v>0</v>
+      </c>
+      <c r="J56" s="48">
+        <v>0</v>
+      </c>
+      <c r="K56" s="48">
+        <v>0</v>
+      </c>
+      <c r="L56" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="48"/>
@@ -6284,7 +6450,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8615,36 +8781,92 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48"/>
-      <c r="J55" s="48"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="48"/>
-      <c r="M55" s="48"/>
-      <c r="N55" s="48"/>
+      <c r="A55" s="217">
+        <v>44036</v>
+      </c>
+      <c r="B55" s="48">
+        <v>0</v>
+      </c>
+      <c r="C55" s="48">
+        <v>1</v>
+      </c>
+      <c r="D55" s="48">
+        <v>0</v>
+      </c>
+      <c r="E55" s="48">
+        <v>0</v>
+      </c>
+      <c r="F55" s="48">
+        <v>0</v>
+      </c>
+      <c r="G55" s="48">
+        <v>0</v>
+      </c>
+      <c r="H55" s="48">
+        <v>1</v>
+      </c>
+      <c r="I55" s="48">
+        <v>0</v>
+      </c>
+      <c r="J55" s="48">
+        <v>0</v>
+      </c>
+      <c r="K55" s="48">
+        <v>1</v>
+      </c>
+      <c r="L55" s="48">
+        <v>0</v>
+      </c>
+      <c r="M55" s="48">
+        <v>0</v>
+      </c>
+      <c r="N55" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="48"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="48"/>
-      <c r="N56" s="48"/>
+      <c r="A56" s="217">
+        <v>44037</v>
+      </c>
+      <c r="B56" s="48">
+        <v>0</v>
+      </c>
+      <c r="C56" s="48">
+        <v>1</v>
+      </c>
+      <c r="D56" s="48">
+        <v>0</v>
+      </c>
+      <c r="E56" s="48">
+        <v>0</v>
+      </c>
+      <c r="F56" s="48">
+        <v>0</v>
+      </c>
+      <c r="G56" s="48">
+        <v>0</v>
+      </c>
+      <c r="H56" s="48">
+        <v>1</v>
+      </c>
+      <c r="I56" s="48">
+        <v>0</v>
+      </c>
+      <c r="J56" s="48">
+        <v>0</v>
+      </c>
+      <c r="K56" s="48">
+        <v>1</v>
+      </c>
+      <c r="L56" s="48">
+        <v>0</v>
+      </c>
+      <c r="M56" s="48">
+        <v>0</v>
+      </c>
+      <c r="N56" s="48">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="48"/>
@@ -8672,8 +8894,8 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10415,31 +10637,71 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="495"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48"/>
-      <c r="J55" s="48"/>
+      <c r="A55" s="495">
+        <v>44036</v>
+      </c>
+      <c r="B55" s="48">
+        <v>0</v>
+      </c>
+      <c r="C55" s="48">
+        <v>0</v>
+      </c>
+      <c r="D55" s="48">
+        <v>0</v>
+      </c>
+      <c r="E55" s="48">
+        <v>0</v>
+      </c>
+      <c r="F55" s="48">
+        <v>2</v>
+      </c>
+      <c r="G55" s="48">
+        <v>1</v>
+      </c>
+      <c r="H55" s="48">
+        <v>1</v>
+      </c>
+      <c r="I55" s="48">
+        <v>1</v>
+      </c>
+      <c r="J55" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="48"/>
+      <c r="A56" s="495">
+        <v>44037</v>
+      </c>
+      <c r="B56" s="48">
+        <v>0</v>
+      </c>
+      <c r="C56" s="48">
+        <v>0</v>
+      </c>
+      <c r="D56" s="48">
+        <v>0</v>
+      </c>
+      <c r="E56" s="48">
+        <v>0</v>
+      </c>
+      <c r="F56" s="48">
+        <v>2</v>
+      </c>
+      <c r="G56" s="48">
+        <v>1</v>
+      </c>
+      <c r="H56" s="48">
+        <v>1</v>
+      </c>
+      <c r="I56" s="48">
+        <v>1</v>
+      </c>
+      <c r="J56" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="48"/>
+      <c r="A57" s="495"/>
       <c r="B57" s="48"/>
       <c r="C57" s="48"/>
       <c r="D57" s="48"/>
@@ -10451,7 +10713,7 @@
       <c r="J57" s="48"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="48"/>
+      <c r="A58" s="495"/>
       <c r="B58" s="48"/>
       <c r="C58" s="48"/>
       <c r="D58" s="48"/>
@@ -10543,8 +10805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:BE20"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BE11" sqref="BE11"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BC17" sqref="BC17:BE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10715,8 +10977,12 @@
       <c r="BB1" s="49">
         <v>44035</v>
       </c>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
+      <c r="BC1" s="49">
+        <v>44036</v>
+      </c>
+      <c r="BD1" s="49">
+        <v>44037</v>
+      </c>
       <c r="BE1" s="48"/>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.2">
@@ -10882,8 +11148,12 @@
       <c r="BB2" s="48">
         <v>4610</v>
       </c>
-      <c r="BC2" s="48"/>
-      <c r="BD2" s="48"/>
+      <c r="BC2" s="48">
+        <v>4642</v>
+      </c>
+      <c r="BD2" s="48">
+        <v>4674</v>
+      </c>
       <c r="BE2" s="48"/>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.2">
@@ -11049,8 +11319,12 @@
       <c r="BB3" s="48">
         <v>4409</v>
       </c>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
+      <c r="BC3" s="48">
+        <v>4441</v>
+      </c>
+      <c r="BD3" s="48">
+        <v>4473</v>
+      </c>
       <c r="BE3" s="48"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.2">
@@ -11216,8 +11490,12 @@
       <c r="BB4" s="48">
         <v>4409</v>
       </c>
-      <c r="BC4" s="48"/>
-      <c r="BD4" s="48"/>
+      <c r="BC4" s="48">
+        <v>4441</v>
+      </c>
+      <c r="BD4" s="48">
+        <v>4473</v>
+      </c>
       <c r="BE4" s="48"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.2">
@@ -11383,8 +11661,12 @@
       <c r="BB5" s="48">
         <v>4409</v>
       </c>
-      <c r="BC5" s="48"/>
-      <c r="BD5" s="48"/>
+      <c r="BC5" s="48">
+        <v>4441</v>
+      </c>
+      <c r="BD5" s="48">
+        <v>4473</v>
+      </c>
       <c r="BE5" s="48"/>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.2">
@@ -11550,8 +11832,12 @@
       <c r="BB6" s="48">
         <v>4409</v>
       </c>
-      <c r="BC6" s="48"/>
-      <c r="BD6" s="48"/>
+      <c r="BC6" s="48">
+        <v>4441</v>
+      </c>
+      <c r="BD6" s="48">
+        <v>4473</v>
+      </c>
       <c r="BE6" s="48"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.2">
@@ -11717,8 +12003,12 @@
       <c r="BB7" s="48">
         <v>3719</v>
       </c>
-      <c r="BC7" s="48"/>
-      <c r="BD7" s="48"/>
+      <c r="BC7" s="48">
+        <v>3751</v>
+      </c>
+      <c r="BD7" s="48">
+        <v>3783</v>
+      </c>
       <c r="BE7" s="48"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.2">
@@ -11884,8 +12174,12 @@
       <c r="BB8" s="48">
         <v>6350</v>
       </c>
-      <c r="BC8" s="48"/>
-      <c r="BD8" s="48"/>
+      <c r="BC8" s="48">
+        <v>6382</v>
+      </c>
+      <c r="BD8" s="48">
+        <v>6414</v>
+      </c>
       <c r="BE8" s="48"/>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.2">
@@ -11943,8 +12237,8 @@
       <c r="AZ9" s="312"/>
       <c r="BA9" s="312"/>
       <c r="BB9" s="312"/>
-      <c r="BC9" s="48"/>
-      <c r="BD9" s="48"/>
+      <c r="BC9" s="312"/>
+      <c r="BD9" s="312"/>
       <c r="BE9" s="48"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.2">
@@ -12110,8 +12404,12 @@
       <c r="BB10" s="48">
         <v>193</v>
       </c>
-      <c r="BC10" s="48"/>
-      <c r="BD10" s="48"/>
+      <c r="BC10" s="48">
+        <v>194</v>
+      </c>
+      <c r="BD10" s="48">
+        <v>195</v>
+      </c>
       <c r="BE10" s="48"/>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.2">
@@ -12277,8 +12575,12 @@
       <c r="BB11" s="48">
         <v>193</v>
       </c>
-      <c r="BC11" s="48"/>
-      <c r="BD11" s="48"/>
+      <c r="BC11" s="48">
+        <v>194</v>
+      </c>
+      <c r="BD11" s="48">
+        <v>195</v>
+      </c>
       <c r="BE11" s="48"/>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
@@ -12444,8 +12746,12 @@
       <c r="BB12" s="48">
         <v>193</v>
       </c>
-      <c r="BC12" s="48"/>
-      <c r="BD12" s="48"/>
+      <c r="BC12" s="48">
+        <v>194</v>
+      </c>
+      <c r="BD12" s="48">
+        <v>195</v>
+      </c>
       <c r="BE12" s="48"/>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
@@ -12611,8 +12917,12 @@
       <c r="BB13" s="48">
         <v>193</v>
       </c>
-      <c r="BC13" s="48"/>
-      <c r="BD13" s="48"/>
+      <c r="BC13" s="48">
+        <v>194</v>
+      </c>
+      <c r="BD13" s="48">
+        <v>195</v>
+      </c>
       <c r="BE13" s="48"/>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
@@ -12778,8 +13088,12 @@
       <c r="BB14" s="48">
         <v>193</v>
       </c>
-      <c r="BC14" s="48"/>
-      <c r="BD14" s="48"/>
+      <c r="BC14" s="48">
+        <v>194</v>
+      </c>
+      <c r="BD14" s="48">
+        <v>195</v>
+      </c>
       <c r="BE14" s="48"/>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.2">
@@ -12945,8 +13259,12 @@
       <c r="BB15" s="48">
         <v>128</v>
       </c>
-      <c r="BC15" s="48"/>
-      <c r="BD15" s="48"/>
+      <c r="BC15" s="48">
+        <v>129</v>
+      </c>
+      <c r="BD15" s="48">
+        <v>130</v>
+      </c>
       <c r="BE15" s="48"/>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.2">
@@ -13112,8 +13430,12 @@
       <c r="BB16" s="48">
         <v>205</v>
       </c>
-      <c r="BC16" s="48"/>
-      <c r="BD16" s="48"/>
+      <c r="BC16" s="48">
+        <v>206</v>
+      </c>
+      <c r="BD16" s="48">
+        <v>207</v>
+      </c>
       <c r="BE16" s="48"/>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.2">
@@ -13171,9 +13493,9 @@
       <c r="AZ17" s="312"/>
       <c r="BA17" s="312"/>
       <c r="BB17" s="312"/>
-      <c r="BC17" s="48"/>
-      <c r="BD17" s="48"/>
-      <c r="BE17" s="48"/>
+      <c r="BC17" s="312"/>
+      <c r="BD17" s="312"/>
+      <c r="BE17" s="312"/>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
@@ -13338,8 +13660,12 @@
       <c r="BB18" s="48">
         <v>1080</v>
       </c>
-      <c r="BC18" s="48"/>
-      <c r="BD18" s="48"/>
+      <c r="BC18" s="48">
+        <v>1087</v>
+      </c>
+      <c r="BD18" s="48">
+        <v>1094</v>
+      </c>
       <c r="BE18" s="48"/>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.2">
@@ -13518,7 +13844,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BB20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BD20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -13565,8 +13891,14 @@
         <f t="shared" si="1"/>
         <v>34693</v>
       </c>
-      <c r="BC20" s="48"/>
-      <c r="BD20" s="48"/>
+      <c r="BC20" s="51">
+        <f t="shared" si="1"/>
+        <v>34931</v>
+      </c>
+      <c r="BD20" s="51">
+        <f t="shared" si="1"/>
+        <v>35169</v>
+      </c>
       <c r="BE20" s="48"/>
     </row>
   </sheetData>
@@ -13866,43 +14198,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="514" t="s">
+      <c r="B8" s="532" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="514"/>
+      <c r="B9" s="532"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="514"/>
+      <c r="B10" s="532"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="514"/>
+      <c r="B11" s="532"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="515" t="s">
+      <c r="B12" s="533" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="515"/>
+      <c r="B13" s="533"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="515"/>
+      <c r="B14" s="533"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="516" t="s">
+      <c r="B15" s="534" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="516"/>
+      <c r="B16" s="534"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 26th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833E085D-9B04-0642-9F84-4407D049ACFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9D07CA-A407-4748-8423-7ECFB4235B8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="535">
+  <cellXfs count="544">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2016,6 +2016,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -2454,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4255,6 +4282,38 @@
       </c>
       <c r="J56" s="531">
         <v>911853</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="15">
+        <v>44038</v>
+      </c>
+      <c r="B57" s="532">
+        <v>390516</v>
+      </c>
+      <c r="C57" s="533">
+        <v>438468</v>
+      </c>
+      <c r="D57" s="534">
+        <v>89397</v>
+      </c>
+      <c r="E57" s="535">
+        <v>43680</v>
+      </c>
+      <c r="F57" s="536">
+        <v>27.781192063833494</v>
+      </c>
+      <c r="G57" s="537">
+        <v>108490</v>
+      </c>
+      <c r="H57" s="538">
+        <v>8777</v>
+      </c>
+      <c r="I57" s="539">
+        <v>10356</v>
+      </c>
+      <c r="J57" s="540">
+        <v>918381</v>
       </c>
     </row>
   </sheetData>
@@ -4268,7 +4327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6356,18 +6415,42 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="48"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
+      <c r="A57" s="217">
+        <v>44038</v>
+      </c>
+      <c r="B57" s="48">
+        <v>0</v>
+      </c>
+      <c r="C57" s="48">
+        <v>1</v>
+      </c>
+      <c r="D57" s="48">
+        <v>0</v>
+      </c>
+      <c r="E57" s="48">
+        <v>0</v>
+      </c>
+      <c r="F57" s="48">
+        <v>1</v>
+      </c>
+      <c r="G57" s="48">
+        <v>0</v>
+      </c>
+      <c r="H57" s="48">
+        <v>0</v>
+      </c>
+      <c r="I57" s="48">
+        <v>0</v>
+      </c>
+      <c r="J57" s="48">
+        <v>0</v>
+      </c>
+      <c r="K57" s="48">
+        <v>0</v>
+      </c>
+      <c r="L57" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="48"/>
@@ -6446,11 +6529,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A56"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8869,20 +8952,51 @@
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="48"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="48"/>
-      <c r="N57" s="48"/>
+      <c r="A57" s="217">
+        <v>44038</v>
+      </c>
+      <c r="B57" s="48">
+        <v>0</v>
+      </c>
+      <c r="C57" s="48">
+        <v>1</v>
+      </c>
+      <c r="D57" s="48">
+        <v>0</v>
+      </c>
+      <c r="E57" s="48">
+        <v>0</v>
+      </c>
+      <c r="F57" s="48">
+        <v>0</v>
+      </c>
+      <c r="G57" s="48">
+        <v>0</v>
+      </c>
+      <c r="H57" s="48">
+        <v>1</v>
+      </c>
+      <c r="I57" s="48">
+        <v>0</v>
+      </c>
+      <c r="J57" s="48">
+        <v>0</v>
+      </c>
+      <c r="K57" s="48">
+        <v>1</v>
+      </c>
+      <c r="L57" s="48">
+        <v>0</v>
+      </c>
+      <c r="M57" s="48">
+        <v>0</v>
+      </c>
+      <c r="N57" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8895,7 +9009,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55:A58"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10701,16 +10815,36 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="495"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
+      <c r="A57" s="495">
+        <v>44038</v>
+      </c>
+      <c r="B57" s="48">
+        <v>0</v>
+      </c>
+      <c r="C57" s="48">
+        <v>0</v>
+      </c>
+      <c r="D57" s="48">
+        <v>0</v>
+      </c>
+      <c r="E57" s="48">
+        <v>0</v>
+      </c>
+      <c r="F57" s="48">
+        <v>2</v>
+      </c>
+      <c r="G57" s="48">
+        <v>1</v>
+      </c>
+      <c r="H57" s="48">
+        <v>1</v>
+      </c>
+      <c r="I57" s="48">
+        <v>1</v>
+      </c>
+      <c r="J57" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="495"/>
@@ -10805,8 +10939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:BE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BC17" sqref="BC17:BE17"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BJ30" sqref="BJ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10983,7 +11117,9 @@
       <c r="BD1" s="49">
         <v>44037</v>
       </c>
-      <c r="BE1" s="48"/>
+      <c r="BE1" s="49">
+        <v>44038</v>
+      </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -11154,7 +11290,9 @@
       <c r="BD2" s="48">
         <v>4674</v>
       </c>
-      <c r="BE2" s="48"/>
+      <c r="BE2" s="48">
+        <v>4706</v>
+      </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -11325,7 +11463,9 @@
       <c r="BD3" s="48">
         <v>4473</v>
       </c>
-      <c r="BE3" s="48"/>
+      <c r="BE3" s="48">
+        <v>4505</v>
+      </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -11496,7 +11636,9 @@
       <c r="BD4" s="48">
         <v>4473</v>
       </c>
-      <c r="BE4" s="48"/>
+      <c r="BE4" s="48">
+        <v>4505</v>
+      </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -11667,7 +11809,9 @@
       <c r="BD5" s="48">
         <v>4473</v>
       </c>
-      <c r="BE5" s="48"/>
+      <c r="BE5" s="48">
+        <v>4505</v>
+      </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -11838,7 +11982,9 @@
       <c r="BD6" s="48">
         <v>4473</v>
       </c>
-      <c r="BE6" s="48"/>
+      <c r="BE6" s="48">
+        <v>4505</v>
+      </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -12009,7 +12155,9 @@
       <c r="BD7" s="48">
         <v>3783</v>
       </c>
-      <c r="BE7" s="48"/>
+      <c r="BE7" s="48">
+        <v>3815</v>
+      </c>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -12180,7 +12328,9 @@
       <c r="BD8" s="48">
         <v>6414</v>
       </c>
-      <c r="BE8" s="48"/>
+      <c r="BE8" s="48">
+        <v>6446</v>
+      </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
@@ -12239,7 +12389,7 @@
       <c r="BB9" s="312"/>
       <c r="BC9" s="312"/>
       <c r="BD9" s="312"/>
-      <c r="BE9" s="48"/>
+      <c r="BE9" s="312"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
@@ -12410,7 +12560,9 @@
       <c r="BD10" s="48">
         <v>195</v>
       </c>
-      <c r="BE10" s="48"/>
+      <c r="BE10" s="48">
+        <v>196</v>
+      </c>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -12581,7 +12733,9 @@
       <c r="BD11" s="48">
         <v>195</v>
       </c>
-      <c r="BE11" s="48"/>
+      <c r="BE11" s="48">
+        <v>196</v>
+      </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -12752,7 +12906,9 @@
       <c r="BD12" s="48">
         <v>195</v>
       </c>
-      <c r="BE12" s="48"/>
+      <c r="BE12" s="48">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -12923,7 +13079,9 @@
       <c r="BD13" s="48">
         <v>195</v>
       </c>
-      <c r="BE13" s="48"/>
+      <c r="BE13" s="48">
+        <v>196</v>
+      </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -13094,7 +13252,9 @@
       <c r="BD14" s="48">
         <v>195</v>
       </c>
-      <c r="BE14" s="48"/>
+      <c r="BE14" s="48">
+        <v>196</v>
+      </c>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -13265,7 +13425,9 @@
       <c r="BD15" s="48">
         <v>130</v>
       </c>
-      <c r="BE15" s="48"/>
+      <c r="BE15" s="48">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -13436,7 +13598,9 @@
       <c r="BD16" s="48">
         <v>207</v>
       </c>
-      <c r="BE16" s="48"/>
+      <c r="BE16" s="48">
+        <v>208</v>
+      </c>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
@@ -13666,7 +13830,9 @@
       <c r="BD18" s="48">
         <v>1094</v>
       </c>
-      <c r="BE18" s="48"/>
+      <c r="BE18" s="48">
+        <v>1101</v>
+      </c>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -13844,7 +14010,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BD20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BE20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -13899,7 +14065,10 @@
         <f t="shared" si="1"/>
         <v>35169</v>
       </c>
-      <c r="BE20" s="48"/>
+      <c r="BE20" s="51">
+        <f t="shared" si="1"/>
+        <v>35407</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14198,43 +14367,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="532" t="s">
+      <c r="B8" s="541" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="532"/>
+      <c r="B9" s="541"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="532"/>
+      <c r="B10" s="541"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="532"/>
+      <c r="B11" s="541"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="533" t="s">
+      <c r="B12" s="542" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="533"/>
+      <c r="B13" s="542"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="533"/>
+      <c r="B14" s="542"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="534" t="s">
+      <c r="B15" s="543" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="534"/>
+      <c r="B16" s="543"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 27th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9D07CA-A407-4748-8423-7ECFB4235B8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D00404-2DB1-5949-A7BD-0EE1E4026FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="544">
+  <cellXfs count="554">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2153,6 +2153,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2162,6 +2189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2481,10 +2509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4314,6 +4342,38 @@
       </c>
       <c r="J57" s="540">
         <v>918381</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="15">
+        <v>44039</v>
+      </c>
+      <c r="B58" s="541">
+        <v>395489</v>
+      </c>
+      <c r="C58" s="542">
+        <v>442884</v>
+      </c>
+      <c r="D58" s="543">
+        <v>85986</v>
+      </c>
+      <c r="E58" s="544">
+        <v>44022</v>
+      </c>
+      <c r="F58" s="545">
+        <v>27.719355026309202</v>
+      </c>
+      <c r="G58" s="546">
+        <v>109627</v>
+      </c>
+      <c r="H58" s="547">
+        <v>8877</v>
+      </c>
+      <c r="I58" s="548">
+        <v>10441</v>
+      </c>
+      <c r="J58" s="549">
+        <v>924359</v>
       </c>
     </row>
   </sheetData>
@@ -4327,7 +4387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6453,18 +6513,42 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="48"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="48"/>
-      <c r="J58" s="48"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="48"/>
+      <c r="A58" s="15">
+        <v>44039</v>
+      </c>
+      <c r="B58" s="48">
+        <v>0</v>
+      </c>
+      <c r="C58" s="48">
+        <v>1</v>
+      </c>
+      <c r="D58" s="48">
+        <v>0</v>
+      </c>
+      <c r="E58" s="48">
+        <v>0</v>
+      </c>
+      <c r="F58" s="48">
+        <v>1</v>
+      </c>
+      <c r="G58" s="48">
+        <v>0</v>
+      </c>
+      <c r="H58" s="48">
+        <v>0</v>
+      </c>
+      <c r="I58" s="48">
+        <v>0</v>
+      </c>
+      <c r="J58" s="48">
+        <v>0</v>
+      </c>
+      <c r="K58" s="48">
+        <v>0</v>
+      </c>
+      <c r="L58" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="48"/>
@@ -6533,7 +6617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8996,7 +9080,48 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="217"/>
+      <c r="A58" s="15">
+        <v>44039</v>
+      </c>
+      <c r="B58" s="553">
+        <v>0</v>
+      </c>
+      <c r="C58" s="216">
+        <v>1</v>
+      </c>
+      <c r="D58" s="216">
+        <v>0</v>
+      </c>
+      <c r="E58" s="216">
+        <v>0</v>
+      </c>
+      <c r="F58" s="216">
+        <v>0</v>
+      </c>
+      <c r="G58" s="216">
+        <v>0</v>
+      </c>
+      <c r="H58" s="216">
+        <v>1</v>
+      </c>
+      <c r="I58" s="216">
+        <v>0</v>
+      </c>
+      <c r="J58" s="216">
+        <v>0</v>
+      </c>
+      <c r="K58" s="216">
+        <v>1</v>
+      </c>
+      <c r="L58" s="216">
+        <v>0</v>
+      </c>
+      <c r="M58" s="216">
+        <v>0</v>
+      </c>
+      <c r="N58" s="216">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9009,7 +9134,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10847,16 +10972,36 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="495"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="48"/>
-      <c r="J58" s="48"/>
+      <c r="A58" s="495">
+        <v>44039</v>
+      </c>
+      <c r="B58" s="48">
+        <v>0</v>
+      </c>
+      <c r="C58" s="48">
+        <v>0</v>
+      </c>
+      <c r="D58" s="48">
+        <v>0</v>
+      </c>
+      <c r="E58" s="48">
+        <v>0</v>
+      </c>
+      <c r="F58" s="48">
+        <v>2</v>
+      </c>
+      <c r="G58" s="48">
+        <v>1</v>
+      </c>
+      <c r="H58" s="48">
+        <v>1</v>
+      </c>
+      <c r="I58" s="48">
+        <v>1</v>
+      </c>
+      <c r="J58" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="48"/>
@@ -10937,10 +11082,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:BE20"/>
+  <dimension ref="A1:BF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BJ30" sqref="BJ30"/>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BC22" sqref="BC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10948,7 +11093,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -11120,8 +11265,11 @@
       <c r="BE1" s="49">
         <v>44038</v>
       </c>
-    </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF1" s="49">
+        <v>44039</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -11293,8 +11441,11 @@
       <c r="BE2" s="48">
         <v>4706</v>
       </c>
-    </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF2">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -11466,8 +11617,11 @@
       <c r="BE3" s="48">
         <v>4505</v>
       </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF3">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -11639,8 +11793,11 @@
       <c r="BE4" s="48">
         <v>4505</v>
       </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF4">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -11812,8 +11969,11 @@
       <c r="BE5" s="48">
         <v>4505</v>
       </c>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF5">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -11985,8 +12145,11 @@
       <c r="BE6" s="48">
         <v>4505</v>
       </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF6">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -12158,8 +12321,11 @@
       <c r="BE7" s="48">
         <v>3815</v>
       </c>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF7">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -12331,8 +12497,11 @@
       <c r="BE8" s="48">
         <v>6446</v>
       </c>
-    </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF8">
+        <v>6478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -12390,8 +12559,9 @@
       <c r="BC9" s="312"/>
       <c r="BD9" s="312"/>
       <c r="BE9" s="312"/>
-    </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF9" s="312"/>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -12563,8 +12733,11 @@
       <c r="BE10" s="48">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF10" s="216">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -12736,8 +12909,11 @@
       <c r="BE11" s="48">
         <v>196</v>
       </c>
-    </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF11" s="216">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -12909,8 +13085,11 @@
       <c r="BE12" s="48">
         <v>196</v>
       </c>
-    </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF12" s="216">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -13082,8 +13261,11 @@
       <c r="BE13" s="48">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF13" s="216">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -13255,8 +13437,11 @@
       <c r="BE14" s="48">
         <v>196</v>
       </c>
-    </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF14" s="216">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -13428,8 +13613,11 @@
       <c r="BE15" s="48">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF15" s="216">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -13601,8 +13789,11 @@
       <c r="BE16" s="48">
         <v>208</v>
       </c>
-    </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF16" s="216">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -13660,8 +13851,9 @@
       <c r="BC17" s="312"/>
       <c r="BD17" s="312"/>
       <c r="BE17" s="312"/>
-    </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF17" s="312"/>
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -13833,15 +14025,18 @@
       <c r="BE18" s="48">
         <v>1101</v>
       </c>
-    </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="BF18">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -14010,7 +14205,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BE20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BF20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -14068,6 +14263,10 @@
       <c r="BE20" s="51">
         <f t="shared" si="1"/>
         <v>35407</v>
+      </c>
+      <c r="BF20" s="51">
+        <f t="shared" si="1"/>
+        <v>35640</v>
       </c>
     </row>
   </sheetData>
@@ -14079,8 +14278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14367,43 +14566,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="541" t="s">
+      <c r="B8" s="550" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="541"/>
+      <c r="B9" s="550"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="541"/>
+      <c r="B10" s="550"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="541"/>
+      <c r="B11" s="550"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="542" t="s">
+      <c r="B12" s="551" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="542"/>
+      <c r="B13" s="551"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="542"/>
+      <c r="B14" s="551"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="543" t="s">
+      <c r="B15" s="552" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="543"/>
+      <c r="B16" s="552"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 28th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D00404-2DB1-5949-A7BD-0EE1E4026FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C148F61C-C0F3-A74D-B538-0C8CA1B960EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="554">
+  <cellXfs count="566">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2180,6 +2180,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2189,7 +2217,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2509,10 +2541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4374,6 +4406,38 @@
       </c>
       <c r="J58" s="549">
         <v>924359</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
+        <v>44040</v>
+      </c>
+      <c r="B59" s="551">
+        <v>402697</v>
+      </c>
+      <c r="C59" s="552">
+        <v>449854</v>
+      </c>
+      <c r="D59" s="553">
+        <v>87538</v>
+      </c>
+      <c r="E59" s="554">
+        <v>44876</v>
+      </c>
+      <c r="F59" s="555">
+        <v>27.63492154150639</v>
+      </c>
+      <c r="G59" s="556">
+        <v>111285</v>
+      </c>
+      <c r="H59" s="557">
+        <v>8991</v>
+      </c>
+      <c r="I59" s="558">
+        <v>10635</v>
+      </c>
+      <c r="J59" s="559">
+        <v>940089</v>
       </c>
     </row>
   </sheetData>
@@ -4387,7 +4451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6551,18 +6615,42 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="48"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="48"/>
+      <c r="A59" s="15">
+        <v>44040</v>
+      </c>
+      <c r="B59" s="48">
+        <v>0</v>
+      </c>
+      <c r="C59" s="48">
+        <v>1</v>
+      </c>
+      <c r="D59" s="48">
+        <v>0</v>
+      </c>
+      <c r="E59" s="48">
+        <v>0</v>
+      </c>
+      <c r="F59" s="48">
+        <v>1</v>
+      </c>
+      <c r="G59" s="48">
+        <v>0</v>
+      </c>
+      <c r="H59" s="48">
+        <v>0</v>
+      </c>
+      <c r="I59" s="48">
+        <v>0</v>
+      </c>
+      <c r="J59" s="48">
+        <v>0</v>
+      </c>
+      <c r="K59" s="48">
+        <v>0</v>
+      </c>
+      <c r="L59" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="48"/>
@@ -6613,11 +6701,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomLeft" activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9083,7 +9171,7 @@
       <c r="A58" s="15">
         <v>44039</v>
       </c>
-      <c r="B58" s="553">
+      <c r="B58" s="550">
         <v>0</v>
       </c>
       <c r="C58" s="216">
@@ -9120,6 +9208,50 @@
         <v>0</v>
       </c>
       <c r="N58" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="15">
+        <v>44040</v>
+      </c>
+      <c r="B59" s="216">
+        <v>0</v>
+      </c>
+      <c r="C59" s="216">
+        <v>1</v>
+      </c>
+      <c r="D59" s="216">
+        <v>0</v>
+      </c>
+      <c r="E59" s="216">
+        <v>0</v>
+      </c>
+      <c r="F59" s="216">
+        <v>0</v>
+      </c>
+      <c r="G59" s="216">
+        <v>0</v>
+      </c>
+      <c r="H59" s="216">
+        <v>1</v>
+      </c>
+      <c r="I59" s="216">
+        <v>0</v>
+      </c>
+      <c r="J59" s="216">
+        <v>0</v>
+      </c>
+      <c r="K59" s="216">
+        <v>1</v>
+      </c>
+      <c r="L59" s="216">
+        <v>0</v>
+      </c>
+      <c r="M59" s="216">
+        <v>0</v>
+      </c>
+      <c r="N59" s="216">
         <v>0</v>
       </c>
     </row>
@@ -9134,7 +9266,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11004,16 +11136,36 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="48"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
+      <c r="A59" s="563">
+        <v>44040</v>
+      </c>
+      <c r="B59" s="48">
+        <v>0</v>
+      </c>
+      <c r="C59" s="48">
+        <v>0</v>
+      </c>
+      <c r="D59" s="48">
+        <v>0</v>
+      </c>
+      <c r="E59" s="48">
+        <v>0</v>
+      </c>
+      <c r="F59" s="48">
+        <v>2</v>
+      </c>
+      <c r="G59" s="48">
+        <v>1</v>
+      </c>
+      <c r="H59" s="48">
+        <v>1</v>
+      </c>
+      <c r="I59" s="48">
+        <v>1</v>
+      </c>
+      <c r="J59" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="48"/>
@@ -11082,10 +11234,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:BF20"/>
+  <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BC22" sqref="BC22"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BC23" sqref="BC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11093,7 +11245,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -11265,11 +11417,36 @@
       <c r="BE1" s="49">
         <v>44038</v>
       </c>
-      <c r="BF1" s="49">
+      <c r="BF1" s="228">
         <v>44039</v>
       </c>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG1" s="49">
+        <v>44040</v>
+      </c>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="48"/>
+      <c r="BR1" s="48"/>
+      <c r="BS1" s="48"/>
+      <c r="BT1" s="48"/>
+      <c r="BU1" s="48"/>
+      <c r="BV1" s="48"/>
+      <c r="BW1" s="48"/>
+      <c r="BX1" s="48"/>
+      <c r="BY1" s="48"/>
+      <c r="BZ1" s="48"/>
+      <c r="CA1" s="48"/>
+      <c r="CB1" s="48"/>
+      <c r="CC1" s="48"/>
+    </row>
+    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -11444,8 +11621,33 @@
       <c r="BF2">
         <v>4738</v>
       </c>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG2" s="48">
+        <v>4770</v>
+      </c>
+      <c r="BH2" s="48"/>
+      <c r="BI2" s="48"/>
+      <c r="BJ2" s="48"/>
+      <c r="BK2" s="48"/>
+      <c r="BL2" s="48"/>
+      <c r="BM2" s="48"/>
+      <c r="BN2" s="48"/>
+      <c r="BO2" s="48"/>
+      <c r="BP2" s="48"/>
+      <c r="BQ2" s="48"/>
+      <c r="BR2" s="48"/>
+      <c r="BS2" s="48"/>
+      <c r="BT2" s="48"/>
+      <c r="BU2" s="48"/>
+      <c r="BV2" s="48"/>
+      <c r="BW2" s="48"/>
+      <c r="BX2" s="48"/>
+      <c r="BY2" s="48"/>
+      <c r="BZ2" s="48"/>
+      <c r="CA2" s="48"/>
+      <c r="CB2" s="48"/>
+      <c r="CC2" s="48"/>
+    </row>
+    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -11620,8 +11822,33 @@
       <c r="BF3">
         <v>4537</v>
       </c>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG3" s="48">
+        <v>4569</v>
+      </c>
+      <c r="BH3" s="48"/>
+      <c r="BI3" s="48"/>
+      <c r="BJ3" s="48"/>
+      <c r="BK3" s="48"/>
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="48"/>
+      <c r="BN3" s="48"/>
+      <c r="BO3" s="48"/>
+      <c r="BP3" s="48"/>
+      <c r="BQ3" s="48"/>
+      <c r="BR3" s="48"/>
+      <c r="BS3" s="48"/>
+      <c r="BT3" s="48"/>
+      <c r="BU3" s="48"/>
+      <c r="BV3" s="48"/>
+      <c r="BW3" s="48"/>
+      <c r="BX3" s="48"/>
+      <c r="BY3" s="48"/>
+      <c r="BZ3" s="48"/>
+      <c r="CA3" s="48"/>
+      <c r="CB3" s="48"/>
+      <c r="CC3" s="48"/>
+    </row>
+    <row r="4" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -11796,8 +12023,33 @@
       <c r="BF4">
         <v>4537</v>
       </c>
-    </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG4" s="48">
+        <v>4569</v>
+      </c>
+      <c r="BH4" s="48"/>
+      <c r="BI4" s="48"/>
+      <c r="BJ4" s="48"/>
+      <c r="BK4" s="48"/>
+      <c r="BL4" s="48"/>
+      <c r="BM4" s="48"/>
+      <c r="BN4" s="48"/>
+      <c r="BO4" s="48"/>
+      <c r="BP4" s="48"/>
+      <c r="BQ4" s="48"/>
+      <c r="BR4" s="48"/>
+      <c r="BS4" s="48"/>
+      <c r="BT4" s="48"/>
+      <c r="BU4" s="48"/>
+      <c r="BV4" s="48"/>
+      <c r="BW4" s="48"/>
+      <c r="BX4" s="48"/>
+      <c r="BY4" s="48"/>
+      <c r="BZ4" s="48"/>
+      <c r="CA4" s="48"/>
+      <c r="CB4" s="48"/>
+      <c r="CC4" s="48"/>
+    </row>
+    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -11972,8 +12224,33 @@
       <c r="BF5">
         <v>4537</v>
       </c>
-    </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG5" s="48">
+        <v>4569</v>
+      </c>
+      <c r="BH5" s="48"/>
+      <c r="BI5" s="48"/>
+      <c r="BJ5" s="48"/>
+      <c r="BK5" s="48"/>
+      <c r="BL5" s="48"/>
+      <c r="BM5" s="48"/>
+      <c r="BN5" s="48"/>
+      <c r="BO5" s="48"/>
+      <c r="BP5" s="48"/>
+      <c r="BQ5" s="48"/>
+      <c r="BR5" s="48"/>
+      <c r="BS5" s="48"/>
+      <c r="BT5" s="48"/>
+      <c r="BU5" s="48"/>
+      <c r="BV5" s="48"/>
+      <c r="BW5" s="48"/>
+      <c r="BX5" s="48"/>
+      <c r="BY5" s="48"/>
+      <c r="BZ5" s="48"/>
+      <c r="CA5" s="48"/>
+      <c r="CB5" s="48"/>
+      <c r="CC5" s="48"/>
+    </row>
+    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -12148,8 +12425,33 @@
       <c r="BF6">
         <v>4537</v>
       </c>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG6" s="48">
+        <v>4569</v>
+      </c>
+      <c r="BH6" s="48"/>
+      <c r="BI6" s="48"/>
+      <c r="BJ6" s="48"/>
+      <c r="BK6" s="48"/>
+      <c r="BL6" s="48"/>
+      <c r="BM6" s="48"/>
+      <c r="BN6" s="48"/>
+      <c r="BO6" s="48"/>
+      <c r="BP6" s="48"/>
+      <c r="BQ6" s="48"/>
+      <c r="BR6" s="48"/>
+      <c r="BS6" s="48"/>
+      <c r="BT6" s="48"/>
+      <c r="BU6" s="48"/>
+      <c r="BV6" s="48"/>
+      <c r="BW6" s="48"/>
+      <c r="BX6" s="48"/>
+      <c r="BY6" s="48"/>
+      <c r="BZ6" s="48"/>
+      <c r="CA6" s="48"/>
+      <c r="CB6" s="48"/>
+      <c r="CC6" s="48"/>
+    </row>
+    <row r="7" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -12324,8 +12626,33 @@
       <c r="BF7">
         <v>3847</v>
       </c>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG7" s="48">
+        <v>3879</v>
+      </c>
+      <c r="BH7" s="48"/>
+      <c r="BI7" s="48"/>
+      <c r="BJ7" s="48"/>
+      <c r="BK7" s="48"/>
+      <c r="BL7" s="48"/>
+      <c r="BM7" s="48"/>
+      <c r="BN7" s="48"/>
+      <c r="BO7" s="48"/>
+      <c r="BP7" s="48"/>
+      <c r="BQ7" s="48"/>
+      <c r="BR7" s="48"/>
+      <c r="BS7" s="48"/>
+      <c r="BT7" s="48"/>
+      <c r="BU7" s="48"/>
+      <c r="BV7" s="48"/>
+      <c r="BW7" s="48"/>
+      <c r="BX7" s="48"/>
+      <c r="BY7" s="48"/>
+      <c r="BZ7" s="48"/>
+      <c r="CA7" s="48"/>
+      <c r="CB7" s="48"/>
+      <c r="CC7" s="48"/>
+    </row>
+    <row r="8" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -12500,8 +12827,33 @@
       <c r="BF8">
         <v>6478</v>
       </c>
-    </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG8" s="48">
+        <v>6510</v>
+      </c>
+      <c r="BH8" s="48"/>
+      <c r="BI8" s="48"/>
+      <c r="BJ8" s="48"/>
+      <c r="BK8" s="48"/>
+      <c r="BL8" s="48"/>
+      <c r="BM8" s="48"/>
+      <c r="BN8" s="48"/>
+      <c r="BO8" s="48"/>
+      <c r="BP8" s="48"/>
+      <c r="BQ8" s="48"/>
+      <c r="BR8" s="48"/>
+      <c r="BS8" s="48"/>
+      <c r="BT8" s="48"/>
+      <c r="BU8" s="48"/>
+      <c r="BV8" s="48"/>
+      <c r="BW8" s="48"/>
+      <c r="BX8" s="48"/>
+      <c r="BY8" s="48"/>
+      <c r="BZ8" s="48"/>
+      <c r="CA8" s="48"/>
+      <c r="CB8" s="48"/>
+      <c r="CC8" s="48"/>
+    </row>
+    <row r="9" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -12559,9 +12911,39 @@
       <c r="BC9" s="312"/>
       <c r="BD9" s="312"/>
       <c r="BE9" s="312"/>
-      <c r="BF9" s="312"/>
-    </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BF9" s="564"/>
+      <c r="BG9" s="312"/>
+      <c r="BH9" s="312"/>
+      <c r="BI9" s="312"/>
+      <c r="BJ9" s="312"/>
+      <c r="BK9" s="312"/>
+      <c r="BL9" s="312"/>
+      <c r="BM9" s="312"/>
+      <c r="BN9" s="312"/>
+      <c r="BO9" s="312"/>
+      <c r="BP9" s="312"/>
+      <c r="BQ9" s="312"/>
+      <c r="BR9" s="312"/>
+      <c r="BS9" s="312"/>
+      <c r="BT9" s="312"/>
+      <c r="BU9" s="312"/>
+      <c r="BV9" s="312"/>
+      <c r="BW9" s="312"/>
+      <c r="BX9" s="312"/>
+      <c r="BY9" s="312"/>
+      <c r="BZ9" s="312"/>
+      <c r="CA9" s="312"/>
+      <c r="CB9" s="312"/>
+      <c r="CC9" s="312"/>
+      <c r="CD9" s="565"/>
+      <c r="CE9" s="312"/>
+      <c r="CF9" s="312"/>
+      <c r="CG9" s="312"/>
+      <c r="CH9" s="312"/>
+      <c r="CI9" s="312"/>
+      <c r="CJ9" s="312"/>
+    </row>
+    <row r="10" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -12733,11 +13115,36 @@
       <c r="BE10" s="48">
         <v>196</v>
       </c>
-      <c r="BF10" s="216">
+      <c r="BF10" s="230">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG10" s="74">
+        <v>197</v>
+      </c>
+      <c r="BH10" s="48"/>
+      <c r="BI10" s="48"/>
+      <c r="BJ10" s="48"/>
+      <c r="BK10" s="48"/>
+      <c r="BL10" s="48"/>
+      <c r="BM10" s="48"/>
+      <c r="BN10" s="48"/>
+      <c r="BO10" s="48"/>
+      <c r="BP10" s="48"/>
+      <c r="BQ10" s="48"/>
+      <c r="BR10" s="48"/>
+      <c r="BS10" s="48"/>
+      <c r="BT10" s="48"/>
+      <c r="BU10" s="48"/>
+      <c r="BV10" s="48"/>
+      <c r="BW10" s="48"/>
+      <c r="BX10" s="48"/>
+      <c r="BY10" s="48"/>
+      <c r="BZ10" s="48"/>
+      <c r="CA10" s="48"/>
+      <c r="CB10" s="48"/>
+      <c r="CC10" s="48"/>
+    </row>
+    <row r="11" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -12909,11 +13316,36 @@
       <c r="BE11" s="48">
         <v>196</v>
       </c>
-      <c r="BF11" s="216">
+      <c r="BF11" s="230">
         <v>196</v>
       </c>
-    </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG11" s="74">
+        <v>197</v>
+      </c>
+      <c r="BH11" s="48"/>
+      <c r="BI11" s="48"/>
+      <c r="BJ11" s="48"/>
+      <c r="BK11" s="48"/>
+      <c r="BL11" s="48"/>
+      <c r="BM11" s="48"/>
+      <c r="BN11" s="48"/>
+      <c r="BO11" s="48"/>
+      <c r="BP11" s="48"/>
+      <c r="BQ11" s="48"/>
+      <c r="BR11" s="48"/>
+      <c r="BS11" s="48"/>
+      <c r="BT11" s="48"/>
+      <c r="BU11" s="48"/>
+      <c r="BV11" s="48"/>
+      <c r="BW11" s="48"/>
+      <c r="BX11" s="48"/>
+      <c r="BY11" s="48"/>
+      <c r="BZ11" s="48"/>
+      <c r="CA11" s="48"/>
+      <c r="CB11" s="48"/>
+      <c r="CC11" s="48"/>
+    </row>
+    <row r="12" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -13085,11 +13517,36 @@
       <c r="BE12" s="48">
         <v>196</v>
       </c>
-      <c r="BF12" s="216">
+      <c r="BF12" s="230">
         <v>196</v>
       </c>
-    </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG12" s="74">
+        <v>197</v>
+      </c>
+      <c r="BH12" s="48"/>
+      <c r="BI12" s="48"/>
+      <c r="BJ12" s="48"/>
+      <c r="BK12" s="48"/>
+      <c r="BL12" s="48"/>
+      <c r="BM12" s="48"/>
+      <c r="BN12" s="48"/>
+      <c r="BO12" s="48"/>
+      <c r="BP12" s="48"/>
+      <c r="BQ12" s="48"/>
+      <c r="BR12" s="48"/>
+      <c r="BS12" s="48"/>
+      <c r="BT12" s="48"/>
+      <c r="BU12" s="48"/>
+      <c r="BV12" s="48"/>
+      <c r="BW12" s="48"/>
+      <c r="BX12" s="48"/>
+      <c r="BY12" s="48"/>
+      <c r="BZ12" s="48"/>
+      <c r="CA12" s="48"/>
+      <c r="CB12" s="48"/>
+      <c r="CC12" s="48"/>
+    </row>
+    <row r="13" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -13261,11 +13718,36 @@
       <c r="BE13" s="48">
         <v>196</v>
       </c>
-      <c r="BF13" s="216">
+      <c r="BF13" s="230">
         <v>196</v>
       </c>
-    </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG13" s="74">
+        <v>197</v>
+      </c>
+      <c r="BH13" s="48"/>
+      <c r="BI13" s="48"/>
+      <c r="BJ13" s="48"/>
+      <c r="BK13" s="48"/>
+      <c r="BL13" s="48"/>
+      <c r="BM13" s="48"/>
+      <c r="BN13" s="48"/>
+      <c r="BO13" s="48"/>
+      <c r="BP13" s="48"/>
+      <c r="BQ13" s="48"/>
+      <c r="BR13" s="48"/>
+      <c r="BS13" s="48"/>
+      <c r="BT13" s="48"/>
+      <c r="BU13" s="48"/>
+      <c r="BV13" s="48"/>
+      <c r="BW13" s="48"/>
+      <c r="BX13" s="48"/>
+      <c r="BY13" s="48"/>
+      <c r="BZ13" s="48"/>
+      <c r="CA13" s="48"/>
+      <c r="CB13" s="48"/>
+      <c r="CC13" s="48"/>
+    </row>
+    <row r="14" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -13437,11 +13919,36 @@
       <c r="BE14" s="48">
         <v>196</v>
       </c>
-      <c r="BF14" s="216">
+      <c r="BF14" s="230">
         <v>196</v>
       </c>
-    </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG14" s="74">
+        <v>197</v>
+      </c>
+      <c r="BH14" s="48"/>
+      <c r="BI14" s="48"/>
+      <c r="BJ14" s="48"/>
+      <c r="BK14" s="48"/>
+      <c r="BL14" s="48"/>
+      <c r="BM14" s="48"/>
+      <c r="BN14" s="48"/>
+      <c r="BO14" s="48"/>
+      <c r="BP14" s="48"/>
+      <c r="BQ14" s="48"/>
+      <c r="BR14" s="48"/>
+      <c r="BS14" s="48"/>
+      <c r="BT14" s="48"/>
+      <c r="BU14" s="48"/>
+      <c r="BV14" s="48"/>
+      <c r="BW14" s="48"/>
+      <c r="BX14" s="48"/>
+      <c r="BY14" s="48"/>
+      <c r="BZ14" s="48"/>
+      <c r="CA14" s="48"/>
+      <c r="CB14" s="48"/>
+      <c r="CC14" s="48"/>
+    </row>
+    <row r="15" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -13613,11 +14120,36 @@
       <c r="BE15" s="48">
         <v>131</v>
       </c>
-      <c r="BF15" s="216">
+      <c r="BF15" s="230">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG15" s="74">
+        <v>133</v>
+      </c>
+      <c r="BH15" s="48"/>
+      <c r="BI15" s="48"/>
+      <c r="BJ15" s="48"/>
+      <c r="BK15" s="48"/>
+      <c r="BL15" s="48"/>
+      <c r="BM15" s="48"/>
+      <c r="BN15" s="48"/>
+      <c r="BO15" s="48"/>
+      <c r="BP15" s="48"/>
+      <c r="BQ15" s="48"/>
+      <c r="BR15" s="48"/>
+      <c r="BS15" s="48"/>
+      <c r="BT15" s="48"/>
+      <c r="BU15" s="48"/>
+      <c r="BV15" s="48"/>
+      <c r="BW15" s="48"/>
+      <c r="BX15" s="48"/>
+      <c r="BY15" s="48"/>
+      <c r="BZ15" s="48"/>
+      <c r="CA15" s="48"/>
+      <c r="CB15" s="48"/>
+      <c r="CC15" s="48"/>
+    </row>
+    <row r="16" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -13789,11 +14321,36 @@
       <c r="BE16" s="48">
         <v>208</v>
       </c>
-      <c r="BF16" s="216">
+      <c r="BF16" s="230">
         <v>209</v>
       </c>
-    </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG16" s="74">
+        <v>210</v>
+      </c>
+      <c r="BH16" s="48"/>
+      <c r="BI16" s="48"/>
+      <c r="BJ16" s="48"/>
+      <c r="BK16" s="48"/>
+      <c r="BL16" s="48"/>
+      <c r="BM16" s="48"/>
+      <c r="BN16" s="48"/>
+      <c r="BO16" s="48"/>
+      <c r="BP16" s="48"/>
+      <c r="BQ16" s="48"/>
+      <c r="BR16" s="48"/>
+      <c r="BS16" s="48"/>
+      <c r="BT16" s="48"/>
+      <c r="BU16" s="48"/>
+      <c r="BV16" s="48"/>
+      <c r="BW16" s="48"/>
+      <c r="BX16" s="48"/>
+      <c r="BY16" s="48"/>
+      <c r="BZ16" s="48"/>
+      <c r="CA16" s="48"/>
+      <c r="CB16" s="48"/>
+      <c r="CC16" s="48"/>
+    </row>
+    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -13851,9 +14408,35 @@
       <c r="BC17" s="312"/>
       <c r="BD17" s="312"/>
       <c r="BE17" s="312"/>
-      <c r="BF17" s="312"/>
-    </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BF17" s="564"/>
+      <c r="BG17" s="312"/>
+      <c r="BH17" s="312"/>
+      <c r="BI17" s="312"/>
+      <c r="BJ17" s="312"/>
+      <c r="BK17" s="312"/>
+      <c r="BL17" s="312"/>
+      <c r="BM17" s="312"/>
+      <c r="BN17" s="312"/>
+      <c r="BO17" s="312"/>
+      <c r="BP17" s="312"/>
+      <c r="BQ17" s="312"/>
+      <c r="BR17" s="312"/>
+      <c r="BS17" s="312"/>
+      <c r="BT17" s="312"/>
+      <c r="BU17" s="312"/>
+      <c r="BV17" s="312"/>
+      <c r="BW17" s="312"/>
+      <c r="BX17" s="312"/>
+      <c r="BY17" s="312"/>
+      <c r="BZ17" s="312"/>
+      <c r="CA17" s="312"/>
+      <c r="CB17" s="312"/>
+      <c r="CC17" s="312"/>
+      <c r="CD17" s="565"/>
+      <c r="CE17" s="312"/>
+      <c r="CF17" s="312"/>
+    </row>
+    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -14028,15 +14611,18 @@
       <c r="BF18">
         <v>1108</v>
       </c>
-    </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BG18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -14205,7 +14791,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BF20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BG20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -14267,6 +14853,10 @@
       <c r="BF20" s="51">
         <f t="shared" si="1"/>
         <v>35640</v>
+      </c>
+      <c r="BG20" s="51">
+        <f t="shared" si="1"/>
+        <v>34878</v>
       </c>
     </row>
   </sheetData>
@@ -14278,8 +14868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14566,43 +15156,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="550" t="s">
+      <c r="B8" s="560" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="550"/>
+      <c r="B9" s="560"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="550"/>
+      <c r="B10" s="560"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="550"/>
+      <c r="B11" s="560"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="551" t="s">
+      <c r="B12" s="561" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="551"/>
+      <c r="B13" s="561"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="551"/>
+      <c r="B14" s="561"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="552" t="s">
+      <c r="B15" s="562" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="552"/>
+      <c r="B16" s="562"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 29th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C148F61C-C0F3-A74D-B538-0C8CA1B960EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD25A75-B64F-3F4D-86C2-E883D6B7449C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>29 de Julio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El número de observaciones de sx /nal hasta uci/nal subio en dos observaciones </t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="566">
+  <cellXfs count="574">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2208,6 +2214,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2217,11 +2252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2541,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4438,6 +4468,38 @@
       </c>
       <c r="J59" s="559">
         <v>940089</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="15">
+        <v>44041</v>
+      </c>
+      <c r="B60" s="562">
+        <v>408449</v>
+      </c>
+      <c r="C60" s="563">
+        <v>455087</v>
+      </c>
+      <c r="D60" s="564">
+        <v>89978</v>
+      </c>
+      <c r="E60" s="565">
+        <v>45361</v>
+      </c>
+      <c r="F60" s="566">
+        <v>27.520204480853177</v>
+      </c>
+      <c r="G60" s="567">
+        <v>112406</v>
+      </c>
+      <c r="H60" s="568">
+        <v>9077</v>
+      </c>
+      <c r="I60" s="569">
+        <v>10772</v>
+      </c>
+      <c r="J60" s="570">
+        <v>953514</v>
       </c>
     </row>
   </sheetData>
@@ -4451,7 +4513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6577,7 +6639,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="15">
+      <c r="A58" s="217">
         <v>44039</v>
       </c>
       <c r="B58" s="48">
@@ -6615,7 +6677,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="15">
+      <c r="A59" s="217">
         <v>44040</v>
       </c>
       <c r="B59" s="48">
@@ -6653,18 +6715,42 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
+      <c r="A60" s="217">
+        <v>44041</v>
+      </c>
+      <c r="B60" s="48">
+        <v>0</v>
+      </c>
+      <c r="C60" s="48">
+        <v>1</v>
+      </c>
+      <c r="D60" s="48">
+        <v>0</v>
+      </c>
+      <c r="E60" s="48">
+        <v>0</v>
+      </c>
+      <c r="F60" s="48">
+        <v>1</v>
+      </c>
+      <c r="G60" s="48">
+        <v>0</v>
+      </c>
+      <c r="H60" s="48">
+        <v>0</v>
+      </c>
+      <c r="I60" s="48">
+        <v>0</v>
+      </c>
+      <c r="J60" s="48">
+        <v>0</v>
+      </c>
+      <c r="K60" s="48">
+        <v>0</v>
+      </c>
+      <c r="L60" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="48"/>
@@ -6701,11 +6787,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O59" sqref="O59"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9168,7 +9254,7 @@
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="15">
+      <c r="A58" s="217">
         <v>44039</v>
       </c>
       <c r="B58" s="550">
@@ -9212,7 +9298,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="15">
+      <c r="A59" s="217">
         <v>44040</v>
       </c>
       <c r="B59" s="216">
@@ -9254,6 +9340,53 @@
       <c r="N59" s="216">
         <v>0</v>
       </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="217">
+        <v>44041</v>
+      </c>
+      <c r="B60" s="216">
+        <v>0</v>
+      </c>
+      <c r="C60" s="216">
+        <v>1</v>
+      </c>
+      <c r="D60" s="216">
+        <v>0</v>
+      </c>
+      <c r="E60" s="216">
+        <v>0</v>
+      </c>
+      <c r="F60" s="216">
+        <v>0</v>
+      </c>
+      <c r="G60" s="216">
+        <v>0</v>
+      </c>
+      <c r="H60" s="216">
+        <v>1</v>
+      </c>
+      <c r="I60" s="216">
+        <v>0</v>
+      </c>
+      <c r="J60" s="216">
+        <v>0</v>
+      </c>
+      <c r="K60" s="216">
+        <v>1</v>
+      </c>
+      <c r="L60" s="216">
+        <v>0</v>
+      </c>
+      <c r="M60" s="216">
+        <v>0</v>
+      </c>
+      <c r="N60" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9266,7 +9399,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11136,7 +11269,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="563">
+      <c r="A59" s="495">
         <v>44040</v>
       </c>
       <c r="B59" s="48">
@@ -11168,16 +11301,36 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
+      <c r="A60" s="495">
+        <v>44041</v>
+      </c>
+      <c r="B60" s="48">
+        <v>0</v>
+      </c>
+      <c r="C60" s="48">
+        <v>0</v>
+      </c>
+      <c r="D60" s="48">
+        <v>0</v>
+      </c>
+      <c r="E60" s="48">
+        <v>0</v>
+      </c>
+      <c r="F60" s="48">
+        <v>2</v>
+      </c>
+      <c r="G60" s="48">
+        <v>1</v>
+      </c>
+      <c r="H60" s="48">
+        <v>1</v>
+      </c>
+      <c r="I60" s="48">
+        <v>1</v>
+      </c>
+      <c r="J60" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="48"/>
@@ -11236,8 +11389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BC23" sqref="BC23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BH14" sqref="BH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11423,7 +11576,9 @@
       <c r="BG1" s="49">
         <v>44040</v>
       </c>
-      <c r="BH1" s="48"/>
+      <c r="BH1" s="49">
+        <v>44041</v>
+      </c>
       <c r="BI1" s="48"/>
       <c r="BJ1" s="48"/>
       <c r="BK1" s="48"/>
@@ -11624,7 +11779,9 @@
       <c r="BG2" s="48">
         <v>4770</v>
       </c>
-      <c r="BH2" s="48"/>
+      <c r="BH2" s="48">
+        <v>4802</v>
+      </c>
       <c r="BI2" s="48"/>
       <c r="BJ2" s="48"/>
       <c r="BK2" s="48"/>
@@ -11825,7 +11982,9 @@
       <c r="BG3" s="48">
         <v>4569</v>
       </c>
-      <c r="BH3" s="48"/>
+      <c r="BH3" s="48">
+        <v>4601</v>
+      </c>
       <c r="BI3" s="48"/>
       <c r="BJ3" s="48"/>
       <c r="BK3" s="48"/>
@@ -12026,7 +12185,9 @@
       <c r="BG4" s="48">
         <v>4569</v>
       </c>
-      <c r="BH4" s="48"/>
+      <c r="BH4" s="48">
+        <v>4601</v>
+      </c>
       <c r="BI4" s="48"/>
       <c r="BJ4" s="48"/>
       <c r="BK4" s="48"/>
@@ -12227,7 +12388,9 @@
       <c r="BG5" s="48">
         <v>4569</v>
       </c>
-      <c r="BH5" s="48"/>
+      <c r="BH5" s="48">
+        <v>4601</v>
+      </c>
       <c r="BI5" s="48"/>
       <c r="BJ5" s="48"/>
       <c r="BK5" s="48"/>
@@ -12428,7 +12591,9 @@
       <c r="BG6" s="48">
         <v>4569</v>
       </c>
-      <c r="BH6" s="48"/>
+      <c r="BH6" s="48">
+        <v>4601</v>
+      </c>
       <c r="BI6" s="48"/>
       <c r="BJ6" s="48"/>
       <c r="BK6" s="48"/>
@@ -12629,7 +12794,9 @@
       <c r="BG7" s="48">
         <v>3879</v>
       </c>
-      <c r="BH7" s="48"/>
+      <c r="BH7" s="48">
+        <v>3911</v>
+      </c>
       <c r="BI7" s="48"/>
       <c r="BJ7" s="48"/>
       <c r="BK7" s="48"/>
@@ -12830,7 +12997,9 @@
       <c r="BG8" s="48">
         <v>6510</v>
       </c>
-      <c r="BH8" s="48"/>
+      <c r="BH8" s="48">
+        <v>6542</v>
+      </c>
       <c r="BI8" s="48"/>
       <c r="BJ8" s="48"/>
       <c r="BK8" s="48"/>
@@ -12911,7 +13080,7 @@
       <c r="BC9" s="312"/>
       <c r="BD9" s="312"/>
       <c r="BE9" s="312"/>
-      <c r="BF9" s="564"/>
+      <c r="BF9" s="560"/>
       <c r="BG9" s="312"/>
       <c r="BH9" s="312"/>
       <c r="BI9" s="312"/>
@@ -12935,7 +13104,7 @@
       <c r="CA9" s="312"/>
       <c r="CB9" s="312"/>
       <c r="CC9" s="312"/>
-      <c r="CD9" s="565"/>
+      <c r="CD9" s="561"/>
       <c r="CE9" s="312"/>
       <c r="CF9" s="312"/>
       <c r="CG9" s="312"/>
@@ -13115,13 +13284,15 @@
       <c r="BE10" s="48">
         <v>196</v>
       </c>
-      <c r="BF10" s="230">
+      <c r="BF10" s="74">
         <v>196</v>
       </c>
       <c r="BG10" s="74">
         <v>197</v>
       </c>
-      <c r="BH10" s="48"/>
+      <c r="BH10" s="74">
+        <v>199</v>
+      </c>
       <c r="BI10" s="48"/>
       <c r="BJ10" s="48"/>
       <c r="BK10" s="48"/>
@@ -13316,13 +13487,15 @@
       <c r="BE11" s="48">
         <v>196</v>
       </c>
-      <c r="BF11" s="230">
+      <c r="BF11" s="74">
         <v>196</v>
       </c>
       <c r="BG11" s="74">
         <v>197</v>
       </c>
-      <c r="BH11" s="48"/>
+      <c r="BH11" s="48">
+        <v>199</v>
+      </c>
       <c r="BI11" s="48"/>
       <c r="BJ11" s="48"/>
       <c r="BK11" s="48"/>
@@ -13517,13 +13690,15 @@
       <c r="BE12" s="48">
         <v>196</v>
       </c>
-      <c r="BF12" s="230">
+      <c r="BF12" s="74">
         <v>196</v>
       </c>
       <c r="BG12" s="74">
         <v>197</v>
       </c>
-      <c r="BH12" s="48"/>
+      <c r="BH12" s="48">
+        <v>199</v>
+      </c>
       <c r="BI12" s="48"/>
       <c r="BJ12" s="48"/>
       <c r="BK12" s="48"/>
@@ -13718,13 +13893,15 @@
       <c r="BE13" s="48">
         <v>196</v>
       </c>
-      <c r="BF13" s="230">
+      <c r="BF13" s="74">
         <v>196</v>
       </c>
       <c r="BG13" s="74">
         <v>197</v>
       </c>
-      <c r="BH13" s="48"/>
+      <c r="BH13" s="48">
+        <v>199</v>
+      </c>
       <c r="BI13" s="48"/>
       <c r="BJ13" s="48"/>
       <c r="BK13" s="48"/>
@@ -13919,13 +14096,15 @@
       <c r="BE14" s="48">
         <v>196</v>
       </c>
-      <c r="BF14" s="230">
+      <c r="BF14" s="74">
         <v>196</v>
       </c>
       <c r="BG14" s="74">
         <v>197</v>
       </c>
-      <c r="BH14" s="48"/>
+      <c r="BH14" s="48">
+        <v>199</v>
+      </c>
       <c r="BI14" s="48"/>
       <c r="BJ14" s="48"/>
       <c r="BK14" s="48"/>
@@ -14120,13 +14299,15 @@
       <c r="BE15" s="48">
         <v>131</v>
       </c>
-      <c r="BF15" s="230">
+      <c r="BF15" s="74">
         <v>132</v>
       </c>
       <c r="BG15" s="74">
         <v>133</v>
       </c>
-      <c r="BH15" s="48"/>
+      <c r="BH15" s="48">
+        <v>134</v>
+      </c>
       <c r="BI15" s="48"/>
       <c r="BJ15" s="48"/>
       <c r="BK15" s="48"/>
@@ -14321,13 +14502,15 @@
       <c r="BE16" s="48">
         <v>208</v>
       </c>
-      <c r="BF16" s="230">
+      <c r="BF16" s="74">
         <v>209</v>
       </c>
       <c r="BG16" s="74">
         <v>210</v>
       </c>
-      <c r="BH16" s="48"/>
+      <c r="BH16" s="48">
+        <v>211</v>
+      </c>
       <c r="BI16" s="48"/>
       <c r="BJ16" s="48"/>
       <c r="BK16" s="48"/>
@@ -14408,7 +14591,7 @@
       <c r="BC17" s="312"/>
       <c r="BD17" s="312"/>
       <c r="BE17" s="312"/>
-      <c r="BF17" s="564"/>
+      <c r="BF17" s="560"/>
       <c r="BG17" s="312"/>
       <c r="BH17" s="312"/>
       <c r="BI17" s="312"/>
@@ -14432,7 +14615,7 @@
       <c r="CA17" s="312"/>
       <c r="CB17" s="312"/>
       <c r="CC17" s="312"/>
-      <c r="CD17" s="565"/>
+      <c r="CD17" s="561"/>
       <c r="CE17" s="312"/>
       <c r="CF17" s="312"/>
     </row>
@@ -14612,7 +14795,10 @@
         <v>1108</v>
       </c>
       <c r="BG18">
-        <v>115</v>
+        <v>1115</v>
+      </c>
+      <c r="BH18" s="216">
+        <v>1122</v>
       </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
@@ -14791,7 +14977,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BG20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BH20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -14856,7 +15042,11 @@
       </c>
       <c r="BG20" s="51">
         <f t="shared" si="1"/>
-        <v>34878</v>
+        <v>35878</v>
+      </c>
+      <c r="BH20" s="51">
+        <f t="shared" si="1"/>
+        <v>36121</v>
       </c>
     </row>
   </sheetData>
@@ -15071,10 +15261,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15156,43 +15346,51 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="560" t="s">
+      <c r="B8" s="571" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="560"/>
+      <c r="B9" s="571"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="560"/>
+      <c r="B10" s="571"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="560"/>
+      <c r="B11" s="571"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="561" t="s">
+      <c r="B12" s="572" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="561"/>
+      <c r="B13" s="572"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="561"/>
+      <c r="B14" s="572"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="562" t="s">
+      <c r="B15" s="573" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="562"/>
+      <c r="B16" s="573"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
County data and State data by age groups using raw data from July 29th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD25A75-B64F-3F4D-86C2-E883D6B7449C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2F221D-4210-2C42-A9B0-83C4AB4126A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -2275,7 +2275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4512,7 +4512,7 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
@@ -6790,8 +6790,8 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:A61"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15058,8 +15058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15083,7 +15083,9 @@
       <c r="F1" s="38">
         <v>44025</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="38">
+        <v>44041</v>
+      </c>
       <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -15105,6 +15107,9 @@
       <c r="F2">
         <v>158794</v>
       </c>
+      <c r="G2">
+        <v>193601</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -15125,6 +15130,9 @@
       <c r="F3">
         <v>149677</v>
       </c>
+      <c r="G3">
+        <v>184038</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
@@ -15145,6 +15153,9 @@
       <c r="F4">
         <v>149677</v>
       </c>
+      <c r="G4">
+        <v>184038</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -15165,6 +15176,9 @@
       <c r="F5">
         <v>149677</v>
       </c>
+      <c r="G5">
+        <v>184038</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
@@ -15185,6 +15199,9 @@
       <c r="F6">
         <v>149677</v>
       </c>
+      <c r="G6">
+        <v>184038</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
@@ -15205,6 +15222,9 @@
       <c r="F7">
         <v>86350</v>
       </c>
+      <c r="G7">
+        <v>111725</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
@@ -15225,6 +15245,9 @@
       <c r="F8">
         <v>224128</v>
       </c>
+      <c r="G8">
+        <v>261066</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -15252,6 +15275,10 @@
       <c r="F10">
         <f>SUM(F2:F8)</f>
         <v>1067980</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G2:G8)</f>
+        <v>1302544</v>
       </c>
     </row>
   </sheetData>
@@ -15263,7 +15290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for July 30th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2F221D-4210-2C42-A9B0-83C4AB4126A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDAFDF2-EA1C-074C-BB06-B896814C179D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="574">
+  <cellXfs count="583">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2216,6 +2216,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2275,7 +2302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2571,10 +2598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4502,6 +4529,38 @@
         <v>953514</v>
       </c>
     </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="15">
+        <v>44042</v>
+      </c>
+      <c r="B61" s="571">
+        <v>416179</v>
+      </c>
+      <c r="C61" s="572">
+        <v>461775</v>
+      </c>
+      <c r="D61" s="573">
+        <v>90582</v>
+      </c>
+      <c r="E61" s="574">
+        <v>46000</v>
+      </c>
+      <c r="F61" s="575">
+        <v>27.380045605376534</v>
+      </c>
+      <c r="G61" s="576">
+        <v>113950</v>
+      </c>
+      <c r="H61" s="577">
+        <v>9188</v>
+      </c>
+      <c r="I61" s="578">
+        <v>10909</v>
+      </c>
+      <c r="J61" s="579">
+        <v>968536</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4512,8 +4571,8 @@
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6753,18 +6812,42 @@
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
+      <c r="A61" s="15">
+        <v>44042</v>
+      </c>
+      <c r="B61" s="48">
+        <v>0</v>
+      </c>
+      <c r="C61" s="48">
+        <v>1</v>
+      </c>
+      <c r="D61" s="48">
+        <v>0</v>
+      </c>
+      <c r="E61" s="48">
+        <v>0</v>
+      </c>
+      <c r="F61" s="48">
+        <v>1</v>
+      </c>
+      <c r="G61" s="48">
+        <v>0</v>
+      </c>
+      <c r="H61" s="48">
+        <v>0</v>
+      </c>
+      <c r="I61" s="48">
+        <v>0</v>
+      </c>
+      <c r="J61" s="48">
+        <v>0</v>
+      </c>
+      <c r="K61" s="48">
+        <v>0</v>
+      </c>
+      <c r="L61" s="48">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="48"/>
@@ -6790,8 +6873,8 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K60" sqref="K60"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9386,7 +9469,48 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="217"/>
+      <c r="A61" s="15">
+        <v>44042</v>
+      </c>
+      <c r="B61" s="216">
+        <v>0</v>
+      </c>
+      <c r="C61" s="216">
+        <v>1</v>
+      </c>
+      <c r="D61" s="216">
+        <v>0</v>
+      </c>
+      <c r="E61" s="216">
+        <v>0</v>
+      </c>
+      <c r="F61" s="216">
+        <v>0</v>
+      </c>
+      <c r="G61" s="216">
+        <v>0</v>
+      </c>
+      <c r="H61" s="216">
+        <v>1</v>
+      </c>
+      <c r="I61" s="216">
+        <v>0</v>
+      </c>
+      <c r="J61" s="216">
+        <v>0</v>
+      </c>
+      <c r="K61" s="216">
+        <v>1</v>
+      </c>
+      <c r="L61" s="216">
+        <v>0</v>
+      </c>
+      <c r="M61" s="216">
+        <v>0</v>
+      </c>
+      <c r="N61" s="216">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9399,7 +9523,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59:A60"/>
+      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11333,16 +11457,36 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
+      <c r="A61" s="15">
+        <v>44042</v>
+      </c>
+      <c r="B61" s="48">
+        <v>0</v>
+      </c>
+      <c r="C61" s="48">
+        <v>0</v>
+      </c>
+      <c r="D61" s="48">
+        <v>0</v>
+      </c>
+      <c r="E61" s="48">
+        <v>0</v>
+      </c>
+      <c r="F61" s="48">
+        <v>2</v>
+      </c>
+      <c r="G61" s="48">
+        <v>1</v>
+      </c>
+      <c r="H61" s="48">
+        <v>1</v>
+      </c>
+      <c r="I61" s="48">
+        <v>1</v>
+      </c>
+      <c r="J61" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="48"/>
@@ -11389,8 +11533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BH14" sqref="BH14"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BH29" sqref="BH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11579,7 +11723,9 @@
       <c r="BH1" s="49">
         <v>44041</v>
       </c>
-      <c r="BI1" s="48"/>
+      <c r="BI1" s="15">
+        <v>44042</v>
+      </c>
       <c r="BJ1" s="48"/>
       <c r="BK1" s="48"/>
       <c r="BL1" s="48"/>
@@ -11782,7 +11928,9 @@
       <c r="BH2" s="48">
         <v>4802</v>
       </c>
-      <c r="BI2" s="48"/>
+      <c r="BI2" s="48">
+        <v>4834</v>
+      </c>
       <c r="BJ2" s="48"/>
       <c r="BK2" s="48"/>
       <c r="BL2" s="48"/>
@@ -11985,7 +12133,9 @@
       <c r="BH3" s="48">
         <v>4601</v>
       </c>
-      <c r="BI3" s="48"/>
+      <c r="BI3" s="48">
+        <v>4633</v>
+      </c>
       <c r="BJ3" s="48"/>
       <c r="BK3" s="48"/>
       <c r="BL3" s="48"/>
@@ -12188,7 +12338,9 @@
       <c r="BH4" s="48">
         <v>4601</v>
       </c>
-      <c r="BI4" s="48"/>
+      <c r="BI4" s="48">
+        <v>4633</v>
+      </c>
       <c r="BJ4" s="48"/>
       <c r="BK4" s="48"/>
       <c r="BL4" s="48"/>
@@ -12391,7 +12543,9 @@
       <c r="BH5" s="48">
         <v>4601</v>
       </c>
-      <c r="BI5" s="48"/>
+      <c r="BI5" s="48">
+        <v>4633</v>
+      </c>
       <c r="BJ5" s="48"/>
       <c r="BK5" s="48"/>
       <c r="BL5" s="48"/>
@@ -12594,7 +12748,9 @@
       <c r="BH6" s="48">
         <v>4601</v>
       </c>
-      <c r="BI6" s="48"/>
+      <c r="BI6" s="48">
+        <v>4633</v>
+      </c>
       <c r="BJ6" s="48"/>
       <c r="BK6" s="48"/>
       <c r="BL6" s="48"/>
@@ -12797,7 +12953,9 @@
       <c r="BH7" s="48">
         <v>3911</v>
       </c>
-      <c r="BI7" s="48"/>
+      <c r="BI7" s="48">
+        <v>3943</v>
+      </c>
       <c r="BJ7" s="48"/>
       <c r="BK7" s="48"/>
       <c r="BL7" s="48"/>
@@ -13000,7 +13158,9 @@
       <c r="BH8" s="48">
         <v>6542</v>
       </c>
-      <c r="BI8" s="48"/>
+      <c r="BI8" s="48">
+        <v>6574</v>
+      </c>
       <c r="BJ8" s="48"/>
       <c r="BK8" s="48"/>
       <c r="BL8" s="48"/>
@@ -13293,7 +13453,9 @@
       <c r="BH10" s="74">
         <v>199</v>
       </c>
-      <c r="BI10" s="48"/>
+      <c r="BI10" s="48">
+        <v>200</v>
+      </c>
       <c r="BJ10" s="48"/>
       <c r="BK10" s="48"/>
       <c r="BL10" s="48"/>
@@ -13496,7 +13658,9 @@
       <c r="BH11" s="48">
         <v>199</v>
       </c>
-      <c r="BI11" s="48"/>
+      <c r="BI11" s="48">
+        <v>200</v>
+      </c>
       <c r="BJ11" s="48"/>
       <c r="BK11" s="48"/>
       <c r="BL11" s="48"/>
@@ -13699,7 +13863,9 @@
       <c r="BH12" s="48">
         <v>199</v>
       </c>
-      <c r="BI12" s="48"/>
+      <c r="BI12" s="48">
+        <v>200</v>
+      </c>
       <c r="BJ12" s="48"/>
       <c r="BK12" s="48"/>
       <c r="BL12" s="48"/>
@@ -13902,7 +14068,9 @@
       <c r="BH13" s="48">
         <v>199</v>
       </c>
-      <c r="BI13" s="48"/>
+      <c r="BI13" s="48">
+        <v>200</v>
+      </c>
       <c r="BJ13" s="48"/>
       <c r="BK13" s="48"/>
       <c r="BL13" s="48"/>
@@ -14105,7 +14273,9 @@
       <c r="BH14" s="48">
         <v>199</v>
       </c>
-      <c r="BI14" s="48"/>
+      <c r="BI14" s="48">
+        <v>200</v>
+      </c>
       <c r="BJ14" s="48"/>
       <c r="BK14" s="48"/>
       <c r="BL14" s="48"/>
@@ -14308,7 +14478,9 @@
       <c r="BH15" s="48">
         <v>134</v>
       </c>
-      <c r="BI15" s="48"/>
+      <c r="BI15" s="48">
+        <v>135</v>
+      </c>
       <c r="BJ15" s="48"/>
       <c r="BK15" s="48"/>
       <c r="BL15" s="48"/>
@@ -14511,7 +14683,9 @@
       <c r="BH16" s="48">
         <v>211</v>
       </c>
-      <c r="BI16" s="48"/>
+      <c r="BI16" s="48">
+        <v>212</v>
+      </c>
       <c r="BJ16" s="48"/>
       <c r="BK16" s="48"/>
       <c r="BL16" s="48"/>
@@ -14800,6 +14974,9 @@
       <c r="BH18" s="216">
         <v>1122</v>
       </c>
+      <c r="BI18" s="216">
+        <v>1129</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -14977,7 +15154,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BH20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BI20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -15047,6 +15224,10 @@
       <c r="BH20" s="51">
         <f t="shared" si="1"/>
         <v>36121</v>
+      </c>
+      <c r="BI20" s="51">
+        <f t="shared" si="1"/>
+        <v>36359</v>
       </c>
     </row>
   </sheetData>
@@ -15058,8 +15239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15083,9 +15264,7 @@
       <c r="F1" s="38">
         <v>44025</v>
       </c>
-      <c r="G1" s="38">
-        <v>44041</v>
-      </c>
+      <c r="G1" s="38"/>
       <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -15107,9 +15286,6 @@
       <c r="F2">
         <v>158794</v>
       </c>
-      <c r="G2">
-        <v>193601</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -15130,9 +15306,6 @@
       <c r="F3">
         <v>149677</v>
       </c>
-      <c r="G3">
-        <v>184038</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
@@ -15153,9 +15326,6 @@
       <c r="F4">
         <v>149677</v>
       </c>
-      <c r="G4">
-        <v>184038</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -15176,9 +15346,6 @@
       <c r="F5">
         <v>149677</v>
       </c>
-      <c r="G5">
-        <v>184038</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
@@ -15199,9 +15366,6 @@
       <c r="F6">
         <v>149677</v>
       </c>
-      <c r="G6">
-        <v>184038</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
@@ -15222,9 +15386,6 @@
       <c r="F7">
         <v>86350</v>
       </c>
-      <c r="G7">
-        <v>111725</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
@@ -15245,9 +15406,6 @@
       <c r="F8">
         <v>224128</v>
       </c>
-      <c r="G8">
-        <v>261066</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -15275,10 +15433,6 @@
       <c r="F10">
         <f>SUM(F2:F8)</f>
         <v>1067980</v>
-      </c>
-      <c r="G10">
-        <f>SUM(G2:G8)</f>
-        <v>1302544</v>
       </c>
     </row>
   </sheetData>
@@ -15373,43 +15527,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="571" t="s">
+      <c r="B8" s="580" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="571"/>
+      <c r="B9" s="580"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="571"/>
+      <c r="B10" s="580"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="571"/>
+      <c r="B11" s="580"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="572" t="s">
+      <c r="B12" s="581" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="572"/>
+      <c r="B13" s="581"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="572"/>
+      <c r="B14" s="581"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="573" t="s">
+      <c r="B15" s="582" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="573"/>
+      <c r="B16" s="582"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 1st
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDAFDF2-EA1C-074C-BB06-B896814C179D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D6ADC4-11CB-FD44-89A8-0F2A4BCD2A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="4220" windowWidth="26140" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33420" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="583">
+  <cellXfs count="602">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2243,6 +2243,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2598,10 +2653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4561,6 +4616,70 @@
         <v>968536</v>
       </c>
     </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="15">
+        <v>44043</v>
+      </c>
+      <c r="B62" s="580">
+        <v>424637</v>
+      </c>
+      <c r="C62" s="581">
+        <v>469629</v>
+      </c>
+      <c r="D62" s="582">
+        <v>90022</v>
+      </c>
+      <c r="E62" s="583">
+        <v>46688</v>
+      </c>
+      <c r="F62" s="584">
+        <v>27.164378045248061</v>
+      </c>
+      <c r="G62" s="585">
+        <v>115350</v>
+      </c>
+      <c r="H62" s="586">
+        <v>9312</v>
+      </c>
+      <c r="I62" s="587">
+        <v>11076</v>
+      </c>
+      <c r="J62" s="588">
+        <v>984288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="15">
+        <v>44044</v>
+      </c>
+      <c r="B63" s="590">
+        <v>434193</v>
+      </c>
+      <c r="C63" s="591">
+        <v>477733</v>
+      </c>
+      <c r="D63" s="592">
+        <v>87771</v>
+      </c>
+      <c r="E63" s="593">
+        <v>47472</v>
+      </c>
+      <c r="F63" s="594">
+        <v>27.023236210625228</v>
+      </c>
+      <c r="G63" s="595">
+        <v>117333</v>
+      </c>
+      <c r="H63" s="596">
+        <v>9400</v>
+      </c>
+      <c r="I63" s="597">
+        <v>11273</v>
+      </c>
+      <c r="J63" s="598">
+        <v>999697</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4568,11 +4687,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6850,18 +6969,80 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="48"/>
-      <c r="J62" s="48"/>
-      <c r="K62" s="48"/>
-      <c r="L62" s="48"/>
+      <c r="A62" s="15">
+        <v>44043</v>
+      </c>
+      <c r="B62" s="48">
+        <v>0</v>
+      </c>
+      <c r="C62" s="48">
+        <v>1</v>
+      </c>
+      <c r="D62" s="48">
+        <v>0</v>
+      </c>
+      <c r="E62" s="48">
+        <v>0</v>
+      </c>
+      <c r="F62" s="48">
+        <v>1</v>
+      </c>
+      <c r="G62" s="48">
+        <v>0</v>
+      </c>
+      <c r="H62" s="48">
+        <v>0</v>
+      </c>
+      <c r="I62" s="48">
+        <v>0</v>
+      </c>
+      <c r="J62" s="48">
+        <v>0</v>
+      </c>
+      <c r="K62" s="48">
+        <v>0</v>
+      </c>
+      <c r="L62" s="48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="15">
+        <v>44044</v>
+      </c>
+      <c r="B63" s="216">
+        <v>0</v>
+      </c>
+      <c r="C63" s="216">
+        <v>1</v>
+      </c>
+      <c r="D63" s="216">
+        <v>0</v>
+      </c>
+      <c r="E63" s="216">
+        <v>0</v>
+      </c>
+      <c r="F63" s="216">
+        <v>1</v>
+      </c>
+      <c r="G63" s="216">
+        <v>0</v>
+      </c>
+      <c r="H63" s="216">
+        <v>0</v>
+      </c>
+      <c r="I63" s="216">
+        <v>0</v>
+      </c>
+      <c r="J63" s="216">
+        <v>0</v>
+      </c>
+      <c r="K63" s="216">
+        <v>0</v>
+      </c>
+      <c r="L63" s="216">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6870,11 +7051,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O61" sqref="O61"/>
+      <selection pane="bottomLeft" activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9509,6 +9690,94 @@
         <v>0</v>
       </c>
       <c r="N61" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="15">
+        <v>44043</v>
+      </c>
+      <c r="B62" s="216">
+        <v>0</v>
+      </c>
+      <c r="C62" s="216">
+        <v>1</v>
+      </c>
+      <c r="D62" s="216">
+        <v>0</v>
+      </c>
+      <c r="E62" s="216">
+        <v>0</v>
+      </c>
+      <c r="F62" s="216">
+        <v>0</v>
+      </c>
+      <c r="G62" s="216">
+        <v>0</v>
+      </c>
+      <c r="H62" s="216">
+        <v>1</v>
+      </c>
+      <c r="I62" s="216">
+        <v>0</v>
+      </c>
+      <c r="J62" s="216">
+        <v>0</v>
+      </c>
+      <c r="K62" s="216">
+        <v>1</v>
+      </c>
+      <c r="L62" s="216">
+        <v>0</v>
+      </c>
+      <c r="M62" s="216">
+        <v>0</v>
+      </c>
+      <c r="N62" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="15">
+        <v>44044</v>
+      </c>
+      <c r="B63" s="216">
+        <v>0</v>
+      </c>
+      <c r="C63" s="216">
+        <v>1</v>
+      </c>
+      <c r="D63" s="216">
+        <v>0</v>
+      </c>
+      <c r="E63" s="216">
+        <v>0</v>
+      </c>
+      <c r="F63" s="216">
+        <v>0</v>
+      </c>
+      <c r="G63" s="216">
+        <v>0</v>
+      </c>
+      <c r="H63" s="216">
+        <v>1</v>
+      </c>
+      <c r="I63" s="216">
+        <v>0</v>
+      </c>
+      <c r="J63" s="216">
+        <v>0</v>
+      </c>
+      <c r="K63" s="216">
+        <v>1</v>
+      </c>
+      <c r="L63" s="216">
+        <v>0</v>
+      </c>
+      <c r="M63" s="216">
+        <v>0</v>
+      </c>
+      <c r="N63" s="216">
         <v>0</v>
       </c>
     </row>
@@ -9523,7 +9792,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K61" sqref="K61"/>
+      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11489,28 +11758,68 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="48"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="48"/>
-      <c r="J62" s="48"/>
+      <c r="A62" s="15">
+        <v>44043</v>
+      </c>
+      <c r="B62" s="48">
+        <v>0</v>
+      </c>
+      <c r="C62" s="48">
+        <v>0</v>
+      </c>
+      <c r="D62" s="48">
+        <v>0</v>
+      </c>
+      <c r="E62" s="48">
+        <v>0</v>
+      </c>
+      <c r="F62" s="48">
+        <v>2</v>
+      </c>
+      <c r="G62" s="48">
+        <v>1</v>
+      </c>
+      <c r="H62" s="48">
+        <v>1</v>
+      </c>
+      <c r="I62" s="48">
+        <v>1</v>
+      </c>
+      <c r="J62" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="48"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
+      <c r="A63" s="15">
+        <v>44044</v>
+      </c>
+      <c r="B63" s="48">
+        <v>0</v>
+      </c>
+      <c r="C63" s="48">
+        <v>0</v>
+      </c>
+      <c r="D63" s="48">
+        <v>0</v>
+      </c>
+      <c r="E63" s="48">
+        <v>0</v>
+      </c>
+      <c r="F63" s="48">
+        <v>2</v>
+      </c>
+      <c r="G63" s="48">
+        <v>1</v>
+      </c>
+      <c r="H63" s="48">
+        <v>1</v>
+      </c>
+      <c r="I63" s="48">
+        <v>1</v>
+      </c>
+      <c r="J63" s="48">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="48"/>
@@ -11533,8 +11842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BH29" sqref="BH29"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11723,11 +12032,15 @@
       <c r="BH1" s="49">
         <v>44041</v>
       </c>
-      <c r="BI1" s="15">
+      <c r="BI1" s="49">
         <v>44042</v>
       </c>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
+      <c r="BJ1" s="49">
+        <v>44043</v>
+      </c>
+      <c r="BK1" s="15">
+        <v>44044</v>
+      </c>
       <c r="BL1" s="48"/>
       <c r="BM1" s="48"/>
       <c r="BN1" s="48"/>
@@ -11931,8 +12244,12 @@
       <c r="BI2" s="48">
         <v>4834</v>
       </c>
-      <c r="BJ2" s="48"/>
-      <c r="BK2" s="48"/>
+      <c r="BJ2" s="48">
+        <v>4866</v>
+      </c>
+      <c r="BK2" s="48">
+        <v>4898</v>
+      </c>
       <c r="BL2" s="48"/>
       <c r="BM2" s="48"/>
       <c r="BN2" s="48"/>
@@ -12136,8 +12453,12 @@
       <c r="BI3" s="48">
         <v>4633</v>
       </c>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="48"/>
+      <c r="BJ3" s="48">
+        <v>4665</v>
+      </c>
+      <c r="BK3" s="48">
+        <v>4697</v>
+      </c>
       <c r="BL3" s="48"/>
       <c r="BM3" s="48"/>
       <c r="BN3" s="48"/>
@@ -12341,8 +12662,12 @@
       <c r="BI4" s="48">
         <v>4633</v>
       </c>
-      <c r="BJ4" s="48"/>
-      <c r="BK4" s="48"/>
+      <c r="BJ4" s="48">
+        <v>4665</v>
+      </c>
+      <c r="BK4" s="48">
+        <v>4697</v>
+      </c>
       <c r="BL4" s="48"/>
       <c r="BM4" s="48"/>
       <c r="BN4" s="48"/>
@@ -12546,8 +12871,12 @@
       <c r="BI5" s="48">
         <v>4633</v>
       </c>
-      <c r="BJ5" s="48"/>
-      <c r="BK5" s="48"/>
+      <c r="BJ5" s="48">
+        <v>4665</v>
+      </c>
+      <c r="BK5" s="48">
+        <v>4697</v>
+      </c>
       <c r="BL5" s="48"/>
       <c r="BM5" s="48"/>
       <c r="BN5" s="48"/>
@@ -12751,8 +13080,12 @@
       <c r="BI6" s="48">
         <v>4633</v>
       </c>
-      <c r="BJ6" s="48"/>
-      <c r="BK6" s="48"/>
+      <c r="BJ6" s="48">
+        <v>4665</v>
+      </c>
+      <c r="BK6" s="48">
+        <v>4697</v>
+      </c>
       <c r="BL6" s="48"/>
       <c r="BM6" s="48"/>
       <c r="BN6" s="48"/>
@@ -12956,8 +13289,12 @@
       <c r="BI7" s="48">
         <v>3943</v>
       </c>
-      <c r="BJ7" s="48"/>
-      <c r="BK7" s="48"/>
+      <c r="BJ7" s="48">
+        <v>3975</v>
+      </c>
+      <c r="BK7" s="48">
+        <v>4007</v>
+      </c>
       <c r="BL7" s="48"/>
       <c r="BM7" s="48"/>
       <c r="BN7" s="48"/>
@@ -13161,8 +13498,12 @@
       <c r="BI8" s="48">
         <v>6574</v>
       </c>
-      <c r="BJ8" s="48"/>
-      <c r="BK8" s="48"/>
+      <c r="BJ8" s="48">
+        <v>6606</v>
+      </c>
+      <c r="BK8" s="48">
+        <v>6638</v>
+      </c>
       <c r="BL8" s="48"/>
       <c r="BM8" s="48"/>
       <c r="BN8" s="48"/>
@@ -13456,8 +13797,12 @@
       <c r="BI10" s="48">
         <v>200</v>
       </c>
-      <c r="BJ10" s="48"/>
-      <c r="BK10" s="48"/>
+      <c r="BJ10" s="48">
+        <v>201</v>
+      </c>
+      <c r="BK10" s="48">
+        <v>202</v>
+      </c>
       <c r="BL10" s="48"/>
       <c r="BM10" s="48"/>
       <c r="BN10" s="48"/>
@@ -13661,8 +14006,12 @@
       <c r="BI11" s="48">
         <v>200</v>
       </c>
-      <c r="BJ11" s="48"/>
-      <c r="BK11" s="48"/>
+      <c r="BJ11" s="48">
+        <v>201</v>
+      </c>
+      <c r="BK11" s="48">
+        <v>202</v>
+      </c>
       <c r="BL11" s="48"/>
       <c r="BM11" s="48"/>
       <c r="BN11" s="48"/>
@@ -13866,8 +14215,12 @@
       <c r="BI12" s="48">
         <v>200</v>
       </c>
-      <c r="BJ12" s="48"/>
-      <c r="BK12" s="48"/>
+      <c r="BJ12" s="48">
+        <v>201</v>
+      </c>
+      <c r="BK12" s="48">
+        <v>202</v>
+      </c>
       <c r="BL12" s="48"/>
       <c r="BM12" s="48"/>
       <c r="BN12" s="48"/>
@@ -14071,8 +14424,12 @@
       <c r="BI13" s="48">
         <v>200</v>
       </c>
-      <c r="BJ13" s="48"/>
-      <c r="BK13" s="48"/>
+      <c r="BJ13" s="48">
+        <v>201</v>
+      </c>
+      <c r="BK13" s="48">
+        <v>202</v>
+      </c>
       <c r="BL13" s="48"/>
       <c r="BM13" s="48"/>
       <c r="BN13" s="48"/>
@@ -14276,8 +14633,12 @@
       <c r="BI14" s="48">
         <v>200</v>
       </c>
-      <c r="BJ14" s="48"/>
-      <c r="BK14" s="48"/>
+      <c r="BJ14" s="48">
+        <v>201</v>
+      </c>
+      <c r="BK14" s="48">
+        <v>202</v>
+      </c>
       <c r="BL14" s="48"/>
       <c r="BM14" s="48"/>
       <c r="BN14" s="48"/>
@@ -14481,8 +14842,12 @@
       <c r="BI15" s="48">
         <v>135</v>
       </c>
-      <c r="BJ15" s="48"/>
-      <c r="BK15" s="48"/>
+      <c r="BJ15" s="48">
+        <v>136</v>
+      </c>
+      <c r="BK15" s="48">
+        <v>137</v>
+      </c>
       <c r="BL15" s="48"/>
       <c r="BM15" s="48"/>
       <c r="BN15" s="48"/>
@@ -14686,8 +15051,12 @@
       <c r="BI16" s="48">
         <v>212</v>
       </c>
-      <c r="BJ16" s="48"/>
-      <c r="BK16" s="48"/>
+      <c r="BJ16" s="48">
+        <v>213</v>
+      </c>
+      <c r="BK16" s="48">
+        <v>214</v>
+      </c>
       <c r="BL16" s="48"/>
       <c r="BM16" s="48"/>
       <c r="BN16" s="48"/>
@@ -14977,6 +15346,12 @@
       <c r="BI18" s="216">
         <v>1129</v>
       </c>
+      <c r="BJ18" s="589">
+        <v>1136</v>
+      </c>
+      <c r="BK18" s="589">
+        <v>1143</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -15154,7 +15529,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BI20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BK20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -15228,6 +15603,14 @@
       <c r="BI20" s="51">
         <f t="shared" si="1"/>
         <v>36359</v>
+      </c>
+      <c r="BJ20" s="51">
+        <f t="shared" si="1"/>
+        <v>36597</v>
+      </c>
+      <c r="BK20" s="51">
+        <f t="shared" si="1"/>
+        <v>36835</v>
       </c>
     </row>
   </sheetData>
@@ -15527,43 +15910,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="580" t="s">
+      <c r="B8" s="599" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="580"/>
+      <c r="B9" s="599"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="580"/>
+      <c r="B10" s="599"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="580"/>
+      <c r="B11" s="599"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="581" t="s">
+      <c r="B12" s="600" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="581"/>
+      <c r="B13" s="600"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="581"/>
+      <c r="B14" s="600"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="582" t="s">
+      <c r="B15" s="601" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="582"/>
+      <c r="B16" s="601"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 2nd
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D6ADC4-11CB-FD44-89A8-0F2A4BCD2A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC05D2C2-EAB9-B440-8861-F696FFE1C42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33420" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-33420" yWindow="4220" windowWidth="26140" windowHeight="16420" activeTab="1" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="602">
+  <cellXfs count="611">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2653,10 +2680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4680,6 +4707,38 @@
         <v>999697</v>
       </c>
     </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="15">
+        <v>44045</v>
+      </c>
+      <c r="B64" s="599">
+        <v>439046</v>
+      </c>
+      <c r="C64" s="600">
+        <v>483333</v>
+      </c>
+      <c r="D64" s="601">
+        <v>83119</v>
+      </c>
+      <c r="E64" s="602">
+        <v>47746</v>
+      </c>
+      <c r="F64" s="603">
+        <v>26.919958273165001</v>
+      </c>
+      <c r="G64" s="604">
+        <v>118191</v>
+      </c>
+      <c r="H64" s="605">
+        <v>9467</v>
+      </c>
+      <c r="I64" s="606">
+        <v>11325</v>
+      </c>
+      <c r="J64" s="607">
+        <v>1005498</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4687,11 +4746,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7044,6 +7103,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="15">
+        <v>44045</v>
+      </c>
+      <c r="B64" s="216">
+        <v>0</v>
+      </c>
+      <c r="C64" s="216">
+        <v>1</v>
+      </c>
+      <c r="D64" s="216">
+        <v>0</v>
+      </c>
+      <c r="E64" s="216">
+        <v>0</v>
+      </c>
+      <c r="F64" s="216">
+        <v>1</v>
+      </c>
+      <c r="G64" s="216">
+        <v>0</v>
+      </c>
+      <c r="H64" s="216">
+        <v>0</v>
+      </c>
+      <c r="I64" s="216">
+        <v>0</v>
+      </c>
+      <c r="J64" s="216">
+        <v>0</v>
+      </c>
+      <c r="K64" s="216">
+        <v>0</v>
+      </c>
+      <c r="L64" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7051,11 +7148,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O63" sqref="O63"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9779,6 +9876,11 @@
       </c>
       <c r="N63" s="216">
         <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="15">
+        <v>44045</v>
       </c>
     </row>
   </sheetData>
@@ -9792,7 +9894,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11822,7 +11924,9 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="48"/>
+      <c r="A64" s="15">
+        <v>44045</v>
+      </c>
       <c r="B64" s="48"/>
       <c r="C64" s="48"/>
       <c r="D64" s="48"/>
@@ -11842,7 +11946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
@@ -15910,43 +16014,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="599" t="s">
+      <c r="B8" s="608" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="599"/>
+      <c r="B9" s="608"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="599"/>
+      <c r="B10" s="608"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="599"/>
+      <c r="B11" s="608"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="600" t="s">
+      <c r="B12" s="609" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="600"/>
+      <c r="B13" s="609"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="600"/>
+      <c r="B14" s="609"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="601" t="s">
+      <c r="B15" s="610" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="601"/>
+      <c r="B16" s="610"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 4th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAD3E55-6710-0D4D-A740-2BBA8426CDC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717F50EB-C592-C841-84E1-91B75773C20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32600" yWindow="4180" windowWidth="26140" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="611">
+  <cellXfs count="620">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2680,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4739,6 +4766,38 @@
         <v>1005498</v>
       </c>
     </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
+        <v>44046</v>
+      </c>
+      <c r="B65" s="608">
+        <v>443813</v>
+      </c>
+      <c r="C65" s="609">
+        <v>488207</v>
+      </c>
+      <c r="D65" s="610">
+        <v>79030</v>
+      </c>
+      <c r="E65" s="611">
+        <v>48012</v>
+      </c>
+      <c r="F65" s="612">
+        <v>26.875733698652361</v>
+      </c>
+      <c r="G65" s="613">
+        <v>119278</v>
+      </c>
+      <c r="H65" s="614">
+        <v>9554</v>
+      </c>
+      <c r="I65" s="615">
+        <v>11422</v>
+      </c>
+      <c r="J65" s="616">
+        <v>1011050</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4746,11 +4805,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7141,6 +7200,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
+        <v>44046</v>
+      </c>
+      <c r="B65" s="216">
+        <v>0</v>
+      </c>
+      <c r="C65" s="216">
+        <v>1</v>
+      </c>
+      <c r="D65" s="216">
+        <v>0</v>
+      </c>
+      <c r="E65" s="216">
+        <v>0</v>
+      </c>
+      <c r="F65" s="216">
+        <v>1</v>
+      </c>
+      <c r="G65" s="216">
+        <v>0</v>
+      </c>
+      <c r="H65" s="216">
+        <v>0</v>
+      </c>
+      <c r="I65" s="216">
+        <v>0</v>
+      </c>
+      <c r="J65" s="216">
+        <v>0</v>
+      </c>
+      <c r="K65" s="216">
+        <v>0</v>
+      </c>
+      <c r="L65" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7148,11 +7245,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N64" sqref="N64"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9919,6 +10016,50 @@
         <v>0</v>
       </c>
       <c r="N64" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
+        <v>44046</v>
+      </c>
+      <c r="B65" s="216">
+        <v>0</v>
+      </c>
+      <c r="C65" s="216">
+        <v>1</v>
+      </c>
+      <c r="D65" s="216">
+        <v>0</v>
+      </c>
+      <c r="E65" s="216">
+        <v>0</v>
+      </c>
+      <c r="F65" s="216">
+        <v>0</v>
+      </c>
+      <c r="G65" s="216">
+        <v>0</v>
+      </c>
+      <c r="H65" s="216">
+        <v>1</v>
+      </c>
+      <c r="I65" s="216">
+        <v>0</v>
+      </c>
+      <c r="J65" s="216">
+        <v>0</v>
+      </c>
+      <c r="K65" s="216">
+        <v>1</v>
+      </c>
+      <c r="L65" s="216">
+        <v>0</v>
+      </c>
+      <c r="M65" s="216">
+        <v>0</v>
+      </c>
+      <c r="N65" s="216">
         <v>0</v>
       </c>
     </row>
@@ -9929,11 +10070,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K64" sqref="K64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11994,6 +12135,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="15">
+        <v>44046</v>
+      </c>
+      <c r="B65" s="216">
+        <v>0</v>
+      </c>
+      <c r="C65" s="216">
+        <v>0</v>
+      </c>
+      <c r="D65" s="216">
+        <v>0</v>
+      </c>
+      <c r="E65" s="216">
+        <v>0</v>
+      </c>
+      <c r="F65" s="216">
+        <v>2</v>
+      </c>
+      <c r="G65" s="216">
+        <v>1</v>
+      </c>
+      <c r="H65" s="216">
+        <v>1</v>
+      </c>
+      <c r="I65" s="216">
+        <v>1</v>
+      </c>
+      <c r="J65" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12003,8 +12176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BK26" sqref="BK26"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BS5" sqref="BS5:BT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12205,17 +12378,19 @@
       <c r="BL1" s="49">
         <v>44045</v>
       </c>
-      <c r="BM1" s="48"/>
-      <c r="BN1" s="48"/>
-      <c r="BO1" s="48"/>
-      <c r="BP1" s="48"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="48"/>
-      <c r="BS1" s="48"/>
-      <c r="BT1" s="48"/>
-      <c r="BU1" s="48"/>
-      <c r="BV1" s="48"/>
-      <c r="BW1" s="48"/>
+      <c r="BM1" s="49">
+        <v>44046</v>
+      </c>
+      <c r="BN1" s="49"/>
+      <c r="BO1" s="49"/>
+      <c r="BP1" s="49"/>
+      <c r="BQ1" s="49"/>
+      <c r="BR1" s="49"/>
+      <c r="BS1" s="49"/>
+      <c r="BT1" s="49"/>
+      <c r="BU1" s="49"/>
+      <c r="BV1" s="49"/>
+      <c r="BW1" s="49"/>
       <c r="BX1" s="48"/>
       <c r="BY1" s="48"/>
       <c r="BZ1" s="48"/>
@@ -12416,7 +12591,9 @@
       <c r="BL2" s="48">
         <v>4930</v>
       </c>
-      <c r="BM2" s="48"/>
+      <c r="BM2" s="48">
+        <v>4962</v>
+      </c>
       <c r="BN2" s="48"/>
       <c r="BO2" s="48"/>
       <c r="BP2" s="48"/>
@@ -12627,7 +12804,9 @@
       <c r="BL3" s="48">
         <v>4729</v>
       </c>
-      <c r="BM3" s="48"/>
+      <c r="BM3" s="48">
+        <v>4761</v>
+      </c>
       <c r="BN3" s="48"/>
       <c r="BO3" s="48"/>
       <c r="BP3" s="48"/>
@@ -12838,7 +13017,9 @@
       <c r="BL4" s="48">
         <v>4729</v>
       </c>
-      <c r="BM4" s="48"/>
+      <c r="BM4" s="48">
+        <v>4761</v>
+      </c>
       <c r="BN4" s="48"/>
       <c r="BO4" s="48"/>
       <c r="BP4" s="48"/>
@@ -13049,7 +13230,9 @@
       <c r="BL5" s="48">
         <v>4729</v>
       </c>
-      <c r="BM5" s="48"/>
+      <c r="BM5" s="48">
+        <v>4761</v>
+      </c>
       <c r="BN5" s="48"/>
       <c r="BO5" s="48"/>
       <c r="BP5" s="48"/>
@@ -13260,7 +13443,9 @@
       <c r="BL6" s="48">
         <v>4729</v>
       </c>
-      <c r="BM6" s="48"/>
+      <c r="BM6" s="48">
+        <v>4761</v>
+      </c>
       <c r="BN6" s="48"/>
       <c r="BO6" s="48"/>
       <c r="BP6" s="48"/>
@@ -13471,7 +13656,9 @@
       <c r="BL7" s="48">
         <v>4039</v>
       </c>
-      <c r="BM7" s="48"/>
+      <c r="BM7" s="48">
+        <v>4071</v>
+      </c>
       <c r="BN7" s="48"/>
       <c r="BO7" s="48"/>
       <c r="BP7" s="48"/>
@@ -13682,7 +13869,9 @@
       <c r="BL8" s="48">
         <v>6670</v>
       </c>
-      <c r="BM8" s="48"/>
+      <c r="BM8" s="48">
+        <v>6702</v>
+      </c>
       <c r="BN8" s="48"/>
       <c r="BO8" s="48"/>
       <c r="BP8" s="48"/>
@@ -13983,7 +14172,9 @@
       <c r="BL10" s="48">
         <v>203</v>
       </c>
-      <c r="BM10" s="48"/>
+      <c r="BM10" s="48">
+        <v>204</v>
+      </c>
       <c r="BN10" s="48"/>
       <c r="BO10" s="48"/>
       <c r="BP10" s="48"/>
@@ -14194,7 +14385,9 @@
       <c r="BL11" s="48">
         <v>203</v>
       </c>
-      <c r="BM11" s="48"/>
+      <c r="BM11" s="48">
+        <v>204</v>
+      </c>
       <c r="BN11" s="48"/>
       <c r="BO11" s="48"/>
       <c r="BP11" s="48"/>
@@ -14405,7 +14598,9 @@
       <c r="BL12" s="48">
         <v>203</v>
       </c>
-      <c r="BM12" s="48"/>
+      <c r="BM12" s="48">
+        <v>204</v>
+      </c>
       <c r="BN12" s="48"/>
       <c r="BO12" s="48"/>
       <c r="BP12" s="48"/>
@@ -14616,7 +14811,9 @@
       <c r="BL13" s="48">
         <v>203</v>
       </c>
-      <c r="BM13" s="48"/>
+      <c r="BM13" s="48">
+        <v>204</v>
+      </c>
       <c r="BN13" s="48"/>
       <c r="BO13" s="48"/>
       <c r="BP13" s="48"/>
@@ -14827,7 +15024,9 @@
       <c r="BL14" s="48">
         <v>203</v>
       </c>
-      <c r="BM14" s="48"/>
+      <c r="BM14" s="48">
+        <v>204</v>
+      </c>
       <c r="BN14" s="48"/>
       <c r="BO14" s="48"/>
       <c r="BP14" s="48"/>
@@ -15038,7 +15237,9 @@
       <c r="BL15" s="48">
         <v>138</v>
       </c>
-      <c r="BM15" s="48"/>
+      <c r="BM15" s="48">
+        <v>149</v>
+      </c>
       <c r="BN15" s="48"/>
       <c r="BO15" s="48"/>
       <c r="BP15" s="48"/>
@@ -15249,7 +15450,9 @@
       <c r="BL16" s="48">
         <v>215</v>
       </c>
-      <c r="BM16" s="48"/>
+      <c r="BM16" s="48">
+        <v>216</v>
+      </c>
       <c r="BN16" s="48"/>
       <c r="BO16" s="48"/>
       <c r="BP16" s="48"/>
@@ -15546,6 +15749,9 @@
       <c r="BL18" s="216">
         <v>1150</v>
       </c>
+      <c r="BM18" s="216">
+        <v>1157</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -15723,7 +15929,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BL20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BM20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -15809,6 +16015,10 @@
       <c r="BL20" s="51">
         <f t="shared" si="1"/>
         <v>37073</v>
+      </c>
+      <c r="BM20" s="51">
+        <f t="shared" si="1"/>
+        <v>37321</v>
       </c>
     </row>
   </sheetData>
@@ -16108,43 +16318,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="608" t="s">
+      <c r="B8" s="617" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="608"/>
+      <c r="B9" s="617"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="608"/>
+      <c r="B10" s="617"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="608"/>
+      <c r="B11" s="617"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="609" t="s">
+      <c r="B12" s="618" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="609"/>
+      <c r="B13" s="618"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="609"/>
+      <c r="B14" s="618"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="610" t="s">
+      <c r="B15" s="619" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="610"/>
+      <c r="B16" s="619"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 5th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4470627D-77AB-1A47-BE64-311CDC85F93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12106EA1-D79A-8C43-8D12-187F926054CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="629">
+  <cellXfs count="638">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2734,10 +2761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4857,6 +4884,38 @@
         <v>1026294</v>
       </c>
     </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
+        <v>44048</v>
+      </c>
+      <c r="B67" s="626">
+        <v>456100</v>
+      </c>
+      <c r="C67" s="627">
+        <v>499915</v>
+      </c>
+      <c r="D67" s="628">
+        <v>85845</v>
+      </c>
+      <c r="E67" s="629">
+        <v>49698</v>
+      </c>
+      <c r="F67" s="630">
+        <v>26.829642622231965</v>
+      </c>
+      <c r="G67" s="631">
+        <v>122370</v>
+      </c>
+      <c r="H67" s="632">
+        <v>9830</v>
+      </c>
+      <c r="I67" s="633">
+        <v>11770</v>
+      </c>
+      <c r="J67" s="634">
+        <v>1041860</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4864,11 +4923,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L66"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60:A66"/>
+      <selection pane="bottomLeft" activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7335,6 +7394,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
+        <v>44048</v>
+      </c>
+      <c r="B67" s="216">
+        <v>0</v>
+      </c>
+      <c r="C67" s="216">
+        <v>1</v>
+      </c>
+      <c r="D67" s="216">
+        <v>0</v>
+      </c>
+      <c r="E67" s="216">
+        <v>0</v>
+      </c>
+      <c r="F67" s="216">
+        <v>1</v>
+      </c>
+      <c r="G67" s="216">
+        <v>0</v>
+      </c>
+      <c r="H67" s="216">
+        <v>0</v>
+      </c>
+      <c r="I67" s="216">
+        <v>0</v>
+      </c>
+      <c r="J67" s="216">
+        <v>0</v>
+      </c>
+      <c r="K67" s="216">
+        <v>0</v>
+      </c>
+      <c r="L67" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7342,11 +7439,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10201,6 +10298,50 @@
         <v>0</v>
       </c>
       <c r="N66" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
+        <v>44048</v>
+      </c>
+      <c r="B67" s="216">
+        <v>0</v>
+      </c>
+      <c r="C67" s="216">
+        <v>1</v>
+      </c>
+      <c r="D67" s="216">
+        <v>0</v>
+      </c>
+      <c r="E67" s="216">
+        <v>0</v>
+      </c>
+      <c r="F67" s="216">
+        <v>0</v>
+      </c>
+      <c r="G67" s="216">
+        <v>0</v>
+      </c>
+      <c r="H67" s="216">
+        <v>1</v>
+      </c>
+      <c r="I67" s="216">
+        <v>0</v>
+      </c>
+      <c r="J67" s="216">
+        <v>0</v>
+      </c>
+      <c r="K67" s="216">
+        <v>1</v>
+      </c>
+      <c r="L67" s="216">
+        <v>0</v>
+      </c>
+      <c r="M67" s="216">
+        <v>0</v>
+      </c>
+      <c r="N67" s="216">
         <v>0</v>
       </c>
     </row>
@@ -10211,11 +10352,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12340,6 +12481,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="15">
+        <v>44048</v>
+      </c>
+      <c r="B67" s="216">
+        <v>0</v>
+      </c>
+      <c r="C67" s="216">
+        <v>0</v>
+      </c>
+      <c r="D67" s="216">
+        <v>0</v>
+      </c>
+      <c r="E67" s="216">
+        <v>0</v>
+      </c>
+      <c r="F67" s="216">
+        <v>2</v>
+      </c>
+      <c r="G67" s="216">
+        <v>1</v>
+      </c>
+      <c r="H67" s="216">
+        <v>1</v>
+      </c>
+      <c r="I67" s="216">
+        <v>1</v>
+      </c>
+      <c r="J67" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12349,8 +12522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BO23" sqref="BO23"/>
+    <sheetView topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BJ20" sqref="BJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12557,7 +12730,9 @@
       <c r="BN1" s="49">
         <v>44047</v>
       </c>
-      <c r="BO1" s="49"/>
+      <c r="BO1" s="49">
+        <v>44048</v>
+      </c>
       <c r="BP1" s="49"/>
       <c r="BQ1" s="49"/>
       <c r="BR1" s="49"/>
@@ -12772,7 +12947,9 @@
       <c r="BN2" s="48">
         <v>4994</v>
       </c>
-      <c r="BO2" s="48"/>
+      <c r="BO2" s="48">
+        <v>5026</v>
+      </c>
       <c r="BP2" s="48"/>
       <c r="BQ2" s="48"/>
       <c r="BR2" s="48"/>
@@ -12987,7 +13164,9 @@
       <c r="BN3" s="48">
         <v>4793</v>
       </c>
-      <c r="BO3" s="48"/>
+      <c r="BO3" s="48">
+        <v>4825</v>
+      </c>
       <c r="BP3" s="48"/>
       <c r="BQ3" s="48"/>
       <c r="BR3" s="48"/>
@@ -13202,7 +13381,9 @@
       <c r="BN4" s="48">
         <v>4793</v>
       </c>
-      <c r="BO4" s="48"/>
+      <c r="BO4" s="48">
+        <v>4825</v>
+      </c>
       <c r="BP4" s="48"/>
       <c r="BQ4" s="48"/>
       <c r="BR4" s="48"/>
@@ -13417,7 +13598,9 @@
       <c r="BN5" s="48">
         <v>4793</v>
       </c>
-      <c r="BO5" s="48"/>
+      <c r="BO5" s="48">
+        <v>4825</v>
+      </c>
       <c r="BP5" s="48"/>
       <c r="BQ5" s="48"/>
       <c r="BR5" s="48"/>
@@ -13632,7 +13815,9 @@
       <c r="BN6" s="48">
         <v>4793</v>
       </c>
-      <c r="BO6" s="48"/>
+      <c r="BO6" s="48">
+        <v>4825</v>
+      </c>
       <c r="BP6" s="48"/>
       <c r="BQ6" s="48"/>
       <c r="BR6" s="48"/>
@@ -13847,7 +14032,9 @@
       <c r="BN7" s="48">
         <v>4103</v>
       </c>
-      <c r="BO7" s="48"/>
+      <c r="BO7" s="48">
+        <v>4135</v>
+      </c>
       <c r="BP7" s="48"/>
       <c r="BQ7" s="48"/>
       <c r="BR7" s="48"/>
@@ -14062,7 +14249,9 @@
       <c r="BN8" s="48">
         <v>6734</v>
       </c>
-      <c r="BO8" s="48"/>
+      <c r="BO8" s="48">
+        <v>6766</v>
+      </c>
       <c r="BP8" s="48"/>
       <c r="BQ8" s="48"/>
       <c r="BR8" s="48"/>
@@ -14367,7 +14556,9 @@
       <c r="BN10" s="48">
         <v>205</v>
       </c>
-      <c r="BO10" s="48"/>
+      <c r="BO10" s="48">
+        <v>206</v>
+      </c>
       <c r="BP10" s="48"/>
       <c r="BQ10" s="48"/>
       <c r="BR10" s="48"/>
@@ -14582,7 +14773,9 @@
       <c r="BN11" s="48">
         <v>205</v>
       </c>
-      <c r="BO11" s="48"/>
+      <c r="BO11" s="48">
+        <v>206</v>
+      </c>
       <c r="BP11" s="48"/>
       <c r="BQ11" s="48"/>
       <c r="BR11" s="48"/>
@@ -14797,7 +14990,9 @@
       <c r="BN12" s="48">
         <v>205</v>
       </c>
-      <c r="BO12" s="48"/>
+      <c r="BO12" s="48">
+        <v>206</v>
+      </c>
       <c r="BP12" s="48"/>
       <c r="BQ12" s="48"/>
       <c r="BR12" s="48"/>
@@ -15012,7 +15207,9 @@
       <c r="BN13" s="48">
         <v>205</v>
       </c>
-      <c r="BO13" s="48"/>
+      <c r="BO13" s="48">
+        <v>206</v>
+      </c>
       <c r="BP13" s="48"/>
       <c r="BQ13" s="48"/>
       <c r="BR13" s="48"/>
@@ -15227,7 +15424,9 @@
       <c r="BN14" s="48">
         <v>205</v>
       </c>
-      <c r="BO14" s="48"/>
+      <c r="BO14" s="48">
+        <v>206</v>
+      </c>
       <c r="BP14" s="48"/>
       <c r="BQ14" s="48"/>
       <c r="BR14" s="48"/>
@@ -15442,7 +15641,9 @@
       <c r="BN15" s="48">
         <v>140</v>
       </c>
-      <c r="BO15" s="48"/>
+      <c r="BO15" s="48">
+        <v>141</v>
+      </c>
       <c r="BP15" s="48"/>
       <c r="BQ15" s="48"/>
       <c r="BR15" s="48"/>
@@ -15657,7 +15858,9 @@
       <c r="BN16" s="48">
         <v>217</v>
       </c>
-      <c r="BO16" s="48"/>
+      <c r="BO16" s="48">
+        <v>218</v>
+      </c>
       <c r="BP16" s="48"/>
       <c r="BQ16" s="48"/>
       <c r="BR16" s="48"/>
@@ -15958,6 +16161,9 @@
       <c r="BN18">
         <v>1164</v>
       </c>
+      <c r="BO18">
+        <v>1171</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -16135,7 +16341,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BN20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BO20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -16229,6 +16435,10 @@
       <c r="BN20" s="51">
         <f t="shared" si="1"/>
         <v>37549</v>
+      </c>
+      <c r="BO20" s="51">
+        <f t="shared" si="1"/>
+        <v>37787</v>
       </c>
     </row>
   </sheetData>
@@ -16445,8 +16655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16528,43 +16738,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="626" t="s">
+      <c r="B8" s="635" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="626"/>
+      <c r="B9" s="635"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="626"/>
+      <c r="B10" s="635"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="626"/>
+      <c r="B11" s="635"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="627" t="s">
+      <c r="B12" s="636" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="627"/>
+      <c r="B13" s="636"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="627"/>
+      <c r="B14" s="636"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="628" t="s">
+      <c r="B15" s="637" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="628"/>
+      <c r="B16" s="637"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 6th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12106EA1-D79A-8C43-8D12-187F926054CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B0435-01AF-3444-8AAF-4CF52F62FE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="638">
+  <cellXfs count="647">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2761,10 +2788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4916,6 +4943,38 @@
         <v>1041860</v>
       </c>
     </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="15">
+        <v>44049</v>
+      </c>
+      <c r="B68" s="635">
+        <v>462690</v>
+      </c>
+      <c r="C68" s="636">
+        <v>506252</v>
+      </c>
+      <c r="D68" s="637">
+        <v>87973</v>
+      </c>
+      <c r="E68" s="638">
+        <v>50517</v>
+      </c>
+      <c r="F68" s="639">
+        <v>26.799152780479368</v>
+      </c>
+      <c r="G68" s="640">
+        <v>123997</v>
+      </c>
+      <c r="H68" s="641">
+        <v>9935</v>
+      </c>
+      <c r="I68" s="642">
+        <v>11928</v>
+      </c>
+      <c r="J68" s="643">
+        <v>1056915</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4923,11 +4982,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M67" sqref="M67"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7395,7 +7454,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="15">
+      <c r="A67" s="217">
         <v>44048</v>
       </c>
       <c r="B67" s="216">
@@ -7429,6 +7488,44 @@
         <v>0</v>
       </c>
       <c r="L67" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="217">
+        <v>44049</v>
+      </c>
+      <c r="B68" s="216">
+        <v>0</v>
+      </c>
+      <c r="C68" s="216">
+        <v>1</v>
+      </c>
+      <c r="D68" s="216">
+        <v>0</v>
+      </c>
+      <c r="E68" s="216">
+        <v>0</v>
+      </c>
+      <c r="F68" s="216">
+        <v>1</v>
+      </c>
+      <c r="G68" s="216">
+        <v>0</v>
+      </c>
+      <c r="H68" s="216">
+        <v>0</v>
+      </c>
+      <c r="I68" s="216">
+        <v>0</v>
+      </c>
+      <c r="J68" s="216">
+        <v>0</v>
+      </c>
+      <c r="K68" s="216">
+        <v>0</v>
+      </c>
+      <c r="L68" s="216">
         <v>4</v>
       </c>
     </row>
@@ -7439,11 +7536,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O67" sqref="O67"/>
+      <selection pane="bottomLeft" activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10302,7 +10399,7 @@
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A67" s="15">
+      <c r="A67" s="217">
         <v>44048</v>
       </c>
       <c r="B67" s="216">
@@ -10342,6 +10439,50 @@
         <v>0</v>
       </c>
       <c r="N67" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="217">
+        <v>44049</v>
+      </c>
+      <c r="B68" s="216">
+        <v>0</v>
+      </c>
+      <c r="C68" s="216">
+        <v>1</v>
+      </c>
+      <c r="D68" s="216">
+        <v>0</v>
+      </c>
+      <c r="E68" s="216">
+        <v>0</v>
+      </c>
+      <c r="F68" s="216">
+        <v>0</v>
+      </c>
+      <c r="G68" s="216">
+        <v>0</v>
+      </c>
+      <c r="H68" s="216">
+        <v>1</v>
+      </c>
+      <c r="I68" s="216">
+        <v>0</v>
+      </c>
+      <c r="J68" s="216">
+        <v>0</v>
+      </c>
+      <c r="K68" s="216">
+        <v>1</v>
+      </c>
+      <c r="L68" s="216">
+        <v>0</v>
+      </c>
+      <c r="M68" s="216">
+        <v>0</v>
+      </c>
+      <c r="N68" s="216">
         <v>0</v>
       </c>
     </row>
@@ -10352,11 +10493,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12513,6 +12654,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="15">
+        <v>44049</v>
+      </c>
+      <c r="B68" s="216">
+        <v>0</v>
+      </c>
+      <c r="C68" s="216">
+        <v>0</v>
+      </c>
+      <c r="D68" s="216">
+        <v>0</v>
+      </c>
+      <c r="E68" s="216">
+        <v>0</v>
+      </c>
+      <c r="F68" s="216">
+        <v>2</v>
+      </c>
+      <c r="G68" s="216">
+        <v>1</v>
+      </c>
+      <c r="H68" s="216">
+        <v>1</v>
+      </c>
+      <c r="I68" s="216">
+        <v>1</v>
+      </c>
+      <c r="J68" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12523,7 +12696,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BJ20" sqref="BJ20"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12733,7 +12906,9 @@
       <c r="BO1" s="49">
         <v>44048</v>
       </c>
-      <c r="BP1" s="49"/>
+      <c r="BP1" s="49">
+        <v>44049</v>
+      </c>
       <c r="BQ1" s="49"/>
       <c r="BR1" s="49"/>
       <c r="BS1" s="49"/>
@@ -12950,7 +13125,9 @@
       <c r="BO2" s="48">
         <v>5026</v>
       </c>
-      <c r="BP2" s="48"/>
+      <c r="BP2" s="48">
+        <v>5058</v>
+      </c>
       <c r="BQ2" s="48"/>
       <c r="BR2" s="48"/>
       <c r="BS2" s="48"/>
@@ -13167,7 +13344,9 @@
       <c r="BO3" s="48">
         <v>4825</v>
       </c>
-      <c r="BP3" s="48"/>
+      <c r="BP3" s="48">
+        <v>4857</v>
+      </c>
       <c r="BQ3" s="48"/>
       <c r="BR3" s="48"/>
       <c r="BS3" s="48"/>
@@ -13384,7 +13563,9 @@
       <c r="BO4" s="48">
         <v>4825</v>
       </c>
-      <c r="BP4" s="48"/>
+      <c r="BP4" s="48">
+        <v>4857</v>
+      </c>
       <c r="BQ4" s="48"/>
       <c r="BR4" s="48"/>
       <c r="BS4" s="48"/>
@@ -13601,7 +13782,9 @@
       <c r="BO5" s="48">
         <v>4825</v>
       </c>
-      <c r="BP5" s="48"/>
+      <c r="BP5" s="48">
+        <v>4857</v>
+      </c>
       <c r="BQ5" s="48"/>
       <c r="BR5" s="48"/>
       <c r="BS5" s="48"/>
@@ -13818,7 +14001,9 @@
       <c r="BO6" s="48">
         <v>4825</v>
       </c>
-      <c r="BP6" s="48"/>
+      <c r="BP6" s="48">
+        <v>4857</v>
+      </c>
       <c r="BQ6" s="48"/>
       <c r="BR6" s="48"/>
       <c r="BS6" s="48"/>
@@ -14035,7 +14220,9 @@
       <c r="BO7" s="48">
         <v>4135</v>
       </c>
-      <c r="BP7" s="48"/>
+      <c r="BP7" s="48">
+        <v>4167</v>
+      </c>
       <c r="BQ7" s="48"/>
       <c r="BR7" s="48"/>
       <c r="BS7" s="48"/>
@@ -14252,7 +14439,9 @@
       <c r="BO8" s="48">
         <v>6766</v>
       </c>
-      <c r="BP8" s="48"/>
+      <c r="BP8" s="48">
+        <v>6798</v>
+      </c>
       <c r="BQ8" s="48"/>
       <c r="BR8" s="48"/>
       <c r="BS8" s="48"/>
@@ -14559,7 +14748,9 @@
       <c r="BO10" s="48">
         <v>206</v>
       </c>
-      <c r="BP10" s="48"/>
+      <c r="BP10" s="48">
+        <v>207</v>
+      </c>
       <c r="BQ10" s="48"/>
       <c r="BR10" s="48"/>
       <c r="BS10" s="48"/>
@@ -14776,7 +14967,9 @@
       <c r="BO11" s="48">
         <v>206</v>
       </c>
-      <c r="BP11" s="48"/>
+      <c r="BP11" s="48">
+        <v>207</v>
+      </c>
       <c r="BQ11" s="48"/>
       <c r="BR11" s="48"/>
       <c r="BS11" s="48"/>
@@ -14993,7 +15186,9 @@
       <c r="BO12" s="48">
         <v>206</v>
       </c>
-      <c r="BP12" s="48"/>
+      <c r="BP12" s="48">
+        <v>207</v>
+      </c>
       <c r="BQ12" s="48"/>
       <c r="BR12" s="48"/>
       <c r="BS12" s="48"/>
@@ -15210,7 +15405,9 @@
       <c r="BO13" s="48">
         <v>206</v>
       </c>
-      <c r="BP13" s="48"/>
+      <c r="BP13" s="48">
+        <v>207</v>
+      </c>
       <c r="BQ13" s="48"/>
       <c r="BR13" s="48"/>
       <c r="BS13" s="48"/>
@@ -15427,7 +15624,9 @@
       <c r="BO14" s="48">
         <v>206</v>
       </c>
-      <c r="BP14" s="48"/>
+      <c r="BP14" s="48">
+        <v>207</v>
+      </c>
       <c r="BQ14" s="48"/>
       <c r="BR14" s="48"/>
       <c r="BS14" s="48"/>
@@ -15644,7 +15843,9 @@
       <c r="BO15" s="48">
         <v>141</v>
       </c>
-      <c r="BP15" s="48"/>
+      <c r="BP15" s="48">
+        <v>142</v>
+      </c>
       <c r="BQ15" s="48"/>
       <c r="BR15" s="48"/>
       <c r="BS15" s="48"/>
@@ -15861,7 +16062,9 @@
       <c r="BO16" s="48">
         <v>218</v>
       </c>
-      <c r="BP16" s="48"/>
+      <c r="BP16" s="48">
+        <v>219</v>
+      </c>
       <c r="BQ16" s="48"/>
       <c r="BR16" s="48"/>
       <c r="BS16" s="48"/>
@@ -16164,6 +16367,9 @@
       <c r="BO18">
         <v>1171</v>
       </c>
+      <c r="BP18" s="216">
+        <v>1178</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -16341,7 +16547,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BO20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BP20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -16439,6 +16645,10 @@
       <c r="BO20" s="51">
         <f t="shared" si="1"/>
         <v>37787</v>
+      </c>
+      <c r="BP20" s="51">
+        <f t="shared" si="1"/>
+        <v>38025</v>
       </c>
     </row>
   </sheetData>
@@ -16451,7 +16661,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16655,7 +16865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -16738,43 +16948,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="635" t="s">
+      <c r="B8" s="644" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="635"/>
+      <c r="B9" s="644"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="635"/>
+      <c r="B10" s="644"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="635"/>
+      <c r="B11" s="644"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="636" t="s">
+      <c r="B12" s="645" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="636"/>
+      <c r="B13" s="645"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="636"/>
+      <c r="B14" s="645"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="637" t="s">
+      <c r="B15" s="646" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="637"/>
+      <c r="B16" s="646"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and clean data from SSA for August 8th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16B0435-01AF-3444-8AAF-4CF52F62FE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12273E8-935C-CC4E-960B-103006BB8E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="647">
+  <cellXfs count="665">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2788,10 +2842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4975,6 +5029,70 @@
         <v>1056915</v>
       </c>
     </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="15">
+        <v>44050</v>
+      </c>
+      <c r="B69" s="644">
+        <v>469407</v>
+      </c>
+      <c r="C69" s="645">
+        <v>513144</v>
+      </c>
+      <c r="D69" s="646">
+        <v>89155</v>
+      </c>
+      <c r="E69" s="647">
+        <v>51311</v>
+      </c>
+      <c r="F69" s="648">
+        <v>26.742890498011317</v>
+      </c>
+      <c r="G69" s="649">
+        <v>125533</v>
+      </c>
+      <c r="H69" s="650">
+        <v>10049</v>
+      </c>
+      <c r="I69" s="651">
+        <v>12104</v>
+      </c>
+      <c r="J69" s="652">
+        <v>1071706</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="15">
+        <v>44051</v>
+      </c>
+      <c r="B70" s="653">
+        <v>475902</v>
+      </c>
+      <c r="C70" s="654">
+        <v>520970</v>
+      </c>
+      <c r="D70" s="655">
+        <v>89025</v>
+      </c>
+      <c r="E70" s="656">
+        <v>52006</v>
+      </c>
+      <c r="F70" s="657">
+        <v>26.671247441700181</v>
+      </c>
+      <c r="G70" s="658">
+        <v>126929</v>
+      </c>
+      <c r="H70" s="659">
+        <v>10141</v>
+      </c>
+      <c r="I70" s="660">
+        <v>12213</v>
+      </c>
+      <c r="J70" s="661">
+        <v>1085897</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4982,11 +5100,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66:A68"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7529,6 +7647,85 @@
         <v>4</v>
       </c>
     </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="217">
+        <v>44050</v>
+      </c>
+      <c r="B69" s="216">
+        <v>0</v>
+      </c>
+      <c r="C69" s="216">
+        <v>1</v>
+      </c>
+      <c r="D69" s="216">
+        <v>0</v>
+      </c>
+      <c r="E69" s="216">
+        <v>0</v>
+      </c>
+      <c r="F69" s="216">
+        <v>1</v>
+      </c>
+      <c r="G69" s="216">
+        <v>0</v>
+      </c>
+      <c r="H69" s="216">
+        <v>0</v>
+      </c>
+      <c r="I69" s="216">
+        <v>0</v>
+      </c>
+      <c r="J69" s="216">
+        <v>0</v>
+      </c>
+      <c r="K69" s="216">
+        <v>0</v>
+      </c>
+      <c r="L69" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="217">
+        <v>44051</v>
+      </c>
+      <c r="B70" s="216">
+        <v>0</v>
+      </c>
+      <c r="C70" s="216">
+        <v>1</v>
+      </c>
+      <c r="D70" s="216">
+        <v>0</v>
+      </c>
+      <c r="E70" s="216">
+        <v>0</v>
+      </c>
+      <c r="F70" s="216">
+        <v>1</v>
+      </c>
+      <c r="G70" s="216">
+        <v>0</v>
+      </c>
+      <c r="H70" s="216">
+        <v>0</v>
+      </c>
+      <c r="I70" s="216">
+        <v>0</v>
+      </c>
+      <c r="J70" s="216">
+        <v>0</v>
+      </c>
+      <c r="K70" s="216">
+        <v>0</v>
+      </c>
+      <c r="L70" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="217"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7536,11 +7733,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O68" sqref="O68"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10485,6 +10682,97 @@
       <c r="N68" s="216">
         <v>0</v>
       </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="217">
+        <v>44050</v>
+      </c>
+      <c r="B69" s="216">
+        <v>0</v>
+      </c>
+      <c r="C69" s="216">
+        <v>1</v>
+      </c>
+      <c r="D69" s="550">
+        <v>0</v>
+      </c>
+      <c r="E69" s="216">
+        <v>0</v>
+      </c>
+      <c r="F69" s="216">
+        <v>0</v>
+      </c>
+      <c r="G69" s="216">
+        <v>0</v>
+      </c>
+      <c r="H69" s="216">
+        <v>1</v>
+      </c>
+      <c r="I69" s="216">
+        <v>0</v>
+      </c>
+      <c r="J69" s="216">
+        <v>0</v>
+      </c>
+      <c r="K69" s="216">
+        <v>1</v>
+      </c>
+      <c r="L69" s="216">
+        <v>0</v>
+      </c>
+      <c r="M69" s="216">
+        <v>0</v>
+      </c>
+      <c r="N69" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="217">
+        <v>44051</v>
+      </c>
+      <c r="B70" s="216">
+        <v>0</v>
+      </c>
+      <c r="C70" s="216">
+        <v>1</v>
+      </c>
+      <c r="D70" s="216">
+        <v>0</v>
+      </c>
+      <c r="E70" s="216">
+        <v>0</v>
+      </c>
+      <c r="F70" s="216">
+        <v>0</v>
+      </c>
+      <c r="G70" s="216">
+        <v>0</v>
+      </c>
+      <c r="H70" s="216">
+        <v>1</v>
+      </c>
+      <c r="I70" s="216">
+        <v>0</v>
+      </c>
+      <c r="J70" s="216">
+        <v>0</v>
+      </c>
+      <c r="K70" s="216">
+        <v>1</v>
+      </c>
+      <c r="L70" s="216">
+        <v>0</v>
+      </c>
+      <c r="M70" s="216">
+        <v>0</v>
+      </c>
+      <c r="N70" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10493,11 +10781,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12623,7 +12911,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="15">
+      <c r="A67" s="495">
         <v>44048</v>
       </c>
       <c r="B67" s="216">
@@ -12655,7 +12943,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="15">
+      <c r="A68" s="495">
         <v>44049</v>
       </c>
       <c r="B68" s="216">
@@ -12683,6 +12971,70 @@
         <v>1</v>
       </c>
       <c r="J68" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="495">
+        <v>44050</v>
+      </c>
+      <c r="B69" s="216">
+        <v>0</v>
+      </c>
+      <c r="C69" s="216">
+        <v>0</v>
+      </c>
+      <c r="D69" s="216">
+        <v>0</v>
+      </c>
+      <c r="E69" s="216">
+        <v>0</v>
+      </c>
+      <c r="F69" s="216">
+        <v>2</v>
+      </c>
+      <c r="G69" s="216">
+        <v>1</v>
+      </c>
+      <c r="H69" s="216">
+        <v>1</v>
+      </c>
+      <c r="I69" s="216">
+        <v>1</v>
+      </c>
+      <c r="J69" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="495">
+        <v>44051</v>
+      </c>
+      <c r="B70" s="216">
+        <v>0</v>
+      </c>
+      <c r="C70" s="216">
+        <v>0</v>
+      </c>
+      <c r="D70" s="216">
+        <v>0</v>
+      </c>
+      <c r="E70" s="216">
+        <v>0</v>
+      </c>
+      <c r="F70" s="216">
+        <v>2</v>
+      </c>
+      <c r="G70" s="216">
+        <v>1</v>
+      </c>
+      <c r="H70" s="216">
+        <v>1</v>
+      </c>
+      <c r="I70" s="216">
+        <v>1</v>
+      </c>
+      <c r="J70" s="216">
         <v>2</v>
       </c>
     </row>
@@ -12695,8 +13047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BU4" sqref="BU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12909,8 +13261,12 @@
       <c r="BP1" s="49">
         <v>44049</v>
       </c>
-      <c r="BQ1" s="49"/>
-      <c r="BR1" s="49"/>
+      <c r="BQ1" s="49">
+        <v>44050</v>
+      </c>
+      <c r="BR1" s="49">
+        <v>44051</v>
+      </c>
       <c r="BS1" s="49"/>
       <c r="BT1" s="49"/>
       <c r="BU1" s="49"/>
@@ -13128,8 +13484,12 @@
       <c r="BP2" s="48">
         <v>5058</v>
       </c>
-      <c r="BQ2" s="48"/>
-      <c r="BR2" s="48"/>
+      <c r="BQ2" s="48">
+        <v>5090</v>
+      </c>
+      <c r="BR2" s="48">
+        <v>5122</v>
+      </c>
       <c r="BS2" s="48"/>
       <c r="BT2" s="48"/>
       <c r="BU2" s="48"/>
@@ -13347,8 +13707,12 @@
       <c r="BP3" s="48">
         <v>4857</v>
       </c>
-      <c r="BQ3" s="48"/>
-      <c r="BR3" s="48"/>
+      <c r="BQ3" s="48">
+        <v>4889</v>
+      </c>
+      <c r="BR3" s="48">
+        <v>4921</v>
+      </c>
       <c r="BS3" s="48"/>
       <c r="BT3" s="48"/>
       <c r="BU3" s="48"/>
@@ -13566,8 +13930,12 @@
       <c r="BP4" s="48">
         <v>4857</v>
       </c>
-      <c r="BQ4" s="48"/>
-      <c r="BR4" s="48"/>
+      <c r="BQ4" s="48">
+        <v>4889</v>
+      </c>
+      <c r="BR4" s="48">
+        <v>4921</v>
+      </c>
       <c r="BS4" s="48"/>
       <c r="BT4" s="48"/>
       <c r="BU4" s="48"/>
@@ -13785,8 +14153,12 @@
       <c r="BP5" s="48">
         <v>4857</v>
       </c>
-      <c r="BQ5" s="48"/>
-      <c r="BR5" s="48"/>
+      <c r="BQ5" s="48">
+        <v>4889</v>
+      </c>
+      <c r="BR5" s="48">
+        <v>4921</v>
+      </c>
       <c r="BS5" s="48"/>
       <c r="BT5" s="48"/>
       <c r="BU5" s="48"/>
@@ -14004,8 +14376,12 @@
       <c r="BP6" s="48">
         <v>4857</v>
       </c>
-      <c r="BQ6" s="48"/>
-      <c r="BR6" s="48"/>
+      <c r="BQ6" s="48">
+        <v>4889</v>
+      </c>
+      <c r="BR6" s="48">
+        <v>4921</v>
+      </c>
       <c r="BS6" s="48"/>
       <c r="BT6" s="48"/>
       <c r="BU6" s="48"/>
@@ -14223,8 +14599,12 @@
       <c r="BP7" s="48">
         <v>4167</v>
       </c>
-      <c r="BQ7" s="48"/>
-      <c r="BR7" s="48"/>
+      <c r="BQ7" s="48">
+        <v>4199</v>
+      </c>
+      <c r="BR7" s="48">
+        <v>4231</v>
+      </c>
       <c r="BS7" s="48"/>
       <c r="BT7" s="48"/>
       <c r="BU7" s="48"/>
@@ -14442,8 +14822,12 @@
       <c r="BP8" s="48">
         <v>6798</v>
       </c>
-      <c r="BQ8" s="48"/>
-      <c r="BR8" s="48"/>
+      <c r="BQ8" s="48">
+        <v>6830</v>
+      </c>
+      <c r="BR8" s="48">
+        <v>6862</v>
+      </c>
       <c r="BS8" s="48"/>
       <c r="BT8" s="48"/>
       <c r="BU8" s="48"/>
@@ -14751,8 +15135,12 @@
       <c r="BP10" s="48">
         <v>207</v>
       </c>
-      <c r="BQ10" s="48"/>
-      <c r="BR10" s="48"/>
+      <c r="BQ10" s="48">
+        <v>208</v>
+      </c>
+      <c r="BR10" s="48">
+        <v>209</v>
+      </c>
       <c r="BS10" s="48"/>
       <c r="BT10" s="48"/>
       <c r="BU10" s="48"/>
@@ -14970,8 +15358,12 @@
       <c r="BP11" s="48">
         <v>207</v>
       </c>
-      <c r="BQ11" s="48"/>
-      <c r="BR11" s="48"/>
+      <c r="BQ11" s="48">
+        <v>208</v>
+      </c>
+      <c r="BR11" s="48">
+        <v>209</v>
+      </c>
       <c r="BS11" s="48"/>
       <c r="BT11" s="48"/>
       <c r="BU11" s="48"/>
@@ -15189,8 +15581,12 @@
       <c r="BP12" s="48">
         <v>207</v>
       </c>
-      <c r="BQ12" s="48"/>
-      <c r="BR12" s="48"/>
+      <c r="BQ12" s="48">
+        <v>208</v>
+      </c>
+      <c r="BR12" s="48">
+        <v>209</v>
+      </c>
       <c r="BS12" s="48"/>
       <c r="BT12" s="48"/>
       <c r="BU12" s="48"/>
@@ -15408,8 +15804,12 @@
       <c r="BP13" s="48">
         <v>207</v>
       </c>
-      <c r="BQ13" s="48"/>
-      <c r="BR13" s="48"/>
+      <c r="BQ13" s="48">
+        <v>208</v>
+      </c>
+      <c r="BR13" s="48">
+        <v>209</v>
+      </c>
       <c r="BS13" s="48"/>
       <c r="BT13" s="48"/>
       <c r="BU13" s="48"/>
@@ -15627,8 +16027,12 @@
       <c r="BP14" s="48">
         <v>207</v>
       </c>
-      <c r="BQ14" s="48"/>
-      <c r="BR14" s="48"/>
+      <c r="BQ14" s="48">
+        <v>208</v>
+      </c>
+      <c r="BR14" s="48">
+        <v>209</v>
+      </c>
       <c r="BS14" s="48"/>
       <c r="BT14" s="48"/>
       <c r="BU14" s="48"/>
@@ -15846,8 +16250,12 @@
       <c r="BP15" s="48">
         <v>142</v>
       </c>
-      <c r="BQ15" s="48"/>
-      <c r="BR15" s="48"/>
+      <c r="BQ15" s="48">
+        <v>143</v>
+      </c>
+      <c r="BR15" s="48">
+        <v>144</v>
+      </c>
       <c r="BS15" s="48"/>
       <c r="BT15" s="48"/>
       <c r="BU15" s="48"/>
@@ -16065,8 +16473,12 @@
       <c r="BP16" s="48">
         <v>219</v>
       </c>
-      <c r="BQ16" s="48"/>
-      <c r="BR16" s="48"/>
+      <c r="BQ16" s="48">
+        <v>220</v>
+      </c>
+      <c r="BR16" s="48">
+        <v>221</v>
+      </c>
       <c r="BS16" s="48"/>
       <c r="BT16" s="48"/>
       <c r="BU16" s="48"/>
@@ -16370,6 +16782,12 @@
       <c r="BP18" s="216">
         <v>1178</v>
       </c>
+      <c r="BQ18">
+        <v>1185</v>
+      </c>
+      <c r="BR18" s="216">
+        <v>1192</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -16547,7 +16965,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BP20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BR20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -16649,6 +17067,14 @@
       <c r="BP20" s="51">
         <f t="shared" si="1"/>
         <v>38025</v>
+      </c>
+      <c r="BQ20" s="51">
+        <f t="shared" si="1"/>
+        <v>38263</v>
+      </c>
+      <c r="BR20" s="51">
+        <f t="shared" si="1"/>
+        <v>38501</v>
       </c>
     </row>
   </sheetData>
@@ -16661,7 +17087,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16865,8 +17291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16948,43 +17374,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="644" t="s">
+      <c r="B8" s="662" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="644"/>
+      <c r="B9" s="662"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="644"/>
+      <c r="B10" s="662"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="644"/>
+      <c r="B11" s="662"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="645" t="s">
+      <c r="B12" s="663" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="645"/>
+      <c r="B13" s="663"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="645"/>
+      <c r="B14" s="663"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="646" t="s">
+      <c r="B15" s="664" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="646"/>
+      <c r="B16" s="664"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 9th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12273E8-935C-CC4E-960B-103006BB8E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E084A9-2450-0243-A1AE-C0158B2263A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="665">
+  <cellXfs count="674">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2842,10 +2869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5091,6 +5118,38 @@
       </c>
       <c r="J70" s="661">
         <v>1085897</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="15">
+        <v>44052</v>
+      </c>
+      <c r="B71" s="662">
+        <v>480278</v>
+      </c>
+      <c r="C71" s="663">
+        <v>526911</v>
+      </c>
+      <c r="D71" s="664">
+        <v>84506</v>
+      </c>
+      <c r="E71" s="665">
+        <v>52298</v>
+      </c>
+      <c r="F71" s="666">
+        <v>26.612087166182917</v>
+      </c>
+      <c r="G71" s="667">
+        <v>127812</v>
+      </c>
+      <c r="H71" s="668">
+        <v>10212</v>
+      </c>
+      <c r="I71" s="669">
+        <v>12288</v>
+      </c>
+      <c r="J71" s="670">
+        <v>1091695</v>
       </c>
     </row>
   </sheetData>
@@ -5104,7 +5163,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69:A71"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7724,7 +7783,42 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="217"/>
+      <c r="A71" s="15">
+        <v>44052</v>
+      </c>
+      <c r="B71" s="216">
+        <v>0</v>
+      </c>
+      <c r="C71" s="216">
+        <v>1</v>
+      </c>
+      <c r="D71" s="216">
+        <v>0</v>
+      </c>
+      <c r="E71" s="216">
+        <v>0</v>
+      </c>
+      <c r="F71" s="216">
+        <v>1</v>
+      </c>
+      <c r="G71" s="216">
+        <v>0</v>
+      </c>
+      <c r="H71" s="216">
+        <v>0</v>
+      </c>
+      <c r="I71" s="216">
+        <v>0</v>
+      </c>
+      <c r="J71" s="216">
+        <v>0</v>
+      </c>
+      <c r="K71" s="216">
+        <v>0</v>
+      </c>
+      <c r="L71" s="216">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7737,7 +7831,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69:A71"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10772,7 +10866,48 @@
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A71" s="217"/>
+      <c r="A71" s="15">
+        <v>44052</v>
+      </c>
+      <c r="B71" s="216">
+        <v>0</v>
+      </c>
+      <c r="C71" s="216">
+        <v>1</v>
+      </c>
+      <c r="D71" s="216">
+        <v>0</v>
+      </c>
+      <c r="E71" s="216">
+        <v>0</v>
+      </c>
+      <c r="F71" s="216">
+        <v>0</v>
+      </c>
+      <c r="G71" s="216">
+        <v>0</v>
+      </c>
+      <c r="H71" s="216">
+        <v>1</v>
+      </c>
+      <c r="I71" s="216">
+        <v>0</v>
+      </c>
+      <c r="J71" s="216">
+        <v>0</v>
+      </c>
+      <c r="K71" s="216">
+        <v>1</v>
+      </c>
+      <c r="L71" s="216">
+        <v>0</v>
+      </c>
+      <c r="M71" s="216">
+        <v>0</v>
+      </c>
+      <c r="N71" s="216">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10781,11 +10916,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66:A70"/>
+      <selection pane="bottomLeft" activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13038,6 +13173,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="15">
+        <v>44052</v>
+      </c>
+      <c r="B71" s="216">
+        <v>0</v>
+      </c>
+      <c r="C71" s="216">
+        <v>0</v>
+      </c>
+      <c r="D71" s="216">
+        <v>0</v>
+      </c>
+      <c r="E71" s="216">
+        <v>0</v>
+      </c>
+      <c r="F71" s="216">
+        <v>2</v>
+      </c>
+      <c r="G71" s="216">
+        <v>1</v>
+      </c>
+      <c r="H71" s="216">
+        <v>1</v>
+      </c>
+      <c r="I71" s="216">
+        <v>1</v>
+      </c>
+      <c r="J71" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13047,8 +13214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BU4" sqref="BU4"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BK6" sqref="BK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13267,7 +13434,9 @@
       <c r="BR1" s="49">
         <v>44051</v>
       </c>
-      <c r="BS1" s="49"/>
+      <c r="BS1" s="49">
+        <v>44052</v>
+      </c>
       <c r="BT1" s="49"/>
       <c r="BU1" s="49"/>
       <c r="BV1" s="49"/>
@@ -13490,7 +13659,9 @@
       <c r="BR2" s="48">
         <v>5122</v>
       </c>
-      <c r="BS2" s="48"/>
+      <c r="BS2" s="48">
+        <v>5154</v>
+      </c>
       <c r="BT2" s="48"/>
       <c r="BU2" s="48"/>
       <c r="BV2" s="48"/>
@@ -13713,7 +13884,9 @@
       <c r="BR3" s="48">
         <v>4921</v>
       </c>
-      <c r="BS3" s="48"/>
+      <c r="BS3" s="48">
+        <v>4953</v>
+      </c>
       <c r="BT3" s="48"/>
       <c r="BU3" s="48"/>
       <c r="BV3" s="48"/>
@@ -13936,7 +14109,9 @@
       <c r="BR4" s="48">
         <v>4921</v>
       </c>
-      <c r="BS4" s="48"/>
+      <c r="BS4" s="48">
+        <v>4953</v>
+      </c>
       <c r="BT4" s="48"/>
       <c r="BU4" s="48"/>
       <c r="BV4" s="48"/>
@@ -14159,7 +14334,9 @@
       <c r="BR5" s="48">
         <v>4921</v>
       </c>
-      <c r="BS5" s="48"/>
+      <c r="BS5" s="48">
+        <v>4953</v>
+      </c>
       <c r="BT5" s="48"/>
       <c r="BU5" s="48"/>
       <c r="BV5" s="48"/>
@@ -14382,7 +14559,9 @@
       <c r="BR6" s="48">
         <v>4921</v>
       </c>
-      <c r="BS6" s="48"/>
+      <c r="BS6" s="48">
+        <v>4953</v>
+      </c>
       <c r="BT6" s="48"/>
       <c r="BU6" s="48"/>
       <c r="BV6" s="48"/>
@@ -14605,7 +14784,9 @@
       <c r="BR7" s="48">
         <v>4231</v>
       </c>
-      <c r="BS7" s="48"/>
+      <c r="BS7" s="48">
+        <v>4263</v>
+      </c>
       <c r="BT7" s="48"/>
       <c r="BU7" s="48"/>
       <c r="BV7" s="48"/>
@@ -14828,7 +15009,9 @@
       <c r="BR8" s="48">
         <v>6862</v>
       </c>
-      <c r="BS8" s="48"/>
+      <c r="BS8" s="48">
+        <v>6894</v>
+      </c>
       <c r="BT8" s="48"/>
       <c r="BU8" s="48"/>
       <c r="BV8" s="48"/>
@@ -15141,7 +15324,9 @@
       <c r="BR10" s="48">
         <v>209</v>
       </c>
-      <c r="BS10" s="48"/>
+      <c r="BS10" s="48">
+        <v>210</v>
+      </c>
       <c r="BT10" s="48"/>
       <c r="BU10" s="48"/>
       <c r="BV10" s="48"/>
@@ -15364,7 +15549,9 @@
       <c r="BR11" s="48">
         <v>209</v>
       </c>
-      <c r="BS11" s="48"/>
+      <c r="BS11" s="48">
+        <v>210</v>
+      </c>
       <c r="BT11" s="48"/>
       <c r="BU11" s="48"/>
       <c r="BV11" s="48"/>
@@ -15587,7 +15774,9 @@
       <c r="BR12" s="48">
         <v>209</v>
       </c>
-      <c r="BS12" s="48"/>
+      <c r="BS12" s="48">
+        <v>210</v>
+      </c>
       <c r="BT12" s="48"/>
       <c r="BU12" s="48"/>
       <c r="BV12" s="48"/>
@@ -15810,7 +15999,9 @@
       <c r="BR13" s="48">
         <v>209</v>
       </c>
-      <c r="BS13" s="48"/>
+      <c r="BS13" s="48">
+        <v>210</v>
+      </c>
       <c r="BT13" s="48"/>
       <c r="BU13" s="48"/>
       <c r="BV13" s="48"/>
@@ -16256,7 +16447,9 @@
       <c r="BR15" s="48">
         <v>144</v>
       </c>
-      <c r="BS15" s="48"/>
+      <c r="BS15" s="48">
+        <v>145</v>
+      </c>
       <c r="BT15" s="48"/>
       <c r="BU15" s="48"/>
       <c r="BV15" s="48"/>
@@ -16479,7 +16672,9 @@
       <c r="BR16" s="48">
         <v>221</v>
       </c>
-      <c r="BS16" s="48"/>
+      <c r="BS16" s="48">
+        <v>22</v>
+      </c>
       <c r="BT16" s="48"/>
       <c r="BU16" s="48"/>
       <c r="BV16" s="48"/>
@@ -16788,6 +16983,9 @@
       <c r="BR18" s="216">
         <v>1192</v>
       </c>
+      <c r="BS18" s="216">
+        <v>1199</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -16965,7 +17163,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BR20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BS20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -17075,6 +17273,10 @@
       <c r="BR20" s="51">
         <f t="shared" si="1"/>
         <v>38501</v>
+      </c>
+      <c r="BS20" s="51">
+        <f t="shared" si="1"/>
+        <v>38329</v>
       </c>
     </row>
   </sheetData>
@@ -17291,7 +17493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -17374,43 +17576,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="662" t="s">
+      <c r="B8" s="671" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="662"/>
+      <c r="B9" s="671"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="662"/>
+      <c r="B10" s="671"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="662"/>
+      <c r="B11" s="671"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="663" t="s">
+      <c r="B12" s="672" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="663"/>
+      <c r="B13" s="672"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="663"/>
+      <c r="B14" s="672"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="664" t="s">
+      <c r="B15" s="673" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="664"/>
+      <c r="B16" s="673"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data for August 10th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E084A9-2450-0243-A1AE-C0158B2263A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E6480-6151-5A45-A38E-EF5BDDC0713E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35220" yWindow="5120" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="674">
+  <cellXfs count="683">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2298,6 +2298,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2869,10 +2896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5152,6 +5179,38 @@
         <v>1091695</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="15">
+        <v>44053</v>
+      </c>
+      <c r="B72" s="671">
+        <v>485836</v>
+      </c>
+      <c r="C72" s="672">
+        <v>532028</v>
+      </c>
+      <c r="D72" s="673">
+        <v>79213</v>
+      </c>
+      <c r="E72" s="674">
+        <v>53003</v>
+      </c>
+      <c r="F72" s="675">
+        <v>26.557521468149748</v>
+      </c>
+      <c r="G72" s="676">
+        <v>129026</v>
+      </c>
+      <c r="H72" s="677">
+        <v>10282</v>
+      </c>
+      <c r="I72" s="678">
+        <v>12383</v>
+      </c>
+      <c r="J72" s="679">
+        <v>1097077</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5159,11 +5218,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <selection pane="bottomLeft" activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7820,6 +7879,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="15">
+        <v>44053</v>
+      </c>
+      <c r="B72" s="216">
+        <v>0</v>
+      </c>
+      <c r="C72" s="216">
+        <v>1</v>
+      </c>
+      <c r="D72" s="216">
+        <v>0</v>
+      </c>
+      <c r="E72" s="216">
+        <v>0</v>
+      </c>
+      <c r="F72" s="216">
+        <v>1</v>
+      </c>
+      <c r="G72" s="216">
+        <v>0</v>
+      </c>
+      <c r="H72" s="216">
+        <v>0</v>
+      </c>
+      <c r="I72" s="216">
+        <v>0</v>
+      </c>
+      <c r="J72" s="216">
+        <v>0</v>
+      </c>
+      <c r="K72" s="216">
+        <v>0</v>
+      </c>
+      <c r="L72" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7827,11 +7924,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <selection pane="bottomLeft" activeCell="O72" sqref="O72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10906,6 +11003,50 @@
         <v>0</v>
       </c>
       <c r="N71" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="15">
+        <v>44053</v>
+      </c>
+      <c r="B72" s="216">
+        <v>0</v>
+      </c>
+      <c r="C72" s="216">
+        <v>1</v>
+      </c>
+      <c r="D72" s="216">
+        <v>0</v>
+      </c>
+      <c r="E72" s="216">
+        <v>0</v>
+      </c>
+      <c r="F72" s="216">
+        <v>0</v>
+      </c>
+      <c r="G72" s="216">
+        <v>0</v>
+      </c>
+      <c r="H72" s="216">
+        <v>1</v>
+      </c>
+      <c r="I72" s="216">
+        <v>0</v>
+      </c>
+      <c r="J72" s="216">
+        <v>0</v>
+      </c>
+      <c r="K72" s="216">
+        <v>1</v>
+      </c>
+      <c r="L72" s="216">
+        <v>0</v>
+      </c>
+      <c r="M72" s="216">
+        <v>0</v>
+      </c>
+      <c r="N72" s="216">
         <v>0</v>
       </c>
     </row>
@@ -10916,11 +11057,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K71" sqref="K71"/>
+      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13205,6 +13346,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="15">
+        <v>44053</v>
+      </c>
+      <c r="B72" s="216">
+        <v>0</v>
+      </c>
+      <c r="C72" s="216">
+        <v>0</v>
+      </c>
+      <c r="D72" s="216">
+        <v>0</v>
+      </c>
+      <c r="E72" s="216">
+        <v>0</v>
+      </c>
+      <c r="F72" s="216">
+        <v>2</v>
+      </c>
+      <c r="G72" s="216">
+        <v>1</v>
+      </c>
+      <c r="H72" s="216">
+        <v>1</v>
+      </c>
+      <c r="I72" s="216">
+        <v>1</v>
+      </c>
+      <c r="J72" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13214,8 +13387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BK6" sqref="BK6"/>
+    <sheetView topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BR28" sqref="BR28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13437,7 +13610,9 @@
       <c r="BS1" s="49">
         <v>44052</v>
       </c>
-      <c r="BT1" s="49"/>
+      <c r="BT1" s="49">
+        <v>44053</v>
+      </c>
       <c r="BU1" s="49"/>
       <c r="BV1" s="49"/>
       <c r="BW1" s="49"/>
@@ -13662,7 +13837,9 @@
       <c r="BS2" s="48">
         <v>5154</v>
       </c>
-      <c r="BT2" s="48"/>
+      <c r="BT2" s="48">
+        <v>5186</v>
+      </c>
       <c r="BU2" s="48"/>
       <c r="BV2" s="48"/>
       <c r="BW2" s="48"/>
@@ -13887,7 +14064,9 @@
       <c r="BS3" s="48">
         <v>4953</v>
       </c>
-      <c r="BT3" s="48"/>
+      <c r="BT3" s="48">
+        <v>4985</v>
+      </c>
       <c r="BU3" s="48"/>
       <c r="BV3" s="48"/>
       <c r="BW3" s="48"/>
@@ -14112,7 +14291,9 @@
       <c r="BS4" s="48">
         <v>4953</v>
       </c>
-      <c r="BT4" s="48"/>
+      <c r="BT4" s="48">
+        <v>4985</v>
+      </c>
       <c r="BU4" s="48"/>
       <c r="BV4" s="48"/>
       <c r="BW4" s="48"/>
@@ -14337,7 +14518,9 @@
       <c r="BS5" s="48">
         <v>4953</v>
       </c>
-      <c r="BT5" s="48"/>
+      <c r="BT5" s="48">
+        <v>4985</v>
+      </c>
       <c r="BU5" s="48"/>
       <c r="BV5" s="48"/>
       <c r="BW5" s="48"/>
@@ -14562,7 +14745,9 @@
       <c r="BS6" s="48">
         <v>4953</v>
       </c>
-      <c r="BT6" s="48"/>
+      <c r="BT6" s="48">
+        <v>4985</v>
+      </c>
       <c r="BU6" s="48"/>
       <c r="BV6" s="48"/>
       <c r="BW6" s="48"/>
@@ -14787,7 +14972,9 @@
       <c r="BS7" s="48">
         <v>4263</v>
       </c>
-      <c r="BT7" s="48"/>
+      <c r="BT7" s="48">
+        <v>4295</v>
+      </c>
       <c r="BU7" s="48"/>
       <c r="BV7" s="48"/>
       <c r="BW7" s="48"/>
@@ -15012,7 +15199,9 @@
       <c r="BS8" s="48">
         <v>6894</v>
       </c>
-      <c r="BT8" s="48"/>
+      <c r="BT8" s="48">
+        <v>6926</v>
+      </c>
       <c r="BU8" s="48"/>
       <c r="BV8" s="48"/>
       <c r="BW8" s="48"/>
@@ -15327,7 +15516,9 @@
       <c r="BS10" s="48">
         <v>210</v>
       </c>
-      <c r="BT10" s="48"/>
+      <c r="BT10" s="48">
+        <v>211</v>
+      </c>
       <c r="BU10" s="48"/>
       <c r="BV10" s="48"/>
       <c r="BW10" s="48"/>
@@ -15552,7 +15743,9 @@
       <c r="BS11" s="48">
         <v>210</v>
       </c>
-      <c r="BT11" s="48"/>
+      <c r="BT11" s="48">
+        <v>211</v>
+      </c>
       <c r="BU11" s="48"/>
       <c r="BV11" s="48"/>
       <c r="BW11" s="48"/>
@@ -15777,7 +15970,9 @@
       <c r="BS12" s="48">
         <v>210</v>
       </c>
-      <c r="BT12" s="48"/>
+      <c r="BT12" s="48">
+        <v>211</v>
+      </c>
       <c r="BU12" s="48"/>
       <c r="BV12" s="48"/>
       <c r="BW12" s="48"/>
@@ -16002,7 +16197,9 @@
       <c r="BS13" s="48">
         <v>210</v>
       </c>
-      <c r="BT13" s="48"/>
+      <c r="BT13" s="48">
+        <v>211</v>
+      </c>
       <c r="BU13" s="48"/>
       <c r="BV13" s="48"/>
       <c r="BW13" s="48"/>
@@ -16224,8 +16421,12 @@
       <c r="BR14" s="48">
         <v>209</v>
       </c>
-      <c r="BS14" s="48"/>
-      <c r="BT14" s="48"/>
+      <c r="BS14" s="48">
+        <v>210</v>
+      </c>
+      <c r="BT14" s="48">
+        <v>211</v>
+      </c>
       <c r="BU14" s="48"/>
       <c r="BV14" s="48"/>
       <c r="BW14" s="48"/>
@@ -16450,7 +16651,9 @@
       <c r="BS15" s="48">
         <v>145</v>
       </c>
-      <c r="BT15" s="48"/>
+      <c r="BT15" s="48">
+        <v>146</v>
+      </c>
       <c r="BU15" s="48"/>
       <c r="BV15" s="48"/>
       <c r="BW15" s="48"/>
@@ -16673,9 +16876,11 @@
         <v>221</v>
       </c>
       <c r="BS16" s="48">
-        <v>22</v>
-      </c>
-      <c r="BT16" s="48"/>
+        <v>222</v>
+      </c>
+      <c r="BT16" s="48">
+        <v>223</v>
+      </c>
       <c r="BU16" s="48"/>
       <c r="BV16" s="48"/>
       <c r="BW16" s="48"/>
@@ -16986,6 +17191,9 @@
       <c r="BS18" s="216">
         <v>1199</v>
       </c>
+      <c r="BT18" s="216">
+        <v>1206</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -17163,7 +17371,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BS20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BT20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -17276,7 +17484,11 @@
       </c>
       <c r="BS20" s="51">
         <f t="shared" si="1"/>
-        <v>38329</v>
+        <v>38739</v>
+      </c>
+      <c r="BT20" s="51">
+        <f t="shared" si="1"/>
+        <v>38977</v>
       </c>
     </row>
   </sheetData>
@@ -17288,8 +17500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17576,43 +17788,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="671" t="s">
+      <c r="B8" s="680" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="671"/>
+      <c r="B9" s="680"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="671"/>
+      <c r="B10" s="680"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="671"/>
+      <c r="B11" s="680"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="672" t="s">
+      <c r="B12" s="681" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="672"/>
+      <c r="B13" s="681"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="672"/>
+      <c r="B14" s="681"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="673" t="s">
+      <c r="B15" s="682" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="673"/>
+      <c r="B16" s="682"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 11th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E6480-6151-5A45-A38E-EF5BDDC0713E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBF5F37-1E63-2145-B681-3A15CFF5A67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="11280" yWindow="460" windowWidth="17520" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -280,6 +280,12 @@
   <si>
     <t xml:space="preserve">El número de observaciones de sx /nal hasta uci/nal subio en dos observaciones </t>
   </si>
+  <si>
+    <t>11 de agosto 2020</t>
+  </si>
+  <si>
+    <t>Las observaciones de sx_nal se mantuvieron</t>
+  </si>
 </sst>
 </file>
 
@@ -362,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +476,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -585,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="683">
+  <cellXfs count="693">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2568,6 +2580,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2896,10 +2936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5211,6 +5251,38 @@
         <v>1097077</v>
       </c>
     </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>44054</v>
+      </c>
+      <c r="B73" s="680">
+        <v>492522</v>
+      </c>
+      <c r="C73" s="681">
+        <v>538333</v>
+      </c>
+      <c r="D73" s="682">
+        <v>81259</v>
+      </c>
+      <c r="E73" s="683">
+        <v>53929</v>
+      </c>
+      <c r="F73" s="684">
+        <v>26.508460535773022</v>
+      </c>
+      <c r="G73" s="685">
+        <v>130560</v>
+      </c>
+      <c r="H73" s="686">
+        <v>10452</v>
+      </c>
+      <c r="I73" s="687">
+        <v>12562</v>
+      </c>
+      <c r="J73" s="688">
+        <v>1112114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5218,11 +5290,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L72" sqref="L72"/>
+      <selection pane="bottomLeft" activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7917,6 +7989,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>44054</v>
+      </c>
+      <c r="B73" s="216">
+        <v>0</v>
+      </c>
+      <c r="C73" s="216">
+        <v>1</v>
+      </c>
+      <c r="D73" s="216">
+        <v>0</v>
+      </c>
+      <c r="E73" s="216">
+        <v>0</v>
+      </c>
+      <c r="F73" s="216">
+        <v>1</v>
+      </c>
+      <c r="G73" s="216">
+        <v>0</v>
+      </c>
+      <c r="H73" s="216">
+        <v>0</v>
+      </c>
+      <c r="I73" s="216">
+        <v>0</v>
+      </c>
+      <c r="J73" s="216">
+        <v>0</v>
+      </c>
+      <c r="K73" s="216">
+        <v>0</v>
+      </c>
+      <c r="L73" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7924,11 +8034,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O72" sqref="O72"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11047,6 +11157,50 @@
         <v>0</v>
       </c>
       <c r="N72" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>44054</v>
+      </c>
+      <c r="B73" s="216">
+        <v>0</v>
+      </c>
+      <c r="C73" s="216">
+        <v>1</v>
+      </c>
+      <c r="D73" s="216">
+        <v>0</v>
+      </c>
+      <c r="E73" s="216">
+        <v>0</v>
+      </c>
+      <c r="F73" s="216">
+        <v>0</v>
+      </c>
+      <c r="G73" s="216">
+        <v>0</v>
+      </c>
+      <c r="H73" s="216">
+        <v>1</v>
+      </c>
+      <c r="I73" s="216">
+        <v>0</v>
+      </c>
+      <c r="J73" s="216">
+        <v>0</v>
+      </c>
+      <c r="K73" s="216">
+        <v>1</v>
+      </c>
+      <c r="L73" s="216">
+        <v>0</v>
+      </c>
+      <c r="M73" s="216">
+        <v>0</v>
+      </c>
+      <c r="N73" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11057,11 +11211,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
+      <selection pane="bottomLeft" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13378,6 +13532,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="15">
+        <v>44054</v>
+      </c>
+      <c r="B73" s="216">
+        <v>0</v>
+      </c>
+      <c r="C73" s="216">
+        <v>0</v>
+      </c>
+      <c r="D73" s="216">
+        <v>0</v>
+      </c>
+      <c r="E73" s="216">
+        <v>0</v>
+      </c>
+      <c r="F73" s="216">
+        <v>2</v>
+      </c>
+      <c r="G73" s="216">
+        <v>1</v>
+      </c>
+      <c r="H73" s="216">
+        <v>1</v>
+      </c>
+      <c r="I73" s="216">
+        <v>1</v>
+      </c>
+      <c r="J73" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13387,8 +13573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BR28" sqref="BR28"/>
+    <sheetView topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BV16" sqref="BV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13613,7 +13799,9 @@
       <c r="BT1" s="49">
         <v>44053</v>
       </c>
-      <c r="BU1" s="49"/>
+      <c r="BU1" s="49">
+        <v>44054</v>
+      </c>
       <c r="BV1" s="49"/>
       <c r="BW1" s="49"/>
       <c r="BX1" s="48"/>
@@ -13840,7 +14028,9 @@
       <c r="BT2" s="48">
         <v>5186</v>
       </c>
-      <c r="BU2" s="48"/>
+      <c r="BU2" s="48">
+        <v>5218</v>
+      </c>
       <c r="BV2" s="48"/>
       <c r="BW2" s="48"/>
       <c r="BX2" s="48"/>
@@ -14067,7 +14257,9 @@
       <c r="BT3" s="48">
         <v>4985</v>
       </c>
-      <c r="BU3" s="48"/>
+      <c r="BU3" s="48">
+        <v>5017</v>
+      </c>
       <c r="BV3" s="48"/>
       <c r="BW3" s="48"/>
       <c r="BX3" s="48"/>
@@ -14294,7 +14486,9 @@
       <c r="BT4" s="48">
         <v>4985</v>
       </c>
-      <c r="BU4" s="48"/>
+      <c r="BU4" s="48">
+        <v>5017</v>
+      </c>
       <c r="BV4" s="48"/>
       <c r="BW4" s="48"/>
       <c r="BX4" s="48"/>
@@ -14521,7 +14715,9 @@
       <c r="BT5" s="48">
         <v>4985</v>
       </c>
-      <c r="BU5" s="48"/>
+      <c r="BU5" s="48">
+        <v>5017</v>
+      </c>
       <c r="BV5" s="48"/>
       <c r="BW5" s="48"/>
       <c r="BX5" s="48"/>
@@ -14748,7 +14944,9 @@
       <c r="BT6" s="48">
         <v>4985</v>
       </c>
-      <c r="BU6" s="48"/>
+      <c r="BU6" s="48">
+        <v>5017</v>
+      </c>
       <c r="BV6" s="48"/>
       <c r="BW6" s="48"/>
       <c r="BX6" s="48"/>
@@ -14975,7 +15173,9 @@
       <c r="BT7" s="48">
         <v>4295</v>
       </c>
-      <c r="BU7" s="48"/>
+      <c r="BU7" s="48">
+        <v>4327</v>
+      </c>
       <c r="BV7" s="48"/>
       <c r="BW7" s="48"/>
       <c r="BX7" s="48"/>
@@ -15202,7 +15402,9 @@
       <c r="BT8" s="48">
         <v>6926</v>
       </c>
-      <c r="BU8" s="48"/>
+      <c r="BU8" s="48">
+        <v>6958</v>
+      </c>
       <c r="BV8" s="48"/>
       <c r="BW8" s="48"/>
       <c r="BX8" s="48"/>
@@ -15516,10 +15718,12 @@
       <c r="BS10" s="48">
         <v>210</v>
       </c>
-      <c r="BT10" s="48">
+      <c r="BT10" s="689">
         <v>211</v>
       </c>
-      <c r="BU10" s="48"/>
+      <c r="BU10" s="689">
+        <v>212</v>
+      </c>
       <c r="BV10" s="48"/>
       <c r="BW10" s="48"/>
       <c r="BX10" s="48"/>
@@ -15746,7 +15950,9 @@
       <c r="BT11" s="48">
         <v>211</v>
       </c>
-      <c r="BU11" s="48"/>
+      <c r="BU11" s="48">
+        <v>212</v>
+      </c>
       <c r="BV11" s="48"/>
       <c r="BW11" s="48"/>
       <c r="BX11" s="48"/>
@@ -15973,7 +16179,9 @@
       <c r="BT12" s="48">
         <v>211</v>
       </c>
-      <c r="BU12" s="48"/>
+      <c r="BU12" s="48">
+        <v>212</v>
+      </c>
       <c r="BV12" s="48"/>
       <c r="BW12" s="48"/>
       <c r="BX12" s="48"/>
@@ -16200,7 +16408,9 @@
       <c r="BT13" s="48">
         <v>211</v>
       </c>
-      <c r="BU13" s="48"/>
+      <c r="BU13" s="48">
+        <v>212</v>
+      </c>
       <c r="BV13" s="48"/>
       <c r="BW13" s="48"/>
       <c r="BX13" s="48"/>
@@ -16427,7 +16637,9 @@
       <c r="BT14" s="48">
         <v>211</v>
       </c>
-      <c r="BU14" s="48"/>
+      <c r="BU14" s="48">
+        <v>212</v>
+      </c>
       <c r="BV14" s="48"/>
       <c r="BW14" s="48"/>
       <c r="BX14" s="48"/>
@@ -16654,7 +16866,9 @@
       <c r="BT15" s="48">
         <v>146</v>
       </c>
-      <c r="BU15" s="48"/>
+      <c r="BU15" s="48">
+        <v>147</v>
+      </c>
       <c r="BV15" s="48"/>
       <c r="BW15" s="48"/>
       <c r="BX15" s="48"/>
@@ -16881,7 +17095,9 @@
       <c r="BT16" s="48">
         <v>223</v>
       </c>
-      <c r="BU16" s="48"/>
+      <c r="BU16" s="48">
+        <v>224</v>
+      </c>
       <c r="BV16" s="48"/>
       <c r="BW16" s="48"/>
       <c r="BX16" s="48"/>
@@ -17194,6 +17410,9 @@
       <c r="BT18" s="216">
         <v>1206</v>
       </c>
+      <c r="BU18">
+        <v>1213</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -17371,7 +17590,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BT20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BU20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -17489,6 +17708,10 @@
       <c r="BT20" s="51">
         <f t="shared" si="1"/>
         <v>38977</v>
+      </c>
+      <c r="BU20" s="51">
+        <f t="shared" si="1"/>
+        <v>39215</v>
       </c>
     </row>
   </sheetData>
@@ -17500,7 +17723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -17703,10 +17926,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17788,43 +18011,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="680" t="s">
+      <c r="B8" s="690" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="680"/>
+      <c r="B9" s="690"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="680"/>
+      <c r="B10" s="690"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="680"/>
+      <c r="B11" s="690"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="681" t="s">
+      <c r="B12" s="691" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="681"/>
+      <c r="B13" s="691"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="681"/>
+      <c r="B14" s="691"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="682" t="s">
+      <c r="B15" s="692" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="682"/>
+      <c r="B16" s="692"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -17832,6 +18055,14 @@
       </c>
       <c r="B17" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 12th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBF5F37-1E63-2145-B681-3A15CFF5A67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB27511C-0814-7245-B139-78DA306B9251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="460" windowWidth="17520" windowHeight="16420" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="7060" yWindow="920" windowWidth="17520" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="693">
+  <cellXfs count="702">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2936,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5283,6 +5310,38 @@
         <v>1112114</v>
       </c>
     </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="15">
+        <v>44055</v>
+      </c>
+      <c r="B74" s="690">
+        <v>498380</v>
+      </c>
+      <c r="C74" s="691">
+        <v>545262</v>
+      </c>
+      <c r="D74" s="692">
+        <v>83473</v>
+      </c>
+      <c r="E74" s="693">
+        <v>54666</v>
+      </c>
+      <c r="F74" s="694">
+        <v>26.485412737268749</v>
+      </c>
+      <c r="G74" s="695">
+        <v>131998</v>
+      </c>
+      <c r="H74" s="696">
+        <v>10528</v>
+      </c>
+      <c r="I74" s="697">
+        <v>12742</v>
+      </c>
+      <c r="J74" s="698">
+        <v>1127115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5290,11 +5349,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L73" sqref="L73"/>
+      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8027,6 +8086,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="15">
+        <v>44055</v>
+      </c>
+      <c r="B74" s="216">
+        <v>0</v>
+      </c>
+      <c r="C74" s="216">
+        <v>1</v>
+      </c>
+      <c r="D74" s="216">
+        <v>0</v>
+      </c>
+      <c r="E74" s="216">
+        <v>0</v>
+      </c>
+      <c r="F74" s="216">
+        <v>1</v>
+      </c>
+      <c r="G74" s="216">
+        <v>0</v>
+      </c>
+      <c r="H74" s="216">
+        <v>0</v>
+      </c>
+      <c r="I74" s="216">
+        <v>0</v>
+      </c>
+      <c r="J74" s="216">
+        <v>0</v>
+      </c>
+      <c r="K74" s="216">
+        <v>0</v>
+      </c>
+      <c r="L74" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8034,11 +8131,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O73" sqref="O73"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O74" sqref="O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11201,6 +11298,50 @@
         <v>0</v>
       </c>
       <c r="N73" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="15">
+        <v>44055</v>
+      </c>
+      <c r="B74" s="216">
+        <v>0</v>
+      </c>
+      <c r="C74" s="216">
+        <v>1</v>
+      </c>
+      <c r="D74" s="216">
+        <v>0</v>
+      </c>
+      <c r="E74" s="216">
+        <v>0</v>
+      </c>
+      <c r="F74" s="216">
+        <v>0</v>
+      </c>
+      <c r="G74" s="216">
+        <v>0</v>
+      </c>
+      <c r="H74" s="216">
+        <v>1</v>
+      </c>
+      <c r="I74" s="216">
+        <v>0</v>
+      </c>
+      <c r="J74" s="216">
+        <v>0</v>
+      </c>
+      <c r="K74" s="216">
+        <v>1</v>
+      </c>
+      <c r="L74" s="216">
+        <v>0</v>
+      </c>
+      <c r="M74" s="216">
+        <v>0</v>
+      </c>
+      <c r="N74" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11211,11 +11352,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J73" sqref="J73"/>
+      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13564,6 +13705,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="15">
+        <v>44055</v>
+      </c>
+      <c r="B74" s="216">
+        <v>0</v>
+      </c>
+      <c r="C74" s="216">
+        <v>0</v>
+      </c>
+      <c r="D74" s="216">
+        <v>0</v>
+      </c>
+      <c r="E74" s="216">
+        <v>0</v>
+      </c>
+      <c r="F74" s="216">
+        <v>2</v>
+      </c>
+      <c r="G74" s="216">
+        <v>1</v>
+      </c>
+      <c r="H74" s="216">
+        <v>1</v>
+      </c>
+      <c r="I74" s="216">
+        <v>1</v>
+      </c>
+      <c r="J74" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13573,8 +13746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BV16" sqref="BV16"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BW25" sqref="BW25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13802,7 +13975,9 @@
       <c r="BU1" s="49">
         <v>44054</v>
       </c>
-      <c r="BV1" s="49"/>
+      <c r="BV1" s="15">
+        <v>44055</v>
+      </c>
       <c r="BW1" s="49"/>
       <c r="BX1" s="48"/>
       <c r="BY1" s="48"/>
@@ -14031,7 +14206,9 @@
       <c r="BU2" s="48">
         <v>5218</v>
       </c>
-      <c r="BV2" s="48"/>
+      <c r="BV2" s="48">
+        <v>5250</v>
+      </c>
       <c r="BW2" s="48"/>
       <c r="BX2" s="48"/>
       <c r="BY2" s="48"/>
@@ -14260,7 +14437,9 @@
       <c r="BU3" s="48">
         <v>5017</v>
       </c>
-      <c r="BV3" s="48"/>
+      <c r="BV3" s="48">
+        <v>5049</v>
+      </c>
       <c r="BW3" s="48"/>
       <c r="BX3" s="48"/>
       <c r="BY3" s="48"/>
@@ -14489,7 +14668,9 @@
       <c r="BU4" s="48">
         <v>5017</v>
       </c>
-      <c r="BV4" s="48"/>
+      <c r="BV4" s="48">
+        <v>5049</v>
+      </c>
       <c r="BW4" s="48"/>
       <c r="BX4" s="48"/>
       <c r="BY4" s="48"/>
@@ -14718,7 +14899,9 @@
       <c r="BU5" s="48">
         <v>5017</v>
       </c>
-      <c r="BV5" s="48"/>
+      <c r="BV5" s="48">
+        <v>5049</v>
+      </c>
       <c r="BW5" s="48"/>
       <c r="BX5" s="48"/>
       <c r="BY5" s="48"/>
@@ -14947,7 +15130,9 @@
       <c r="BU6" s="48">
         <v>5017</v>
       </c>
-      <c r="BV6" s="48"/>
+      <c r="BV6" s="48">
+        <v>5049</v>
+      </c>
       <c r="BW6" s="48"/>
       <c r="BX6" s="48"/>
       <c r="BY6" s="48"/>
@@ -15176,7 +15361,9 @@
       <c r="BU7" s="48">
         <v>4327</v>
       </c>
-      <c r="BV7" s="48"/>
+      <c r="BV7" s="48">
+        <v>4359</v>
+      </c>
       <c r="BW7" s="48"/>
       <c r="BX7" s="48"/>
       <c r="BY7" s="48"/>
@@ -15405,7 +15592,9 @@
       <c r="BU8" s="48">
         <v>6958</v>
       </c>
-      <c r="BV8" s="48"/>
+      <c r="BV8" s="48">
+        <v>6990</v>
+      </c>
       <c r="BW8" s="48"/>
       <c r="BX8" s="48"/>
       <c r="BY8" s="48"/>
@@ -15724,7 +15913,9 @@
       <c r="BU10" s="689">
         <v>212</v>
       </c>
-      <c r="BV10" s="48"/>
+      <c r="BV10" s="48">
+        <v>213</v>
+      </c>
       <c r="BW10" s="48"/>
       <c r="BX10" s="48"/>
       <c r="BY10" s="48"/>
@@ -15953,7 +16144,9 @@
       <c r="BU11" s="48">
         <v>212</v>
       </c>
-      <c r="BV11" s="48"/>
+      <c r="BV11" s="48">
+        <v>213</v>
+      </c>
       <c r="BW11" s="48"/>
       <c r="BX11" s="48"/>
       <c r="BY11" s="48"/>
@@ -16182,7 +16375,9 @@
       <c r="BU12" s="48">
         <v>212</v>
       </c>
-      <c r="BV12" s="48"/>
+      <c r="BV12" s="48">
+        <v>213</v>
+      </c>
       <c r="BW12" s="48"/>
       <c r="BX12" s="48"/>
       <c r="BY12" s="48"/>
@@ -16411,7 +16606,9 @@
       <c r="BU13" s="48">
         <v>212</v>
       </c>
-      <c r="BV13" s="48"/>
+      <c r="BV13" s="48">
+        <v>213</v>
+      </c>
       <c r="BW13" s="48"/>
       <c r="BX13" s="48"/>
       <c r="BY13" s="48"/>
@@ -16640,7 +16837,9 @@
       <c r="BU14" s="48">
         <v>212</v>
       </c>
-      <c r="BV14" s="48"/>
+      <c r="BV14" s="48">
+        <v>213</v>
+      </c>
       <c r="BW14" s="48"/>
       <c r="BX14" s="48"/>
       <c r="BY14" s="48"/>
@@ -16869,7 +17068,9 @@
       <c r="BU15" s="48">
         <v>147</v>
       </c>
-      <c r="BV15" s="48"/>
+      <c r="BV15" s="48">
+        <v>148</v>
+      </c>
       <c r="BW15" s="48"/>
       <c r="BX15" s="48"/>
       <c r="BY15" s="48"/>
@@ -17098,7 +17299,9 @@
       <c r="BU16" s="48">
         <v>224</v>
       </c>
-      <c r="BV16" s="48"/>
+      <c r="BV16" s="48">
+        <v>225</v>
+      </c>
       <c r="BW16" s="48"/>
       <c r="BX16" s="48"/>
       <c r="BY16" s="48"/>
@@ -17413,6 +17616,9 @@
       <c r="BU18">
         <v>1213</v>
       </c>
+      <c r="BV18" s="216">
+        <v>1220</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -17590,7 +17796,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BU20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BV20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -17712,6 +17918,10 @@
       <c r="BU20" s="51">
         <f t="shared" si="1"/>
         <v>39215</v>
+      </c>
+      <c r="BV20" s="51">
+        <f t="shared" si="1"/>
+        <v>39453</v>
       </c>
     </row>
   </sheetData>
@@ -18011,43 +18221,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="690" t="s">
+      <c r="B8" s="699" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="690"/>
+      <c r="B9" s="699"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="690"/>
+      <c r="B10" s="699"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="690"/>
+      <c r="B11" s="699"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="691" t="s">
+      <c r="B12" s="700" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="691"/>
+      <c r="B13" s="700"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="691"/>
+      <c r="B14" s="700"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="692" t="s">
+      <c r="B15" s="701" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="692"/>
+      <c r="B16" s="701"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 14th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB27511C-0814-7245-B139-78DA306B9251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F12D4A-4997-254F-8D48-E3DD0D2298E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="920" windowWidth="17520" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="-28100" yWindow="5020" windowWidth="17520" windowHeight="16420" activeTab="2" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="702">
+  <cellXfs count="711">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -2963,10 +2990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5342,6 +5369,38 @@
         <v>1127115</v>
       </c>
     </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>44056</v>
+      </c>
+      <c r="B75" s="699">
+        <v>505751</v>
+      </c>
+      <c r="C75" s="700">
+        <v>553219</v>
+      </c>
+      <c r="D75" s="701">
+        <v>83075</v>
+      </c>
+      <c r="E75" s="702">
+        <v>55293</v>
+      </c>
+      <c r="F75" s="703">
+        <v>26.385316094283549</v>
+      </c>
+      <c r="G75" s="704">
+        <v>133444</v>
+      </c>
+      <c r="H75" s="705">
+        <v>10662</v>
+      </c>
+      <c r="I75" s="706">
+        <v>12893</v>
+      </c>
+      <c r="J75" s="707">
+        <v>1142045</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5349,11 +5408,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8124,6 +8183,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>44056</v>
+      </c>
+      <c r="B75" s="216">
+        <v>0</v>
+      </c>
+      <c r="C75" s="216">
+        <v>1</v>
+      </c>
+      <c r="D75" s="216">
+        <v>0</v>
+      </c>
+      <c r="E75" s="216">
+        <v>0</v>
+      </c>
+      <c r="F75" s="216">
+        <v>1</v>
+      </c>
+      <c r="G75" s="216">
+        <v>0</v>
+      </c>
+      <c r="H75" s="216">
+        <v>0</v>
+      </c>
+      <c r="I75" s="216">
+        <v>0</v>
+      </c>
+      <c r="J75" s="216">
+        <v>0</v>
+      </c>
+      <c r="K75" s="216">
+        <v>0</v>
+      </c>
+      <c r="L75" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8131,11 +8228,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11342,6 +11439,50 @@
         <v>0</v>
       </c>
       <c r="N74" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>44056</v>
+      </c>
+      <c r="B75" s="216">
+        <v>0</v>
+      </c>
+      <c r="C75" s="216">
+        <v>1</v>
+      </c>
+      <c r="D75" s="216">
+        <v>0</v>
+      </c>
+      <c r="E75" s="216">
+        <v>0</v>
+      </c>
+      <c r="F75" s="216">
+        <v>0</v>
+      </c>
+      <c r="G75" s="216">
+        <v>0</v>
+      </c>
+      <c r="H75" s="216">
+        <v>1</v>
+      </c>
+      <c r="I75" s="216">
+        <v>0</v>
+      </c>
+      <c r="J75" s="216">
+        <v>0</v>
+      </c>
+      <c r="K75" s="216">
+        <v>1</v>
+      </c>
+      <c r="L75" s="216">
+        <v>0</v>
+      </c>
+      <c r="M75" s="216">
+        <v>0</v>
+      </c>
+      <c r="N75" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11352,11 +11493,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13737,6 +13878,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="15">
+        <v>44056</v>
+      </c>
+      <c r="B75" s="216">
+        <v>0</v>
+      </c>
+      <c r="C75" s="216">
+        <v>0</v>
+      </c>
+      <c r="D75" s="216">
+        <v>0</v>
+      </c>
+      <c r="E75" s="216">
+        <v>0</v>
+      </c>
+      <c r="F75" s="216">
+        <v>2</v>
+      </c>
+      <c r="G75" s="216">
+        <v>1</v>
+      </c>
+      <c r="H75" s="216">
+        <v>1</v>
+      </c>
+      <c r="I75" s="216">
+        <v>1</v>
+      </c>
+      <c r="J75" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13746,8 +13919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BW25" sqref="BW25"/>
+    <sheetView topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BW26" sqref="BW26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13978,7 +14151,9 @@
       <c r="BV1" s="15">
         <v>44055</v>
       </c>
-      <c r="BW1" s="49"/>
+      <c r="BW1" s="15">
+        <v>44056</v>
+      </c>
       <c r="BX1" s="48"/>
       <c r="BY1" s="48"/>
       <c r="BZ1" s="48"/>
@@ -14209,7 +14384,9 @@
       <c r="BV2" s="48">
         <v>5250</v>
       </c>
-      <c r="BW2" s="48"/>
+      <c r="BW2" s="48">
+        <v>5282</v>
+      </c>
       <c r="BX2" s="48"/>
       <c r="BY2" s="48"/>
       <c r="BZ2" s="48"/>
@@ -14440,7 +14617,9 @@
       <c r="BV3" s="48">
         <v>5049</v>
       </c>
-      <c r="BW3" s="48"/>
+      <c r="BW3" s="48">
+        <v>5081</v>
+      </c>
       <c r="BX3" s="48"/>
       <c r="BY3" s="48"/>
       <c r="BZ3" s="48"/>
@@ -14671,7 +14850,9 @@
       <c r="BV4" s="48">
         <v>5049</v>
       </c>
-      <c r="BW4" s="48"/>
+      <c r="BW4" s="48">
+        <v>5081</v>
+      </c>
       <c r="BX4" s="48"/>
       <c r="BY4" s="48"/>
       <c r="BZ4" s="48"/>
@@ -14902,7 +15083,9 @@
       <c r="BV5" s="48">
         <v>5049</v>
       </c>
-      <c r="BW5" s="48"/>
+      <c r="BW5" s="48">
+        <v>5081</v>
+      </c>
       <c r="BX5" s="48"/>
       <c r="BY5" s="48"/>
       <c r="BZ5" s="48"/>
@@ -15133,7 +15316,9 @@
       <c r="BV6" s="48">
         <v>5049</v>
       </c>
-      <c r="BW6" s="48"/>
+      <c r="BW6" s="48">
+        <v>5081</v>
+      </c>
       <c r="BX6" s="48"/>
       <c r="BY6" s="48"/>
       <c r="BZ6" s="48"/>
@@ -15364,7 +15549,9 @@
       <c r="BV7" s="48">
         <v>4359</v>
       </c>
-      <c r="BW7" s="48"/>
+      <c r="BW7" s="48">
+        <v>4391</v>
+      </c>
       <c r="BX7" s="48"/>
       <c r="BY7" s="48"/>
       <c r="BZ7" s="48"/>
@@ -15595,7 +15782,9 @@
       <c r="BV8" s="48">
         <v>6990</v>
       </c>
-      <c r="BW8" s="48"/>
+      <c r="BW8" s="48">
+        <v>7022</v>
+      </c>
       <c r="BX8" s="48"/>
       <c r="BY8" s="48"/>
       <c r="BZ8" s="48"/>
@@ -15916,7 +16105,9 @@
       <c r="BV10" s="48">
         <v>213</v>
       </c>
-      <c r="BW10" s="48"/>
+      <c r="BW10" s="48">
+        <v>214</v>
+      </c>
       <c r="BX10" s="48"/>
       <c r="BY10" s="48"/>
       <c r="BZ10" s="48"/>
@@ -16147,7 +16338,9 @@
       <c r="BV11" s="48">
         <v>213</v>
       </c>
-      <c r="BW11" s="48"/>
+      <c r="BW11" s="48">
+        <v>214</v>
+      </c>
       <c r="BX11" s="48"/>
       <c r="BY11" s="48"/>
       <c r="BZ11" s="48"/>
@@ -16378,7 +16571,9 @@
       <c r="BV12" s="48">
         <v>213</v>
       </c>
-      <c r="BW12" s="48"/>
+      <c r="BW12" s="48">
+        <v>214</v>
+      </c>
       <c r="BX12" s="48"/>
       <c r="BY12" s="48"/>
       <c r="BZ12" s="48"/>
@@ -16609,7 +16804,9 @@
       <c r="BV13" s="48">
         <v>213</v>
       </c>
-      <c r="BW13" s="48"/>
+      <c r="BW13" s="48">
+        <v>214</v>
+      </c>
       <c r="BX13" s="48"/>
       <c r="BY13" s="48"/>
       <c r="BZ13" s="48"/>
@@ -16840,7 +17037,9 @@
       <c r="BV14" s="48">
         <v>213</v>
       </c>
-      <c r="BW14" s="48"/>
+      <c r="BW14" s="48">
+        <v>214</v>
+      </c>
       <c r="BX14" s="48"/>
       <c r="BY14" s="48"/>
       <c r="BZ14" s="48"/>
@@ -17071,7 +17270,9 @@
       <c r="BV15" s="48">
         <v>148</v>
       </c>
-      <c r="BW15" s="48"/>
+      <c r="BW15" s="48">
+        <v>149</v>
+      </c>
       <c r="BX15" s="48"/>
       <c r="BY15" s="48"/>
       <c r="BZ15" s="48"/>
@@ -17302,7 +17503,9 @@
       <c r="BV16" s="48">
         <v>225</v>
       </c>
-      <c r="BW16" s="48"/>
+      <c r="BW16" s="48">
+        <v>226</v>
+      </c>
       <c r="BX16" s="48"/>
       <c r="BY16" s="48"/>
       <c r="BZ16" s="48"/>
@@ -17619,6 +17822,9 @@
       <c r="BV18" s="216">
         <v>1220</v>
       </c>
+      <c r="BW18">
+        <v>1227</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -17796,7 +18002,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BV20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BW20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -17922,6 +18128,10 @@
       <c r="BV20" s="51">
         <f t="shared" si="1"/>
         <v>39453</v>
+      </c>
+      <c r="BW20" s="51">
+        <f t="shared" si="1"/>
+        <v>39691</v>
       </c>
     </row>
   </sheetData>
@@ -18221,43 +18431,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="699" t="s">
+      <c r="B8" s="708" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="699"/>
+      <c r="B9" s="708"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="699"/>
+      <c r="B10" s="708"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="699"/>
+      <c r="B11" s="708"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="700" t="s">
+      <c r="B12" s="709" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="700"/>
+      <c r="B13" s="709"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="700"/>
+      <c r="B14" s="709"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="701" t="s">
+      <c r="B15" s="710" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="701"/>
+      <c r="B16" s="710"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 16th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C7B810-48DC-C643-BBC9-34D3E265C4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA86839-4EB6-FE4F-A2A3-976BB72927B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28100" yWindow="5020" windowWidth="17520" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Las observaciones de sx_nal se mantuvieron</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="720">
+  <cellXfs count="730">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2689,6 +2692,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2698,6 +2728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3017,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5460,6 +5491,38 @@
         <v>1156852</v>
       </c>
     </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="15">
+        <v>44058</v>
+      </c>
+      <c r="B77" s="717">
+        <v>517714</v>
+      </c>
+      <c r="C77" s="718">
+        <v>568359</v>
+      </c>
+      <c r="D77" s="719">
+        <v>84934</v>
+      </c>
+      <c r="E77" s="720">
+        <v>56543</v>
+      </c>
+      <c r="F77" s="721">
+        <v>26.25233236883685</v>
+      </c>
+      <c r="G77" s="722">
+        <v>135912</v>
+      </c>
+      <c r="H77" s="723">
+        <v>10932</v>
+      </c>
+      <c r="I77" s="724">
+        <v>13162</v>
+      </c>
+      <c r="J77" s="725">
+        <v>1171007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5467,11 +5530,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L76"/>
+  <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8318,6 +8381,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="15">
+        <v>44058</v>
+      </c>
+      <c r="B77" s="729" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="216">
+        <v>1</v>
+      </c>
+      <c r="D77" s="216">
+        <v>0</v>
+      </c>
+      <c r="E77" s="216">
+        <v>0</v>
+      </c>
+      <c r="F77" s="216">
+        <v>1</v>
+      </c>
+      <c r="G77" s="216">
+        <v>0</v>
+      </c>
+      <c r="H77" s="216">
+        <v>0</v>
+      </c>
+      <c r="I77" s="216">
+        <v>0</v>
+      </c>
+      <c r="J77" s="216">
+        <v>0</v>
+      </c>
+      <c r="K77" s="216">
+        <v>0</v>
+      </c>
+      <c r="L77" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8325,11 +8426,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O76" sqref="O76"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O77" sqref="O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11624,6 +11725,50 @@
         <v>0</v>
       </c>
       <c r="N76" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" s="15">
+        <v>44058</v>
+      </c>
+      <c r="B77" s="216">
+        <v>0</v>
+      </c>
+      <c r="C77" s="216">
+        <v>1</v>
+      </c>
+      <c r="D77" s="216">
+        <v>0</v>
+      </c>
+      <c r="E77" s="216">
+        <v>0</v>
+      </c>
+      <c r="F77" s="216">
+        <v>0</v>
+      </c>
+      <c r="G77" s="216">
+        <v>0</v>
+      </c>
+      <c r="H77" s="216">
+        <v>1</v>
+      </c>
+      <c r="I77" s="216">
+        <v>0</v>
+      </c>
+      <c r="J77" s="216">
+        <v>0</v>
+      </c>
+      <c r="K77" s="216">
+        <v>1</v>
+      </c>
+      <c r="L77" s="216">
+        <v>0</v>
+      </c>
+      <c r="M77" s="216">
+        <v>0</v>
+      </c>
+      <c r="N77" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11634,11 +11779,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J76" sqref="J76"/>
+      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14083,6 +14228,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="15">
+        <v>44058</v>
+      </c>
+      <c r="B77" s="216">
+        <v>0</v>
+      </c>
+      <c r="C77" s="216">
+        <v>0</v>
+      </c>
+      <c r="D77" s="216">
+        <v>0</v>
+      </c>
+      <c r="E77" s="216">
+        <v>0</v>
+      </c>
+      <c r="F77" s="216">
+        <v>2</v>
+      </c>
+      <c r="G77" s="216">
+        <v>1</v>
+      </c>
+      <c r="H77" s="216">
+        <v>1</v>
+      </c>
+      <c r="I77" s="216">
+        <v>1</v>
+      </c>
+      <c r="J77" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14093,7 +14270,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BW26" sqref="BW26"/>
+      <selection activeCell="CB21" sqref="CB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14330,7 +14507,9 @@
       <c r="BX1" s="49">
         <v>44057</v>
       </c>
-      <c r="BY1" s="48"/>
+      <c r="BY1" s="49">
+        <v>44058</v>
+      </c>
       <c r="BZ1" s="48"/>
       <c r="CA1" s="48"/>
       <c r="CB1" s="48"/>
@@ -14565,7 +14744,9 @@
       <c r="BX2" s="48">
         <v>5314</v>
       </c>
-      <c r="BY2" s="48"/>
+      <c r="BY2" s="48">
+        <v>5346</v>
+      </c>
       <c r="BZ2" s="48"/>
       <c r="CA2" s="48"/>
       <c r="CB2" s="48"/>
@@ -14800,7 +14981,9 @@
       <c r="BX3" s="48">
         <v>5113</v>
       </c>
-      <c r="BY3" s="48"/>
+      <c r="BY3" s="48">
+        <v>5145</v>
+      </c>
       <c r="BZ3" s="48"/>
       <c r="CA3" s="48"/>
       <c r="CB3" s="48"/>
@@ -15035,7 +15218,9 @@
       <c r="BX4" s="48">
         <v>5113</v>
       </c>
-      <c r="BY4" s="48"/>
+      <c r="BY4" s="48">
+        <v>5145</v>
+      </c>
       <c r="BZ4" s="48"/>
       <c r="CA4" s="48"/>
       <c r="CB4" s="48"/>
@@ -15270,7 +15455,9 @@
       <c r="BX5" s="48">
         <v>5113</v>
       </c>
-      <c r="BY5" s="48"/>
+      <c r="BY5" s="48">
+        <v>5145</v>
+      </c>
       <c r="BZ5" s="48"/>
       <c r="CA5" s="48"/>
       <c r="CB5" s="48"/>
@@ -15505,7 +15692,9 @@
       <c r="BX6" s="48">
         <v>5113</v>
       </c>
-      <c r="BY6" s="48"/>
+      <c r="BY6" s="48">
+        <v>5145</v>
+      </c>
       <c r="BZ6" s="48"/>
       <c r="CA6" s="48"/>
       <c r="CB6" s="48"/>
@@ -15740,7 +15929,9 @@
       <c r="BX7" s="48">
         <v>4423</v>
       </c>
-      <c r="BY7" s="48"/>
+      <c r="BY7" s="48">
+        <v>4455</v>
+      </c>
       <c r="BZ7" s="48"/>
       <c r="CA7" s="48"/>
       <c r="CB7" s="48"/>
@@ -15975,7 +16166,9 @@
       <c r="BX8" s="48">
         <v>7054</v>
       </c>
-      <c r="BY8" s="48"/>
+      <c r="BY8" s="48">
+        <v>7086</v>
+      </c>
       <c r="BZ8" s="48"/>
       <c r="CA8" s="48"/>
       <c r="CB8" s="48"/>
@@ -16300,7 +16493,9 @@
       <c r="BX10" s="48">
         <v>215</v>
       </c>
-      <c r="BY10" s="48"/>
+      <c r="BY10" s="48">
+        <v>216</v>
+      </c>
       <c r="BZ10" s="48"/>
       <c r="CA10" s="48"/>
       <c r="CB10" s="48"/>
@@ -16535,7 +16730,9 @@
       <c r="BX11" s="48">
         <v>215</v>
       </c>
-      <c r="BY11" s="48"/>
+      <c r="BY11" s="48">
+        <v>216</v>
+      </c>
       <c r="BZ11" s="48"/>
       <c r="CA11" s="48"/>
       <c r="CB11" s="48"/>
@@ -16770,7 +16967,9 @@
       <c r="BX12" s="48">
         <v>215</v>
       </c>
-      <c r="BY12" s="48"/>
+      <c r="BY12" s="48">
+        <v>216</v>
+      </c>
       <c r="BZ12" s="48"/>
       <c r="CA12" s="48"/>
       <c r="CB12" s="48"/>
@@ -17005,7 +17204,9 @@
       <c r="BX13" s="48">
         <v>215</v>
       </c>
-      <c r="BY13" s="48"/>
+      <c r="BY13" s="48">
+        <v>216</v>
+      </c>
       <c r="BZ13" s="48"/>
       <c r="CA13" s="48"/>
       <c r="CB13" s="48"/>
@@ -17240,7 +17441,9 @@
       <c r="BX14" s="48">
         <v>215</v>
       </c>
-      <c r="BY14" s="48"/>
+      <c r="BY14" s="48">
+        <v>216</v>
+      </c>
       <c r="BZ14" s="48"/>
       <c r="CA14" s="48"/>
       <c r="CB14" s="48"/>
@@ -17475,7 +17678,9 @@
       <c r="BX15" s="48">
         <v>150</v>
       </c>
-      <c r="BY15" s="48"/>
+      <c r="BY15" s="48">
+        <v>151</v>
+      </c>
       <c r="BZ15" s="48"/>
       <c r="CA15" s="48"/>
       <c r="CB15" s="48"/>
@@ -17710,7 +17915,9 @@
       <c r="BX16" s="48">
         <v>227</v>
       </c>
-      <c r="BY16" s="48"/>
+      <c r="BY16" s="48">
+        <v>228</v>
+      </c>
       <c r="BZ16" s="48"/>
       <c r="CA16" s="48"/>
       <c r="CB16" s="48"/>
@@ -18031,6 +18238,9 @@
       <c r="BX18">
         <v>1234</v>
       </c>
+      <c r="BY18" s="216">
+        <v>1241</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -18208,7 +18418,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BX20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BY20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -18342,6 +18552,10 @@
       <c r="BX20" s="51">
         <f t="shared" si="1"/>
         <v>39929</v>
+      </c>
+      <c r="BY20" s="51">
+        <f t="shared" si="1"/>
+        <v>40167</v>
       </c>
     </row>
   </sheetData>
@@ -18641,43 +18855,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="717" t="s">
+      <c r="B8" s="726" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="717"/>
+      <c r="B9" s="726"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="717"/>
+      <c r="B10" s="726"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="717"/>
+      <c r="B11" s="726"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="718" t="s">
+      <c r="B12" s="727" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="718"/>
+      <c r="B13" s="727"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="718"/>
+      <c r="B14" s="727"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="719" t="s">
+      <c r="B15" s="728" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="719"/>
+      <c r="B16" s="728"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean from SSA for July 17th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA86839-4EB6-FE4F-A2A3-976BB72927B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99D036-3D4B-0149-A408-CB16F6F04896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>Las observaciones de sx_nal se mantuvieron</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -600,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="730">
+  <cellXfs count="739">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2719,6 +2716,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2728,7 +2752,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3048,7 +3074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
@@ -5523,6 +5549,38 @@
         <v>1171007</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="15">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="726">
+        <v>522162</v>
+      </c>
+      <c r="C78" s="727">
+        <v>573723</v>
+      </c>
+      <c r="D78" s="728">
+        <v>81046</v>
+      </c>
+      <c r="E78" s="729">
+        <v>56757</v>
+      </c>
+      <c r="F78" s="730">
+        <v>26.206426358103425</v>
+      </c>
+      <c r="G78" s="731">
+        <v>136840</v>
+      </c>
+      <c r="H78" s="732">
+        <v>11021</v>
+      </c>
+      <c r="I78" s="733">
+        <v>13295</v>
+      </c>
+      <c r="J78" s="734">
+        <v>1176931</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5530,11 +5588,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
+      <selection pane="bottomLeft" activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8385,8 +8443,8 @@
       <c r="A77" s="15">
         <v>44058</v>
       </c>
-      <c r="B77" s="729" t="s">
-        <v>82</v>
+      <c r="B77" s="550">
+        <v>0</v>
       </c>
       <c r="C77" s="216">
         <v>1</v>
@@ -8416,6 +8474,44 @@
         <v>0</v>
       </c>
       <c r="L77" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>1</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>1</v>
+      </c>
+      <c r="G78" s="216">
+        <v>0</v>
+      </c>
+      <c r="H78" s="216">
+        <v>0</v>
+      </c>
+      <c r="I78" s="216">
+        <v>0</v>
+      </c>
+      <c r="J78" s="216">
+        <v>0</v>
+      </c>
+      <c r="K78" s="216">
+        <v>0</v>
+      </c>
+      <c r="L78" s="216">
         <v>4</v>
       </c>
     </row>
@@ -8426,11 +8522,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O77" sqref="O77"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11769,6 +11865,50 @@
         <v>0</v>
       </c>
       <c r="N77" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>1</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>0</v>
+      </c>
+      <c r="G78" s="216">
+        <v>0</v>
+      </c>
+      <c r="H78" s="216">
+        <v>1</v>
+      </c>
+      <c r="I78" s="216">
+        <v>0</v>
+      </c>
+      <c r="J78" s="216">
+        <v>0</v>
+      </c>
+      <c r="K78" s="216">
+        <v>1</v>
+      </c>
+      <c r="L78" s="216">
+        <v>0</v>
+      </c>
+      <c r="M78" s="216">
+        <v>0</v>
+      </c>
+      <c r="N78" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11779,11 +11919,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <selection pane="bottomLeft" activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14260,6 +14400,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>0</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>2</v>
+      </c>
+      <c r="G78" s="216">
+        <v>1</v>
+      </c>
+      <c r="H78" s="216">
+        <v>1</v>
+      </c>
+      <c r="I78" s="216">
+        <v>1</v>
+      </c>
+      <c r="J78" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14270,7 +14442,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="CB21" sqref="CB21"/>
+      <selection activeCell="BY1" sqref="BY1:BZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14510,7 +14682,9 @@
       <c r="BY1" s="49">
         <v>44058</v>
       </c>
-      <c r="BZ1" s="48"/>
+      <c r="BZ1" s="49">
+        <v>44059</v>
+      </c>
       <c r="CA1" s="48"/>
       <c r="CB1" s="48"/>
       <c r="CC1" s="48"/>
@@ -14747,7 +14921,9 @@
       <c r="BY2" s="48">
         <v>5346</v>
       </c>
-      <c r="BZ2" s="48"/>
+      <c r="BZ2" s="48">
+        <v>5378</v>
+      </c>
       <c r="CA2" s="48"/>
       <c r="CB2" s="48"/>
       <c r="CC2" s="48"/>
@@ -14984,7 +15160,9 @@
       <c r="BY3" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ3" s="48"/>
+      <c r="BZ3" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA3" s="48"/>
       <c r="CB3" s="48"/>
       <c r="CC3" s="48"/>
@@ -15221,7 +15399,9 @@
       <c r="BY4" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ4" s="48"/>
+      <c r="BZ4" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA4" s="48"/>
       <c r="CB4" s="48"/>
       <c r="CC4" s="48"/>
@@ -15458,7 +15638,9 @@
       <c r="BY5" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ5" s="48"/>
+      <c r="BZ5" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA5" s="48"/>
       <c r="CB5" s="48"/>
       <c r="CC5" s="48"/>
@@ -15695,7 +15877,9 @@
       <c r="BY6" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ6" s="48"/>
+      <c r="BZ6" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="48"/>
       <c r="CC6" s="48"/>
@@ -15932,7 +16116,9 @@
       <c r="BY7" s="48">
         <v>4455</v>
       </c>
-      <c r="BZ7" s="48"/>
+      <c r="BZ7" s="48">
+        <v>4487</v>
+      </c>
       <c r="CA7" s="48"/>
       <c r="CB7" s="48"/>
       <c r="CC7" s="48"/>
@@ -16169,7 +16355,9 @@
       <c r="BY8" s="48">
         <v>7086</v>
       </c>
-      <c r="BZ8" s="48"/>
+      <c r="BZ8" s="48">
+        <v>7118</v>
+      </c>
       <c r="CA8" s="48"/>
       <c r="CB8" s="48"/>
       <c r="CC8" s="48"/>
@@ -16496,7 +16684,9 @@
       <c r="BY10" s="48">
         <v>216</v>
       </c>
-      <c r="BZ10" s="48"/>
+      <c r="BZ10" s="48">
+        <v>217</v>
+      </c>
       <c r="CA10" s="48"/>
       <c r="CB10" s="48"/>
       <c r="CC10" s="48"/>
@@ -16733,7 +16923,9 @@
       <c r="BY11" s="48">
         <v>216</v>
       </c>
-      <c r="BZ11" s="48"/>
+      <c r="BZ11" s="48">
+        <v>217</v>
+      </c>
       <c r="CA11" s="48"/>
       <c r="CB11" s="48"/>
       <c r="CC11" s="48"/>
@@ -16970,7 +17162,9 @@
       <c r="BY12" s="48">
         <v>216</v>
       </c>
-      <c r="BZ12" s="48"/>
+      <c r="BZ12" s="48">
+        <v>217</v>
+      </c>
       <c r="CA12" s="48"/>
       <c r="CB12" s="48"/>
       <c r="CC12" s="48"/>
@@ -17207,7 +17401,9 @@
       <c r="BY13" s="48">
         <v>216</v>
       </c>
-      <c r="BZ13" s="48"/>
+      <c r="BZ13" s="48">
+        <v>217</v>
+      </c>
       <c r="CA13" s="48"/>
       <c r="CB13" s="48"/>
       <c r="CC13" s="48"/>
@@ -17444,7 +17640,9 @@
       <c r="BY14" s="48">
         <v>216</v>
       </c>
-      <c r="BZ14" s="48"/>
+      <c r="BZ14" s="48">
+        <v>217</v>
+      </c>
       <c r="CA14" s="48"/>
       <c r="CB14" s="48"/>
       <c r="CC14" s="48"/>
@@ -17681,7 +17879,9 @@
       <c r="BY15" s="48">
         <v>151</v>
       </c>
-      <c r="BZ15" s="48"/>
+      <c r="BZ15" s="48">
+        <v>152</v>
+      </c>
       <c r="CA15" s="48"/>
       <c r="CB15" s="48"/>
       <c r="CC15" s="48"/>
@@ -17918,7 +18118,9 @@
       <c r="BY16" s="48">
         <v>228</v>
       </c>
-      <c r="BZ16" s="48"/>
+      <c r="BZ16" s="48">
+        <v>229</v>
+      </c>
       <c r="CA16" s="48"/>
       <c r="CB16" s="48"/>
       <c r="CC16" s="48"/>
@@ -18241,6 +18443,9 @@
       <c r="BY18" s="216">
         <v>1241</v>
       </c>
+      <c r="BZ18" s="216">
+        <v>1248</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -18418,7 +18623,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BY20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BZ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -18556,6 +18761,10 @@
       <c r="BY20" s="51">
         <f t="shared" si="1"/>
         <v>40167</v>
+      </c>
+      <c r="BZ20" s="51">
+        <f t="shared" si="1"/>
+        <v>40405</v>
       </c>
     </row>
   </sheetData>
@@ -18855,43 +19064,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="726" t="s">
+      <c r="B8" s="735" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="726"/>
+      <c r="B9" s="735"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="726"/>
+      <c r="B10" s="735"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="726"/>
+      <c r="B11" s="735"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="727" t="s">
+      <c r="B12" s="736" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="727"/>
+      <c r="B13" s="736"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="727"/>
+      <c r="B14" s="736"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="728" t="s">
+      <c r="B15" s="737" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="728"/>
+      <c r="B16" s="737"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA dor August 16th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA86839-4EB6-FE4F-A2A3-976BB72927B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99D036-3D4B-0149-A408-CB16F6F04896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>Las observaciones de sx_nal se mantuvieron</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -600,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="730">
+  <cellXfs count="739">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2719,6 +2716,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2728,7 +2752,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3048,7 +3074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
@@ -5523,6 +5549,38 @@
         <v>1171007</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="15">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="726">
+        <v>522162</v>
+      </c>
+      <c r="C78" s="727">
+        <v>573723</v>
+      </c>
+      <c r="D78" s="728">
+        <v>81046</v>
+      </c>
+      <c r="E78" s="729">
+        <v>56757</v>
+      </c>
+      <c r="F78" s="730">
+        <v>26.206426358103425</v>
+      </c>
+      <c r="G78" s="731">
+        <v>136840</v>
+      </c>
+      <c r="H78" s="732">
+        <v>11021</v>
+      </c>
+      <c r="I78" s="733">
+        <v>13295</v>
+      </c>
+      <c r="J78" s="734">
+        <v>1176931</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5530,11 +5588,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
+      <selection pane="bottomLeft" activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8385,8 +8443,8 @@
       <c r="A77" s="15">
         <v>44058</v>
       </c>
-      <c r="B77" s="729" t="s">
-        <v>82</v>
+      <c r="B77" s="550">
+        <v>0</v>
       </c>
       <c r="C77" s="216">
         <v>1</v>
@@ -8416,6 +8474,44 @@
         <v>0</v>
       </c>
       <c r="L77" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>1</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>1</v>
+      </c>
+      <c r="G78" s="216">
+        <v>0</v>
+      </c>
+      <c r="H78" s="216">
+        <v>0</v>
+      </c>
+      <c r="I78" s="216">
+        <v>0</v>
+      </c>
+      <c r="J78" s="216">
+        <v>0</v>
+      </c>
+      <c r="K78" s="216">
+        <v>0</v>
+      </c>
+      <c r="L78" s="216">
         <v>4</v>
       </c>
     </row>
@@ -8426,11 +8522,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O77" sqref="O77"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11769,6 +11865,50 @@
         <v>0</v>
       </c>
       <c r="N77" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>1</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>0</v>
+      </c>
+      <c r="G78" s="216">
+        <v>0</v>
+      </c>
+      <c r="H78" s="216">
+        <v>1</v>
+      </c>
+      <c r="I78" s="216">
+        <v>0</v>
+      </c>
+      <c r="J78" s="216">
+        <v>0</v>
+      </c>
+      <c r="K78" s="216">
+        <v>1</v>
+      </c>
+      <c r="L78" s="216">
+        <v>0</v>
+      </c>
+      <c r="M78" s="216">
+        <v>0</v>
+      </c>
+      <c r="N78" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11779,11 +11919,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <selection pane="bottomLeft" activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14260,6 +14400,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="738">
+        <v>44059</v>
+      </c>
+      <c r="B78" s="216">
+        <v>0</v>
+      </c>
+      <c r="C78" s="216">
+        <v>0</v>
+      </c>
+      <c r="D78" s="216">
+        <v>0</v>
+      </c>
+      <c r="E78" s="216">
+        <v>0</v>
+      </c>
+      <c r="F78" s="216">
+        <v>2</v>
+      </c>
+      <c r="G78" s="216">
+        <v>1</v>
+      </c>
+      <c r="H78" s="216">
+        <v>1</v>
+      </c>
+      <c r="I78" s="216">
+        <v>1</v>
+      </c>
+      <c r="J78" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14270,7 +14442,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="CB21" sqref="CB21"/>
+      <selection activeCell="BY1" sqref="BY1:BZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14510,7 +14682,9 @@
       <c r="BY1" s="49">
         <v>44058</v>
       </c>
-      <c r="BZ1" s="48"/>
+      <c r="BZ1" s="49">
+        <v>44059</v>
+      </c>
       <c r="CA1" s="48"/>
       <c r="CB1" s="48"/>
       <c r="CC1" s="48"/>
@@ -14747,7 +14921,9 @@
       <c r="BY2" s="48">
         <v>5346</v>
       </c>
-      <c r="BZ2" s="48"/>
+      <c r="BZ2" s="48">
+        <v>5378</v>
+      </c>
       <c r="CA2" s="48"/>
       <c r="CB2" s="48"/>
       <c r="CC2" s="48"/>
@@ -14984,7 +15160,9 @@
       <c r="BY3" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ3" s="48"/>
+      <c r="BZ3" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA3" s="48"/>
       <c r="CB3" s="48"/>
       <c r="CC3" s="48"/>
@@ -15221,7 +15399,9 @@
       <c r="BY4" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ4" s="48"/>
+      <c r="BZ4" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA4" s="48"/>
       <c r="CB4" s="48"/>
       <c r="CC4" s="48"/>
@@ -15458,7 +15638,9 @@
       <c r="BY5" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ5" s="48"/>
+      <c r="BZ5" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA5" s="48"/>
       <c r="CB5" s="48"/>
       <c r="CC5" s="48"/>
@@ -15695,7 +15877,9 @@
       <c r="BY6" s="48">
         <v>5145</v>
       </c>
-      <c r="BZ6" s="48"/>
+      <c r="BZ6" s="48">
+        <v>5177</v>
+      </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="48"/>
       <c r="CC6" s="48"/>
@@ -15932,7 +16116,9 @@
       <c r="BY7" s="48">
         <v>4455</v>
       </c>
-      <c r="BZ7" s="48"/>
+      <c r="BZ7" s="48">
+        <v>4487</v>
+      </c>
       <c r="CA7" s="48"/>
       <c r="CB7" s="48"/>
       <c r="CC7" s="48"/>
@@ -16169,7 +16355,9 @@
       <c r="BY8" s="48">
         <v>7086</v>
       </c>
-      <c r="BZ8" s="48"/>
+      <c r="BZ8" s="48">
+        <v>7118</v>
+      </c>
       <c r="CA8" s="48"/>
       <c r="CB8" s="48"/>
       <c r="CC8" s="48"/>
@@ -16496,7 +16684,9 @@
       <c r="BY10" s="48">
         <v>216</v>
       </c>
-      <c r="BZ10" s="48"/>
+      <c r="BZ10" s="48">
+        <v>217</v>
+      </c>
       <c r="CA10" s="48"/>
       <c r="CB10" s="48"/>
       <c r="CC10" s="48"/>
@@ -16733,7 +16923,9 @@
       <c r="BY11" s="48">
         <v>216</v>
       </c>
-      <c r="BZ11" s="48"/>
+      <c r="BZ11" s="48">
+        <v>217</v>
+      </c>
       <c r="CA11" s="48"/>
       <c r="CB11" s="48"/>
       <c r="CC11" s="48"/>
@@ -16970,7 +17162,9 @@
       <c r="BY12" s="48">
         <v>216</v>
       </c>
-      <c r="BZ12" s="48"/>
+      <c r="BZ12" s="48">
+        <v>217</v>
+      </c>
       <c r="CA12" s="48"/>
       <c r="CB12" s="48"/>
       <c r="CC12" s="48"/>
@@ -17207,7 +17401,9 @@
       <c r="BY13" s="48">
         <v>216</v>
       </c>
-      <c r="BZ13" s="48"/>
+      <c r="BZ13" s="48">
+        <v>217</v>
+      </c>
       <c r="CA13" s="48"/>
       <c r="CB13" s="48"/>
       <c r="CC13" s="48"/>
@@ -17444,7 +17640,9 @@
       <c r="BY14" s="48">
         <v>216</v>
       </c>
-      <c r="BZ14" s="48"/>
+      <c r="BZ14" s="48">
+        <v>217</v>
+      </c>
       <c r="CA14" s="48"/>
       <c r="CB14" s="48"/>
       <c r="CC14" s="48"/>
@@ -17681,7 +17879,9 @@
       <c r="BY15" s="48">
         <v>151</v>
       </c>
-      <c r="BZ15" s="48"/>
+      <c r="BZ15" s="48">
+        <v>152</v>
+      </c>
       <c r="CA15" s="48"/>
       <c r="CB15" s="48"/>
       <c r="CC15" s="48"/>
@@ -17918,7 +18118,9 @@
       <c r="BY16" s="48">
         <v>228</v>
       </c>
-      <c r="BZ16" s="48"/>
+      <c r="BZ16" s="48">
+        <v>229</v>
+      </c>
       <c r="CA16" s="48"/>
       <c r="CB16" s="48"/>
       <c r="CC16" s="48"/>
@@ -18241,6 +18443,9 @@
       <c r="BY18" s="216">
         <v>1241</v>
       </c>
+      <c r="BZ18" s="216">
+        <v>1248</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -18418,7 +18623,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BY20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:BZ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -18556,6 +18761,10 @@
       <c r="BY20" s="51">
         <f t="shared" si="1"/>
         <v>40167</v>
+      </c>
+      <c r="BZ20" s="51">
+        <f t="shared" si="1"/>
+        <v>40405</v>
       </c>
     </row>
   </sheetData>
@@ -18855,43 +19064,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="726" t="s">
+      <c r="B8" s="735" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="726"/>
+      <c r="B9" s="735"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="726"/>
+      <c r="B10" s="735"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="726"/>
+      <c r="B11" s="735"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="727" t="s">
+      <c r="B12" s="736" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="727"/>
+      <c r="B13" s="736"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="727"/>
+      <c r="B14" s="736"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="728" t="s">
+      <c r="B15" s="737" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="728"/>
+      <c r="B16" s="737"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 17th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99D036-3D4B-0149-A408-CB16F6F04896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23DD838-9E07-2D4F-A480-73063CFB5EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="9800" yWindow="460" windowWidth="24720" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="739">
+  <cellXfs count="748">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2743,6 +2743,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2751,9 +2781,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3074,10 +3101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5581,6 +5608,38 @@
         <v>1176931</v>
       </c>
     </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="15">
+        <v>44060</v>
+      </c>
+      <c r="B79" s="736">
+        <v>525733</v>
+      </c>
+      <c r="C79" s="737">
+        <v>577531</v>
+      </c>
+      <c r="D79" s="738">
+        <v>78431</v>
+      </c>
+      <c r="E79" s="739">
+        <v>57023</v>
+      </c>
+      <c r="F79" s="740">
+        <v>26.171840078518944</v>
+      </c>
+      <c r="G79" s="741">
+        <v>137594</v>
+      </c>
+      <c r="H79" s="742">
+        <v>11065</v>
+      </c>
+      <c r="I79" s="743">
+        <v>13335</v>
+      </c>
+      <c r="J79" s="744">
+        <v>1181695</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5588,11 +5647,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L78" sqref="L78"/>
+      <selection pane="bottomLeft" activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8478,7 +8537,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A78" s="738">
+      <c r="A78" s="735">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -8512,6 +8571,44 @@
         <v>0</v>
       </c>
       <c r="L78" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="15">
+        <v>44060</v>
+      </c>
+      <c r="B79" s="216">
+        <v>0</v>
+      </c>
+      <c r="C79" s="216">
+        <v>1</v>
+      </c>
+      <c r="D79" s="216">
+        <v>0</v>
+      </c>
+      <c r="E79" s="216">
+        <v>0</v>
+      </c>
+      <c r="F79" s="216">
+        <v>1</v>
+      </c>
+      <c r="G79" s="216">
+        <v>0</v>
+      </c>
+      <c r="H79" s="216">
+        <v>0</v>
+      </c>
+      <c r="I79" s="216">
+        <v>0</v>
+      </c>
+      <c r="J79" s="216">
+        <v>0</v>
+      </c>
+      <c r="K79" s="216">
+        <v>0</v>
+      </c>
+      <c r="L79" s="216">
         <v>4</v>
       </c>
     </row>
@@ -8522,11 +8619,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O78" sqref="O78"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O79" sqref="O79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11869,7 +11966,7 @@
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A78" s="738">
+      <c r="A78" s="735">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -11909,6 +12006,50 @@
         <v>0</v>
       </c>
       <c r="N78" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="15">
+        <v>44060</v>
+      </c>
+      <c r="B79" s="216">
+        <v>0</v>
+      </c>
+      <c r="C79" s="216">
+        <v>1</v>
+      </c>
+      <c r="D79" s="216">
+        <v>0</v>
+      </c>
+      <c r="E79" s="216">
+        <v>0</v>
+      </c>
+      <c r="F79" s="216">
+        <v>0</v>
+      </c>
+      <c r="G79" s="216">
+        <v>0</v>
+      </c>
+      <c r="H79" s="216">
+        <v>1</v>
+      </c>
+      <c r="I79" s="216">
+        <v>0</v>
+      </c>
+      <c r="J79" s="216">
+        <v>0</v>
+      </c>
+      <c r="K79" s="216">
+        <v>1</v>
+      </c>
+      <c r="L79" s="216">
+        <v>0</v>
+      </c>
+      <c r="M79" s="216">
+        <v>0</v>
+      </c>
+      <c r="N79" s="216">
         <v>0</v>
       </c>
     </row>
@@ -11919,11 +12060,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K78" sqref="K78"/>
+      <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14401,7 +14542,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" s="738">
+      <c r="A78" s="735">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -14429,6 +14570,38 @@
         <v>1</v>
       </c>
       <c r="J78" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" s="15">
+        <v>44060</v>
+      </c>
+      <c r="B79" s="216">
+        <v>0</v>
+      </c>
+      <c r="C79" s="216">
+        <v>0</v>
+      </c>
+      <c r="D79" s="216">
+        <v>0</v>
+      </c>
+      <c r="E79" s="216">
+        <v>0</v>
+      </c>
+      <c r="F79" s="216">
+        <v>2</v>
+      </c>
+      <c r="G79" s="216">
+        <v>1</v>
+      </c>
+      <c r="H79" s="216">
+        <v>1</v>
+      </c>
+      <c r="I79" s="216">
+        <v>1</v>
+      </c>
+      <c r="J79" s="216">
         <v>2</v>
       </c>
     </row>
@@ -14441,8 +14614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BY1" sqref="BY1:BZ1"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="CA24" sqref="CA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14685,7 +14858,9 @@
       <c r="BZ1" s="49">
         <v>44059</v>
       </c>
-      <c r="CA1" s="48"/>
+      <c r="CA1" s="49">
+        <v>44060</v>
+      </c>
       <c r="CB1" s="48"/>
       <c r="CC1" s="48"/>
     </row>
@@ -14924,7 +15099,9 @@
       <c r="BZ2" s="48">
         <v>5378</v>
       </c>
-      <c r="CA2" s="48"/>
+      <c r="CA2" s="48">
+        <v>5410</v>
+      </c>
       <c r="CB2" s="48"/>
       <c r="CC2" s="48"/>
     </row>
@@ -15163,7 +15340,9 @@
       <c r="BZ3" s="48">
         <v>5177</v>
       </c>
-      <c r="CA3" s="48"/>
+      <c r="CA3" s="48">
+        <v>5209</v>
+      </c>
       <c r="CB3" s="48"/>
       <c r="CC3" s="48"/>
     </row>
@@ -15402,7 +15581,9 @@
       <c r="BZ4" s="48">
         <v>5177</v>
       </c>
-      <c r="CA4" s="48"/>
+      <c r="CA4" s="48">
+        <v>5209</v>
+      </c>
       <c r="CB4" s="48"/>
       <c r="CC4" s="48"/>
     </row>
@@ -15641,7 +15822,9 @@
       <c r="BZ5" s="48">
         <v>5177</v>
       </c>
-      <c r="CA5" s="48"/>
+      <c r="CA5" s="48">
+        <v>5209</v>
+      </c>
       <c r="CB5" s="48"/>
       <c r="CC5" s="48"/>
     </row>
@@ -15880,7 +16063,9 @@
       <c r="BZ6" s="48">
         <v>5177</v>
       </c>
-      <c r="CA6" s="48"/>
+      <c r="CA6" s="48">
+        <v>5209</v>
+      </c>
       <c r="CB6" s="48"/>
       <c r="CC6" s="48"/>
     </row>
@@ -16119,7 +16304,9 @@
       <c r="BZ7" s="48">
         <v>4487</v>
       </c>
-      <c r="CA7" s="48"/>
+      <c r="CA7" s="48">
+        <v>4519</v>
+      </c>
       <c r="CB7" s="48"/>
       <c r="CC7" s="48"/>
     </row>
@@ -16358,7 +16545,9 @@
       <c r="BZ8" s="48">
         <v>7118</v>
       </c>
-      <c r="CA8" s="48"/>
+      <c r="CA8" s="48">
+        <v>7150</v>
+      </c>
       <c r="CB8" s="48"/>
       <c r="CC8" s="48"/>
     </row>
@@ -16687,7 +16876,9 @@
       <c r="BZ10" s="48">
         <v>217</v>
       </c>
-      <c r="CA10" s="48"/>
+      <c r="CA10" s="48">
+        <v>218</v>
+      </c>
       <c r="CB10" s="48"/>
       <c r="CC10" s="48"/>
     </row>
@@ -16926,7 +17117,9 @@
       <c r="BZ11" s="48">
         <v>217</v>
       </c>
-      <c r="CA11" s="48"/>
+      <c r="CA11" s="48">
+        <v>218</v>
+      </c>
       <c r="CB11" s="48"/>
       <c r="CC11" s="48"/>
     </row>
@@ -17165,7 +17358,9 @@
       <c r="BZ12" s="48">
         <v>217</v>
       </c>
-      <c r="CA12" s="48"/>
+      <c r="CA12" s="48">
+        <v>218</v>
+      </c>
       <c r="CB12" s="48"/>
       <c r="CC12" s="48"/>
     </row>
@@ -17404,7 +17599,9 @@
       <c r="BZ13" s="48">
         <v>217</v>
       </c>
-      <c r="CA13" s="48"/>
+      <c r="CA13" s="48">
+        <v>218</v>
+      </c>
       <c r="CB13" s="48"/>
       <c r="CC13" s="48"/>
     </row>
@@ -17643,7 +17840,9 @@
       <c r="BZ14" s="48">
         <v>217</v>
       </c>
-      <c r="CA14" s="48"/>
+      <c r="CA14" s="48">
+        <v>218</v>
+      </c>
       <c r="CB14" s="48"/>
       <c r="CC14" s="48"/>
     </row>
@@ -17882,7 +18081,9 @@
       <c r="BZ15" s="48">
         <v>152</v>
       </c>
-      <c r="CA15" s="48"/>
+      <c r="CA15" s="48">
+        <v>153</v>
+      </c>
       <c r="CB15" s="48"/>
       <c r="CC15" s="48"/>
     </row>
@@ -18121,7 +18322,9 @@
       <c r="BZ16" s="48">
         <v>229</v>
       </c>
-      <c r="CA16" s="48"/>
+      <c r="CA16" s="48">
+        <v>230</v>
+      </c>
       <c r="CB16" s="48"/>
       <c r="CC16" s="48"/>
     </row>
@@ -18446,6 +18649,9 @@
       <c r="BZ18" s="216">
         <v>1248</v>
       </c>
+      <c r="CA18">
+        <v>1255</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -18623,7 +18829,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:BZ20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CA20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -18765,6 +18971,10 @@
       <c r="BZ20" s="51">
         <f t="shared" si="1"/>
         <v>40405</v>
+      </c>
+      <c r="CA20" s="51">
+        <f t="shared" si="1"/>
+        <v>40643</v>
       </c>
     </row>
   </sheetData>
@@ -19064,43 +19274,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="735" t="s">
+      <c r="B8" s="745" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="735"/>
+      <c r="B9" s="745"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="735"/>
+      <c r="B10" s="745"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="735"/>
+      <c r="B11" s="745"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="736" t="s">
+      <c r="B12" s="746" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="736"/>
+      <c r="B13" s="746"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="736"/>
+      <c r="B14" s="746"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="737" t="s">
+      <c r="B15" s="747" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="737"/>
+      <c r="B16" s="747"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 18th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23DD838-9E07-2D4F-A480-73063CFB5EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C12A5C-E6F1-C244-9649-DF859127A6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="460" windowWidth="24720" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="4080" yWindow="460" windowWidth="24720" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="748">
+  <cellXfs count="757">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2744,6 +2744,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3101,10 +3128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5640,6 +5667,38 @@
         <v>1181695</v>
       </c>
     </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="15">
+        <v>44061</v>
+      </c>
+      <c r="B80" s="745">
+        <v>531239</v>
+      </c>
+      <c r="C80" s="746">
+        <v>584293</v>
+      </c>
+      <c r="D80" s="747">
+        <v>81175</v>
+      </c>
+      <c r="E80" s="748">
+        <v>57774</v>
+      </c>
+      <c r="F80" s="749">
+        <v>26.150941478317669</v>
+      </c>
+      <c r="G80" s="750">
+        <v>138924</v>
+      </c>
+      <c r="H80" s="751">
+        <v>11220</v>
+      </c>
+      <c r="I80" s="752">
+        <v>13507</v>
+      </c>
+      <c r="J80" s="753">
+        <v>1196707</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5647,11 +5706,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L79" sqref="L79"/>
+      <selection pane="bottomLeft" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8612,6 +8671,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="15">
+        <v>44061</v>
+      </c>
+      <c r="B80" s="216">
+        <v>0</v>
+      </c>
+      <c r="C80" s="216">
+        <v>1</v>
+      </c>
+      <c r="D80" s="216">
+        <v>0</v>
+      </c>
+      <c r="E80" s="216">
+        <v>0</v>
+      </c>
+      <c r="F80" s="216">
+        <v>1</v>
+      </c>
+      <c r="G80" s="216">
+        <v>0</v>
+      </c>
+      <c r="H80" s="216">
+        <v>0</v>
+      </c>
+      <c r="I80" s="216">
+        <v>0</v>
+      </c>
+      <c r="J80" s="216">
+        <v>0</v>
+      </c>
+      <c r="K80" s="216">
+        <v>0</v>
+      </c>
+      <c r="L80" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8619,11 +8716,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O79"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O79" sqref="O79"/>
+      <selection pane="bottomLeft" activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12050,6 +12147,50 @@
         <v>0</v>
       </c>
       <c r="N79" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="15">
+        <v>44061</v>
+      </c>
+      <c r="B80" s="216">
+        <v>0</v>
+      </c>
+      <c r="C80" s="216">
+        <v>1</v>
+      </c>
+      <c r="D80" s="216">
+        <v>0</v>
+      </c>
+      <c r="E80" s="216">
+        <v>0</v>
+      </c>
+      <c r="F80" s="216">
+        <v>0</v>
+      </c>
+      <c r="G80" s="216">
+        <v>0</v>
+      </c>
+      <c r="H80" s="216">
+        <v>1</v>
+      </c>
+      <c r="I80" s="216">
+        <v>0</v>
+      </c>
+      <c r="J80" s="216">
+        <v>0</v>
+      </c>
+      <c r="K80" s="216">
+        <v>1</v>
+      </c>
+      <c r="L80" s="216">
+        <v>0</v>
+      </c>
+      <c r="M80" s="216">
+        <v>0</v>
+      </c>
+      <c r="N80" s="216">
         <v>0</v>
       </c>
     </row>
@@ -12060,11 +12201,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K79" sqref="K79"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14605,6 +14746,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="15">
+        <v>44061</v>
+      </c>
+      <c r="B80" s="216">
+        <v>0</v>
+      </c>
+      <c r="C80" s="216">
+        <v>0</v>
+      </c>
+      <c r="D80" s="216">
+        <v>0</v>
+      </c>
+      <c r="E80" s="216">
+        <v>0</v>
+      </c>
+      <c r="F80" s="216">
+        <v>2</v>
+      </c>
+      <c r="G80" s="216">
+        <v>1</v>
+      </c>
+      <c r="H80" s="216">
+        <v>1</v>
+      </c>
+      <c r="I80" s="216">
+        <v>1</v>
+      </c>
+      <c r="J80" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14615,7 +14788,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="CA24" sqref="CA24"/>
+      <selection activeCell="CB23" sqref="CB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14861,7 +15034,9 @@
       <c r="CA1" s="49">
         <v>44060</v>
       </c>
-      <c r="CB1" s="48"/>
+      <c r="CB1" s="49">
+        <v>44061</v>
+      </c>
       <c r="CC1" s="48"/>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
@@ -15102,7 +15277,9 @@
       <c r="CA2" s="48">
         <v>5410</v>
       </c>
-      <c r="CB2" s="48"/>
+      <c r="CB2" s="48">
+        <v>5442</v>
+      </c>
       <c r="CC2" s="48"/>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.2">
@@ -15343,7 +15520,9 @@
       <c r="CA3" s="48">
         <v>5209</v>
       </c>
-      <c r="CB3" s="48"/>
+      <c r="CB3" s="48">
+        <v>5241</v>
+      </c>
       <c r="CC3" s="48"/>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.2">
@@ -15584,7 +15763,9 @@
       <c r="CA4" s="48">
         <v>5209</v>
       </c>
-      <c r="CB4" s="48"/>
+      <c r="CB4" s="48">
+        <v>5241</v>
+      </c>
       <c r="CC4" s="48"/>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.2">
@@ -15825,7 +16006,9 @@
       <c r="CA5" s="48">
         <v>5209</v>
       </c>
-      <c r="CB5" s="48"/>
+      <c r="CB5" s="48">
+        <v>5241</v>
+      </c>
       <c r="CC5" s="48"/>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
@@ -16066,7 +16249,9 @@
       <c r="CA6" s="48">
         <v>5209</v>
       </c>
-      <c r="CB6" s="48"/>
+      <c r="CB6" s="48">
+        <v>5241</v>
+      </c>
       <c r="CC6" s="48"/>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.2">
@@ -16307,7 +16492,9 @@
       <c r="CA7" s="48">
         <v>4519</v>
       </c>
-      <c r="CB7" s="48"/>
+      <c r="CB7" s="48">
+        <v>4551</v>
+      </c>
       <c r="CC7" s="48"/>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.2">
@@ -16548,7 +16735,9 @@
       <c r="CA8" s="48">
         <v>7150</v>
       </c>
-      <c r="CB8" s="48"/>
+      <c r="CB8" s="48">
+        <v>7182</v>
+      </c>
       <c r="CC8" s="48"/>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.2">
@@ -16879,7 +17068,9 @@
       <c r="CA10" s="48">
         <v>218</v>
       </c>
-      <c r="CB10" s="48"/>
+      <c r="CB10" s="48">
+        <v>219</v>
+      </c>
       <c r="CC10" s="48"/>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.2">
@@ -17120,7 +17311,9 @@
       <c r="CA11" s="48">
         <v>218</v>
       </c>
-      <c r="CB11" s="48"/>
+      <c r="CB11" s="48">
+        <v>219</v>
+      </c>
       <c r="CC11" s="48"/>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.2">
@@ -17361,7 +17554,9 @@
       <c r="CA12" s="48">
         <v>218</v>
       </c>
-      <c r="CB12" s="48"/>
+      <c r="CB12" s="48">
+        <v>219</v>
+      </c>
       <c r="CC12" s="48"/>
     </row>
     <row r="13" spans="1:88" x14ac:dyDescent="0.2">
@@ -17602,7 +17797,9 @@
       <c r="CA13" s="48">
         <v>218</v>
       </c>
-      <c r="CB13" s="48"/>
+      <c r="CB13" s="48">
+        <v>219</v>
+      </c>
       <c r="CC13" s="48"/>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.2">
@@ -17843,7 +18040,9 @@
       <c r="CA14" s="48">
         <v>218</v>
       </c>
-      <c r="CB14" s="48"/>
+      <c r="CB14" s="48">
+        <v>219</v>
+      </c>
       <c r="CC14" s="48"/>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.2">
@@ -18084,7 +18283,9 @@
       <c r="CA15" s="48">
         <v>153</v>
       </c>
-      <c r="CB15" s="48"/>
+      <c r="CB15" s="48">
+        <v>154</v>
+      </c>
       <c r="CC15" s="48"/>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.2">
@@ -18325,7 +18526,9 @@
       <c r="CA16" s="48">
         <v>230</v>
       </c>
-      <c r="CB16" s="48"/>
+      <c r="CB16" s="48">
+        <v>231</v>
+      </c>
       <c r="CC16" s="48"/>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.2">
@@ -18652,6 +18855,9 @@
       <c r="CA18">
         <v>1255</v>
       </c>
+      <c r="CB18" s="216">
+        <v>1262</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -18829,7 +19035,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CA20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CB20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -18975,6 +19181,10 @@
       <c r="CA20" s="51">
         <f t="shared" si="1"/>
         <v>40643</v>
+      </c>
+      <c r="CB20" s="51">
+        <f t="shared" si="1"/>
+        <v>40881</v>
       </c>
     </row>
   </sheetData>
@@ -19274,43 +19484,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="745" t="s">
+      <c r="B8" s="754" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="745"/>
+      <c r="B9" s="754"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="745"/>
+      <c r="B10" s="754"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="745"/>
+      <c r="B11" s="754"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="746" t="s">
+      <c r="B12" s="755" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="746"/>
+      <c r="B13" s="755"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="746"/>
+      <c r="B14" s="755"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="747" t="s">
+      <c r="B15" s="756" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="747"/>
+      <c r="B16" s="756"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 20th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C12A5C-E6F1-C244-9649-DF859127A6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50811E09-E9C9-D44E-981E-9EF33B6AF221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="460" windowWidth="24720" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="34480" yWindow="3100" windowWidth="24720" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="757">
+  <cellXfs count="765">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2743,7 +2743,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3128,10 +3152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5639,31 +5663,31 @@
       <c r="A79" s="15">
         <v>44060</v>
       </c>
-      <c r="B79" s="736">
+      <c r="B79" s="735">
         <v>525733</v>
       </c>
-      <c r="C79" s="737">
+      <c r="C79" s="736">
         <v>577531</v>
       </c>
-      <c r="D79" s="738">
+      <c r="D79" s="737">
         <v>78431</v>
       </c>
-      <c r="E79" s="739">
+      <c r="E79" s="738">
         <v>57023</v>
       </c>
-      <c r="F79" s="740">
+      <c r="F79" s="739">
         <v>26.171840078518944</v>
       </c>
-      <c r="G79" s="741">
+      <c r="G79" s="740">
         <v>137594</v>
       </c>
-      <c r="H79" s="742">
+      <c r="H79" s="741">
         <v>11065</v>
       </c>
-      <c r="I79" s="743">
+      <c r="I79" s="742">
         <v>13335</v>
       </c>
-      <c r="J79" s="744">
+      <c r="J79" s="743">
         <v>1181695</v>
       </c>
     </row>
@@ -5671,32 +5695,64 @@
       <c r="A80" s="15">
         <v>44061</v>
       </c>
-      <c r="B80" s="745">
+      <c r="B80" s="744">
         <v>531239</v>
       </c>
-      <c r="C80" s="746">
+      <c r="C80" s="745">
         <v>584293</v>
       </c>
-      <c r="D80" s="747">
+      <c r="D80" s="746">
         <v>81175</v>
       </c>
-      <c r="E80" s="748">
+      <c r="E80" s="747">
         <v>57774</v>
       </c>
-      <c r="F80" s="749">
+      <c r="F80" s="748">
         <v>26.150941478317669</v>
       </c>
-      <c r="G80" s="750">
+      <c r="G80" s="749">
         <v>138924</v>
       </c>
-      <c r="H80" s="751">
+      <c r="H80" s="750">
         <v>11220</v>
       </c>
-      <c r="I80" s="752">
+      <c r="I80" s="751">
         <v>13507</v>
       </c>
-      <c r="J80" s="753">
+      <c r="J80" s="752">
         <v>1196707</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="15">
+        <v>44062</v>
+      </c>
+      <c r="B81" s="753">
+        <v>537031</v>
+      </c>
+      <c r="C81" s="754">
+        <v>591637</v>
+      </c>
+      <c r="D81" s="755">
+        <v>82884</v>
+      </c>
+      <c r="E81" s="756">
+        <v>58481</v>
+      </c>
+      <c r="F81" s="757">
+        <v>26.089555351553262</v>
+      </c>
+      <c r="G81" s="758">
+        <v>140109</v>
+      </c>
+      <c r="H81" s="759">
+        <v>11364</v>
+      </c>
+      <c r="I81" s="760">
+        <v>13686</v>
+      </c>
+      <c r="J81" s="761">
+        <v>1211552</v>
       </c>
     </row>
   </sheetData>
@@ -5706,11 +5762,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I81" sqref="I81"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8330,7 +8386,7 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="15">
+      <c r="A71" s="217">
         <v>44052</v>
       </c>
       <c r="B71" s="216">
@@ -8368,7 +8424,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="15">
+      <c r="A72" s="217">
         <v>44053</v>
       </c>
       <c r="B72" s="216">
@@ -8406,7 +8462,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="15">
+      <c r="A73" s="217">
         <v>44054</v>
       </c>
       <c r="B73" s="216">
@@ -8444,7 +8500,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="15">
+      <c r="A74" s="217">
         <v>44055</v>
       </c>
       <c r="B74" s="216">
@@ -8482,7 +8538,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A75" s="15">
+      <c r="A75" s="217">
         <v>44056</v>
       </c>
       <c r="B75" s="216">
@@ -8520,7 +8576,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A76" s="15">
+      <c r="A76" s="217">
         <v>44057</v>
       </c>
       <c r="B76" s="216">
@@ -8558,7 +8614,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A77" s="15">
+      <c r="A77" s="217">
         <v>44058</v>
       </c>
       <c r="B77" s="550">
@@ -8596,7 +8652,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A78" s="735">
+      <c r="A78" s="217">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -8634,7 +8690,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A79" s="15">
+      <c r="A79" s="217">
         <v>44060</v>
       </c>
       <c r="B79" s="216">
@@ -8672,7 +8728,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" s="15">
+      <c r="A80" s="217">
         <v>44061</v>
       </c>
       <c r="B80" s="216">
@@ -8706,6 +8762,44 @@
         <v>0</v>
       </c>
       <c r="L80" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="217">
+        <v>44062</v>
+      </c>
+      <c r="B81" s="216">
+        <v>0</v>
+      </c>
+      <c r="C81" s="216">
+        <v>1</v>
+      </c>
+      <c r="D81" s="216">
+        <v>0</v>
+      </c>
+      <c r="E81" s="216">
+        <v>0</v>
+      </c>
+      <c r="F81" s="216">
+        <v>1</v>
+      </c>
+      <c r="G81" s="216">
+        <v>0</v>
+      </c>
+      <c r="H81" s="216">
+        <v>0</v>
+      </c>
+      <c r="I81" s="216">
+        <v>0</v>
+      </c>
+      <c r="J81" s="216">
+        <v>0</v>
+      </c>
+      <c r="K81" s="216">
+        <v>0</v>
+      </c>
+      <c r="L81" s="216">
         <v>4</v>
       </c>
     </row>
@@ -8716,11 +8810,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O80" sqref="O80"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11755,7 +11849,7 @@
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A71" s="15">
+      <c r="A71" s="217">
         <v>44052</v>
       </c>
       <c r="B71" s="216">
@@ -11799,7 +11893,7 @@
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A72" s="15">
+      <c r="A72" s="217">
         <v>44053</v>
       </c>
       <c r="B72" s="216">
@@ -11843,7 +11937,7 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="15">
+      <c r="A73" s="217">
         <v>44054</v>
       </c>
       <c r="B73" s="216">
@@ -11887,7 +11981,7 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="15">
+      <c r="A74" s="217">
         <v>44055</v>
       </c>
       <c r="B74" s="216">
@@ -11931,7 +12025,7 @@
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A75" s="15">
+      <c r="A75" s="217">
         <v>44056</v>
       </c>
       <c r="B75" s="216">
@@ -11975,7 +12069,7 @@
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A76" s="15">
+      <c r="A76" s="217">
         <v>44057</v>
       </c>
       <c r="B76" s="216">
@@ -12019,7 +12113,7 @@
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A77" s="15">
+      <c r="A77" s="217">
         <v>44058</v>
       </c>
       <c r="B77" s="216">
@@ -12063,7 +12157,7 @@
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A78" s="735">
+      <c r="A78" s="217">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -12107,7 +12201,7 @@
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A79" s="15">
+      <c r="A79" s="217">
         <v>44060</v>
       </c>
       <c r="B79" s="216">
@@ -12151,7 +12245,7 @@
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A80" s="15">
+      <c r="A80" s="217">
         <v>44061</v>
       </c>
       <c r="B80" s="216">
@@ -12191,6 +12285,50 @@
         <v>0</v>
       </c>
       <c r="N80" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" s="217">
+        <v>44062</v>
+      </c>
+      <c r="B81" s="216">
+        <v>0</v>
+      </c>
+      <c r="C81" s="216">
+        <v>1</v>
+      </c>
+      <c r="D81" s="216">
+        <v>0</v>
+      </c>
+      <c r="E81" s="216">
+        <v>0</v>
+      </c>
+      <c r="F81" s="216">
+        <v>0</v>
+      </c>
+      <c r="G81" s="216">
+        <v>0</v>
+      </c>
+      <c r="H81" s="216">
+        <v>1</v>
+      </c>
+      <c r="I81" s="216">
+        <v>0</v>
+      </c>
+      <c r="J81" s="216">
+        <v>0</v>
+      </c>
+      <c r="K81" s="216">
+        <v>1</v>
+      </c>
+      <c r="L81" s="216">
+        <v>0</v>
+      </c>
+      <c r="M81" s="216">
+        <v>0</v>
+      </c>
+      <c r="N81" s="216">
         <v>0</v>
       </c>
     </row>
@@ -12201,11 +12339,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14459,7 +14597,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" s="15">
+      <c r="A71" s="495">
         <v>44052</v>
       </c>
       <c r="B71" s="216">
@@ -14491,7 +14629,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" s="15">
+      <c r="A72" s="495">
         <v>44053</v>
       </c>
       <c r="B72" s="216">
@@ -14523,7 +14661,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" s="15">
+      <c r="A73" s="495">
         <v>44054</v>
       </c>
       <c r="B73" s="216">
@@ -14555,7 +14693,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" s="15">
+      <c r="A74" s="495">
         <v>44055</v>
       </c>
       <c r="B74" s="216">
@@ -14587,7 +14725,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" s="15">
+      <c r="A75" s="495">
         <v>44056</v>
       </c>
       <c r="B75" s="216">
@@ -14619,7 +14757,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="15">
+      <c r="A76" s="495">
         <v>44057</v>
       </c>
       <c r="B76" s="216">
@@ -14651,7 +14789,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" s="15">
+      <c r="A77" s="495">
         <v>44058</v>
       </c>
       <c r="B77" s="216">
@@ -14683,7 +14821,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" s="735">
+      <c r="A78" s="495">
         <v>44059</v>
       </c>
       <c r="B78" s="216">
@@ -14715,7 +14853,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="15">
+      <c r="A79" s="495">
         <v>44060</v>
       </c>
       <c r="B79" s="216">
@@ -14747,7 +14885,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80" s="15">
+      <c r="A80" s="495">
         <v>44061</v>
       </c>
       <c r="B80" s="216">
@@ -14775,6 +14913,38 @@
         <v>1</v>
       </c>
       <c r="J80" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="495">
+        <v>44062</v>
+      </c>
+      <c r="B81" s="216">
+        <v>0</v>
+      </c>
+      <c r="C81" s="216">
+        <v>0</v>
+      </c>
+      <c r="D81" s="216">
+        <v>0</v>
+      </c>
+      <c r="E81" s="216">
+        <v>0</v>
+      </c>
+      <c r="F81" s="216">
+        <v>2</v>
+      </c>
+      <c r="G81" s="216">
+        <v>1</v>
+      </c>
+      <c r="H81" s="216">
+        <v>1</v>
+      </c>
+      <c r="I81" s="216">
+        <v>1</v>
+      </c>
+      <c r="J81" s="216">
         <v>2</v>
       </c>
     </row>
@@ -14788,7 +14958,7 @@
   <dimension ref="A1:CJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="CB23" sqref="CB23"/>
+      <selection activeCell="CA13" sqref="CA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15037,7 +15207,13 @@
       <c r="CB1" s="49">
         <v>44061</v>
       </c>
-      <c r="CC1" s="48"/>
+      <c r="CC1" s="49">
+        <v>44062</v>
+      </c>
+      <c r="CD1" s="49"/>
+      <c r="CE1" s="49"/>
+      <c r="CF1" s="49"/>
+      <c r="CG1" s="49"/>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -15280,7 +15456,9 @@
       <c r="CB2" s="48">
         <v>5442</v>
       </c>
-      <c r="CC2" s="48"/>
+      <c r="CC2" s="48">
+        <v>5474</v>
+      </c>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -15523,7 +15701,9 @@
       <c r="CB3" s="48">
         <v>5241</v>
       </c>
-      <c r="CC3" s="48"/>
+      <c r="CC3" s="48">
+        <v>5273</v>
+      </c>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -15766,7 +15946,9 @@
       <c r="CB4" s="48">
         <v>5241</v>
       </c>
-      <c r="CC4" s="48"/>
+      <c r="CC4" s="48">
+        <v>5273</v>
+      </c>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -16009,7 +16191,9 @@
       <c r="CB5" s="48">
         <v>5241</v>
       </c>
-      <c r="CC5" s="48"/>
+      <c r="CC5" s="48">
+        <v>5273</v>
+      </c>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -16252,7 +16436,9 @@
       <c r="CB6" s="48">
         <v>5241</v>
       </c>
-      <c r="CC6" s="48"/>
+      <c r="CC6" s="48">
+        <v>5273</v>
+      </c>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -16495,7 +16681,9 @@
       <c r="CB7" s="48">
         <v>4551</v>
       </c>
-      <c r="CC7" s="48"/>
+      <c r="CC7" s="48">
+        <v>4583</v>
+      </c>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -16738,7 +16926,9 @@
       <c r="CB8" s="48">
         <v>7182</v>
       </c>
-      <c r="CC8" s="48"/>
+      <c r="CC8" s="48">
+        <v>7214</v>
+      </c>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
@@ -17071,7 +17261,9 @@
       <c r="CB10" s="48">
         <v>219</v>
       </c>
-      <c r="CC10" s="48"/>
+      <c r="CC10" s="48">
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -17314,7 +17506,9 @@
       <c r="CB11" s="48">
         <v>219</v>
       </c>
-      <c r="CC11" s="48"/>
+      <c r="CC11" s="48">
+        <v>220</v>
+      </c>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -17557,7 +17751,9 @@
       <c r="CB12" s="48">
         <v>219</v>
       </c>
-      <c r="CC12" s="48"/>
+      <c r="CC12" s="48">
+        <v>220</v>
+      </c>
     </row>
     <row r="13" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -17800,7 +17996,9 @@
       <c r="CB13" s="48">
         <v>219</v>
       </c>
-      <c r="CC13" s="48"/>
+      <c r="CC13" s="48">
+        <v>220</v>
+      </c>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -18043,7 +18241,9 @@
       <c r="CB14" s="48">
         <v>219</v>
       </c>
-      <c r="CC14" s="48"/>
+      <c r="CC14" s="48">
+        <v>220</v>
+      </c>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -18286,7 +18486,9 @@
       <c r="CB15" s="48">
         <v>154</v>
       </c>
-      <c r="CC15" s="48"/>
+      <c r="CC15" s="48">
+        <v>155</v>
+      </c>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -18529,7 +18731,9 @@
       <c r="CB16" s="48">
         <v>231</v>
       </c>
-      <c r="CC16" s="48"/>
+      <c r="CC16" s="48">
+        <v>232</v>
+      </c>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
@@ -18858,6 +19062,9 @@
       <c r="CB18" s="216">
         <v>1262</v>
       </c>
+      <c r="CC18">
+        <v>1269</v>
+      </c>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -19035,7 +19242,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CB20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CC20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -19185,6 +19392,10 @@
       <c r="CB20" s="51">
         <f t="shared" si="1"/>
         <v>40881</v>
+      </c>
+      <c r="CC20" s="51">
+        <f t="shared" si="1"/>
+        <v>41119</v>
       </c>
     </row>
   </sheetData>
@@ -19197,7 +19408,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19484,43 +19695,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="754" t="s">
+      <c r="B8" s="762" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="754"/>
+      <c r="B9" s="762"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="754"/>
+      <c r="B10" s="762"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="754"/>
+      <c r="B11" s="762"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="755" t="s">
+      <c r="B12" s="763" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="755"/>
+      <c r="B13" s="763"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="755"/>
+      <c r="B14" s="763"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="756" t="s">
+      <c r="B15" s="764" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="756"/>
+      <c r="B16" s="764"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 21th & 22th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F67F57-6F26-2F4A-B0F6-8459A2DEE5AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1EC0EC-7CA3-AE4D-8C17-12E0837A90C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="774">
+  <cellXfs count="792">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3179,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5814,6 +5868,70 @@
         <v>1226117</v>
       </c>
     </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="15">
+        <v>44064</v>
+      </c>
+      <c r="B83" s="771">
+        <v>549734</v>
+      </c>
+      <c r="C83" s="772">
+        <v>606446</v>
+      </c>
+      <c r="D83" s="773">
+        <v>82953</v>
+      </c>
+      <c r="E83" s="774">
+        <v>59610</v>
+      </c>
+      <c r="F83" s="775">
+        <v>25.901072154896731</v>
+      </c>
+      <c r="G83" s="776">
+        <v>142387</v>
+      </c>
+      <c r="H83" s="777">
+        <v>12200</v>
+      </c>
+      <c r="I83" s="778">
+        <v>17669</v>
+      </c>
+      <c r="J83" s="779">
+        <v>1239133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="15">
+        <v>44065</v>
+      </c>
+      <c r="B84" s="780">
+        <v>556216</v>
+      </c>
+      <c r="C84" s="781">
+        <v>614070</v>
+      </c>
+      <c r="D84" s="782">
+        <v>83146</v>
+      </c>
+      <c r="E84" s="783">
+        <v>60254</v>
+      </c>
+      <c r="F84" s="784">
+        <v>25.859737943532728</v>
+      </c>
+      <c r="G84" s="785">
+        <v>143836</v>
+      </c>
+      <c r="H84" s="786">
+        <v>12323</v>
+      </c>
+      <c r="I84" s="787">
+        <v>17809</v>
+      </c>
+      <c r="J84" s="788">
+        <v>1253432</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5821,11 +5939,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L82" sqref="L82"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8900,6 +9018,82 @@
         <v>4</v>
       </c>
     </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" s="15">
+        <v>44064</v>
+      </c>
+      <c r="B83" s="216">
+        <v>0</v>
+      </c>
+      <c r="C83" s="216">
+        <v>1</v>
+      </c>
+      <c r="D83" s="216">
+        <v>0</v>
+      </c>
+      <c r="E83" s="216">
+        <v>0</v>
+      </c>
+      <c r="F83" s="216">
+        <v>1</v>
+      </c>
+      <c r="G83" s="216">
+        <v>0</v>
+      </c>
+      <c r="H83" s="216">
+        <v>0</v>
+      </c>
+      <c r="I83" s="216">
+        <v>0</v>
+      </c>
+      <c r="J83" s="216">
+        <v>0</v>
+      </c>
+      <c r="K83" s="216">
+        <v>0</v>
+      </c>
+      <c r="L83" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" s="15">
+        <v>44065</v>
+      </c>
+      <c r="B84" s="216">
+        <v>0</v>
+      </c>
+      <c r="C84" s="216">
+        <v>1</v>
+      </c>
+      <c r="D84" s="216">
+        <v>0</v>
+      </c>
+      <c r="E84" s="216">
+        <v>0</v>
+      </c>
+      <c r="F84" s="216">
+        <v>1</v>
+      </c>
+      <c r="G84" s="216">
+        <v>0</v>
+      </c>
+      <c r="H84" s="216">
+        <v>0</v>
+      </c>
+      <c r="I84" s="216">
+        <v>0</v>
+      </c>
+      <c r="J84" s="216">
+        <v>0</v>
+      </c>
+      <c r="K84" s="216">
+        <v>0</v>
+      </c>
+      <c r="L84" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8907,11 +9101,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O82"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
+      <selection pane="bottomLeft" activeCell="O84" sqref="O84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12470,6 +12664,94 @@
         <v>0</v>
       </c>
       <c r="N82" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" s="15">
+        <v>44064</v>
+      </c>
+      <c r="B83" s="216">
+        <v>0</v>
+      </c>
+      <c r="C83" s="216">
+        <v>1</v>
+      </c>
+      <c r="D83" s="216">
+        <v>0</v>
+      </c>
+      <c r="E83" s="216">
+        <v>0</v>
+      </c>
+      <c r="F83" s="216">
+        <v>0</v>
+      </c>
+      <c r="G83" s="216">
+        <v>0</v>
+      </c>
+      <c r="H83" s="216">
+        <v>1</v>
+      </c>
+      <c r="I83" s="216">
+        <v>0</v>
+      </c>
+      <c r="J83" s="216">
+        <v>0</v>
+      </c>
+      <c r="K83" s="216">
+        <v>1</v>
+      </c>
+      <c r="L83" s="216">
+        <v>0</v>
+      </c>
+      <c r="M83" s="216">
+        <v>0</v>
+      </c>
+      <c r="N83" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84" s="15">
+        <v>44065</v>
+      </c>
+      <c r="B84" s="216">
+        <v>0</v>
+      </c>
+      <c r="C84" s="216">
+        <v>1</v>
+      </c>
+      <c r="D84" s="216">
+        <v>0</v>
+      </c>
+      <c r="E84" s="216">
+        <v>0</v>
+      </c>
+      <c r="F84" s="216">
+        <v>0</v>
+      </c>
+      <c r="G84" s="216">
+        <v>0</v>
+      </c>
+      <c r="H84" s="216">
+        <v>1</v>
+      </c>
+      <c r="I84" s="216">
+        <v>0</v>
+      </c>
+      <c r="J84" s="216">
+        <v>0</v>
+      </c>
+      <c r="K84" s="216">
+        <v>1</v>
+      </c>
+      <c r="L84" s="216">
+        <v>0</v>
+      </c>
+      <c r="M84" s="216">
+        <v>0</v>
+      </c>
+      <c r="N84" s="216">
         <v>0</v>
       </c>
     </row>
@@ -12480,11 +12762,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K82" sqref="K82"/>
+      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15121,6 +15403,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="15">
+        <v>44064</v>
+      </c>
+      <c r="B83" s="216">
+        <v>0</v>
+      </c>
+      <c r="C83" s="216">
+        <v>0</v>
+      </c>
+      <c r="D83" s="216">
+        <v>0</v>
+      </c>
+      <c r="E83" s="216">
+        <v>0</v>
+      </c>
+      <c r="F83" s="216">
+        <v>2</v>
+      </c>
+      <c r="G83" s="216">
+        <v>1</v>
+      </c>
+      <c r="H83" s="216">
+        <v>1</v>
+      </c>
+      <c r="I83" s="216">
+        <v>1</v>
+      </c>
+      <c r="J83" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="15">
+        <v>44065</v>
+      </c>
+      <c r="B84" s="216">
+        <v>0</v>
+      </c>
+      <c r="C84" s="216">
+        <v>0</v>
+      </c>
+      <c r="D84" s="216">
+        <v>0</v>
+      </c>
+      <c r="E84" s="216">
+        <v>0</v>
+      </c>
+      <c r="F84" s="216">
+        <v>2</v>
+      </c>
+      <c r="G84" s="216">
+        <v>1</v>
+      </c>
+      <c r="H84" s="216">
+        <v>1</v>
+      </c>
+      <c r="I84" s="216">
+        <v>1</v>
+      </c>
+      <c r="J84" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15130,8 +15476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="CC21" sqref="CC21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BC15" sqref="I15:BC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15386,8 +15732,12 @@
       <c r="CD1" s="49">
         <v>44063</v>
       </c>
-      <c r="CE1" s="49"/>
-      <c r="CF1" s="49"/>
+      <c r="CE1" s="49">
+        <v>44064</v>
+      </c>
+      <c r="CF1" s="49">
+        <v>44065</v>
+      </c>
       <c r="CG1" s="49"/>
       <c r="CH1" s="48"/>
     </row>
@@ -15638,8 +15988,12 @@
       <c r="CD2" s="48">
         <v>5510</v>
       </c>
-      <c r="CE2" s="48"/>
-      <c r="CF2" s="48"/>
+      <c r="CE2" s="48">
+        <v>5542</v>
+      </c>
+      <c r="CF2" s="48">
+        <v>5574</v>
+      </c>
       <c r="CG2" s="48"/>
       <c r="CH2" s="48"/>
     </row>
@@ -15890,8 +16244,12 @@
       <c r="CD3" s="48">
         <v>5306</v>
       </c>
-      <c r="CE3" s="48"/>
-      <c r="CF3" s="48"/>
+      <c r="CE3" s="48">
+        <v>5343</v>
+      </c>
+      <c r="CF3" s="48">
+        <v>5375</v>
+      </c>
       <c r="CG3" s="48"/>
       <c r="CH3" s="48"/>
     </row>
@@ -16142,8 +16500,12 @@
       <c r="CD4" s="48">
         <v>5306</v>
       </c>
-      <c r="CE4" s="48"/>
-      <c r="CF4" s="48"/>
+      <c r="CE4" s="48">
+        <v>5343</v>
+      </c>
+      <c r="CF4" s="48">
+        <v>5375</v>
+      </c>
       <c r="CG4" s="48"/>
       <c r="CH4" s="48"/>
     </row>
@@ -16394,8 +16756,12 @@
       <c r="CD5" s="48">
         <v>5306</v>
       </c>
-      <c r="CE5" s="48"/>
-      <c r="CF5" s="48"/>
+      <c r="CE5" s="48">
+        <v>5343</v>
+      </c>
+      <c r="CF5" s="48">
+        <v>5375</v>
+      </c>
       <c r="CG5" s="48"/>
       <c r="CH5" s="48"/>
     </row>
@@ -16646,8 +17012,12 @@
       <c r="CD6" s="48">
         <v>5306</v>
       </c>
-      <c r="CE6" s="48"/>
-      <c r="CF6" s="48"/>
+      <c r="CE6" s="48">
+        <v>5343</v>
+      </c>
+      <c r="CF6" s="48">
+        <v>5375</v>
+      </c>
       <c r="CG6" s="48"/>
       <c r="CH6" s="48"/>
     </row>
@@ -16898,8 +17268,12 @@
       <c r="CD7" s="48">
         <v>4615</v>
       </c>
-      <c r="CE7" s="48"/>
-      <c r="CF7" s="48"/>
+      <c r="CE7" s="48">
+        <v>4647</v>
+      </c>
+      <c r="CF7" s="48">
+        <v>4679</v>
+      </c>
       <c r="CG7" s="48"/>
       <c r="CH7" s="48"/>
     </row>
@@ -17150,8 +17524,12 @@
       <c r="CD8" s="48">
         <v>7246</v>
       </c>
-      <c r="CE8" s="48"/>
-      <c r="CF8" s="48"/>
+      <c r="CE8" s="48">
+        <v>7278</v>
+      </c>
+      <c r="CF8" s="48">
+        <v>7309</v>
+      </c>
       <c r="CG8" s="48"/>
       <c r="CH8" s="48"/>
     </row>
@@ -17492,8 +17870,12 @@
       <c r="CD10" s="48">
         <v>221</v>
       </c>
-      <c r="CE10" s="48"/>
-      <c r="CF10" s="48"/>
+      <c r="CE10" s="48">
+        <v>222</v>
+      </c>
+      <c r="CF10" s="48">
+        <v>223</v>
+      </c>
       <c r="CG10" s="48"/>
       <c r="CH10" s="48"/>
     </row>
@@ -17744,8 +18126,12 @@
       <c r="CD11" s="48">
         <v>221</v>
       </c>
-      <c r="CE11" s="48"/>
-      <c r="CF11" s="48"/>
+      <c r="CE11" s="48">
+        <v>222</v>
+      </c>
+      <c r="CF11" s="48">
+        <v>223</v>
+      </c>
       <c r="CG11" s="48"/>
       <c r="CH11" s="48"/>
     </row>
@@ -17996,8 +18382,12 @@
       <c r="CD12" s="48">
         <v>221</v>
       </c>
-      <c r="CE12" s="48"/>
-      <c r="CF12" s="48"/>
+      <c r="CE12" s="48">
+        <v>222</v>
+      </c>
+      <c r="CF12" s="48">
+        <v>223</v>
+      </c>
       <c r="CG12" s="48"/>
       <c r="CH12" s="48"/>
     </row>
@@ -18248,8 +18638,12 @@
       <c r="CD13" s="48">
         <v>221</v>
       </c>
-      <c r="CE13" s="48"/>
-      <c r="CF13" s="48"/>
+      <c r="CE13" s="48">
+        <v>222</v>
+      </c>
+      <c r="CF13" s="48">
+        <v>223</v>
+      </c>
       <c r="CG13" s="48"/>
       <c r="CH13" s="48"/>
     </row>
@@ -18500,8 +18894,12 @@
       <c r="CD14" s="48">
         <v>221</v>
       </c>
-      <c r="CE14" s="48"/>
-      <c r="CF14" s="48"/>
+      <c r="CE14" s="48">
+        <v>222</v>
+      </c>
+      <c r="CF14" s="48">
+        <v>223</v>
+      </c>
       <c r="CG14" s="48"/>
       <c r="CH14" s="48"/>
     </row>
@@ -18752,8 +19150,12 @@
       <c r="CD15" s="48">
         <v>156</v>
       </c>
-      <c r="CE15" s="48"/>
-      <c r="CF15" s="48"/>
+      <c r="CE15" s="48">
+        <v>157</v>
+      </c>
+      <c r="CF15" s="48">
+        <v>158</v>
+      </c>
       <c r="CG15" s="48"/>
       <c r="CH15" s="48"/>
     </row>
@@ -19004,8 +19406,12 @@
       <c r="CD16" s="48">
         <v>233</v>
       </c>
-      <c r="CE16" s="48"/>
-      <c r="CF16" s="48"/>
+      <c r="CE16" s="48">
+        <v>234</v>
+      </c>
+      <c r="CF16" s="48">
+        <v>235</v>
+      </c>
       <c r="CG16" s="48"/>
       <c r="CH16" s="48"/>
     </row>
@@ -19344,8 +19750,12 @@
       <c r="CD18" s="48">
         <v>1276</v>
       </c>
-      <c r="CE18" s="48"/>
-      <c r="CF18" s="48"/>
+      <c r="CE18" s="48">
+        <v>1283</v>
+      </c>
+      <c r="CF18" s="48">
+        <v>1290</v>
+      </c>
       <c r="CG18" s="48"/>
       <c r="CH18" s="48"/>
     </row>
@@ -19525,7 +19935,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CD20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CF20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -19683,6 +20093,14 @@
       <c r="CD20" s="51">
         <f t="shared" si="1"/>
         <v>41365</v>
+      </c>
+      <c r="CE20" s="51">
+        <f t="shared" si="1"/>
+        <v>41623</v>
+      </c>
+      <c r="CF20" s="51">
+        <f t="shared" si="1"/>
+        <v>41860</v>
       </c>
     </row>
   </sheetData>
@@ -19694,8 +20112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19982,43 +20400,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="771" t="s">
+      <c r="B8" s="789" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="771"/>
+      <c r="B9" s="789"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="771"/>
+      <c r="B10" s="789"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="771"/>
+      <c r="B11" s="789"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="772" t="s">
+      <c r="B12" s="790" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="772"/>
+      <c r="B13" s="790"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="772"/>
+      <c r="B14" s="790"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="773" t="s">
+      <c r="B15" s="791" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="773"/>
+      <c r="B16" s="791"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 24th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1EC0EC-7CA3-AE4D-8C17-12E0837A90C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0103A554-A6C3-6643-9A4D-B51A6C9A8BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="792">
+  <cellXfs count="801">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3233,10 +3260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5932,6 +5959,38 @@
         <v>1253432</v>
       </c>
     </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="15">
+        <v>44066</v>
+      </c>
+      <c r="B85" s="789">
+        <v>560164</v>
+      </c>
+      <c r="C85" s="790">
+        <v>618779</v>
+      </c>
+      <c r="D85" s="791">
+        <v>80198</v>
+      </c>
+      <c r="E85" s="792">
+        <v>60480</v>
+      </c>
+      <c r="F85" s="793">
+        <v>25.811191008347556</v>
+      </c>
+      <c r="G85" s="794">
+        <v>144585</v>
+      </c>
+      <c r="H85" s="795">
+        <v>12367</v>
+      </c>
+      <c r="I85" s="796">
+        <v>17859</v>
+      </c>
+      <c r="J85" s="797">
+        <v>1259141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5939,11 +5998,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L84"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M84" sqref="M84"/>
+      <selection pane="bottomLeft" activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9094,6 +9153,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" s="15">
+        <v>44066</v>
+      </c>
+      <c r="B85" s="216">
+        <v>0</v>
+      </c>
+      <c r="C85" s="216">
+        <v>1</v>
+      </c>
+      <c r="D85" s="216">
+        <v>0</v>
+      </c>
+      <c r="E85" s="216">
+        <v>0</v>
+      </c>
+      <c r="F85" s="216">
+        <v>1</v>
+      </c>
+      <c r="G85" s="216">
+        <v>0</v>
+      </c>
+      <c r="H85" s="216">
+        <v>0</v>
+      </c>
+      <c r="I85" s="216">
+        <v>0</v>
+      </c>
+      <c r="J85" s="216">
+        <v>0</v>
+      </c>
+      <c r="K85" s="216">
+        <v>0</v>
+      </c>
+      <c r="L85" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9101,11 +9198,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O84" sqref="O84"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O85" sqref="O85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12752,6 +12849,50 @@
         <v>0</v>
       </c>
       <c r="N84" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" s="15">
+        <v>44066</v>
+      </c>
+      <c r="B85" s="216">
+        <v>0</v>
+      </c>
+      <c r="C85" s="216">
+        <v>1</v>
+      </c>
+      <c r="D85" s="216">
+        <v>0</v>
+      </c>
+      <c r="E85" s="216">
+        <v>0</v>
+      </c>
+      <c r="F85" s="216">
+        <v>0</v>
+      </c>
+      <c r="G85" s="216">
+        <v>0</v>
+      </c>
+      <c r="H85" s="216">
+        <v>1</v>
+      </c>
+      <c r="I85" s="216">
+        <v>0</v>
+      </c>
+      <c r="J85" s="216">
+        <v>0</v>
+      </c>
+      <c r="K85" s="216">
+        <v>1</v>
+      </c>
+      <c r="L85" s="216">
+        <v>0</v>
+      </c>
+      <c r="M85" s="216">
+        <v>0</v>
+      </c>
+      <c r="N85" s="216">
         <v>0</v>
       </c>
     </row>
@@ -12762,11 +12903,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15467,6 +15608,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="15">
+        <v>44066</v>
+      </c>
+      <c r="B85" s="216">
+        <v>0</v>
+      </c>
+      <c r="C85" s="216">
+        <v>0</v>
+      </c>
+      <c r="D85" s="216">
+        <v>0</v>
+      </c>
+      <c r="E85" s="216">
+        <v>0</v>
+      </c>
+      <c r="F85" s="216">
+        <v>2</v>
+      </c>
+      <c r="G85" s="216">
+        <v>1</v>
+      </c>
+      <c r="H85" s="216">
+        <v>1</v>
+      </c>
+      <c r="I85" s="216">
+        <v>1</v>
+      </c>
+      <c r="J85" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15476,8 +15649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CJ20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BC15" sqref="I15:BC15"/>
+    <sheetView topLeftCell="BU1" workbookViewId="0">
+      <selection activeCell="CI2" sqref="CI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15738,7 +15911,9 @@
       <c r="CF1" s="49">
         <v>44065</v>
       </c>
-      <c r="CG1" s="49"/>
+      <c r="CG1" s="49">
+        <v>44066</v>
+      </c>
       <c r="CH1" s="48"/>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
@@ -15994,7 +16169,9 @@
       <c r="CF2" s="48">
         <v>5574</v>
       </c>
-      <c r="CG2" s="48"/>
+      <c r="CG2" s="48">
+        <v>5606</v>
+      </c>
       <c r="CH2" s="48"/>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.2">
@@ -16250,7 +16427,9 @@
       <c r="CF3" s="48">
         <v>5375</v>
       </c>
-      <c r="CG3" s="48"/>
+      <c r="CG3" s="48">
+        <v>5407</v>
+      </c>
       <c r="CH3" s="48"/>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.2">
@@ -16506,7 +16685,9 @@
       <c r="CF4" s="48">
         <v>5375</v>
       </c>
-      <c r="CG4" s="48"/>
+      <c r="CG4" s="48">
+        <v>5407</v>
+      </c>
       <c r="CH4" s="48"/>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.2">
@@ -16762,7 +16943,9 @@
       <c r="CF5" s="48">
         <v>5375</v>
       </c>
-      <c r="CG5" s="48"/>
+      <c r="CG5" s="48">
+        <v>5407</v>
+      </c>
       <c r="CH5" s="48"/>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
@@ -17018,7 +17201,9 @@
       <c r="CF6" s="48">
         <v>5375</v>
       </c>
-      <c r="CG6" s="48"/>
+      <c r="CG6" s="48">
+        <v>5407</v>
+      </c>
       <c r="CH6" s="48"/>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.2">
@@ -17274,7 +17459,9 @@
       <c r="CF7" s="48">
         <v>4679</v>
       </c>
-      <c r="CG7" s="48"/>
+      <c r="CG7" s="48">
+        <v>4711</v>
+      </c>
       <c r="CH7" s="48"/>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.2">
@@ -17530,7 +17717,9 @@
       <c r="CF8" s="48">
         <v>7309</v>
       </c>
-      <c r="CG8" s="48"/>
+      <c r="CG8" s="48">
+        <v>7341</v>
+      </c>
       <c r="CH8" s="48"/>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.2">
@@ -17876,7 +18065,9 @@
       <c r="CF10" s="48">
         <v>223</v>
       </c>
-      <c r="CG10" s="48"/>
+      <c r="CG10" s="48">
+        <v>224</v>
+      </c>
       <c r="CH10" s="48"/>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.2">
@@ -18132,7 +18323,9 @@
       <c r="CF11" s="48">
         <v>223</v>
       </c>
-      <c r="CG11" s="48"/>
+      <c r="CG11" s="48">
+        <v>224</v>
+      </c>
       <c r="CH11" s="48"/>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.2">
@@ -18388,7 +18581,9 @@
       <c r="CF12" s="48">
         <v>223</v>
       </c>
-      <c r="CG12" s="48"/>
+      <c r="CG12" s="48">
+        <v>224</v>
+      </c>
       <c r="CH12" s="48"/>
     </row>
     <row r="13" spans="1:88" x14ac:dyDescent="0.2">
@@ -18644,7 +18839,9 @@
       <c r="CF13" s="48">
         <v>223</v>
       </c>
-      <c r="CG13" s="48"/>
+      <c r="CG13" s="48">
+        <v>224</v>
+      </c>
       <c r="CH13" s="48"/>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.2">
@@ -18900,7 +19097,9 @@
       <c r="CF14" s="48">
         <v>223</v>
       </c>
-      <c r="CG14" s="48"/>
+      <c r="CG14" s="48">
+        <v>224</v>
+      </c>
       <c r="CH14" s="48"/>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.2">
@@ -19156,7 +19355,9 @@
       <c r="CF15" s="48">
         <v>158</v>
       </c>
-      <c r="CG15" s="48"/>
+      <c r="CG15" s="48">
+        <v>159</v>
+      </c>
       <c r="CH15" s="48"/>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.2">
@@ -19412,7 +19613,9 @@
       <c r="CF16" s="48">
         <v>235</v>
       </c>
-      <c r="CG16" s="48"/>
+      <c r="CG16" s="48">
+        <v>236</v>
+      </c>
       <c r="CH16" s="48"/>
     </row>
     <row r="17" spans="1:86" x14ac:dyDescent="0.2">
@@ -19756,7 +19959,9 @@
       <c r="CF18" s="48">
         <v>1290</v>
       </c>
-      <c r="CG18" s="48"/>
+      <c r="CG18" s="48">
+        <v>1297</v>
+      </c>
       <c r="CH18" s="48"/>
     </row>
     <row r="19" spans="1:86" x14ac:dyDescent="0.2">
@@ -19935,7 +20140,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CF20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CG20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -20101,6 +20306,10 @@
       <c r="CF20" s="51">
         <f t="shared" si="1"/>
         <v>41860</v>
+      </c>
+      <c r="CG20" s="51">
+        <f t="shared" si="1"/>
+        <v>42098</v>
       </c>
     </row>
   </sheetData>
@@ -20112,7 +20321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -20400,43 +20609,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="789" t="s">
+      <c r="B8" s="798" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="789"/>
+      <c r="B9" s="798"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="789"/>
+      <c r="B10" s="798"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="789"/>
+      <c r="B11" s="798"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="790" t="s">
+      <c r="B12" s="799" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="790"/>
+      <c r="B13" s="799"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="790"/>
+      <c r="B14" s="799"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="791" t="s">
+      <c r="B15" s="800" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="791"/>
+      <c r="B16" s="800"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data for August 25th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3A2B61-DEDA-1D4A-8F06-CFC31319CC67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D9A1C-69CA-6949-B816-3FBC6660E8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="810">
+  <cellXfs count="819">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3287,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6050,6 +6077,38 @@
         <v>1263835</v>
       </c>
     </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="15">
+        <v>44068</v>
+      </c>
+      <c r="B87" s="807">
+        <v>568621</v>
+      </c>
+      <c r="C87" s="808">
+        <v>628937</v>
+      </c>
+      <c r="D87" s="809">
+        <v>80878</v>
+      </c>
+      <c r="E87" s="810">
+        <v>61450</v>
+      </c>
+      <c r="F87" s="811">
+        <v>25.763909528490856</v>
+      </c>
+      <c r="G87" s="812">
+        <v>146499</v>
+      </c>
+      <c r="H87" s="813">
+        <v>12548</v>
+      </c>
+      <c r="I87" s="814">
+        <v>18086</v>
+      </c>
+      <c r="J87" s="815">
+        <v>1278436</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6057,11 +6116,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L86" sqref="L86"/>
+      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9099,7 +9158,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" s="15">
+      <c r="A82" s="217">
         <v>44063</v>
       </c>
       <c r="B82" s="216">
@@ -9137,7 +9196,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A83" s="15">
+      <c r="A83" s="217">
         <v>44064</v>
       </c>
       <c r="B83" s="216">
@@ -9175,7 +9234,7 @@
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A84" s="15">
+      <c r="A84" s="217">
         <v>44065</v>
       </c>
       <c r="B84" s="216">
@@ -9213,7 +9272,7 @@
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A85" s="15">
+      <c r="A85" s="217">
         <v>44066</v>
       </c>
       <c r="B85" s="216">
@@ -9251,7 +9310,7 @@
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="15">
+      <c r="A86" s="217">
         <v>44067</v>
       </c>
       <c r="B86" s="216">
@@ -9285,6 +9344,44 @@
         <v>0</v>
       </c>
       <c r="L86" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" s="217">
+        <v>44068</v>
+      </c>
+      <c r="B87" s="216">
+        <v>0</v>
+      </c>
+      <c r="C87" s="216">
+        <v>1</v>
+      </c>
+      <c r="D87" s="216">
+        <v>0</v>
+      </c>
+      <c r="E87" s="216">
+        <v>0</v>
+      </c>
+      <c r="F87" s="216">
+        <v>1</v>
+      </c>
+      <c r="G87" s="216">
+        <v>0</v>
+      </c>
+      <c r="H87" s="216">
+        <v>0</v>
+      </c>
+      <c r="I87" s="216">
+        <v>0</v>
+      </c>
+      <c r="J87" s="216">
+        <v>0</v>
+      </c>
+      <c r="K87" s="216">
+        <v>0</v>
+      </c>
+      <c r="L87" s="216">
         <v>4</v>
       </c>
     </row>
@@ -9295,11 +9392,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12818,7 +12915,7 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A82" s="15">
+      <c r="A82" s="217">
         <v>44063</v>
       </c>
       <c r="B82" s="216">
@@ -12862,7 +12959,7 @@
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A83" s="15">
+      <c r="A83" s="217">
         <v>44064</v>
       </c>
       <c r="B83" s="216">
@@ -12906,7 +13003,7 @@
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="15">
+      <c r="A84" s="217">
         <v>44065</v>
       </c>
       <c r="B84" s="216">
@@ -12950,7 +13047,7 @@
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="15">
+      <c r="A85" s="217">
         <v>44066</v>
       </c>
       <c r="B85" s="216">
@@ -12994,7 +13091,7 @@
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A86" s="15">
+      <c r="A86" s="217">
         <v>44067</v>
       </c>
       <c r="B86" s="216">
@@ -13034,6 +13131,50 @@
         <v>0</v>
       </c>
       <c r="N86" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="217">
+        <v>44068</v>
+      </c>
+      <c r="B87" s="216">
+        <v>0</v>
+      </c>
+      <c r="C87" s="216">
+        <v>1</v>
+      </c>
+      <c r="D87" s="216">
+        <v>0</v>
+      </c>
+      <c r="E87" s="216">
+        <v>0</v>
+      </c>
+      <c r="F87" s="216">
+        <v>0</v>
+      </c>
+      <c r="G87" s="216">
+        <v>0</v>
+      </c>
+      <c r="H87" s="216">
+        <v>1</v>
+      </c>
+      <c r="I87" s="216">
+        <v>0</v>
+      </c>
+      <c r="J87" s="216">
+        <v>0</v>
+      </c>
+      <c r="K87" s="216">
+        <v>1</v>
+      </c>
+      <c r="L87" s="216">
+        <v>0</v>
+      </c>
+      <c r="M87" s="216">
+        <v>0</v>
+      </c>
+      <c r="N87" s="216">
         <v>0</v>
       </c>
     </row>
@@ -13044,11 +13185,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
+      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15654,7 +15795,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" s="15">
+      <c r="A82" s="495">
         <v>44063</v>
       </c>
       <c r="B82" s="216">
@@ -15686,7 +15827,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="15">
+      <c r="A83" s="495">
         <v>44064</v>
       </c>
       <c r="B83" s="216">
@@ -15718,7 +15859,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" s="15">
+      <c r="A84" s="495">
         <v>44065</v>
       </c>
       <c r="B84" s="216">
@@ -15750,7 +15891,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" s="15">
+      <c r="A85" s="495">
         <v>44066</v>
       </c>
       <c r="B85" s="216">
@@ -15782,7 +15923,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" s="15">
+      <c r="A86" s="495">
         <v>44067</v>
       </c>
       <c r="B86" s="216">
@@ -15810,6 +15951,38 @@
         <v>1</v>
       </c>
       <c r="J86" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="495">
+        <v>44068</v>
+      </c>
+      <c r="B87" s="216">
+        <v>0</v>
+      </c>
+      <c r="C87" s="216">
+        <v>0</v>
+      </c>
+      <c r="D87" s="216">
+        <v>0</v>
+      </c>
+      <c r="E87" s="216">
+        <v>0</v>
+      </c>
+      <c r="F87" s="216">
+        <v>2</v>
+      </c>
+      <c r="G87" s="216">
+        <v>1</v>
+      </c>
+      <c r="H87" s="216">
+        <v>1</v>
+      </c>
+      <c r="I87" s="216">
+        <v>1</v>
+      </c>
+      <c r="J87" s="216">
         <v>2</v>
       </c>
     </row>
@@ -15822,8 +15995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CL20"/>
   <sheetViews>
-    <sheetView topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="CF17" sqref="CF17:CL17"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
+      <selection activeCell="CH14" sqref="CH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16090,6 +16263,9 @@
       <c r="CH1" s="49">
         <v>44067</v>
       </c>
+      <c r="CI1" s="49">
+        <v>44068</v>
+      </c>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -16350,6 +16526,9 @@
       <c r="CH2" s="48">
         <v>5638</v>
       </c>
+      <c r="CI2">
+        <v>5670</v>
+      </c>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -16610,6 +16789,9 @@
       <c r="CH3" s="48">
         <v>5439</v>
       </c>
+      <c r="CI3">
+        <v>5471</v>
+      </c>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -16870,6 +17052,9 @@
       <c r="CH4" s="48">
         <v>5439</v>
       </c>
+      <c r="CI4">
+        <v>5471</v>
+      </c>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -17130,6 +17315,9 @@
       <c r="CH5" s="48">
         <v>5439</v>
       </c>
+      <c r="CI5">
+        <v>5471</v>
+      </c>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -17390,6 +17578,9 @@
       <c r="CH6" s="48">
         <v>5439</v>
       </c>
+      <c r="CI6">
+        <v>5471</v>
+      </c>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -17650,6 +17841,9 @@
       <c r="CH7" s="48">
         <v>4743</v>
       </c>
+      <c r="CI7">
+        <v>4775</v>
+      </c>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -17909,6 +18103,9 @@
       </c>
       <c r="CH8" s="48">
         <v>7373</v>
+      </c>
+      <c r="CI8">
+        <v>7405</v>
       </c>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.2">
@@ -18260,6 +18457,9 @@
       <c r="CH10" s="48">
         <v>225</v>
       </c>
+      <c r="CI10" s="216">
+        <v>226</v>
+      </c>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -18520,6 +18720,9 @@
       <c r="CH11" s="48">
         <v>225</v>
       </c>
+      <c r="CI11" s="216">
+        <v>226</v>
+      </c>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -18780,6 +18983,9 @@
       <c r="CH12" s="48">
         <v>225</v>
       </c>
+      <c r="CI12" s="216">
+        <v>226</v>
+      </c>
     </row>
     <row r="13" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -19040,6 +19246,9 @@
       <c r="CH13" s="48">
         <v>225</v>
       </c>
+      <c r="CI13" s="216">
+        <v>226</v>
+      </c>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -19300,6 +19509,9 @@
       <c r="CH14" s="48">
         <v>225</v>
       </c>
+      <c r="CI14" s="216">
+        <v>226</v>
+      </c>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -19560,6 +19772,9 @@
       <c r="CH15" s="48">
         <v>160</v>
       </c>
+      <c r="CI15" s="216">
+        <v>161</v>
+      </c>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -19819,6 +20034,9 @@
       </c>
       <c r="CH16" s="48">
         <v>237</v>
+      </c>
+      <c r="CI16" s="216">
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:90" x14ac:dyDescent="0.2">
@@ -20172,6 +20390,9 @@
       <c r="CH18" s="48">
         <v>1304</v>
       </c>
+      <c r="CI18" s="216">
+        <v>1311</v>
+      </c>
     </row>
     <row r="19" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -20349,7 +20570,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CH20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CI20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -20523,6 +20744,10 @@
       <c r="CH20" s="51">
         <f t="shared" si="1"/>
         <v>42336</v>
+      </c>
+      <c r="CI20" s="51">
+        <f t="shared" si="1"/>
+        <v>42574</v>
       </c>
     </row>
   </sheetData>
@@ -20822,43 +21047,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="807" t="s">
+      <c r="B8" s="816" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="807"/>
+      <c r="B9" s="816"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="807"/>
+      <c r="B10" s="816"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="807"/>
+      <c r="B11" s="816"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="808" t="s">
+      <c r="B12" s="817" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="808"/>
+      <c r="B13" s="817"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="808"/>
+      <c r="B14" s="817"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="809" t="s">
+      <c r="B15" s="818" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="809"/>
+      <c r="B16" s="818"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 26th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1D9A1C-69CA-6949-B816-3FBC6660E8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3EA32B-DC77-1540-B563-A9B2086FE78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="819">
+  <cellXfs count="828">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2608,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3314,10 +3341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6109,6 +6136,38 @@
         <v>1278436</v>
       </c>
     </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="15">
+        <v>44069</v>
+      </c>
+      <c r="B88" s="816">
+        <v>573888</v>
+      </c>
+      <c r="C88" s="817">
+        <v>635729</v>
+      </c>
+      <c r="D88" s="818">
+        <v>81466</v>
+      </c>
+      <c r="E88" s="819">
+        <v>62076</v>
+      </c>
+      <c r="F88" s="820">
+        <v>25.70431861269098</v>
+      </c>
+      <c r="G88" s="821">
+        <v>147514</v>
+      </c>
+      <c r="H88" s="822">
+        <v>12639</v>
+      </c>
+      <c r="I88" s="823">
+        <v>18248</v>
+      </c>
+      <c r="J88" s="824">
+        <v>1291083</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6116,11 +6175,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9385,6 +9444,44 @@
         <v>4</v>
       </c>
     </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A88" s="15">
+        <v>44069</v>
+      </c>
+      <c r="B88" s="216">
+        <v>0</v>
+      </c>
+      <c r="C88" s="216">
+        <v>1</v>
+      </c>
+      <c r="D88" s="216">
+        <v>0</v>
+      </c>
+      <c r="E88" s="216">
+        <v>0</v>
+      </c>
+      <c r="F88" s="216">
+        <v>1</v>
+      </c>
+      <c r="G88" s="216">
+        <v>0</v>
+      </c>
+      <c r="H88" s="216">
+        <v>0</v>
+      </c>
+      <c r="I88" s="216">
+        <v>0</v>
+      </c>
+      <c r="J88" s="216">
+        <v>0</v>
+      </c>
+      <c r="K88" s="216">
+        <v>0</v>
+      </c>
+      <c r="L88" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9392,11 +9489,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O87"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
+      <selection pane="bottomLeft" activeCell="O88" sqref="O88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13175,6 +13272,50 @@
         <v>0</v>
       </c>
       <c r="N87" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="15">
+        <v>44069</v>
+      </c>
+      <c r="B88" s="216">
+        <v>0</v>
+      </c>
+      <c r="C88" s="216">
+        <v>1</v>
+      </c>
+      <c r="D88" s="216">
+        <v>0</v>
+      </c>
+      <c r="E88" s="216">
+        <v>0</v>
+      </c>
+      <c r="F88" s="216">
+        <v>0</v>
+      </c>
+      <c r="G88" s="216">
+        <v>0</v>
+      </c>
+      <c r="H88" s="216">
+        <v>1</v>
+      </c>
+      <c r="I88" s="216">
+        <v>0</v>
+      </c>
+      <c r="J88" s="216">
+        <v>0</v>
+      </c>
+      <c r="K88" s="216">
+        <v>1</v>
+      </c>
+      <c r="L88" s="216">
+        <v>0</v>
+      </c>
+      <c r="M88" s="216">
+        <v>0</v>
+      </c>
+      <c r="N88" s="216">
         <v>0</v>
       </c>
     </row>
@@ -13185,11 +13326,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81:A87"/>
+      <selection pane="bottomLeft" activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15986,6 +16127,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="15">
+        <v>44069</v>
+      </c>
+      <c r="B88" s="216">
+        <v>0</v>
+      </c>
+      <c r="C88" s="216">
+        <v>0</v>
+      </c>
+      <c r="D88" s="216">
+        <v>0</v>
+      </c>
+      <c r="E88" s="216">
+        <v>0</v>
+      </c>
+      <c r="F88" s="216">
+        <v>2</v>
+      </c>
+      <c r="G88" s="216">
+        <v>1</v>
+      </c>
+      <c r="H88" s="216">
+        <v>1</v>
+      </c>
+      <c r="I88" s="216">
+        <v>1</v>
+      </c>
+      <c r="J88" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15995,8 +16168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="CH14" sqref="CH14"/>
+    <sheetView topLeftCell="BU1" workbookViewId="0">
+      <selection activeCell="CK23" sqref="CK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16266,6 +16439,9 @@
       <c r="CI1" s="49">
         <v>44068</v>
       </c>
+      <c r="CJ1" s="49">
+        <v>44069</v>
+      </c>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -16529,6 +16705,9 @@
       <c r="CI2">
         <v>5670</v>
       </c>
+      <c r="CJ2">
+        <v>5702</v>
+      </c>
     </row>
     <row r="3" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -16792,6 +16971,9 @@
       <c r="CI3">
         <v>5471</v>
       </c>
+      <c r="CJ3">
+        <v>5503</v>
+      </c>
     </row>
     <row r="4" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -17055,6 +17237,9 @@
       <c r="CI4">
         <v>5471</v>
       </c>
+      <c r="CJ4">
+        <v>5503</v>
+      </c>
     </row>
     <row r="5" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -17318,6 +17503,9 @@
       <c r="CI5">
         <v>5471</v>
       </c>
+      <c r="CJ5">
+        <v>5503</v>
+      </c>
     </row>
     <row r="6" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -17581,6 +17769,9 @@
       <c r="CI6">
         <v>5471</v>
       </c>
+      <c r="CJ6">
+        <v>5503</v>
+      </c>
     </row>
     <row r="7" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -17844,6 +18035,9 @@
       <c r="CI7">
         <v>4775</v>
       </c>
+      <c r="CJ7">
+        <v>4807</v>
+      </c>
     </row>
     <row r="8" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -18106,6 +18300,9 @@
       </c>
       <c r="CI8">
         <v>7405</v>
+      </c>
+      <c r="CJ8">
+        <v>7437</v>
       </c>
     </row>
     <row r="9" spans="1:88" x14ac:dyDescent="0.2">
@@ -18460,6 +18657,9 @@
       <c r="CI10" s="216">
         <v>226</v>
       </c>
+      <c r="CJ10" s="216">
+        <v>227</v>
+      </c>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -18723,6 +18923,9 @@
       <c r="CI11" s="216">
         <v>226</v>
       </c>
+      <c r="CJ11" s="216">
+        <v>227</v>
+      </c>
     </row>
     <row r="12" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -18986,6 +19189,9 @@
       <c r="CI12" s="216">
         <v>226</v>
       </c>
+      <c r="CJ12" s="216">
+        <v>227</v>
+      </c>
     </row>
     <row r="13" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -19249,6 +19455,9 @@
       <c r="CI13" s="216">
         <v>226</v>
       </c>
+      <c r="CJ13" s="216">
+        <v>227</v>
+      </c>
     </row>
     <row r="14" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -19512,6 +19721,9 @@
       <c r="CI14" s="216">
         <v>226</v>
       </c>
+      <c r="CJ14" s="216">
+        <v>227</v>
+      </c>
     </row>
     <row r="15" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -19775,6 +19987,9 @@
       <c r="CI15" s="216">
         <v>161</v>
       </c>
+      <c r="CJ15" s="216">
+        <v>162</v>
+      </c>
     </row>
     <row r="16" spans="1:88" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -20037,6 +20252,9 @@
       </c>
       <c r="CI16" s="216">
         <v>238</v>
+      </c>
+      <c r="CJ16" s="216">
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:90" x14ac:dyDescent="0.2">
@@ -20393,6 +20611,9 @@
       <c r="CI18" s="216">
         <v>1311</v>
       </c>
+      <c r="CJ18">
+        <v>1318</v>
+      </c>
     </row>
     <row r="19" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -20570,7 +20791,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CI20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CJ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -20748,6 +20969,10 @@
       <c r="CI20" s="51">
         <f t="shared" si="1"/>
         <v>42574</v>
+      </c>
+      <c r="CJ20" s="51">
+        <f t="shared" si="1"/>
+        <v>42812</v>
       </c>
     </row>
   </sheetData>
@@ -21047,43 +21272,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="816" t="s">
+      <c r="B8" s="825" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="816"/>
+      <c r="B9" s="825"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="816"/>
+      <c r="B10" s="825"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="816"/>
+      <c r="B11" s="825"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="817" t="s">
+      <c r="B12" s="826" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="817"/>
+      <c r="B13" s="826"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="817"/>
+      <c r="B14" s="826"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="818" t="s">
+      <c r="B15" s="827" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="818"/>
+      <c r="B16" s="827"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 27th and 28th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3EA32B-DC77-1540-B563-A9B2086FE78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DD9157-345E-CD44-8CA4-C2F0674F681B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="1300" windowWidth="28800" windowHeight="16560" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Las observaciones de sx_nal se mantuvieron</t>
+  </si>
+  <si>
+    <t>24 de febrero</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="828">
+  <cellXfs count="846">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2608,6 +2611,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3341,10 +3398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6168,6 +6225,70 @@
         <v>1291083</v>
       </c>
     </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="15">
+        <v>44070</v>
+      </c>
+      <c r="B89" s="825">
+        <v>579914</v>
+      </c>
+      <c r="C89" s="826">
+        <v>643265</v>
+      </c>
+      <c r="D89" s="827">
+        <v>81597</v>
+      </c>
+      <c r="E89" s="828">
+        <v>62594</v>
+      </c>
+      <c r="F89" s="829">
+        <v>25.635180388816277</v>
+      </c>
+      <c r="G89" s="830">
+        <v>148662</v>
+      </c>
+      <c r="H89" s="831">
+        <v>12729</v>
+      </c>
+      <c r="I89" s="832">
+        <v>18374</v>
+      </c>
+      <c r="J89" s="833">
+        <v>1304776</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="15">
+        <v>44071</v>
+      </c>
+      <c r="B90" s="834">
+        <v>585738</v>
+      </c>
+      <c r="C90" s="835">
+        <v>650862</v>
+      </c>
+      <c r="D90" s="836">
+        <v>83357</v>
+      </c>
+      <c r="E90" s="837">
+        <v>63146</v>
+      </c>
+      <c r="F90" s="838">
+        <v>25.570818352232568</v>
+      </c>
+      <c r="G90" s="839">
+        <v>149778</v>
+      </c>
+      <c r="H90" s="840">
+        <v>12821</v>
+      </c>
+      <c r="I90" s="841">
+        <v>18491</v>
+      </c>
+      <c r="J90" s="842">
+        <v>1319957</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6175,11 +6296,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:L88"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6190,7 +6311,7 @@
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -6225,10 +6346,13 @@
         <v>7</v>
       </c>
       <c r="L1" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="47">
         <v>43983</v>
       </c>
@@ -6260,11 +6384,12 @@
       <c r="K2" s="48">
         <v>0</v>
       </c>
-      <c r="L2" s="48">
+      <c r="L2" s="48"/>
+      <c r="M2" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="47">
         <v>43984</v>
       </c>
@@ -6296,11 +6421,12 @@
       <c r="K3" s="48">
         <v>0</v>
       </c>
-      <c r="L3" s="48">
+      <c r="L3" s="48"/>
+      <c r="M3" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="47">
         <v>43985</v>
       </c>
@@ -6332,11 +6458,12 @@
       <c r="K4" s="48">
         <v>0</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="48"/>
+      <c r="M4" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="47">
         <v>43986</v>
       </c>
@@ -6368,11 +6495,12 @@
       <c r="K5" s="48">
         <v>0</v>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="48"/>
+      <c r="M5" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="47">
         <v>43987</v>
       </c>
@@ -6404,11 +6532,12 @@
       <c r="K6" s="48">
         <v>0</v>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="48"/>
+      <c r="M6" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="47">
         <v>43988</v>
       </c>
@@ -6440,11 +6569,12 @@
       <c r="K7" s="48">
         <v>0</v>
       </c>
-      <c r="L7" s="48">
+      <c r="L7" s="48"/>
+      <c r="M7" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="47">
         <v>43989</v>
       </c>
@@ -6476,11 +6606,12 @@
       <c r="K8" s="48">
         <v>0</v>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="48"/>
+      <c r="M8" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="47">
         <v>43990</v>
       </c>
@@ -6512,11 +6643,12 @@
       <c r="K9" s="48">
         <v>0</v>
       </c>
-      <c r="L9" s="48">
+      <c r="L9" s="48"/>
+      <c r="M9" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="47">
         <v>43991</v>
       </c>
@@ -6548,11 +6680,12 @@
       <c r="K10" s="48">
         <v>0</v>
       </c>
-      <c r="L10" s="48">
+      <c r="L10" s="48"/>
+      <c r="M10" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="47">
         <v>43992</v>
       </c>
@@ -6584,11 +6717,12 @@
       <c r="K11" s="48">
         <v>0</v>
       </c>
-      <c r="L11" s="48">
+      <c r="L11" s="48"/>
+      <c r="M11" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="47">
         <v>43993</v>
       </c>
@@ -6620,11 +6754,12 @@
       <c r="K12" s="48">
         <v>0</v>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="48"/>
+      <c r="M12" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="47">
         <v>43994</v>
       </c>
@@ -6656,11 +6791,12 @@
       <c r="K13" s="48">
         <v>0</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="48"/>
+      <c r="M13" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="47">
         <v>43995</v>
       </c>
@@ -6692,11 +6828,12 @@
       <c r="K14" s="48">
         <v>0</v>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="48"/>
+      <c r="M14" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="47">
         <v>43996</v>
       </c>
@@ -6728,11 +6865,12 @@
       <c r="K15" s="48">
         <v>0</v>
       </c>
-      <c r="L15" s="48">
+      <c r="L15" s="48"/>
+      <c r="M15" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="47">
         <v>43997</v>
       </c>
@@ -6764,11 +6902,12 @@
       <c r="K16" s="48">
         <v>0</v>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="48"/>
+      <c r="M16" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="47">
         <v>43998</v>
       </c>
@@ -6800,11 +6939,12 @@
       <c r="K17" s="48">
         <v>0</v>
       </c>
-      <c r="L17" s="48">
+      <c r="L17" s="48"/>
+      <c r="M17" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="47">
         <v>43999</v>
       </c>
@@ -6836,11 +6976,12 @@
       <c r="K18" s="48">
         <v>0</v>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="47">
         <v>44000</v>
       </c>
@@ -6872,11 +7013,12 @@
       <c r="K19" s="48">
         <v>0</v>
       </c>
-      <c r="L19" s="48">
+      <c r="L19" s="48"/>
+      <c r="M19" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="47">
         <v>44001</v>
       </c>
@@ -6908,11 +7050,12 @@
       <c r="K20" s="48">
         <v>0</v>
       </c>
-      <c r="L20" s="48">
+      <c r="L20" s="48"/>
+      <c r="M20" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="47">
         <v>44002</v>
       </c>
@@ -6944,11 +7087,12 @@
       <c r="K21" s="48">
         <v>0</v>
       </c>
-      <c r="L21" s="48">
+      <c r="L21" s="48"/>
+      <c r="M21" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="217">
         <v>44003</v>
       </c>
@@ -6980,11 +7124,12 @@
       <c r="K22" s="216">
         <v>0</v>
       </c>
-      <c r="L22" s="216">
+      <c r="L22" s="216"/>
+      <c r="M22" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="217">
         <v>44004</v>
       </c>
@@ -7016,11 +7161,12 @@
       <c r="K23" s="48">
         <v>0</v>
       </c>
-      <c r="L23" s="48">
+      <c r="L23" s="48"/>
+      <c r="M23" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="217">
         <v>44005</v>
       </c>
@@ -7052,11 +7198,12 @@
       <c r="K24" s="48">
         <v>0</v>
       </c>
-      <c r="L24" s="48">
+      <c r="L24" s="48"/>
+      <c r="M24" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="217">
         <v>44006</v>
       </c>
@@ -7088,11 +7235,12 @@
       <c r="K25" s="48">
         <v>0</v>
       </c>
-      <c r="L25" s="48">
+      <c r="L25" s="48"/>
+      <c r="M25" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="217">
         <v>44007</v>
       </c>
@@ -7124,11 +7272,12 @@
       <c r="K26" s="48">
         <v>0</v>
       </c>
-      <c r="L26" s="48">
+      <c r="L26" s="48"/>
+      <c r="M26" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="217">
         <v>44008</v>
       </c>
@@ -7160,11 +7309,12 @@
       <c r="K27" s="48">
         <v>0</v>
       </c>
-      <c r="L27" s="48">
+      <c r="L27" s="48"/>
+      <c r="M27" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="217">
         <v>44009</v>
       </c>
@@ -7198,11 +7348,12 @@
       <c r="K28" s="48">
         <v>0</v>
       </c>
-      <c r="L28" s="48">
+      <c r="L28" s="48"/>
+      <c r="M28" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="217">
         <v>44010</v>
       </c>
@@ -7236,11 +7387,12 @@
       <c r="K29" s="48">
         <v>0</v>
       </c>
-      <c r="L29" s="48">
+      <c r="L29" s="48"/>
+      <c r="M29" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="217">
         <v>44011</v>
       </c>
@@ -7274,11 +7426,12 @@
       <c r="K30" s="48">
         <v>0</v>
       </c>
-      <c r="L30" s="48">
+      <c r="L30" s="48"/>
+      <c r="M30" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="217">
         <v>44012</v>
       </c>
@@ -7312,11 +7465,12 @@
       <c r="K31" s="48">
         <v>0</v>
       </c>
-      <c r="L31" s="48">
+      <c r="L31" s="48"/>
+      <c r="M31" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="217">
         <v>44013</v>
       </c>
@@ -7350,11 +7504,12 @@
       <c r="K32" s="48">
         <v>0</v>
       </c>
-      <c r="L32" s="48">
+      <c r="L32" s="48"/>
+      <c r="M32" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="217">
         <v>44014</v>
       </c>
@@ -7388,11 +7543,12 @@
       <c r="K33" s="48">
         <v>0</v>
       </c>
-      <c r="L33" s="48">
+      <c r="L33" s="48"/>
+      <c r="M33" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="217">
         <v>44015</v>
       </c>
@@ -7426,11 +7582,12 @@
       <c r="K34" s="48">
         <v>0</v>
       </c>
-      <c r="L34" s="48">
+      <c r="L34" s="48"/>
+      <c r="M34" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="217">
         <v>44016</v>
       </c>
@@ -7464,11 +7621,12 @@
       <c r="K35" s="48">
         <v>0</v>
       </c>
-      <c r="L35" s="48">
+      <c r="L35" s="48"/>
+      <c r="M35" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="217">
         <v>44017</v>
       </c>
@@ -7502,11 +7660,12 @@
       <c r="K36" s="48">
         <v>0</v>
       </c>
-      <c r="L36" s="48">
+      <c r="L36" s="48"/>
+      <c r="M36" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="217">
         <v>44018</v>
       </c>
@@ -7540,11 +7699,12 @@
       <c r="K37" s="48">
         <v>0</v>
       </c>
-      <c r="L37" s="48">
+      <c r="L37" s="48"/>
+      <c r="M37" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="47">
         <v>44019</v>
       </c>
@@ -7578,11 +7738,12 @@
       <c r="K38" s="74">
         <v>0</v>
       </c>
-      <c r="L38" s="74">
+      <c r="L38" s="74"/>
+      <c r="M38" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="47">
         <v>44020</v>
       </c>
@@ -7616,11 +7777,12 @@
       <c r="K39" s="74">
         <v>0</v>
       </c>
-      <c r="L39" s="74">
+      <c r="L39" s="74"/>
+      <c r="M39" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="47">
         <v>44021</v>
       </c>
@@ -7654,11 +7816,12 @@
       <c r="K40" s="74">
         <v>0</v>
       </c>
-      <c r="L40" s="74">
+      <c r="L40" s="74"/>
+      <c r="M40" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="47">
         <v>44022</v>
       </c>
@@ -7692,11 +7855,12 @@
       <c r="K41" s="74">
         <v>0</v>
       </c>
-      <c r="L41" s="74">
+      <c r="L41" s="74"/>
+      <c r="M41" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="47">
         <v>44023</v>
       </c>
@@ -7730,11 +7894,12 @@
       <c r="K42" s="74">
         <v>0</v>
       </c>
-      <c r="L42" s="74">
+      <c r="L42" s="74"/>
+      <c r="M42" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="47">
         <v>44024</v>
       </c>
@@ -7768,11 +7933,12 @@
       <c r="K43" s="74">
         <v>0</v>
       </c>
-      <c r="L43" s="74">
+      <c r="L43" s="74"/>
+      <c r="M43" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="47">
         <v>44025</v>
       </c>
@@ -7806,11 +7972,12 @@
       <c r="K44" s="48">
         <v>0</v>
       </c>
-      <c r="L44" s="48">
+      <c r="L44" s="48"/>
+      <c r="M44" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="47">
         <v>44026</v>
       </c>
@@ -7844,11 +8011,12 @@
       <c r="K45" s="74">
         <v>0</v>
       </c>
-      <c r="L45" s="74">
+      <c r="L45" s="74"/>
+      <c r="M45" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="47">
         <v>44027</v>
       </c>
@@ -7882,11 +8050,12 @@
       <c r="K46" s="48">
         <v>0</v>
       </c>
-      <c r="L46" s="48">
+      <c r="L46" s="48"/>
+      <c r="M46" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="47">
         <v>44028</v>
       </c>
@@ -7920,11 +8089,12 @@
       <c r="K47" s="74">
         <v>0</v>
       </c>
-      <c r="L47" s="74">
+      <c r="L47" s="74"/>
+      <c r="M47" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="217">
         <v>44029</v>
       </c>
@@ -7958,11 +8128,12 @@
       <c r="K48" s="74">
         <v>0</v>
       </c>
-      <c r="L48" s="74">
+      <c r="L48" s="74"/>
+      <c r="M48" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="217">
         <v>44030</v>
       </c>
@@ -7996,11 +8167,12 @@
       <c r="K49" s="74">
         <v>0</v>
       </c>
-      <c r="L49" s="74">
+      <c r="L49" s="74"/>
+      <c r="M49" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="217">
         <v>44031</v>
       </c>
@@ -8034,11 +8206,12 @@
       <c r="K50" s="74">
         <v>0</v>
       </c>
-      <c r="L50" s="74">
+      <c r="L50" s="74"/>
+      <c r="M50" s="74">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="217">
         <v>44032</v>
       </c>
@@ -8072,11 +8245,12 @@
       <c r="K51" s="48">
         <v>0</v>
       </c>
-      <c r="L51" s="48">
+      <c r="L51" s="48"/>
+      <c r="M51" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="217">
         <v>44033</v>
       </c>
@@ -8110,11 +8284,12 @@
       <c r="K52" s="48">
         <v>0</v>
       </c>
-      <c r="L52" s="48">
+      <c r="L52" s="48"/>
+      <c r="M52" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="217">
         <v>44034</v>
       </c>
@@ -8148,11 +8323,12 @@
       <c r="K53" s="48">
         <v>0</v>
       </c>
-      <c r="L53" s="48">
+      <c r="L53" s="48"/>
+      <c r="M53" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="217">
         <v>44035</v>
       </c>
@@ -8186,11 +8362,12 @@
       <c r="K54" s="48">
         <v>0</v>
       </c>
-      <c r="L54" s="48">
+      <c r="L54" s="48"/>
+      <c r="M54" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="217">
         <v>44036</v>
       </c>
@@ -8224,11 +8401,12 @@
       <c r="K55" s="48">
         <v>0</v>
       </c>
-      <c r="L55" s="48">
+      <c r="L55" s="48"/>
+      <c r="M55" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="217">
         <v>44037</v>
       </c>
@@ -8262,11 +8440,12 @@
       <c r="K56" s="48">
         <v>0</v>
       </c>
-      <c r="L56" s="48">
+      <c r="L56" s="48"/>
+      <c r="M56" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="217">
         <v>44038</v>
       </c>
@@ -8300,11 +8479,12 @@
       <c r="K57" s="48">
         <v>0</v>
       </c>
-      <c r="L57" s="48">
+      <c r="L57" s="48"/>
+      <c r="M57" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="217">
         <v>44039</v>
       </c>
@@ -8338,11 +8518,12 @@
       <c r="K58" s="48">
         <v>0</v>
       </c>
-      <c r="L58" s="48">
+      <c r="L58" s="48"/>
+      <c r="M58" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="217">
         <v>44040</v>
       </c>
@@ -8376,11 +8557,12 @@
       <c r="K59" s="48">
         <v>0</v>
       </c>
-      <c r="L59" s="48">
+      <c r="L59" s="48"/>
+      <c r="M59" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="217">
         <v>44041</v>
       </c>
@@ -8414,11 +8596,12 @@
       <c r="K60" s="48">
         <v>0</v>
       </c>
-      <c r="L60" s="48">
+      <c r="L60" s="48"/>
+      <c r="M60" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="217">
         <v>44042</v>
       </c>
@@ -8452,11 +8635,12 @@
       <c r="K61" s="48">
         <v>0</v>
       </c>
-      <c r="L61" s="48">
+      <c r="L61" s="48"/>
+      <c r="M61" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="217">
         <v>44043</v>
       </c>
@@ -8490,11 +8674,12 @@
       <c r="K62" s="48">
         <v>0</v>
       </c>
-      <c r="L62" s="48">
+      <c r="L62" s="48"/>
+      <c r="M62" s="48">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="217">
         <v>44044</v>
       </c>
@@ -8528,11 +8713,12 @@
       <c r="K63" s="216">
         <v>0</v>
       </c>
-      <c r="L63" s="216">
+      <c r="L63" s="216"/>
+      <c r="M63" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="217">
         <v>44045</v>
       </c>
@@ -8566,11 +8752,12 @@
       <c r="K64" s="216">
         <v>0</v>
       </c>
-      <c r="L64" s="216">
+      <c r="L64" s="216"/>
+      <c r="M64" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="217">
         <v>44046</v>
       </c>
@@ -8604,11 +8791,12 @@
       <c r="K65" s="216">
         <v>0</v>
       </c>
-      <c r="L65" s="216">
+      <c r="L65" s="216"/>
+      <c r="M65" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="217">
         <v>44047</v>
       </c>
@@ -8642,11 +8830,12 @@
       <c r="K66" s="216">
         <v>0</v>
       </c>
-      <c r="L66" s="216">
+      <c r="L66" s="216"/>
+      <c r="M66" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="217">
         <v>44048</v>
       </c>
@@ -8680,11 +8869,12 @@
       <c r="K67" s="216">
         <v>0</v>
       </c>
-      <c r="L67" s="216">
+      <c r="L67" s="216"/>
+      <c r="M67" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="217">
         <v>44049</v>
       </c>
@@ -8718,11 +8908,12 @@
       <c r="K68" s="216">
         <v>0</v>
       </c>
-      <c r="L68" s="216">
+      <c r="L68" s="216"/>
+      <c r="M68" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="217">
         <v>44050</v>
       </c>
@@ -8756,11 +8947,12 @@
       <c r="K69" s="216">
         <v>0</v>
       </c>
-      <c r="L69" s="216">
+      <c r="L69" s="216"/>
+      <c r="M69" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="217">
         <v>44051</v>
       </c>
@@ -8794,11 +8986,12 @@
       <c r="K70" s="216">
         <v>0</v>
       </c>
-      <c r="L70" s="216">
+      <c r="L70" s="216"/>
+      <c r="M70" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="217">
         <v>44052</v>
       </c>
@@ -8832,11 +9025,12 @@
       <c r="K71" s="216">
         <v>0</v>
       </c>
-      <c r="L71" s="216">
+      <c r="L71" s="216"/>
+      <c r="M71" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="217">
         <v>44053</v>
       </c>
@@ -8870,11 +9064,12 @@
       <c r="K72" s="216">
         <v>0</v>
       </c>
-      <c r="L72" s="216">
+      <c r="L72" s="216"/>
+      <c r="M72" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="217">
         <v>44054</v>
       </c>
@@ -8908,11 +9103,12 @@
       <c r="K73" s="216">
         <v>0</v>
       </c>
-      <c r="L73" s="216">
+      <c r="L73" s="216"/>
+      <c r="M73" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="217">
         <v>44055</v>
       </c>
@@ -8946,11 +9142,12 @@
       <c r="K74" s="216">
         <v>0</v>
       </c>
-      <c r="L74" s="216">
+      <c r="L74" s="216"/>
+      <c r="M74" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="217">
         <v>44056</v>
       </c>
@@ -8984,11 +9181,12 @@
       <c r="K75" s="216">
         <v>0</v>
       </c>
-      <c r="L75" s="216">
+      <c r="L75" s="216"/>
+      <c r="M75" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="217">
         <v>44057</v>
       </c>
@@ -9022,11 +9220,12 @@
       <c r="K76" s="216">
         <v>0</v>
       </c>
-      <c r="L76" s="216">
+      <c r="L76" s="216"/>
+      <c r="M76" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="217">
         <v>44058</v>
       </c>
@@ -9060,11 +9259,12 @@
       <c r="K77" s="216">
         <v>0</v>
       </c>
-      <c r="L77" s="216">
+      <c r="L77" s="216"/>
+      <c r="M77" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="217">
         <v>44059</v>
       </c>
@@ -9098,11 +9298,12 @@
       <c r="K78" s="216">
         <v>0</v>
       </c>
-      <c r="L78" s="216">
+      <c r="L78" s="216"/>
+      <c r="M78" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="217">
         <v>44060</v>
       </c>
@@ -9136,11 +9337,12 @@
       <c r="K79" s="216">
         <v>0</v>
       </c>
-      <c r="L79" s="216">
+      <c r="L79" s="216"/>
+      <c r="M79" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="217">
         <v>44061</v>
       </c>
@@ -9174,11 +9376,12 @@
       <c r="K80" s="216">
         <v>0</v>
       </c>
-      <c r="L80" s="216">
+      <c r="L80" s="216"/>
+      <c r="M80" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="217">
         <v>44062</v>
       </c>
@@ -9212,11 +9415,12 @@
       <c r="K81" s="216">
         <v>0</v>
       </c>
-      <c r="L81" s="216">
+      <c r="L81" s="216"/>
+      <c r="M81" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="217">
         <v>44063</v>
       </c>
@@ -9250,11 +9454,12 @@
       <c r="K82" s="216">
         <v>0</v>
       </c>
-      <c r="L82" s="216">
+      <c r="L82" s="216"/>
+      <c r="M82" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="217">
         <v>44064</v>
       </c>
@@ -9288,11 +9493,12 @@
       <c r="K83" s="216">
         <v>0</v>
       </c>
-      <c r="L83" s="216">
+      <c r="L83" s="216"/>
+      <c r="M83" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="217">
         <v>44065</v>
       </c>
@@ -9326,11 +9532,12 @@
       <c r="K84" s="216">
         <v>0</v>
       </c>
-      <c r="L84" s="216">
+      <c r="L84" s="216"/>
+      <c r="M84" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="217">
         <v>44066</v>
       </c>
@@ -9364,11 +9571,12 @@
       <c r="K85" s="216">
         <v>0</v>
       </c>
-      <c r="L85" s="216">
+      <c r="L85" s="216"/>
+      <c r="M85" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="217">
         <v>44067</v>
       </c>
@@ -9402,11 +9610,12 @@
       <c r="K86" s="216">
         <v>0</v>
       </c>
-      <c r="L86" s="216">
+      <c r="L86" s="216"/>
+      <c r="M86" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="217">
         <v>44068</v>
       </c>
@@ -9440,11 +9649,12 @@
       <c r="K87" s="216">
         <v>0</v>
       </c>
-      <c r="L87" s="216">
+      <c r="L87" s="216"/>
+      <c r="M87" s="216">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="15">
         <v>44069</v>
       </c>
@@ -9478,7 +9688,90 @@
       <c r="K88" s="216">
         <v>0</v>
       </c>
-      <c r="L88" s="216">
+      <c r="L88" s="216"/>
+      <c r="M88" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="15">
+        <v>44070</v>
+      </c>
+      <c r="B89" s="216">
+        <v>0</v>
+      </c>
+      <c r="C89" s="216">
+        <v>1</v>
+      </c>
+      <c r="D89" s="216">
+        <v>0</v>
+      </c>
+      <c r="E89" s="216">
+        <v>0</v>
+      </c>
+      <c r="F89" s="216">
+        <v>1</v>
+      </c>
+      <c r="G89" s="216">
+        <v>0</v>
+      </c>
+      <c r="H89" s="216">
+        <v>0</v>
+      </c>
+      <c r="I89" s="216">
+        <v>0</v>
+      </c>
+      <c r="J89" s="216">
+        <v>0</v>
+      </c>
+      <c r="K89" s="216">
+        <v>0</v>
+      </c>
+      <c r="L89" s="216">
+        <v>1</v>
+      </c>
+      <c r="M89" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="15">
+        <v>44071</v>
+      </c>
+      <c r="B90" s="216">
+        <v>0</v>
+      </c>
+      <c r="C90" s="216">
+        <v>1</v>
+      </c>
+      <c r="D90" s="216">
+        <v>0</v>
+      </c>
+      <c r="E90" s="216">
+        <v>0</v>
+      </c>
+      <c r="F90" s="216">
+        <v>1</v>
+      </c>
+      <c r="G90" s="216">
+        <v>0</v>
+      </c>
+      <c r="H90" s="216">
+        <v>0</v>
+      </c>
+      <c r="I90" s="216">
+        <v>0</v>
+      </c>
+      <c r="J90" s="216">
+        <v>0</v>
+      </c>
+      <c r="K90" s="216">
+        <v>0</v>
+      </c>
+      <c r="L90" s="216">
+        <v>1</v>
+      </c>
+      <c r="M90" s="216">
         <v>4</v>
       </c>
     </row>
@@ -9489,11 +9782,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O88"/>
+  <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O88" sqref="O88"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13316,6 +13609,94 @@
         <v>0</v>
       </c>
       <c r="N88" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="15">
+        <v>44070</v>
+      </c>
+      <c r="B89" s="216">
+        <v>0</v>
+      </c>
+      <c r="C89" s="216">
+        <v>1</v>
+      </c>
+      <c r="D89" s="216">
+        <v>0</v>
+      </c>
+      <c r="E89" s="216">
+        <v>0</v>
+      </c>
+      <c r="F89" s="216">
+        <v>0</v>
+      </c>
+      <c r="G89" s="216">
+        <v>0</v>
+      </c>
+      <c r="H89" s="216">
+        <v>1</v>
+      </c>
+      <c r="I89" s="216">
+        <v>0</v>
+      </c>
+      <c r="J89" s="216">
+        <v>0</v>
+      </c>
+      <c r="K89" s="216">
+        <v>1</v>
+      </c>
+      <c r="L89" s="216">
+        <v>0</v>
+      </c>
+      <c r="M89" s="216">
+        <v>0</v>
+      </c>
+      <c r="N89" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="15">
+        <v>44071</v>
+      </c>
+      <c r="B90" s="216">
+        <v>0</v>
+      </c>
+      <c r="C90" s="216">
+        <v>1</v>
+      </c>
+      <c r="D90" s="216">
+        <v>0</v>
+      </c>
+      <c r="E90" s="216">
+        <v>0</v>
+      </c>
+      <c r="F90" s="216">
+        <v>0</v>
+      </c>
+      <c r="G90" s="216">
+        <v>0</v>
+      </c>
+      <c r="H90" s="216">
+        <v>1</v>
+      </c>
+      <c r="I90" s="216">
+        <v>0</v>
+      </c>
+      <c r="J90" s="216">
+        <v>0</v>
+      </c>
+      <c r="K90" s="216">
+        <v>1</v>
+      </c>
+      <c r="L90" s="216">
+        <v>0</v>
+      </c>
+      <c r="M90" s="216">
+        <v>0</v>
+      </c>
+      <c r="N90" s="216">
         <v>0</v>
       </c>
     </row>
@@ -13326,11 +13707,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K88" sqref="K88"/>
+      <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16159,6 +16540,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="15">
+        <v>44070</v>
+      </c>
+      <c r="B89" s="216">
+        <v>0</v>
+      </c>
+      <c r="C89" s="216">
+        <v>0</v>
+      </c>
+      <c r="D89" s="216">
+        <v>0</v>
+      </c>
+      <c r="E89" s="216">
+        <v>0</v>
+      </c>
+      <c r="F89" s="216">
+        <v>2</v>
+      </c>
+      <c r="G89" s="216">
+        <v>1</v>
+      </c>
+      <c r="H89" s="216">
+        <v>1</v>
+      </c>
+      <c r="I89" s="216">
+        <v>1</v>
+      </c>
+      <c r="J89" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="15">
+        <v>44071</v>
+      </c>
+      <c r="B90" s="216">
+        <v>0</v>
+      </c>
+      <c r="C90" s="216">
+        <v>0</v>
+      </c>
+      <c r="D90" s="216">
+        <v>0</v>
+      </c>
+      <c r="E90" s="216">
+        <v>0</v>
+      </c>
+      <c r="F90" s="216">
+        <v>2</v>
+      </c>
+      <c r="G90" s="216">
+        <v>1</v>
+      </c>
+      <c r="H90" s="216">
+        <v>1</v>
+      </c>
+      <c r="I90" s="216">
+        <v>1</v>
+      </c>
+      <c r="J90" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16166,10 +16611,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:CL20"/>
+  <dimension ref="A1:CQ20"/>
   <sheetViews>
-    <sheetView topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="CK23" sqref="CK23"/>
+    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
+      <selection activeCell="CN17" sqref="CN17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16177,7 +16622,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -16442,8 +16887,14 @@
       <c r="CJ1" s="49">
         <v>44069</v>
       </c>
-    </row>
-    <row r="2" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK1" s="49">
+        <v>44070</v>
+      </c>
+      <c r="CL1" s="49">
+        <v>44071</v>
+      </c>
+    </row>
+    <row r="2" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -16708,8 +17159,14 @@
       <c r="CJ2">
         <v>5702</v>
       </c>
-    </row>
-    <row r="3" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK2">
+        <v>5734</v>
+      </c>
+      <c r="CL2">
+        <v>5766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -16974,8 +17431,14 @@
       <c r="CJ3">
         <v>5503</v>
       </c>
-    </row>
-    <row r="4" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK3">
+        <v>5538</v>
+      </c>
+      <c r="CL3">
+        <v>5570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -17240,8 +17703,14 @@
       <c r="CJ4">
         <v>5503</v>
       </c>
-    </row>
-    <row r="5" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK4">
+        <v>5538</v>
+      </c>
+      <c r="CL4">
+        <v>5570</v>
+      </c>
+    </row>
+    <row r="5" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -17506,8 +17975,14 @@
       <c r="CJ5">
         <v>5503</v>
       </c>
-    </row>
-    <row r="6" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK5">
+        <v>5538</v>
+      </c>
+      <c r="CL5">
+        <v>5570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -17772,8 +18247,14 @@
       <c r="CJ6">
         <v>5503</v>
       </c>
-    </row>
-    <row r="7" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK6">
+        <v>5538</v>
+      </c>
+      <c r="CL6">
+        <v>5570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -18038,8 +18519,14 @@
       <c r="CJ7">
         <v>4807</v>
       </c>
-    </row>
-    <row r="8" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK7">
+        <v>4839</v>
+      </c>
+      <c r="CL7">
+        <v>4871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -18304,8 +18791,14 @@
       <c r="CJ8">
         <v>7437</v>
       </c>
-    </row>
-    <row r="9" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK8">
+        <v>7469</v>
+      </c>
+      <c r="CL8">
+        <v>7501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -18394,8 +18887,14 @@
       <c r="CH9" s="312"/>
       <c r="CI9" s="561"/>
       <c r="CJ9" s="312"/>
-    </row>
-    <row r="10" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK9" s="312"/>
+      <c r="CL9" s="312"/>
+      <c r="CM9" s="312"/>
+      <c r="CN9" s="312"/>
+      <c r="CO9" s="312"/>
+      <c r="CP9" s="312"/>
+    </row>
+    <row r="10" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -18660,8 +19159,14 @@
       <c r="CJ10" s="216">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK10" s="216">
+        <v>228</v>
+      </c>
+      <c r="CL10" s="216">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -18926,8 +19431,14 @@
       <c r="CJ11" s="216">
         <v>227</v>
       </c>
-    </row>
-    <row r="12" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK11" s="216">
+        <v>228</v>
+      </c>
+      <c r="CL11" s="216">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -19192,8 +19703,14 @@
       <c r="CJ12" s="216">
         <v>227</v>
       </c>
-    </row>
-    <row r="13" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK12" s="216">
+        <v>228</v>
+      </c>
+      <c r="CL12" s="216">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -19458,8 +19975,14 @@
       <c r="CJ13" s="216">
         <v>227</v>
       </c>
-    </row>
-    <row r="14" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK13" s="216">
+        <v>228</v>
+      </c>
+      <c r="CL13" s="216">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -19724,8 +20247,14 @@
       <c r="CJ14" s="216">
         <v>227</v>
       </c>
-    </row>
-    <row r="15" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK14" s="216">
+        <v>228</v>
+      </c>
+      <c r="CL14" s="216">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -19990,8 +20519,14 @@
       <c r="CJ15" s="216">
         <v>162</v>
       </c>
-    </row>
-    <row r="16" spans="1:88" x14ac:dyDescent="0.2">
+      <c r="CK15" s="216">
+        <v>163</v>
+      </c>
+      <c r="CL15" s="216">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -20256,8 +20791,14 @@
       <c r="CJ16" s="216">
         <v>239</v>
       </c>
-    </row>
-    <row r="17" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="CK16" s="216">
+        <v>240</v>
+      </c>
+      <c r="CL16" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -20348,8 +20889,13 @@
       <c r="CJ17" s="312"/>
       <c r="CK17" s="312"/>
       <c r="CL17" s="312"/>
-    </row>
-    <row r="18" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="CM17" s="312"/>
+      <c r="CN17" s="312"/>
+      <c r="CO17" s="312"/>
+      <c r="CP17" s="312"/>
+      <c r="CQ17" s="312"/>
+    </row>
+    <row r="18" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -20614,15 +21160,21 @@
       <c r="CJ18">
         <v>1318</v>
       </c>
-    </row>
-    <row r="19" spans="1:90" x14ac:dyDescent="0.2">
+      <c r="CK18">
+        <v>1337</v>
+      </c>
+      <c r="CL18" s="216">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:90" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -20791,7 +21343,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CJ20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CL20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -20973,6 +21525,14 @@
       <c r="CJ20" s="51">
         <f t="shared" si="1"/>
         <v>42812</v>
+      </c>
+      <c r="CK20" s="51">
+        <f t="shared" si="1"/>
+        <v>43074</v>
+      </c>
+      <c r="CL20" s="51">
+        <f t="shared" si="1"/>
+        <v>43312</v>
       </c>
     </row>
   </sheetData>
@@ -21272,43 +21832,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="825" t="s">
+      <c r="B8" s="843" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="825"/>
+      <c r="B9" s="843"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="825"/>
+      <c r="B10" s="843"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="825"/>
+      <c r="B11" s="843"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="826" t="s">
+      <c r="B12" s="844" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="826"/>
+      <c r="B13" s="844"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="826"/>
+      <c r="B14" s="844"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="827" t="s">
+      <c r="B15" s="845" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="827"/>
+      <c r="B16" s="845"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 29th and 30th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DD9157-345E-CD44-8CA4-C2F0674F681B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF84C0D-5AD7-A74D-93CF-AA4F262A6188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="846">
+  <cellXfs count="864">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2611,6 +2611,60 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3398,10 +3452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6289,6 +6343,70 @@
         <v>1319957</v>
       </c>
     </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="15">
+        <v>44072</v>
+      </c>
+      <c r="B91" s="843">
+        <v>591712</v>
+      </c>
+      <c r="C91" s="844">
+        <v>658309</v>
+      </c>
+      <c r="D91" s="845">
+        <v>84310</v>
+      </c>
+      <c r="E91" s="846">
+        <v>63819</v>
+      </c>
+      <c r="F91" s="847">
+        <v>25.503285382077767</v>
+      </c>
+      <c r="G91" s="848">
+        <v>150906</v>
+      </c>
+      <c r="H91" s="849">
+        <v>12930</v>
+      </c>
+      <c r="I91" s="850">
+        <v>18623</v>
+      </c>
+      <c r="J91" s="851">
+        <v>1334331</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="15">
+        <v>44073</v>
+      </c>
+      <c r="B92" s="852">
+        <v>595841</v>
+      </c>
+      <c r="C92" s="853">
+        <v>663474</v>
+      </c>
+      <c r="D92" s="854">
+        <v>81151</v>
+      </c>
+      <c r="E92" s="855">
+        <v>64158</v>
+      </c>
+      <c r="F92" s="856">
+        <v>25.459140945319302</v>
+      </c>
+      <c r="G92" s="857">
+        <v>151696</v>
+      </c>
+      <c r="H92" s="858">
+        <v>12998</v>
+      </c>
+      <c r="I92" s="859">
+        <v>18712</v>
+      </c>
+      <c r="J92" s="860">
+        <v>1340466</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6296,11 +6414,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9655,7 +9773,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A88" s="15">
+      <c r="A88" s="217">
         <v>44069</v>
       </c>
       <c r="B88" s="216">
@@ -9694,7 +9812,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A89" s="15">
+      <c r="A89" s="217">
         <v>44070</v>
       </c>
       <c r="B89" s="216">
@@ -9735,7 +9853,7 @@
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A90" s="15">
+      <c r="A90" s="217">
         <v>44071</v>
       </c>
       <c r="B90" s="216">
@@ -9774,6 +9892,91 @@
       <c r="M90" s="216">
         <v>4</v>
       </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="217">
+        <v>44072</v>
+      </c>
+      <c r="B91" s="216">
+        <v>0</v>
+      </c>
+      <c r="C91" s="216">
+        <v>1</v>
+      </c>
+      <c r="D91" s="216">
+        <v>0</v>
+      </c>
+      <c r="E91" s="216">
+        <v>0</v>
+      </c>
+      <c r="F91" s="216">
+        <v>1</v>
+      </c>
+      <c r="G91" s="216">
+        <v>0</v>
+      </c>
+      <c r="H91" s="216">
+        <v>0</v>
+      </c>
+      <c r="I91" s="216">
+        <v>0</v>
+      </c>
+      <c r="J91" s="216">
+        <v>0</v>
+      </c>
+      <c r="K91" s="216">
+        <v>0</v>
+      </c>
+      <c r="L91" s="216">
+        <v>1</v>
+      </c>
+      <c r="M91" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="217">
+        <v>44073</v>
+      </c>
+      <c r="B92" s="216">
+        <v>0</v>
+      </c>
+      <c r="C92" s="216">
+        <v>1</v>
+      </c>
+      <c r="D92" s="216">
+        <v>0</v>
+      </c>
+      <c r="E92" s="216">
+        <v>0</v>
+      </c>
+      <c r="F92" s="216">
+        <v>1</v>
+      </c>
+      <c r="G92" s="216">
+        <v>0</v>
+      </c>
+      <c r="H92" s="216">
+        <v>0</v>
+      </c>
+      <c r="I92" s="216">
+        <v>0</v>
+      </c>
+      <c r="J92" s="216">
+        <v>0</v>
+      </c>
+      <c r="K92" s="216">
+        <v>0</v>
+      </c>
+      <c r="L92" s="216">
+        <v>1</v>
+      </c>
+      <c r="M92" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9782,11 +9985,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O90"/>
+  <dimension ref="A1:O92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O90" sqref="O90"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13569,7 +13772,7 @@
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" s="15">
+      <c r="A88" s="217">
         <v>44069</v>
       </c>
       <c r="B88" s="216">
@@ -13613,7 +13816,7 @@
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A89" s="15">
+      <c r="A89" s="217">
         <v>44070</v>
       </c>
       <c r="B89" s="216">
@@ -13657,7 +13860,7 @@
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A90" s="15">
+      <c r="A90" s="217">
         <v>44071</v>
       </c>
       <c r="B90" s="216">
@@ -13697,6 +13900,94 @@
         <v>0</v>
       </c>
       <c r="N90" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="217">
+        <v>44072</v>
+      </c>
+      <c r="B91" s="216">
+        <v>0</v>
+      </c>
+      <c r="C91" s="216">
+        <v>1</v>
+      </c>
+      <c r="D91" s="216">
+        <v>0</v>
+      </c>
+      <c r="E91" s="216">
+        <v>0</v>
+      </c>
+      <c r="F91" s="216">
+        <v>0</v>
+      </c>
+      <c r="G91" s="216">
+        <v>0</v>
+      </c>
+      <c r="H91" s="216">
+        <v>1</v>
+      </c>
+      <c r="I91" s="216">
+        <v>0</v>
+      </c>
+      <c r="J91" s="216">
+        <v>0</v>
+      </c>
+      <c r="K91" s="216">
+        <v>1</v>
+      </c>
+      <c r="L91" s="216">
+        <v>0</v>
+      </c>
+      <c r="M91" s="216">
+        <v>0</v>
+      </c>
+      <c r="N91" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" s="217">
+        <v>44073</v>
+      </c>
+      <c r="B92" s="216">
+        <v>0</v>
+      </c>
+      <c r="C92" s="216">
+        <v>1</v>
+      </c>
+      <c r="D92" s="216">
+        <v>0</v>
+      </c>
+      <c r="E92" s="216">
+        <v>0</v>
+      </c>
+      <c r="F92" s="216">
+        <v>0</v>
+      </c>
+      <c r="G92" s="216">
+        <v>0</v>
+      </c>
+      <c r="H92" s="216">
+        <v>1</v>
+      </c>
+      <c r="I92" s="216">
+        <v>0</v>
+      </c>
+      <c r="J92" s="216">
+        <v>0</v>
+      </c>
+      <c r="K92" s="216">
+        <v>1</v>
+      </c>
+      <c r="L92" s="216">
+        <v>0</v>
+      </c>
+      <c r="M92" s="216">
+        <v>0</v>
+      </c>
+      <c r="N92" s="216">
         <v>0</v>
       </c>
     </row>
@@ -13707,11 +13998,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16509,7 +16800,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" s="15">
+      <c r="A88" s="495">
         <v>44069</v>
       </c>
       <c r="B88" s="216">
@@ -16541,7 +16832,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="15">
+      <c r="A89" s="495">
         <v>44070</v>
       </c>
       <c r="B89" s="216">
@@ -16573,7 +16864,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" s="15">
+      <c r="A90" s="495">
         <v>44071</v>
       </c>
       <c r="B90" s="216">
@@ -16601,6 +16892,70 @@
         <v>1</v>
       </c>
       <c r="J90" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="495">
+        <v>44072</v>
+      </c>
+      <c r="B91" s="216">
+        <v>0</v>
+      </c>
+      <c r="C91" s="216">
+        <v>0</v>
+      </c>
+      <c r="D91" s="216">
+        <v>0</v>
+      </c>
+      <c r="E91" s="216">
+        <v>0</v>
+      </c>
+      <c r="F91" s="216">
+        <v>2</v>
+      </c>
+      <c r="G91" s="216">
+        <v>1</v>
+      </c>
+      <c r="H91" s="216">
+        <v>1</v>
+      </c>
+      <c r="I91" s="216">
+        <v>1</v>
+      </c>
+      <c r="J91" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="495">
+        <v>44073</v>
+      </c>
+      <c r="B92" s="216">
+        <v>0</v>
+      </c>
+      <c r="C92" s="216">
+        <v>0</v>
+      </c>
+      <c r="D92" s="216">
+        <v>0</v>
+      </c>
+      <c r="E92" s="216">
+        <v>0</v>
+      </c>
+      <c r="F92" s="216">
+        <v>2</v>
+      </c>
+      <c r="G92" s="216">
+        <v>1</v>
+      </c>
+      <c r="H92" s="216">
+        <v>1</v>
+      </c>
+      <c r="I92" s="216">
+        <v>1</v>
+      </c>
+      <c r="J92" s="216">
         <v>2</v>
       </c>
     </row>
@@ -16611,10 +16966,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:CQ20"/>
+  <dimension ref="A1:CR20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CN17" sqref="CN17"/>
+      <selection activeCell="CI24" sqref="CI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16622,7 +16977,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -16884,7 +17239,7 @@
       <c r="CI1" s="49">
         <v>44068</v>
       </c>
-      <c r="CJ1" s="49">
+      <c r="CJ1" s="228">
         <v>44069</v>
       </c>
       <c r="CK1" s="49">
@@ -16893,8 +17248,18 @@
       <c r="CL1" s="49">
         <v>44071</v>
       </c>
-    </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM1" s="49">
+        <v>44072</v>
+      </c>
+      <c r="CN1" s="49">
+        <v>44073</v>
+      </c>
+      <c r="CO1" s="48"/>
+      <c r="CP1" s="48"/>
+      <c r="CQ1" s="48"/>
+      <c r="CR1" s="48"/>
+    </row>
+    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -17159,14 +17524,24 @@
       <c r="CJ2">
         <v>5702</v>
       </c>
-      <c r="CK2">
+      <c r="CK2" s="48">
         <v>5734</v>
       </c>
-      <c r="CL2">
+      <c r="CL2" s="48">
         <v>5766</v>
       </c>
-    </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM2" s="48">
+        <v>5798</v>
+      </c>
+      <c r="CN2" s="48">
+        <v>5830</v>
+      </c>
+      <c r="CO2" s="48"/>
+      <c r="CP2" s="48"/>
+      <c r="CQ2" s="48"/>
+      <c r="CR2" s="48"/>
+    </row>
+    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -17431,14 +17806,24 @@
       <c r="CJ3">
         <v>5503</v>
       </c>
-      <c r="CK3">
+      <c r="CK3" s="48">
         <v>5538</v>
       </c>
-      <c r="CL3">
+      <c r="CL3" s="48">
         <v>5570</v>
       </c>
-    </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM3" s="48">
+        <v>5602</v>
+      </c>
+      <c r="CN3" s="48">
+        <v>5634</v>
+      </c>
+      <c r="CO3" s="48"/>
+      <c r="CP3" s="48"/>
+      <c r="CQ3" s="48"/>
+      <c r="CR3" s="48"/>
+    </row>
+    <row r="4" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -17703,14 +18088,24 @@
       <c r="CJ4">
         <v>5503</v>
       </c>
-      <c r="CK4">
+      <c r="CK4" s="48">
         <v>5538</v>
       </c>
-      <c r="CL4">
+      <c r="CL4" s="48">
         <v>5570</v>
       </c>
-    </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM4" s="48">
+        <v>5602</v>
+      </c>
+      <c r="CN4" s="48">
+        <v>5634</v>
+      </c>
+      <c r="CO4" s="48"/>
+      <c r="CP4" s="48"/>
+      <c r="CQ4" s="48"/>
+      <c r="CR4" s="48"/>
+    </row>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -17975,14 +18370,24 @@
       <c r="CJ5">
         <v>5503</v>
       </c>
-      <c r="CK5">
+      <c r="CK5" s="48">
         <v>5538</v>
       </c>
-      <c r="CL5">
+      <c r="CL5" s="48">
         <v>5570</v>
       </c>
-    </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM5" s="48">
+        <v>5602</v>
+      </c>
+      <c r="CN5" s="48">
+        <v>5634</v>
+      </c>
+      <c r="CO5" s="48"/>
+      <c r="CP5" s="48"/>
+      <c r="CQ5" s="48"/>
+      <c r="CR5" s="48"/>
+    </row>
+    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -18247,14 +18652,24 @@
       <c r="CJ6">
         <v>5503</v>
       </c>
-      <c r="CK6">
+      <c r="CK6" s="48">
         <v>5538</v>
       </c>
-      <c r="CL6">
+      <c r="CL6" s="48">
         <v>5570</v>
       </c>
-    </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM6" s="48">
+        <v>5602</v>
+      </c>
+      <c r="CN6" s="48">
+        <v>5634</v>
+      </c>
+      <c r="CO6" s="48"/>
+      <c r="CP6" s="48"/>
+      <c r="CQ6" s="48"/>
+      <c r="CR6" s="48"/>
+    </row>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -18519,14 +18934,24 @@
       <c r="CJ7">
         <v>4807</v>
       </c>
-      <c r="CK7">
+      <c r="CK7" s="48">
         <v>4839</v>
       </c>
-      <c r="CL7">
+      <c r="CL7" s="48">
         <v>4871</v>
       </c>
-    </row>
-    <row r="8" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM7" s="48">
+        <v>4903</v>
+      </c>
+      <c r="CN7" s="48">
+        <v>4935</v>
+      </c>
+      <c r="CO7" s="48"/>
+      <c r="CP7" s="48"/>
+      <c r="CQ7" s="48"/>
+      <c r="CR7" s="48"/>
+    </row>
+    <row r="8" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -18791,14 +19216,24 @@
       <c r="CJ8">
         <v>7437</v>
       </c>
-      <c r="CK8">
+      <c r="CK8" s="48">
         <v>7469</v>
       </c>
-      <c r="CL8">
+      <c r="CL8" s="48">
         <v>7501</v>
       </c>
-    </row>
-    <row r="9" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM8" s="48">
+        <v>7533</v>
+      </c>
+      <c r="CN8" s="48">
+        <v>7565</v>
+      </c>
+      <c r="CO8" s="48"/>
+      <c r="CP8" s="48"/>
+      <c r="CQ8" s="48"/>
+      <c r="CR8" s="48"/>
+    </row>
+    <row r="9" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -18886,15 +19321,17 @@
       <c r="CG9" s="312"/>
       <c r="CH9" s="312"/>
       <c r="CI9" s="561"/>
-      <c r="CJ9" s="312"/>
+      <c r="CJ9" s="560"/>
       <c r="CK9" s="312"/>
       <c r="CL9" s="312"/>
       <c r="CM9" s="312"/>
       <c r="CN9" s="312"/>
       <c r="CO9" s="312"/>
       <c r="CP9" s="312"/>
-    </row>
-    <row r="10" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CQ9" s="48"/>
+      <c r="CR9" s="48"/>
+    </row>
+    <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -19156,17 +19593,27 @@
       <c r="CI10" s="216">
         <v>226</v>
       </c>
-      <c r="CJ10" s="216">
+      <c r="CJ10" s="230">
         <v>227</v>
       </c>
-      <c r="CK10" s="216">
+      <c r="CK10" s="74">
         <v>228</v>
       </c>
-      <c r="CL10" s="216">
+      <c r="CL10" s="74">
         <v>229</v>
       </c>
-    </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM10" s="74">
+        <v>230</v>
+      </c>
+      <c r="CN10" s="74">
+        <v>231</v>
+      </c>
+      <c r="CO10" s="48"/>
+      <c r="CP10" s="48"/>
+      <c r="CQ10" s="48"/>
+      <c r="CR10" s="48"/>
+    </row>
+    <row r="11" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -19428,17 +19875,27 @@
       <c r="CI11" s="216">
         <v>226</v>
       </c>
-      <c r="CJ11" s="216">
+      <c r="CJ11" s="230">
         <v>227</v>
       </c>
-      <c r="CK11" s="216">
+      <c r="CK11" s="74">
         <v>228</v>
       </c>
-      <c r="CL11" s="216">
+      <c r="CL11" s="74">
         <v>229</v>
       </c>
-    </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM11" s="74">
+        <v>230</v>
+      </c>
+      <c r="CN11" s="74">
+        <v>231</v>
+      </c>
+      <c r="CO11" s="48"/>
+      <c r="CP11" s="48"/>
+      <c r="CQ11" s="48"/>
+      <c r="CR11" s="48"/>
+    </row>
+    <row r="12" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -19700,17 +20157,27 @@
       <c r="CI12" s="216">
         <v>226</v>
       </c>
-      <c r="CJ12" s="216">
+      <c r="CJ12" s="230">
         <v>227</v>
       </c>
-      <c r="CK12" s="216">
+      <c r="CK12" s="74">
         <v>228</v>
       </c>
-      <c r="CL12" s="216">
+      <c r="CL12" s="74">
         <v>229</v>
       </c>
-    </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM12" s="74">
+        <v>230</v>
+      </c>
+      <c r="CN12" s="74">
+        <v>231</v>
+      </c>
+      <c r="CO12" s="48"/>
+      <c r="CP12" s="48"/>
+      <c r="CQ12" s="48"/>
+      <c r="CR12" s="48"/>
+    </row>
+    <row r="13" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -19972,17 +20439,27 @@
       <c r="CI13" s="216">
         <v>226</v>
       </c>
-      <c r="CJ13" s="216">
+      <c r="CJ13" s="230">
         <v>227</v>
       </c>
-      <c r="CK13" s="216">
+      <c r="CK13" s="74">
         <v>228</v>
       </c>
-      <c r="CL13" s="216">
+      <c r="CL13" s="74">
         <v>229</v>
       </c>
-    </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM13" s="74">
+        <v>230</v>
+      </c>
+      <c r="CN13" s="74">
+        <v>231</v>
+      </c>
+      <c r="CO13" s="48"/>
+      <c r="CP13" s="48"/>
+      <c r="CQ13" s="48"/>
+      <c r="CR13" s="48"/>
+    </row>
+    <row r="14" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -20244,17 +20721,27 @@
       <c r="CI14" s="216">
         <v>226</v>
       </c>
-      <c r="CJ14" s="216">
+      <c r="CJ14" s="230">
         <v>227</v>
       </c>
-      <c r="CK14" s="216">
+      <c r="CK14" s="74">
         <v>228</v>
       </c>
-      <c r="CL14" s="216">
+      <c r="CL14" s="74">
         <v>229</v>
       </c>
-    </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM14" s="74">
+        <v>230</v>
+      </c>
+      <c r="CN14" s="74">
+        <v>231</v>
+      </c>
+      <c r="CO14" s="48"/>
+      <c r="CP14" s="48"/>
+      <c r="CQ14" s="48"/>
+      <c r="CR14" s="48"/>
+    </row>
+    <row r="15" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -20516,17 +21003,27 @@
       <c r="CI15" s="216">
         <v>161</v>
       </c>
-      <c r="CJ15" s="216">
+      <c r="CJ15" s="230">
         <v>162</v>
       </c>
-      <c r="CK15" s="216">
+      <c r="CK15" s="74">
         <v>163</v>
       </c>
-      <c r="CL15" s="216">
+      <c r="CL15" s="74">
         <v>164</v>
       </c>
-    </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.2">
+      <c r="CM15" s="74">
+        <v>165</v>
+      </c>
+      <c r="CN15" s="48">
+        <v>166</v>
+      </c>
+      <c r="CO15" s="48"/>
+      <c r="CP15" s="48"/>
+      <c r="CQ15" s="48"/>
+      <c r="CR15" s="48"/>
+    </row>
+    <row r="16" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -20788,17 +21285,27 @@
       <c r="CI16" s="216">
         <v>238</v>
       </c>
-      <c r="CJ16" s="216">
+      <c r="CJ16" s="230">
         <v>239</v>
       </c>
-      <c r="CK16" s="216">
+      <c r="CK16" s="74">
         <v>240</v>
       </c>
-      <c r="CL16" s="216">
+      <c r="CL16" s="74">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="CM16" s="74">
+        <v>242</v>
+      </c>
+      <c r="CN16" s="74">
+        <v>243</v>
+      </c>
+      <c r="CO16" s="48"/>
+      <c r="CP16" s="48"/>
+      <c r="CQ16" s="48"/>
+      <c r="CR16" s="48"/>
+    </row>
+    <row r="17" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -20886,7 +21393,7 @@
       <c r="CG17" s="312"/>
       <c r="CH17" s="312"/>
       <c r="CI17" s="312"/>
-      <c r="CJ17" s="312"/>
+      <c r="CJ17" s="560"/>
       <c r="CK17" s="312"/>
       <c r="CL17" s="312"/>
       <c r="CM17" s="312"/>
@@ -20894,8 +21401,9 @@
       <c r="CO17" s="312"/>
       <c r="CP17" s="312"/>
       <c r="CQ17" s="312"/>
-    </row>
-    <row r="18" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="CR17" s="48"/>
+    </row>
+    <row r="18" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -21160,21 +21668,31 @@
       <c r="CJ18">
         <v>1318</v>
       </c>
-      <c r="CK18">
+      <c r="CK18" s="48">
         <v>1337</v>
       </c>
-      <c r="CL18" s="216">
+      <c r="CL18" s="74">
         <v>1344</v>
       </c>
-    </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="CM18" s="74">
+        <v>1351</v>
+      </c>
+      <c r="CN18" s="48">
+        <v>1358</v>
+      </c>
+      <c r="CO18" s="48"/>
+      <c r="CP18" s="48"/>
+      <c r="CQ18" s="48"/>
+      <c r="CR18" s="48"/>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -21343,7 +21861,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CL20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CN20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -21533,6 +22051,14 @@
       <c r="CL20" s="51">
         <f t="shared" si="1"/>
         <v>43312</v>
+      </c>
+      <c r="CM20" s="51">
+        <f t="shared" si="1"/>
+        <v>43550</v>
+      </c>
+      <c r="CN20" s="51">
+        <f t="shared" si="1"/>
+        <v>43788</v>
       </c>
     </row>
   </sheetData>
@@ -21832,43 +22358,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="843" t="s">
+      <c r="B8" s="861" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="843"/>
+      <c r="B9" s="861"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="843"/>
+      <c r="B10" s="861"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="843"/>
+      <c r="B11" s="861"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="844" t="s">
+      <c r="B12" s="862" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="844"/>
+      <c r="B13" s="862"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="844"/>
+      <c r="B14" s="862"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="845" t="s">
+      <c r="B15" s="863" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="845"/>
+      <c r="B16" s="863"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for August 31th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF84C0D-5AD7-A74D-93CF-AA4F262A6188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6808C43-41D6-8340-882A-26E45BAA1A0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="864">
+  <cellXfs count="874">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3124,6 +3124,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3132,6 +3159,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3452,10 +3482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6405,6 +6435,38 @@
       </c>
       <c r="J92" s="860">
         <v>1340466</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="15">
+        <v>44074</v>
+      </c>
+      <c r="B93" s="861">
+        <v>599560</v>
+      </c>
+      <c r="C93" s="862">
+        <v>668193</v>
+      </c>
+      <c r="D93" s="863">
+        <v>77730</v>
+      </c>
+      <c r="E93" s="864">
+        <v>64414</v>
+      </c>
+      <c r="F93" s="865">
+        <v>25.420141437053839</v>
+      </c>
+      <c r="G93" s="866">
+        <v>152409</v>
+      </c>
+      <c r="H93" s="867">
+        <v>13046</v>
+      </c>
+      <c r="I93" s="868">
+        <v>18766</v>
+      </c>
+      <c r="J93" s="869">
+        <v>1345483</v>
       </c>
     </row>
   </sheetData>
@@ -6418,7 +6480,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A93"/>
+      <selection pane="bottomLeft" activeCell="N93" sqref="N93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9976,7 +10038,45 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="217"/>
+      <c r="A93" s="15">
+        <v>44074</v>
+      </c>
+      <c r="B93" s="216">
+        <v>0</v>
+      </c>
+      <c r="C93" s="216">
+        <v>1</v>
+      </c>
+      <c r="D93" s="216">
+        <v>0</v>
+      </c>
+      <c r="E93" s="216">
+        <v>0</v>
+      </c>
+      <c r="F93" s="216">
+        <v>1</v>
+      </c>
+      <c r="G93" s="216">
+        <v>0</v>
+      </c>
+      <c r="H93" s="216">
+        <v>0</v>
+      </c>
+      <c r="I93" s="216">
+        <v>0</v>
+      </c>
+      <c r="J93" s="216">
+        <v>0</v>
+      </c>
+      <c r="K93" s="216">
+        <v>0</v>
+      </c>
+      <c r="L93" s="216">
+        <v>1</v>
+      </c>
+      <c r="M93" s="216">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9985,11 +10085,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O92"/>
+  <dimension ref="A1:O93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A92"/>
+      <selection pane="bottomLeft" activeCell="O93" sqref="O93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13988,6 +14088,50 @@
         <v>0</v>
       </c>
       <c r="N92" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="873">
+        <v>44074</v>
+      </c>
+      <c r="B93" s="216">
+        <v>0</v>
+      </c>
+      <c r="C93" s="216">
+        <v>1</v>
+      </c>
+      <c r="D93" s="216">
+        <v>0</v>
+      </c>
+      <c r="E93" s="216">
+        <v>0</v>
+      </c>
+      <c r="F93" s="216">
+        <v>0</v>
+      </c>
+      <c r="G93" s="216">
+        <v>0</v>
+      </c>
+      <c r="H93" s="216">
+        <v>1</v>
+      </c>
+      <c r="I93" s="216">
+        <v>0</v>
+      </c>
+      <c r="J93" s="216">
+        <v>0</v>
+      </c>
+      <c r="K93" s="216">
+        <v>1</v>
+      </c>
+      <c r="L93" s="216">
+        <v>0</v>
+      </c>
+      <c r="M93" s="216">
+        <v>0</v>
+      </c>
+      <c r="N93" s="216">
         <v>0</v>
       </c>
     </row>
@@ -13998,11 +14142,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87:A92"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16959,6 +17103,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="873">
+        <v>44074</v>
+      </c>
+      <c r="B93" s="216">
+        <v>0</v>
+      </c>
+      <c r="C93" s="216">
+        <v>0</v>
+      </c>
+      <c r="D93" s="216">
+        <v>0</v>
+      </c>
+      <c r="E93" s="216">
+        <v>0</v>
+      </c>
+      <c r="F93" s="216">
+        <v>2</v>
+      </c>
+      <c r="G93" s="216">
+        <v>1</v>
+      </c>
+      <c r="H93" s="216">
+        <v>1</v>
+      </c>
+      <c r="I93" s="216">
+        <v>1</v>
+      </c>
+      <c r="J93" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16969,7 +17145,7 @@
   <dimension ref="A1:CR20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CI24" sqref="CI24"/>
+      <selection activeCell="CQ22" sqref="CQ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17254,7 +17430,9 @@
       <c r="CN1" s="49">
         <v>44073</v>
       </c>
-      <c r="CO1" s="48"/>
+      <c r="CO1" s="49">
+        <v>44074</v>
+      </c>
       <c r="CP1" s="48"/>
       <c r="CQ1" s="48"/>
       <c r="CR1" s="48"/>
@@ -17536,7 +17714,9 @@
       <c r="CN2" s="48">
         <v>5830</v>
       </c>
-      <c r="CO2" s="48"/>
+      <c r="CO2" s="48">
+        <v>5862</v>
+      </c>
       <c r="CP2" s="48"/>
       <c r="CQ2" s="48"/>
       <c r="CR2" s="48"/>
@@ -17818,7 +17998,9 @@
       <c r="CN3" s="48">
         <v>5634</v>
       </c>
-      <c r="CO3" s="48"/>
+      <c r="CO3" s="48">
+        <v>5666</v>
+      </c>
       <c r="CP3" s="48"/>
       <c r="CQ3" s="48"/>
       <c r="CR3" s="48"/>
@@ -18100,7 +18282,9 @@
       <c r="CN4" s="48">
         <v>5634</v>
       </c>
-      <c r="CO4" s="48"/>
+      <c r="CO4" s="48">
+        <v>5666</v>
+      </c>
       <c r="CP4" s="48"/>
       <c r="CQ4" s="48"/>
       <c r="CR4" s="48"/>
@@ -18382,7 +18566,9 @@
       <c r="CN5" s="48">
         <v>5634</v>
       </c>
-      <c r="CO5" s="48"/>
+      <c r="CO5" s="48">
+        <v>5666</v>
+      </c>
       <c r="CP5" s="48"/>
       <c r="CQ5" s="48"/>
       <c r="CR5" s="48"/>
@@ -18664,7 +18850,9 @@
       <c r="CN6" s="48">
         <v>5634</v>
       </c>
-      <c r="CO6" s="48"/>
+      <c r="CO6" s="48">
+        <v>5666</v>
+      </c>
       <c r="CP6" s="48"/>
       <c r="CQ6" s="48"/>
       <c r="CR6" s="48"/>
@@ -18946,7 +19134,9 @@
       <c r="CN7" s="48">
         <v>4935</v>
       </c>
-      <c r="CO7" s="48"/>
+      <c r="CO7" s="48">
+        <v>4967</v>
+      </c>
       <c r="CP7" s="48"/>
       <c r="CQ7" s="48"/>
       <c r="CR7" s="48"/>
@@ -19228,7 +19418,9 @@
       <c r="CN8" s="48">
         <v>7565</v>
       </c>
-      <c r="CO8" s="48"/>
+      <c r="CO8" s="48">
+        <v>7597</v>
+      </c>
       <c r="CP8" s="48"/>
       <c r="CQ8" s="48"/>
       <c r="CR8" s="48"/>
@@ -19608,7 +19800,9 @@
       <c r="CN10" s="74">
         <v>231</v>
       </c>
-      <c r="CO10" s="48"/>
+      <c r="CO10" s="74">
+        <v>232</v>
+      </c>
       <c r="CP10" s="48"/>
       <c r="CQ10" s="48"/>
       <c r="CR10" s="48"/>
@@ -19890,7 +20084,9 @@
       <c r="CN11" s="74">
         <v>231</v>
       </c>
-      <c r="CO11" s="48"/>
+      <c r="CO11" s="74">
+        <v>232</v>
+      </c>
       <c r="CP11" s="48"/>
       <c r="CQ11" s="48"/>
       <c r="CR11" s="48"/>
@@ -20172,7 +20368,9 @@
       <c r="CN12" s="74">
         <v>231</v>
       </c>
-      <c r="CO12" s="48"/>
+      <c r="CO12" s="74">
+        <v>232</v>
+      </c>
       <c r="CP12" s="48"/>
       <c r="CQ12" s="48"/>
       <c r="CR12" s="48"/>
@@ -20454,7 +20652,9 @@
       <c r="CN13" s="74">
         <v>231</v>
       </c>
-      <c r="CO13" s="48"/>
+      <c r="CO13" s="74">
+        <v>232</v>
+      </c>
       <c r="CP13" s="48"/>
       <c r="CQ13" s="48"/>
       <c r="CR13" s="48"/>
@@ -20736,7 +20936,9 @@
       <c r="CN14" s="74">
         <v>231</v>
       </c>
-      <c r="CO14" s="48"/>
+      <c r="CO14" s="74">
+        <v>232</v>
+      </c>
       <c r="CP14" s="48"/>
       <c r="CQ14" s="48"/>
       <c r="CR14" s="48"/>
@@ -21018,7 +21220,9 @@
       <c r="CN15" s="48">
         <v>166</v>
       </c>
-      <c r="CO15" s="48"/>
+      <c r="CO15" s="48">
+        <v>167</v>
+      </c>
       <c r="CP15" s="48"/>
       <c r="CQ15" s="48"/>
       <c r="CR15" s="48"/>
@@ -21300,7 +21504,9 @@
       <c r="CN16" s="74">
         <v>243</v>
       </c>
-      <c r="CO16" s="48"/>
+      <c r="CO16" s="48">
+        <v>244</v>
+      </c>
       <c r="CP16" s="48"/>
       <c r="CQ16" s="48"/>
       <c r="CR16" s="48"/>
@@ -21680,7 +21886,9 @@
       <c r="CN18" s="48">
         <v>1358</v>
       </c>
-      <c r="CO18" s="48"/>
+      <c r="CO18" s="48">
+        <v>1365</v>
+      </c>
       <c r="CP18" s="48"/>
       <c r="CQ18" s="48"/>
       <c r="CR18" s="48"/>
@@ -21861,7 +22069,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CN20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CO20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -22059,6 +22267,10 @@
       <c r="CN20" s="51">
         <f t="shared" si="1"/>
         <v>43788</v>
+      </c>
+      <c r="CO20" s="51">
+        <f t="shared" si="1"/>
+        <v>44026</v>
       </c>
     </row>
   </sheetData>
@@ -22358,43 +22570,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="861" t="s">
+      <c r="B8" s="870" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="861"/>
+      <c r="B9" s="870"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="861"/>
+      <c r="B10" s="870"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="861"/>
+      <c r="B11" s="870"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="862" t="s">
+      <c r="B12" s="871" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="862"/>
+      <c r="B13" s="871"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="862"/>
+      <c r="B14" s="871"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="863" t="s">
+      <c r="B15" s="872" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="863"/>
+      <c r="B16" s="872"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 1st
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6808C43-41D6-8340-882A-26E45BAA1A0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AFC1FF-35D0-9443-8185-A43AB278AFF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="874">
+  <cellXfs count="883">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3151,6 +3151,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3159,9 +3189,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3482,10 +3509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6469,6 +6496,38 @@
         <v>1345483</v>
       </c>
     </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="15">
+        <v>44075</v>
+      </c>
+      <c r="B94" s="871">
+        <v>606036</v>
+      </c>
+      <c r="C94" s="872">
+        <v>676958</v>
+      </c>
+      <c r="D94" s="873">
+        <v>77129</v>
+      </c>
+      <c r="E94" s="874">
+        <v>65241</v>
+      </c>
+      <c r="F94" s="875">
+        <v>25.364004778594012</v>
+      </c>
+      <c r="G94" s="876">
+        <v>153715</v>
+      </c>
+      <c r="H94" s="877">
+        <v>13174</v>
+      </c>
+      <c r="I94" s="878">
+        <v>18935</v>
+      </c>
+      <c r="J94" s="879">
+        <v>1360123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6476,11 +6535,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N93" sqref="N93"/>
+      <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10078,6 +10137,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="15">
+        <v>44075</v>
+      </c>
+      <c r="B94" s="216">
+        <v>0</v>
+      </c>
+      <c r="C94" s="216">
+        <v>1</v>
+      </c>
+      <c r="D94" s="216">
+        <v>0</v>
+      </c>
+      <c r="E94" s="216">
+        <v>0</v>
+      </c>
+      <c r="F94" s="216">
+        <v>1</v>
+      </c>
+      <c r="G94" s="216">
+        <v>0</v>
+      </c>
+      <c r="H94" s="216">
+        <v>0</v>
+      </c>
+      <c r="I94" s="216">
+        <v>0</v>
+      </c>
+      <c r="J94" s="216">
+        <v>0</v>
+      </c>
+      <c r="K94" s="216">
+        <v>0</v>
+      </c>
+      <c r="L94" s="216">
+        <v>1</v>
+      </c>
+      <c r="M94" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10085,11 +10185,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O93" sqref="O93"/>
+      <selection pane="bottomLeft" activeCell="O94" sqref="O94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14092,7 +14192,7 @@
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A93" s="873">
+      <c r="A93" s="870">
         <v>44074</v>
       </c>
       <c r="B93" s="216">
@@ -14132,6 +14232,50 @@
         <v>0</v>
       </c>
       <c r="N93" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="15">
+        <v>44075</v>
+      </c>
+      <c r="B94" s="216">
+        <v>0</v>
+      </c>
+      <c r="C94" s="216">
+        <v>1</v>
+      </c>
+      <c r="D94" s="216">
+        <v>0</v>
+      </c>
+      <c r="E94" s="216">
+        <v>0</v>
+      </c>
+      <c r="F94" s="216">
+        <v>0</v>
+      </c>
+      <c r="G94" s="216">
+        <v>0</v>
+      </c>
+      <c r="H94" s="216">
+        <v>1</v>
+      </c>
+      <c r="I94" s="216">
+        <v>0</v>
+      </c>
+      <c r="J94" s="216">
+        <v>0</v>
+      </c>
+      <c r="K94" s="216">
+        <v>1</v>
+      </c>
+      <c r="L94" s="216">
+        <v>0</v>
+      </c>
+      <c r="M94" s="216">
+        <v>0</v>
+      </c>
+      <c r="N94" s="216">
         <v>0</v>
       </c>
     </row>
@@ -14142,11 +14286,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
+      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17104,7 +17248,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="873">
+      <c r="A93" s="870">
         <v>44074</v>
       </c>
       <c r="B93" s="216">
@@ -17132,6 +17276,38 @@
         <v>1</v>
       </c>
       <c r="J93" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="15">
+        <v>44075</v>
+      </c>
+      <c r="B94" s="216">
+        <v>0</v>
+      </c>
+      <c r="C94" s="216">
+        <v>0</v>
+      </c>
+      <c r="D94" s="216">
+        <v>0</v>
+      </c>
+      <c r="E94" s="216">
+        <v>0</v>
+      </c>
+      <c r="F94" s="216">
+        <v>2</v>
+      </c>
+      <c r="G94" s="216">
+        <v>1</v>
+      </c>
+      <c r="H94" s="216">
+        <v>1</v>
+      </c>
+      <c r="I94" s="216">
+        <v>1</v>
+      </c>
+      <c r="J94" s="216">
         <v>2</v>
       </c>
     </row>
@@ -17145,7 +17321,7 @@
   <dimension ref="A1:CR20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CQ22" sqref="CQ22"/>
+      <selection activeCell="CI9" sqref="CI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17433,7 +17609,9 @@
       <c r="CO1" s="49">
         <v>44074</v>
       </c>
-      <c r="CP1" s="48"/>
+      <c r="CP1" s="15">
+        <v>44075</v>
+      </c>
       <c r="CQ1" s="48"/>
       <c r="CR1" s="48"/>
     </row>
@@ -17717,7 +17895,9 @@
       <c r="CO2" s="48">
         <v>5862</v>
       </c>
-      <c r="CP2" s="48"/>
+      <c r="CP2" s="48">
+        <v>5894</v>
+      </c>
       <c r="CQ2" s="48"/>
       <c r="CR2" s="48"/>
     </row>
@@ -18001,7 +18181,9 @@
       <c r="CO3" s="48">
         <v>5666</v>
       </c>
-      <c r="CP3" s="48"/>
+      <c r="CP3" s="48">
+        <v>5698</v>
+      </c>
       <c r="CQ3" s="48"/>
       <c r="CR3" s="48"/>
     </row>
@@ -18285,7 +18467,9 @@
       <c r="CO4" s="48">
         <v>5666</v>
       </c>
-      <c r="CP4" s="48"/>
+      <c r="CP4" s="48">
+        <v>5698</v>
+      </c>
       <c r="CQ4" s="48"/>
       <c r="CR4" s="48"/>
     </row>
@@ -18569,7 +18753,9 @@
       <c r="CO5" s="48">
         <v>5666</v>
       </c>
-      <c r="CP5" s="48"/>
+      <c r="CP5" s="48">
+        <v>5698</v>
+      </c>
       <c r="CQ5" s="48"/>
       <c r="CR5" s="48"/>
     </row>
@@ -18853,7 +19039,9 @@
       <c r="CO6" s="48">
         <v>5666</v>
       </c>
-      <c r="CP6" s="48"/>
+      <c r="CP6" s="48">
+        <v>5698</v>
+      </c>
       <c r="CQ6" s="48"/>
       <c r="CR6" s="48"/>
     </row>
@@ -19137,7 +19325,9 @@
       <c r="CO7" s="48">
         <v>4967</v>
       </c>
-      <c r="CP7" s="48"/>
+      <c r="CP7" s="48">
+        <v>4999</v>
+      </c>
       <c r="CQ7" s="48"/>
       <c r="CR7" s="48"/>
     </row>
@@ -19421,7 +19611,9 @@
       <c r="CO8" s="48">
         <v>7597</v>
       </c>
-      <c r="CP8" s="48"/>
+      <c r="CP8" s="48">
+        <v>7629</v>
+      </c>
       <c r="CQ8" s="48"/>
       <c r="CR8" s="48"/>
     </row>
@@ -19803,7 +19995,9 @@
       <c r="CO10" s="74">
         <v>232</v>
       </c>
-      <c r="CP10" s="48"/>
+      <c r="CP10" s="48">
+        <v>233</v>
+      </c>
       <c r="CQ10" s="48"/>
       <c r="CR10" s="48"/>
     </row>
@@ -20087,7 +20281,9 @@
       <c r="CO11" s="74">
         <v>232</v>
       </c>
-      <c r="CP11" s="48"/>
+      <c r="CP11" s="48">
+        <v>233</v>
+      </c>
       <c r="CQ11" s="48"/>
       <c r="CR11" s="48"/>
     </row>
@@ -20371,7 +20567,9 @@
       <c r="CO12" s="74">
         <v>232</v>
       </c>
-      <c r="CP12" s="48"/>
+      <c r="CP12" s="48">
+        <v>233</v>
+      </c>
       <c r="CQ12" s="48"/>
       <c r="CR12" s="48"/>
     </row>
@@ -20655,7 +20853,9 @@
       <c r="CO13" s="74">
         <v>232</v>
       </c>
-      <c r="CP13" s="48"/>
+      <c r="CP13" s="48">
+        <v>233</v>
+      </c>
       <c r="CQ13" s="48"/>
       <c r="CR13" s="48"/>
     </row>
@@ -20939,7 +21139,9 @@
       <c r="CO14" s="74">
         <v>232</v>
       </c>
-      <c r="CP14" s="48"/>
+      <c r="CP14" s="48">
+        <v>233</v>
+      </c>
       <c r="CQ14" s="48"/>
       <c r="CR14" s="48"/>
     </row>
@@ -21223,7 +21425,9 @@
       <c r="CO15" s="48">
         <v>167</v>
       </c>
-      <c r="CP15" s="48"/>
+      <c r="CP15" s="48">
+        <v>168</v>
+      </c>
       <c r="CQ15" s="48"/>
       <c r="CR15" s="48"/>
     </row>
@@ -21507,7 +21711,9 @@
       <c r="CO16" s="48">
         <v>244</v>
       </c>
-      <c r="CP16" s="48"/>
+      <c r="CP16" s="48">
+        <v>245</v>
+      </c>
       <c r="CQ16" s="48"/>
       <c r="CR16" s="48"/>
     </row>
@@ -21889,7 +22095,9 @@
       <c r="CO18" s="48">
         <v>1365</v>
       </c>
-      <c r="CP18" s="48"/>
+      <c r="CP18" s="48">
+        <v>1372</v>
+      </c>
       <c r="CQ18" s="48"/>
       <c r="CR18" s="48"/>
     </row>
@@ -22069,7 +22277,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CO20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CP20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -22271,6 +22479,10 @@
       <c r="CO20" s="51">
         <f t="shared" si="1"/>
         <v>44026</v>
+      </c>
+      <c r="CP20" s="51">
+        <f t="shared" si="1"/>
+        <v>44264</v>
       </c>
     </row>
   </sheetData>
@@ -22570,43 +22782,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="870" t="s">
+      <c r="B8" s="880" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="870"/>
+      <c r="B9" s="880"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="870"/>
+      <c r="B10" s="880"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="870"/>
+      <c r="B11" s="880"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="871" t="s">
+      <c r="B12" s="881" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="871"/>
+      <c r="B13" s="881"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="871"/>
+      <c r="B14" s="881"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="872" t="s">
+      <c r="B15" s="882" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="872"/>
+      <c r="B16" s="882"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 2
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AFC1FF-35D0-9443-8185-A43AB278AFF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94349636-27B3-AF45-AFEC-17DBF09EACA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="10540" yWindow="2160" windowWidth="18260" windowHeight="14720" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="883">
+  <cellXfs count="891">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3151,7 +3151,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3509,10 +3533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6500,32 +6524,64 @@
       <c r="A94" s="15">
         <v>44075</v>
       </c>
-      <c r="B94" s="871">
+      <c r="B94" s="870">
         <v>606036</v>
       </c>
-      <c r="C94" s="872">
+      <c r="C94" s="871">
         <v>676958</v>
       </c>
-      <c r="D94" s="873">
+      <c r="D94" s="872">
         <v>77129</v>
       </c>
-      <c r="E94" s="874">
+      <c r="E94" s="873">
         <v>65241</v>
       </c>
-      <c r="F94" s="875">
+      <c r="F94" s="874">
         <v>25.364004778594012</v>
       </c>
-      <c r="G94" s="876">
+      <c r="G94" s="875">
         <v>153715</v>
       </c>
-      <c r="H94" s="877">
+      <c r="H94" s="876">
         <v>13174</v>
       </c>
-      <c r="I94" s="878">
+      <c r="I94" s="877">
         <v>18935</v>
       </c>
-      <c r="J94" s="879">
+      <c r="J94" s="878">
         <v>1360123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="15">
+        <v>44076</v>
+      </c>
+      <c r="B95" s="879">
+        <v>610957</v>
+      </c>
+      <c r="C95" s="880">
+        <v>683438</v>
+      </c>
+      <c r="D95" s="881">
+        <v>81775</v>
+      </c>
+      <c r="E95" s="882">
+        <v>65816</v>
+      </c>
+      <c r="F95" s="883">
+        <v>25.317330024862635</v>
+      </c>
+      <c r="G95" s="884">
+        <v>154678</v>
+      </c>
+      <c r="H95" s="885">
+        <v>13275</v>
+      </c>
+      <c r="I95" s="886">
+        <v>19031</v>
+      </c>
+      <c r="J95" s="887">
+        <v>1376170</v>
       </c>
     </row>
   </sheetData>
@@ -6535,11 +6591,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10097,7 +10153,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="15">
+      <c r="A93" s="217">
         <v>44074</v>
       </c>
       <c r="B93" s="216">
@@ -10138,7 +10194,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A94" s="15">
+      <c r="A94" s="217">
         <v>44075</v>
       </c>
       <c r="B94" s="216">
@@ -10177,6 +10233,50 @@
       <c r="M94" s="216">
         <v>4</v>
       </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="217">
+        <v>44076</v>
+      </c>
+      <c r="B95" s="216">
+        <v>0</v>
+      </c>
+      <c r="C95" s="216">
+        <v>1</v>
+      </c>
+      <c r="D95" s="216">
+        <v>0</v>
+      </c>
+      <c r="E95" s="216">
+        <v>0</v>
+      </c>
+      <c r="F95" s="216">
+        <v>1</v>
+      </c>
+      <c r="G95" s="216">
+        <v>0</v>
+      </c>
+      <c r="H95" s="216">
+        <v>0</v>
+      </c>
+      <c r="I95" s="216">
+        <v>0</v>
+      </c>
+      <c r="J95" s="216">
+        <v>0</v>
+      </c>
+      <c r="K95" s="216">
+        <v>0</v>
+      </c>
+      <c r="L95" s="216">
+        <v>1</v>
+      </c>
+      <c r="M95" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10185,11 +10285,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O94" sqref="O94"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14192,7 +14292,7 @@
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A93" s="870">
+      <c r="A93" s="217">
         <v>44074</v>
       </c>
       <c r="B93" s="216">
@@ -14236,7 +14336,7 @@
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A94" s="15">
+      <c r="A94" s="217">
         <v>44075</v>
       </c>
       <c r="B94" s="216">
@@ -14278,6 +14378,53 @@
       <c r="N94" s="216">
         <v>0</v>
       </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="217">
+        <v>44076</v>
+      </c>
+      <c r="B95" s="216">
+        <v>0</v>
+      </c>
+      <c r="C95" s="216">
+        <v>1</v>
+      </c>
+      <c r="D95" s="216">
+        <v>0</v>
+      </c>
+      <c r="E95" s="216">
+        <v>0</v>
+      </c>
+      <c r="F95" s="216">
+        <v>0</v>
+      </c>
+      <c r="G95" s="216">
+        <v>0</v>
+      </c>
+      <c r="H95" s="216">
+        <v>1</v>
+      </c>
+      <c r="I95" s="216">
+        <v>0</v>
+      </c>
+      <c r="J95" s="216">
+        <v>0</v>
+      </c>
+      <c r="K95" s="216">
+        <v>1</v>
+      </c>
+      <c r="L95" s="216">
+        <v>0</v>
+      </c>
+      <c r="M95" s="216">
+        <v>0</v>
+      </c>
+      <c r="N95" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="217"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14286,11 +14433,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17248,7 +17395,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="870">
+      <c r="A93" s="495">
         <v>44074</v>
       </c>
       <c r="B93" s="216">
@@ -17280,7 +17427,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="15">
+      <c r="A94" s="495">
         <v>44075</v>
       </c>
       <c r="B94" s="216">
@@ -17310,6 +17457,47 @@
       <c r="J94" s="216">
         <v>2</v>
       </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="495">
+        <v>44076</v>
+      </c>
+      <c r="B95" s="216">
+        <v>0</v>
+      </c>
+      <c r="C95" s="216">
+        <v>0</v>
+      </c>
+      <c r="D95" s="216">
+        <v>0</v>
+      </c>
+      <c r="E95" s="216">
+        <v>0</v>
+      </c>
+      <c r="F95" s="216">
+        <v>2</v>
+      </c>
+      <c r="G95" s="216">
+        <v>1</v>
+      </c>
+      <c r="H95" s="216">
+        <v>1</v>
+      </c>
+      <c r="I95" s="216">
+        <v>1</v>
+      </c>
+      <c r="J95" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="495"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="495"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="495"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17320,8 +17508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CR20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
-      <selection activeCell="CI9" sqref="CI9"/>
+    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="CQ17" sqref="CQ17:CR17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17609,10 +17797,12 @@
       <c r="CO1" s="49">
         <v>44074</v>
       </c>
-      <c r="CP1" s="15">
+      <c r="CP1" s="49">
         <v>44075</v>
       </c>
-      <c r="CQ1" s="48"/>
+      <c r="CQ1" s="49">
+        <v>44076</v>
+      </c>
       <c r="CR1" s="48"/>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.2">
@@ -17898,7 +18088,9 @@
       <c r="CP2" s="48">
         <v>5894</v>
       </c>
-      <c r="CQ2" s="48"/>
+      <c r="CQ2" s="48">
+        <v>5926</v>
+      </c>
       <c r="CR2" s="48"/>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.2">
@@ -18184,7 +18376,9 @@
       <c r="CP3" s="48">
         <v>5698</v>
       </c>
-      <c r="CQ3" s="48"/>
+      <c r="CQ3" s="48">
+        <v>5730</v>
+      </c>
       <c r="CR3" s="48"/>
     </row>
     <row r="4" spans="1:96" x14ac:dyDescent="0.2">
@@ -18470,7 +18664,9 @@
       <c r="CP4" s="48">
         <v>5698</v>
       </c>
-      <c r="CQ4" s="48"/>
+      <c r="CQ4" s="48">
+        <v>5730</v>
+      </c>
       <c r="CR4" s="48"/>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.2">
@@ -18756,7 +18952,9 @@
       <c r="CP5" s="48">
         <v>5698</v>
       </c>
-      <c r="CQ5" s="48"/>
+      <c r="CQ5" s="48">
+        <v>5730</v>
+      </c>
       <c r="CR5" s="48"/>
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.2">
@@ -19042,7 +19240,9 @@
       <c r="CP6" s="48">
         <v>5698</v>
       </c>
-      <c r="CQ6" s="48"/>
+      <c r="CQ6" s="48">
+        <v>5730</v>
+      </c>
       <c r="CR6" s="48"/>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.2">
@@ -19328,7 +19528,9 @@
       <c r="CP7" s="48">
         <v>4999</v>
       </c>
-      <c r="CQ7" s="48"/>
+      <c r="CQ7" s="48">
+        <v>5031</v>
+      </c>
       <c r="CR7" s="48"/>
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.2">
@@ -19614,7 +19816,9 @@
       <c r="CP8" s="48">
         <v>7629</v>
       </c>
-      <c r="CQ8" s="48"/>
+      <c r="CQ8" s="48">
+        <v>7661</v>
+      </c>
       <c r="CR8" s="48"/>
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.2">
@@ -19712,8 +19916,8 @@
       <c r="CN9" s="312"/>
       <c r="CO9" s="312"/>
       <c r="CP9" s="312"/>
-      <c r="CQ9" s="48"/>
-      <c r="CR9" s="48"/>
+      <c r="CQ9" s="312"/>
+      <c r="CR9" s="312"/>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
@@ -19998,7 +20202,9 @@
       <c r="CP10" s="48">
         <v>233</v>
       </c>
-      <c r="CQ10" s="48"/>
+      <c r="CQ10" s="48">
+        <v>234</v>
+      </c>
       <c r="CR10" s="48"/>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.2">
@@ -20284,7 +20490,9 @@
       <c r="CP11" s="48">
         <v>233</v>
       </c>
-      <c r="CQ11" s="48"/>
+      <c r="CQ11" s="48">
+        <v>234</v>
+      </c>
       <c r="CR11" s="48"/>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.2">
@@ -20570,7 +20778,9 @@
       <c r="CP12" s="48">
         <v>233</v>
       </c>
-      <c r="CQ12" s="48"/>
+      <c r="CQ12" s="48">
+        <v>234</v>
+      </c>
       <c r="CR12" s="48"/>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.2">
@@ -20856,7 +21066,9 @@
       <c r="CP13" s="48">
         <v>233</v>
       </c>
-      <c r="CQ13" s="48"/>
+      <c r="CQ13" s="48">
+        <v>234</v>
+      </c>
       <c r="CR13" s="48"/>
     </row>
     <row r="14" spans="1:96" x14ac:dyDescent="0.2">
@@ -21142,7 +21354,9 @@
       <c r="CP14" s="48">
         <v>233</v>
       </c>
-      <c r="CQ14" s="48"/>
+      <c r="CQ14" s="48">
+        <v>234</v>
+      </c>
       <c r="CR14" s="48"/>
     </row>
     <row r="15" spans="1:96" x14ac:dyDescent="0.2">
@@ -21428,7 +21642,9 @@
       <c r="CP15" s="48">
         <v>168</v>
       </c>
-      <c r="CQ15" s="48"/>
+      <c r="CQ15" s="48">
+        <v>169</v>
+      </c>
       <c r="CR15" s="48"/>
     </row>
     <row r="16" spans="1:96" x14ac:dyDescent="0.2">
@@ -21714,7 +21930,9 @@
       <c r="CP16" s="48">
         <v>245</v>
       </c>
-      <c r="CQ16" s="48"/>
+      <c r="CQ16" s="48">
+        <v>246</v>
+      </c>
       <c r="CR16" s="48"/>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.2">
@@ -21813,7 +22031,7 @@
       <c r="CO17" s="312"/>
       <c r="CP17" s="312"/>
       <c r="CQ17" s="312"/>
-      <c r="CR17" s="48"/>
+      <c r="CR17" s="312"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
@@ -22098,7 +22316,9 @@
       <c r="CP18" s="48">
         <v>1372</v>
       </c>
-      <c r="CQ18" s="48"/>
+      <c r="CQ18" s="48">
+        <v>1379</v>
+      </c>
       <c r="CR18" s="48"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.2">
@@ -22277,7 +22497,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CP20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CQ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -22483,6 +22703,10 @@
       <c r="CP20" s="51">
         <f t="shared" si="1"/>
         <v>44264</v>
+      </c>
+      <c r="CQ20" s="51">
+        <f t="shared" si="1"/>
+        <v>44502</v>
       </c>
     </row>
   </sheetData>
@@ -22782,43 +23006,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="880" t="s">
+      <c r="B8" s="888" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="880"/>
+      <c r="B9" s="888"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="880"/>
+      <c r="B10" s="888"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="880"/>
+      <c r="B11" s="888"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="881" t="s">
+      <c r="B12" s="889" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="881"/>
+      <c r="B13" s="889"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="881"/>
+      <c r="B14" s="889"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="882" t="s">
+      <c r="B15" s="890" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="882"/>
+      <c r="B16" s="890"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA September 3rd
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94349636-27B3-AF45-AFEC-17DBF09EACA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAACA463-874B-964B-A90D-92419D36E361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="2160" windowWidth="18260" windowHeight="14720" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="32680" yWindow="4900" windowWidth="18260" windowHeight="14720" activeTab="3" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="891">
+  <cellXfs count="900">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2611,6 +2611,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3533,10 +3560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6584,6 +6611,38 @@
         <v>1376170</v>
       </c>
     </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="15">
+        <v>44077</v>
+      </c>
+      <c r="B96" s="888">
+        <v>616894</v>
+      </c>
+      <c r="C96" s="889">
+        <v>692319</v>
+      </c>
+      <c r="D96" s="890">
+        <v>83820</v>
+      </c>
+      <c r="E96" s="891">
+        <v>66329</v>
+      </c>
+      <c r="F96" s="892">
+        <v>25.249232445120228</v>
+      </c>
+      <c r="G96" s="893">
+        <v>155761</v>
+      </c>
+      <c r="H96" s="894">
+        <v>13349</v>
+      </c>
+      <c r="I96" s="895">
+        <v>19128</v>
+      </c>
+      <c r="J96" s="896">
+        <v>1393033</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6593,9 +6652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A96"/>
+      <selection pane="bottomLeft" activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10276,7 +10335,45 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="217"/>
+      <c r="A96" s="15">
+        <v>44077</v>
+      </c>
+      <c r="B96" s="216">
+        <v>0</v>
+      </c>
+      <c r="C96" s="216">
+        <v>1</v>
+      </c>
+      <c r="D96" s="550">
+        <v>0</v>
+      </c>
+      <c r="E96" s="550">
+        <v>0</v>
+      </c>
+      <c r="F96" s="216">
+        <v>1</v>
+      </c>
+      <c r="G96" s="216">
+        <v>0</v>
+      </c>
+      <c r="H96" s="216">
+        <v>0</v>
+      </c>
+      <c r="I96" s="216">
+        <v>0</v>
+      </c>
+      <c r="J96" s="216">
+        <v>0</v>
+      </c>
+      <c r="K96" s="216">
+        <v>0</v>
+      </c>
+      <c r="L96" s="216">
+        <v>1</v>
+      </c>
+      <c r="M96" s="216">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10287,9 +10384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A96"/>
+      <selection pane="bottomLeft" activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14424,7 +14521,48 @@
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A96" s="217"/>
+      <c r="A96" s="15">
+        <v>44077</v>
+      </c>
+      <c r="B96" s="216">
+        <v>0</v>
+      </c>
+      <c r="C96" s="216">
+        <v>1</v>
+      </c>
+      <c r="D96" s="216">
+        <v>0</v>
+      </c>
+      <c r="E96" s="216">
+        <v>0</v>
+      </c>
+      <c r="F96" s="216">
+        <v>0</v>
+      </c>
+      <c r="G96" s="216">
+        <v>0</v>
+      </c>
+      <c r="H96" s="216">
+        <v>1</v>
+      </c>
+      <c r="I96" s="216">
+        <v>0</v>
+      </c>
+      <c r="J96" s="216">
+        <v>0</v>
+      </c>
+      <c r="K96" s="216">
+        <v>1</v>
+      </c>
+      <c r="L96" s="216">
+        <v>0</v>
+      </c>
+      <c r="M96" s="216">
+        <v>0</v>
+      </c>
+      <c r="N96" s="216">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14435,9 +14573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92:A98"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17491,7 +17629,36 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="495"/>
+      <c r="A96" s="495">
+        <v>44077</v>
+      </c>
+      <c r="B96" s="216">
+        <v>0</v>
+      </c>
+      <c r="C96" s="216">
+        <v>0</v>
+      </c>
+      <c r="D96" s="216">
+        <v>0</v>
+      </c>
+      <c r="E96" s="216">
+        <v>0</v>
+      </c>
+      <c r="F96" s="216">
+        <v>2</v>
+      </c>
+      <c r="G96" s="216">
+        <v>1</v>
+      </c>
+      <c r="H96" s="216">
+        <v>1</v>
+      </c>
+      <c r="I96" s="216">
+        <v>1</v>
+      </c>
+      <c r="J96" s="216">
+        <v>2</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="495"/>
@@ -17506,10 +17673,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:CR20"/>
+  <dimension ref="A1:CS20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="CQ17" sqref="CQ17:CR17"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="CS21" sqref="CS21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17517,7 +17684,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -17803,9 +17970,12 @@
       <c r="CQ1" s="49">
         <v>44076</v>
       </c>
-      <c r="CR1" s="48"/>
-    </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR1" s="49">
+        <v>44077</v>
+      </c>
+      <c r="CS1" s="49"/>
+    </row>
+    <row r="2" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -18091,9 +18261,11 @@
       <c r="CQ2" s="48">
         <v>5926</v>
       </c>
-      <c r="CR2" s="48"/>
-    </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR2" s="48">
+        <v>5958</v>
+      </c>
+    </row>
+    <row r="3" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -18379,9 +18551,11 @@
       <c r="CQ3" s="48">
         <v>5730</v>
       </c>
-      <c r="CR3" s="48"/>
-    </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR3" s="48">
+        <v>5762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -18667,9 +18841,11 @@
       <c r="CQ4" s="48">
         <v>5730</v>
       </c>
-      <c r="CR4" s="48"/>
-    </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR4" s="48">
+        <v>5762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -18955,9 +19131,11 @@
       <c r="CQ5" s="48">
         <v>5730</v>
       </c>
-      <c r="CR5" s="48"/>
-    </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR5" s="48">
+        <v>5762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -19243,9 +19421,11 @@
       <c r="CQ6" s="48">
         <v>5730</v>
       </c>
-      <c r="CR6" s="48"/>
-    </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR6" s="48">
+        <v>5762</v>
+      </c>
+    </row>
+    <row r="7" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -19531,9 +19711,11 @@
       <c r="CQ7" s="48">
         <v>5031</v>
       </c>
-      <c r="CR7" s="48"/>
-    </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR7" s="48">
+        <v>5063</v>
+      </c>
+    </row>
+    <row r="8" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -19819,9 +20001,11 @@
       <c r="CQ8" s="48">
         <v>7661</v>
       </c>
-      <c r="CR8" s="48"/>
-    </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR8" s="48">
+        <v>7693</v>
+      </c>
+    </row>
+    <row r="9" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -19919,7 +20103,7 @@
       <c r="CQ9" s="312"/>
       <c r="CR9" s="312"/>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -20205,9 +20389,11 @@
       <c r="CQ10" s="48">
         <v>234</v>
       </c>
-      <c r="CR10" s="48"/>
-    </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR10" s="48">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -20493,9 +20679,11 @@
       <c r="CQ11" s="48">
         <v>234</v>
       </c>
-      <c r="CR11" s="48"/>
-    </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR11" s="48">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -20781,9 +20969,11 @@
       <c r="CQ12" s="48">
         <v>234</v>
       </c>
-      <c r="CR12" s="48"/>
-    </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR12" s="48">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -21069,9 +21259,11 @@
       <c r="CQ13" s="48">
         <v>234</v>
       </c>
-      <c r="CR13" s="48"/>
-    </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR13" s="48">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -21357,9 +21549,11 @@
       <c r="CQ14" s="48">
         <v>234</v>
       </c>
-      <c r="CR14" s="48"/>
-    </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR14" s="48">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -21645,9 +21839,11 @@
       <c r="CQ15" s="48">
         <v>169</v>
       </c>
-      <c r="CR15" s="48"/>
-    </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="CR15" s="48">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -21933,7 +22129,9 @@
       <c r="CQ16" s="48">
         <v>246</v>
       </c>
-      <c r="CR16" s="48"/>
+      <c r="CR16" s="48">
+        <v>247</v>
+      </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
@@ -22319,7 +22517,9 @@
       <c r="CQ18" s="48">
         <v>1379</v>
       </c>
-      <c r="CR18" s="48"/>
+      <c r="CR18" s="48">
+        <v>1386</v>
+      </c>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -22497,7 +22697,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CQ20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CR20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -22707,6 +22907,10 @@
       <c r="CQ20" s="51">
         <f t="shared" si="1"/>
         <v>44502</v>
+      </c>
+      <c r="CR20" s="51">
+        <f t="shared" si="1"/>
+        <v>44740</v>
       </c>
     </row>
   </sheetData>
@@ -23006,43 +23210,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="888" t="s">
+      <c r="B8" s="897" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="888"/>
+      <c r="B9" s="897"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="888"/>
+      <c r="B10" s="897"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="888"/>
+      <c r="B11" s="897"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="889" t="s">
+      <c r="B12" s="898" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="889"/>
+      <c r="B13" s="898"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="889"/>
+      <c r="B14" s="898"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="890" t="s">
+      <c r="B15" s="899" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="890"/>
+      <c r="B16" s="899"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
County and age-group clean data as of 2020-09-03
Updated bitacora historica and added clean RData for county and state_age_groups
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yadi/Documents/GitHub/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAACA463-874B-964B-A90D-92419D36E361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F9F8DB-D338-8243-8CE3-3B87042DEAF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32680" yWindow="4900" windowWidth="18260" windowHeight="14720" activeTab="3" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -3264,7 +3264,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3562,7 +3562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
@@ -6652,9 +6652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N96" sqref="N96"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L96" sqref="L96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10384,8 +10384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
@@ -14573,9 +14573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22922,8 +22922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22947,7 +22947,9 @@
       <c r="F1" s="38">
         <v>44025</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="38">
+        <v>44077</v>
+      </c>
       <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -22969,6 +22971,9 @@
       <c r="F2">
         <v>158794</v>
       </c>
+      <c r="G2">
+        <v>274625</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
@@ -22989,6 +22994,9 @@
       <c r="F3">
         <v>149677</v>
       </c>
+      <c r="G3">
+        <v>264608</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
@@ -23009,6 +23017,9 @@
       <c r="F4">
         <v>149677</v>
       </c>
+      <c r="G4">
+        <v>264608</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -23029,6 +23040,9 @@
       <c r="F5">
         <v>149677</v>
       </c>
+      <c r="G5">
+        <v>264608</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
@@ -23049,6 +23063,9 @@
       <c r="F6">
         <v>149677</v>
       </c>
+      <c r="G6">
+        <v>264608</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
@@ -23069,6 +23086,9 @@
       <c r="F7">
         <v>86350</v>
       </c>
+      <c r="G7">
+        <v>175075</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
@@ -23089,6 +23109,9 @@
       <c r="F8">
         <v>224128</v>
       </c>
+      <c r="G8">
+        <v>345800</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -23116,6 +23139,10 @@
       <c r="F10">
         <f>SUM(F2:F8)</f>
         <v>1067980</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G2:G8)</f>
+        <v>1853932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 5th,6th and 7th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD9EE45-8F07-8C48-8C7F-41EA6ED26A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF88768-CB3A-DE4C-A2FA-94939CA37DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34860" yWindow="4260" windowWidth="25600" windowHeight="15540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="910">
+  <cellXfs count="937">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3259,6 +3259,90 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3267,9 +3351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3590,10 +3671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6705,6 +6786,102 @@
         <v>1409384</v>
       </c>
     </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="15">
+        <v>44079</v>
+      </c>
+      <c r="B98" s="907">
+        <v>629409</v>
+      </c>
+      <c r="C98" s="908">
+        <v>709182</v>
+      </c>
+      <c r="D98" s="909">
+        <v>86616</v>
+      </c>
+      <c r="E98" s="910">
+        <v>67326</v>
+      </c>
+      <c r="F98" s="911">
+        <v>25.060334377169696</v>
+      </c>
+      <c r="G98" s="912">
+        <v>157732</v>
+      </c>
+      <c r="H98" s="913">
+        <v>13523</v>
+      </c>
+      <c r="I98" s="914">
+        <v>19370</v>
+      </c>
+      <c r="J98" s="915">
+        <v>1425207</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="15">
+        <v>44080</v>
+      </c>
+      <c r="B99" s="916">
+        <v>634023</v>
+      </c>
+      <c r="C99" s="917">
+        <v>715395</v>
+      </c>
+      <c r="D99" s="918">
+        <v>82215</v>
+      </c>
+      <c r="E99" s="919">
+        <v>67558</v>
+      </c>
+      <c r="F99" s="920">
+        <v>25.009029640880538</v>
+      </c>
+      <c r="G99" s="921">
+        <v>158563</v>
+      </c>
+      <c r="H99" s="922">
+        <v>13582</v>
+      </c>
+      <c r="I99" s="923">
+        <v>19437</v>
+      </c>
+      <c r="J99" s="924">
+        <v>1431633</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="15">
+        <v>44081</v>
+      </c>
+      <c r="B100" s="925">
+        <v>637509</v>
+      </c>
+      <c r="C100" s="926">
+        <v>719981</v>
+      </c>
+      <c r="D100" s="927">
+        <v>78213</v>
+      </c>
+      <c r="E100" s="928">
+        <v>67781</v>
+      </c>
+      <c r="F100" s="929">
+        <v>24.982862987032341</v>
+      </c>
+      <c r="G100" s="930">
+        <v>159268</v>
+      </c>
+      <c r="H100" s="931">
+        <v>13651</v>
+      </c>
+      <c r="I100" s="932">
+        <v>19531</v>
+      </c>
+      <c r="J100" s="933">
+        <v>1435703</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6712,11 +6889,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M97" sqref="M97"/>
+      <selection pane="bottomLeft" activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10478,6 +10655,129 @@
         <v>4</v>
       </c>
     </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A98" s="15">
+        <v>44079</v>
+      </c>
+      <c r="B98" s="216">
+        <v>0</v>
+      </c>
+      <c r="C98" s="216">
+        <v>1</v>
+      </c>
+      <c r="D98" s="550">
+        <v>0</v>
+      </c>
+      <c r="E98" s="550">
+        <v>0</v>
+      </c>
+      <c r="F98" s="216">
+        <v>1</v>
+      </c>
+      <c r="G98" s="216">
+        <v>0</v>
+      </c>
+      <c r="H98" s="216">
+        <v>0</v>
+      </c>
+      <c r="I98" s="216">
+        <v>0</v>
+      </c>
+      <c r="J98" s="216">
+        <v>0</v>
+      </c>
+      <c r="K98" s="216">
+        <v>0</v>
+      </c>
+      <c r="L98" s="216">
+        <v>1</v>
+      </c>
+      <c r="M98" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" s="15">
+        <v>44080</v>
+      </c>
+      <c r="B99" s="216">
+        <v>0</v>
+      </c>
+      <c r="C99" s="216">
+        <v>1</v>
+      </c>
+      <c r="D99" s="550">
+        <v>0</v>
+      </c>
+      <c r="E99" s="550">
+        <v>0</v>
+      </c>
+      <c r="F99" s="216">
+        <v>1</v>
+      </c>
+      <c r="G99" s="216">
+        <v>0</v>
+      </c>
+      <c r="H99" s="216">
+        <v>0</v>
+      </c>
+      <c r="I99" s="216">
+        <v>0</v>
+      </c>
+      <c r="J99" s="216">
+        <v>0</v>
+      </c>
+      <c r="K99" s="216">
+        <v>0</v>
+      </c>
+      <c r="L99" s="216">
+        <v>1</v>
+      </c>
+      <c r="M99" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A100" s="15">
+        <v>44081</v>
+      </c>
+      <c r="B100" s="216">
+        <v>0</v>
+      </c>
+      <c r="C100" s="216">
+        <v>1</v>
+      </c>
+      <c r="D100" s="550">
+        <v>0</v>
+      </c>
+      <c r="E100" s="550">
+        <v>0</v>
+      </c>
+      <c r="F100" s="216">
+        <v>1</v>
+      </c>
+      <c r="G100" s="216">
+        <v>0</v>
+      </c>
+      <c r="H100" s="216">
+        <v>0</v>
+      </c>
+      <c r="I100" s="216">
+        <v>0</v>
+      </c>
+      <c r="J100" s="216">
+        <v>0</v>
+      </c>
+      <c r="K100" s="216">
+        <v>0</v>
+      </c>
+      <c r="L100" s="216">
+        <v>1</v>
+      </c>
+      <c r="M100" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10485,11 +10785,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O97" sqref="O97"/>
+      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14668,7 +14968,7 @@
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A97" s="909">
+      <c r="A97" s="906">
         <v>44078</v>
       </c>
       <c r="B97" s="216">
@@ -14708,6 +15008,138 @@
         <v>0</v>
       </c>
       <c r="N97" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="15">
+        <v>44079</v>
+      </c>
+      <c r="B98" s="216">
+        <v>0</v>
+      </c>
+      <c r="C98" s="216">
+        <v>1</v>
+      </c>
+      <c r="D98" s="216">
+        <v>0</v>
+      </c>
+      <c r="E98" s="216">
+        <v>0</v>
+      </c>
+      <c r="F98" s="216">
+        <v>0</v>
+      </c>
+      <c r="G98" s="216">
+        <v>0</v>
+      </c>
+      <c r="H98" s="216">
+        <v>1</v>
+      </c>
+      <c r="I98" s="216">
+        <v>0</v>
+      </c>
+      <c r="J98" s="216">
+        <v>0</v>
+      </c>
+      <c r="K98" s="216">
+        <v>1</v>
+      </c>
+      <c r="L98" s="216">
+        <v>0</v>
+      </c>
+      <c r="M98" s="216">
+        <v>0</v>
+      </c>
+      <c r="N98" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="15">
+        <v>44080</v>
+      </c>
+      <c r="B99" s="216">
+        <v>0</v>
+      </c>
+      <c r="C99" s="216">
+        <v>1</v>
+      </c>
+      <c r="D99" s="216">
+        <v>0</v>
+      </c>
+      <c r="E99" s="216">
+        <v>0</v>
+      </c>
+      <c r="F99" s="216">
+        <v>0</v>
+      </c>
+      <c r="G99" s="216">
+        <v>0</v>
+      </c>
+      <c r="H99" s="216">
+        <v>1</v>
+      </c>
+      <c r="I99" s="216">
+        <v>0</v>
+      </c>
+      <c r="J99" s="216">
+        <v>0</v>
+      </c>
+      <c r="K99" s="216">
+        <v>1</v>
+      </c>
+      <c r="L99" s="216">
+        <v>0</v>
+      </c>
+      <c r="M99" s="216">
+        <v>0</v>
+      </c>
+      <c r="N99" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="15">
+        <v>44081</v>
+      </c>
+      <c r="B100" s="216">
+        <v>0</v>
+      </c>
+      <c r="C100" s="216">
+        <v>1</v>
+      </c>
+      <c r="D100" s="216">
+        <v>0</v>
+      </c>
+      <c r="E100" s="216">
+        <v>0</v>
+      </c>
+      <c r="F100" s="216">
+        <v>0</v>
+      </c>
+      <c r="G100" s="216">
+        <v>0</v>
+      </c>
+      <c r="H100" s="216">
+        <v>1</v>
+      </c>
+      <c r="I100" s="216">
+        <v>0</v>
+      </c>
+      <c r="J100" s="216">
+        <v>0</v>
+      </c>
+      <c r="K100" s="216">
+        <v>1</v>
+      </c>
+      <c r="L100" s="216">
+        <v>0</v>
+      </c>
+      <c r="M100" s="216">
+        <v>0</v>
+      </c>
+      <c r="N100" s="216">
         <v>0</v>
       </c>
     </row>
@@ -14718,11 +15150,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K97" sqref="K97"/>
+      <selection pane="bottomLeft" activeCell="J97" sqref="J97:J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17808,7 +18240,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A97" s="909">
+      <c r="A97" s="906">
         <v>44078</v>
       </c>
       <c r="B97" s="216">
@@ -17840,7 +18272,100 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A98" s="495"/>
+      <c r="A98" s="15">
+        <v>44079</v>
+      </c>
+      <c r="B98" s="216">
+        <v>0</v>
+      </c>
+      <c r="C98" s="216">
+        <v>0</v>
+      </c>
+      <c r="D98" s="216">
+        <v>0</v>
+      </c>
+      <c r="E98" s="216">
+        <v>0</v>
+      </c>
+      <c r="F98" s="216">
+        <v>2</v>
+      </c>
+      <c r="G98" s="216">
+        <v>1</v>
+      </c>
+      <c r="H98" s="216">
+        <v>1</v>
+      </c>
+      <c r="I98" s="216">
+        <v>1</v>
+      </c>
+      <c r="J98" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="15">
+        <v>44080</v>
+      </c>
+      <c r="B99" s="216">
+        <v>0</v>
+      </c>
+      <c r="C99" s="216">
+        <v>0</v>
+      </c>
+      <c r="D99" s="216">
+        <v>0</v>
+      </c>
+      <c r="E99" s="216">
+        <v>0</v>
+      </c>
+      <c r="F99" s="216">
+        <v>2</v>
+      </c>
+      <c r="G99" s="216">
+        <v>1</v>
+      </c>
+      <c r="H99" s="216">
+        <v>1</v>
+      </c>
+      <c r="I99" s="216">
+        <v>1</v>
+      </c>
+      <c r="J99" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="15">
+        <v>44081</v>
+      </c>
+      <c r="B100" s="216">
+        <v>0</v>
+      </c>
+      <c r="C100" s="216">
+        <v>0</v>
+      </c>
+      <c r="D100" s="216">
+        <v>0</v>
+      </c>
+      <c r="E100" s="216">
+        <v>0</v>
+      </c>
+      <c r="F100" s="216">
+        <v>2</v>
+      </c>
+      <c r="G100" s="216">
+        <v>1</v>
+      </c>
+      <c r="H100" s="216">
+        <v>1</v>
+      </c>
+      <c r="I100" s="216">
+        <v>1</v>
+      </c>
+      <c r="J100" s="216">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17849,10 +18374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:CS20"/>
+  <dimension ref="A1:CY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CV16" sqref="CV16"/>
+    <sheetView topLeftCell="CG1" workbookViewId="0">
+      <selection activeCell="CO30" sqref="CO30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17860,7 +18385,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -18152,8 +18677,17 @@
       <c r="CS1" s="49">
         <v>44078</v>
       </c>
-    </row>
-    <row r="2" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT1" s="49">
+        <v>44079</v>
+      </c>
+      <c r="CU1" s="49">
+        <v>44080</v>
+      </c>
+      <c r="CV1" s="49">
+        <v>44081</v>
+      </c>
+    </row>
+    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -18445,8 +18979,17 @@
       <c r="CS2">
         <v>5990</v>
       </c>
-    </row>
-    <row r="3" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT2">
+        <v>6022</v>
+      </c>
+      <c r="CU2">
+        <v>6054</v>
+      </c>
+      <c r="CV2">
+        <v>6086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -18738,8 +19281,17 @@
       <c r="CS3">
         <v>5794</v>
       </c>
-    </row>
-    <row r="4" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT3">
+        <v>5826</v>
+      </c>
+      <c r="CU3">
+        <v>5858</v>
+      </c>
+      <c r="CV3">
+        <v>5890</v>
+      </c>
+    </row>
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -19031,8 +19583,17 @@
       <c r="CS4">
         <v>5794</v>
       </c>
-    </row>
-    <row r="5" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT4">
+        <v>5826</v>
+      </c>
+      <c r="CU4">
+        <v>5858</v>
+      </c>
+      <c r="CV4">
+        <v>5890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -19324,8 +19885,17 @@
       <c r="CS5">
         <v>5794</v>
       </c>
-    </row>
-    <row r="6" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT5">
+        <v>5826</v>
+      </c>
+      <c r="CU5">
+        <v>5858</v>
+      </c>
+      <c r="CV5">
+        <v>5890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -19617,8 +20187,17 @@
       <c r="CS6">
         <v>5794</v>
       </c>
-    </row>
-    <row r="7" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT6">
+        <v>5826</v>
+      </c>
+      <c r="CU6">
+        <v>5858</v>
+      </c>
+      <c r="CV6">
+        <v>5890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -19910,8 +20489,17 @@
       <c r="CS7">
         <v>5095</v>
       </c>
-    </row>
-    <row r="8" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT7">
+        <v>5127</v>
+      </c>
+      <c r="CU7">
+        <v>5159</v>
+      </c>
+      <c r="CV7">
+        <v>5191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -20203,8 +20791,17 @@
       <c r="CS8">
         <v>7725</v>
       </c>
-    </row>
-    <row r="9" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT8">
+        <v>7757</v>
+      </c>
+      <c r="CU8">
+        <v>7789</v>
+      </c>
+      <c r="CV8">
+        <v>7821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -20302,8 +20899,12 @@
       <c r="CQ9" s="312"/>
       <c r="CR9" s="312"/>
       <c r="CS9" s="312"/>
-    </row>
-    <row r="10" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT9" s="312"/>
+      <c r="CU9" s="312"/>
+      <c r="CV9" s="312"/>
+      <c r="CW9" s="312"/>
+    </row>
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -20595,8 +21196,17 @@
       <c r="CS10" s="216">
         <v>236</v>
       </c>
-    </row>
-    <row r="11" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT10" s="216">
+        <v>237</v>
+      </c>
+      <c r="CU10" s="216">
+        <v>238</v>
+      </c>
+      <c r="CV10" s="216">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -20888,8 +21498,17 @@
       <c r="CS11" s="216">
         <v>236</v>
       </c>
-    </row>
-    <row r="12" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT11" s="216">
+        <v>237</v>
+      </c>
+      <c r="CU11" s="216">
+        <v>238</v>
+      </c>
+      <c r="CV11" s="216">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -21181,8 +21800,17 @@
       <c r="CS12" s="216">
         <v>236</v>
       </c>
-    </row>
-    <row r="13" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT12" s="216">
+        <v>237</v>
+      </c>
+      <c r="CU12" s="216">
+        <v>238</v>
+      </c>
+      <c r="CV12" s="216">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -21474,8 +22102,17 @@
       <c r="CS13" s="216">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT13" s="216">
+        <v>237</v>
+      </c>
+      <c r="CU13" s="216">
+        <v>238</v>
+      </c>
+      <c r="CV13" s="216">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -21767,8 +22404,17 @@
       <c r="CS14" s="216">
         <v>236</v>
       </c>
-    </row>
-    <row r="15" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT14" s="216">
+        <v>237</v>
+      </c>
+      <c r="CU14" s="216">
+        <v>238</v>
+      </c>
+      <c r="CV14" s="216">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -22060,8 +22706,17 @@
       <c r="CS15" s="216">
         <v>171</v>
       </c>
-    </row>
-    <row r="16" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT15" s="216">
+        <v>172</v>
+      </c>
+      <c r="CU15" s="216">
+        <v>173</v>
+      </c>
+      <c r="CV15" s="216">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -22353,8 +23008,17 @@
       <c r="CS16" s="216">
         <v>248</v>
       </c>
-    </row>
-    <row r="17" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT16" s="216">
+        <v>249</v>
+      </c>
+      <c r="CU16" s="216">
+        <v>250</v>
+      </c>
+      <c r="CV16" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -22452,8 +23116,14 @@
       <c r="CQ17" s="312"/>
       <c r="CR17" s="312"/>
       <c r="CS17" s="312"/>
-    </row>
-    <row r="18" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT17" s="312"/>
+      <c r="CU17" s="312"/>
+      <c r="CV17" s="312"/>
+      <c r="CW17" s="312"/>
+      <c r="CX17" s="312"/>
+      <c r="CY17" s="312"/>
+    </row>
+    <row r="18" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -22745,15 +23415,24 @@
       <c r="CS18">
         <v>1393</v>
       </c>
-    </row>
-    <row r="19" spans="1:97" x14ac:dyDescent="0.2">
+      <c r="CT18">
+        <v>1400</v>
+      </c>
+      <c r="CU18">
+        <v>1407</v>
+      </c>
+      <c r="CV18">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:97" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -22922,7 +23601,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CS20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CV20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -23140,6 +23819,18 @@
       <c r="CS20" s="51">
         <f t="shared" si="1"/>
         <v>44978</v>
+      </c>
+      <c r="CT20" s="51">
+        <f t="shared" si="1"/>
+        <v>45216</v>
+      </c>
+      <c r="CU20" s="51">
+        <f t="shared" si="1"/>
+        <v>45454</v>
+      </c>
+      <c r="CV20" s="51">
+        <f t="shared" si="1"/>
+        <v>45692</v>
       </c>
     </row>
   </sheetData>
@@ -23466,43 +24157,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="906" t="s">
+      <c r="B8" s="934" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="906"/>
+      <c r="B9" s="934"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="906"/>
+      <c r="B10" s="934"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="906"/>
+      <c r="B11" s="934"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="907" t="s">
+      <c r="B12" s="935" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="907"/>
+      <c r="B13" s="935"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="907"/>
+      <c r="B14" s="935"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="908" t="s">
+      <c r="B15" s="936" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="908"/>
+      <c r="B16" s="936"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 8th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF88768-CB3A-DE4C-A2FA-94939CA37DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD02FB6-C050-254E-B0DB-245F3B036425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30340" yWindow="1000" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="937">
+  <cellXfs count="946">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3260,6 +3260,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3671,10 +3698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6882,6 +6909,38 @@
         <v>1435703</v>
       </c>
     </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="15">
+        <v>44082</v>
+      </c>
+      <c r="B101" s="934">
+        <v>642860</v>
+      </c>
+      <c r="C101" s="935">
+        <v>727817</v>
+      </c>
+      <c r="D101" s="936">
+        <v>79720</v>
+      </c>
+      <c r="E101" s="937">
+        <v>68484</v>
+      </c>
+      <c r="F101" s="938">
+        <v>24.92502255545531</v>
+      </c>
+      <c r="G101" s="939">
+        <v>160233</v>
+      </c>
+      <c r="H101" s="940">
+        <v>13779</v>
+      </c>
+      <c r="I101" s="941">
+        <v>19667</v>
+      </c>
+      <c r="J101" s="942">
+        <v>1450397</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6889,11 +6948,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O96" sqref="O96"/>
+      <selection pane="bottomLeft" activeCell="N101" sqref="N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10778,6 +10837,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A101" s="15">
+        <v>44082</v>
+      </c>
+      <c r="B101" s="216">
+        <v>0</v>
+      </c>
+      <c r="C101" s="216">
+        <v>1</v>
+      </c>
+      <c r="D101" s="216">
+        <v>0</v>
+      </c>
+      <c r="E101" s="216">
+        <v>0</v>
+      </c>
+      <c r="F101" s="216">
+        <v>1</v>
+      </c>
+      <c r="G101" s="216">
+        <v>0</v>
+      </c>
+      <c r="H101" s="216">
+        <v>0</v>
+      </c>
+      <c r="I101" s="216">
+        <v>0</v>
+      </c>
+      <c r="J101" s="216">
+        <v>0</v>
+      </c>
+      <c r="K101" s="216">
+        <v>0</v>
+      </c>
+      <c r="L101" s="216">
+        <v>1</v>
+      </c>
+      <c r="M101" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10785,11 +10885,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
+      <selection pane="bottomLeft" activeCell="O101" sqref="O101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15140,6 +15240,50 @@
         <v>0</v>
       </c>
       <c r="N100" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="15">
+        <v>44082</v>
+      </c>
+      <c r="B101" s="216">
+        <v>0</v>
+      </c>
+      <c r="C101" s="216">
+        <v>1</v>
+      </c>
+      <c r="D101" s="216">
+        <v>0</v>
+      </c>
+      <c r="E101" s="216">
+        <v>0</v>
+      </c>
+      <c r="F101" s="216">
+        <v>0</v>
+      </c>
+      <c r="G101" s="216">
+        <v>0</v>
+      </c>
+      <c r="H101" s="216">
+        <v>1</v>
+      </c>
+      <c r="I101" s="216">
+        <v>0</v>
+      </c>
+      <c r="J101" s="216">
+        <v>0</v>
+      </c>
+      <c r="K101" s="216">
+        <v>1</v>
+      </c>
+      <c r="L101" s="216">
+        <v>0</v>
+      </c>
+      <c r="M101" s="216">
+        <v>0</v>
+      </c>
+      <c r="N101" s="216">
         <v>0</v>
       </c>
     </row>
@@ -15150,11 +15294,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J97" sqref="J97:J100"/>
+      <selection pane="bottomLeft" activeCell="K101" sqref="K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18367,6 +18511,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="15">
+        <v>44082</v>
+      </c>
+      <c r="B101" s="216">
+        <v>0</v>
+      </c>
+      <c r="C101" s="216">
+        <v>0</v>
+      </c>
+      <c r="D101" s="216">
+        <v>0</v>
+      </c>
+      <c r="E101" s="216">
+        <v>0</v>
+      </c>
+      <c r="F101" s="216">
+        <v>2</v>
+      </c>
+      <c r="G101" s="216">
+        <v>1</v>
+      </c>
+      <c r="H101" s="216">
+        <v>1</v>
+      </c>
+      <c r="I101" s="216">
+        <v>1</v>
+      </c>
+      <c r="J101" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18376,8 +18552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CY20"/>
   <sheetViews>
-    <sheetView topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CO30" sqref="CO30"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
+      <selection activeCell="CV24" sqref="CV24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18686,6 +18862,9 @@
       <c r="CV1" s="49">
         <v>44081</v>
       </c>
+      <c r="CW1" s="49">
+        <v>44082</v>
+      </c>
     </row>
     <row r="2" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -18988,6 +19167,9 @@
       <c r="CV2">
         <v>6086</v>
       </c>
+      <c r="CW2">
+        <v>6118</v>
+      </c>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -19290,6 +19472,9 @@
       <c r="CV3">
         <v>5890</v>
       </c>
+      <c r="CW3">
+        <v>5922</v>
+      </c>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -19592,6 +19777,9 @@
       <c r="CV4">
         <v>5890</v>
       </c>
+      <c r="CW4">
+        <v>5922</v>
+      </c>
     </row>
     <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -19894,6 +20082,9 @@
       <c r="CV5">
         <v>5890</v>
       </c>
+      <c r="CW5">
+        <v>5922</v>
+      </c>
     </row>
     <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -20196,6 +20387,9 @@
       <c r="CV6">
         <v>5890</v>
       </c>
+      <c r="CW6">
+        <v>5922</v>
+      </c>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -20498,6 +20692,9 @@
       <c r="CV7">
         <v>5191</v>
       </c>
+      <c r="CW7">
+        <v>5223</v>
+      </c>
     </row>
     <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -20799,6 +20996,9 @@
       </c>
       <c r="CV8">
         <v>7821</v>
+      </c>
+      <c r="CW8">
+        <v>7853</v>
       </c>
     </row>
     <row r="9" spans="1:101" x14ac:dyDescent="0.2">
@@ -21205,6 +21405,9 @@
       <c r="CV10" s="216">
         <v>239</v>
       </c>
+      <c r="CW10" s="216">
+        <v>240</v>
+      </c>
     </row>
     <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -21507,6 +21710,9 @@
       <c r="CV11" s="216">
         <v>239</v>
       </c>
+      <c r="CW11" s="216">
+        <v>240</v>
+      </c>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -21809,6 +22015,9 @@
       <c r="CV12" s="216">
         <v>239</v>
       </c>
+      <c r="CW12" s="216">
+        <v>240</v>
+      </c>
     </row>
     <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -22111,6 +22320,9 @@
       <c r="CV13" s="216">
         <v>239</v>
       </c>
+      <c r="CW13" s="216">
+        <v>240</v>
+      </c>
     </row>
     <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -22413,6 +22625,9 @@
       <c r="CV14" s="216">
         <v>239</v>
       </c>
+      <c r="CW14" s="216">
+        <v>240</v>
+      </c>
     </row>
     <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -22715,6 +22930,9 @@
       <c r="CV15" s="216">
         <v>174</v>
       </c>
+      <c r="CW15" s="216">
+        <v>175</v>
+      </c>
     </row>
     <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -23016,6 +23234,9 @@
       </c>
       <c r="CV16" s="216">
         <v>251</v>
+      </c>
+      <c r="CW16" s="216">
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:103" x14ac:dyDescent="0.2">
@@ -23424,6 +23645,9 @@
       <c r="CV18">
         <v>1414</v>
       </c>
+      <c r="CW18" s="216">
+        <v>1421</v>
+      </c>
     </row>
     <row r="19" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -23601,7 +23825,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CV20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CW20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -23831,6 +24055,10 @@
       <c r="CV20" s="51">
         <f t="shared" si="1"/>
         <v>45692</v>
+      </c>
+      <c r="CW20" s="51">
+        <f t="shared" si="1"/>
+        <v>45930</v>
       </c>
     </row>
   </sheetData>
@@ -24157,43 +24385,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="934" t="s">
+      <c r="B8" s="943" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="934"/>
+      <c r="B9" s="943"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="934"/>
+      <c r="B10" s="943"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="934"/>
+      <c r="B11" s="943"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="935" t="s">
+      <c r="B12" s="944" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="935"/>
+      <c r="B13" s="944"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="935"/>
+      <c r="B14" s="944"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="936" t="s">
+      <c r="B15" s="945" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="936"/>
+      <c r="B16" s="945"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 9th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD02FB6-C050-254E-B0DB-245F3B036425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E482DA-DBA0-AF4B-A6BE-E97E43B4D4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30340" yWindow="1000" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30340" yWindow="1000" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="946">
+  <cellXfs count="955">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3260,6 +3260,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3698,10 +3725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6941,6 +6968,38 @@
         <v>1450397</v>
       </c>
     </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="15">
+        <v>44083</v>
+      </c>
+      <c r="B102" s="943">
+        <v>647507</v>
+      </c>
+      <c r="C102" s="944">
+        <v>734649</v>
+      </c>
+      <c r="D102" s="945">
+        <v>83537</v>
+      </c>
+      <c r="E102" s="946">
+        <v>69095</v>
+      </c>
+      <c r="F102" s="947">
+        <v>24.875406752359432</v>
+      </c>
+      <c r="G102" s="948">
+        <v>161070</v>
+      </c>
+      <c r="H102" s="949">
+        <v>13878</v>
+      </c>
+      <c r="I102" s="950">
+        <v>29570</v>
+      </c>
+      <c r="J102" s="951">
+        <v>1465693</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6948,11 +7007,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N101" sqref="N101"/>
+      <selection pane="bottomLeft" activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10878,6 +10937,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A102" s="15">
+        <v>44083</v>
+      </c>
+      <c r="B102" s="216">
+        <v>0</v>
+      </c>
+      <c r="C102" s="216">
+        <v>1</v>
+      </c>
+      <c r="D102" s="216">
+        <v>0</v>
+      </c>
+      <c r="E102" s="216">
+        <v>0</v>
+      </c>
+      <c r="F102" s="216">
+        <v>1</v>
+      </c>
+      <c r="G102" s="216">
+        <v>0</v>
+      </c>
+      <c r="H102" s="216">
+        <v>0</v>
+      </c>
+      <c r="I102" s="216">
+        <v>0</v>
+      </c>
+      <c r="J102" s="216">
+        <v>0</v>
+      </c>
+      <c r="K102" s="216">
+        <v>0</v>
+      </c>
+      <c r="L102" s="216">
+        <v>1</v>
+      </c>
+      <c r="M102" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10885,11 +10985,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O101" sqref="O101"/>
+      <selection pane="bottomLeft" activeCell="M108" sqref="M108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15284,6 +15384,50 @@
         <v>0</v>
       </c>
       <c r="N101" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="15">
+        <v>44083</v>
+      </c>
+      <c r="B102" s="216">
+        <v>0</v>
+      </c>
+      <c r="C102" s="216">
+        <v>1</v>
+      </c>
+      <c r="D102" s="216">
+        <v>0</v>
+      </c>
+      <c r="E102" s="216">
+        <v>0</v>
+      </c>
+      <c r="F102" s="216">
+        <v>0</v>
+      </c>
+      <c r="G102" s="216">
+        <v>0</v>
+      </c>
+      <c r="H102" s="216">
+        <v>1</v>
+      </c>
+      <c r="I102" s="216">
+        <v>0</v>
+      </c>
+      <c r="J102" s="216">
+        <v>0</v>
+      </c>
+      <c r="K102" s="216">
+        <v>1</v>
+      </c>
+      <c r="L102" s="216">
+        <v>0</v>
+      </c>
+      <c r="M102" s="216">
+        <v>0</v>
+      </c>
+      <c r="N102" s="216">
         <v>0</v>
       </c>
     </row>
@@ -15294,11 +15438,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K101" sqref="K101"/>
+      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18543,6 +18687,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="15">
+        <v>44083</v>
+      </c>
+      <c r="B102" s="216">
+        <v>0</v>
+      </c>
+      <c r="C102" s="216">
+        <v>0</v>
+      </c>
+      <c r="D102" s="216">
+        <v>0</v>
+      </c>
+      <c r="E102" s="216">
+        <v>0</v>
+      </c>
+      <c r="F102" s="216">
+        <v>2</v>
+      </c>
+      <c r="G102" s="216">
+        <v>1</v>
+      </c>
+      <c r="H102" s="216">
+        <v>1</v>
+      </c>
+      <c r="I102" s="216">
+        <v>1</v>
+      </c>
+      <c r="J102" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18552,8 +18728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CV24" sqref="CV24"/>
+    <sheetView topLeftCell="CG1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="CZ15" sqref="CZ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18561,7 +18737,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -18865,8 +19041,11 @@
       <c r="CW1" s="49">
         <v>44082</v>
       </c>
-    </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX1" s="49">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="2" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -19170,8 +19349,11 @@
       <c r="CW2">
         <v>6118</v>
       </c>
-    </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX2">
+        <v>6150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -19475,8 +19657,11 @@
       <c r="CW3">
         <v>5922</v>
       </c>
-    </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX3">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -19780,8 +19965,11 @@
       <c r="CW4">
         <v>5922</v>
       </c>
-    </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX4">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -20085,8 +20273,11 @@
       <c r="CW5">
         <v>5922</v>
       </c>
-    </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX5">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="6" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -20390,8 +20581,11 @@
       <c r="CW6">
         <v>5922</v>
       </c>
-    </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX6">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -20695,8 +20889,11 @@
       <c r="CW7">
         <v>5223</v>
       </c>
-    </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX7">
+        <v>5255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -21000,8 +21197,11 @@
       <c r="CW8">
         <v>7853</v>
       </c>
-    </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX8">
+        <v>7885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -21104,7 +21304,7 @@
       <c r="CV9" s="312"/>
       <c r="CW9" s="312"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -21408,8 +21608,11 @@
       <c r="CW10" s="216">
         <v>240</v>
       </c>
-    </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX10" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -21713,8 +21916,11 @@
       <c r="CW11" s="216">
         <v>240</v>
       </c>
-    </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX11" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -22018,8 +22224,11 @@
       <c r="CW12" s="216">
         <v>240</v>
       </c>
-    </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX12" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -22323,8 +22532,11 @@
       <c r="CW13" s="216">
         <v>240</v>
       </c>
-    </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX13" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -22628,8 +22840,11 @@
       <c r="CW14" s="216">
         <v>240</v>
       </c>
-    </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX14" s="216">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -22933,8 +23148,11 @@
       <c r="CW15" s="216">
         <v>175</v>
       </c>
-    </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="CX15" s="216">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:102" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -23237,6 +23455,9 @@
       </c>
       <c r="CW16" s="216">
         <v>252</v>
+      </c>
+      <c r="CX16" s="216">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:103" x14ac:dyDescent="0.2">
@@ -23648,6 +23869,9 @@
       <c r="CW18" s="216">
         <v>1421</v>
       </c>
+      <c r="CX18">
+        <v>1428</v>
+      </c>
     </row>
     <row r="19" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -23825,7 +24049,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CW20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CX20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -24059,6 +24283,10 @@
       <c r="CW20" s="51">
         <f t="shared" si="1"/>
         <v>45930</v>
+      </c>
+      <c r="CX20" s="51">
+        <f t="shared" si="1"/>
+        <v>46168</v>
       </c>
     </row>
   </sheetData>
@@ -24385,43 +24613,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="943" t="s">
+      <c r="B8" s="952" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="943"/>
+      <c r="B9" s="952"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="943"/>
+      <c r="B10" s="952"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="943"/>
+      <c r="B11" s="952"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="944" t="s">
+      <c r="B12" s="953" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="944"/>
+      <c r="B13" s="953"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="944"/>
+      <c r="B14" s="953"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="945" t="s">
+      <c r="B15" s="954" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="945"/>
+      <c r="B16" s="954"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 10th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E482DA-DBA0-AF4B-A6BE-E97E43B4D4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B6C81C-133E-FD4D-82C1-3AD9E55C4C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30340" yWindow="1000" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="955">
+  <cellXfs count="964">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3260,6 +3260,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3725,10 +3752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7000,6 +7027,38 @@
         <v>1465693</v>
       </c>
     </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="15">
+        <v>44084</v>
+      </c>
+      <c r="B103" s="952">
+        <v>652364</v>
+      </c>
+      <c r="C103" s="953">
+        <v>742268</v>
+      </c>
+      <c r="D103" s="954">
+        <v>86270</v>
+      </c>
+      <c r="E103" s="955">
+        <v>69649</v>
+      </c>
+      <c r="F103" s="956">
+        <v>24.810535222667099</v>
+      </c>
+      <c r="G103" s="957">
+        <v>161855</v>
+      </c>
+      <c r="H103" s="958">
+        <v>13942</v>
+      </c>
+      <c r="I103" s="959">
+        <v>29650</v>
+      </c>
+      <c r="J103" s="960">
+        <v>1480902</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7007,11 +7066,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M102" sqref="M102"/>
+      <selection pane="bottomLeft" activeCell="N103" sqref="N103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10978,6 +11037,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A103" s="15">
+        <v>44084</v>
+      </c>
+      <c r="B103" s="216">
+        <v>0</v>
+      </c>
+      <c r="C103" s="216">
+        <v>1</v>
+      </c>
+      <c r="D103" s="216">
+        <v>0</v>
+      </c>
+      <c r="E103" s="216">
+        <v>0</v>
+      </c>
+      <c r="F103" s="216">
+        <v>1</v>
+      </c>
+      <c r="G103" s="216">
+        <v>0</v>
+      </c>
+      <c r="H103" s="216">
+        <v>0</v>
+      </c>
+      <c r="I103" s="216">
+        <v>0</v>
+      </c>
+      <c r="J103" s="216">
+        <v>0</v>
+      </c>
+      <c r="K103" s="216">
+        <v>0</v>
+      </c>
+      <c r="L103" s="216">
+        <v>1</v>
+      </c>
+      <c r="M103" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10985,11 +11085,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M108" sqref="M108"/>
+      <selection pane="bottomLeft" activeCell="O103" sqref="O103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15428,6 +15528,50 @@
         <v>0</v>
       </c>
       <c r="N102" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="15">
+        <v>44084</v>
+      </c>
+      <c r="B103" s="216">
+        <v>0</v>
+      </c>
+      <c r="C103" s="216">
+        <v>1</v>
+      </c>
+      <c r="D103" s="216">
+        <v>0</v>
+      </c>
+      <c r="E103" s="216">
+        <v>0</v>
+      </c>
+      <c r="F103" s="216">
+        <v>0</v>
+      </c>
+      <c r="G103" s="216">
+        <v>0</v>
+      </c>
+      <c r="H103" s="216">
+        <v>1</v>
+      </c>
+      <c r="I103" s="216">
+        <v>0</v>
+      </c>
+      <c r="J103" s="216">
+        <v>0</v>
+      </c>
+      <c r="K103" s="216">
+        <v>1</v>
+      </c>
+      <c r="L103" s="216">
+        <v>0</v>
+      </c>
+      <c r="M103" s="216">
+        <v>0</v>
+      </c>
+      <c r="N103" s="216">
         <v>0</v>
       </c>
     </row>
@@ -15438,11 +15582,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
+      <selection pane="bottomLeft" activeCell="K103" sqref="K103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18719,6 +18863,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="15">
+        <v>44084</v>
+      </c>
+      <c r="B103" s="216">
+        <v>0</v>
+      </c>
+      <c r="C103" s="216">
+        <v>0</v>
+      </c>
+      <c r="D103" s="216">
+        <v>0</v>
+      </c>
+      <c r="E103" s="216">
+        <v>0</v>
+      </c>
+      <c r="F103" s="216">
+        <v>2</v>
+      </c>
+      <c r="G103" s="216">
+        <v>1</v>
+      </c>
+      <c r="H103" s="216">
+        <v>1</v>
+      </c>
+      <c r="I103" s="216">
+        <v>1</v>
+      </c>
+      <c r="J103" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18728,8 +18904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:CY20"/>
   <sheetViews>
-    <sheetView topLeftCell="CG1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="CZ15" sqref="CZ15"/>
+    <sheetView topLeftCell="CE1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="CX17" sqref="CX17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18737,7 +18913,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -19044,8 +19220,11 @@
       <c r="CX1" s="49">
         <v>44083</v>
       </c>
-    </row>
-    <row r="2" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY1" s="49">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -19352,8 +19531,11 @@
       <c r="CX2">
         <v>6150</v>
       </c>
-    </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY2">
+        <v>6182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -19660,8 +19842,11 @@
       <c r="CX3">
         <v>5954</v>
       </c>
-    </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY3">
+        <v>5986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -19968,8 +20153,11 @@
       <c r="CX4">
         <v>5954</v>
       </c>
-    </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY4">
+        <v>5986</v>
+      </c>
+    </row>
+    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -20276,8 +20464,11 @@
       <c r="CX5">
         <v>5954</v>
       </c>
-    </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY5">
+        <v>5986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -20584,8 +20775,11 @@
       <c r="CX6">
         <v>5954</v>
       </c>
-    </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY6">
+        <v>5986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -20892,8 +21086,11 @@
       <c r="CX7">
         <v>5255</v>
       </c>
-    </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY7">
+        <v>5287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -21200,8 +21397,11 @@
       <c r="CX8">
         <v>7885</v>
       </c>
-    </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY8">
+        <v>7917</v>
+      </c>
+    </row>
+    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -21304,7 +21504,7 @@
       <c r="CV9" s="312"/>
       <c r="CW9" s="312"/>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -21611,8 +21811,11 @@
       <c r="CX10" s="216">
         <v>241</v>
       </c>
-    </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY10" s="216">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -21919,8 +22122,11 @@
       <c r="CX11" s="216">
         <v>241</v>
       </c>
-    </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY11" s="216">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -22227,8 +22433,11 @@
       <c r="CX12" s="216">
         <v>241</v>
       </c>
-    </row>
-    <row r="13" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY12" s="216">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -22535,8 +22744,11 @@
       <c r="CX13" s="216">
         <v>241</v>
       </c>
-    </row>
-    <row r="14" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY13" s="216">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -22843,8 +23055,11 @@
       <c r="CX14" s="216">
         <v>241</v>
       </c>
-    </row>
-    <row r="15" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY14" s="216">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -23151,8 +23366,11 @@
       <c r="CX15" s="216">
         <v>176</v>
       </c>
-    </row>
-    <row r="16" spans="1:102" x14ac:dyDescent="0.2">
+      <c r="CY15" s="216">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -23458,6 +23676,9 @@
       </c>
       <c r="CX16" s="216">
         <v>253</v>
+      </c>
+      <c r="CY16" s="216">
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:103" x14ac:dyDescent="0.2">
@@ -23872,6 +24093,9 @@
       <c r="CX18">
         <v>1428</v>
       </c>
+      <c r="CY18">
+        <v>1435</v>
+      </c>
     </row>
     <row r="19" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -24049,7 +24273,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CX20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:CY20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -24287,6 +24511,10 @@
       <c r="CX20" s="51">
         <f t="shared" si="1"/>
         <v>46168</v>
+      </c>
+      <c r="CY20" s="51">
+        <f t="shared" si="1"/>
+        <v>46406</v>
       </c>
     </row>
   </sheetData>
@@ -24298,8 +24526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24531,7 +24759,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24613,43 +24841,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="952" t="s">
+      <c r="B8" s="961" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="952"/>
+      <c r="B9" s="961"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="952"/>
+      <c r="B10" s="961"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="952"/>
+      <c r="B11" s="961"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="953" t="s">
+      <c r="B12" s="962" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="953"/>
+      <c r="B13" s="962"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="953"/>
+      <c r="B14" s="962"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="954" t="s">
+      <c r="B15" s="963" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="954"/>
+      <c r="B16" s="963"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean data from SSA for September 11th-13th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B6C81C-133E-FD4D-82C1-3AD9E55C4C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3C5565-9570-464F-AFB2-20D726954B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="5" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="32380" yWindow="3360" windowWidth="28800" windowHeight="16420" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -581,6 +581,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -600,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="964">
+  <cellXfs count="992">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3424,6 +3433,87 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3433,6 +3523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3752,10 +3843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7059,6 +7150,102 @@
         <v>1480902</v>
       </c>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="15">
+        <v>44085</v>
+      </c>
+      <c r="B104" s="961">
+        <v>658299</v>
+      </c>
+      <c r="C104" s="962">
+        <v>750813</v>
+      </c>
+      <c r="D104" s="963">
+        <v>87210</v>
+      </c>
+      <c r="E104" s="964">
+        <v>70183</v>
+      </c>
+      <c r="F104" s="965">
+        <v>24.73070747487084</v>
+      </c>
+      <c r="G104" s="966">
+        <v>162802</v>
+      </c>
+      <c r="H104" s="967">
+        <v>14023</v>
+      </c>
+      <c r="I104" s="968">
+        <v>29760</v>
+      </c>
+      <c r="J104" s="969">
+        <v>1496322</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" s="15">
+        <v>44086</v>
+      </c>
+      <c r="B105" s="970">
+        <v>663973</v>
+      </c>
+      <c r="C105" s="971">
+        <v>759188</v>
+      </c>
+      <c r="D105" s="972">
+        <v>87150</v>
+      </c>
+      <c r="E105" s="973">
+        <v>70604</v>
+      </c>
+      <c r="F105" s="974">
+        <v>24.666665662609773</v>
+      </c>
+      <c r="G105" s="975">
+        <v>163780</v>
+      </c>
+      <c r="H105" s="976">
+        <v>14115</v>
+      </c>
+      <c r="I105" s="977">
+        <v>29850</v>
+      </c>
+      <c r="J105" s="978">
+        <v>1510311</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="15">
+        <v>44087</v>
+      </c>
+      <c r="B106" s="979">
+        <v>668381</v>
+      </c>
+      <c r="C106" s="980">
+        <v>765337</v>
+      </c>
+      <c r="D106" s="981">
+        <v>82870</v>
+      </c>
+      <c r="E106" s="982">
+        <v>70821</v>
+      </c>
+      <c r="F106" s="983">
+        <v>24.594205999272869</v>
+      </c>
+      <c r="G106" s="984">
+        <v>164383</v>
+      </c>
+      <c r="H106" s="985">
+        <v>14166</v>
+      </c>
+      <c r="I106" s="986">
+        <v>29902</v>
+      </c>
+      <c r="J106" s="987">
+        <v>1516588</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7066,11 +7253,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N103" sqref="N103"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11078,6 +11265,129 @@
         <v>4</v>
       </c>
     </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A104" s="15">
+        <v>44085</v>
+      </c>
+      <c r="B104" s="216">
+        <v>0</v>
+      </c>
+      <c r="C104" s="216">
+        <v>1</v>
+      </c>
+      <c r="D104" s="216">
+        <v>0</v>
+      </c>
+      <c r="E104" s="216">
+        <v>0</v>
+      </c>
+      <c r="F104" s="216">
+        <v>1</v>
+      </c>
+      <c r="G104" s="216">
+        <v>0</v>
+      </c>
+      <c r="H104" s="216">
+        <v>0</v>
+      </c>
+      <c r="I104" s="216">
+        <v>0</v>
+      </c>
+      <c r="J104" s="216">
+        <v>0</v>
+      </c>
+      <c r="K104" s="216">
+        <v>0</v>
+      </c>
+      <c r="L104" s="216">
+        <v>1</v>
+      </c>
+      <c r="M104" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A105" s="15">
+        <v>44086</v>
+      </c>
+      <c r="B105" s="216">
+        <v>0</v>
+      </c>
+      <c r="C105" s="216">
+        <v>1</v>
+      </c>
+      <c r="D105" s="216">
+        <v>0</v>
+      </c>
+      <c r="E105" s="216">
+        <v>0</v>
+      </c>
+      <c r="F105" s="216">
+        <v>1</v>
+      </c>
+      <c r="G105" s="216">
+        <v>0</v>
+      </c>
+      <c r="H105" s="216">
+        <v>0</v>
+      </c>
+      <c r="I105" s="216">
+        <v>0</v>
+      </c>
+      <c r="J105" s="216">
+        <v>0</v>
+      </c>
+      <c r="K105" s="216">
+        <v>0</v>
+      </c>
+      <c r="L105" s="216">
+        <v>1</v>
+      </c>
+      <c r="M105" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A106" s="15">
+        <v>44087</v>
+      </c>
+      <c r="B106" s="216">
+        <v>0</v>
+      </c>
+      <c r="C106" s="216">
+        <v>1</v>
+      </c>
+      <c r="D106" s="216">
+        <v>0</v>
+      </c>
+      <c r="E106" s="216">
+        <v>0</v>
+      </c>
+      <c r="F106" s="216">
+        <v>1</v>
+      </c>
+      <c r="G106" s="216">
+        <v>0</v>
+      </c>
+      <c r="H106" s="216">
+        <v>0</v>
+      </c>
+      <c r="I106" s="216">
+        <v>0</v>
+      </c>
+      <c r="J106" s="216">
+        <v>0</v>
+      </c>
+      <c r="K106" s="216">
+        <v>0</v>
+      </c>
+      <c r="L106" s="216">
+        <v>1</v>
+      </c>
+      <c r="M106" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11085,11 +11395,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O103"/>
+  <dimension ref="A1:O106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O103" sqref="O103"/>
+      <selection pane="bottomLeft" activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15572,6 +15882,138 @@
         <v>0</v>
       </c>
       <c r="N103" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" s="15">
+        <v>44085</v>
+      </c>
+      <c r="B104" s="216">
+        <v>0</v>
+      </c>
+      <c r="C104" s="216">
+        <v>1</v>
+      </c>
+      <c r="D104" s="216">
+        <v>0</v>
+      </c>
+      <c r="E104" s="216">
+        <v>0</v>
+      </c>
+      <c r="F104" s="216">
+        <v>0</v>
+      </c>
+      <c r="G104" s="216">
+        <v>0</v>
+      </c>
+      <c r="H104" s="216">
+        <v>1</v>
+      </c>
+      <c r="I104" s="216">
+        <v>0</v>
+      </c>
+      <c r="J104" s="216">
+        <v>0</v>
+      </c>
+      <c r="K104" s="216">
+        <v>1</v>
+      </c>
+      <c r="L104" s="216">
+        <v>0</v>
+      </c>
+      <c r="M104" s="216">
+        <v>0</v>
+      </c>
+      <c r="N104" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" s="15">
+        <v>44086</v>
+      </c>
+      <c r="B105" s="216">
+        <v>0</v>
+      </c>
+      <c r="C105" s="216">
+        <v>1</v>
+      </c>
+      <c r="D105" s="216">
+        <v>0</v>
+      </c>
+      <c r="E105" s="216">
+        <v>0</v>
+      </c>
+      <c r="F105" s="216">
+        <v>0</v>
+      </c>
+      <c r="G105" s="216">
+        <v>0</v>
+      </c>
+      <c r="H105" s="216">
+        <v>1</v>
+      </c>
+      <c r="I105" s="216">
+        <v>0</v>
+      </c>
+      <c r="J105" s="216">
+        <v>0</v>
+      </c>
+      <c r="K105" s="216">
+        <v>1</v>
+      </c>
+      <c r="L105" s="216">
+        <v>0</v>
+      </c>
+      <c r="M105" s="216">
+        <v>0</v>
+      </c>
+      <c r="N105" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" s="15">
+        <v>44087</v>
+      </c>
+      <c r="B106" s="216">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106" s="216">
+        <v>0</v>
+      </c>
+      <c r="E106" s="991">
+        <v>0</v>
+      </c>
+      <c r="F106" s="216">
+        <v>0</v>
+      </c>
+      <c r="G106" s="216">
+        <v>0</v>
+      </c>
+      <c r="H106" s="216">
+        <v>1</v>
+      </c>
+      <c r="I106" s="216">
+        <v>0</v>
+      </c>
+      <c r="J106" s="216">
+        <v>0</v>
+      </c>
+      <c r="K106" s="216">
+        <v>1</v>
+      </c>
+      <c r="L106" s="216">
+        <v>0</v>
+      </c>
+      <c r="M106" s="216">
+        <v>0</v>
+      </c>
+      <c r="N106" s="216">
         <v>0</v>
       </c>
     </row>
@@ -15582,11 +16024,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K103" sqref="K103"/>
+      <selection pane="bottomLeft" activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18895,6 +19337,102 @@
         <v>2</v>
       </c>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="15">
+        <v>44085</v>
+      </c>
+      <c r="B104" s="216">
+        <v>0</v>
+      </c>
+      <c r="C104" s="216">
+        <v>0</v>
+      </c>
+      <c r="D104" s="216">
+        <v>0</v>
+      </c>
+      <c r="E104" s="216">
+        <v>0</v>
+      </c>
+      <c r="F104" s="216">
+        <v>2</v>
+      </c>
+      <c r="G104" s="216">
+        <v>1</v>
+      </c>
+      <c r="H104" s="216">
+        <v>1</v>
+      </c>
+      <c r="I104" s="216">
+        <v>1</v>
+      </c>
+      <c r="J104" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" s="15">
+        <v>44086</v>
+      </c>
+      <c r="B105" s="216">
+        <v>0</v>
+      </c>
+      <c r="C105" s="216">
+        <v>0</v>
+      </c>
+      <c r="D105" s="216">
+        <v>0</v>
+      </c>
+      <c r="E105" s="216">
+        <v>0</v>
+      </c>
+      <c r="F105" s="216">
+        <v>2</v>
+      </c>
+      <c r="G105" s="216">
+        <v>1</v>
+      </c>
+      <c r="H105" s="216">
+        <v>1</v>
+      </c>
+      <c r="I105" s="216">
+        <v>1</v>
+      </c>
+      <c r="J105" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="15">
+        <v>44087</v>
+      </c>
+      <c r="B106" s="216">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106" s="216">
+        <v>0</v>
+      </c>
+      <c r="E106" s="991">
+        <v>0</v>
+      </c>
+      <c r="F106" s="216">
+        <v>2</v>
+      </c>
+      <c r="G106" s="216">
+        <v>1</v>
+      </c>
+      <c r="H106" s="216">
+        <v>1</v>
+      </c>
+      <c r="I106" s="216">
+        <v>1</v>
+      </c>
+      <c r="J106" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18902,10 +19440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:CY20"/>
+  <dimension ref="A1:DC20"/>
   <sheetViews>
-    <sheetView topLeftCell="CE1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="CX17" sqref="CX17"/>
+    <sheetView topLeftCell="CQ1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="DC5" sqref="DC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18913,7 +19451,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -19223,8 +19761,18 @@
       <c r="CY1" s="49">
         <v>44084</v>
       </c>
-    </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ1" s="49">
+        <v>44085</v>
+      </c>
+      <c r="DA1" s="49">
+        <v>44086</v>
+      </c>
+      <c r="DB1" s="49">
+        <v>44087</v>
+      </c>
+      <c r="DC1" s="49"/>
+    </row>
+    <row r="2" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -19534,8 +20082,17 @@
       <c r="CY2">
         <v>6182</v>
       </c>
-    </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ2">
+        <v>6214</v>
+      </c>
+      <c r="DA2">
+        <v>6246</v>
+      </c>
+      <c r="DB2">
+        <v>6278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -19845,8 +20402,17 @@
       <c r="CY3">
         <v>5986</v>
       </c>
-    </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ3">
+        <v>6018</v>
+      </c>
+      <c r="DA3">
+        <v>6050</v>
+      </c>
+      <c r="DB3">
+        <v>6082</v>
+      </c>
+    </row>
+    <row r="4" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -20156,8 +20722,17 @@
       <c r="CY4">
         <v>5986</v>
       </c>
-    </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ4">
+        <v>6018</v>
+      </c>
+      <c r="DA4">
+        <v>6050</v>
+      </c>
+      <c r="DB4">
+        <v>6082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -20467,8 +21042,17 @@
       <c r="CY5">
         <v>5986</v>
       </c>
-    </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ5">
+        <v>6018</v>
+      </c>
+      <c r="DA5">
+        <v>6050</v>
+      </c>
+      <c r="DB5">
+        <v>6082</v>
+      </c>
+    </row>
+    <row r="6" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -20778,8 +21362,17 @@
       <c r="CY6">
         <v>5986</v>
       </c>
-    </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ6">
+        <v>6018</v>
+      </c>
+      <c r="DA6">
+        <v>6050</v>
+      </c>
+      <c r="DB6">
+        <v>6082</v>
+      </c>
+    </row>
+    <row r="7" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -21089,8 +21682,17 @@
       <c r="CY7">
         <v>5287</v>
       </c>
-    </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ7">
+        <v>5319</v>
+      </c>
+      <c r="DA7">
+        <v>5351</v>
+      </c>
+      <c r="DB7">
+        <v>5383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -21400,8 +22002,17 @@
       <c r="CY8">
         <v>7917</v>
       </c>
-    </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ8">
+        <v>7949</v>
+      </c>
+      <c r="DA8">
+        <v>7981</v>
+      </c>
+      <c r="DB8">
+        <v>8013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -21503,8 +22114,14 @@
       <c r="CU9" s="312"/>
       <c r="CV9" s="312"/>
       <c r="CW9" s="312"/>
-    </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CX9" s="312"/>
+      <c r="CY9" s="312"/>
+      <c r="CZ9" s="312"/>
+      <c r="DA9" s="312"/>
+      <c r="DB9" s="312"/>
+      <c r="DC9" s="312"/>
+    </row>
+    <row r="10" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -21814,8 +22431,17 @@
       <c r="CY10" s="216">
         <v>242</v>
       </c>
-    </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ10" s="216">
+        <v>243</v>
+      </c>
+      <c r="DA10" s="216">
+        <v>244</v>
+      </c>
+      <c r="DB10" s="216">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -22125,8 +22751,17 @@
       <c r="CY11" s="216">
         <v>242</v>
       </c>
-    </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ11" s="216">
+        <v>243</v>
+      </c>
+      <c r="DA11" s="216">
+        <v>244</v>
+      </c>
+      <c r="DB11" s="216">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -22436,8 +23071,17 @@
       <c r="CY12" s="216">
         <v>242</v>
       </c>
-    </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ12" s="216">
+        <v>243</v>
+      </c>
+      <c r="DA12" s="216">
+        <v>244</v>
+      </c>
+      <c r="DB12" s="216">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -22747,8 +23391,17 @@
       <c r="CY13" s="216">
         <v>242</v>
       </c>
-    </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ13" s="216">
+        <v>243</v>
+      </c>
+      <c r="DA13" s="216">
+        <v>244</v>
+      </c>
+      <c r="DB13" s="216">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -23058,8 +23711,17 @@
       <c r="CY14" s="216">
         <v>242</v>
       </c>
-    </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ14" s="216">
+        <v>243</v>
+      </c>
+      <c r="DA14" s="216">
+        <v>244</v>
+      </c>
+      <c r="DB14" s="216">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -23369,8 +24031,17 @@
       <c r="CY15" s="216">
         <v>177</v>
       </c>
-    </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ15" s="216">
+        <v>178</v>
+      </c>
+      <c r="DA15" s="216">
+        <v>179</v>
+      </c>
+      <c r="DB15" s="216">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -23680,8 +24351,17 @@
       <c r="CY16" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ16" s="216">
+        <v>255</v>
+      </c>
+      <c r="DA16" s="216">
+        <v>256</v>
+      </c>
+      <c r="DB16" s="216">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -23785,8 +24465,12 @@
       <c r="CW17" s="312"/>
       <c r="CX17" s="312"/>
       <c r="CY17" s="312"/>
-    </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ17" s="312"/>
+      <c r="DA17" s="312"/>
+      <c r="DB17" s="312"/>
+      <c r="DC17" s="312"/>
+    </row>
+    <row r="18" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -24096,15 +24780,24 @@
       <c r="CY18">
         <v>1435</v>
       </c>
-    </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.2">
+      <c r="CZ18">
+        <v>1442</v>
+      </c>
+      <c r="DA18">
+        <v>1449</v>
+      </c>
+      <c r="DB18">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -24273,7 +24966,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:CY20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DB20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -24515,6 +25208,18 @@
       <c r="CY20" s="51">
         <f t="shared" si="1"/>
         <v>46406</v>
+      </c>
+      <c r="CZ20" s="51">
+        <f t="shared" si="1"/>
+        <v>46644</v>
+      </c>
+      <c r="DA20" s="51">
+        <f t="shared" si="1"/>
+        <v>46882</v>
+      </c>
+      <c r="DB20" s="51">
+        <f t="shared" si="1"/>
+        <v>47120</v>
       </c>
     </row>
   </sheetData>
@@ -24526,8 +25231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610D31D3-402F-2A4F-A746-AC1D6E48FFD9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24758,8 +25463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24841,43 +25546,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="961" t="s">
+      <c r="B8" s="988" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="961"/>
+      <c r="B9" s="988"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="961"/>
+      <c r="B10" s="988"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="961"/>
+      <c r="B11" s="988"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="962" t="s">
+      <c r="B12" s="989" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="962"/>
+      <c r="B13" s="989"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="962"/>
+      <c r="B14" s="989"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="963" t="s">
+      <c r="B15" s="990" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="963"/>
+      <c r="B16" s="990"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 14th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3C5565-9570-464F-AFB2-20D726954B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CCF71-089C-D84C-BB7A-179BFF3D574F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32380" yWindow="3360" windowWidth="28800" windowHeight="16420" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="992">
+  <cellXfs count="1001">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3514,6 +3514,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3523,7 +3551,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3843,10 +3870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B110" sqref="B110"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7246,6 +7273,38 @@
         <v>1516588</v>
       </c>
     </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="15">
+        <v>44088</v>
+      </c>
+      <c r="B107" s="989">
+        <v>671716</v>
+      </c>
+      <c r="C107" s="990">
+        <v>770197</v>
+      </c>
+      <c r="D107" s="991">
+        <v>78550</v>
+      </c>
+      <c r="E107" s="992">
+        <v>71049</v>
+      </c>
+      <c r="F107" s="993">
+        <v>24.569758648000047</v>
+      </c>
+      <c r="G107" s="994">
+        <v>165039</v>
+      </c>
+      <c r="H107" s="995">
+        <v>14205</v>
+      </c>
+      <c r="I107" s="996">
+        <v>29946</v>
+      </c>
+      <c r="J107" s="997">
+        <v>1520463</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7253,11 +7312,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11388,6 +11447,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A107" s="15">
+        <v>44088</v>
+      </c>
+      <c r="B107" s="216">
+        <v>0</v>
+      </c>
+      <c r="C107" s="216">
+        <v>1</v>
+      </c>
+      <c r="D107" s="216">
+        <v>0</v>
+      </c>
+      <c r="E107" s="216">
+        <v>0</v>
+      </c>
+      <c r="F107" s="216">
+        <v>1</v>
+      </c>
+      <c r="G107" s="216">
+        <v>0</v>
+      </c>
+      <c r="H107" s="216">
+        <v>0</v>
+      </c>
+      <c r="I107" s="216">
+        <v>0</v>
+      </c>
+      <c r="J107" s="216">
+        <v>0</v>
+      </c>
+      <c r="K107" s="216">
+        <v>0</v>
+      </c>
+      <c r="L107" s="216">
+        <v>1</v>
+      </c>
+      <c r="M107" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11395,11 +11495,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N106" sqref="N106"/>
+      <selection pane="bottomLeft" activeCell="O107" sqref="O107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15986,7 +16086,7 @@
       <c r="D106" s="216">
         <v>0</v>
       </c>
-      <c r="E106" s="991">
+      <c r="E106" s="988">
         <v>0</v>
       </c>
       <c r="F106" s="216">
@@ -16014,6 +16114,50 @@
         <v>0</v>
       </c>
       <c r="N106" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" s="15">
+        <v>44088</v>
+      </c>
+      <c r="B107" s="216">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107" s="216">
+        <v>0</v>
+      </c>
+      <c r="E107" s="988">
+        <v>0</v>
+      </c>
+      <c r="F107" s="216">
+        <v>0</v>
+      </c>
+      <c r="G107" s="216">
+        <v>0</v>
+      </c>
+      <c r="H107" s="216">
+        <v>1</v>
+      </c>
+      <c r="I107" s="216">
+        <v>0</v>
+      </c>
+      <c r="J107" s="216">
+        <v>0</v>
+      </c>
+      <c r="K107" s="216">
+        <v>1</v>
+      </c>
+      <c r="L107" s="216">
+        <v>0</v>
+      </c>
+      <c r="M107" s="216">
+        <v>0</v>
+      </c>
+      <c r="N107" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16024,11 +16168,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G106" sqref="G106"/>
+      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19414,7 +19558,7 @@
       <c r="D106" s="216">
         <v>0</v>
       </c>
-      <c r="E106" s="991">
+      <c r="E106" s="988">
         <v>0</v>
       </c>
       <c r="F106" s="216">
@@ -19430,6 +19574,38 @@
         <v>1</v>
       </c>
       <c r="J106" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="15">
+        <v>44088</v>
+      </c>
+      <c r="B107" s="216">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107" s="216">
+        <v>0</v>
+      </c>
+      <c r="E107" s="988">
+        <v>0</v>
+      </c>
+      <c r="F107" s="216">
+        <v>2</v>
+      </c>
+      <c r="G107" s="216">
+        <v>1</v>
+      </c>
+      <c r="H107" s="216">
+        <v>1</v>
+      </c>
+      <c r="I107" s="216">
+        <v>1</v>
+      </c>
+      <c r="J107" s="216">
         <v>2</v>
       </c>
     </row>
@@ -19442,8 +19618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:DC20"/>
   <sheetViews>
-    <sheetView topLeftCell="CQ1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DC5" sqref="DC5"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="DB20" sqref="DB20:DC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19770,7 +19946,9 @@
       <c r="DB1" s="49">
         <v>44087</v>
       </c>
-      <c r="DC1" s="49"/>
+      <c r="DC1" s="49">
+        <v>44088</v>
+      </c>
     </row>
     <row r="2" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -20091,6 +20269,9 @@
       <c r="DB2">
         <v>6278</v>
       </c>
+      <c r="DC2">
+        <v>6310</v>
+      </c>
     </row>
     <row r="3" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -20411,6 +20592,9 @@
       <c r="DB3">
         <v>6082</v>
       </c>
+      <c r="DC3">
+        <v>6114</v>
+      </c>
     </row>
     <row r="4" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -20731,6 +20915,9 @@
       <c r="DB4">
         <v>6082</v>
       </c>
+      <c r="DC4">
+        <v>6114</v>
+      </c>
     </row>
     <row r="5" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -21051,6 +21238,9 @@
       <c r="DB5">
         <v>6082</v>
       </c>
+      <c r="DC5">
+        <v>6114</v>
+      </c>
     </row>
     <row r="6" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -21371,6 +21561,9 @@
       <c r="DB6">
         <v>6082</v>
       </c>
+      <c r="DC6">
+        <v>6114</v>
+      </c>
     </row>
     <row r="7" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -21691,6 +21884,9 @@
       <c r="DB7">
         <v>5383</v>
       </c>
+      <c r="DC7">
+        <v>5415</v>
+      </c>
     </row>
     <row r="8" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -22010,6 +22206,9 @@
       </c>
       <c r="DB8">
         <v>8013</v>
+      </c>
+      <c r="DC8">
+        <v>8045</v>
       </c>
     </row>
     <row r="9" spans="1:107" x14ac:dyDescent="0.2">
@@ -22440,6 +22639,9 @@
       <c r="DB10" s="216">
         <v>245</v>
       </c>
+      <c r="DC10" s="216">
+        <v>246</v>
+      </c>
     </row>
     <row r="11" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -22760,6 +22962,9 @@
       <c r="DB11" s="216">
         <v>245</v>
       </c>
+      <c r="DC11" s="216">
+        <v>246</v>
+      </c>
     </row>
     <row r="12" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -23080,6 +23285,9 @@
       <c r="DB12" s="216">
         <v>245</v>
       </c>
+      <c r="DC12" s="216">
+        <v>246</v>
+      </c>
     </row>
     <row r="13" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -23400,6 +23608,9 @@
       <c r="DB13" s="216">
         <v>245</v>
       </c>
+      <c r="DC13" s="216">
+        <v>246</v>
+      </c>
     </row>
     <row r="14" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -23720,6 +23931,9 @@
       <c r="DB14" s="216">
         <v>245</v>
       </c>
+      <c r="DC14" s="216">
+        <v>246</v>
+      </c>
     </row>
     <row r="15" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -24040,6 +24254,9 @@
       <c r="DB15" s="216">
         <v>180</v>
       </c>
+      <c r="DC15" s="216">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -24359,6 +24576,9 @@
       </c>
       <c r="DB16" s="216">
         <v>257</v>
+      </c>
+      <c r="DC16" s="216">
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:107" x14ac:dyDescent="0.2">
@@ -24789,6 +25009,9 @@
       <c r="DB18">
         <v>1456</v>
       </c>
+      <c r="DC18">
+        <v>1463</v>
+      </c>
     </row>
     <row r="19" spans="1:107" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
@@ -24966,7 +25189,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DB20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DC20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -25220,6 +25443,10 @@
       <c r="DB20" s="51">
         <f t="shared" si="1"/>
         <v>47120</v>
+      </c>
+      <c r="DC20" s="51">
+        <f t="shared" si="1"/>
+        <v>47358</v>
       </c>
     </row>
   </sheetData>
@@ -25463,7 +25690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E78EC-272C-5848-A336-E1FF0CC85A4A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B11"/>
     </sheetView>
   </sheetViews>
@@ -25546,43 +25773,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="988" t="s">
+      <c r="B8" s="998" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="988"/>
+      <c r="B9" s="998"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="988"/>
+      <c r="B10" s="998"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="988"/>
+      <c r="B11" s="998"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="989" t="s">
+      <c r="B12" s="999" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="989"/>
+      <c r="B13" s="999"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="989"/>
+      <c r="B14" s="999"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="990" t="s">
+      <c r="B15" s="1000" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="990"/>
+      <c r="B16" s="1000"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 15th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CCF71-089C-D84C-BB7A-179BFF3D574F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4F45D8-588B-9D40-A556-BDE111D3DB1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1001">
+  <cellXfs count="1010">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3870,10 +3897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7305,6 +7332,38 @@
         <v>1520463</v>
       </c>
     </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>44089</v>
+      </c>
+      <c r="B108" s="998">
+        <v>676487</v>
+      </c>
+      <c r="C108" s="999">
+        <v>777715</v>
+      </c>
+      <c r="D108" s="1000">
+        <v>80407</v>
+      </c>
+      <c r="E108" s="1001">
+        <v>71678</v>
+      </c>
+      <c r="F108" s="1002">
+        <v>24.553021713647123</v>
+      </c>
+      <c r="G108" s="1003">
+        <v>166098</v>
+      </c>
+      <c r="H108" s="1004">
+        <v>14273</v>
+      </c>
+      <c r="I108" s="1005">
+        <v>30048</v>
+      </c>
+      <c r="J108" s="1006">
+        <v>1534609</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7312,11 +7371,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:M108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+      <selection pane="bottomLeft" activeCell="N108" sqref="N108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11488,6 +11547,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>44089</v>
+      </c>
+      <c r="B108" s="216">
+        <v>0</v>
+      </c>
+      <c r="C108" s="216">
+        <v>1</v>
+      </c>
+      <c r="D108" s="550">
+        <v>0</v>
+      </c>
+      <c r="E108" s="216">
+        <v>0</v>
+      </c>
+      <c r="F108" s="216">
+        <v>1</v>
+      </c>
+      <c r="G108" s="216">
+        <v>0</v>
+      </c>
+      <c r="H108" s="216">
+        <v>0</v>
+      </c>
+      <c r="I108" s="216">
+        <v>0</v>
+      </c>
+      <c r="J108" s="216">
+        <v>0</v>
+      </c>
+      <c r="K108" s="216">
+        <v>0</v>
+      </c>
+      <c r="L108" s="216">
+        <v>1</v>
+      </c>
+      <c r="M108" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11495,11 +11595,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O107"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O107" sqref="O107"/>
+      <selection pane="bottomLeft" activeCell="O108" sqref="O108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16158,6 +16258,50 @@
         <v>0</v>
       </c>
       <c r="N107" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>44089</v>
+      </c>
+      <c r="B108" s="216">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" s="216">
+        <v>0</v>
+      </c>
+      <c r="E108" s="988">
+        <v>0</v>
+      </c>
+      <c r="F108" s="216">
+        <v>0</v>
+      </c>
+      <c r="G108" s="216">
+        <v>0</v>
+      </c>
+      <c r="H108" s="216">
+        <v>1</v>
+      </c>
+      <c r="I108" s="216">
+        <v>0</v>
+      </c>
+      <c r="J108" s="216">
+        <v>0</v>
+      </c>
+      <c r="K108" s="216">
+        <v>1</v>
+      </c>
+      <c r="L108" s="216">
+        <v>0</v>
+      </c>
+      <c r="M108" s="216">
+        <v>0</v>
+      </c>
+      <c r="N108" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16168,11 +16312,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
+      <selection pane="bottomLeft" activeCell="K108" sqref="K108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19609,6 +19753,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="15">
+        <v>44089</v>
+      </c>
+      <c r="B108" s="216">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108" s="216">
+        <v>0</v>
+      </c>
+      <c r="E108" s="988">
+        <v>0</v>
+      </c>
+      <c r="F108" s="216">
+        <v>2</v>
+      </c>
+      <c r="G108" s="216">
+        <v>1</v>
+      </c>
+      <c r="H108" s="216">
+        <v>1</v>
+      </c>
+      <c r="I108" s="216">
+        <v>1</v>
+      </c>
+      <c r="J108" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19616,10 +19792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DC20"/>
+  <dimension ref="A1:DD20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DB20" sqref="DB20:DC20"/>
+      <selection activeCell="DG11" sqref="DG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19627,7 +19803,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -19949,8 +20125,11 @@
       <c r="DC1" s="49">
         <v>44088</v>
       </c>
-    </row>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD1" s="49">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="2" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -20272,8 +20451,11 @@
       <c r="DC2">
         <v>6310</v>
       </c>
-    </row>
-    <row r="3" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD2">
+        <v>6342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -20595,8 +20777,11 @@
       <c r="DC3">
         <v>6114</v>
       </c>
-    </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD3">
+        <v>6146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -20918,8 +21103,11 @@
       <c r="DC4">
         <v>6114</v>
       </c>
-    </row>
-    <row r="5" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD4">
+        <v>6146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -21241,8 +21429,11 @@
       <c r="DC5">
         <v>6114</v>
       </c>
-    </row>
-    <row r="6" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD5">
+        <v>6146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -21564,8 +21755,11 @@
       <c r="DC6">
         <v>6114</v>
       </c>
-    </row>
-    <row r="7" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD6">
+        <v>6146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -21887,8 +22081,11 @@
       <c r="DC7">
         <v>5415</v>
       </c>
-    </row>
-    <row r="8" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD7">
+        <v>5447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -22210,8 +22407,11 @@
       <c r="DC8">
         <v>8045</v>
       </c>
-    </row>
-    <row r="9" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD8">
+        <v>8077</v>
+      </c>
+    </row>
+    <row r="9" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -22320,7 +22520,7 @@
       <c r="DB9" s="312"/>
       <c r="DC9" s="312"/>
     </row>
-    <row r="10" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -22642,8 +22842,11 @@
       <c r="DC10" s="216">
         <v>246</v>
       </c>
-    </row>
-    <row r="11" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD10" s="216">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -22965,8 +23168,11 @@
       <c r="DC11" s="216">
         <v>246</v>
       </c>
-    </row>
-    <row r="12" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD11" s="216">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -23288,8 +23494,11 @@
       <c r="DC12" s="216">
         <v>246</v>
       </c>
-    </row>
-    <row r="13" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD12" s="216">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -23611,8 +23820,11 @@
       <c r="DC13" s="216">
         <v>246</v>
       </c>
-    </row>
-    <row r="14" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD13" s="216">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -23934,8 +24146,11 @@
       <c r="DC14" s="216">
         <v>246</v>
       </c>
-    </row>
-    <row r="15" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD14" s="216">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -24257,8 +24472,11 @@
       <c r="DC15" s="216">
         <v>181</v>
       </c>
-    </row>
-    <row r="16" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD15" s="216">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -24580,8 +24798,11 @@
       <c r="DC16" s="216">
         <v>258</v>
       </c>
-    </row>
-    <row r="17" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD16" s="216">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -24690,7 +24911,7 @@
       <c r="DB17" s="312"/>
       <c r="DC17" s="312"/>
     </row>
-    <row r="18" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -25012,15 +25233,18 @@
       <c r="DC18">
         <v>1463</v>
       </c>
-    </row>
-    <row r="19" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="DD18">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="19" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:107" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:108" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -25189,7 +25413,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DC20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DD20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -25447,6 +25671,10 @@
       <c r="DC20" s="51">
         <f t="shared" si="1"/>
         <v>47358</v>
+      </c>
+      <c r="DD20" s="51">
+        <f t="shared" si="1"/>
+        <v>47596</v>
       </c>
     </row>
   </sheetData>
@@ -25773,43 +26001,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="998" t="s">
+      <c r="B8" s="1007" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="998"/>
+      <c r="B9" s="1007"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="998"/>
+      <c r="B10" s="1007"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="998"/>
+      <c r="B11" s="1007"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="999" t="s">
+      <c r="B12" s="1008" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="999"/>
+      <c r="B13" s="1008"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="999"/>
+      <c r="B14" s="1008"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1000" t="s">
+      <c r="B15" s="1009" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1000"/>
+      <c r="B16" s="1009"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 16th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4F45D8-588B-9D40-A556-BDE111D3DB1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392893E3-A56A-1A45-88D5-1F84358D61E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1010">
+  <cellXfs count="1019">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3897,10 +3924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7364,6 +7391,38 @@
         <v>1534609</v>
       </c>
     </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="15">
+        <v>44090</v>
+      </c>
+      <c r="B109" s="1007">
+        <v>680931</v>
+      </c>
+      <c r="C109" s="1008">
+        <v>785019</v>
+      </c>
+      <c r="D109" s="1009">
+        <v>79622</v>
+      </c>
+      <c r="E109" s="1010">
+        <v>71978</v>
+      </c>
+      <c r="F109" s="1011">
+        <v>24.500720337302898</v>
+      </c>
+      <c r="G109" s="1012">
+        <v>166833</v>
+      </c>
+      <c r="H109" s="1013">
+        <v>14346</v>
+      </c>
+      <c r="I109" s="1014">
+        <v>30113</v>
+      </c>
+      <c r="J109" s="1015">
+        <v>1545572</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7371,11 +7430,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N108" sqref="N108"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M109" sqref="M109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11588,6 +11647,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" s="15">
+        <v>44090</v>
+      </c>
+      <c r="B109" s="216">
+        <v>0</v>
+      </c>
+      <c r="C109" s="216">
+        <v>1</v>
+      </c>
+      <c r="D109" s="216">
+        <v>0</v>
+      </c>
+      <c r="E109" s="216">
+        <v>0</v>
+      </c>
+      <c r="F109" s="216">
+        <v>1</v>
+      </c>
+      <c r="G109" s="216">
+        <v>0</v>
+      </c>
+      <c r="H109" s="216">
+        <v>0</v>
+      </c>
+      <c r="I109" s="216">
+        <v>0</v>
+      </c>
+      <c r="J109" s="216">
+        <v>0</v>
+      </c>
+      <c r="K109" s="216">
+        <v>0</v>
+      </c>
+      <c r="L109" s="216">
+        <v>1</v>
+      </c>
+      <c r="M109" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11595,11 +11695,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O108"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O108" sqref="O108"/>
+      <selection pane="bottomLeft" activeCell="O109" sqref="O109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16302,6 +16402,50 @@
         <v>0</v>
       </c>
       <c r="N108" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A109" s="906">
+        <v>44090</v>
+      </c>
+      <c r="B109" s="216">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" s="216">
+        <v>0</v>
+      </c>
+      <c r="E109" s="988">
+        <v>0</v>
+      </c>
+      <c r="F109" s="216">
+        <v>0</v>
+      </c>
+      <c r="G109" s="216">
+        <v>0</v>
+      </c>
+      <c r="H109" s="216">
+        <v>1</v>
+      </c>
+      <c r="I109" s="216">
+        <v>0</v>
+      </c>
+      <c r="J109" s="216">
+        <v>0</v>
+      </c>
+      <c r="K109" s="216">
+        <v>1</v>
+      </c>
+      <c r="L109" s="216">
+        <v>0</v>
+      </c>
+      <c r="M109" s="216">
+        <v>0</v>
+      </c>
+      <c r="N109" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16312,11 +16456,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J108"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K108" sqref="K108"/>
+      <selection pane="bottomLeft" activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19785,6 +19929,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="906">
+        <v>44090</v>
+      </c>
+      <c r="B109" s="216">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109" s="216">
+        <v>0</v>
+      </c>
+      <c r="E109" s="988">
+        <v>0</v>
+      </c>
+      <c r="F109" s="216">
+        <v>2</v>
+      </c>
+      <c r="G109" s="216">
+        <v>1</v>
+      </c>
+      <c r="H109" s="216">
+        <v>1</v>
+      </c>
+      <c r="I109" s="216">
+        <v>1</v>
+      </c>
+      <c r="J109" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19792,10 +19968,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DD20"/>
+  <dimension ref="A1:DF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DG11" sqref="DG11"/>
+    <sheetView tabSelected="1" topLeftCell="CM1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="DB23" sqref="DB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19803,7 +19979,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -20128,8 +20304,11 @@
       <c r="DD1" s="49">
         <v>44089</v>
       </c>
-    </row>
-    <row r="2" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE1" s="49">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -20454,8 +20633,11 @@
       <c r="DD2">
         <v>6342</v>
       </c>
-    </row>
-    <row r="3" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE2">
+        <v>6374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -20780,8 +20962,11 @@
       <c r="DD3">
         <v>6146</v>
       </c>
-    </row>
-    <row r="4" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE3">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -21106,8 +21291,11 @@
       <c r="DD4">
         <v>6146</v>
       </c>
-    </row>
-    <row r="5" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE4">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -21432,8 +21620,11 @@
       <c r="DD5">
         <v>6146</v>
       </c>
-    </row>
-    <row r="6" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE5">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -21758,8 +21949,11 @@
       <c r="DD6">
         <v>6146</v>
       </c>
-    </row>
-    <row r="7" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE6">
+        <v>6178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -22084,8 +22278,11 @@
       <c r="DD7">
         <v>5447</v>
       </c>
-    </row>
-    <row r="8" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE7">
+        <v>5479</v>
+      </c>
+    </row>
+    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -22410,8 +22607,11 @@
       <c r="DD8">
         <v>8077</v>
       </c>
-    </row>
-    <row r="9" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE8">
+        <v>8109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -22520,7 +22720,7 @@
       <c r="DB9" s="312"/>
       <c r="DC9" s="312"/>
     </row>
-    <row r="10" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -22845,8 +23045,11 @@
       <c r="DD10" s="216">
         <v>247</v>
       </c>
-    </row>
-    <row r="11" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE10" s="216">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -23171,8 +23374,11 @@
       <c r="DD11" s="216">
         <v>247</v>
       </c>
-    </row>
-    <row r="12" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE11" s="216">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -23497,8 +23703,11 @@
       <c r="DD12" s="216">
         <v>247</v>
       </c>
-    </row>
-    <row r="13" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE12" s="216">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -23823,8 +24032,11 @@
       <c r="DD13" s="216">
         <v>247</v>
       </c>
-    </row>
-    <row r="14" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE13" s="216">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -24149,8 +24361,11 @@
       <c r="DD14" s="216">
         <v>247</v>
       </c>
-    </row>
-    <row r="15" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE14" s="216">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -24475,8 +24690,12 @@
       <c r="DD15" s="216">
         <v>182</v>
       </c>
-    </row>
-    <row r="16" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE15" s="216">
+        <v>183</v>
+      </c>
+      <c r="DF15" s="216"/>
+    </row>
+    <row r="16" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -24801,8 +25020,11 @@
       <c r="DD16" s="216">
         <v>259</v>
       </c>
-    </row>
-    <row r="17" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE16" s="216">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -24911,7 +25133,7 @@
       <c r="DB17" s="312"/>
       <c r="DC17" s="312"/>
     </row>
-    <row r="18" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -25236,15 +25458,18 @@
       <c r="DD18">
         <v>1470</v>
       </c>
-    </row>
-    <row r="19" spans="1:108" x14ac:dyDescent="0.2">
+      <c r="DE18">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="19" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:108" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -25413,7 +25638,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DD20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DE20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -25675,6 +25900,10 @@
       <c r="DD20" s="51">
         <f t="shared" si="1"/>
         <v>47596</v>
+      </c>
+      <c r="DE20" s="51">
+        <f t="shared" si="1"/>
+        <v>47834</v>
       </c>
     </row>
   </sheetData>
@@ -26001,43 +26230,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1007" t="s">
+      <c r="B8" s="1016" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1007"/>
+      <c r="B9" s="1016"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1007"/>
+      <c r="B10" s="1016"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1007"/>
+      <c r="B11" s="1016"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1008" t="s">
+      <c r="B12" s="1017" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1008"/>
+      <c r="B13" s="1017"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1008"/>
+      <c r="B14" s="1017"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1009" t="s">
+      <c r="B15" s="1018" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1009"/>
+      <c r="B16" s="1018"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 17th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392893E3-A56A-1A45-88D5-1F84358D61E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6C06B-6CCB-8C4D-8F7B-66ABE005ABD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="30400" yWindow="4440" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1019">
+  <cellXfs count="1028">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -3924,10 +3951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7423,6 +7450,38 @@
         <v>1545572</v>
       </c>
     </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="15">
+        <v>44091</v>
+      </c>
+      <c r="B110" s="1016">
+        <v>684113</v>
+      </c>
+      <c r="C110" s="1017">
+        <v>789978</v>
+      </c>
+      <c r="D110" s="1018">
+        <v>75552</v>
+      </c>
+      <c r="E110" s="1019">
+        <v>72179</v>
+      </c>
+      <c r="F110" s="1020">
+        <v>24.481774209816216</v>
+      </c>
+      <c r="G110" s="1021">
+        <v>167483</v>
+      </c>
+      <c r="H110" s="1022">
+        <v>14384</v>
+      </c>
+      <c r="I110" s="1023">
+        <v>30161</v>
+      </c>
+      <c r="J110" s="1024">
+        <v>1549643</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7430,11 +7489,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M109"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M109" sqref="M109"/>
+      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11688,6 +11747,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A110" s="15">
+        <v>44091</v>
+      </c>
+      <c r="B110" s="216">
+        <v>0</v>
+      </c>
+      <c r="C110" s="216">
+        <v>1</v>
+      </c>
+      <c r="D110" s="216">
+        <v>0</v>
+      </c>
+      <c r="E110" s="216">
+        <v>0</v>
+      </c>
+      <c r="F110" s="216">
+        <v>1</v>
+      </c>
+      <c r="G110" s="216">
+        <v>0</v>
+      </c>
+      <c r="H110" s="216">
+        <v>0</v>
+      </c>
+      <c r="I110" s="216">
+        <v>0</v>
+      </c>
+      <c r="J110" s="216">
+        <v>0</v>
+      </c>
+      <c r="K110" s="216">
+        <v>0</v>
+      </c>
+      <c r="L110" s="216">
+        <v>1</v>
+      </c>
+      <c r="M110" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11695,11 +11795,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O109"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O109" sqref="O109"/>
+      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16446,6 +16546,50 @@
         <v>0</v>
       </c>
       <c r="N109" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A110" s="906">
+        <v>44091</v>
+      </c>
+      <c r="B110" s="216">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" s="216">
+        <v>0</v>
+      </c>
+      <c r="E110" s="988">
+        <v>0</v>
+      </c>
+      <c r="F110" s="216">
+        <v>0</v>
+      </c>
+      <c r="G110" s="216">
+        <v>0</v>
+      </c>
+      <c r="H110" s="216">
+        <v>1</v>
+      </c>
+      <c r="I110" s="216">
+        <v>0</v>
+      </c>
+      <c r="J110" s="216">
+        <v>0</v>
+      </c>
+      <c r="K110" s="216">
+        <v>1</v>
+      </c>
+      <c r="L110" s="216">
+        <v>0</v>
+      </c>
+      <c r="M110" s="216">
+        <v>0</v>
+      </c>
+      <c r="N110" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16456,11 +16600,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K109" sqref="K109"/>
+      <selection pane="bottomLeft" activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19961,6 +20105,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="906">
+        <v>44091</v>
+      </c>
+      <c r="B110" s="216">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110" s="216">
+        <v>0</v>
+      </c>
+      <c r="E110" s="988">
+        <v>0</v>
+      </c>
+      <c r="F110" s="216">
+        <v>2</v>
+      </c>
+      <c r="G110" s="216">
+        <v>1</v>
+      </c>
+      <c r="H110" s="216">
+        <v>1</v>
+      </c>
+      <c r="I110" s="216">
+        <v>1</v>
+      </c>
+      <c r="J110" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19970,8 +20146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
   <dimension ref="A1:DF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CM1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DB23" sqref="DB23"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="DH20" sqref="DH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20307,6 +20483,9 @@
       <c r="DE1" s="49">
         <v>44090</v>
       </c>
+      <c r="DF1" s="49">
+        <v>44091</v>
+      </c>
     </row>
     <row r="2" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -20636,6 +20815,9 @@
       <c r="DE2">
         <v>6374</v>
       </c>
+      <c r="DF2">
+        <v>6406</v>
+      </c>
     </row>
     <row r="3" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -20965,6 +21147,9 @@
       <c r="DE3">
         <v>6178</v>
       </c>
+      <c r="DF3">
+        <v>6210</v>
+      </c>
     </row>
     <row r="4" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -21294,6 +21479,9 @@
       <c r="DE4">
         <v>6178</v>
       </c>
+      <c r="DF4">
+        <v>6210</v>
+      </c>
     </row>
     <row r="5" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -21623,6 +21811,9 @@
       <c r="DE5">
         <v>6178</v>
       </c>
+      <c r="DF5">
+        <v>6210</v>
+      </c>
     </row>
     <row r="6" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -21952,6 +22143,9 @@
       <c r="DE6">
         <v>6178</v>
       </c>
+      <c r="DF6">
+        <v>6210</v>
+      </c>
     </row>
     <row r="7" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -22281,6 +22475,9 @@
       <c r="DE7">
         <v>5479</v>
       </c>
+      <c r="DF7">
+        <v>5511</v>
+      </c>
     </row>
     <row r="8" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -22609,6 +22806,9 @@
       </c>
       <c r="DE8">
         <v>8109</v>
+      </c>
+      <c r="DF8">
+        <v>8141</v>
       </c>
     </row>
     <row r="9" spans="1:110" x14ac:dyDescent="0.2">
@@ -23048,6 +23248,9 @@
       <c r="DE10" s="216">
         <v>248</v>
       </c>
+      <c r="DF10" s="216">
+        <v>249</v>
+      </c>
     </row>
     <row r="11" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -23377,6 +23580,9 @@
       <c r="DE11" s="216">
         <v>248</v>
       </c>
+      <c r="DF11" s="216">
+        <v>249</v>
+      </c>
     </row>
     <row r="12" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -23706,6 +23912,9 @@
       <c r="DE12" s="216">
         <v>248</v>
       </c>
+      <c r="DF12" s="216">
+        <v>249</v>
+      </c>
     </row>
     <row r="13" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -24035,6 +24244,9 @@
       <c r="DE13" s="216">
         <v>248</v>
       </c>
+      <c r="DF13" s="216">
+        <v>249</v>
+      </c>
     </row>
     <row r="14" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -24364,6 +24576,9 @@
       <c r="DE14" s="216">
         <v>248</v>
       </c>
+      <c r="DF14" s="216">
+        <v>249</v>
+      </c>
     </row>
     <row r="15" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -24693,7 +24908,9 @@
       <c r="DE15" s="216">
         <v>183</v>
       </c>
-      <c r="DF15" s="216"/>
+      <c r="DF15" s="216">
+        <v>184</v>
+      </c>
     </row>
     <row r="16" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -25023,8 +25240,11 @@
       <c r="DE16" s="216">
         <v>260</v>
       </c>
-    </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.2">
+      <c r="DF16" s="216">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -25133,7 +25353,7 @@
       <c r="DB17" s="312"/>
       <c r="DC17" s="312"/>
     </row>
-    <row r="18" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -25461,15 +25681,18 @@
       <c r="DE18">
         <v>1477</v>
       </c>
-    </row>
-    <row r="19" spans="1:109" x14ac:dyDescent="0.2">
+      <c r="DF18">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -25638,7 +25861,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DE20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DF20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -25904,6 +26127,10 @@
       <c r="DE20" s="51">
         <f t="shared" si="1"/>
         <v>47834</v>
+      </c>
+      <c r="DF20" s="51">
+        <f t="shared" si="1"/>
+        <v>48072</v>
       </c>
     </row>
   </sheetData>
@@ -26230,43 +26457,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1016" t="s">
+      <c r="B8" s="1025" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1016"/>
+      <c r="B9" s="1025"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1016"/>
+      <c r="B10" s="1025"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1016"/>
+      <c r="B11" s="1025"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1017" t="s">
+      <c r="B12" s="1026" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1017"/>
+      <c r="B13" s="1026"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1017"/>
+      <c r="B14" s="1026"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1018" t="s">
+      <c r="B15" s="1027" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1018"/>
+      <c r="B16" s="1027"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 18th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA6C06B-6CCB-8C4D-8F7B-66ABE005ABD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEA4EB-1851-AA47-9841-73B67F96B9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="4440" windowWidth="28800" windowHeight="16420" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>24 de febrero</t>
+  </si>
+  <si>
+    <t>2020-09-18</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1028">
+  <cellXfs count="1038">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3594,6 +3597,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3951,7 +3984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="A110" sqref="A110"/>
@@ -7480,6 +7513,38 @@
       </c>
       <c r="J110" s="1024">
         <v>1549643</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="1025" t="s">
+        <v>83</v>
+      </c>
+      <c r="B111" s="1026">
+        <v>688954</v>
+      </c>
+      <c r="C111" s="1027">
+        <v>797447</v>
+      </c>
+      <c r="D111" s="1028">
+        <v>79051</v>
+      </c>
+      <c r="E111" s="1029">
+        <v>72803</v>
+      </c>
+      <c r="F111" s="1030">
+        <v>24.436464553511556</v>
+      </c>
+      <c r="G111" s="1031">
+        <v>168356</v>
+      </c>
+      <c r="H111" s="1032">
+        <v>14490</v>
+      </c>
+      <c r="I111" s="1033">
+        <v>30268</v>
+      </c>
+      <c r="J111" s="1034">
+        <v>1565452</v>
       </c>
     </row>
   </sheetData>
@@ -16604,7 +16669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K110" sqref="K110"/>
+      <selection pane="bottomLeft" activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20144,10 +20209,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DF20"/>
+  <dimension ref="A1:DG20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DH20" sqref="DH20"/>
+      <selection activeCell="CS25" sqref="CS25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20155,7 +20220,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -20486,8 +20551,11 @@
       <c r="DF1" s="49">
         <v>44091</v>
       </c>
-    </row>
-    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG1" s="49">
+        <v>44092</v>
+      </c>
+    </row>
+    <row r="2" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -20818,8 +20886,11 @@
       <c r="DF2">
         <v>6406</v>
       </c>
-    </row>
-    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG2">
+        <v>6438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -21150,8 +21221,11 @@
       <c r="DF3">
         <v>6210</v>
       </c>
-    </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG3">
+        <v>6242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -21482,8 +21556,11 @@
       <c r="DF4">
         <v>6210</v>
       </c>
-    </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG4">
+        <v>6242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -21814,8 +21891,11 @@
       <c r="DF5">
         <v>6210</v>
       </c>
-    </row>
-    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG5">
+        <v>6242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -22146,8 +22226,11 @@
       <c r="DF6">
         <v>6210</v>
       </c>
-    </row>
-    <row r="7" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG6">
+        <v>6242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -22478,8 +22561,11 @@
       <c r="DF7">
         <v>5511</v>
       </c>
-    </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG7">
+        <v>5543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -22810,8 +22896,11 @@
       <c r="DF8">
         <v>8141</v>
       </c>
-    </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG8">
+        <v>8173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -22920,7 +23009,7 @@
       <c r="DB9" s="312"/>
       <c r="DC9" s="312"/>
     </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -23251,8 +23340,11 @@
       <c r="DF10" s="216">
         <v>249</v>
       </c>
-    </row>
-    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG10" s="216">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -23583,8 +23675,11 @@
       <c r="DF11" s="216">
         <v>249</v>
       </c>
-    </row>
-    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG11" s="216">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -23915,8 +24010,11 @@
       <c r="DF12" s="216">
         <v>249</v>
       </c>
-    </row>
-    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG12" s="216">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -24247,8 +24345,11 @@
       <c r="DF13" s="216">
         <v>249</v>
       </c>
-    </row>
-    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG13" s="216">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -24579,8 +24680,11 @@
       <c r="DF14" s="216">
         <v>249</v>
       </c>
-    </row>
-    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG14" s="216">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -24911,8 +25015,11 @@
       <c r="DF15" s="216">
         <v>184</v>
       </c>
-    </row>
-    <row r="16" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG15" s="216">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -25243,8 +25350,11 @@
       <c r="DF16" s="216">
         <v>261</v>
       </c>
-    </row>
-    <row r="17" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG16" s="216">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -25353,7 +25463,7 @@
       <c r="DB17" s="312"/>
       <c r="DC17" s="312"/>
     </row>
-    <row r="18" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -25684,15 +25794,18 @@
       <c r="DF18">
         <v>1484</v>
       </c>
-    </row>
-    <row r="19" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DG18">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -25861,7 +25974,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DF20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DG20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -26131,6 +26244,10 @@
       <c r="DF20" s="51">
         <f t="shared" si="1"/>
         <v>48072</v>
+      </c>
+      <c r="DG20" s="51">
+        <f t="shared" si="1"/>
+        <v>48310</v>
       </c>
     </row>
   </sheetData>
@@ -26457,43 +26574,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1025" t="s">
+      <c r="B8" s="1035" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1025"/>
+      <c r="B9" s="1035"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1025"/>
+      <c r="B10" s="1035"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1025"/>
+      <c r="B11" s="1035"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1026" t="s">
+      <c r="B12" s="1036" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1026"/>
+      <c r="B13" s="1036"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1026"/>
+      <c r="B14" s="1036"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1027" t="s">
+      <c r="B15" s="1037" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1027"/>
+      <c r="B16" s="1037"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 19th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEA4EB-1851-AA47-9841-73B67F96B9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6845CE-BFAE-9C45-A133-0B67141A1933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="32180" yWindow="2320" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>24 de febrero</t>
-  </si>
-  <si>
-    <t>2020-09-18</t>
   </si>
 </sst>
 </file>
@@ -612,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1038">
+  <cellXfs count="1046">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3626,7 +3623,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -3984,10 +4005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="A111" sqref="A111:A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7515,36 +7536,68 @@
         <v>1549643</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="1025" t="s">
-        <v>83</v>
-      </c>
-      <c r="B111" s="1026">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="15">
+        <v>44092</v>
+      </c>
+      <c r="B111" s="1025">
         <v>688954</v>
       </c>
-      <c r="C111" s="1027">
+      <c r="C111" s="1026">
         <v>797447</v>
       </c>
-      <c r="D111" s="1028">
+      <c r="D111" s="1027">
         <v>79051</v>
       </c>
-      <c r="E111" s="1029">
+      <c r="E111" s="1028">
         <v>72803</v>
       </c>
-      <c r="F111" s="1030">
+      <c r="F111" s="1029">
         <v>24.436464553511556</v>
       </c>
-      <c r="G111" s="1031">
+      <c r="G111" s="1030">
         <v>168356</v>
       </c>
-      <c r="H111" s="1032">
+      <c r="H111" s="1031">
         <v>14490</v>
       </c>
-      <c r="I111" s="1033">
+      <c r="I111" s="1032">
         <v>30268</v>
       </c>
-      <c r="J111" s="1034">
+      <c r="J111" s="1033">
         <v>1565452</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="15">
+        <v>44093</v>
+      </c>
+      <c r="B112" s="1034">
+        <v>694121</v>
+      </c>
+      <c r="C112" s="1035">
+        <v>804832</v>
+      </c>
+      <c r="D112" s="1036">
+        <v>81424</v>
+      </c>
+      <c r="E112" s="1037">
+        <v>73258</v>
+      </c>
+      <c r="F112" s="1038">
+        <v>24.38522966456857</v>
+      </c>
+      <c r="G112" s="1039">
+        <v>169263</v>
+      </c>
+      <c r="H112" s="1040">
+        <v>14565</v>
+      </c>
+      <c r="I112" s="1041">
+        <v>30357</v>
+      </c>
+      <c r="J112" s="1042">
+        <v>1580377</v>
       </c>
     </row>
   </sheetData>
@@ -7554,11 +7607,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
+      <selection pane="bottomLeft" activeCell="M113" sqref="M113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11853,6 +11906,88 @@
         <v>4</v>
       </c>
     </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" s="15">
+        <v>44092</v>
+      </c>
+      <c r="B111" s="216">
+        <v>0</v>
+      </c>
+      <c r="C111" s="216">
+        <v>1</v>
+      </c>
+      <c r="D111" s="216">
+        <v>0</v>
+      </c>
+      <c r="E111" s="216">
+        <v>0</v>
+      </c>
+      <c r="F111" s="216">
+        <v>1</v>
+      </c>
+      <c r="G111" s="216">
+        <v>0</v>
+      </c>
+      <c r="H111" s="216">
+        <v>0</v>
+      </c>
+      <c r="I111" s="216">
+        <v>0</v>
+      </c>
+      <c r="J111" s="216">
+        <v>0</v>
+      </c>
+      <c r="K111" s="216">
+        <v>0</v>
+      </c>
+      <c r="L111" s="216">
+        <v>1</v>
+      </c>
+      <c r="M111" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112" s="15">
+        <v>44093</v>
+      </c>
+      <c r="B112" s="216">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" s="216">
+        <v>0</v>
+      </c>
+      <c r="E112" s="988">
+        <v>0</v>
+      </c>
+      <c r="F112" s="216">
+        <v>1</v>
+      </c>
+      <c r="G112" s="216">
+        <v>0</v>
+      </c>
+      <c r="H112" s="216">
+        <v>0</v>
+      </c>
+      <c r="I112" s="216">
+        <v>0</v>
+      </c>
+      <c r="J112" s="216">
+        <v>0</v>
+      </c>
+      <c r="K112" s="216">
+        <v>0</v>
+      </c>
+      <c r="L112" s="216">
+        <v>1</v>
+      </c>
+      <c r="M112" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11860,11 +11995,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:O112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
+      <selection pane="bottomLeft" activeCell="N112" sqref="N112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16655,6 +16790,94 @@
         <v>0</v>
       </c>
       <c r="N110" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A111" s="906">
+        <v>44092</v>
+      </c>
+      <c r="B111" s="216">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" s="216">
+        <v>0</v>
+      </c>
+      <c r="E111" s="988">
+        <v>0</v>
+      </c>
+      <c r="F111" s="216">
+        <v>0</v>
+      </c>
+      <c r="G111" s="216">
+        <v>0</v>
+      </c>
+      <c r="H111" s="216">
+        <v>1</v>
+      </c>
+      <c r="I111" s="216">
+        <v>0</v>
+      </c>
+      <c r="J111" s="216">
+        <v>0</v>
+      </c>
+      <c r="K111" s="216">
+        <v>1</v>
+      </c>
+      <c r="L111" s="216">
+        <v>0</v>
+      </c>
+      <c r="M111" s="216">
+        <v>0</v>
+      </c>
+      <c r="N111" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A112" s="906">
+        <v>44093</v>
+      </c>
+      <c r="B112" s="216">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" s="216">
+        <v>0</v>
+      </c>
+      <c r="E112" s="988">
+        <v>0</v>
+      </c>
+      <c r="F112" s="216">
+        <v>0</v>
+      </c>
+      <c r="G112" s="216">
+        <v>0</v>
+      </c>
+      <c r="H112" s="216">
+        <v>1</v>
+      </c>
+      <c r="I112" s="216">
+        <v>0</v>
+      </c>
+      <c r="J112" s="216">
+        <v>0</v>
+      </c>
+      <c r="K112" s="216">
+        <v>1</v>
+      </c>
+      <c r="L112" s="216">
+        <v>0</v>
+      </c>
+      <c r="M112" s="216">
+        <v>0</v>
+      </c>
+      <c r="N112" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16665,11 +16888,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F115" sqref="F115"/>
+      <selection pane="bottomLeft" activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20202,6 +20425,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="906">
+        <v>44092</v>
+      </c>
+      <c r="B111" s="216">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111" s="216">
+        <v>0</v>
+      </c>
+      <c r="E111" s="988">
+        <v>0</v>
+      </c>
+      <c r="F111" s="216">
+        <v>2</v>
+      </c>
+      <c r="G111" s="216">
+        <v>1</v>
+      </c>
+      <c r="H111" s="216">
+        <v>1</v>
+      </c>
+      <c r="I111" s="216">
+        <v>1</v>
+      </c>
+      <c r="J111" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="906">
+        <v>44093</v>
+      </c>
+      <c r="B112" s="216">
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112" s="216">
+        <v>0</v>
+      </c>
+      <c r="E112" s="988">
+        <v>0</v>
+      </c>
+      <c r="F112" s="216">
+        <v>2</v>
+      </c>
+      <c r="G112" s="216">
+        <v>1</v>
+      </c>
+      <c r="H112" s="216">
+        <v>1</v>
+      </c>
+      <c r="I112" s="216">
+        <v>1</v>
+      </c>
+      <c r="J112" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20209,10 +20496,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DG20"/>
+  <dimension ref="A1:DH20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="CS25" sqref="CS25"/>
+      <selection activeCell="DG18" sqref="DG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20220,7 +20507,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:111" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -20554,8 +20841,11 @@
       <c r="DG1" s="49">
         <v>44092</v>
       </c>
-    </row>
-    <row r="2" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH1" s="49">
+        <v>44093</v>
+      </c>
+    </row>
+    <row r="2" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -20889,8 +21179,11 @@
       <c r="DG2">
         <v>6438</v>
       </c>
-    </row>
-    <row r="3" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH2">
+        <v>6470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -21224,8 +21517,11 @@
       <c r="DG3">
         <v>6242</v>
       </c>
-    </row>
-    <row r="4" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH3">
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -21559,8 +21855,11 @@
       <c r="DG4">
         <v>6242</v>
       </c>
-    </row>
-    <row r="5" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH4">
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -21894,8 +22193,11 @@
       <c r="DG5">
         <v>6242</v>
       </c>
-    </row>
-    <row r="6" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH5">
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -22229,8 +22531,11 @@
       <c r="DG6">
         <v>6242</v>
       </c>
-    </row>
-    <row r="7" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH6">
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -22564,8 +22869,11 @@
       <c r="DG7">
         <v>5543</v>
       </c>
-    </row>
-    <row r="8" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH7">
+        <v>5575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -22899,8 +23207,11 @@
       <c r="DG8">
         <v>8173</v>
       </c>
-    </row>
-    <row r="9" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH8">
+        <v>8205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -23008,8 +23319,13 @@
       <c r="DA9" s="312"/>
       <c r="DB9" s="312"/>
       <c r="DC9" s="312"/>
-    </row>
-    <row r="10" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DD9" s="312"/>
+      <c r="DE9" s="312"/>
+      <c r="DF9" s="312"/>
+      <c r="DG9" s="312"/>
+      <c r="DH9" s="312"/>
+    </row>
+    <row r="10" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -23343,8 +23659,11 @@
       <c r="DG10" s="216">
         <v>250</v>
       </c>
-    </row>
-    <row r="11" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH10" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -23678,8 +23997,11 @@
       <c r="DG11" s="216">
         <v>250</v>
       </c>
-    </row>
-    <row r="12" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH11" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -24013,8 +24335,11 @@
       <c r="DG12" s="216">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH12" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -24348,8 +24673,11 @@
       <c r="DG13" s="216">
         <v>250</v>
       </c>
-    </row>
-    <row r="14" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH13" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -24683,8 +25011,11 @@
       <c r="DG14" s="216">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH14" s="216">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -25018,8 +25349,11 @@
       <c r="DG15" s="216">
         <v>185</v>
       </c>
-    </row>
-    <row r="16" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH15" s="216">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -25353,8 +25687,11 @@
       <c r="DG16" s="216">
         <v>262</v>
       </c>
-    </row>
-    <row r="17" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH16" s="216">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -25462,8 +25799,13 @@
       <c r="DA17" s="312"/>
       <c r="DB17" s="312"/>
       <c r="DC17" s="312"/>
-    </row>
-    <row r="18" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DD17" s="312"/>
+      <c r="DE17" s="312"/>
+      <c r="DF17" s="312"/>
+      <c r="DG17" s="312"/>
+      <c r="DH17" s="312"/>
+    </row>
+    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -25797,15 +26139,18 @@
       <c r="DG18">
         <v>1491</v>
       </c>
-    </row>
-    <row r="19" spans="1:111" x14ac:dyDescent="0.2">
+      <c r="DH18">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:111" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -25974,7 +26319,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DG20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DH20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -26248,6 +26593,10 @@
       <c r="DG20" s="51">
         <f t="shared" si="1"/>
         <v>48310</v>
+      </c>
+      <c r="DH20" s="51">
+        <f t="shared" si="1"/>
+        <v>48548</v>
       </c>
     </row>
   </sheetData>
@@ -26574,43 +26923,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1035" t="s">
+      <c r="B8" s="1043" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1035"/>
+      <c r="B9" s="1043"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1035"/>
+      <c r="B10" s="1043"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1035"/>
+      <c r="B11" s="1043"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1036" t="s">
+      <c r="B12" s="1044" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1036"/>
+      <c r="B13" s="1044"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1036"/>
+      <c r="B14" s="1044"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1037" t="s">
+      <c r="B15" s="1045" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1037"/>
+      <c r="B16" s="1045"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 20th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6845CE-BFAE-9C45-A133-0B67141A1933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C42D7E-34D6-A841-A3C2-178BE1A49992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32180" yWindow="2320" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1046">
+  <cellXfs count="1055">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -4005,10 +4032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111:A112"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7600,6 +7627,38 @@
         <v>1580377</v>
       </c>
     </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" s="15">
+        <v>44094</v>
+      </c>
+      <c r="B113" s="1043">
+        <v>697663</v>
+      </c>
+      <c r="C113" s="1044">
+        <v>809373</v>
+      </c>
+      <c r="D113" s="1045">
+        <v>79155</v>
+      </c>
+      <c r="E113" s="1046">
+        <v>73493</v>
+      </c>
+      <c r="F113" s="1047">
+        <v>24.371652216041269</v>
+      </c>
+      <c r="G113" s="1048">
+        <v>170032</v>
+      </c>
+      <c r="H113" s="1049">
+        <v>14605</v>
+      </c>
+      <c r="I113" s="1050">
+        <v>30404</v>
+      </c>
+      <c r="J113" s="1051">
+        <v>1586191</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7607,11 +7666,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M113" sqref="M113"/>
+      <selection pane="bottomLeft" activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11988,6 +12047,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" s="15">
+        <v>44094</v>
+      </c>
+      <c r="B113" s="216">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" s="216">
+        <v>0</v>
+      </c>
+      <c r="E113" s="988">
+        <v>0</v>
+      </c>
+      <c r="F113" s="216">
+        <v>1</v>
+      </c>
+      <c r="G113" s="216">
+        <v>0</v>
+      </c>
+      <c r="H113" s="216">
+        <v>0</v>
+      </c>
+      <c r="I113" s="216">
+        <v>0</v>
+      </c>
+      <c r="J113" s="216">
+        <v>0</v>
+      </c>
+      <c r="K113" s="216">
+        <v>0</v>
+      </c>
+      <c r="L113" s="216">
+        <v>1</v>
+      </c>
+      <c r="M113" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11995,11 +12095,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O112"/>
+  <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N112" sqref="N112"/>
+      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16878,6 +16978,50 @@
         <v>0</v>
       </c>
       <c r="N112" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A113" s="906">
+        <v>44094</v>
+      </c>
+      <c r="B113" s="216">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" s="216">
+        <v>0</v>
+      </c>
+      <c r="E113" s="988">
+        <v>0</v>
+      </c>
+      <c r="F113" s="216">
+        <v>0</v>
+      </c>
+      <c r="G113" s="216">
+        <v>0</v>
+      </c>
+      <c r="H113" s="216">
+        <v>1</v>
+      </c>
+      <c r="I113" s="216">
+        <v>0</v>
+      </c>
+      <c r="J113" s="216">
+        <v>0</v>
+      </c>
+      <c r="K113" s="216">
+        <v>1</v>
+      </c>
+      <c r="L113" s="216">
+        <v>0</v>
+      </c>
+      <c r="M113" s="216">
+        <v>0</v>
+      </c>
+      <c r="N113" s="216">
         <v>0</v>
       </c>
     </row>
@@ -16888,11 +17032,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K111" sqref="K111"/>
+      <selection pane="bottomLeft" activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20489,6 +20633,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" s="906">
+        <v>44094</v>
+      </c>
+      <c r="B113" s="216">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113" s="216">
+        <v>0</v>
+      </c>
+      <c r="E113" s="988">
+        <v>0</v>
+      </c>
+      <c r="F113" s="216">
+        <v>2</v>
+      </c>
+      <c r="G113" s="216">
+        <v>1</v>
+      </c>
+      <c r="H113" s="216">
+        <v>1</v>
+      </c>
+      <c r="I113" s="216">
+        <v>1</v>
+      </c>
+      <c r="J113" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20496,10 +20672,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DH20"/>
+  <dimension ref="A1:DI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DG18" sqref="DG18"/>
+    <sheetView tabSelected="1" topLeftCell="CS1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="DL18" sqref="DL18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20507,7 +20683,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -20844,8 +21020,11 @@
       <c r="DH1" s="49">
         <v>44093</v>
       </c>
-    </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI1" s="49">
+        <v>44094</v>
+      </c>
+    </row>
+    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -21182,8 +21361,11 @@
       <c r="DH2">
         <v>6470</v>
       </c>
-    </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI2">
+        <v>6502</v>
+      </c>
+    </row>
+    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -21520,8 +21702,11 @@
       <c r="DH3">
         <v>6274</v>
       </c>
-    </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI3">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -21858,8 +22043,11 @@
       <c r="DH4">
         <v>6274</v>
       </c>
-    </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI4">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -22196,8 +22384,11 @@
       <c r="DH5">
         <v>6274</v>
       </c>
-    </row>
-    <row r="6" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI5">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -22534,8 +22725,11 @@
       <c r="DH6">
         <v>6274</v>
       </c>
-    </row>
-    <row r="7" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI6">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -22872,8 +23066,11 @@
       <c r="DH7">
         <v>5575</v>
       </c>
-    </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI7">
+        <v>5607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -23210,8 +23407,11 @@
       <c r="DH8">
         <v>8205</v>
       </c>
-    </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI8">
+        <v>8237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -23325,7 +23525,7 @@
       <c r="DG9" s="312"/>
       <c r="DH9" s="312"/>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -23662,8 +23862,11 @@
       <c r="DH10" s="216">
         <v>251</v>
       </c>
-    </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI10" s="216">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -24000,8 +24203,11 @@
       <c r="DH11" s="216">
         <v>251</v>
       </c>
-    </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI11" s="216">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -24338,8 +24544,11 @@
       <c r="DH12" s="216">
         <v>251</v>
       </c>
-    </row>
-    <row r="13" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI12" s="216">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -24676,8 +24885,11 @@
       <c r="DH13" s="216">
         <v>251</v>
       </c>
-    </row>
-    <row r="14" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI13" s="216">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -25014,8 +25226,11 @@
       <c r="DH14" s="216">
         <v>251</v>
       </c>
-    </row>
-    <row r="15" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI14" s="216">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -25352,8 +25567,11 @@
       <c r="DH15" s="216">
         <v>186</v>
       </c>
-    </row>
-    <row r="16" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI15" s="216">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -25690,8 +25908,11 @@
       <c r="DH16" s="216">
         <v>263</v>
       </c>
-    </row>
-    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI16" s="216">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -25805,7 +26026,7 @@
       <c r="DG17" s="312"/>
       <c r="DH17" s="312"/>
     </row>
-    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -26142,15 +26363,18 @@
       <c r="DH18">
         <v>1498</v>
       </c>
-    </row>
-    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
+      <c r="DI18">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:112" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -26319,7 +26543,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DH20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DI20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -26597,6 +26821,10 @@
       <c r="DH20" s="51">
         <f t="shared" si="1"/>
         <v>48548</v>
+      </c>
+      <c r="DI20" s="51">
+        <f t="shared" si="1"/>
+        <v>48786</v>
       </c>
     </row>
   </sheetData>
@@ -26923,43 +27151,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1043" t="s">
+      <c r="B8" s="1052" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1043"/>
+      <c r="B9" s="1052"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1043"/>
+      <c r="B10" s="1052"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1043"/>
+      <c r="B11" s="1052"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1044" t="s">
+      <c r="B12" s="1053" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1044"/>
+      <c r="B13" s="1053"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1044"/>
+      <c r="B14" s="1053"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1045" t="s">
+      <c r="B15" s="1054" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1045"/>
+      <c r="B16" s="1054"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 21th
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C42D7E-34D6-A841-A3C2-178BE1A49992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121417B1-6B45-FD45-919A-0B99D5F930A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32180" yWindow="2320" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>24 de febrero</t>
+  </si>
+  <si>
+    <t>2020-09-21</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1055">
+  <cellXfs count="1065">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3675,6 +3678,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -4032,7 +4065,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="A113" sqref="A113"/>
@@ -7657,6 +7690,38 @@
       </c>
       <c r="J113" s="1051">
         <v>1586191</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="1052" t="s">
+        <v>83</v>
+      </c>
+      <c r="B114" s="1053">
+        <v>700580</v>
+      </c>
+      <c r="C114" s="1054">
+        <v>813641</v>
+      </c>
+      <c r="D114" s="1055">
+        <v>75754</v>
+      </c>
+      <c r="E114" s="1056">
+        <v>73697</v>
+      </c>
+      <c r="F114" s="1057">
+        <v>24.347683348083017</v>
+      </c>
+      <c r="G114" s="1058">
+        <v>170575</v>
+      </c>
+      <c r="H114" s="1059">
+        <v>14629</v>
+      </c>
+      <c r="I114" s="1060">
+        <v>30445</v>
+      </c>
+      <c r="J114" s="1061">
+        <v>1589975</v>
       </c>
     </row>
   </sheetData>
@@ -20672,10 +20737,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DI20"/>
+  <dimension ref="A1:DK20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CS1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DL18" sqref="DL18"/>
+      <selection activeCell="DI16" sqref="DI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20683,7 +20748,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -21023,8 +21088,11 @@
       <c r="DI1" s="49">
         <v>44094</v>
       </c>
-    </row>
-    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ1" s="49">
+        <v>44095</v>
+      </c>
+    </row>
+    <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -21364,8 +21432,11 @@
       <c r="DI2">
         <v>6502</v>
       </c>
-    </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ2">
+        <v>6534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -21705,8 +21776,11 @@
       <c r="DI3">
         <v>6306</v>
       </c>
-    </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ3">
+        <v>6338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -22046,8 +22120,11 @@
       <c r="DI4">
         <v>6306</v>
       </c>
-    </row>
-    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ4">
+        <v>6338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -22387,8 +22464,11 @@
       <c r="DI5">
         <v>6306</v>
       </c>
-    </row>
-    <row r="6" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ5">
+        <v>6338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -22728,8 +22808,11 @@
       <c r="DI6">
         <v>6306</v>
       </c>
-    </row>
-    <row r="7" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ6">
+        <v>6338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -23069,8 +23152,11 @@
       <c r="DI7">
         <v>5607</v>
       </c>
-    </row>
-    <row r="8" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ7">
+        <v>5639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -23410,8 +23496,11 @@
       <c r="DI8">
         <v>8237</v>
       </c>
-    </row>
-    <row r="9" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ8">
+        <v>8269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -23524,8 +23613,11 @@
       <c r="DF9" s="312"/>
       <c r="DG9" s="312"/>
       <c r="DH9" s="312"/>
-    </row>
-    <row r="10" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DI9" s="312"/>
+      <c r="DJ9" s="312"/>
+      <c r="DK9" s="312"/>
+    </row>
+    <row r="10" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -23865,8 +23957,11 @@
       <c r="DI10" s="216">
         <v>252</v>
       </c>
-    </row>
-    <row r="11" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ10" s="216">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -24206,8 +24301,11 @@
       <c r="DI11" s="216">
         <v>252</v>
       </c>
-    </row>
-    <row r="12" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ11" s="216">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -24547,8 +24645,11 @@
       <c r="DI12" s="216">
         <v>252</v>
       </c>
-    </row>
-    <row r="13" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ12" s="216">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -24888,8 +24989,11 @@
       <c r="DI13" s="216">
         <v>252</v>
       </c>
-    </row>
-    <row r="14" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ13" s="216">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -25229,8 +25333,11 @@
       <c r="DI14" s="216">
         <v>252</v>
       </c>
-    </row>
-    <row r="15" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ14" s="216">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -25570,8 +25677,11 @@
       <c r="DI15" s="216">
         <v>187</v>
       </c>
-    </row>
-    <row r="16" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ15" s="216">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -25911,8 +26021,11 @@
       <c r="DI16" s="216">
         <v>264</v>
       </c>
-    </row>
-    <row r="17" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ16" s="216">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -26025,8 +26138,10 @@
       <c r="DF17" s="312"/>
       <c r="DG17" s="312"/>
       <c r="DH17" s="312"/>
-    </row>
-    <row r="18" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DI17" s="312"/>
+      <c r="DJ17" s="312"/>
+    </row>
+    <row r="18" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -26366,15 +26481,18 @@
       <c r="DI18">
         <v>1505</v>
       </c>
-    </row>
-    <row r="19" spans="1:113" x14ac:dyDescent="0.2">
+      <c r="DJ18">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -26543,7 +26661,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DI20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DJ20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -26825,6 +26943,10 @@
       <c r="DI20" s="51">
         <f t="shared" si="1"/>
         <v>48786</v>
+      </c>
+      <c r="DJ20" s="51">
+        <f t="shared" si="1"/>
+        <v>49024</v>
       </c>
     </row>
   </sheetData>
@@ -27151,43 +27273,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1052" t="s">
+      <c r="B8" s="1062" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1052"/>
+      <c r="B9" s="1062"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1052"/>
+      <c r="B10" s="1062"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1052"/>
+      <c r="B11" s="1062"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1053" t="s">
+      <c r="B12" s="1063" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1053"/>
+      <c r="B13" s="1063"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1053"/>
+      <c r="B14" s="1063"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1054" t="s">
+      <c r="B15" s="1064" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1054"/>
+      <c r="B16" s="1064"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 22
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121417B1-6B45-FD45-919A-0B99D5F930A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB231AC0-99EA-D345-80E8-7515F1B73948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Fecha del reporte</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>24 de febrero</t>
-  </si>
-  <si>
-    <t>2020-09-21</t>
   </si>
 </sst>
 </file>
@@ -612,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1065">
+  <cellXfs count="1073">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3707,7 +3704,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -4065,10 +4086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7692,36 +7713,68 @@
         <v>1586191</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="1052" t="s">
-        <v>83</v>
-      </c>
-      <c r="B114" s="1053">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" s="15">
+        <v>44095</v>
+      </c>
+      <c r="B114" s="1052">
         <v>700580</v>
       </c>
-      <c r="C114" s="1054">
+      <c r="C114" s="1053">
         <v>813641</v>
       </c>
-      <c r="D114" s="1055">
+      <c r="D114" s="1054">
         <v>75754</v>
       </c>
-      <c r="E114" s="1056">
+      <c r="E114" s="1055">
         <v>73697</v>
       </c>
-      <c r="F114" s="1057">
+      <c r="F114" s="1056">
         <v>24.347683348083017</v>
       </c>
-      <c r="G114" s="1058">
+      <c r="G114" s="1057">
         <v>170575</v>
       </c>
-      <c r="H114" s="1059">
+      <c r="H114" s="1058">
         <v>14629</v>
       </c>
-      <c r="I114" s="1060">
+      <c r="I114" s="1059">
         <v>30445</v>
       </c>
-      <c r="J114" s="1061">
+      <c r="J114" s="1060">
         <v>1589975</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" s="15">
+        <v>44096</v>
+      </c>
+      <c r="B115" s="1061">
+        <v>705263</v>
+      </c>
+      <c r="C115" s="1062">
+        <v>820675</v>
+      </c>
+      <c r="D115" s="1063">
+        <v>78907</v>
+      </c>
+      <c r="E115" s="1064">
+        <v>74348</v>
+      </c>
+      <c r="F115" s="1065">
+        <v>24.322132310925141</v>
+      </c>
+      <c r="G115" s="1066">
+        <v>171535</v>
+      </c>
+      <c r="H115" s="1067">
+        <v>14711</v>
+      </c>
+      <c r="I115" s="1068">
+        <v>30625</v>
+      </c>
+      <c r="J115" s="1069">
+        <v>1604845</v>
       </c>
     </row>
   </sheetData>
@@ -7731,11 +7784,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M113"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N113" sqref="N113"/>
+      <selection pane="bottomLeft" activeCell="N114" sqref="N114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12112,7 +12165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="15">
         <v>44094</v>
       </c>
@@ -12150,6 +12203,88 @@
         <v>1</v>
       </c>
       <c r="M113" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="15">
+        <v>44095</v>
+      </c>
+      <c r="B114" s="216">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" s="216">
+        <v>0</v>
+      </c>
+      <c r="E114" s="988">
+        <v>0</v>
+      </c>
+      <c r="F114" s="216">
+        <v>1</v>
+      </c>
+      <c r="G114" s="216">
+        <v>0</v>
+      </c>
+      <c r="H114" s="216">
+        <v>0</v>
+      </c>
+      <c r="I114" s="216">
+        <v>0</v>
+      </c>
+      <c r="J114" s="216">
+        <v>0</v>
+      </c>
+      <c r="K114" s="216">
+        <v>0</v>
+      </c>
+      <c r="L114" s="216">
+        <v>1</v>
+      </c>
+      <c r="M114" s="216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" s="15">
+        <v>44096</v>
+      </c>
+      <c r="B115" s="216">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" s="216">
+        <v>0</v>
+      </c>
+      <c r="E115" s="988">
+        <v>0</v>
+      </c>
+      <c r="F115" s="216">
+        <v>1</v>
+      </c>
+      <c r="G115" s="216">
+        <v>0</v>
+      </c>
+      <c r="H115" s="216">
+        <v>0</v>
+      </c>
+      <c r="I115" s="216">
+        <v>0</v>
+      </c>
+      <c r="J115" s="216">
+        <v>0</v>
+      </c>
+      <c r="K115" s="216">
+        <v>0</v>
+      </c>
+      <c r="L115" s="216">
+        <v>1</v>
+      </c>
+      <c r="M115" s="216">
         <v>4</v>
       </c>
     </row>
@@ -12160,11 +12295,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O113"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17087,6 +17222,94 @@
         <v>0</v>
       </c>
       <c r="N113" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A114" s="15">
+        <v>44095</v>
+      </c>
+      <c r="B114" s="216">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" s="216">
+        <v>0</v>
+      </c>
+      <c r="E114" s="988">
+        <v>0</v>
+      </c>
+      <c r="F114" s="216">
+        <v>0</v>
+      </c>
+      <c r="G114" s="216">
+        <v>0</v>
+      </c>
+      <c r="H114" s="216">
+        <v>1</v>
+      </c>
+      <c r="I114" s="216">
+        <v>0</v>
+      </c>
+      <c r="J114" s="216">
+        <v>0</v>
+      </c>
+      <c r="K114" s="216">
+        <v>1</v>
+      </c>
+      <c r="L114" s="216">
+        <v>0</v>
+      </c>
+      <c r="M114" s="216">
+        <v>0</v>
+      </c>
+      <c r="N114" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="15">
+        <v>44096</v>
+      </c>
+      <c r="B115" s="216">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" s="216">
+        <v>0</v>
+      </c>
+      <c r="E115" s="988">
+        <v>0</v>
+      </c>
+      <c r="F115" s="216">
+        <v>0</v>
+      </c>
+      <c r="G115" s="216">
+        <v>0</v>
+      </c>
+      <c r="H115" s="216">
+        <v>1</v>
+      </c>
+      <c r="I115" s="216">
+        <v>0</v>
+      </c>
+      <c r="J115" s="216">
+        <v>0</v>
+      </c>
+      <c r="K115" s="216">
+        <v>1</v>
+      </c>
+      <c r="L115" s="216">
+        <v>0</v>
+      </c>
+      <c r="M115" s="216">
+        <v>0</v>
+      </c>
+      <c r="N115" s="216">
         <v>0</v>
       </c>
     </row>
@@ -17097,11 +17320,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K113" sqref="K113"/>
+      <selection pane="bottomLeft" activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20730,6 +20953,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" s="15">
+        <v>44095</v>
+      </c>
+      <c r="B114" s="216">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114" s="216">
+        <v>0</v>
+      </c>
+      <c r="E114" s="988">
+        <v>0</v>
+      </c>
+      <c r="F114" s="216">
+        <v>2</v>
+      </c>
+      <c r="G114" s="216">
+        <v>1</v>
+      </c>
+      <c r="H114" s="216">
+        <v>1</v>
+      </c>
+      <c r="I114" s="216">
+        <v>1</v>
+      </c>
+      <c r="J114" s="216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" s="15">
+        <v>44096</v>
+      </c>
+      <c r="B115" s="216">
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115" s="216">
+        <v>0</v>
+      </c>
+      <c r="E115" s="988">
+        <v>0</v>
+      </c>
+      <c r="F115" s="216">
+        <v>2</v>
+      </c>
+      <c r="G115" s="216">
+        <v>1</v>
+      </c>
+      <c r="H115" s="216">
+        <v>1</v>
+      </c>
+      <c r="I115" s="216">
+        <v>1</v>
+      </c>
+      <c r="J115" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20740,7 +21027,7 @@
   <dimension ref="A1:DK20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CS1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DI16" sqref="DI16"/>
+      <selection activeCell="DL25" sqref="DL25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21091,6 +21378,9 @@
       <c r="DJ1" s="49">
         <v>44095</v>
       </c>
+      <c r="DK1" s="49">
+        <v>44096</v>
+      </c>
     </row>
     <row r="2" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -21435,6 +21725,9 @@
       <c r="DJ2">
         <v>6534</v>
       </c>
+      <c r="DK2">
+        <v>6566</v>
+      </c>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
@@ -21779,6 +22072,9 @@
       <c r="DJ3">
         <v>6338</v>
       </c>
+      <c r="DK3">
+        <v>6370</v>
+      </c>
     </row>
     <row r="4" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
@@ -22123,6 +22419,9 @@
       <c r="DJ4">
         <v>6338</v>
       </c>
+      <c r="DK4">
+        <v>6370</v>
+      </c>
     </row>
     <row r="5" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
@@ -22467,6 +22766,9 @@
       <c r="DJ5">
         <v>6338</v>
       </c>
+      <c r="DK5">
+        <v>6370</v>
+      </c>
     </row>
     <row r="6" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
@@ -22811,6 +23113,9 @@
       <c r="DJ6">
         <v>6338</v>
       </c>
+      <c r="DK6">
+        <v>6370</v>
+      </c>
     </row>
     <row r="7" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -23155,6 +23460,9 @@
       <c r="DJ7">
         <v>5639</v>
       </c>
+      <c r="DK7">
+        <v>5671</v>
+      </c>
     </row>
     <row r="8" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -23498,6 +23806,9 @@
       </c>
       <c r="DJ8">
         <v>8269</v>
+      </c>
+      <c r="DK8">
+        <v>8301</v>
       </c>
     </row>
     <row r="9" spans="1:115" x14ac:dyDescent="0.2">
@@ -23960,6 +24271,9 @@
       <c r="DJ10" s="216">
         <v>253</v>
       </c>
+      <c r="DK10" s="216">
+        <v>254</v>
+      </c>
     </row>
     <row r="11" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -24304,6 +24618,9 @@
       <c r="DJ11" s="216">
         <v>253</v>
       </c>
+      <c r="DK11" s="216">
+        <v>254</v>
+      </c>
     </row>
     <row r="12" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
@@ -24648,6 +24965,9 @@
       <c r="DJ12" s="216">
         <v>253</v>
       </c>
+      <c r="DK12" s="216">
+        <v>254</v>
+      </c>
     </row>
     <row r="13" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
@@ -24992,6 +25312,9 @@
       <c r="DJ13" s="216">
         <v>253</v>
       </c>
+      <c r="DK13" s="216">
+        <v>254</v>
+      </c>
     </row>
     <row r="14" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
@@ -25336,6 +25659,9 @@
       <c r="DJ14" s="216">
         <v>253</v>
       </c>
+      <c r="DK14" s="216">
+        <v>254</v>
+      </c>
     </row>
     <row r="15" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
@@ -25680,6 +26006,9 @@
       <c r="DJ15" s="216">
         <v>188</v>
       </c>
+      <c r="DK15" s="216">
+        <v>189</v>
+      </c>
     </row>
     <row r="16" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
@@ -26024,8 +26353,11 @@
       <c r="DJ16" s="216">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:114" x14ac:dyDescent="0.2">
+      <c r="DK16" s="216">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -26141,7 +26473,7 @@
       <c r="DI17" s="312"/>
       <c r="DJ17" s="312"/>
     </row>
-    <row r="18" spans="1:114" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -26484,15 +26816,18 @@
       <c r="DJ18">
         <v>1512</v>
       </c>
-    </row>
-    <row r="19" spans="1:114" x14ac:dyDescent="0.2">
+      <c r="DK18">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:114" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:115" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -26661,7 +26996,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DJ20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DK20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -26947,6 +27282,10 @@
       <c r="DJ20" s="51">
         <f t="shared" si="1"/>
         <v>49024</v>
+      </c>
+      <c r="DK20" s="51">
+        <f t="shared" si="1"/>
+        <v>49262</v>
       </c>
     </row>
   </sheetData>
@@ -27273,43 +27612,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1062" t="s">
+      <c r="B8" s="1070" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1062"/>
+      <c r="B9" s="1070"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1062"/>
+      <c r="B10" s="1070"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1062"/>
+      <c r="B11" s="1070"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1063" t="s">
+      <c r="B12" s="1071" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1063"/>
+      <c r="B13" s="1071"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1063"/>
+      <c r="B14" s="1071"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1064" t="s">
+      <c r="B15" s="1072" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1064"/>
+      <c r="B16" s="1072"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 23
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB231AC0-99EA-D345-80E8-7515F1B73948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446E838E-9F51-B946-9B83-4AF910C7C9DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1073">
+  <cellXfs count="1082">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -4086,10 +4113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7777,6 +7804,38 @@
         <v>1604845</v>
       </c>
     </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="15">
+        <v>44097</v>
+      </c>
+      <c r="B116" s="1070">
+        <v>710049</v>
+      </c>
+      <c r="C116" s="1071">
+        <v>828280</v>
+      </c>
+      <c r="D116" s="1072">
+        <v>82549</v>
+      </c>
+      <c r="E116" s="1073">
+        <v>74949</v>
+      </c>
+      <c r="F116" s="1074">
+        <v>24.279451136470865</v>
+      </c>
+      <c r="G116" s="1075">
+        <v>172396</v>
+      </c>
+      <c r="H116" s="1076">
+        <v>14796</v>
+      </c>
+      <c r="I116" s="1077">
+        <v>30737</v>
+      </c>
+      <c r="J116" s="1078">
+        <v>1620878</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7784,11 +7843,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N114" sqref="N114"/>
+      <selection pane="bottomLeft" activeCell="N116" sqref="N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12288,6 +12347,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="15">
+        <v>44097</v>
+      </c>
+      <c r="B116" s="216">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" s="216">
+        <v>0</v>
+      </c>
+      <c r="E116" s="988">
+        <v>0</v>
+      </c>
+      <c r="F116" s="216">
+        <v>1</v>
+      </c>
+      <c r="G116" s="216">
+        <v>0</v>
+      </c>
+      <c r="H116" s="216">
+        <v>0</v>
+      </c>
+      <c r="I116" s="216">
+        <v>0</v>
+      </c>
+      <c r="J116" s="216">
+        <v>0</v>
+      </c>
+      <c r="K116" s="216">
+        <v>0</v>
+      </c>
+      <c r="L116" s="216">
+        <v>1</v>
+      </c>
+      <c r="M116" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12295,11 +12395,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
+      <selection pane="bottomLeft" activeCell="O116" sqref="O116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17310,6 +17410,50 @@
         <v>0</v>
       </c>
       <c r="N115" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="906">
+        <v>44097</v>
+      </c>
+      <c r="B116" s="216">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" s="216">
+        <v>0</v>
+      </c>
+      <c r="E116" s="988">
+        <v>0</v>
+      </c>
+      <c r="F116" s="216">
+        <v>0</v>
+      </c>
+      <c r="G116" s="216">
+        <v>0</v>
+      </c>
+      <c r="H116" s="216">
+        <v>1</v>
+      </c>
+      <c r="I116" s="216">
+        <v>0</v>
+      </c>
+      <c r="J116" s="216">
+        <v>0</v>
+      </c>
+      <c r="K116" s="216">
+        <v>1</v>
+      </c>
+      <c r="L116" s="216">
+        <v>0</v>
+      </c>
+      <c r="M116" s="216">
+        <v>0</v>
+      </c>
+      <c r="N116" s="216">
         <v>0</v>
       </c>
     </row>
@@ -17320,11 +17464,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89B5D0E-982D-C94A-83B9-13567C2B7BAD}">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K115" sqref="K115"/>
+      <selection pane="bottomLeft" activeCell="K116" sqref="K116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21017,6 +21161,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="906">
+        <v>44097</v>
+      </c>
+      <c r="B116" s="216">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116" s="216">
+        <v>0</v>
+      </c>
+      <c r="E116" s="988">
+        <v>0</v>
+      </c>
+      <c r="F116" s="216">
+        <v>2</v>
+      </c>
+      <c r="G116" s="216">
+        <v>1</v>
+      </c>
+      <c r="H116" s="216">
+        <v>1</v>
+      </c>
+      <c r="I116" s="216">
+        <v>1</v>
+      </c>
+      <c r="J116" s="216">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21024,10 +21200,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD28A3-AE8D-9347-ADB6-2FE78E30A53F}">
-  <dimension ref="A1:DK20"/>
+  <dimension ref="A1:DL20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CS1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="DL25" sqref="DL25"/>
+      <selection activeCell="DO18" sqref="DO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21035,7 +21211,7 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -21381,8 +21557,11 @@
       <c r="DK1" s="49">
         <v>44096</v>
       </c>
-    </row>
-    <row r="2" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL1" s="49">
+        <v>44097</v>
+      </c>
+    </row>
+    <row r="2" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
@@ -21728,8 +21907,11 @@
       <c r="DK2">
         <v>6566</v>
       </c>
-    </row>
-    <row r="3" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL2">
+        <v>6598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
@@ -22075,8 +22257,11 @@
       <c r="DK3">
         <v>6370</v>
       </c>
-    </row>
-    <row r="4" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL3">
+        <v>6402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
@@ -22422,8 +22607,11 @@
       <c r="DK4">
         <v>6370</v>
       </c>
-    </row>
-    <row r="5" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL4">
+        <v>6402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>26</v>
       </c>
@@ -22769,8 +22957,11 @@
       <c r="DK5">
         <v>6370</v>
       </c>
-    </row>
-    <row r="6" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL5">
+        <v>6402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
@@ -23116,8 +23307,11 @@
       <c r="DK6">
         <v>6370</v>
       </c>
-    </row>
-    <row r="7" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL6">
+        <v>6402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>28</v>
       </c>
@@ -23463,8 +23657,11 @@
       <c r="DK7">
         <v>5671</v>
       </c>
-    </row>
-    <row r="8" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL7">
+        <v>5703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>29</v>
       </c>
@@ -23810,8 +24007,11 @@
       <c r="DK8">
         <v>8301</v>
       </c>
-    </row>
-    <row r="9" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL8">
+        <v>8333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -23928,7 +24128,7 @@
       <c r="DJ9" s="312"/>
       <c r="DK9" s="312"/>
     </row>
-    <row r="10" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>30</v>
       </c>
@@ -24274,8 +24474,11 @@
       <c r="DK10" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="11" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL10" s="216">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
@@ -24621,8 +24824,11 @@
       <c r="DK11" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="12" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL11" s="216">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
@@ -24968,8 +25174,11 @@
       <c r="DK12" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="13" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL12" s="216">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>33</v>
       </c>
@@ -25315,8 +25524,11 @@
       <c r="DK13" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="14" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL13" s="216">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>34</v>
       </c>
@@ -25662,8 +25874,11 @@
       <c r="DK14" s="216">
         <v>254</v>
       </c>
-    </row>
-    <row r="15" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL14" s="216">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>35</v>
       </c>
@@ -26009,8 +26224,11 @@
       <c r="DK15" s="216">
         <v>189</v>
       </c>
-    </row>
-    <row r="16" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL15" s="216">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>36</v>
       </c>
@@ -26356,8 +26574,11 @@
       <c r="DK16" s="216">
         <v>266</v>
       </c>
-    </row>
-    <row r="17" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL16" s="216">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A17" s="75"/>
       <c r="B17" s="76"/>
       <c r="C17" s="76"/>
@@ -26473,7 +26694,7 @@
       <c r="DI17" s="312"/>
       <c r="DJ17" s="312"/>
     </row>
-    <row r="18" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>37</v>
       </c>
@@ -26819,15 +27040,18 @@
       <c r="DK18">
         <v>1519</v>
       </c>
-    </row>
-    <row r="19" spans="1:115" x14ac:dyDescent="0.2">
+      <c r="DL18">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
     </row>
-    <row r="20" spans="1:115" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:116" x14ac:dyDescent="0.2">
       <c r="A20" s="37" t="s">
         <v>38</v>
       </c>
@@ -26996,7 +27220,7 @@
         <v>32123</v>
       </c>
       <c r="AQ20" s="51">
-        <f t="shared" ref="AQ20:DK20" si="1">SUM(AQ2:AQ18)</f>
+        <f t="shared" ref="AQ20:DL20" si="1">SUM(AQ2:AQ18)</f>
         <v>32361</v>
       </c>
       <c r="AR20" s="51">
@@ -27286,6 +27510,10 @@
       <c r="DK20" s="51">
         <f t="shared" si="1"/>
         <v>49262</v>
+      </c>
+      <c r="DL20" s="51">
+        <f t="shared" si="1"/>
+        <v>49500</v>
       </c>
     </row>
   </sheetData>
@@ -27612,43 +27840,43 @@
       <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="1070" t="s">
+      <c r="B8" s="1079" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1070"/>
+      <c r="B9" s="1079"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1070"/>
+      <c r="B10" s="1079"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="1070"/>
+      <c r="B11" s="1079"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="1071" t="s">
+      <c r="B12" s="1080" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="1071"/>
+      <c r="B13" s="1080"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="1071"/>
+      <c r="B14" s="1080"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="1072" t="s">
+      <c r="B15" s="1081" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1072"/>
+      <c r="B16" s="1081"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for September 24
</commit_message>
<xml_diff>
--- a/data-validation/bitacora_historica_datos_abiertos.xlsx
+++ b/data-validation/bitacora_historica_datos_abiertos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/PADeCI/covid19-mx-data/data-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446E838E-9F51-B946-9B83-4AF910C7C9DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DFDD04-64F9-F645-B28D-F2CDFB54F139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="6" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="out_vars" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1082">
+  <cellXfs count="1091">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3515,6 +3515,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -4113,10 +4140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7836,6 +7863,38 @@
         <v>1620878</v>
       </c>
     </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" s="15">
+        <v>44098</v>
+      </c>
+      <c r="B117" s="1079">
+        <v>715457</v>
+      </c>
+      <c r="C117" s="1080">
+        <v>835985</v>
+      </c>
+      <c r="D117" s="1081">
+        <v>84348</v>
+      </c>
+      <c r="E117" s="1082">
+        <v>75439</v>
+      </c>
+      <c r="F117" s="1083">
+        <v>24.219764430287217</v>
+      </c>
+      <c r="G117" s="1084">
+        <v>173282</v>
+      </c>
+      <c r="H117" s="1085">
+        <v>14884</v>
+      </c>
+      <c r="I117" s="1086">
+        <v>30835</v>
+      </c>
+      <c r="J117" s="1087">
+        <v>1635790</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7843,11 +7902,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC80AF03-9DC5-3341-A7B9-960FFE6C934F}">
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:M117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N116" sqref="N116"/>
+      <selection pane="bottomLeft" activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12388,6 +12447,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" s="15">
+        <v>44098</v>
+      </c>
+      <c r="B117" s="216">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" s="216">
+        <v>0</v>
+      </c>
+      <c r="E117" s="988">
+        <v>0</v>
+      </c>
+      <c r="F117" s="216">
+        <v>1</v>
+      </c>
+      <c r="G117" s="216">
+        <v>0</v>
+      </c>
+      <c r="H117" s="216">
+        <v>0</v>
+      </c>
+      <c r="I117" s="216">
+        <v>0</v>
+      </c>
+      <c r="J117" s="216">
+        <v>0</v>
+      </c>
+      <c r="K117" s="216">
+        <v>0</v>
+      </c>
+      <c r="L117" s="216">
+        <v>1</v>
+      </c>
+      <c r="M117" s="216">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12395,11 +12495,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06A027-128D-604F-AB62-F8E54138A11A}">
-  <dimension ref="A1:O116"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O116" sqref="O116"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17454,6 +17554,50 @@
         <v>0</v>
       </c>
       <c r="N116" s="216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" s="906">
+        <v>44098</v>
+      </c>
+      <c r="B117" s="216">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117" s="216">
+        <v>0</v>
+      </c>
+      <c r="E117" s="988">
+        <v>0</v>
+      </c>
+      <c r="F117" s="216">
+        <v>0</v>
+      </c>
+      <c r="G117" s="216">
+        <v>0</v>
+      </c>
+      <c r="H117" s="216">
+        <v>1</v>
+      </c>
+      <c r="I117" s="216">
+        <v>0</v>
+      </c>
+      <c r="J117" s="216">
+        <v>0</v>
+      </c>
+      <c r="K117" s="216">
+        <v>1</v>
+      </c>
+      <c r="L117" s="216">
+        <v>0</v>
+      </c>
+      <c r="M117" s="216">
+        <v>0</v>
+      </c>
+      <c r="N117" s="216">
         <v>0</v>
       </c>
     </row>
@@ -17464,11 +17608,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.or